<commit_message>
Add Try to GetDataWithIndicator
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/COP-19-Target-Setting/data-raw/model_calculations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36970B55-FB50-084B-841E-09BCD9577CCA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6BFBC34-5E66-8A44-8DB7-176FF5DF95E9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4000" yWindow="720" windowWidth="25600" windowHeight="20020" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="4000" yWindow="720" windowWidth="25600" windowHeight="20020" activeTab="1" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1869" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="440">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1321,6 +1321,42 @@
   </si>
   <si>
     <t>HTS Modality (USE ONLY for FY18 Results/FY19 Targets)</t>
+  </si>
+  <si>
+    <t>gdHE7Kk9Q1k.PmA9jG2I2PY</t>
+  </si>
+  <si>
+    <t>PrEP_NEW (N, TA, KeyPop) TARGET MSM</t>
+  </si>
+  <si>
+    <t>gdHE7Kk9Q1k.bQfzRTksp0Y</t>
+  </si>
+  <si>
+    <t>PrEP_NEW (N, TA, KeyPop) TARGET FSW</t>
+  </si>
+  <si>
+    <t>lXqlw8UxoqF.RbB7UEptrN6</t>
+  </si>
+  <si>
+    <t>PrEP_NEW (N, DSD, KeyPop) TARGET TG</t>
+  </si>
+  <si>
+    <t>lXqlw8UxoqF.j8AfwCZj95X</t>
+  </si>
+  <si>
+    <t>PrEP_NEW (N, DSD, KeyPop) TARGET Other Key Populations</t>
+  </si>
+  <si>
+    <t>lXqlw8UxoqF.PmA9jG2I2PY</t>
+  </si>
+  <si>
+    <t>PrEP_NEW (N, DSD, KeyPop) TARGET MSM</t>
+  </si>
+  <si>
+    <t>lXqlw8UxoqF.bQfzRTksp0Y</t>
+  </si>
+  <si>
+    <t>PrEP_NEW (N, DSD, KeyPop) TARGET FSW</t>
   </si>
 </sst>
 </file>
@@ -1739,8 +1775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
   <dimension ref="A1:V54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="K30" sqref="K30"/>
     </sheetView>
@@ -5342,15 +5378,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D15FCD2F-A9CC-CD4F-8AF1-79C36D527EBB}">
-  <dimension ref="A1:AF44"/>
+  <dimension ref="A1:AF46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37.5" customWidth="1"/>
+    <col min="2" max="2" width="72.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49.1640625" bestFit="1" customWidth="1"/>
@@ -5990,23 +6027,107 @@
     <row r="38" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="F38" s="16"/>
     </row>
-    <row r="39" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="F39" s="16"/>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" t="s">
+        <v>107</v>
+      </c>
+      <c r="C39" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>108</v>
+      </c>
+      <c r="E39" t="s">
+        <v>4</v>
+      </c>
+      <c r="F39" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>352</v>
+      </c>
+      <c r="B40" t="s">
+        <v>353</v>
+      </c>
+      <c r="C40" t="s">
+        <v>356</v>
+      </c>
       <c r="F40" s="16"/>
     </row>
     <row r="41" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>428</v>
+      </c>
+      <c r="B41" t="s">
+        <v>429</v>
+      </c>
+      <c r="C41">
+        <v>485</v>
+      </c>
       <c r="F41" s="16"/>
     </row>
     <row r="42" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>430</v>
+      </c>
+      <c r="B42" t="s">
+        <v>431</v>
+      </c>
+      <c r="C42">
+        <v>3101</v>
+      </c>
       <c r="F42" s="16"/>
     </row>
     <row r="43" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>432</v>
+      </c>
+      <c r="B43" t="s">
+        <v>433</v>
+      </c>
+      <c r="C43">
+        <v>1784</v>
+      </c>
       <c r="F43" s="16"/>
     </row>
     <row r="44" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>434</v>
+      </c>
+      <c r="B44" t="s">
+        <v>435</v>
+      </c>
+      <c r="C44">
+        <v>17684</v>
+      </c>
       <c r="F44" s="16"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>436</v>
+      </c>
+      <c r="B45" t="s">
+        <v>437</v>
+      </c>
+      <c r="C45">
+        <v>24950</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>438</v>
+      </c>
+      <c r="B46" t="s">
+        <v>439</v>
+      </c>
+      <c r="C46">
+        <v>39981</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add indicator codes for hts_tst items
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6BFBC34-5E66-8A44-8DB7-176FF5DF95E9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04809BCB-1702-E44B-9C01-7E6D8656C8AB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4000" yWindow="720" windowWidth="25600" windowHeight="20020" activeTab="1" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="8580" yWindow="980" windowWidth="25600" windowHeight="20020" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1922" uniqueCount="444">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1357,6 +1357,18 @@
   </si>
   <si>
     <t>PrEP_NEW (N, DSD, KeyPop) TARGET FSW</t>
+  </si>
+  <si>
+    <t>HTS_TST.N.Pos</t>
+  </si>
+  <si>
+    <t>HTS_TST.N.yield</t>
+  </si>
+  <si>
+    <t>HTS_SELF.N.Age/Sex/SelfTest.19T.Directly_Assisted</t>
+  </si>
+  <si>
+    <t>HTS_SELF.N.KeyPop.19T.Directly_Assisted</t>
   </si>
 </sst>
 </file>
@@ -1379,12 +1391,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1415,6 +1421,12 @@
       <name val="Courier New"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF1A1AA6"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1440,25 +1452,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1775,10 +1787,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
   <dimension ref="A1:V54"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="K30" sqref="K30"/>
+      <selection pane="bottomLeft" activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1789,7 +1801,7 @@
     <col min="4" max="4" width="255.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
-    <col min="7" max="7" width="56.6640625" customWidth="1"/>
+    <col min="7" max="7" width="68.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="14" width="17.33203125" customWidth="1"/>
     <col min="15" max="15" width="27" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="24" bestFit="1" customWidth="1"/>
@@ -2233,7 +2245,7 @@
       <c r="I7" t="s">
         <v>240</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="5" t="s">
         <v>310</v>
       </c>
       <c r="K7" t="s">
@@ -2301,7 +2313,7 @@
       <c r="I8" t="s">
         <v>240</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="5" t="s">
         <v>310</v>
       </c>
       <c r="K8" t="s">
@@ -2331,7 +2343,7 @@
       <c r="S8" t="s">
         <v>241</v>
       </c>
-      <c r="T8" s="6" t="s">
+      <c r="T8" s="5" t="s">
         <v>310</v>
       </c>
       <c r="U8" t="s">
@@ -2369,7 +2381,7 @@
       <c r="I9" t="s">
         <v>241</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="5" t="s">
         <v>310</v>
       </c>
       <c r="K9" t="s">
@@ -2437,7 +2449,7 @@
       <c r="I10" t="s">
         <v>241</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="J10" s="5" t="s">
         <v>310</v>
       </c>
       <c r="K10" t="s">
@@ -2836,7 +2848,9 @@
       <c r="F16" t="s">
         <v>244</v>
       </c>
-      <c r="G16" s="1"/>
+      <c r="G16" t="s">
+        <v>440</v>
+      </c>
       <c r="H16" s="1" t="s">
         <v>146</v>
       </c>
@@ -2852,7 +2866,7 @@
       <c r="L16" t="s">
         <v>245</v>
       </c>
-      <c r="M16" s="16" t="s">
+      <c r="M16" s="15" t="s">
         <v>427</v>
       </c>
       <c r="N16" t="s">
@@ -2864,13 +2878,16 @@
       <c r="P16" t="s">
         <v>261</v>
       </c>
+      <c r="Q16" t="s">
+        <v>440</v>
+      </c>
       <c r="R16" s="1" t="s">
         <v>146</v>
       </c>
       <c r="S16" t="s">
         <v>241</v>
       </c>
-      <c r="T16" s="14" t="s">
+      <c r="T16" s="13" t="s">
         <v>416</v>
       </c>
       <c r="U16" t="s">
@@ -2899,6 +2916,9 @@
       <c r="F17" t="s">
         <v>244</v>
       </c>
+      <c r="G17" t="s">
+        <v>440</v>
+      </c>
       <c r="H17" s="1" t="s">
         <v>146</v>
       </c>
@@ -2914,7 +2934,7 @@
       <c r="L17" t="s">
         <v>245</v>
       </c>
-      <c r="M17" s="16" t="s">
+      <c r="M17" s="15" t="s">
         <v>427</v>
       </c>
       <c r="N17" t="s">
@@ -2926,13 +2946,16 @@
       <c r="P17" t="s">
         <v>270</v>
       </c>
+      <c r="Q17" t="s">
+        <v>440</v>
+      </c>
       <c r="R17" s="1" t="s">
         <v>146</v>
       </c>
       <c r="S17" t="s">
         <v>241</v>
       </c>
-      <c r="T17" s="14" t="s">
+      <c r="T17" s="13" t="s">
         <v>416</v>
       </c>
       <c r="U17" t="s">
@@ -2961,6 +2984,9 @@
       <c r="F18" t="s">
         <v>244</v>
       </c>
+      <c r="G18" t="s">
+        <v>440</v>
+      </c>
       <c r="H18" s="1" t="s">
         <v>146</v>
       </c>
@@ -2976,7 +3002,7 @@
       <c r="L18" t="s">
         <v>245</v>
       </c>
-      <c r="M18" s="16" t="s">
+      <c r="M18" s="15" t="s">
         <v>427</v>
       </c>
       <c r="N18" t="s">
@@ -2988,13 +3014,16 @@
       <c r="P18" t="s">
         <v>284</v>
       </c>
+      <c r="Q18" t="s">
+        <v>440</v>
+      </c>
       <c r="R18" s="1" t="s">
         <v>146</v>
       </c>
       <c r="S18" t="s">
         <v>241</v>
       </c>
-      <c r="T18" s="14" t="s">
+      <c r="T18" s="13" t="s">
         <v>416</v>
       </c>
       <c r="U18" t="s">
@@ -3023,6 +3052,9 @@
       <c r="F19" t="s">
         <v>244</v>
       </c>
+      <c r="G19" t="s">
+        <v>440</v>
+      </c>
       <c r="H19" s="1" t="s">
         <v>146</v>
       </c>
@@ -3038,7 +3070,7 @@
       <c r="L19" t="s">
         <v>245</v>
       </c>
-      <c r="M19" s="16" t="s">
+      <c r="M19" s="15" t="s">
         <v>427</v>
       </c>
       <c r="N19" t="s">
@@ -3050,13 +3082,16 @@
       <c r="P19" t="s">
         <v>274</v>
       </c>
+      <c r="Q19" t="s">
+        <v>440</v>
+      </c>
       <c r="R19" s="1" t="s">
         <v>146</v>
       </c>
       <c r="S19" t="s">
         <v>241</v>
       </c>
-      <c r="T19" s="14" t="s">
+      <c r="T19" s="13" t="s">
         <v>416</v>
       </c>
       <c r="U19" t="s">
@@ -3085,6 +3120,9 @@
       <c r="F20" t="s">
         <v>244</v>
       </c>
+      <c r="G20" t="s">
+        <v>440</v>
+      </c>
       <c r="H20" s="1" t="s">
         <v>146</v>
       </c>
@@ -3100,7 +3138,7 @@
       <c r="L20" t="s">
         <v>245</v>
       </c>
-      <c r="M20" s="16" t="s">
+      <c r="M20" s="15" t="s">
         <v>427</v>
       </c>
       <c r="N20" t="s">
@@ -3112,13 +3150,16 @@
       <c r="P20" t="s">
         <v>276</v>
       </c>
+      <c r="Q20" t="s">
+        <v>440</v>
+      </c>
       <c r="R20" s="1" t="s">
         <v>146</v>
       </c>
       <c r="S20" t="s">
         <v>241</v>
       </c>
-      <c r="T20" s="14" t="s">
+      <c r="T20" s="13" t="s">
         <v>416</v>
       </c>
       <c r="U20" t="s">
@@ -3147,13 +3188,16 @@
       <c r="F21" t="s">
         <v>244</v>
       </c>
+      <c r="G21" t="s">
+        <v>440</v>
+      </c>
       <c r="H21" s="1" t="s">
         <v>146</v>
       </c>
       <c r="I21" t="s">
         <v>241</v>
       </c>
-      <c r="J21" s="7" t="s">
+      <c r="J21" s="6" t="s">
         <v>184</v>
       </c>
       <c r="K21" t="s">
@@ -3162,7 +3206,7 @@
       <c r="L21" t="s">
         <v>245</v>
       </c>
-      <c r="M21" s="16" t="s">
+      <c r="M21" s="15" t="s">
         <v>427</v>
       </c>
       <c r="N21" t="s">
@@ -3174,13 +3218,16 @@
       <c r="P21" t="s">
         <v>278</v>
       </c>
+      <c r="Q21" t="s">
+        <v>440</v>
+      </c>
       <c r="R21" s="1" t="s">
         <v>146</v>
       </c>
       <c r="S21" t="s">
         <v>241</v>
       </c>
-      <c r="T21" s="7" t="s">
+      <c r="T21" s="6" t="s">
         <v>184</v>
       </c>
       <c r="U21" t="s">
@@ -3209,13 +3256,16 @@
       <c r="F22" t="s">
         <v>244</v>
       </c>
+      <c r="G22" t="s">
+        <v>440</v>
+      </c>
       <c r="H22" s="1" t="s">
         <v>146</v>
       </c>
       <c r="I22" t="s">
         <v>241</v>
       </c>
-      <c r="J22" s="7" t="s">
+      <c r="J22" s="6" t="s">
         <v>184</v>
       </c>
       <c r="K22" t="s">
@@ -3224,7 +3274,7 @@
       <c r="L22" t="s">
         <v>245</v>
       </c>
-      <c r="M22" s="16" t="s">
+      <c r="M22" s="15" t="s">
         <v>427</v>
       </c>
       <c r="N22" t="s">
@@ -3236,13 +3286,16 @@
       <c r="P22" t="s">
         <v>280</v>
       </c>
+      <c r="Q22" t="s">
+        <v>440</v>
+      </c>
       <c r="R22" s="1" t="s">
         <v>146</v>
       </c>
       <c r="S22" t="s">
         <v>241</v>
       </c>
-      <c r="T22" s="7" t="s">
+      <c r="T22" s="6" t="s">
         <v>184</v>
       </c>
       <c r="U22" t="s">
@@ -3271,6 +3324,9 @@
       <c r="F23" t="s">
         <v>244</v>
       </c>
+      <c r="G23" t="s">
+        <v>440</v>
+      </c>
       <c r="H23" s="1" t="s">
         <v>146</v>
       </c>
@@ -3286,7 +3342,7 @@
       <c r="L23" t="s">
         <v>245</v>
       </c>
-      <c r="M23" s="16" t="s">
+      <c r="M23" s="15" t="s">
         <v>427</v>
       </c>
       <c r="N23" t="s">
@@ -3298,13 +3354,16 @@
       <c r="P23" t="s">
         <v>282</v>
       </c>
+      <c r="Q23" t="s">
+        <v>440</v>
+      </c>
       <c r="R23" s="1" t="s">
         <v>146</v>
       </c>
       <c r="S23" t="s">
         <v>241</v>
       </c>
-      <c r="T23" s="14" t="s">
+      <c r="T23" s="13" t="s">
         <v>416</v>
       </c>
       <c r="U23" t="s">
@@ -3333,6 +3392,9 @@
       <c r="F24" t="s">
         <v>244</v>
       </c>
+      <c r="G24" t="s">
+        <v>440</v>
+      </c>
       <c r="H24" s="1" t="s">
         <v>146</v>
       </c>
@@ -3348,7 +3410,7 @@
       <c r="L24" t="s">
         <v>245</v>
       </c>
-      <c r="M24" s="16" t="s">
+      <c r="M24" s="15" t="s">
         <v>427</v>
       </c>
       <c r="N24" t="s">
@@ -3360,13 +3422,16 @@
       <c r="P24" t="s">
         <v>272</v>
       </c>
+      <c r="Q24" t="s">
+        <v>440</v>
+      </c>
       <c r="R24" s="1" t="s">
         <v>146</v>
       </c>
       <c r="S24" t="s">
         <v>241</v>
       </c>
-      <c r="T24" s="14" t="s">
+      <c r="T24" s="13" t="s">
         <v>416</v>
       </c>
       <c r="U24" t="s">
@@ -3395,6 +3460,9 @@
       <c r="F25" t="s">
         <v>244</v>
       </c>
+      <c r="G25" t="s">
+        <v>440</v>
+      </c>
       <c r="H25" s="1" t="s">
         <v>146</v>
       </c>
@@ -3410,7 +3478,7 @@
       <c r="L25" t="s">
         <v>245</v>
       </c>
-      <c r="M25" s="16" t="s">
+      <c r="M25" s="15" t="s">
         <v>427</v>
       </c>
       <c r="N25" t="s">
@@ -3422,13 +3490,16 @@
       <c r="P25" t="s">
         <v>286</v>
       </c>
+      <c r="Q25" t="s">
+        <v>440</v>
+      </c>
       <c r="R25" s="1" t="s">
         <v>146</v>
       </c>
       <c r="S25" t="s">
         <v>241</v>
       </c>
-      <c r="T25" s="14" t="s">
+      <c r="T25" s="13" t="s">
         <v>416</v>
       </c>
       <c r="U25" t="s">
@@ -3457,6 +3528,9 @@
       <c r="F26" s="1" t="s">
         <v>246</v>
       </c>
+      <c r="G26" t="s">
+        <v>441</v>
+      </c>
       <c r="H26" s="1" t="s">
         <v>147</v>
       </c>
@@ -3472,7 +3546,7 @@
       <c r="L26" t="s">
         <v>245</v>
       </c>
-      <c r="M26" s="16" t="s">
+      <c r="M26" s="15" t="s">
         <v>427</v>
       </c>
       <c r="N26" t="s">
@@ -3522,6 +3596,9 @@
       <c r="F27" s="1" t="s">
         <v>246</v>
       </c>
+      <c r="G27" t="s">
+        <v>441</v>
+      </c>
       <c r="H27" s="1" t="s">
         <v>147</v>
       </c>
@@ -3537,7 +3614,7 @@
       <c r="L27" t="s">
         <v>245</v>
       </c>
-      <c r="M27" s="16" t="s">
+      <c r="M27" s="15" t="s">
         <v>427</v>
       </c>
       <c r="N27" t="s">
@@ -3587,6 +3664,9 @@
       <c r="F28" s="1" t="s">
         <v>246</v>
       </c>
+      <c r="G28" t="s">
+        <v>441</v>
+      </c>
       <c r="H28" s="1" t="s">
         <v>147</v>
       </c>
@@ -3602,7 +3682,7 @@
       <c r="L28" t="s">
         <v>245</v>
       </c>
-      <c r="M28" s="16" t="s">
+      <c r="M28" s="15" t="s">
         <v>427</v>
       </c>
       <c r="N28" t="s">
@@ -3652,6 +3732,9 @@
       <c r="F29" s="1" t="s">
         <v>246</v>
       </c>
+      <c r="G29" t="s">
+        <v>441</v>
+      </c>
       <c r="H29" s="1" t="s">
         <v>147</v>
       </c>
@@ -3667,7 +3750,7 @@
       <c r="L29" t="s">
         <v>245</v>
       </c>
-      <c r="M29" s="16" t="s">
+      <c r="M29" s="15" t="s">
         <v>427</v>
       </c>
       <c r="N29" t="s">
@@ -3717,6 +3800,9 @@
       <c r="F30" s="1" t="s">
         <v>246</v>
       </c>
+      <c r="G30" t="s">
+        <v>441</v>
+      </c>
       <c r="H30" s="1" t="s">
         <v>147</v>
       </c>
@@ -3732,7 +3818,7 @@
       <c r="L30" t="s">
         <v>245</v>
       </c>
-      <c r="M30" s="16" t="s">
+      <c r="M30" s="15" t="s">
         <v>427</v>
       </c>
       <c r="N30" t="s">
@@ -3782,13 +3868,16 @@
       <c r="F31" s="1" t="s">
         <v>246</v>
       </c>
+      <c r="G31" t="s">
+        <v>441</v>
+      </c>
       <c r="H31" s="1" t="s">
         <v>147</v>
       </c>
       <c r="I31" t="s">
         <v>241</v>
       </c>
-      <c r="J31" s="7" t="s">
+      <c r="J31" s="6" t="s">
         <v>184</v>
       </c>
       <c r="K31" s="1" t="s">
@@ -3797,7 +3886,7 @@
       <c r="L31" t="s">
         <v>245</v>
       </c>
-      <c r="M31" s="16" t="s">
+      <c r="M31" s="15" t="s">
         <v>427</v>
       </c>
       <c r="N31" t="s">
@@ -3847,13 +3936,16 @@
       <c r="F32" s="1" t="s">
         <v>246</v>
       </c>
+      <c r="G32" t="s">
+        <v>441</v>
+      </c>
       <c r="H32" s="1" t="s">
         <v>147</v>
       </c>
       <c r="I32" t="s">
         <v>241</v>
       </c>
-      <c r="J32" s="7" t="s">
+      <c r="J32" s="6" t="s">
         <v>184</v>
       </c>
       <c r="K32" s="1" t="s">
@@ -3862,7 +3954,7 @@
       <c r="L32" t="s">
         <v>245</v>
       </c>
-      <c r="M32" s="16" t="s">
+      <c r="M32" s="15" t="s">
         <v>427</v>
       </c>
       <c r="N32" t="s">
@@ -3912,6 +4004,9 @@
       <c r="F33" s="1" t="s">
         <v>246</v>
       </c>
+      <c r="G33" t="s">
+        <v>441</v>
+      </c>
       <c r="H33" s="1" t="s">
         <v>147</v>
       </c>
@@ -3927,7 +4022,7 @@
       <c r="L33" t="s">
         <v>245</v>
       </c>
-      <c r="M33" s="16" t="s">
+      <c r="M33" s="15" t="s">
         <v>427</v>
       </c>
       <c r="N33" t="s">
@@ -3977,6 +4072,9 @@
       <c r="F34" s="1" t="s">
         <v>246</v>
       </c>
+      <c r="G34" t="s">
+        <v>441</v>
+      </c>
       <c r="H34" s="1" t="s">
         <v>147</v>
       </c>
@@ -3992,7 +4090,7 @@
       <c r="L34" t="s">
         <v>245</v>
       </c>
-      <c r="M34" s="16" t="s">
+      <c r="M34" s="15" t="s">
         <v>427</v>
       </c>
       <c r="N34" t="s">
@@ -4042,6 +4140,9 @@
       <c r="F35" s="1" t="s">
         <v>246</v>
       </c>
+      <c r="G35" t="s">
+        <v>441</v>
+      </c>
       <c r="H35" s="1" t="s">
         <v>147</v>
       </c>
@@ -4057,7 +4158,7 @@
       <c r="L35" t="s">
         <v>245</v>
       </c>
-      <c r="M35" s="16" t="s">
+      <c r="M35" s="15" t="s">
         <v>427</v>
       </c>
       <c r="N35" t="s">
@@ -4088,7 +4189,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="36" spans="1:22" ht="18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -4106,6 +4207,9 @@
       </c>
       <c r="F36" s="1" t="s">
         <v>244</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>442</v>
       </c>
       <c r="H36" t="s">
         <v>148</v>
@@ -4277,7 +4381,7 @@
       <c r="S38" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="T38" s="14" t="s">
+      <c r="T38" s="13" t="s">
         <v>328</v>
       </c>
       <c r="U38" t="s">
@@ -4628,7 +4732,7 @@
       </c>
     </row>
     <row r="44" spans="1:22" ht="18" x14ac:dyDescent="0.2">
-      <c r="A44" s="17" t="s">
+      <c r="A44" s="16" t="s">
         <v>92</v>
       </c>
       <c r="B44" t="s">
@@ -4696,7 +4800,7 @@
       </c>
     </row>
     <row r="45" spans="1:22" ht="18" x14ac:dyDescent="0.2">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="16" t="s">
         <v>92</v>
       </c>
       <c r="B45" t="s">
@@ -4763,7 +4867,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="46" spans="1:22" ht="18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>92</v>
       </c>
@@ -4782,7 +4886,9 @@
       <c r="F46" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="G46" s="3"/>
+      <c r="G46" s="17" t="s">
+        <v>443</v>
+      </c>
       <c r="H46" t="s">
         <v>158</v>
       </c>
@@ -5088,7 +5194,7 @@
       <c r="S50" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="T50" s="14" t="s">
+      <c r="T50" s="13" t="s">
         <v>328</v>
       </c>
       <c r="U50" t="s">
@@ -5380,7 +5486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D15FCD2F-A9CC-CD4F-8AF1-79C36D527EBB}">
   <dimension ref="A1:AF46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="A41" sqref="A41:B46"/>
     </sheetView>
   </sheetViews>
@@ -6022,10 +6128,10 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="F37" s="16"/>
+      <c r="F37" s="15"/>
     </row>
     <row r="38" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="F38" s="16"/>
+      <c r="F38" s="15"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
@@ -6057,7 +6163,7 @@
       <c r="C40" t="s">
         <v>356</v>
       </c>
-      <c r="F40" s="16"/>
+      <c r="F40" s="15"/>
     </row>
     <row r="41" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -6069,7 +6175,7 @@
       <c r="C41">
         <v>485</v>
       </c>
-      <c r="F41" s="16"/>
+      <c r="F41" s="15"/>
     </row>
     <row r="42" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -6081,7 +6187,7 @@
       <c r="C42">
         <v>3101</v>
       </c>
-      <c r="F42" s="16"/>
+      <c r="F42" s="15"/>
     </row>
     <row r="43" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -6093,7 +6199,7 @@
       <c r="C43">
         <v>1784</v>
       </c>
-      <c r="F43" s="16"/>
+      <c r="F43" s="15"/>
     </row>
     <row r="44" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -6105,7 +6211,7 @@
       <c r="C44">
         <v>17684</v>
       </c>
-      <c r="F44" s="16"/>
+      <c r="F44" s="15"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
@@ -6138,8 +6244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
   <dimension ref="A1:X59"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6188,34 +6294,34 @@
       <c r="J1" t="s">
         <v>304</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="13" t="s">
         <v>291</v>
       </c>
       <c r="O1" t="s">
         <v>422</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="13" t="s">
         <v>310</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="Q1" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="R1" s="13" t="s">
         <v>416</v>
       </c>
       <c r="S1" t="s">
         <v>425</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="T1" s="13" t="s">
         <v>328</v>
       </c>
       <c r="U1" t="s">
@@ -6238,37 +6344,37 @@
       <c r="B2" t="s">
         <v>426</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="10">
         <v>10</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="8">
         <v>1</v>
       </c>
-      <c r="J2" s="8" t="str">
+      <c r="J2" s="7" t="str">
         <f t="shared" ref="J2:J27" si="0">_xlfn.TEXTJOIN(";",1,K2,L2,M2,N2,O2,P2,Q2,S2,T2,U2,V2,W2,R2,X2)</f>
         <v>&lt;1-50+;&lt;1-18+</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
       <c r="O2" t="s">
         <v>422</v>
       </c>
@@ -6280,33 +6386,33 @@
       <c r="B3" t="s">
         <v>426</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="10">
         <v>10</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="8">
         <v>0.25</v>
       </c>
-      <c r="J3" s="8" t="str">
+      <c r="J3" s="7" t="str">
         <f t="shared" si="0"/>
         <v>&lt;15/&gt;15.d</v>
       </c>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14" t="s">
+      <c r="O3" s="13"/>
+      <c r="P3" s="13" t="s">
         <v>310</v>
       </c>
     </row>
@@ -6320,25 +6426,25 @@
       <c r="C4" t="s">
         <v>289</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="9">
         <v>10</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="7">
         <v>0.2</v>
       </c>
-      <c r="J4" s="8" t="str">
+      <c r="J4" s="7" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -6350,46 +6456,46 @@
       <c r="B5" t="s">
         <v>426</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="10">
         <v>20</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="8">
         <v>0.5</v>
       </c>
-      <c r="J5" s="8" t="str">
+      <c r="J5" s="7" t="str">
         <f t="shared" si="0"/>
         <v>&lt;1-50+;1-50+;&lt;1-18+;1-4;1-50+/&lt;5</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="L5" s="14" t="s">
+      <c r="L5" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
       <c r="O5" t="s">
         <v>422</v>
       </c>
-      <c r="Q5" s="14" t="s">
+      <c r="Q5" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="R5" s="14" t="s">
+      <c r="R5" s="13" t="s">
         <v>416</v>
       </c>
     </row>
@@ -6400,32 +6506,32 @@
       <c r="B6" t="s">
         <v>426</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="10">
         <v>20</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="8">
         <v>0.25</v>
       </c>
-      <c r="J6" s="8" t="str">
+      <c r="J6" s="7" t="str">
         <f t="shared" si="0"/>
         <v>&lt;15/&gt;15.d</v>
       </c>
-      <c r="P6" s="14" t="s">
+      <c r="P6" s="13" t="s">
         <v>310</v>
       </c>
     </row>
@@ -6439,32 +6545,32 @@
       <c r="C7" t="s">
         <v>289</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="9">
         <v>20</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="7">
         <v>1</v>
       </c>
-      <c r="J7" s="8" t="str">
+      <c r="J7" s="7" t="str">
         <f t="shared" si="0"/>
         <v>1-4;1-50+/&lt;5</v>
       </c>
-      <c r="Q7" s="14" t="s">
+      <c r="Q7" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="R7" s="14" t="s">
+      <c r="R7" s="13" t="s">
         <v>416</v>
       </c>
     </row>
@@ -6475,43 +6581,43 @@
       <c r="B8" t="s">
         <v>426</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="10">
         <v>30</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="8">
         <v>0.5</v>
       </c>
-      <c r="J8" s="8" t="str">
+      <c r="J8" s="7" t="str">
         <f t="shared" si="0"/>
         <v>&lt;1-50+;1-50+;&lt;1-18+;1-50+/&lt;5</v>
       </c>
-      <c r="K8" s="14" t="s">
+      <c r="K8" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="L8" s="14" t="s">
+      <c r="L8" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
       <c r="O8" t="s">
         <v>422</v>
       </c>
-      <c r="R8" s="14" t="s">
+      <c r="R8" s="13" t="s">
         <v>416</v>
       </c>
     </row>
@@ -6522,32 +6628,32 @@
       <c r="B9" t="s">
         <v>426</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="10">
         <v>30</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="8">
         <v>0.25</v>
       </c>
-      <c r="J9" s="8" t="str">
+      <c r="J9" s="7" t="str">
         <f t="shared" si="0"/>
         <v>&lt;15/&gt;15.d</v>
       </c>
-      <c r="P9" s="14" t="s">
+      <c r="P9" s="13" t="s">
         <v>310</v>
       </c>
     </row>
@@ -6558,48 +6664,48 @@
       <c r="B10" t="s">
         <v>426</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="10">
         <v>40</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="8">
         <v>1</v>
       </c>
-      <c r="J10" s="8" t="str">
+      <c r="J10" s="7" t="str">
         <f t="shared" si="0"/>
         <v>&lt;1-50+;1-50+;10-50+;&lt;1-18+;10-50+.all;1-50+/&lt;5</v>
       </c>
-      <c r="K10" s="14" t="s">
+      <c r="K10" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="L10" s="14" t="s">
+      <c r="L10" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="M10" s="14" t="s">
+      <c r="M10" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="N10" s="14"/>
+      <c r="N10" s="13"/>
       <c r="O10" t="s">
         <v>422</v>
       </c>
-      <c r="R10" s="14" t="s">
+      <c r="R10" s="13" t="s">
         <v>416</v>
       </c>
-      <c r="T10" s="14" t="s">
+      <c r="T10" s="13" t="s">
         <v>328</v>
       </c>
     </row>
@@ -6610,32 +6716,32 @@
       <c r="B11" t="s">
         <v>426</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="10">
         <v>40</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="8">
         <v>0.25</v>
       </c>
-      <c r="J11" s="8" t="str">
+      <c r="J11" s="7" t="str">
         <f t="shared" si="0"/>
         <v>&lt;15/&gt;15.d</v>
       </c>
-      <c r="P11" s="14" t="s">
+      <c r="P11" s="13" t="s">
         <v>310</v>
       </c>
     </row>
@@ -6646,38 +6752,38 @@
       <c r="B12" t="s">
         <v>245</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="C12" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="F12" s="4" t="s">
+      <c r="E12" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="10">
         <v>40</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="7">
         <f>1/9</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="J12" s="8" t="str">
+      <c r="J12" s="7" t="str">
         <f t="shared" si="0"/>
         <v>missing_age_1</v>
       </c>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
       <c r="S12" t="s">
         <v>306</v>
       </c>
@@ -6689,32 +6795,32 @@
       <c r="B13" t="s">
         <v>426</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="10">
         <v>45</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="7">
         <v>1</v>
       </c>
-      <c r="J13" s="8" t="str">
+      <c r="J13" s="7" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P13" s="14"/>
+      <c r="P13" s="13"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
@@ -6725,28 +6831,28 @@
       <c r="B14" t="s">
         <v>245</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="C14" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>245</v>
       </c>
       <c r="F14" t="s">
         <v>203</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="10">
         <v>45</v>
       </c>
       <c r="I14">
         <v>0.5</v>
       </c>
-      <c r="J14" s="8" t="str">
+      <c r="J14" s="7" t="str">
         <f t="shared" si="0"/>
         <v>missing_age_2</v>
       </c>
@@ -6761,28 +6867,28 @@
       <c r="B15" t="s">
         <v>426</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="G15" s="13" t="s">
+      <c r="G15" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="10">
         <v>50</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="8">
         <v>1</v>
       </c>
-      <c r="J15" s="8" t="str">
+      <c r="J15" s="7" t="str">
         <f t="shared" si="0"/>
         <v>&lt;1-18+</v>
       </c>
@@ -6797,32 +6903,32 @@
       <c r="B16" t="s">
         <v>426</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="10">
         <v>60</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="7">
         <v>0.125</v>
       </c>
-      <c r="J16" s="8" t="str">
+      <c r="J16" s="7" t="str">
         <f t="shared" si="0"/>
         <v>&lt;15/&gt;15.d</v>
       </c>
-      <c r="P16" s="14" t="s">
+      <c r="P16" s="13" t="s">
         <v>310</v>
       </c>
     </row>
@@ -6833,47 +6939,47 @@
       <c r="B17" t="s">
         <v>426</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="H17" s="11">
+      <c r="H17" s="10">
         <v>60</v>
       </c>
-      <c r="I17" s="9">
+      <c r="I17" s="8">
         <v>1</v>
       </c>
-      <c r="J17" s="8" t="str">
+      <c r="J17" s="7" t="str">
         <f t="shared" si="0"/>
         <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
       </c>
-      <c r="K17" s="14" t="s">
+      <c r="K17" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="L17" s="14" t="s">
+      <c r="L17" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="M17" s="14" t="s">
+      <c r="M17" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="N17" s="14" t="s">
+      <c r="N17" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="R17" s="14" t="s">
+      <c r="R17" s="13" t="s">
         <v>416</v>
       </c>
-      <c r="T17" s="14" t="s">
+      <c r="T17" s="13" t="s">
         <v>328</v>
       </c>
     </row>
@@ -6884,38 +6990,38 @@
       <c r="B18" t="s">
         <v>245</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="C18" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="F18" s="4" t="s">
+      <c r="E18" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="10">
         <v>60</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I18" s="7">
         <f>1/9</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="J18" s="8" t="str">
+      <c r="J18" s="7" t="str">
         <f t="shared" si="0"/>
         <v>missing_age_1</v>
       </c>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
       <c r="S18" t="s">
         <v>306</v>
       </c>
@@ -6927,32 +7033,32 @@
       <c r="B19" t="s">
         <v>426</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H19" s="11">
         <v>65</v>
       </c>
-      <c r="I19" s="8">
+      <c r="I19" s="7">
         <v>1</v>
       </c>
-      <c r="J19" s="8" t="str">
+      <c r="J19" s="7" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P19" s="15"/>
+      <c r="P19" s="14"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
@@ -6961,37 +7067,37 @@
       <c r="B20" t="s">
         <v>245</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="D20" s="4" t="s">
+      <c r="C20" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="3" t="s">
         <v>245</v>
       </c>
       <c r="F20" t="s">
         <v>205</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="H20" s="11">
+      <c r="H20" s="10">
         <v>65</v>
       </c>
       <c r="I20">
         <v>0.5</v>
       </c>
-      <c r="J20" s="8" t="str">
+      <c r="J20" s="7" t="str">
         <f t="shared" si="0"/>
         <v>missing_age_2</v>
       </c>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
       <c r="S20" t="s">
         <v>307</v>
       </c>
@@ -7003,39 +7109,39 @@
       <c r="B21" t="s">
         <v>426</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="3" t="s">
         <v>423</v>
       </c>
-      <c r="G21" s="13" t="s">
+      <c r="G21" s="12" t="s">
         <v>424</v>
       </c>
-      <c r="H21" s="11">
+      <c r="H21" s="10">
         <v>70</v>
       </c>
-      <c r="I21" s="9">
+      <c r="I21" s="8">
         <v>1</v>
       </c>
-      <c r="J21" s="8" t="str">
+      <c r="J21" s="7" t="str">
         <f t="shared" si="0"/>
         <v>&lt;1-18+</v>
       </c>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
       <c r="O21" t="s">
         <v>422</v>
       </c>
-      <c r="P21" s="9"/>
+      <c r="P21" s="8"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -7044,32 +7150,32 @@
       <c r="B22" t="s">
         <v>426</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="G22" s="13" t="s">
+      <c r="G22" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="H22" s="11">
+      <c r="H22" s="10">
         <v>80</v>
       </c>
-      <c r="I22" s="9">
+      <c r="I22" s="8">
         <v>0.125</v>
       </c>
-      <c r="J22" s="8" t="str">
+      <c r="J22" s="7" t="str">
         <f t="shared" si="0"/>
         <v>&lt;15/&gt;15.d</v>
       </c>
-      <c r="P22" s="14" t="s">
+      <c r="P22" s="13" t="s">
         <v>310</v>
       </c>
     </row>
@@ -7080,47 +7186,47 @@
       <c r="B23" t="s">
         <v>426</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="G23" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="H23" s="11">
+      <c r="H23" s="10">
         <v>80</v>
       </c>
-      <c r="I23" s="9">
+      <c r="I23" s="8">
         <v>1</v>
       </c>
-      <c r="J23" s="8" t="str">
+      <c r="J23" s="7" t="str">
         <f t="shared" si="0"/>
         <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
       </c>
-      <c r="K23" s="14" t="s">
+      <c r="K23" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="L23" s="14" t="s">
+      <c r="L23" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="M23" s="14" t="s">
+      <c r="M23" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="N23" s="14" t="s">
+      <c r="N23" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="R23" s="14" t="s">
+      <c r="R23" s="13" t="s">
         <v>416</v>
       </c>
-      <c r="T23" s="14" t="s">
+      <c r="T23" s="13" t="s">
         <v>328</v>
       </c>
     </row>
@@ -7131,38 +7237,38 @@
       <c r="B24" t="s">
         <v>245</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="D24" s="4" t="s">
+      <c r="C24" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="F24" s="4" t="s">
+      <c r="E24" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G24" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="H24" s="11">
+      <c r="H24" s="10">
         <v>80</v>
       </c>
-      <c r="I24" s="8">
+      <c r="I24" s="7">
         <f>1/9</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="J24" s="8" t="str">
+      <c r="J24" s="7" t="str">
         <f t="shared" si="0"/>
         <v>missing_age_1</v>
       </c>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
       <c r="S24" t="s">
         <v>306</v>
       </c>
@@ -7174,32 +7280,32 @@
       <c r="B25" t="s">
         <v>426</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="G25" s="13" t="s">
+      <c r="G25" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="H25" s="11">
+      <c r="H25" s="10">
         <v>90</v>
       </c>
-      <c r="I25" s="9">
+      <c r="I25" s="8">
         <v>0.125</v>
       </c>
-      <c r="J25" s="8" t="str">
+      <c r="J25" s="7" t="str">
         <f t="shared" si="0"/>
         <v>&lt;15/&gt;15.d</v>
       </c>
-      <c r="P25" s="14" t="s">
+      <c r="P25" s="13" t="s">
         <v>310</v>
       </c>
     </row>
@@ -7210,49 +7316,49 @@
       <c r="B26" t="s">
         <v>426</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="G26" s="13" t="s">
+      <c r="G26" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="H26" s="11">
+      <c r="H26" s="10">
         <v>90</v>
       </c>
-      <c r="I26" s="9">
+      <c r="I26" s="8">
         <v>1</v>
       </c>
-      <c r="J26" s="8" t="str">
+      <c r="J26" s="7" t="str">
         <f t="shared" si="0"/>
         <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
       </c>
-      <c r="K26" s="14" t="s">
+      <c r="K26" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="L26" s="14" t="s">
+      <c r="L26" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="M26" s="14" t="s">
+      <c r="M26" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="N26" s="14" t="s">
+      <c r="N26" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
-      <c r="R26" s="14" t="s">
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="R26" s="13" t="s">
         <v>416</v>
       </c>
-      <c r="T26" s="14" t="s">
+      <c r="T26" s="13" t="s">
         <v>328</v>
       </c>
     </row>
@@ -7263,28 +7369,28 @@
       <c r="B27" t="s">
         <v>426</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="G27" s="13" t="s">
+      <c r="G27" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="H27" s="11">
+      <c r="H27" s="10">
         <v>90</v>
       </c>
-      <c r="I27" s="9">
+      <c r="I27" s="8">
         <v>0.2</v>
       </c>
-      <c r="J27" s="8" t="str">
+      <c r="J27" s="7" t="str">
         <f t="shared" si="0"/>
         <v>10-50+.all</v>
       </c>
@@ -7299,38 +7405,38 @@
       <c r="B28" t="s">
         <v>245</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="D28" s="4" t="s">
+      <c r="C28" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E28" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="F28" s="4" t="s">
+      <c r="E28" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="G28" s="13" t="s">
+      <c r="G28" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="H28" s="11">
+      <c r="H28" s="10">
         <v>90</v>
       </c>
-      <c r="I28" s="8">
+      <c r="I28" s="7">
         <f>1/9</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="J28" s="8" t="str">
+      <c r="J28" s="7" t="str">
         <f t="shared" ref="J28:J58" si="1">_xlfn.TEXTJOIN(";",1,K28,L28,M28,N28,O28,P28,Q28,S28,T28,U28,V28,W28,R28,X28)</f>
         <v>missing_age_1</v>
       </c>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
       <c r="S28" t="s">
         <v>306</v>
       </c>
@@ -7342,28 +7448,28 @@
       <c r="B29" t="s">
         <v>426</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F29" s="3" t="s">
         <v>423</v>
       </c>
-      <c r="G29" s="13" t="s">
+      <c r="G29" s="12" t="s">
         <v>424</v>
       </c>
-      <c r="H29" s="11">
+      <c r="H29" s="10">
         <v>100</v>
       </c>
-      <c r="I29" s="9">
+      <c r="I29" s="8">
         <v>1</v>
       </c>
-      <c r="J29" s="8" t="str">
+      <c r="J29" s="7" t="str">
         <f t="shared" si="1"/>
         <v>&lt;1-18+</v>
       </c>
@@ -7378,32 +7484,32 @@
       <c r="B30" t="s">
         <v>426</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="G30" s="13" t="s">
+      <c r="G30" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="H30" s="11">
+      <c r="H30" s="10">
         <v>110</v>
       </c>
-      <c r="I30" s="9">
+      <c r="I30" s="8">
         <v>0.125</v>
       </c>
-      <c r="J30" s="8" t="str">
+      <c r="J30" s="7" t="str">
         <f t="shared" si="1"/>
         <v>&lt;15/&gt;15.d</v>
       </c>
-      <c r="P30" s="14" t="s">
+      <c r="P30" s="13" t="s">
         <v>310</v>
       </c>
     </row>
@@ -7414,28 +7520,28 @@
       <c r="B31" t="s">
         <v>426</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="F31" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="G31" s="13" t="s">
+      <c r="G31" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="H31" s="11">
+      <c r="H31" s="10">
         <v>110</v>
       </c>
-      <c r="I31" s="9">
+      <c r="I31" s="8">
         <v>0.2</v>
       </c>
-      <c r="J31" s="8" t="str">
+      <c r="J31" s="7" t="str">
         <f t="shared" si="1"/>
         <v>10-50+.all</v>
       </c>
@@ -7450,49 +7556,49 @@
       <c r="B32" t="s">
         <v>426</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F32" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="G32" s="13" t="s">
+      <c r="G32" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="H32" s="11">
+      <c r="H32" s="10">
         <v>110</v>
       </c>
-      <c r="I32" s="9">
+      <c r="I32" s="8">
         <v>1</v>
       </c>
-      <c r="J32" s="8" t="str">
+      <c r="J32" s="7" t="str">
         <f t="shared" si="1"/>
         <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
       </c>
-      <c r="K32" s="14" t="s">
+      <c r="K32" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="L32" s="14" t="s">
+      <c r="L32" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="M32" s="14" t="s">
+      <c r="M32" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="N32" s="14" t="s">
+      <c r="N32" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="O32" s="9"/>
-      <c r="P32" s="9"/>
-      <c r="R32" s="14" t="s">
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+      <c r="R32" s="13" t="s">
         <v>416</v>
       </c>
-      <c r="T32" s="14" t="s">
+      <c r="T32" s="13" t="s">
         <v>328</v>
       </c>
     </row>
@@ -7503,38 +7609,38 @@
       <c r="B33" t="s">
         <v>245</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="D33" s="4" t="s">
+      <c r="C33" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E33" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="F33" s="4" t="s">
+      <c r="E33" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="G33" s="13" t="s">
+      <c r="G33" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="H33" s="11">
+      <c r="H33" s="10">
         <v>110</v>
       </c>
-      <c r="I33" s="8">
+      <c r="I33" s="7">
         <f>1/9</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="J33" s="8" t="str">
+      <c r="J33" s="7" t="str">
         <f t="shared" si="1"/>
         <v>missing_age_1</v>
       </c>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
       <c r="S33" t="s">
         <v>306</v>
       </c>
@@ -7546,32 +7652,32 @@
       <c r="B34" t="s">
         <v>426</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="F34" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="G34" s="4" t="s">
+      <c r="G34" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="H34" s="11">
+      <c r="H34" s="10">
         <v>120</v>
       </c>
-      <c r="I34" s="9">
+      <c r="I34" s="8">
         <v>0.125</v>
       </c>
-      <c r="J34" s="8" t="str">
+      <c r="J34" s="7" t="str">
         <f t="shared" si="1"/>
         <v>&lt;15/&gt;15.d</v>
       </c>
-      <c r="P34" s="14" t="s">
+      <c r="P34" s="13" t="s">
         <v>310</v>
       </c>
     </row>
@@ -7582,28 +7688,28 @@
       <c r="B35" t="s">
         <v>426</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="F35" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="G35" s="4" t="s">
+      <c r="G35" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="H35" s="11">
+      <c r="H35" s="10">
         <v>120</v>
       </c>
-      <c r="I35" s="9">
+      <c r="I35" s="8">
         <v>0.2</v>
       </c>
-      <c r="J35" s="8" t="str">
+      <c r="J35" s="7" t="str">
         <f t="shared" si="1"/>
         <v>10-50+.all</v>
       </c>
@@ -7618,47 +7724,47 @@
       <c r="B36" t="s">
         <v>426</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="F36" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="G36" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="H36" s="11">
+      <c r="H36" s="10">
         <v>120</v>
       </c>
-      <c r="I36" s="9">
+      <c r="I36" s="8">
         <v>1</v>
       </c>
-      <c r="J36" s="8" t="str">
+      <c r="J36" s="7" t="str">
         <f t="shared" si="1"/>
         <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
       </c>
-      <c r="K36" s="14" t="s">
+      <c r="K36" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="L36" s="14" t="s">
+      <c r="L36" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="M36" s="14" t="s">
+      <c r="M36" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="N36" s="14" t="s">
+      <c r="N36" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="R36" s="14" t="s">
+      <c r="R36" s="13" t="s">
         <v>416</v>
       </c>
-      <c r="T36" s="14" t="s">
+      <c r="T36" s="13" t="s">
         <v>328</v>
       </c>
     </row>
@@ -7669,38 +7775,38 @@
       <c r="B37" t="s">
         <v>245</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="D37" s="4" t="s">
+      <c r="C37" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E37" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="F37" s="4" t="s">
+      <c r="E37" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="G37" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="H37" s="11">
+      <c r="H37" s="10">
         <v>120</v>
       </c>
-      <c r="I37" s="8">
+      <c r="I37" s="7">
         <f>1/9</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="J37" s="8" t="str">
+      <c r="J37" s="7" t="str">
         <f t="shared" si="1"/>
         <v>missing_age_1</v>
       </c>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="7"/>
       <c r="S37" t="s">
         <v>306</v>
       </c>
@@ -7712,32 +7818,32 @@
       <c r="B38" t="s">
         <v>426</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="F38" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="G38" s="4" t="s">
+      <c r="G38" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="H38" s="11">
+      <c r="H38" s="10">
         <v>130</v>
       </c>
-      <c r="I38" s="9">
+      <c r="I38" s="8">
         <v>0.125</v>
       </c>
-      <c r="J38" s="8" t="str">
+      <c r="J38" s="7" t="str">
         <f t="shared" si="1"/>
         <v>&lt;15/&gt;15.d</v>
       </c>
-      <c r="P38" s="14" t="s">
+      <c r="P38" s="13" t="s">
         <v>310</v>
       </c>
     </row>
@@ -7748,28 +7854,28 @@
       <c r="B39" t="s">
         <v>426</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E39" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="F39" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="G39" s="4" t="s">
+      <c r="G39" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="H39" s="11">
+      <c r="H39" s="10">
         <v>130</v>
       </c>
-      <c r="I39" s="9">
+      <c r="I39" s="8">
         <v>0.2</v>
       </c>
-      <c r="J39" s="8" t="str">
+      <c r="J39" s="7" t="str">
         <f t="shared" si="1"/>
         <v>10-50+.all</v>
       </c>
@@ -7784,47 +7890,47 @@
       <c r="B40" t="s">
         <v>426</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E40" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="F40" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="G40" s="4" t="s">
+      <c r="G40" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="H40" s="11">
+      <c r="H40" s="10">
         <v>130</v>
       </c>
-      <c r="I40" s="9">
+      <c r="I40" s="8">
         <v>0.5</v>
       </c>
-      <c r="J40" s="8" t="str">
+      <c r="J40" s="7" t="str">
         <f t="shared" si="1"/>
         <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
       </c>
-      <c r="K40" s="14" t="s">
+      <c r="K40" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="L40" s="14" t="s">
+      <c r="L40" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="M40" s="14" t="s">
+      <c r="M40" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="N40" s="14" t="s">
+      <c r="N40" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="R40" s="14" t="s">
+      <c r="R40" s="13" t="s">
         <v>416</v>
       </c>
-      <c r="T40" s="14" t="s">
+      <c r="T40" s="13" t="s">
         <v>328</v>
       </c>
     </row>
@@ -7835,38 +7941,38 @@
       <c r="B41" t="s">
         <v>245</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="D41" s="4" t="s">
+      <c r="C41" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E41" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="F41" s="4" t="s">
+      <c r="E41" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F41" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="G41" s="4" t="s">
+      <c r="G41" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="H41" s="11">
+      <c r="H41" s="10">
         <v>130</v>
       </c>
-      <c r="I41" s="8">
+      <c r="I41" s="7">
         <f>1/9</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="J41" s="8" t="str">
+      <c r="J41" s="7" t="str">
         <f t="shared" si="1"/>
         <v>missing_age_1</v>
       </c>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
-      <c r="M41" s="8"/>
-      <c r="N41" s="8"/>
-      <c r="O41" s="8"/>
-      <c r="P41" s="8"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="7"/>
       <c r="S41" t="s">
         <v>306</v>
       </c>
@@ -7878,32 +7984,32 @@
       <c r="B42" t="s">
         <v>426</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="F42" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="G42" s="4" t="s">
+      <c r="G42" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="H42" s="11">
+      <c r="H42" s="10">
         <v>140</v>
       </c>
-      <c r="I42" s="9">
+      <c r="I42" s="8">
         <v>0.125</v>
       </c>
-      <c r="J42" s="8" t="str">
+      <c r="J42" s="7" t="str">
         <f t="shared" si="1"/>
         <v>&lt;15/&gt;15.d</v>
       </c>
-      <c r="P42" s="14" t="s">
+      <c r="P42" s="13" t="s">
         <v>310</v>
       </c>
     </row>
@@ -7914,28 +8020,28 @@
       <c r="B43" t="s">
         <v>426</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E43" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="F43" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="G43" s="4" t="s">
+      <c r="G43" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="H43" s="11">
+      <c r="H43" s="10">
         <v>140</v>
       </c>
-      <c r="I43" s="9">
+      <c r="I43" s="8">
         <v>0.2</v>
       </c>
-      <c r="J43" s="8" t="str">
+      <c r="J43" s="7" t="str">
         <f t="shared" si="1"/>
         <v>10-50+.all</v>
       </c>
@@ -7950,47 +8056,47 @@
       <c r="B44" t="s">
         <v>426</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E44" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="F44" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="G44" s="4" t="s">
+      <c r="G44" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="H44" s="11">
+      <c r="H44" s="10">
         <v>140</v>
       </c>
-      <c r="I44" s="9">
+      <c r="I44" s="8">
         <v>0.5</v>
       </c>
-      <c r="J44" s="8" t="str">
+      <c r="J44" s="7" t="str">
         <f t="shared" si="1"/>
         <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
       </c>
-      <c r="K44" s="14" t="s">
+      <c r="K44" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="L44" s="14" t="s">
+      <c r="L44" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="M44" s="14" t="s">
+      <c r="M44" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="N44" s="14" t="s">
+      <c r="N44" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="R44" s="14" t="s">
+      <c r="R44" s="13" t="s">
         <v>416</v>
       </c>
-      <c r="T44" s="14" t="s">
+      <c r="T44" s="13" t="s">
         <v>328</v>
       </c>
     </row>
@@ -8001,38 +8107,38 @@
       <c r="B45" t="s">
         <v>245</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="D45" s="4" t="s">
+      <c r="C45" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E45" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="F45" s="4" t="s">
+      <c r="E45" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="G45" s="4" t="s">
+      <c r="G45" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="H45" s="11">
+      <c r="H45" s="10">
         <v>140</v>
       </c>
-      <c r="I45" s="8">
+      <c r="I45" s="7">
         <f>1/9</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="J45" s="8" t="str">
+      <c r="J45" s="7" t="str">
         <f t="shared" si="1"/>
         <v>missing_age_1</v>
       </c>
-      <c r="K45" s="8"/>
-      <c r="L45" s="8"/>
-      <c r="M45" s="8"/>
-      <c r="N45" s="8"/>
-      <c r="O45" s="8"/>
-      <c r="P45" s="8"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="7"/>
+      <c r="P45" s="7"/>
       <c r="S45" t="s">
         <v>306</v>
       </c>
@@ -8044,32 +8150,32 @@
       <c r="B46" t="s">
         <v>426</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D46" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E46" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="F46" s="5" t="s">
+      <c r="F46" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="G46" s="4" t="s">
+      <c r="G46" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="H46" s="11">
+      <c r="H46" s="10">
         <v>150</v>
       </c>
-      <c r="I46" s="9">
+      <c r="I46" s="8">
         <v>0.125</v>
       </c>
-      <c r="J46" s="8" t="str">
+      <c r="J46" s="7" t="str">
         <f t="shared" si="1"/>
         <v>&lt;15/&gt;15.d</v>
       </c>
-      <c r="P46" s="14" t="s">
+      <c r="P46" s="13" t="s">
         <v>310</v>
       </c>
     </row>
@@ -8080,47 +8186,47 @@
       <c r="B47" t="s">
         <v>426</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E47" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="F47" s="5" t="s">
+      <c r="F47" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="G47" s="4" t="s">
+      <c r="G47" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="H47" s="11">
+      <c r="H47" s="10">
         <v>150</v>
       </c>
-      <c r="I47" s="9">
+      <c r="I47" s="8">
         <v>1</v>
       </c>
-      <c r="J47" s="8" t="str">
+      <c r="J47" s="7" t="str">
         <f t="shared" si="1"/>
         <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
       </c>
-      <c r="K47" s="14" t="s">
+      <c r="K47" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="L47" s="14" t="s">
+      <c r="L47" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="M47" s="14" t="s">
+      <c r="M47" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="N47" s="14" t="s">
+      <c r="N47" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="R47" s="14" t="s">
+      <c r="R47" s="13" t="s">
         <v>416</v>
       </c>
-      <c r="T47" s="14" t="s">
+      <c r="T47" s="13" t="s">
         <v>328</v>
       </c>
     </row>
@@ -8131,38 +8237,38 @@
       <c r="B48" t="s">
         <v>245</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="D48" s="4" t="s">
+      <c r="C48" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E48" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="F48" s="5" t="s">
+      <c r="E48" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F48" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="G48" s="4" t="s">
+      <c r="G48" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="H48" s="11">
+      <c r="H48" s="10">
         <v>150</v>
       </c>
-      <c r="I48" s="8">
+      <c r="I48" s="7">
         <f>1/9</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="J48" s="8" t="str">
+      <c r="J48" s="7" t="str">
         <f t="shared" si="1"/>
         <v>missing_age_1</v>
       </c>
-      <c r="K48" s="8"/>
-      <c r="L48" s="8"/>
-      <c r="M48" s="8"/>
-      <c r="N48" s="8"/>
-      <c r="O48" s="8"/>
-      <c r="P48" s="8"/>
+      <c r="K48" s="7"/>
+      <c r="L48" s="7"/>
+      <c r="M48" s="7"/>
+      <c r="N48" s="7"/>
+      <c r="O48" s="7"/>
+      <c r="P48" s="7"/>
       <c r="S48" t="s">
         <v>306</v>
       </c>
@@ -8183,19 +8289,19 @@
       <c r="E49" t="s">
         <v>225</v>
       </c>
-      <c r="F49" s="4" t="s">
+      <c r="F49" s="3" t="s">
         <v>230</v>
       </c>
       <c r="G49" t="s">
         <v>232</v>
       </c>
-      <c r="H49" s="11">
+      <c r="H49" s="10">
         <v>201</v>
       </c>
-      <c r="I49" s="9">
+      <c r="I49" s="8">
         <v>1</v>
       </c>
-      <c r="J49" s="8" t="str">
+      <c r="J49" s="7" t="str">
         <f t="shared" si="1"/>
         <v>F;F/M;F/M/U</v>
       </c>
@@ -8216,13 +8322,13 @@
       <c r="B50" t="s">
         <v>245</v>
       </c>
-      <c r="C50" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="D50" s="4" t="s">
+      <c r="C50" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D50" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="E50" s="3" t="s">
         <v>245</v>
       </c>
       <c r="F50" t="s">
@@ -8234,19 +8340,19 @@
       <c r="H50">
         <v>201</v>
       </c>
-      <c r="I50" s="8">
+      <c r="I50" s="7">
         <v>0.5</v>
       </c>
-      <c r="J50" s="8" t="str">
+      <c r="J50" s="7" t="str">
         <f t="shared" si="1"/>
         <v>missing_sex_1</v>
       </c>
-      <c r="K50" s="8"/>
-      <c r="L50" s="8"/>
-      <c r="M50" s="8"/>
-      <c r="N50" s="8"/>
-      <c r="O50" s="8"/>
-      <c r="P50" s="8"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
+      <c r="N50" s="7"/>
+      <c r="O50" s="7"/>
+      <c r="P50" s="7"/>
       <c r="S50" t="s">
         <v>305</v>
       </c>
@@ -8264,31 +8370,31 @@
       <c r="D51" t="s">
         <v>404</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="E51" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="F51" s="4" t="s">
+      <c r="F51" s="3" t="s">
         <v>230</v>
       </c>
       <c r="G51" t="s">
         <v>232</v>
       </c>
-      <c r="H51" s="11">
+      <c r="H51" s="10">
         <v>201</v>
       </c>
-      <c r="I51" s="9">
+      <c r="I51" s="8">
         <v>0.5</v>
       </c>
-      <c r="J51" s="8" t="str">
+      <c r="J51" s="7" t="str">
         <f t="shared" si="1"/>
         <v>U;F/M/U</v>
       </c>
-      <c r="K51" s="9"/>
-      <c r="L51" s="9"/>
-      <c r="M51" s="9"/>
-      <c r="N51" s="9"/>
-      <c r="O51" s="9"/>
-      <c r="P51" s="9"/>
+      <c r="K51" s="8"/>
+      <c r="L51" s="8"/>
+      <c r="M51" s="8"/>
+      <c r="N51" s="8"/>
+      <c r="O51" s="8"/>
+      <c r="P51" s="8"/>
       <c r="U51" t="s">
         <v>290</v>
       </c>
@@ -8312,24 +8418,24 @@
       <c r="E52" t="s">
         <v>223</v>
       </c>
-      <c r="F52" s="4" t="s">
+      <c r="F52" s="3" t="s">
         <v>229</v>
       </c>
       <c r="G52" t="s">
         <v>231</v>
       </c>
-      <c r="H52" s="11">
+      <c r="H52" s="10">
         <v>202</v>
       </c>
-      <c r="I52" s="9">
+      <c r="I52" s="8">
         <v>1</v>
       </c>
-      <c r="J52" s="8" t="str">
+      <c r="J52" s="7" t="str">
         <f t="shared" si="1"/>
         <v>M;F/M;F/M/U</v>
       </c>
-      <c r="S52" s="9"/>
-      <c r="T52" s="9"/>
+      <c r="S52" s="8"/>
+      <c r="T52" s="8"/>
       <c r="U52" t="s">
         <v>257</v>
       </c>
@@ -8347,13 +8453,13 @@
       <c r="B53" t="s">
         <v>245</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="D53" s="4" t="s">
+      <c r="C53" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="E53" s="4" t="s">
+      <c r="E53" s="3" t="s">
         <v>245</v>
       </c>
       <c r="F53" t="s">
@@ -8362,22 +8468,22 @@
       <c r="G53" t="s">
         <v>231</v>
       </c>
-      <c r="H53" s="11">
+      <c r="H53" s="10">
         <v>202</v>
       </c>
-      <c r="I53" s="8">
+      <c r="I53" s="7">
         <v>0.5</v>
       </c>
-      <c r="J53" s="8" t="str">
+      <c r="J53" s="7" t="str">
         <f t="shared" si="1"/>
         <v>missing_sex_1</v>
       </c>
-      <c r="K53" s="8"/>
-      <c r="L53" s="8"/>
-      <c r="M53" s="8"/>
-      <c r="N53" s="8"/>
-      <c r="O53" s="8"/>
-      <c r="P53" s="8"/>
+      <c r="K53" s="7"/>
+      <c r="L53" s="7"/>
+      <c r="M53" s="7"/>
+      <c r="N53" s="7"/>
+      <c r="O53" s="7"/>
+      <c r="P53" s="7"/>
       <c r="S53" t="s">
         <v>305</v>
       </c>
@@ -8395,27 +8501,27 @@
       <c r="D54" t="s">
         <v>404</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="E54" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="F54" s="4" t="s">
+      <c r="F54" s="3" t="s">
         <v>229</v>
       </c>
       <c r="G54" t="s">
         <v>231</v>
       </c>
-      <c r="H54" s="11">
+      <c r="H54" s="10">
         <v>202</v>
       </c>
-      <c r="I54" s="9">
+      <c r="I54" s="8">
         <v>0.5</v>
       </c>
-      <c r="J54" s="8" t="str">
+      <c r="J54" s="7" t="str">
         <f t="shared" si="1"/>
         <v>U;F/M/U</v>
       </c>
-      <c r="S54" s="9"/>
-      <c r="T54" s="9"/>
+      <c r="S54" s="8"/>
+      <c r="T54" s="8"/>
       <c r="U54" t="s">
         <v>290</v>
       </c>
@@ -8427,13 +8533,13 @@
       <c r="A55" t="s">
         <v>329</v>
       </c>
-      <c r="B55" s="16" t="s">
+      <c r="B55" s="15" t="s">
         <v>340</v>
       </c>
       <c r="C55" t="s">
         <v>334</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D55" s="3" t="s">
         <v>406</v>
       </c>
       <c r="E55" t="s">
@@ -8448,10 +8554,10 @@
       <c r="H55">
         <v>300</v>
       </c>
-      <c r="I55" s="9">
+      <c r="I55" s="8">
         <v>1</v>
       </c>
-      <c r="J55" s="8" t="str">
+      <c r="J55" s="7" t="str">
         <f t="shared" si="1"/>
         <v>kp1</v>
       </c>
@@ -8463,13 +8569,13 @@
       <c r="A56" t="s">
         <v>329</v>
       </c>
-      <c r="B56" s="16" t="s">
+      <c r="B56" s="15" t="s">
         <v>340</v>
       </c>
       <c r="C56" t="s">
         <v>332</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="D56" s="3" t="s">
         <v>406</v>
       </c>
       <c r="E56" t="s">
@@ -8484,10 +8590,10 @@
       <c r="H56">
         <v>310</v>
       </c>
-      <c r="I56" s="9">
+      <c r="I56" s="8">
         <v>1</v>
       </c>
-      <c r="J56" s="8" t="str">
+      <c r="J56" s="7" t="str">
         <f t="shared" si="1"/>
         <v>kp1</v>
       </c>
@@ -8499,13 +8605,13 @@
       <c r="A57" t="s">
         <v>329</v>
       </c>
-      <c r="B57" s="16" t="s">
+      <c r="B57" s="15" t="s">
         <v>340</v>
       </c>
       <c r="C57" t="s">
         <v>338</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D57" s="3" t="s">
         <v>406</v>
       </c>
       <c r="E57" t="s">
@@ -8520,10 +8626,10 @@
       <c r="H57">
         <v>320</v>
       </c>
-      <c r="I57" s="9">
+      <c r="I57" s="8">
         <v>1</v>
       </c>
-      <c r="J57" s="8" t="str">
+      <c r="J57" s="7" t="str">
         <f t="shared" si="1"/>
         <v>kp1</v>
       </c>
@@ -8535,13 +8641,13 @@
       <c r="A58" t="s">
         <v>329</v>
       </c>
-      <c r="B58" s="16" t="s">
+      <c r="B58" s="15" t="s">
         <v>340</v>
       </c>
       <c r="C58" t="s">
         <v>330</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="D58" s="3" t="s">
         <v>406</v>
       </c>
       <c r="E58" t="s">
@@ -8553,13 +8659,13 @@
       <c r="G58" t="s">
         <v>330</v>
       </c>
-      <c r="H58" s="11">
+      <c r="H58" s="10">
         <v>330</v>
       </c>
-      <c r="I58" s="9">
+      <c r="I58" s="8">
         <v>1</v>
       </c>
-      <c r="J58" s="8" t="str">
+      <c r="J58" s="7" t="str">
         <f t="shared" si="1"/>
         <v>kp1</v>
       </c>
@@ -8571,13 +8677,13 @@
       <c r="A59" t="s">
         <v>329</v>
       </c>
-      <c r="B59" s="16" t="s">
+      <c r="B59" s="15" t="s">
         <v>340</v>
       </c>
       <c r="C59" t="s">
         <v>336</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="3" t="s">
         <v>406</v>
       </c>
       <c r="E59" t="s">
@@ -8592,10 +8698,10 @@
       <c r="H59">
         <v>340</v>
       </c>
-      <c r="I59" s="9">
+      <c r="I59" s="8">
         <v>1</v>
       </c>
-      <c r="J59" s="8" t="str">
+      <c r="J59" s="7" t="str">
         <f t="shared" ref="J59" si="2">_xlfn.TEXTJOIN(";",1,K59,L59,M59,N59,O59,P59,Q59,S59,T59,U59,V59,W59,R59,X59)</f>
         <v>kp1</v>
       </c>

</xml_diff>

<commit_message>
Add additional dimension item columns for b indicator
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0BFA15-B897-4C44-8D5E-F49F63CDB166}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70EF508-B624-A84E-B125-039256E92B0B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="0" windowWidth="25600" windowHeight="20480" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data_required!$A$1:$V$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data_required!$A$1:$Z$55</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">dimension_Item_sets!$A$1:$X$59</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1944" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2164" uniqueCount="453">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1384,6 +1384,18 @@
   </si>
   <si>
     <t>sk2aTYKnZNz</t>
+  </si>
+  <si>
+    <t>B.add_dim_1</t>
+  </si>
+  <si>
+    <t>B.add_dim_1_uid</t>
+  </si>
+  <si>
+    <t>B.add_dim_1_items</t>
+  </si>
+  <si>
+    <t>B.add_dim_1_items_uid</t>
   </si>
 </sst>
 </file>
@@ -1800,12 +1812,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
-  <dimension ref="A1:V55"/>
+  <dimension ref="A1:Z55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomLeft" activeCell="Y61" sqref="Y61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1824,7 +1836,7 @@
     <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>292</v>
       </c>
@@ -1889,10 +1901,22 @@
         <v>296</v>
       </c>
       <c r="V1" t="s">
+        <v>449</v>
+      </c>
+      <c r="W1" t="s">
+        <v>450</v>
+      </c>
+      <c r="X1" t="s">
+        <v>451</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>452</v>
+      </c>
+      <c r="Z1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1959,8 +1983,20 @@
       <c r="V2" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W2" t="s">
+        <v>244</v>
+      </c>
+      <c r="X2" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2027,8 +2063,20 @@
       <c r="V3" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W3" t="s">
+        <v>244</v>
+      </c>
+      <c r="X3" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2095,8 +2143,20 @@
       <c r="V4" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W4" t="s">
+        <v>244</v>
+      </c>
+      <c r="X4" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -2163,8 +2223,20 @@
       <c r="V5" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W5" t="s">
+        <v>244</v>
+      </c>
+      <c r="X5" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2231,8 +2303,20 @@
       <c r="V6" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W6" t="s">
+        <v>244</v>
+      </c>
+      <c r="X6" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -2299,8 +2383,20 @@
       <c r="V7" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W7" t="s">
+        <v>244</v>
+      </c>
+      <c r="X7" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -2365,10 +2461,22 @@
         <v>248</v>
       </c>
       <c r="V8" t="s">
+        <v>244</v>
+      </c>
+      <c r="W8" t="s">
+        <v>244</v>
+      </c>
+      <c r="X8" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z8" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2435,8 +2543,20 @@
       <c r="V9" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W9" t="s">
+        <v>244</v>
+      </c>
+      <c r="X9" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2503,8 +2623,20 @@
       <c r="V10" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W10" t="s">
+        <v>244</v>
+      </c>
+      <c r="X10" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -2571,8 +2703,20 @@
       <c r="V11" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W11" t="s">
+        <v>244</v>
+      </c>
+      <c r="X11" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -2639,8 +2783,20 @@
       <c r="V12" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W12" t="s">
+        <v>244</v>
+      </c>
+      <c r="X12" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -2707,8 +2863,20 @@
       <c r="V13" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W13" t="s">
+        <v>244</v>
+      </c>
+      <c r="X13" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -2775,8 +2943,20 @@
       <c r="V14" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" ht="18" x14ac:dyDescent="0.25">
+      <c r="W14" t="s">
+        <v>244</v>
+      </c>
+      <c r="X14" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -2843,8 +3023,20 @@
       <c r="V15" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" ht="18" x14ac:dyDescent="0.25">
+      <c r="W15" t="s">
+        <v>244</v>
+      </c>
+      <c r="X15" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -2911,8 +3103,20 @@
       <c r="V16" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="17" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="W16" t="s">
+        <v>244</v>
+      </c>
+      <c r="X16" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -2977,10 +3181,22 @@
         <v>258</v>
       </c>
       <c r="V17" t="s">
+        <v>244</v>
+      </c>
+      <c r="W17" t="s">
+        <v>244</v>
+      </c>
+      <c r="X17" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z17" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -3045,10 +3261,22 @@
         <v>258</v>
       </c>
       <c r="V18" t="s">
+        <v>244</v>
+      </c>
+      <c r="W18" t="s">
+        <v>244</v>
+      </c>
+      <c r="X18" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z18" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -3113,10 +3341,22 @@
         <v>258</v>
       </c>
       <c r="V19" t="s">
+        <v>244</v>
+      </c>
+      <c r="W19" t="s">
+        <v>244</v>
+      </c>
+      <c r="X19" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z19" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -3181,10 +3421,22 @@
         <v>258</v>
       </c>
       <c r="V20" t="s">
+        <v>244</v>
+      </c>
+      <c r="W20" t="s">
+        <v>244</v>
+      </c>
+      <c r="X20" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z20" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -3249,10 +3501,22 @@
         <v>258</v>
       </c>
       <c r="V21" t="s">
+        <v>244</v>
+      </c>
+      <c r="W21" t="s">
+        <v>244</v>
+      </c>
+      <c r="X21" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z21" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -3317,10 +3581,22 @@
         <v>258</v>
       </c>
       <c r="V22" t="s">
+        <v>244</v>
+      </c>
+      <c r="W22" t="s">
+        <v>244</v>
+      </c>
+      <c r="X22" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z22" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -3385,10 +3661,22 @@
         <v>258</v>
       </c>
       <c r="V23" t="s">
+        <v>244</v>
+      </c>
+      <c r="W23" t="s">
+        <v>244</v>
+      </c>
+      <c r="X23" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z23" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -3453,10 +3741,22 @@
         <v>258</v>
       </c>
       <c r="V24" t="s">
+        <v>244</v>
+      </c>
+      <c r="W24" t="s">
+        <v>244</v>
+      </c>
+      <c r="X24" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z24" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -3521,10 +3821,22 @@
         <v>258</v>
       </c>
       <c r="V25" t="s">
+        <v>244</v>
+      </c>
+      <c r="W25" t="s">
+        <v>244</v>
+      </c>
+      <c r="X25" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z25" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -3589,10 +3901,22 @@
         <v>258</v>
       </c>
       <c r="V26" t="s">
+        <v>244</v>
+      </c>
+      <c r="W26" t="s">
+        <v>244</v>
+      </c>
+      <c r="X26" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z26" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -3659,8 +3983,20 @@
       <c r="V27" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="28" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="W27" t="s">
+        <v>244</v>
+      </c>
+      <c r="X27" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -3727,8 +4063,20 @@
       <c r="V28" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="29" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="W28" t="s">
+        <v>244</v>
+      </c>
+      <c r="X28" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -3795,8 +4143,20 @@
       <c r="V29" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="30" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="W29" t="s">
+        <v>244</v>
+      </c>
+      <c r="X29" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -3863,8 +4223,20 @@
       <c r="V30" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="31" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="W30" t="s">
+        <v>244</v>
+      </c>
+      <c r="X30" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -3931,8 +4303,20 @@
       <c r="V31" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="32" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="W31" t="s">
+        <v>244</v>
+      </c>
+      <c r="X31" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -3999,8 +4383,20 @@
       <c r="V32" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="33" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="W32" t="s">
+        <v>244</v>
+      </c>
+      <c r="X32" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -4067,8 +4463,20 @@
       <c r="V33" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="34" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="W33" t="s">
+        <v>244</v>
+      </c>
+      <c r="X33" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -4135,8 +4543,20 @@
       <c r="V34" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="35" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="W34" t="s">
+        <v>244</v>
+      </c>
+      <c r="X34" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -4203,8 +4623,20 @@
       <c r="V35" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="36" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="W35" t="s">
+        <v>244</v>
+      </c>
+      <c r="X35" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -4271,8 +4703,20 @@
       <c r="V36" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="37" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="W36" t="s">
+        <v>244</v>
+      </c>
+      <c r="X36" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -4336,11 +4780,23 @@
       <c r="U37" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="V37" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="38" spans="1:22" ht="18" x14ac:dyDescent="0.2">
+      <c r="V37" t="s">
+        <v>244</v>
+      </c>
+      <c r="W37" t="s">
+        <v>244</v>
+      </c>
+      <c r="X37" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z37" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -4402,11 +4858,23 @@
       <c r="U38" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="V38" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="39" spans="1:22" ht="18" x14ac:dyDescent="0.2">
+      <c r="V38" t="s">
+        <v>244</v>
+      </c>
+      <c r="W38" t="s">
+        <v>244</v>
+      </c>
+      <c r="X38" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z38" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -4471,10 +4939,22 @@
         <v>248</v>
       </c>
       <c r="V39" t="s">
+        <v>244</v>
+      </c>
+      <c r="W39" t="s">
+        <v>244</v>
+      </c>
+      <c r="X39" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z39" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="40" spans="1:22" ht="18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>82</v>
       </c>
@@ -4538,11 +5018,23 @@
       <c r="U40" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="V40" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22" ht="18" x14ac:dyDescent="0.2">
+      <c r="V40" t="s">
+        <v>244</v>
+      </c>
+      <c r="W40" t="s">
+        <v>244</v>
+      </c>
+      <c r="X40" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z40" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>82</v>
       </c>
@@ -4606,11 +5098,23 @@
       <c r="U41" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="V41" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22" ht="18" x14ac:dyDescent="0.2">
+      <c r="V41" t="s">
+        <v>244</v>
+      </c>
+      <c r="W41" t="s">
+        <v>244</v>
+      </c>
+      <c r="X41" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z41" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>87</v>
       </c>
@@ -4674,11 +5178,23 @@
       <c r="U42" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="V42" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="43" spans="1:22" ht="18" x14ac:dyDescent="0.2">
+      <c r="V42" t="s">
+        <v>244</v>
+      </c>
+      <c r="W42" t="s">
+        <v>244</v>
+      </c>
+      <c r="X42" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z42" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>87</v>
       </c>
@@ -4743,10 +5259,22 @@
         <v>258</v>
       </c>
       <c r="V43" t="s">
+        <v>244</v>
+      </c>
+      <c r="W43" t="s">
+        <v>244</v>
+      </c>
+      <c r="X43" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y43" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z43" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="44" spans="1:22" ht="18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>91</v>
       </c>
@@ -4810,11 +5338,23 @@
       <c r="U44" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="V44" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22" ht="18" x14ac:dyDescent="0.2">
+      <c r="V44" t="s">
+        <v>244</v>
+      </c>
+      <c r="W44" t="s">
+        <v>244</v>
+      </c>
+      <c r="X44" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z44" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="16" t="s">
         <v>91</v>
       </c>
@@ -4878,11 +5418,23 @@
       <c r="U45" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="V45" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="46" spans="1:22" ht="18" x14ac:dyDescent="0.2">
+      <c r="V45" t="s">
+        <v>244</v>
+      </c>
+      <c r="W45" t="s">
+        <v>244</v>
+      </c>
+      <c r="X45" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z45" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="16" t="s">
         <v>91</v>
       </c>
@@ -4946,11 +5498,23 @@
       <c r="U46" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="V46" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="47" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="V46" t="s">
+        <v>244</v>
+      </c>
+      <c r="W46" t="s">
+        <v>244</v>
+      </c>
+      <c r="X46" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y46" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z46" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>91</v>
       </c>
@@ -5014,11 +5578,23 @@
       <c r="U47" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="V47" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="48" spans="1:22" ht="18" x14ac:dyDescent="0.2">
+      <c r="V47" t="s">
+        <v>244</v>
+      </c>
+      <c r="W47" t="s">
+        <v>244</v>
+      </c>
+      <c r="X47" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y47" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z47" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>91</v>
       </c>
@@ -5079,11 +5655,23 @@
       <c r="U48" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="V48" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="49" spans="1:22" ht="18" x14ac:dyDescent="0.2">
+      <c r="V48" t="s">
+        <v>244</v>
+      </c>
+      <c r="W48" t="s">
+        <v>244</v>
+      </c>
+      <c r="X48" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y48" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z48" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>91</v>
       </c>
@@ -5147,11 +5735,23 @@
       <c r="U49" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="V49" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="50" spans="1:22" ht="18" x14ac:dyDescent="0.2">
+      <c r="V49" t="s">
+        <v>244</v>
+      </c>
+      <c r="W49" t="s">
+        <v>244</v>
+      </c>
+      <c r="X49" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y49" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z49" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="50" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>108</v>
       </c>
@@ -5215,11 +5815,23 @@
       <c r="U50" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="V50" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="51" spans="1:22" ht="18" x14ac:dyDescent="0.2">
+      <c r="V50" t="s">
+        <v>244</v>
+      </c>
+      <c r="W50" t="s">
+        <v>244</v>
+      </c>
+      <c r="X50" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y50" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z50" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>108</v>
       </c>
@@ -5284,10 +5896,22 @@
         <v>248</v>
       </c>
       <c r="V51" t="s">
+        <v>244</v>
+      </c>
+      <c r="W51" t="s">
+        <v>244</v>
+      </c>
+      <c r="X51" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y51" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z51" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="52" spans="1:22" ht="18" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>112</v>
       </c>
@@ -5351,11 +5975,23 @@
       <c r="U52" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="V52" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="53" spans="1:22" ht="18" x14ac:dyDescent="0.2">
+      <c r="V52" t="s">
+        <v>244</v>
+      </c>
+      <c r="W52" t="s">
+        <v>244</v>
+      </c>
+      <c r="X52" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y52" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z52" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>115</v>
       </c>
@@ -5422,8 +6058,20 @@
       <c r="V53" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W53" t="s">
+        <v>244</v>
+      </c>
+      <c r="X53" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y53" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z53" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>115</v>
       </c>
@@ -5490,8 +6138,20 @@
       <c r="V54" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="55" spans="1:22" ht="18" x14ac:dyDescent="0.2">
+      <c r="W54" t="s">
+        <v>244</v>
+      </c>
+      <c r="X54" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y54" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z54" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="55" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>115</v>
       </c>
@@ -5556,11 +6216,23 @@
         <v>244</v>
       </c>
       <c r="V55" t="s">
+        <v>244</v>
+      </c>
+      <c r="W55" t="s">
+        <v>244</v>
+      </c>
+      <c r="X55" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y55" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z55" t="s">
         <v>255</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V55" xr:uid="{DF301E54-0E7B-1E4E-9373-0F8968A635A9}"/>
+  <autoFilter ref="A1:Z55" xr:uid="{DF301E54-0E7B-1E4E-9373-0F8968A635A9}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
adding new rows and columns for site tool dimesion to option mapping
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C67C2F-6A84-4148-B0ED-FE8A4B0BFDDE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565E0185-E1E1-9F41-B047-597502952F3F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="-20" yWindow="700" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data_required!$A$1:$Z$56</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">dimension_Item_sets!$A$1:$X$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">dimension_Item_sets!$A$1:$X$61</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2191" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2251" uniqueCount="491">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1429,6 +1429,87 @@
   </si>
   <si>
     <t>HTS_INDEX.N.newYield</t>
+  </si>
+  <si>
+    <t>tr</t>
+  </si>
+  <si>
+    <t>M8W7M5GlOPh</t>
+  </si>
+  <si>
+    <t>&lt;2 Months (Specific)</t>
+  </si>
+  <si>
+    <t>2-12 Months (Specific)</t>
+  </si>
+  <si>
+    <t>V1TzJFJTdHd</t>
+  </si>
+  <si>
+    <t>&lt;2mo</t>
+  </si>
+  <si>
+    <t>2-12mo</t>
+  </si>
+  <si>
+    <t>&lt; 2 months</t>
+  </si>
+  <si>
+    <t>2 - 12 months</t>
+  </si>
+  <si>
+    <t>pbXCUjm50XK</t>
+  </si>
+  <si>
+    <t>pElywX5bn06</t>
+  </si>
+  <si>
+    <t>KnownNewResult</t>
+  </si>
+  <si>
+    <t>bDWsPYyXgWP</t>
+  </si>
+  <si>
+    <t>HIV Test Status (Specific)</t>
+  </si>
+  <si>
+    <t>ts</t>
+  </si>
+  <si>
+    <t>Newly Identified Positive (Specific)</t>
+  </si>
+  <si>
+    <t>mSBg9AZx1lV</t>
+  </si>
+  <si>
+    <t>Known at Entry Positive (Specific)</t>
+  </si>
+  <si>
+    <t>e9fbFnQEyyA</t>
+  </si>
+  <si>
+    <t>Newly Identified Negative (Specific)</t>
+  </si>
+  <si>
+    <t>viYXyEy7wKi</t>
+  </si>
+  <si>
+    <t>Known at Entry Positive</t>
+  </si>
+  <si>
+    <t>LvheCKbuFJZ</t>
+  </si>
+  <si>
+    <t>Newly Identified Negative</t>
+  </si>
+  <si>
+    <t>BiB1MtA7o4A</t>
+  </si>
+  <si>
+    <t>Newly Identified Positive</t>
+  </si>
+  <si>
+    <t>Vr59uUJBySG</t>
   </si>
 </sst>
 </file>
@@ -1840,10 +1921,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
   <dimension ref="A1:Z56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomLeft" activeCell="P51" sqref="P51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7105,20 +7186,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
-  <dimension ref="A1:X59"/>
+  <dimension ref="A1:AB66"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView topLeftCell="A35" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64:F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.83203125" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="41.83203125" customWidth="1"/>
     <col min="11" max="13" width="12.33203125" customWidth="1"/>
@@ -7126,7 +7207,7 @@
     <col min="19" max="19" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>389</v>
       </c>
@@ -7199,368 +7280,383 @@
       <c r="X1" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y1" t="s">
+        <v>464</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>469</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>470</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>294</v>
       </c>
       <c r="B2" t="s">
         <v>406</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" t="s">
+        <v>465</v>
+      </c>
+      <c r="D2" t="s">
         <v>385</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="H2" s="9">
-        <v>10</v>
-      </c>
-      <c r="I2" s="7">
+      <c r="E2" t="s">
+        <v>466</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
         <v>1</v>
       </c>
       <c r="J2" s="6" t="str">
-        <f t="shared" ref="J2:J27" si="0">_xlfn.TEXTJOIN(";",1,K2,L2,M2,N2,O2,P2,Q2,S2,T2,U2,V2,W2,R2,X2)</f>
-        <v>&lt;1-50+;&lt;1-18+</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>250</v>
-      </c>
+        <f>_xlfn.TEXTJOIN(";",1,K2,L2,M2,N2,O2,P2,Q2,S2,T2,U2,V2,W2,R2,X2,Y2,Z2,AA2,AB2)</f>
+        <v>&lt;2mo</v>
+      </c>
+      <c r="K2" s="12"/>
       <c r="L2" s="12"/>
       <c r="M2" s="12"/>
       <c r="N2" s="12"/>
-      <c r="O2" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="Z2" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>294</v>
       </c>
       <c r="B3" t="s">
         <v>406</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
+        <v>468</v>
+      </c>
+      <c r="D3" t="s">
+        <v>385</v>
+      </c>
+      <c r="E3" t="s">
+        <v>467</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" s="6" t="str">
+        <f t="shared" ref="J3:J66" si="0">_xlfn.TEXTJOIN(";",1,K3,L3,M3,N3,O3,P3,Q3,S3,T3,U3,V3,W3,R3,X3,Y3,Z3,AA3,AB3)</f>
+        <v>2-12mo</v>
+      </c>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="T3" s="12"/>
+      <c r="AA3" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B4" t="s">
+        <v>406</v>
+      </c>
+      <c r="C4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" t="s">
+        <v>385</v>
+      </c>
+      <c r="E4" t="s">
+        <v>446</v>
+      </c>
+      <c r="F4" t="s">
+        <v>185</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="H4" s="9">
+        <v>10</v>
+      </c>
+      <c r="I4" s="7">
+        <v>1</v>
+      </c>
+      <c r="J4" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;1-50+;&lt;1-18+</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B5" t="s">
+        <v>406</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H5" s="9">
         <v>10</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I5" s="7">
         <v>0.25</v>
       </c>
-      <c r="J3" s="6" t="str">
+      <c r="J5" s="6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;15/&gt;15.d</v>
       </c>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12" t="s">
+      <c r="O5" s="12"/>
+      <c r="P5" s="12" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>294</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>406</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" t="s">
         <v>270</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H6" s="8">
         <v>10</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I6" s="6">
         <v>0.2</v>
       </c>
-      <c r="J4" s="6" t="str">
+      <c r="J6" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>294</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>406</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H7" s="9">
         <v>20</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I7" s="7">
         <v>0.5</v>
       </c>
-      <c r="J5" s="6" t="str">
+      <c r="J7" s="6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;1-50+;1-50+;&lt;1-18+;1-4;1-50+/&lt;5</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K7" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L7" s="12" t="s">
         <v>252</v>
       </c>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" t="s">
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" t="s">
         <v>402</v>
       </c>
-      <c r="Q5" s="12" t="s">
+      <c r="Q7" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="R5" s="12" t="s">
+      <c r="R7" s="12" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>294</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>406</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H8" s="9">
         <v>20</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I8" s="7">
         <v>0.25</v>
       </c>
-      <c r="J6" s="6" t="str">
+      <c r="J8" s="6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;15/&gt;15.d</v>
       </c>
-      <c r="P6" s="12" t="s">
+      <c r="P8" s="12" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>294</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>406</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C9" t="s">
         <v>270</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H9" s="8">
         <v>20</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I9" s="6">
         <v>1</v>
       </c>
-      <c r="J7" s="6" t="str">
+      <c r="J9" s="6" t="str">
         <f t="shared" si="0"/>
         <v>1-4;1-50+/&lt;5</v>
       </c>
-      <c r="Q7" s="12" t="s">
+      <c r="Q9" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="R7" s="12" t="s">
+      <c r="R9" s="12" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>294</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>406</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H10" s="9">
         <v>30</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I10" s="7">
         <v>0.5</v>
       </c>
-      <c r="J8" s="6" t="str">
+      <c r="J10" s="6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;1-50+;1-50+;&lt;1-18+;1-50+/&lt;5</v>
       </c>
-      <c r="K8" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="L8" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" t="s">
-        <v>402</v>
-      </c>
-      <c r="R8" s="12" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>294</v>
-      </c>
-      <c r="B9" t="s">
-        <v>406</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="H9" s="9">
-        <v>30</v>
-      </c>
-      <c r="I9" s="7">
-        <v>0.25</v>
-      </c>
-      <c r="J9" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;15/&gt;15.d</v>
-      </c>
-      <c r="P9" s="12" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>294</v>
-      </c>
-      <c r="B10" t="s">
-        <v>406</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="H10" s="9">
-        <v>40</v>
-      </c>
-      <c r="I10" s="7">
-        <v>1</v>
-      </c>
-      <c r="J10" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;10-50+;&lt;1-18+;10-50+.all;1-50+/&lt;5</v>
-      </c>
       <c r="K10" s="12" t="s">
         <v>250</v>
       </c>
       <c r="L10" s="12" t="s">
         <v>252</v>
       </c>
-      <c r="M10" s="12" t="s">
-        <v>234</v>
-      </c>
+      <c r="M10" s="12"/>
       <c r="N10" s="12"/>
       <c r="O10" t="s">
         <v>402</v>
@@ -7568,11 +7664,8 @@
       <c r="R10" s="12" t="s">
         <v>396</v>
       </c>
-      <c r="T10" s="12" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>294</v>
       </c>
@@ -7589,13 +7682,13 @@
         <v>447</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>204</v>
+        <v>184</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>213</v>
       </c>
       <c r="H11" s="9">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="I11" s="7">
         <v>0.25</v>
@@ -7608,21 +7701,21 @@
         <v>291</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>237</v>
+        <v>294</v>
       </c>
       <c r="B12" t="s">
-        <v>237</v>
+        <v>406</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>237</v>
+        <v>169</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>237</v>
+        <v>450</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>192</v>
@@ -7633,166 +7726,182 @@
       <c r="H12" s="9">
         <v>40</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="7">
+        <v>1</v>
+      </c>
+      <c r="J12" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;1-50+;1-50+;10-50+;&lt;1-18+;10-50+.all;1-50+/&lt;5</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="N12" s="12"/>
+      <c r="O12" t="s">
+        <v>402</v>
+      </c>
+      <c r="R12" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="T12" s="12" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>294</v>
+      </c>
+      <c r="B13" t="s">
+        <v>406</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="H13" s="9">
+        <v>40</v>
+      </c>
+      <c r="I13" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="J13" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;15/&gt;15.d</v>
+      </c>
+      <c r="P13" s="12" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>237</v>
+      </c>
+      <c r="B14" t="s">
+        <v>237</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="H14" s="9">
+        <v>40</v>
+      </c>
+      <c r="I14" s="6">
         <f>1/9</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="J12" s="6" t="str">
+      <c r="J14" s="6" t="str">
         <f t="shared" si="0"/>
         <v>missing_age_1</v>
       </c>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="S12" t="s">
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="S14" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="15" spans="1:28" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>294</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>406</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G15" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H15" s="9">
         <v>45</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I15" s="6">
         <v>1</v>
       </c>
-      <c r="J13" s="6" t="str">
+      <c r="J15" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>237</v>
-      </c>
-      <c r="B14" t="s">
-        <v>237</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="P15" s="12"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>237</v>
+      </c>
+      <c r="B16" t="s">
+        <v>237</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="E16" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="F16" t="s">
         <v>196</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G16" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H16" s="9">
         <v>45</v>
       </c>
-      <c r="I14">
+      <c r="I16">
         <v>0.5</v>
       </c>
-      <c r="J14" s="6" t="str">
+      <c r="J16" s="6" t="str">
         <f t="shared" si="0"/>
         <v>missing_age_2</v>
       </c>
-      <c r="S14" t="s">
+      <c r="S16" t="s">
         <v>288</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>294</v>
-      </c>
-      <c r="B15" t="s">
-        <v>406</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="H15" s="9">
-        <v>50</v>
-      </c>
-      <c r="I15" s="7">
-        <v>1</v>
-      </c>
-      <c r="J15" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;1-18+</v>
-      </c>
-      <c r="O15" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>294</v>
-      </c>
-      <c r="B16" t="s">
-        <v>406</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="H16" s="9">
-        <v>60</v>
-      </c>
-      <c r="I16" s="6">
-        <v>0.125</v>
-      </c>
-      <c r="J16" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;15/&gt;15.d</v>
-      </c>
-      <c r="P16" s="12" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
@@ -7803,64 +7912,49 @@
         <v>406</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>451</v>
+        <v>460</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H17" s="9">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I17" s="7">
         <v>1</v>
       </c>
       <c r="J17" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
-      </c>
-      <c r="K17" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="L17" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="M17" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="N17" s="12" t="s">
-        <v>272</v>
-      </c>
-      <c r="R17" s="12" t="s">
-        <v>396</v>
-      </c>
-      <c r="T17" s="12" t="s">
-        <v>309</v>
+        <v>&lt;1-18+</v>
+      </c>
+      <c r="O17" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>237</v>
+        <v>294</v>
       </c>
       <c r="B18" t="s">
-        <v>237</v>
+        <v>406</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>237</v>
+        <v>179</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>237</v>
+        <v>461</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>194</v>
@@ -7872,88 +7966,99 @@
         <v>60</v>
       </c>
       <c r="I18" s="6">
+        <v>0.125</v>
+      </c>
+      <c r="J18" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;15/&gt;15.d</v>
+      </c>
+      <c r="P18" s="12" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>294</v>
+      </c>
+      <c r="B19" t="s">
+        <v>406</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="H19" s="9">
+        <v>60</v>
+      </c>
+      <c r="I19" s="7">
+        <v>1</v>
+      </c>
+      <c r="J19" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
+      </c>
+      <c r="K19" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="L19" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="M19" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="N19" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="R19" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="T19" s="12" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>237</v>
+      </c>
+      <c r="B20" t="s">
+        <v>237</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="H20" s="9">
+        <v>60</v>
+      </c>
+      <c r="I20" s="6">
         <f>1/9</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="J18" s="6" t="str">
+      <c r="J20" s="6" t="str">
         <f t="shared" si="0"/>
         <v>missing_age_1</v>
-      </c>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-      <c r="S18" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>294</v>
-      </c>
-      <c r="B19" t="s">
-        <v>406</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="H19" s="10">
-        <v>65</v>
-      </c>
-      <c r="I19" s="6">
-        <v>1</v>
-      </c>
-      <c r="J19" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="P19" s="13"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>237</v>
-      </c>
-      <c r="B20" t="s">
-        <v>237</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="F20" t="s">
-        <v>197</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="H20" s="9">
-        <v>65</v>
-      </c>
-      <c r="I20">
-        <v>0.5</v>
-      </c>
-      <c r="J20" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>missing_age_2</v>
       </c>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
@@ -7962,10 +8067,10 @@
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
       <c r="S20" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>294</v>
       </c>
@@ -7973,73 +8078,72 @@
         <v>406</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>452</v>
+        <v>461</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>403</v>
+        <v>197</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>404</v>
-      </c>
-      <c r="H21" s="9">
-        <v>70</v>
-      </c>
-      <c r="I21" s="7">
+        <v>198</v>
+      </c>
+      <c r="H21" s="10">
+        <v>65</v>
+      </c>
+      <c r="I21" s="6">
         <v>1</v>
       </c>
       <c r="J21" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;1-18+</v>
-      </c>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" t="s">
-        <v>402</v>
-      </c>
-      <c r="P21" s="7"/>
+        <v/>
+      </c>
+      <c r="P21" s="13"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>294</v>
+        <v>237</v>
       </c>
       <c r="B22" t="s">
-        <v>406</v>
+        <v>237</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>179</v>
+        <v>237</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>195</v>
+        <v>237</v>
+      </c>
+      <c r="F22" t="s">
+        <v>197</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="H22" s="9">
-        <v>80</v>
-      </c>
-      <c r="I22" s="7">
-        <v>0.125</v>
+        <v>65</v>
+      </c>
+      <c r="I22">
+        <v>0.5</v>
       </c>
       <c r="J22" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;15/&gt;15.d</v>
-      </c>
-      <c r="P22" s="12" t="s">
-        <v>291</v>
+        <v>missing_age_2</v>
+      </c>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="S22" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
@@ -8050,64 +8154,54 @@
         <v>406</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>195</v>
+        <v>403</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>207</v>
+        <v>404</v>
       </c>
       <c r="H23" s="9">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="I23" s="7">
         <v>1</v>
       </c>
       <c r="J23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
-      </c>
-      <c r="K23" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="L23" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="M23" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="N23" s="12" t="s">
-        <v>272</v>
-      </c>
-      <c r="R23" s="12" t="s">
-        <v>396</v>
-      </c>
-      <c r="T23" s="12" t="s">
-        <v>309</v>
-      </c>
+        <v>&lt;1-18+</v>
+      </c>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" t="s">
+        <v>402</v>
+      </c>
+      <c r="P23" s="7"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>237</v>
+        <v>294</v>
       </c>
       <c r="B24" t="s">
-        <v>237</v>
+        <v>406</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>237</v>
+        <v>179</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>237</v>
+        <v>461</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>195</v>
@@ -8118,22 +8212,15 @@
       <c r="H24" s="9">
         <v>80</v>
       </c>
-      <c r="I24" s="6">
-        <f>1/9</f>
-        <v>0.1111111111111111</v>
+      <c r="I24" s="7">
+        <v>0.125</v>
       </c>
       <c r="J24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>missing_age_1</v>
-      </c>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-      <c r="S24" t="s">
-        <v>287</v>
+        <v>&lt;15/&gt;15.d</v>
+      </c>
+      <c r="P24" s="12" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
@@ -8144,85 +8231,90 @@
         <v>406</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H25" s="9">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="I25" s="7">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="J25" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;15/&gt;15.d</v>
-      </c>
-      <c r="P25" s="12" t="s">
-        <v>291</v>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
+      </c>
+      <c r="K25" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="L25" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="M25" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="N25" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="R25" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="T25" s="12" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>294</v>
+        <v>237</v>
       </c>
       <c r="B26" t="s">
-        <v>406</v>
+        <v>237</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>174</v>
+        <v>237</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>454</v>
+        <v>237</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H26" s="9">
-        <v>90</v>
-      </c>
-      <c r="I26" s="7">
-        <v>1</v>
+        <v>80</v>
+      </c>
+      <c r="I26" s="6">
+        <f>1/9</f>
+        <v>0.1111111111111111</v>
       </c>
       <c r="J26" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
-      </c>
-      <c r="K26" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="L26" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="M26" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="N26" s="12" t="s">
-        <v>272</v>
-      </c>
-      <c r="O26" s="7"/>
-      <c r="P26" s="7"/>
-      <c r="R26" s="12" t="s">
-        <v>396</v>
-      </c>
-      <c r="T26" s="12" t="s">
-        <v>309</v>
+        <v>missing_age_1</v>
+      </c>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="S26" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
@@ -8233,13 +8325,13 @@
         <v>406</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>455</v>
+        <v>461</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>186</v>
@@ -8251,31 +8343,31 @@
         <v>90</v>
       </c>
       <c r="I27" s="7">
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
       <c r="J27" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>10-50+.all</v>
-      </c>
-      <c r="T27" t="s">
-        <v>309</v>
+        <v>&lt;15/&gt;15.d</v>
+      </c>
+      <c r="P27" s="12" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>237</v>
+        <v>294</v>
       </c>
       <c r="B28" t="s">
-        <v>237</v>
+        <v>406</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>237</v>
+        <v>174</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>237</v>
+        <v>454</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>186</v>
@@ -8286,22 +8378,32 @@
       <c r="H28" s="9">
         <v>90</v>
       </c>
-      <c r="I28" s="6">
-        <f>1/9</f>
-        <v>0.1111111111111111</v>
+      <c r="I28" s="7">
+        <v>1</v>
       </c>
       <c r="J28" s="6" t="str">
-        <f t="shared" ref="J28:J58" si="1">_xlfn.TEXTJOIN(";",1,K28,L28,M28,N28,O28,P28,Q28,S28,T28,U28,V28,W28,R28,X28)</f>
-        <v>missing_age_1</v>
-      </c>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="6"/>
-      <c r="P28" s="6"/>
-      <c r="S28" t="s">
-        <v>287</v>
+        <f t="shared" si="0"/>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
+      </c>
+      <c r="K28" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="L28" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="M28" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="N28" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="R28" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="T28" s="12" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
@@ -8312,68 +8414,75 @@
         <v>406</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>403</v>
+        <v>186</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>404</v>
+        <v>208</v>
       </c>
       <c r="H29" s="9">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="I29" s="7">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="J29" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;1-18+</v>
-      </c>
-      <c r="O29" t="s">
-        <v>402</v>
+        <f t="shared" si="0"/>
+        <v>10-50+.all</v>
+      </c>
+      <c r="T29" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>294</v>
+        <v>237</v>
       </c>
       <c r="B30" t="s">
-        <v>406</v>
+        <v>237</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>179</v>
+        <v>237</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>461</v>
+        <v>237</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H30" s="9">
-        <v>110</v>
-      </c>
-      <c r="I30" s="7">
-        <v>0.125</v>
+        <v>90</v>
+      </c>
+      <c r="I30" s="6">
+        <f>1/9</f>
+        <v>0.1111111111111111</v>
       </c>
       <c r="J30" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;15/&gt;15.d</v>
-      </c>
-      <c r="P30" s="12" t="s">
-        <v>291</v>
+        <f t="shared" si="0"/>
+        <v>missing_age_1</v>
+      </c>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
+      <c r="S30" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
@@ -8384,32 +8493,32 @@
         <v>406</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>187</v>
+        <v>403</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>209</v>
+        <v>404</v>
       </c>
       <c r="H31" s="9">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="I31" s="7">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="J31" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>10-50+.all</v>
-      </c>
-      <c r="T31" t="s">
-        <v>309</v>
+        <f t="shared" si="0"/>
+        <v>&lt;1-18+</v>
+      </c>
+      <c r="O31" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
@@ -8420,13 +8529,13 @@
         <v>406</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>187</v>
@@ -8438,48 +8547,31 @@
         <v>110</v>
       </c>
       <c r="I32" s="7">
-        <v>1</v>
+        <v>0.125</v>
       </c>
       <c r="J32" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
-      </c>
-      <c r="K32" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="L32" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="M32" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="N32" s="12" t="s">
-        <v>272</v>
-      </c>
-      <c r="O32" s="7"/>
-      <c r="P32" s="7"/>
-      <c r="R32" s="12" t="s">
-        <v>396</v>
-      </c>
-      <c r="T32" s="12" t="s">
-        <v>309</v>
+        <f t="shared" si="0"/>
+        <v>&lt;15/&gt;15.d</v>
+      </c>
+      <c r="P32" s="12" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>237</v>
+        <v>294</v>
       </c>
       <c r="B33" t="s">
-        <v>237</v>
+        <v>406</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>237</v>
+        <v>182</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>237</v>
+        <v>455</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>187</v>
@@ -8490,22 +8582,15 @@
       <c r="H33" s="9">
         <v>110</v>
       </c>
-      <c r="I33" s="6">
-        <f>1/9</f>
-        <v>0.1111111111111111</v>
+      <c r="I33" s="7">
+        <v>0.2</v>
       </c>
       <c r="J33" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>missing_age_1</v>
-      </c>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
-      <c r="P33" s="6"/>
-      <c r="S33" t="s">
-        <v>287</v>
+        <f t="shared" si="0"/>
+        <v>10-50+.all</v>
+      </c>
+      <c r="T33" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
@@ -8516,68 +8601,92 @@
         <v>406</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>210</v>
+        <v>187</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>209</v>
       </c>
       <c r="H34" s="9">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="I34" s="7">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="J34" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;15/&gt;15.d</v>
-      </c>
-      <c r="P34" s="12" t="s">
-        <v>291</v>
+        <f t="shared" si="0"/>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
+      </c>
+      <c r="K34" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="L34" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="M34" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="N34" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="R34" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="T34" s="12" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>294</v>
+        <v>237</v>
       </c>
       <c r="B35" t="s">
-        <v>406</v>
+        <v>237</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>182</v>
+        <v>237</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>455</v>
+        <v>237</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>210</v>
+        <v>187</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>209</v>
       </c>
       <c r="H35" s="9">
-        <v>120</v>
-      </c>
-      <c r="I35" s="7">
-        <v>0.2</v>
+        <v>110</v>
+      </c>
+      <c r="I35" s="6">
+        <f>1/9</f>
+        <v>0.1111111111111111</v>
       </c>
       <c r="J35" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>10-50+.all</v>
-      </c>
-      <c r="T35" t="s">
-        <v>309</v>
+        <f t="shared" si="0"/>
+        <v>missing_age_1</v>
+      </c>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="6"/>
+      <c r="S35" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.2">
@@ -8588,13 +8697,13 @@
         <v>406</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>188</v>
@@ -8606,46 +8715,31 @@
         <v>120</v>
       </c>
       <c r="I36" s="7">
-        <v>1</v>
+        <v>0.125</v>
       </c>
       <c r="J36" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
-      </c>
-      <c r="K36" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="L36" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="M36" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="N36" s="12" t="s">
-        <v>272</v>
-      </c>
-      <c r="R36" s="12" t="s">
-        <v>396</v>
-      </c>
-      <c r="T36" s="12" t="s">
-        <v>309</v>
+        <f t="shared" si="0"/>
+        <v>&lt;15/&gt;15.d</v>
+      </c>
+      <c r="P36" s="12" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>237</v>
+        <v>294</v>
       </c>
       <c r="B37" t="s">
-        <v>237</v>
+        <v>406</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>237</v>
+        <v>182</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>237</v>
+        <v>455</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>188</v>
@@ -8656,22 +8750,15 @@
       <c r="H37" s="9">
         <v>120</v>
       </c>
-      <c r="I37" s="6">
-        <f>1/9</f>
-        <v>0.1111111111111111</v>
+      <c r="I37" s="7">
+        <v>0.2</v>
       </c>
       <c r="J37" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>missing_age_1</v>
-      </c>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="6"/>
-      <c r="S37" t="s">
-        <v>287</v>
+        <f t="shared" si="0"/>
+        <v>10-50+.all</v>
+      </c>
+      <c r="T37" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
@@ -8682,68 +8769,90 @@
         <v>406</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H38" s="9">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="I38" s="7">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="J38" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;15/&gt;15.d</v>
-      </c>
-      <c r="P38" s="12" t="s">
-        <v>291</v>
+        <f t="shared" si="0"/>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
+      </c>
+      <c r="K38" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="L38" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="M38" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="N38" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="R38" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="T38" s="12" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>294</v>
+        <v>237</v>
       </c>
       <c r="B39" t="s">
-        <v>406</v>
+        <v>237</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>182</v>
+        <v>237</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>455</v>
+        <v>237</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H39" s="9">
-        <v>130</v>
-      </c>
-      <c r="I39" s="7">
-        <v>0.2</v>
+        <v>120</v>
+      </c>
+      <c r="I39" s="6">
+        <f>1/9</f>
+        <v>0.1111111111111111</v>
       </c>
       <c r="J39" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>10-50+.all</v>
-      </c>
-      <c r="T39" t="s">
-        <v>309</v>
+        <f t="shared" si="0"/>
+        <v>missing_age_1</v>
+      </c>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6"/>
+      <c r="O39" s="6"/>
+      <c r="P39" s="6"/>
+      <c r="S39" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.2">
@@ -8754,13 +8863,13 @@
         <v>406</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>189</v>
@@ -8772,46 +8881,31 @@
         <v>130</v>
       </c>
       <c r="I40" s="7">
-        <v>0.5</v>
+        <v>0.125</v>
       </c>
       <c r="J40" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
-      </c>
-      <c r="K40" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="L40" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="M40" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="N40" s="12" t="s">
-        <v>272</v>
-      </c>
-      <c r="R40" s="12" t="s">
-        <v>396</v>
-      </c>
-      <c r="T40" s="12" t="s">
-        <v>309</v>
+        <f t="shared" si="0"/>
+        <v>&lt;15/&gt;15.d</v>
+      </c>
+      <c r="P40" s="12" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>237</v>
+        <v>294</v>
       </c>
       <c r="B41" t="s">
-        <v>237</v>
+        <v>406</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>237</v>
+        <v>182</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>237</v>
+        <v>455</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>189</v>
@@ -8822,22 +8916,15 @@
       <c r="H41" s="9">
         <v>130</v>
       </c>
-      <c r="I41" s="6">
-        <f>1/9</f>
-        <v>0.1111111111111111</v>
+      <c r="I41" s="7">
+        <v>0.2</v>
       </c>
       <c r="J41" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>missing_age_1</v>
-      </c>
-      <c r="K41" s="6"/>
-      <c r="L41" s="6"/>
-      <c r="M41" s="6"/>
-      <c r="N41" s="6"/>
-      <c r="O41" s="6"/>
-      <c r="P41" s="6"/>
-      <c r="S41" t="s">
-        <v>287</v>
+        <f t="shared" si="0"/>
+        <v>10-50+.all</v>
+      </c>
+      <c r="T41" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.2">
@@ -8848,68 +8935,90 @@
         <v>406</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H42" s="9">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="I42" s="7">
-        <v>0.125</v>
+        <v>0.5</v>
       </c>
       <c r="J42" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;15/&gt;15.d</v>
-      </c>
-      <c r="P42" s="12" t="s">
-        <v>291</v>
+        <f t="shared" si="0"/>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
+      </c>
+      <c r="K42" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="L42" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="M42" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="N42" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="R42" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="T42" s="12" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>294</v>
+        <v>237</v>
       </c>
       <c r="B43" t="s">
-        <v>406</v>
+        <v>237</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>182</v>
+        <v>237</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>455</v>
+        <v>237</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H43" s="9">
-        <v>140</v>
-      </c>
-      <c r="I43" s="7">
-        <v>0.2</v>
+        <v>130</v>
+      </c>
+      <c r="I43" s="6">
+        <f>1/9</f>
+        <v>0.1111111111111111</v>
       </c>
       <c r="J43" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>10-50+.all</v>
-      </c>
-      <c r="T43" t="s">
-        <v>309</v>
+        <f t="shared" si="0"/>
+        <v>missing_age_1</v>
+      </c>
+      <c r="K43" s="6"/>
+      <c r="L43" s="6"/>
+      <c r="M43" s="6"/>
+      <c r="N43" s="6"/>
+      <c r="O43" s="6"/>
+      <c r="P43" s="6"/>
+      <c r="S43" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.2">
@@ -8920,13 +9029,13 @@
         <v>406</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>190</v>
@@ -8938,46 +9047,31 @@
         <v>140</v>
       </c>
       <c r="I44" s="7">
-        <v>0.5</v>
+        <v>0.125</v>
       </c>
       <c r="J44" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
-      </c>
-      <c r="K44" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="L44" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="M44" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="N44" s="12" t="s">
-        <v>272</v>
-      </c>
-      <c r="R44" s="12" t="s">
-        <v>396</v>
-      </c>
-      <c r="T44" s="12" t="s">
-        <v>309</v>
+        <f t="shared" si="0"/>
+        <v>&lt;15/&gt;15.d</v>
+      </c>
+      <c r="P44" s="12" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>237</v>
+        <v>294</v>
       </c>
       <c r="B45" t="s">
-        <v>237</v>
+        <v>406</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>237</v>
+        <v>182</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>237</v>
+        <v>455</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>190</v>
@@ -8988,22 +9082,15 @@
       <c r="H45" s="9">
         <v>140</v>
       </c>
-      <c r="I45" s="6">
-        <f>1/9</f>
-        <v>0.1111111111111111</v>
+      <c r="I45" s="7">
+        <v>0.2</v>
       </c>
       <c r="J45" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>missing_age_1</v>
-      </c>
-      <c r="K45" s="6"/>
-      <c r="L45" s="6"/>
-      <c r="M45" s="6"/>
-      <c r="N45" s="6"/>
-      <c r="O45" s="6"/>
-      <c r="P45" s="6"/>
-      <c r="S45" t="s">
-        <v>287</v>
+        <f t="shared" si="0"/>
+        <v>10-50+.all</v>
+      </c>
+      <c r="T45" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.2">
@@ -9014,100 +9101,107 @@
         <v>406</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>191</v>
+        <v>459</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="H46" s="9">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="I46" s="7">
-        <v>0.125</v>
+        <v>0.5</v>
       </c>
       <c r="J46" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;15/&gt;15.d</v>
-      </c>
-      <c r="P46" s="12" t="s">
-        <v>291</v>
+        <f t="shared" si="0"/>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
+      </c>
+      <c r="K46" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="L46" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="M46" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="N46" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="R46" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="T46" s="12" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>294</v>
+        <v>237</v>
       </c>
       <c r="B47" t="s">
-        <v>406</v>
+        <v>237</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>178</v>
+        <v>237</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>191</v>
+        <v>237</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="H47" s="9">
-        <v>150</v>
-      </c>
-      <c r="I47" s="7">
-        <v>1</v>
+        <v>140</v>
+      </c>
+      <c r="I47" s="6">
+        <f>1/9</f>
+        <v>0.1111111111111111</v>
       </c>
       <c r="J47" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
-      </c>
-      <c r="K47" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="L47" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="M47" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="N47" s="12" t="s">
-        <v>272</v>
-      </c>
-      <c r="R47" s="12" t="s">
-        <v>396</v>
-      </c>
-      <c r="T47" s="12" t="s">
-        <v>309</v>
+        <f t="shared" si="0"/>
+        <v>missing_age_1</v>
+      </c>
+      <c r="K47" s="6"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="6"/>
+      <c r="N47" s="6"/>
+      <c r="O47" s="6"/>
+      <c r="P47" s="6"/>
+      <c r="S47" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>237</v>
+        <v>294</v>
       </c>
       <c r="B48" t="s">
-        <v>237</v>
+        <v>406</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>237</v>
+        <v>179</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>385</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>237</v>
+        <v>461</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>191</v>
@@ -9118,97 +9212,100 @@
       <c r="H48" s="9">
         <v>150</v>
       </c>
-      <c r="I48" s="6">
+      <c r="I48" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="J48" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;15/&gt;15.d</v>
+      </c>
+      <c r="P48" s="12" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>294</v>
+      </c>
+      <c r="B49" t="s">
+        <v>406</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="H49" s="9">
+        <v>150</v>
+      </c>
+      <c r="I49" s="7">
+        <v>1</v>
+      </c>
+      <c r="J49" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
+      </c>
+      <c r="K49" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="L49" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="M49" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="N49" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="R49" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="T49" s="12" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>237</v>
+      </c>
+      <c r="B50" t="s">
+        <v>237</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="H50" s="9">
+        <v>150</v>
+      </c>
+      <c r="I50" s="6">
         <f>1/9</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="J48" s="6" t="str">
-        <f t="shared" si="1"/>
+      <c r="J50" s="6" t="str">
+        <f t="shared" si="0"/>
         <v>missing_age_1</v>
-      </c>
-      <c r="K48" s="6"/>
-      <c r="L48" s="6"/>
-      <c r="M48" s="6"/>
-      <c r="N48" s="6"/>
-      <c r="O48" s="6"/>
-      <c r="P48" s="6"/>
-      <c r="S48" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>295</v>
-      </c>
-      <c r="B49" t="s">
-        <v>296</v>
-      </c>
-      <c r="C49" t="s">
-        <v>218</v>
-      </c>
-      <c r="D49" t="s">
-        <v>384</v>
-      </c>
-      <c r="E49" t="s">
-        <v>217</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="G49" t="s">
-        <v>224</v>
-      </c>
-      <c r="H49" s="9">
-        <v>201</v>
-      </c>
-      <c r="I49" s="7">
-        <v>1</v>
-      </c>
-      <c r="J49" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>F;F/M;F/M/U</v>
-      </c>
-      <c r="U49" t="s">
-        <v>235</v>
-      </c>
-      <c r="V49" t="s">
-        <v>241</v>
-      </c>
-      <c r="W49" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>237</v>
-      </c>
-      <c r="B50" t="s">
-        <v>237</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="F50" t="s">
-        <v>222</v>
-      </c>
-      <c r="G50" t="s">
-        <v>224</v>
-      </c>
-      <c r="H50">
-        <v>201</v>
-      </c>
-      <c r="I50" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="J50" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>missing_sex_1</v>
       </c>
       <c r="K50" s="6"/>
       <c r="L50" s="6"/>
@@ -9217,10 +9314,10 @@
       <c r="O50" s="6"/>
       <c r="P50" s="6"/>
       <c r="S50" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.2">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>295</v>
       </c>
@@ -9228,13 +9325,13 @@
         <v>296</v>
       </c>
       <c r="C51" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D51" t="s">
         <v>384</v>
       </c>
-      <c r="E51" s="2" t="s">
-        <v>220</v>
+      <c r="E51" t="s">
+        <v>217</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>222</v>
@@ -9246,112 +9343,110 @@
         <v>201</v>
       </c>
       <c r="I51" s="7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J51" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>U;F/M/U</v>
-      </c>
-      <c r="K51" s="7"/>
-      <c r="L51" s="7"/>
-      <c r="M51" s="7"/>
-      <c r="N51" s="7"/>
-      <c r="O51" s="7"/>
-      <c r="P51" s="7"/>
+        <f t="shared" si="0"/>
+        <v>F;F/M;F/M/U</v>
+      </c>
       <c r="U51" t="s">
-        <v>271</v>
+        <v>235</v>
+      </c>
+      <c r="V51" t="s">
+        <v>241</v>
       </c>
       <c r="W51" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>237</v>
+      </c>
+      <c r="B52" t="s">
+        <v>237</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="F52" t="s">
+        <v>222</v>
+      </c>
+      <c r="G52" t="s">
+        <v>224</v>
+      </c>
+      <c r="H52">
+        <v>201</v>
+      </c>
+      <c r="I52" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="J52" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>missing_sex_1</v>
+      </c>
+      <c r="K52" s="6"/>
+      <c r="L52" s="6"/>
+      <c r="M52" s="6"/>
+      <c r="N52" s="6"/>
+      <c r="O52" s="6"/>
+      <c r="P52" s="6"/>
+      <c r="S52" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>295</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>296</v>
       </c>
-      <c r="C52" t="s">
-        <v>216</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="C53" t="s">
+        <v>219</v>
+      </c>
+      <c r="D53" t="s">
         <v>384</v>
       </c>
-      <c r="E52" t="s">
-        <v>215</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="G52" t="s">
-        <v>223</v>
-      </c>
-      <c r="H52" s="9">
-        <v>202</v>
-      </c>
-      <c r="I52" s="7">
-        <v>1</v>
-      </c>
-      <c r="J52" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>M;F/M;F/M/U</v>
-      </c>
-      <c r="S52" s="7"/>
-      <c r="T52" s="7"/>
-      <c r="U52" t="s">
-        <v>249</v>
-      </c>
-      <c r="V52" t="s">
-        <v>241</v>
-      </c>
-      <c r="W52" t="s">
+      <c r="E53" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="G53" t="s">
+        <v>224</v>
+      </c>
+      <c r="H53" s="9">
+        <v>201</v>
+      </c>
+      <c r="I53" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="J53" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>U;F/M/U</v>
+      </c>
+      <c r="K53" s="7"/>
+      <c r="L53" s="7"/>
+      <c r="M53" s="7"/>
+      <c r="N53" s="7"/>
+      <c r="O53" s="7"/>
+      <c r="P53" s="7"/>
+      <c r="U53" t="s">
+        <v>271</v>
+      </c>
+      <c r="W53" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>237</v>
-      </c>
-      <c r="B53" t="s">
-        <v>237</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="F53" t="s">
-        <v>221</v>
-      </c>
-      <c r="G53" t="s">
-        <v>223</v>
-      </c>
-      <c r="H53" s="9">
-        <v>202</v>
-      </c>
-      <c r="I53" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="J53" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>missing_sex_1</v>
-      </c>
-      <c r="K53" s="6"/>
-      <c r="L53" s="6"/>
-      <c r="M53" s="6"/>
-      <c r="N53" s="6"/>
-      <c r="O53" s="6"/>
-      <c r="P53" s="6"/>
-      <c r="S53" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>295</v>
       </c>
@@ -9359,13 +9454,13 @@
         <v>296</v>
       </c>
       <c r="C54" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D54" t="s">
         <v>384</v>
       </c>
-      <c r="E54" s="2" t="s">
-        <v>220</v>
+      <c r="E54" t="s">
+        <v>215</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>221</v>
@@ -9377,94 +9472,108 @@
         <v>202</v>
       </c>
       <c r="I54" s="7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J54" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>U;F/M/U</v>
+        <f t="shared" si="0"/>
+        <v>M;F/M;F/M/U</v>
       </c>
       <c r="S54" s="7"/>
       <c r="T54" s="7"/>
       <c r="U54" t="s">
-        <v>271</v>
+        <v>249</v>
+      </c>
+      <c r="V54" t="s">
+        <v>241</v>
       </c>
       <c r="W54" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="55" spans="1:24" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>310</v>
-      </c>
-      <c r="B55" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="C55" t="s">
-        <v>315</v>
+        <v>237</v>
+      </c>
+      <c r="B55" t="s">
+        <v>237</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="E55" t="s">
-        <v>316</v>
+        <v>384</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="F55" t="s">
-        <v>316</v>
+        <v>221</v>
       </c>
       <c r="G55" t="s">
-        <v>315</v>
-      </c>
-      <c r="H55">
-        <v>300</v>
-      </c>
-      <c r="I55" s="7">
-        <v>1</v>
+        <v>223</v>
+      </c>
+      <c r="H55" s="9">
+        <v>202</v>
+      </c>
+      <c r="I55" s="6">
+        <v>0.5</v>
       </c>
       <c r="J55" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>kp1</v>
-      </c>
-      <c r="X55" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="56" spans="1:24" ht="18" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>missing_sex_1</v>
+      </c>
+      <c r="K55" s="6"/>
+      <c r="L55" s="6"/>
+      <c r="M55" s="6"/>
+      <c r="N55" s="6"/>
+      <c r="O55" s="6"/>
+      <c r="P55" s="6"/>
+      <c r="S55" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>310</v>
-      </c>
-      <c r="B56" s="14" t="s">
-        <v>320</v>
+        <v>295</v>
+      </c>
+      <c r="B56" t="s">
+        <v>296</v>
       </c>
       <c r="C56" t="s">
-        <v>313</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="E56" t="s">
-        <v>314</v>
-      </c>
-      <c r="F56" t="s">
-        <v>314</v>
+        <v>219</v>
+      </c>
+      <c r="D56" t="s">
+        <v>384</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>221</v>
       </c>
       <c r="G56" t="s">
-        <v>313</v>
-      </c>
-      <c r="H56">
-        <v>310</v>
+        <v>223</v>
+      </c>
+      <c r="H56" s="9">
+        <v>202</v>
       </c>
       <c r="I56" s="7">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J56" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>kp1</v>
-      </c>
-      <c r="X56" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="57" spans="1:24" ht="18" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>U;F/M/U</v>
+      </c>
+      <c r="S56" s="7"/>
+      <c r="T56" s="7"/>
+      <c r="U56" t="s">
+        <v>271</v>
+      </c>
+      <c r="W56" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="57" spans="1:28" ht="18" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>310</v>
       </c>
@@ -9472,35 +9581,35 @@
         <v>320</v>
       </c>
       <c r="C57" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>386</v>
       </c>
       <c r="E57" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F57" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G57" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="H57">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="I57" s="7">
         <v>1</v>
       </c>
       <c r="J57" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>kp1</v>
       </c>
       <c r="X57" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="58" spans="1:24" ht="18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" ht="18" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>310</v>
       </c>
@@ -9508,35 +9617,35 @@
         <v>320</v>
       </c>
       <c r="C58" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>386</v>
       </c>
       <c r="E58" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="F58" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="G58" t="s">
-        <v>311</v>
-      </c>
-      <c r="H58" s="9">
-        <v>330</v>
+        <v>313</v>
+      </c>
+      <c r="H58">
+        <v>310</v>
       </c>
       <c r="I58" s="7">
         <v>1</v>
       </c>
       <c r="J58" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>kp1</v>
       </c>
       <c r="X58" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="59" spans="1:24" ht="18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" ht="18" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>310</v>
       </c>
@@ -9544,37 +9653,289 @@
         <v>320</v>
       </c>
       <c r="C59" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>386</v>
       </c>
       <c r="E59" t="s">
-        <v>382</v>
+        <v>319</v>
       </c>
       <c r="F59" t="s">
-        <v>382</v>
+        <v>319</v>
       </c>
       <c r="G59" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="H59">
-        <v>340</v>
+        <v>320</v>
       </c>
       <c r="I59" s="7">
         <v>1</v>
       </c>
       <c r="J59" s="6" t="str">
-        <f t="shared" ref="J59" si="2">_xlfn.TEXTJOIN(";",1,K59,L59,M59,N59,O59,P59,Q59,S59,T59,U59,V59,W59,R59,X59)</f>
+        <f t="shared" si="0"/>
         <v>kp1</v>
       </c>
       <c r="X59" t="s">
         <v>321</v>
       </c>
     </row>
+    <row r="60" spans="1:28" ht="18" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>310</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="C60" t="s">
+        <v>311</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="E60" t="s">
+        <v>312</v>
+      </c>
+      <c r="F60" t="s">
+        <v>312</v>
+      </c>
+      <c r="G60" t="s">
+        <v>311</v>
+      </c>
+      <c r="H60" s="9">
+        <v>330</v>
+      </c>
+      <c r="I60" s="7">
+        <v>1</v>
+      </c>
+      <c r="J60" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>kp1</v>
+      </c>
+      <c r="X60" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="61" spans="1:28" ht="18" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>310</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="C61" t="s">
+        <v>317</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="E61" t="s">
+        <v>382</v>
+      </c>
+      <c r="F61" t="s">
+        <v>382</v>
+      </c>
+      <c r="G61" t="s">
+        <v>317</v>
+      </c>
+      <c r="H61">
+        <v>340</v>
+      </c>
+      <c r="I61" s="7">
+        <v>1</v>
+      </c>
+      <c r="J61" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>kp1</v>
+      </c>
+      <c r="X61" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="62" spans="1:28" ht="18" x14ac:dyDescent="0.25">
+      <c r="A62" s="16" t="s">
+        <v>322</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>323</v>
+      </c>
+      <c r="C62" s="16" t="s">
+        <v>324</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="E62" s="16" t="s">
+        <v>325</v>
+      </c>
+      <c r="F62" s="16" t="s">
+        <v>325</v>
+      </c>
+      <c r="G62" s="16" t="s">
+        <v>324</v>
+      </c>
+      <c r="H62">
+        <v>10</v>
+      </c>
+      <c r="I62" s="7">
+        <v>1</v>
+      </c>
+      <c r="J62" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>tr</v>
+      </c>
+      <c r="Y62" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="63" spans="1:28" ht="18" x14ac:dyDescent="0.25">
+      <c r="A63" s="16" t="s">
+        <v>322</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>323</v>
+      </c>
+      <c r="C63" s="16" t="s">
+        <v>326</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="E63" s="16" t="s">
+        <v>327</v>
+      </c>
+      <c r="F63" s="16" t="s">
+        <v>327</v>
+      </c>
+      <c r="G63" s="16" t="s">
+        <v>326</v>
+      </c>
+      <c r="H63">
+        <v>20</v>
+      </c>
+      <c r="I63" s="7">
+        <v>1</v>
+      </c>
+      <c r="J63" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>tr</v>
+      </c>
+      <c r="Y63" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="64" spans="1:28" ht="19" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>476</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>477</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>480</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="E64" s="14" t="s">
+        <v>479</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="H64">
+        <v>10</v>
+      </c>
+      <c r="I64" s="7">
+        <v>1</v>
+      </c>
+      <c r="J64" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>KnownNewResult</v>
+      </c>
+      <c r="AB64" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="65" spans="1:28" ht="19" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>476</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>477</v>
+      </c>
+      <c r="C65" s="16" t="s">
+        <v>482</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="E65" s="14" t="s">
+        <v>481</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="H65">
+        <v>20</v>
+      </c>
+      <c r="I65" s="7">
+        <v>1</v>
+      </c>
+      <c r="J65" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>KnownNewResult</v>
+      </c>
+      <c r="AB65" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="66" spans="1:28" ht="19" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>476</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>477</v>
+      </c>
+      <c r="C66" s="16" t="s">
+        <v>484</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="E66" s="16" t="s">
+        <v>483</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="H66">
+        <v>30</v>
+      </c>
+      <c r="I66" s="7">
+        <v>1</v>
+      </c>
+      <c r="J66" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>KnownNewResult</v>
+      </c>
+      <c r="AB66" t="s">
+        <v>475</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:W59">
-    <sortCondition ref="H2:H59"/>
+  <sortState ref="A4:W61">
+    <sortCondition ref="H4:H61"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding Gend_gbv violence type items to dim_item_sets
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565E0185-E1E1-9F41-B047-597502952F3F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C776C5D-5B92-B249-8D96-C192361B9991}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="700" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2251" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2268" uniqueCount="502">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1510,13 +1510,46 @@
   </si>
   <si>
     <t>Vr59uUJBySG</t>
+  </si>
+  <si>
+    <t>co</t>
+  </si>
+  <si>
+    <t>categoryOptionCombo</t>
+  </si>
+  <si>
+    <t>Cieg8r0FOGJ</t>
+  </si>
+  <si>
+    <t>rslp7ddiBzy</t>
+  </si>
+  <si>
+    <t>vt</t>
+  </si>
+  <si>
+    <t>Sexual Violence (Post-Rape Care)</t>
+  </si>
+  <si>
+    <t>bchuAJAMSZO</t>
+  </si>
+  <si>
+    <t>vt_sv</t>
+  </si>
+  <si>
+    <t>vt_pe</t>
+  </si>
+  <si>
+    <t>Physical and/or Emotional Violence</t>
+  </si>
+  <si>
+    <t>USe0kg2Bind</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1562,6 +1595,12 @@
       <name val="Courier New"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1583,7 +1622,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1605,6 +1644,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1921,10 +1961,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
   <dimension ref="A1:Z56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="P51" sqref="P51"/>
+      <selection pane="bottomLeft" activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7186,10 +7226,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
-  <dimension ref="A1:AB66"/>
+  <dimension ref="A1:AC68"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64:F66"/>
+    <sheetView tabSelected="1" topLeftCell="B55" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7199,7 +7239,7 @@
     <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.83203125" customWidth="1"/>
     <col min="5" max="5" width="52.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="41.83203125" customWidth="1"/>
     <col min="11" max="13" width="12.33203125" customWidth="1"/>
@@ -7207,7 +7247,7 @@
     <col min="19" max="19" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>389</v>
       </c>
@@ -7292,8 +7332,11 @@
       <c r="AB1" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" ht="18" x14ac:dyDescent="0.2">
+      <c r="AC1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>294</v>
       </c>
@@ -7322,7 +7365,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K2,L2,M2,N2,O2,P2,Q2,S2,T2,U2,V2,W2,R2,X2,Y2,Z2,AA2,AB2)</f>
+        <f>_xlfn.TEXTJOIN(";",1,K2,L2,M2,N2,O2,P2,Q2,S2,T2,U2,V2,W2,R2,X2,Y2,Z2,AA2,AB2,AC2)</f>
         <v>&lt;2mo</v>
       </c>
       <c r="K2" s="12"/>
@@ -7337,7 +7380,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>294</v>
       </c>
@@ -7366,7 +7409,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="6" t="str">
-        <f t="shared" ref="J3:J66" si="0">_xlfn.TEXTJOIN(";",1,K3,L3,M3,N3,O3,P3,Q3,S3,T3,U3,V3,W3,R3,X3,Y3,Z3,AA3,AB3)</f>
+        <f t="shared" ref="J3:J66" si="0">_xlfn.TEXTJOIN(";",1,K3,L3,M3,N3,O3,P3,Q3,S3,T3,U3,V3,W3,R3,X3,Y3,Z3,AA3,AB3,AC3)</f>
         <v>2-12mo</v>
       </c>
       <c r="K3" s="12"/>
@@ -7381,7 +7424,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>294</v>
       </c>
@@ -7423,7 +7466,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>294</v>
       </c>
@@ -7460,7 +7503,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>294</v>
       </c>
@@ -7493,7 +7536,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>294</v>
       </c>
@@ -7543,7 +7586,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>294</v>
       </c>
@@ -7579,7 +7622,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>294</v>
       </c>
@@ -7618,7 +7661,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>294</v>
       </c>
@@ -7665,7 +7708,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>294</v>
       </c>
@@ -7701,7 +7744,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>294</v>
       </c>
@@ -7753,7 +7796,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>294</v>
       </c>
@@ -7789,7 +7832,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>237</v>
       </c>
@@ -7832,7 +7875,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>294</v>
       </c>
@@ -7868,7 +7911,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>237</v>
       </c>
@@ -9861,7 +9904,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="65" spans="1:28" ht="19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:29" ht="19" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>476</v>
       </c>
@@ -9897,7 +9940,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="66" spans="1:28" ht="19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:29" ht="19" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>476</v>
       </c>
@@ -9931,6 +9974,78 @@
       </c>
       <c r="AB66" t="s">
         <v>475</v>
+      </c>
+    </row>
+    <row r="67" spans="1:29" ht="18" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>491</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>492</v>
+      </c>
+      <c r="C67" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="E67" s="16" t="s">
+        <v>496</v>
+      </c>
+      <c r="F67" s="16" t="s">
+        <v>496</v>
+      </c>
+      <c r="G67" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="H67">
+        <v>1</v>
+      </c>
+      <c r="I67" s="7">
+        <v>1</v>
+      </c>
+      <c r="J67" s="6" t="str">
+        <f t="shared" ref="J67:J68" si="1">_xlfn.TEXTJOIN(";",1,K67,L67,M67,N67,O67,P67,Q67,S67,T67,U67,V67,W67,R67,X67,Y67,Z67,AA67,AB67,AC67)</f>
+        <v>vt_sv</v>
+      </c>
+      <c r="AC67" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="68" spans="1:29" ht="18" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>491</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>492</v>
+      </c>
+      <c r="C68" s="17" t="s">
+        <v>494</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="E68" s="16" t="s">
+        <v>500</v>
+      </c>
+      <c r="F68" s="16" t="s">
+        <v>500</v>
+      </c>
+      <c r="G68" s="16" t="s">
+        <v>501</v>
+      </c>
+      <c r="H68">
+        <v>2</v>
+      </c>
+      <c r="I68" s="7">
+        <v>1</v>
+      </c>
+      <c r="J68" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>vt_pe</v>
+      </c>
+      <c r="AC68" t="s">
+        <v>499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating the model sets column formula in model_calculation.xls
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C776C5D-5B92-B249-8D96-C192361B9991}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40839DCE-5C30-C54A-A712-D9B66C7814ED}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -1473,9 +1473,6 @@
     <t>HIV Test Status (Specific)</t>
   </si>
   <si>
-    <t>ts</t>
-  </si>
-  <si>
     <t>Newly Identified Positive (Specific)</t>
   </si>
   <si>
@@ -1543,6 +1540,9 @@
   </si>
   <si>
     <t>USe0kg2Bind</t>
+  </si>
+  <si>
+    <t>tss</t>
   </si>
 </sst>
 </file>
@@ -7228,8 +7228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
   <dimension ref="A1:AC68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B55" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7333,7 +7333,7 @@
         <v>475</v>
       </c>
       <c r="AC1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="18" x14ac:dyDescent="0.2">
@@ -7365,7 +7365,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K2,L2,M2,N2,O2,P2,Q2,S2,T2,U2,V2,W2,R2,X2,Y2,Z2,AA2,AB2,AC2)</f>
+        <f>_xlfn.TEXTJOIN(";",1,K2:ZZ2)</f>
         <v>&lt;2mo</v>
       </c>
       <c r="K2" s="12"/>
@@ -7409,7 +7409,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="6" t="str">
-        <f t="shared" ref="J3:J66" si="0">_xlfn.TEXTJOIN(";",1,K3,L3,M3,N3,O3,P3,Q3,S3,T3,U3,V3,W3,R3,X3,Y3,Z3,AA3,AB3,AC3)</f>
+        <f>_xlfn.TEXTJOIN(";",1,K3:ZZ3)</f>
         <v>2-12mo</v>
       </c>
       <c r="K3" s="12"/>
@@ -7453,7 +7453,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K4:ZZ4)</f>
         <v>&lt;1-50+;&lt;1-18+</v>
       </c>
       <c r="K4" s="12" t="s">
@@ -7495,7 +7495,7 @@
         <v>0.25</v>
       </c>
       <c r="J5" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K5:ZZ5)</f>
         <v>&lt;15/&gt;15.d</v>
       </c>
       <c r="O5" s="12"/>
@@ -7532,7 +7532,7 @@
         <v>0.2</v>
       </c>
       <c r="J6" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K6:ZZ6)</f>
         <v/>
       </c>
     </row>
@@ -7565,7 +7565,7 @@
         <v>0.5</v>
       </c>
       <c r="J7" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K7:ZZ7)</f>
         <v>&lt;1-50+;1-50+;&lt;1-18+;1-4;1-50+/&lt;5</v>
       </c>
       <c r="K7" s="12" t="s">
@@ -7615,7 +7615,7 @@
         <v>0.25</v>
       </c>
       <c r="J8" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K8:ZZ8)</f>
         <v>&lt;15/&gt;15.d</v>
       </c>
       <c r="P8" s="12" t="s">
@@ -7651,7 +7651,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K9:ZZ9)</f>
         <v>1-4;1-50+/&lt;5</v>
       </c>
       <c r="Q9" s="12" t="s">
@@ -7690,7 +7690,7 @@
         <v>0.5</v>
       </c>
       <c r="J10" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K10:ZZ10)</f>
         <v>&lt;1-50+;1-50+;&lt;1-18+;1-50+/&lt;5</v>
       </c>
       <c r="K10" s="12" t="s">
@@ -7737,7 +7737,7 @@
         <v>0.25</v>
       </c>
       <c r="J11" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K11:ZZ11)</f>
         <v>&lt;15/&gt;15.d</v>
       </c>
       <c r="P11" s="12" t="s">
@@ -7773,8 +7773,8 @@
         <v>1</v>
       </c>
       <c r="J12" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;10-50+;&lt;1-18+;10-50+.all;1-50+/&lt;5</v>
+        <f>_xlfn.TEXTJOIN(";",1,K12:ZZ12)</f>
+        <v>&lt;1-50+;1-50+;10-50+;&lt;1-18+;1-50+/&lt;5;10-50+.all</v>
       </c>
       <c r="K12" s="12" t="s">
         <v>250</v>
@@ -7825,7 +7825,7 @@
         <v>0.25</v>
       </c>
       <c r="J13" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K13:ZZ13)</f>
         <v>&lt;15/&gt;15.d</v>
       </c>
       <c r="P13" s="12" t="s">
@@ -7862,7 +7862,7 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="J14" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K14:ZZ14)</f>
         <v>missing_age_1</v>
       </c>
       <c r="K14" s="6"/>
@@ -7904,7 +7904,7 @@
         <v>1</v>
       </c>
       <c r="J15" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K15:ZZ15)</f>
         <v/>
       </c>
       <c r="P15" s="12"/>
@@ -7940,7 +7940,7 @@
         <v>0.5</v>
       </c>
       <c r="J16" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K16:ZZ16)</f>
         <v>missing_age_2</v>
       </c>
       <c r="S16" t="s">
@@ -7976,7 +7976,7 @@
         <v>1</v>
       </c>
       <c r="J17" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K17:ZZ17)</f>
         <v>&lt;1-18+</v>
       </c>
       <c r="O17" t="s">
@@ -8012,7 +8012,7 @@
         <v>0.125</v>
       </c>
       <c r="J18" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K18:ZZ18)</f>
         <v>&lt;15/&gt;15.d</v>
       </c>
       <c r="P18" s="12" t="s">
@@ -8048,8 +8048,8 @@
         <v>1</v>
       </c>
       <c r="J19" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
+        <f>_xlfn.TEXTJOIN(";",1,K19:ZZ19)</f>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all</v>
       </c>
       <c r="K19" s="12" t="s">
         <v>250</v>
@@ -8100,7 +8100,7 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="J20" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K20:ZZ20)</f>
         <v>missing_age_1</v>
       </c>
       <c r="K20" s="6"/>
@@ -8142,7 +8142,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K21:ZZ21)</f>
         <v/>
       </c>
       <c r="P21" s="13"/>
@@ -8176,7 +8176,7 @@
         <v>0.5</v>
       </c>
       <c r="J22" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K22:ZZ22)</f>
         <v>missing_age_2</v>
       </c>
       <c r="K22" s="6"/>
@@ -8218,7 +8218,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K23:ZZ23)</f>
         <v>&lt;1-18+</v>
       </c>
       <c r="K23" s="7"/>
@@ -8259,7 +8259,7 @@
         <v>0.125</v>
       </c>
       <c r="J24" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K24:ZZ24)</f>
         <v>&lt;15/&gt;15.d</v>
       </c>
       <c r="P24" s="12" t="s">
@@ -8295,8 +8295,8 @@
         <v>1</v>
       </c>
       <c r="J25" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
+        <f>_xlfn.TEXTJOIN(";",1,K25:ZZ25)</f>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all</v>
       </c>
       <c r="K25" s="12" t="s">
         <v>250</v>
@@ -8347,7 +8347,7 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="J26" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K26:ZZ26)</f>
         <v>missing_age_1</v>
       </c>
       <c r="K26" s="6"/>
@@ -8389,7 +8389,7 @@
         <v>0.125</v>
       </c>
       <c r="J27" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K27:ZZ27)</f>
         <v>&lt;15/&gt;15.d</v>
       </c>
       <c r="P27" s="12" t="s">
@@ -8425,8 +8425,8 @@
         <v>1</v>
       </c>
       <c r="J28" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
+        <f>_xlfn.TEXTJOIN(";",1,K28:ZZ28)</f>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all</v>
       </c>
       <c r="K28" s="12" t="s">
         <v>250</v>
@@ -8478,7 +8478,7 @@
         <v>0.2</v>
       </c>
       <c r="J29" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K29:ZZ29)</f>
         <v>10-50+.all</v>
       </c>
       <c r="T29" t="s">
@@ -8515,7 +8515,7 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="J30" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K30:ZZ30)</f>
         <v>missing_age_1</v>
       </c>
       <c r="K30" s="6"/>
@@ -8557,7 +8557,7 @@
         <v>1</v>
       </c>
       <c r="J31" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K31:ZZ31)</f>
         <v>&lt;1-18+</v>
       </c>
       <c r="O31" t="s">
@@ -8593,7 +8593,7 @@
         <v>0.125</v>
       </c>
       <c r="J32" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K32:ZZ32)</f>
         <v>&lt;15/&gt;15.d</v>
       </c>
       <c r="P32" s="12" t="s">
@@ -8629,7 +8629,7 @@
         <v>0.2</v>
       </c>
       <c r="J33" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K33:ZZ33)</f>
         <v>10-50+.all</v>
       </c>
       <c r="T33" t="s">
@@ -8665,8 +8665,8 @@
         <v>1</v>
       </c>
       <c r="J34" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
+        <f>_xlfn.TEXTJOIN(";",1,K34:ZZ34)</f>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all</v>
       </c>
       <c r="K34" s="12" t="s">
         <v>250</v>
@@ -8719,7 +8719,7 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="J35" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K35:ZZ35)</f>
         <v>missing_age_1</v>
       </c>
       <c r="K35" s="6"/>
@@ -8761,7 +8761,7 @@
         <v>0.125</v>
       </c>
       <c r="J36" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K36:ZZ36)</f>
         <v>&lt;15/&gt;15.d</v>
       </c>
       <c r="P36" s="12" t="s">
@@ -8797,7 +8797,7 @@
         <v>0.2</v>
       </c>
       <c r="J37" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K37:ZZ37)</f>
         <v>10-50+.all</v>
       </c>
       <c r="T37" t="s">
@@ -8833,8 +8833,8 @@
         <v>1</v>
       </c>
       <c r="J38" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
+        <f>_xlfn.TEXTJOIN(";",1,K38:ZZ38)</f>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all</v>
       </c>
       <c r="K38" s="12" t="s">
         <v>250</v>
@@ -8885,7 +8885,7 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="J39" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K39:ZZ39)</f>
         <v>missing_age_1</v>
       </c>
       <c r="K39" s="6"/>
@@ -8927,7 +8927,7 @@
         <v>0.125</v>
       </c>
       <c r="J40" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K40:ZZ40)</f>
         <v>&lt;15/&gt;15.d</v>
       </c>
       <c r="P40" s="12" t="s">
@@ -8963,7 +8963,7 @@
         <v>0.2</v>
       </c>
       <c r="J41" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K41:ZZ41)</f>
         <v>10-50+.all</v>
       </c>
       <c r="T41" t="s">
@@ -8999,8 +8999,8 @@
         <v>0.5</v>
       </c>
       <c r="J42" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
+        <f>_xlfn.TEXTJOIN(";",1,K42:ZZ42)</f>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all</v>
       </c>
       <c r="K42" s="12" t="s">
         <v>250</v>
@@ -9051,7 +9051,7 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="J43" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K43:ZZ43)</f>
         <v>missing_age_1</v>
       </c>
       <c r="K43" s="6"/>
@@ -9093,7 +9093,7 @@
         <v>0.125</v>
       </c>
       <c r="J44" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K44:ZZ44)</f>
         <v>&lt;15/&gt;15.d</v>
       </c>
       <c r="P44" s="12" t="s">
@@ -9129,7 +9129,7 @@
         <v>0.2</v>
       </c>
       <c r="J45" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K45:ZZ45)</f>
         <v>10-50+.all</v>
       </c>
       <c r="T45" t="s">
@@ -9165,8 +9165,8 @@
         <v>0.5</v>
       </c>
       <c r="J46" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
+        <f>_xlfn.TEXTJOIN(";",1,K46:ZZ46)</f>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all</v>
       </c>
       <c r="K46" s="12" t="s">
         <v>250</v>
@@ -9217,7 +9217,7 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="J47" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K47:ZZ47)</f>
         <v>missing_age_1</v>
       </c>
       <c r="K47" s="6"/>
@@ -9259,7 +9259,7 @@
         <v>0.125</v>
       </c>
       <c r="J48" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K48:ZZ48)</f>
         <v>&lt;15/&gt;15.d</v>
       </c>
       <c r="P48" s="12" t="s">
@@ -9295,8 +9295,8 @@
         <v>1</v>
       </c>
       <c r="J49" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;10-50+.all;1-50+/&lt;5</v>
+        <f>_xlfn.TEXTJOIN(";",1,K49:ZZ49)</f>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all</v>
       </c>
       <c r="K49" s="12" t="s">
         <v>250</v>
@@ -9347,7 +9347,7 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="J50" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K50:ZZ50)</f>
         <v>missing_age_1</v>
       </c>
       <c r="K50" s="6"/>
@@ -9389,7 +9389,7 @@
         <v>1</v>
       </c>
       <c r="J51" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K51:ZZ51)</f>
         <v>F;F/M;F/M/U</v>
       </c>
       <c r="U51" t="s">
@@ -9431,7 +9431,7 @@
         <v>0.5</v>
       </c>
       <c r="J52" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K52:ZZ52)</f>
         <v>missing_sex_1</v>
       </c>
       <c r="K52" s="6"/>
@@ -9473,7 +9473,7 @@
         <v>0.5</v>
       </c>
       <c r="J53" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K53:ZZ53)</f>
         <v>U;F/M/U</v>
       </c>
       <c r="K53" s="7"/>
@@ -9518,7 +9518,7 @@
         <v>1</v>
       </c>
       <c r="J54" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K54:ZZ54)</f>
         <v>M;F/M;F/M/U</v>
       </c>
       <c r="S54" s="7"/>
@@ -9562,7 +9562,7 @@
         <v>0.5</v>
       </c>
       <c r="J55" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K55:ZZ55)</f>
         <v>missing_sex_1</v>
       </c>
       <c r="K55" s="6"/>
@@ -9604,7 +9604,7 @@
         <v>0.5</v>
       </c>
       <c r="J56" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K56:ZZ56)</f>
         <v>U;F/M/U</v>
       </c>
       <c r="S56" s="7"/>
@@ -9645,7 +9645,7 @@
         <v>1</v>
       </c>
       <c r="J57" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K57:ZZ57)</f>
         <v>kp1</v>
       </c>
       <c r="X57" t="s">
@@ -9681,7 +9681,7 @@
         <v>1</v>
       </c>
       <c r="J58" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K58:ZZ58)</f>
         <v>kp1</v>
       </c>
       <c r="X58" t="s">
@@ -9717,7 +9717,7 @@
         <v>1</v>
       </c>
       <c r="J59" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K59:ZZ59)</f>
         <v>kp1</v>
       </c>
       <c r="X59" t="s">
@@ -9753,7 +9753,7 @@
         <v>1</v>
       </c>
       <c r="J60" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K60:ZZ60)</f>
         <v>kp1</v>
       </c>
       <c r="X60" t="s">
@@ -9789,7 +9789,7 @@
         <v>1</v>
       </c>
       <c r="J61" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K61:ZZ61)</f>
         <v>kp1</v>
       </c>
       <c r="X61" t="s">
@@ -9825,7 +9825,7 @@
         <v>1</v>
       </c>
       <c r="J62" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K62:ZZ62)</f>
         <v>tr</v>
       </c>
       <c r="Y62" t="s">
@@ -9861,7 +9861,7 @@
         <v>1</v>
       </c>
       <c r="J63" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K63:ZZ63)</f>
         <v>tr</v>
       </c>
       <c r="Y63" t="s">
@@ -9876,19 +9876,19 @@
         <v>477</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D64" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="E64" s="14" t="s">
         <v>478</v>
       </c>
-      <c r="E64" s="14" t="s">
-        <v>479</v>
-      </c>
       <c r="F64" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="G64" s="1" t="s">
         <v>489</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>490</v>
       </c>
       <c r="H64">
         <v>10</v>
@@ -9897,7 +9897,7 @@
         <v>1</v>
       </c>
       <c r="J64" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K64:ZZ64)</f>
         <v>KnownNewResult</v>
       </c>
       <c r="AB64" t="s">
@@ -9912,19 +9912,19 @@
         <v>477</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>478</v>
+        <v>501</v>
       </c>
       <c r="E65" s="14" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F65" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="G65" s="1" t="s">
         <v>485</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>486</v>
       </c>
       <c r="H65">
         <v>20</v>
@@ -9933,7 +9933,7 @@
         <v>1</v>
       </c>
       <c r="J65" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K65:ZZ65)</f>
         <v>KnownNewResult</v>
       </c>
       <c r="AB65" t="s">
@@ -9948,19 +9948,19 @@
         <v>477</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>478</v>
+        <v>501</v>
       </c>
       <c r="E66" s="16" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F66" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="G66" s="1" t="s">
         <v>487</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>488</v>
       </c>
       <c r="H66">
         <v>30</v>
@@ -9969,7 +9969,7 @@
         <v>1</v>
       </c>
       <c r="J66" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN(";",1,K66:ZZ66)</f>
         <v>KnownNewResult</v>
       </c>
       <c r="AB66" t="s">
@@ -9978,25 +9978,25 @@
     </row>
     <row r="67" spans="1:29" ht="18" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>490</v>
+      </c>
+      <c r="B67" s="16" t="s">
         <v>491</v>
       </c>
-      <c r="B67" s="16" t="s">
+      <c r="C67" s="17" t="s">
         <v>492</v>
       </c>
-      <c r="C67" s="17" t="s">
-        <v>493</v>
-      </c>
       <c r="D67" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="E67" s="16" t="s">
         <v>495</v>
       </c>
-      <c r="E67" s="16" t="s">
+      <c r="F67" s="16" t="s">
+        <v>495</v>
+      </c>
+      <c r="G67" s="16" t="s">
         <v>496</v>
-      </c>
-      <c r="F67" s="16" t="s">
-        <v>496</v>
-      </c>
-      <c r="G67" s="16" t="s">
-        <v>497</v>
       </c>
       <c r="H67">
         <v>1</v>
@@ -10005,34 +10005,34 @@
         <v>1</v>
       </c>
       <c r="J67" s="6" t="str">
-        <f t="shared" ref="J67:J68" si="1">_xlfn.TEXTJOIN(";",1,K67,L67,M67,N67,O67,P67,Q67,S67,T67,U67,V67,W67,R67,X67,Y67,Z67,AA67,AB67,AC67)</f>
+        <f>_xlfn.TEXTJOIN(";",1,K67:ZZ67)</f>
         <v>vt_sv</v>
       </c>
       <c r="AC67" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="68" spans="1:29" ht="18" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>490</v>
+      </c>
+      <c r="B68" s="16" t="s">
         <v>491</v>
       </c>
-      <c r="B68" s="16" t="s">
-        <v>492</v>
-      </c>
       <c r="C68" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="D68" s="2" t="s">
-        <v>495</v>
-      </c>
       <c r="E68" s="16" t="s">
+        <v>499</v>
+      </c>
+      <c r="F68" s="16" t="s">
+        <v>499</v>
+      </c>
+      <c r="G68" s="16" t="s">
         <v>500</v>
-      </c>
-      <c r="F68" s="16" t="s">
-        <v>500</v>
-      </c>
-      <c r="G68" s="16" t="s">
-        <v>501</v>
       </c>
       <c r="H68">
         <v>2</v>
@@ -10041,11 +10041,11 @@
         <v>1</v>
       </c>
       <c r="J68" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.TEXTJOIN(";",1,K68:ZZ68)</f>
         <v>vt_pe</v>
       </c>
       <c r="AC68" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding self test category options to dim_item_setsconfig file
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40839DCE-5C30-C54A-A712-D9B66C7814ED}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FAA734-A332-774C-856F-F645BCA1A88E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="33600" yWindow="0" windowWidth="25600" windowHeight="20480" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2268" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2525" uniqueCount="573">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1543,6 +1543,219 @@
   </si>
   <si>
     <t>tss</t>
+  </si>
+  <si>
+    <t>st</t>
+  </si>
+  <si>
+    <t>st_da</t>
+  </si>
+  <si>
+    <t>10-14, Female, Directly-Assisted</t>
+  </si>
+  <si>
+    <t>10-14, Male, Directly-Assisted</t>
+  </si>
+  <si>
+    <t>15-19, Female, Directly-Assisted</t>
+  </si>
+  <si>
+    <t>15-19, Male, Directly-Assisted</t>
+  </si>
+  <si>
+    <t>20-24, Female, Directly-Assisted</t>
+  </si>
+  <si>
+    <t>20-24, Male, Directly-Assisted</t>
+  </si>
+  <si>
+    <t>25-29, Female, Directly-Assisted</t>
+  </si>
+  <si>
+    <t>25-29, Male, Directly-Assisted</t>
+  </si>
+  <si>
+    <t>30-34, Female, Directly-Assisted</t>
+  </si>
+  <si>
+    <t>30-34, Male, Directly-Assisted</t>
+  </si>
+  <si>
+    <t>35-39, Female, Directly-Assisted</t>
+  </si>
+  <si>
+    <t>35-39, Male, Directly-Assisted</t>
+  </si>
+  <si>
+    <t>40-49, Female, Directly-Assisted</t>
+  </si>
+  <si>
+    <t>40-49, Male, Directly-Assisted</t>
+  </si>
+  <si>
+    <t>50+, Female, Directly-Assisted</t>
+  </si>
+  <si>
+    <t>50+, Male, Directly-Assisted</t>
+  </si>
+  <si>
+    <t>Nq3ChI5JgmB</t>
+  </si>
+  <si>
+    <t>UPG88XPoXm1</t>
+  </si>
+  <si>
+    <t>KvFHnxsxCYn</t>
+  </si>
+  <si>
+    <t>bKEwJc0xRjD</t>
+  </si>
+  <si>
+    <t>UW4vGFjkLpN</t>
+  </si>
+  <si>
+    <t>C25DdizGeAJ</t>
+  </si>
+  <si>
+    <t>e1cM3liTE75</t>
+  </si>
+  <si>
+    <t>adx4qKyxtQw</t>
+  </si>
+  <si>
+    <t>JtKhIdUeRSG</t>
+  </si>
+  <si>
+    <t>wrQDXRltBiF</t>
+  </si>
+  <si>
+    <t>ZKC0dgWyi2e</t>
+  </si>
+  <si>
+    <t>ZAHTk6C8Bpf</t>
+  </si>
+  <si>
+    <t>aND0YTwZzA5</t>
+  </si>
+  <si>
+    <t>QoPODSAWZJM</t>
+  </si>
+  <si>
+    <t>vOCMa9KoFkZ</t>
+  </si>
+  <si>
+    <t>OmJLpLhpjRs</t>
+  </si>
+  <si>
+    <t>10-14, Female, Unassisted</t>
+  </si>
+  <si>
+    <t>10-14, Male, Unassisted</t>
+  </si>
+  <si>
+    <t>15-19, Female, Unassisted</t>
+  </si>
+  <si>
+    <t>15-19, Male, Unassisted</t>
+  </si>
+  <si>
+    <t>20-24, Female, Unassisted</t>
+  </si>
+  <si>
+    <t>20-24, Male, Unassisted</t>
+  </si>
+  <si>
+    <t>25-29, Female, Unassisted</t>
+  </si>
+  <si>
+    <t>25-29, Male, Unassisted</t>
+  </si>
+  <si>
+    <t>30-34, Female, Unassisted</t>
+  </si>
+  <si>
+    <t>30-34, Male, Unassisted</t>
+  </si>
+  <si>
+    <t>35-39, Female, Unassisted</t>
+  </si>
+  <si>
+    <t>35-39, Male, Unassisted</t>
+  </si>
+  <si>
+    <t>40-49, Female, Unassisted</t>
+  </si>
+  <si>
+    <t>40-49, Male, Unassisted</t>
+  </si>
+  <si>
+    <t>50+, Female, Unassisted</t>
+  </si>
+  <si>
+    <t>50+, Male, Unassisted</t>
+  </si>
+  <si>
+    <t>FZAip9U20FO</t>
+  </si>
+  <si>
+    <t>F5ycS1AO6L9</t>
+  </si>
+  <si>
+    <t>Yygmra0wjfS</t>
+  </si>
+  <si>
+    <t>TmbqdGlsjgU</t>
+  </si>
+  <si>
+    <t>tvFpGPvf1dE</t>
+  </si>
+  <si>
+    <t>r8vRZxiL3On</t>
+  </si>
+  <si>
+    <t>dzebNOszBWB</t>
+  </si>
+  <si>
+    <t>NREmZ5nTjPG</t>
+  </si>
+  <si>
+    <t>RSmTAFblejf</t>
+  </si>
+  <si>
+    <t>iOs0xO0rO9a</t>
+  </si>
+  <si>
+    <t>T0FBc732ciN</t>
+  </si>
+  <si>
+    <t>hjOHLzQd87D</t>
+  </si>
+  <si>
+    <t>s4mTCYfXiCO</t>
+  </si>
+  <si>
+    <t>JutT06Y9k0T</t>
+  </si>
+  <si>
+    <t>wKVNLxXdver</t>
+  </si>
+  <si>
+    <t>XQhaXRu6a7c</t>
+  </si>
+  <si>
+    <t>st_ua</t>
+  </si>
+  <si>
+    <t>Directly-Assisted</t>
+  </si>
+  <si>
+    <t>CM0ud5U3iWD</t>
+  </si>
+  <si>
+    <t>Unassisted</t>
+  </si>
+  <si>
+    <t>QvMZVdK1AkM</t>
   </si>
 </sst>
 </file>
@@ -1962,7 +2175,7 @@
   <dimension ref="A1:Z56"/>
   <sheetViews>
     <sheetView topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="N43" sqref="N43"/>
     </sheetView>
@@ -7226,10 +7439,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
-  <dimension ref="A1:AC68"/>
+  <dimension ref="A1:AD100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7247,7 +7460,7 @@
     <col min="19" max="19" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>389</v>
       </c>
@@ -7335,8 +7548,11 @@
       <c r="AC1" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="2" spans="1:29" ht="18" x14ac:dyDescent="0.2">
+      <c r="AD1" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>294</v>
       </c>
@@ -7365,7 +7581,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K2:ZZ2)</f>
+        <f t="shared" ref="J2:J33" si="0">_xlfn.TEXTJOIN(";",1,K2:ZZ2)</f>
         <v>&lt;2mo</v>
       </c>
       <c r="K2" s="12"/>
@@ -7380,7 +7596,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>294</v>
       </c>
@@ -7409,7 +7625,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K3:ZZ3)</f>
+        <f t="shared" si="0"/>
         <v>2-12mo</v>
       </c>
       <c r="K3" s="12"/>
@@ -7424,7 +7640,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>294</v>
       </c>
@@ -7453,7 +7669,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K4:ZZ4)</f>
+        <f t="shared" si="0"/>
         <v>&lt;1-50+;&lt;1-18+</v>
       </c>
       <c r="K4" s="12" t="s">
@@ -7466,7 +7682,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>294</v>
       </c>
@@ -7495,7 +7711,7 @@
         <v>0.25</v>
       </c>
       <c r="J5" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K5:ZZ5)</f>
+        <f t="shared" si="0"/>
         <v>&lt;15/&gt;15.d</v>
       </c>
       <c r="O5" s="12"/>
@@ -7503,7 +7719,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>294</v>
       </c>
@@ -7532,11 +7748,11 @@
         <v>0.2</v>
       </c>
       <c r="J6" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K6:ZZ6)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>294</v>
       </c>
@@ -7565,7 +7781,7 @@
         <v>0.5</v>
       </c>
       <c r="J7" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K7:ZZ7)</f>
+        <f t="shared" si="0"/>
         <v>&lt;1-50+;1-50+;&lt;1-18+;1-4;1-50+/&lt;5</v>
       </c>
       <c r="K7" s="12" t="s">
@@ -7586,7 +7802,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>294</v>
       </c>
@@ -7615,14 +7831,14 @@
         <v>0.25</v>
       </c>
       <c r="J8" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K8:ZZ8)</f>
+        <f t="shared" si="0"/>
         <v>&lt;15/&gt;15.d</v>
       </c>
       <c r="P8" s="12" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>294</v>
       </c>
@@ -7651,7 +7867,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K9:ZZ9)</f>
+        <f t="shared" si="0"/>
         <v>1-4;1-50+/&lt;5</v>
       </c>
       <c r="Q9" s="12" t="s">
@@ -7661,7 +7877,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>294</v>
       </c>
@@ -7690,7 +7906,7 @@
         <v>0.5</v>
       </c>
       <c r="J10" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K10:ZZ10)</f>
+        <f t="shared" si="0"/>
         <v>&lt;1-50+;1-50+;&lt;1-18+;1-50+/&lt;5</v>
       </c>
       <c r="K10" s="12" t="s">
@@ -7708,7 +7924,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>294</v>
       </c>
@@ -7737,14 +7953,14 @@
         <v>0.25</v>
       </c>
       <c r="J11" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K11:ZZ11)</f>
+        <f t="shared" si="0"/>
         <v>&lt;15/&gt;15.d</v>
       </c>
       <c r="P11" s="12" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>294</v>
       </c>
@@ -7773,7 +7989,7 @@
         <v>1</v>
       </c>
       <c r="J12" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K12:ZZ12)</f>
+        <f t="shared" si="0"/>
         <v>&lt;1-50+;1-50+;10-50+;&lt;1-18+;1-50+/&lt;5;10-50+.all</v>
       </c>
       <c r="K12" s="12" t="s">
@@ -7796,7 +8012,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>294</v>
       </c>
@@ -7825,14 +8041,14 @@
         <v>0.25</v>
       </c>
       <c r="J13" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K13:ZZ13)</f>
+        <f t="shared" si="0"/>
         <v>&lt;15/&gt;15.d</v>
       </c>
       <c r="P13" s="12" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>237</v>
       </c>
@@ -7862,7 +8078,7 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="J14" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K14:ZZ14)</f>
+        <f t="shared" si="0"/>
         <v>missing_age_1</v>
       </c>
       <c r="K14" s="6"/>
@@ -7875,7 +8091,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="15" spans="1:29" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>294</v>
       </c>
@@ -7904,14 +8120,14 @@
         <v>1</v>
       </c>
       <c r="J15" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K15:ZZ15)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="P15" s="12"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>237</v>
       </c>
@@ -7940,7 +8156,7 @@
         <v>0.5</v>
       </c>
       <c r="J16" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K16:ZZ16)</f>
+        <f t="shared" si="0"/>
         <v>missing_age_2</v>
       </c>
       <c r="S16" t="s">
@@ -7976,7 +8192,7 @@
         <v>1</v>
       </c>
       <c r="J17" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K17:ZZ17)</f>
+        <f t="shared" si="0"/>
         <v>&lt;1-18+</v>
       </c>
       <c r="O17" t="s">
@@ -8012,7 +8228,7 @@
         <v>0.125</v>
       </c>
       <c r="J18" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K18:ZZ18)</f>
+        <f t="shared" si="0"/>
         <v>&lt;15/&gt;15.d</v>
       </c>
       <c r="P18" s="12" t="s">
@@ -8048,7 +8264,7 @@
         <v>1</v>
       </c>
       <c r="J19" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K19:ZZ19)</f>
+        <f t="shared" si="0"/>
         <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all</v>
       </c>
       <c r="K19" s="12" t="s">
@@ -8100,7 +8316,7 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="J20" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K20:ZZ20)</f>
+        <f t="shared" si="0"/>
         <v>missing_age_1</v>
       </c>
       <c r="K20" s="6"/>
@@ -8142,7 +8358,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K21:ZZ21)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="P21" s="13"/>
@@ -8176,7 +8392,7 @@
         <v>0.5</v>
       </c>
       <c r="J22" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K22:ZZ22)</f>
+        <f t="shared" si="0"/>
         <v>missing_age_2</v>
       </c>
       <c r="K22" s="6"/>
@@ -8218,7 +8434,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K23:ZZ23)</f>
+        <f t="shared" si="0"/>
         <v>&lt;1-18+</v>
       </c>
       <c r="K23" s="7"/>
@@ -8259,7 +8475,7 @@
         <v>0.125</v>
       </c>
       <c r="J24" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K24:ZZ24)</f>
+        <f t="shared" si="0"/>
         <v>&lt;15/&gt;15.d</v>
       </c>
       <c r="P24" s="12" t="s">
@@ -8295,7 +8511,7 @@
         <v>1</v>
       </c>
       <c r="J25" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K25:ZZ25)</f>
+        <f t="shared" si="0"/>
         <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all</v>
       </c>
       <c r="K25" s="12" t="s">
@@ -8347,7 +8563,7 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="J26" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K26:ZZ26)</f>
+        <f t="shared" si="0"/>
         <v>missing_age_1</v>
       </c>
       <c r="K26" s="6"/>
@@ -8389,7 +8605,7 @@
         <v>0.125</v>
       </c>
       <c r="J27" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K27:ZZ27)</f>
+        <f t="shared" si="0"/>
         <v>&lt;15/&gt;15.d</v>
       </c>
       <c r="P27" s="12" t="s">
@@ -8425,7 +8641,7 @@
         <v>1</v>
       </c>
       <c r="J28" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K28:ZZ28)</f>
+        <f t="shared" si="0"/>
         <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all</v>
       </c>
       <c r="K28" s="12" t="s">
@@ -8478,7 +8694,7 @@
         <v>0.2</v>
       </c>
       <c r="J29" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K29:ZZ29)</f>
+        <f t="shared" si="0"/>
         <v>10-50+.all</v>
       </c>
       <c r="T29" t="s">
@@ -8515,7 +8731,7 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="J30" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K30:ZZ30)</f>
+        <f t="shared" si="0"/>
         <v>missing_age_1</v>
       </c>
       <c r="K30" s="6"/>
@@ -8557,7 +8773,7 @@
         <v>1</v>
       </c>
       <c r="J31" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K31:ZZ31)</f>
+        <f t="shared" si="0"/>
         <v>&lt;1-18+</v>
       </c>
       <c r="O31" t="s">
@@ -8593,7 +8809,7 @@
         <v>0.125</v>
       </c>
       <c r="J32" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K32:ZZ32)</f>
+        <f t="shared" si="0"/>
         <v>&lt;15/&gt;15.d</v>
       </c>
       <c r="P32" s="12" t="s">
@@ -8629,7 +8845,7 @@
         <v>0.2</v>
       </c>
       <c r="J33" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K33:ZZ33)</f>
+        <f t="shared" si="0"/>
         <v>10-50+.all</v>
       </c>
       <c r="T33" t="s">
@@ -8665,7 +8881,7 @@
         <v>1</v>
       </c>
       <c r="J34" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K34:ZZ34)</f>
+        <f t="shared" ref="J34:J65" si="1">_xlfn.TEXTJOIN(";",1,K34:ZZ34)</f>
         <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all</v>
       </c>
       <c r="K34" s="12" t="s">
@@ -8719,7 +8935,7 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="J35" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K35:ZZ35)</f>
+        <f t="shared" si="1"/>
         <v>missing_age_1</v>
       </c>
       <c r="K35" s="6"/>
@@ -8761,7 +8977,7 @@
         <v>0.125</v>
       </c>
       <c r="J36" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K36:ZZ36)</f>
+        <f t="shared" si="1"/>
         <v>&lt;15/&gt;15.d</v>
       </c>
       <c r="P36" s="12" t="s">
@@ -8797,7 +9013,7 @@
         <v>0.2</v>
       </c>
       <c r="J37" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K37:ZZ37)</f>
+        <f t="shared" si="1"/>
         <v>10-50+.all</v>
       </c>
       <c r="T37" t="s">
@@ -8833,7 +9049,7 @@
         <v>1</v>
       </c>
       <c r="J38" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K38:ZZ38)</f>
+        <f t="shared" si="1"/>
         <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all</v>
       </c>
       <c r="K38" s="12" t="s">
@@ -8885,7 +9101,7 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="J39" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K39:ZZ39)</f>
+        <f t="shared" si="1"/>
         <v>missing_age_1</v>
       </c>
       <c r="K39" s="6"/>
@@ -8927,7 +9143,7 @@
         <v>0.125</v>
       </c>
       <c r="J40" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K40:ZZ40)</f>
+        <f t="shared" si="1"/>
         <v>&lt;15/&gt;15.d</v>
       </c>
       <c r="P40" s="12" t="s">
@@ -8963,7 +9179,7 @@
         <v>0.2</v>
       </c>
       <c r="J41" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K41:ZZ41)</f>
+        <f t="shared" si="1"/>
         <v>10-50+.all</v>
       </c>
       <c r="T41" t="s">
@@ -8999,7 +9215,7 @@
         <v>0.5</v>
       </c>
       <c r="J42" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K42:ZZ42)</f>
+        <f t="shared" si="1"/>
         <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all</v>
       </c>
       <c r="K42" s="12" t="s">
@@ -9051,7 +9267,7 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="J43" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K43:ZZ43)</f>
+        <f t="shared" si="1"/>
         <v>missing_age_1</v>
       </c>
       <c r="K43" s="6"/>
@@ -9093,7 +9309,7 @@
         <v>0.125</v>
       </c>
       <c r="J44" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K44:ZZ44)</f>
+        <f t="shared" si="1"/>
         <v>&lt;15/&gt;15.d</v>
       </c>
       <c r="P44" s="12" t="s">
@@ -9129,7 +9345,7 @@
         <v>0.2</v>
       </c>
       <c r="J45" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K45:ZZ45)</f>
+        <f t="shared" si="1"/>
         <v>10-50+.all</v>
       </c>
       <c r="T45" t="s">
@@ -9165,7 +9381,7 @@
         <v>0.5</v>
       </c>
       <c r="J46" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K46:ZZ46)</f>
+        <f t="shared" si="1"/>
         <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all</v>
       </c>
       <c r="K46" s="12" t="s">
@@ -9217,7 +9433,7 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="J47" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K47:ZZ47)</f>
+        <f t="shared" si="1"/>
         <v>missing_age_1</v>
       </c>
       <c r="K47" s="6"/>
@@ -9259,7 +9475,7 @@
         <v>0.125</v>
       </c>
       <c r="J48" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K48:ZZ48)</f>
+        <f t="shared" si="1"/>
         <v>&lt;15/&gt;15.d</v>
       </c>
       <c r="P48" s="12" t="s">
@@ -9295,7 +9511,7 @@
         <v>1</v>
       </c>
       <c r="J49" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K49:ZZ49)</f>
+        <f t="shared" si="1"/>
         <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all</v>
       </c>
       <c r="K49" s="12" t="s">
@@ -9347,7 +9563,7 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="J50" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K50:ZZ50)</f>
+        <f t="shared" si="1"/>
         <v>missing_age_1</v>
       </c>
       <c r="K50" s="6"/>
@@ -9389,7 +9605,7 @@
         <v>1</v>
       </c>
       <c r="J51" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K51:ZZ51)</f>
+        <f t="shared" si="1"/>
         <v>F;F/M;F/M/U</v>
       </c>
       <c r="U51" t="s">
@@ -9431,7 +9647,7 @@
         <v>0.5</v>
       </c>
       <c r="J52" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K52:ZZ52)</f>
+        <f t="shared" si="1"/>
         <v>missing_sex_1</v>
       </c>
       <c r="K52" s="6"/>
@@ -9473,7 +9689,7 @@
         <v>0.5</v>
       </c>
       <c r="J53" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K53:ZZ53)</f>
+        <f t="shared" si="1"/>
         <v>U;F/M/U</v>
       </c>
       <c r="K53" s="7"/>
@@ -9518,7 +9734,7 @@
         <v>1</v>
       </c>
       <c r="J54" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K54:ZZ54)</f>
+        <f t="shared" si="1"/>
         <v>M;F/M;F/M/U</v>
       </c>
       <c r="S54" s="7"/>
@@ -9562,7 +9778,7 @@
         <v>0.5</v>
       </c>
       <c r="J55" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K55:ZZ55)</f>
+        <f t="shared" si="1"/>
         <v>missing_sex_1</v>
       </c>
       <c r="K55" s="6"/>
@@ -9604,7 +9820,7 @@
         <v>0.5</v>
       </c>
       <c r="J56" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K56:ZZ56)</f>
+        <f t="shared" si="1"/>
         <v>U;F/M/U</v>
       </c>
       <c r="S56" s="7"/>
@@ -9645,7 +9861,7 @@
         <v>1</v>
       </c>
       <c r="J57" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K57:ZZ57)</f>
+        <f t="shared" si="1"/>
         <v>kp1</v>
       </c>
       <c r="X57" t="s">
@@ -9681,7 +9897,7 @@
         <v>1</v>
       </c>
       <c r="J58" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K58:ZZ58)</f>
+        <f t="shared" si="1"/>
         <v>kp1</v>
       </c>
       <c r="X58" t="s">
@@ -9717,7 +9933,7 @@
         <v>1</v>
       </c>
       <c r="J59" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K59:ZZ59)</f>
+        <f t="shared" si="1"/>
         <v>kp1</v>
       </c>
       <c r="X59" t="s">
@@ -9753,7 +9969,7 @@
         <v>1</v>
       </c>
       <c r="J60" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K60:ZZ60)</f>
+        <f t="shared" si="1"/>
         <v>kp1</v>
       </c>
       <c r="X60" t="s">
@@ -9789,7 +10005,7 @@
         <v>1</v>
       </c>
       <c r="J61" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K61:ZZ61)</f>
+        <f t="shared" si="1"/>
         <v>kp1</v>
       </c>
       <c r="X61" t="s">
@@ -9825,7 +10041,7 @@
         <v>1</v>
       </c>
       <c r="J62" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K62:ZZ62)</f>
+        <f t="shared" si="1"/>
         <v>tr</v>
       </c>
       <c r="Y62" t="s">
@@ -9861,7 +10077,7 @@
         <v>1</v>
       </c>
       <c r="J63" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K63:ZZ63)</f>
+        <f t="shared" si="1"/>
         <v>tr</v>
       </c>
       <c r="Y63" t="s">
@@ -9897,14 +10113,14 @@
         <v>1</v>
       </c>
       <c r="J64" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K64:ZZ64)</f>
+        <f t="shared" si="1"/>
         <v>KnownNewResult</v>
       </c>
       <c r="AB64" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="65" spans="1:29" ht="19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:30" ht="19" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>476</v>
       </c>
@@ -9933,14 +10149,14 @@
         <v>1</v>
       </c>
       <c r="J65" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K65:ZZ65)</f>
+        <f t="shared" si="1"/>
         <v>KnownNewResult</v>
       </c>
       <c r="AB65" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="66" spans="1:29" ht="19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:30" ht="19" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>476</v>
       </c>
@@ -9969,14 +10185,14 @@
         <v>1</v>
       </c>
       <c r="J66" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K66:ZZ66)</f>
+        <f t="shared" ref="J66:J97" si="2">_xlfn.TEXTJOIN(";",1,K66:ZZ66)</f>
         <v>KnownNewResult</v>
       </c>
       <c r="AB66" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="67" spans="1:29" ht="18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>490</v>
       </c>
@@ -10005,14 +10221,14 @@
         <v>1</v>
       </c>
       <c r="J67" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K67:ZZ67)</f>
+        <f t="shared" si="2"/>
         <v>vt_sv</v>
       </c>
       <c r="AC67" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="68" spans="1:29" ht="18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>490</v>
       </c>
@@ -10041,11 +10257,1099 @@
         <v>1</v>
       </c>
       <c r="J68" s="6" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K68:ZZ68)</f>
+        <f t="shared" si="2"/>
         <v>vt_pe</v>
       </c>
       <c r="AC68" t="s">
         <v>498</v>
+      </c>
+    </row>
+    <row r="69" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>490</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C69" t="s">
+        <v>520</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E69" s="14" t="s">
+        <v>504</v>
+      </c>
+      <c r="F69" t="s">
+        <v>569</v>
+      </c>
+      <c r="G69" t="s">
+        <v>570</v>
+      </c>
+      <c r="H69">
+        <v>10</v>
+      </c>
+      <c r="I69" s="7">
+        <v>1</v>
+      </c>
+      <c r="J69" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_da</v>
+      </c>
+      <c r="AD69" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="70" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>490</v>
+      </c>
+      <c r="B70" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C70" t="s">
+        <v>521</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E70" s="14" t="s">
+        <v>505</v>
+      </c>
+      <c r="F70" t="s">
+        <v>569</v>
+      </c>
+      <c r="G70" t="s">
+        <v>570</v>
+      </c>
+      <c r="H70">
+        <v>20</v>
+      </c>
+      <c r="I70" s="7">
+        <v>1</v>
+      </c>
+      <c r="J70" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_da</v>
+      </c>
+      <c r="AD70" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="71" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>490</v>
+      </c>
+      <c r="B71" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C71" t="s">
+        <v>522</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E71" s="14" t="s">
+        <v>506</v>
+      </c>
+      <c r="F71" t="s">
+        <v>569</v>
+      </c>
+      <c r="G71" t="s">
+        <v>570</v>
+      </c>
+      <c r="H71">
+        <v>30</v>
+      </c>
+      <c r="I71" s="7">
+        <v>1</v>
+      </c>
+      <c r="J71" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_da</v>
+      </c>
+      <c r="AD71" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="72" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>490</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C72" t="s">
+        <v>523</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E72" s="14" t="s">
+        <v>507</v>
+      </c>
+      <c r="F72" t="s">
+        <v>569</v>
+      </c>
+      <c r="G72" t="s">
+        <v>570</v>
+      </c>
+      <c r="H72">
+        <v>40</v>
+      </c>
+      <c r="I72" s="7">
+        <v>1</v>
+      </c>
+      <c r="J72" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_da</v>
+      </c>
+      <c r="AD72" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="73" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>490</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C73" t="s">
+        <v>524</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E73" s="14" t="s">
+        <v>508</v>
+      </c>
+      <c r="F73" t="s">
+        <v>569</v>
+      </c>
+      <c r="G73" t="s">
+        <v>570</v>
+      </c>
+      <c r="H73">
+        <v>50</v>
+      </c>
+      <c r="I73" s="7">
+        <v>1</v>
+      </c>
+      <c r="J73" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_da</v>
+      </c>
+      <c r="AD73" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="74" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>490</v>
+      </c>
+      <c r="B74" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C74" t="s">
+        <v>525</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E74" s="14" t="s">
+        <v>509</v>
+      </c>
+      <c r="F74" t="s">
+        <v>569</v>
+      </c>
+      <c r="G74" t="s">
+        <v>570</v>
+      </c>
+      <c r="H74">
+        <v>60</v>
+      </c>
+      <c r="I74" s="7">
+        <v>1</v>
+      </c>
+      <c r="J74" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_da</v>
+      </c>
+      <c r="AD74" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="75" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>490</v>
+      </c>
+      <c r="B75" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C75" t="s">
+        <v>526</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E75" s="14" t="s">
+        <v>510</v>
+      </c>
+      <c r="F75" t="s">
+        <v>569</v>
+      </c>
+      <c r="G75" t="s">
+        <v>570</v>
+      </c>
+      <c r="H75">
+        <v>70</v>
+      </c>
+      <c r="I75" s="7">
+        <v>1</v>
+      </c>
+      <c r="J75" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_da</v>
+      </c>
+      <c r="AD75" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="76" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>490</v>
+      </c>
+      <c r="B76" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C76" t="s">
+        <v>527</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E76" s="14" t="s">
+        <v>511</v>
+      </c>
+      <c r="F76" t="s">
+        <v>569</v>
+      </c>
+      <c r="G76" t="s">
+        <v>570</v>
+      </c>
+      <c r="H76">
+        <v>80</v>
+      </c>
+      <c r="I76" s="7">
+        <v>1</v>
+      </c>
+      <c r="J76" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_da</v>
+      </c>
+      <c r="AD76" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="77" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>490</v>
+      </c>
+      <c r="B77" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C77" t="s">
+        <v>528</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E77" s="14" t="s">
+        <v>512</v>
+      </c>
+      <c r="F77" t="s">
+        <v>569</v>
+      </c>
+      <c r="G77" t="s">
+        <v>570</v>
+      </c>
+      <c r="H77">
+        <v>90</v>
+      </c>
+      <c r="I77" s="7">
+        <v>1</v>
+      </c>
+      <c r="J77" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_da</v>
+      </c>
+      <c r="AD77" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="78" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>490</v>
+      </c>
+      <c r="B78" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C78" t="s">
+        <v>529</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E78" s="14" t="s">
+        <v>513</v>
+      </c>
+      <c r="F78" t="s">
+        <v>569</v>
+      </c>
+      <c r="G78" t="s">
+        <v>570</v>
+      </c>
+      <c r="H78">
+        <v>100</v>
+      </c>
+      <c r="I78" s="7">
+        <v>1</v>
+      </c>
+      <c r="J78" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_da</v>
+      </c>
+      <c r="AD78" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="79" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>490</v>
+      </c>
+      <c r="B79" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C79" t="s">
+        <v>530</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E79" s="14" t="s">
+        <v>514</v>
+      </c>
+      <c r="F79" t="s">
+        <v>569</v>
+      </c>
+      <c r="G79" t="s">
+        <v>570</v>
+      </c>
+      <c r="H79">
+        <v>110</v>
+      </c>
+      <c r="I79" s="7">
+        <v>1</v>
+      </c>
+      <c r="J79" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_da</v>
+      </c>
+      <c r="AD79" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="80" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>490</v>
+      </c>
+      <c r="B80" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C80" t="s">
+        <v>531</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E80" s="14" t="s">
+        <v>515</v>
+      </c>
+      <c r="F80" t="s">
+        <v>569</v>
+      </c>
+      <c r="G80" t="s">
+        <v>570</v>
+      </c>
+      <c r="H80">
+        <v>120</v>
+      </c>
+      <c r="I80" s="7">
+        <v>1</v>
+      </c>
+      <c r="J80" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_da</v>
+      </c>
+      <c r="AD80" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="81" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>490</v>
+      </c>
+      <c r="B81" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C81" t="s">
+        <v>532</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E81" s="14" t="s">
+        <v>516</v>
+      </c>
+      <c r="F81" t="s">
+        <v>569</v>
+      </c>
+      <c r="G81" t="s">
+        <v>570</v>
+      </c>
+      <c r="H81">
+        <v>130</v>
+      </c>
+      <c r="I81" s="7">
+        <v>1</v>
+      </c>
+      <c r="J81" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_da</v>
+      </c>
+      <c r="AD81" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="82" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>490</v>
+      </c>
+      <c r="B82" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C82" t="s">
+        <v>533</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E82" s="14" t="s">
+        <v>517</v>
+      </c>
+      <c r="F82" t="s">
+        <v>569</v>
+      </c>
+      <c r="G82" t="s">
+        <v>570</v>
+      </c>
+      <c r="H82">
+        <v>140</v>
+      </c>
+      <c r="I82" s="7">
+        <v>1</v>
+      </c>
+      <c r="J82" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_da</v>
+      </c>
+      <c r="AD82" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="83" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>490</v>
+      </c>
+      <c r="B83" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C83" t="s">
+        <v>534</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E83" s="14" t="s">
+        <v>518</v>
+      </c>
+      <c r="F83" t="s">
+        <v>569</v>
+      </c>
+      <c r="G83" t="s">
+        <v>570</v>
+      </c>
+      <c r="H83">
+        <v>150</v>
+      </c>
+      <c r="I83" s="7">
+        <v>1</v>
+      </c>
+      <c r="J83" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_da</v>
+      </c>
+      <c r="AD83" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="84" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>490</v>
+      </c>
+      <c r="B84" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C84" t="s">
+        <v>535</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E84" s="14" t="s">
+        <v>519</v>
+      </c>
+      <c r="F84" t="s">
+        <v>569</v>
+      </c>
+      <c r="G84" t="s">
+        <v>570</v>
+      </c>
+      <c r="H84">
+        <v>160</v>
+      </c>
+      <c r="I84" s="7">
+        <v>1</v>
+      </c>
+      <c r="J84" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_da</v>
+      </c>
+      <c r="AD84" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="85" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>490</v>
+      </c>
+      <c r="B85" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C85" t="s">
+        <v>552</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E85" s="14" t="s">
+        <v>536</v>
+      </c>
+      <c r="F85" t="s">
+        <v>571</v>
+      </c>
+      <c r="G85" t="s">
+        <v>572</v>
+      </c>
+      <c r="H85">
+        <v>170</v>
+      </c>
+      <c r="I85" s="7">
+        <v>1</v>
+      </c>
+      <c r="J85" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="86" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>490</v>
+      </c>
+      <c r="B86" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C86" t="s">
+        <v>553</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E86" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="F86" t="s">
+        <v>571</v>
+      </c>
+      <c r="G86" t="s">
+        <v>572</v>
+      </c>
+      <c r="H86">
+        <v>180</v>
+      </c>
+      <c r="I86" s="7">
+        <v>1</v>
+      </c>
+      <c r="J86" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="87" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>490</v>
+      </c>
+      <c r="B87" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C87" t="s">
+        <v>554</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E87" s="14" t="s">
+        <v>538</v>
+      </c>
+      <c r="F87" t="s">
+        <v>571</v>
+      </c>
+      <c r="G87" t="s">
+        <v>572</v>
+      </c>
+      <c r="H87">
+        <v>190</v>
+      </c>
+      <c r="I87" s="7">
+        <v>1</v>
+      </c>
+      <c r="J87" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="88" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>490</v>
+      </c>
+      <c r="B88" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C88" t="s">
+        <v>555</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E88" s="14" t="s">
+        <v>539</v>
+      </c>
+      <c r="F88" t="s">
+        <v>571</v>
+      </c>
+      <c r="G88" t="s">
+        <v>572</v>
+      </c>
+      <c r="H88">
+        <v>200</v>
+      </c>
+      <c r="I88" s="7">
+        <v>1</v>
+      </c>
+      <c r="J88" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="89" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>490</v>
+      </c>
+      <c r="B89" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C89" t="s">
+        <v>556</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E89" s="14" t="s">
+        <v>540</v>
+      </c>
+      <c r="F89" t="s">
+        <v>571</v>
+      </c>
+      <c r="G89" t="s">
+        <v>572</v>
+      </c>
+      <c r="H89">
+        <v>210</v>
+      </c>
+      <c r="I89" s="7">
+        <v>1</v>
+      </c>
+      <c r="J89" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="90" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>490</v>
+      </c>
+      <c r="B90" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C90" t="s">
+        <v>557</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E90" s="14" t="s">
+        <v>541</v>
+      </c>
+      <c r="F90" t="s">
+        <v>571</v>
+      </c>
+      <c r="G90" t="s">
+        <v>572</v>
+      </c>
+      <c r="H90">
+        <v>220</v>
+      </c>
+      <c r="I90" s="7">
+        <v>1</v>
+      </c>
+      <c r="J90" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="91" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>490</v>
+      </c>
+      <c r="B91" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C91" t="s">
+        <v>558</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E91" s="14" t="s">
+        <v>542</v>
+      </c>
+      <c r="F91" t="s">
+        <v>571</v>
+      </c>
+      <c r="G91" t="s">
+        <v>572</v>
+      </c>
+      <c r="H91">
+        <v>230</v>
+      </c>
+      <c r="I91" s="7">
+        <v>1</v>
+      </c>
+      <c r="J91" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="92" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>490</v>
+      </c>
+      <c r="B92" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C92" t="s">
+        <v>559</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E92" s="14" t="s">
+        <v>543</v>
+      </c>
+      <c r="F92" t="s">
+        <v>571</v>
+      </c>
+      <c r="G92" t="s">
+        <v>572</v>
+      </c>
+      <c r="H92">
+        <v>240</v>
+      </c>
+      <c r="I92" s="7">
+        <v>1</v>
+      </c>
+      <c r="J92" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="93" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>490</v>
+      </c>
+      <c r="B93" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C93" t="s">
+        <v>560</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E93" s="14" t="s">
+        <v>544</v>
+      </c>
+      <c r="F93" t="s">
+        <v>571</v>
+      </c>
+      <c r="G93" t="s">
+        <v>572</v>
+      </c>
+      <c r="H93">
+        <v>250</v>
+      </c>
+      <c r="I93" s="7">
+        <v>1</v>
+      </c>
+      <c r="J93" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="94" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>490</v>
+      </c>
+      <c r="B94" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C94" t="s">
+        <v>561</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E94" s="14" t="s">
+        <v>545</v>
+      </c>
+      <c r="F94" t="s">
+        <v>571</v>
+      </c>
+      <c r="G94" t="s">
+        <v>572</v>
+      </c>
+      <c r="H94">
+        <v>260</v>
+      </c>
+      <c r="I94" s="7">
+        <v>1</v>
+      </c>
+      <c r="J94" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="95" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>490</v>
+      </c>
+      <c r="B95" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C95" t="s">
+        <v>562</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E95" s="14" t="s">
+        <v>546</v>
+      </c>
+      <c r="F95" t="s">
+        <v>571</v>
+      </c>
+      <c r="G95" t="s">
+        <v>572</v>
+      </c>
+      <c r="H95">
+        <v>270</v>
+      </c>
+      <c r="I95" s="7">
+        <v>1</v>
+      </c>
+      <c r="J95" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="96" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>490</v>
+      </c>
+      <c r="B96" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C96" t="s">
+        <v>563</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E96" s="14" t="s">
+        <v>547</v>
+      </c>
+      <c r="F96" t="s">
+        <v>571</v>
+      </c>
+      <c r="G96" t="s">
+        <v>572</v>
+      </c>
+      <c r="H96">
+        <v>280</v>
+      </c>
+      <c r="I96" s="7">
+        <v>1</v>
+      </c>
+      <c r="J96" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>490</v>
+      </c>
+      <c r="B97" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C97" t="s">
+        <v>564</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E97" s="14" t="s">
+        <v>548</v>
+      </c>
+      <c r="F97" t="s">
+        <v>571</v>
+      </c>
+      <c r="G97" t="s">
+        <v>572</v>
+      </c>
+      <c r="H97">
+        <v>290</v>
+      </c>
+      <c r="I97" s="7">
+        <v>1</v>
+      </c>
+      <c r="J97" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>490</v>
+      </c>
+      <c r="B98" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C98" t="s">
+        <v>565</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E98" s="14" t="s">
+        <v>549</v>
+      </c>
+      <c r="F98" t="s">
+        <v>571</v>
+      </c>
+      <c r="G98" t="s">
+        <v>572</v>
+      </c>
+      <c r="H98">
+        <v>300</v>
+      </c>
+      <c r="I98" s="7">
+        <v>1</v>
+      </c>
+      <c r="J98" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>490</v>
+      </c>
+      <c r="B99" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C99" t="s">
+        <v>566</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E99" s="14" t="s">
+        <v>550</v>
+      </c>
+      <c r="F99" t="s">
+        <v>571</v>
+      </c>
+      <c r="G99" t="s">
+        <v>572</v>
+      </c>
+      <c r="H99">
+        <v>310</v>
+      </c>
+      <c r="I99" s="7">
+        <v>1</v>
+      </c>
+      <c r="J99" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>490</v>
+      </c>
+      <c r="B100" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C100" t="s">
+        <v>567</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E100" s="14" t="s">
+        <v>551</v>
+      </c>
+      <c r="F100" t="s">
+        <v>571</v>
+      </c>
+      <c r="G100" t="s">
+        <v>572</v>
+      </c>
+      <c r="H100">
+        <v>320</v>
+      </c>
+      <c r="I100" s="7">
+        <v>1</v>
+      </c>
+      <c r="J100" t="s">
+        <v>568</v>
       </c>
     </row>
   </sheetData>
@@ -10060,9 +11364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C636F64A-C51E-B84F-AE74-B49AD03FC3D9}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>

<commit_message>
Adding self test and kp_prev(keypop) category option combos to dimension_item_sets
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FAA734-A332-774C-856F-F645BCA1A88E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF984974-5216-D14C-A4B3-7BD99DFBEBC2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="0" windowWidth="25600" windowHeight="20480" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2525" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2589" uniqueCount="592">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1756,13 +1756,70 @@
   </si>
   <si>
     <t>QvMZVdK1AkM</t>
+  </si>
+  <si>
+    <t>tr_pos</t>
+  </si>
+  <si>
+    <t>tr_neg</t>
+  </si>
+  <si>
+    <t>AkPJat3QJAW</t>
+  </si>
+  <si>
+    <t>rpwKzAIR5f4</t>
+  </si>
+  <si>
+    <t>uPSmoMfxrjX</t>
+  </si>
+  <si>
+    <t>H4zDlK3nU3e</t>
+  </si>
+  <si>
+    <t>S4ixSeMtEoZ</t>
+  </si>
+  <si>
+    <t>gO96NV54yD4</t>
+  </si>
+  <si>
+    <t>fRj8O5iNQlV</t>
+  </si>
+  <si>
+    <t>edBMVgUohvf</t>
+  </si>
+  <si>
+    <t>kp2</t>
+  </si>
+  <si>
+    <t>(FSW)</t>
+  </si>
+  <si>
+    <t>(Female PWID)</t>
+  </si>
+  <si>
+    <t>(MSM SW)</t>
+  </si>
+  <si>
+    <t>(MSM not SW)</t>
+  </si>
+  <si>
+    <t>(Male PWID)</t>
+  </si>
+  <si>
+    <t>(People in prisons and other enclosed settings)</t>
+  </si>
+  <si>
+    <t>(TG SW)</t>
+  </si>
+  <si>
+    <t>(TG not SW)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1814,6 +1871,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1835,7 +1898,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1858,6 +1921,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2174,10 +2238,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
   <dimension ref="A1:Z56"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="N43" sqref="N43"/>
+      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7439,10 +7503,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
-  <dimension ref="A1:AD100"/>
+  <dimension ref="A1:AD108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A109" sqref="A109:XFD145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10042,10 +10106,10 @@
       </c>
       <c r="J62" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>tr</v>
+        <v>tr_pos</v>
       </c>
       <c r="Y62" t="s">
-        <v>464</v>
+        <v>573</v>
       </c>
     </row>
     <row r="63" spans="1:28" ht="18" x14ac:dyDescent="0.25">
@@ -10078,10 +10142,10 @@
       </c>
       <c r="J63" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>tr</v>
+        <v>tr_neg</v>
       </c>
       <c r="Y63" t="s">
-        <v>464</v>
+        <v>574</v>
       </c>
     </row>
     <row r="64" spans="1:28" ht="19" x14ac:dyDescent="0.25">
@@ -10185,7 +10249,7 @@
         <v>1</v>
       </c>
       <c r="J66" s="6" t="str">
-        <f t="shared" ref="J66:J97" si="2">_xlfn.TEXTJOIN(";",1,K66:ZZ66)</f>
+        <f t="shared" ref="J66:J108" si="2">_xlfn.TEXTJOIN(";",1,K66:ZZ66)</f>
         <v>KnownNewResult</v>
       </c>
       <c r="AB66" t="s">
@@ -10868,7 +10932,11 @@
       <c r="I85" s="7">
         <v>1</v>
       </c>
-      <c r="J85" t="s">
+      <c r="J85" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_ua</v>
+      </c>
+      <c r="AD85" t="s">
         <v>568</v>
       </c>
     </row>
@@ -10900,7 +10968,11 @@
       <c r="I86" s="7">
         <v>1</v>
       </c>
-      <c r="J86" t="s">
+      <c r="J86" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_ua</v>
+      </c>
+      <c r="AD86" t="s">
         <v>568</v>
       </c>
     </row>
@@ -10932,7 +11004,11 @@
       <c r="I87" s="7">
         <v>1</v>
       </c>
-      <c r="J87" t="s">
+      <c r="J87" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_ua</v>
+      </c>
+      <c r="AD87" t="s">
         <v>568</v>
       </c>
     </row>
@@ -10964,7 +11040,11 @@
       <c r="I88" s="7">
         <v>1</v>
       </c>
-      <c r="J88" t="s">
+      <c r="J88" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_ua</v>
+      </c>
+      <c r="AD88" t="s">
         <v>568</v>
       </c>
     </row>
@@ -10996,7 +11076,11 @@
       <c r="I89" s="7">
         <v>1</v>
       </c>
-      <c r="J89" t="s">
+      <c r="J89" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_ua</v>
+      </c>
+      <c r="AD89" t="s">
         <v>568</v>
       </c>
     </row>
@@ -11028,7 +11112,11 @@
       <c r="I90" s="7">
         <v>1</v>
       </c>
-      <c r="J90" t="s">
+      <c r="J90" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_ua</v>
+      </c>
+      <c r="AD90" t="s">
         <v>568</v>
       </c>
     </row>
@@ -11060,7 +11148,11 @@
       <c r="I91" s="7">
         <v>1</v>
       </c>
-      <c r="J91" t="s">
+      <c r="J91" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_ua</v>
+      </c>
+      <c r="AD91" t="s">
         <v>568</v>
       </c>
     </row>
@@ -11092,7 +11184,11 @@
       <c r="I92" s="7">
         <v>1</v>
       </c>
-      <c r="J92" t="s">
+      <c r="J92" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_ua</v>
+      </c>
+      <c r="AD92" t="s">
         <v>568</v>
       </c>
     </row>
@@ -11124,7 +11220,11 @@
       <c r="I93" s="7">
         <v>1</v>
       </c>
-      <c r="J93" t="s">
+      <c r="J93" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_ua</v>
+      </c>
+      <c r="AD93" t="s">
         <v>568</v>
       </c>
     </row>
@@ -11156,7 +11256,11 @@
       <c r="I94" s="7">
         <v>1</v>
       </c>
-      <c r="J94" t="s">
+      <c r="J94" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_ua</v>
+      </c>
+      <c r="AD94" t="s">
         <v>568</v>
       </c>
     </row>
@@ -11188,7 +11292,11 @@
       <c r="I95" s="7">
         <v>1</v>
       </c>
-      <c r="J95" t="s">
+      <c r="J95" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_ua</v>
+      </c>
+      <c r="AD95" t="s">
         <v>568</v>
       </c>
     </row>
@@ -11220,11 +11328,15 @@
       <c r="I96" s="7">
         <v>1</v>
       </c>
-      <c r="J96" t="s">
+      <c r="J96" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_ua</v>
+      </c>
+      <c r="AD96" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>490</v>
       </c>
@@ -11252,11 +11364,15 @@
       <c r="I97" s="7">
         <v>1</v>
       </c>
-      <c r="J97" t="s">
+      <c r="J97" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_ua</v>
+      </c>
+      <c r="AD97" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>490</v>
       </c>
@@ -11284,11 +11400,15 @@
       <c r="I98" s="7">
         <v>1</v>
       </c>
-      <c r="J98" t="s">
+      <c r="J98" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_ua</v>
+      </c>
+      <c r="AD98" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>490</v>
       </c>
@@ -11316,11 +11436,15 @@
       <c r="I99" s="7">
         <v>1</v>
       </c>
-      <c r="J99" t="s">
+      <c r="J99" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_ua</v>
+      </c>
+      <c r="AD99" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>490</v>
       </c>
@@ -11348,8 +11472,300 @@
       <c r="I100" s="7">
         <v>1</v>
       </c>
-      <c r="J100" t="s">
+      <c r="J100" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>st_ua</v>
+      </c>
+      <c r="AD100" t="s">
         <v>568</v>
+      </c>
+    </row>
+    <row r="101" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>490</v>
+      </c>
+      <c r="B101" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C101" s="18" t="s">
+        <v>575</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="E101" s="18" t="s">
+        <v>584</v>
+      </c>
+      <c r="F101" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="G101" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="H101">
+        <v>400</v>
+      </c>
+      <c r="I101" s="7">
+        <v>1</v>
+      </c>
+      <c r="J101" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>kp2</v>
+      </c>
+      <c r="X101" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="102" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>490</v>
+      </c>
+      <c r="B102" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C102" s="18" t="s">
+        <v>576</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="E102" s="18" t="s">
+        <v>585</v>
+      </c>
+      <c r="F102" s="18" t="s">
+        <v>372</v>
+      </c>
+      <c r="G102" s="18" t="s">
+        <v>370</v>
+      </c>
+      <c r="H102">
+        <v>410</v>
+      </c>
+      <c r="I102" s="7">
+        <v>1</v>
+      </c>
+      <c r="J102" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>kp2</v>
+      </c>
+      <c r="X102" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="103" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>490</v>
+      </c>
+      <c r="B103" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C103" s="18" t="s">
+        <v>577</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="E103" s="18" t="s">
+        <v>586</v>
+      </c>
+      <c r="F103" s="18" t="s">
+        <v>375</v>
+      </c>
+      <c r="G103" s="18" t="s">
+        <v>374</v>
+      </c>
+      <c r="H103">
+        <v>420</v>
+      </c>
+      <c r="I103" s="7">
+        <v>1</v>
+      </c>
+      <c r="J103" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>kp2</v>
+      </c>
+      <c r="X103" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="104" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>490</v>
+      </c>
+      <c r="B104" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C104" s="18" t="s">
+        <v>578</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="E104" s="18" t="s">
+        <v>587</v>
+      </c>
+      <c r="F104" s="18" t="s">
+        <v>377</v>
+      </c>
+      <c r="G104" s="18" t="s">
+        <v>376</v>
+      </c>
+      <c r="H104">
+        <v>430</v>
+      </c>
+      <c r="I104" s="7">
+        <v>1</v>
+      </c>
+      <c r="J104" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>kp2</v>
+      </c>
+      <c r="X104" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="105" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>490</v>
+      </c>
+      <c r="B105" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C105" s="18" t="s">
+        <v>579</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="E105" s="18" t="s">
+        <v>588</v>
+      </c>
+      <c r="F105" s="18" t="s">
+        <v>373</v>
+      </c>
+      <c r="G105" s="18" t="s">
+        <v>371</v>
+      </c>
+      <c r="H105">
+        <v>440</v>
+      </c>
+      <c r="I105" s="7">
+        <v>1</v>
+      </c>
+      <c r="J105" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>kp2</v>
+      </c>
+      <c r="X105" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="106" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>490</v>
+      </c>
+      <c r="B106" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C106" s="18" t="s">
+        <v>580</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="E106" s="18" t="s">
+        <v>589</v>
+      </c>
+      <c r="F106" s="18" t="s">
+        <v>382</v>
+      </c>
+      <c r="G106" s="18" t="s">
+        <v>317</v>
+      </c>
+      <c r="H106">
+        <v>450</v>
+      </c>
+      <c r="I106" s="7">
+        <v>1</v>
+      </c>
+      <c r="J106" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>kp2</v>
+      </c>
+      <c r="X106" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="107" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>490</v>
+      </c>
+      <c r="B107" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C107" s="18" t="s">
+        <v>581</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="E107" s="18" t="s">
+        <v>590</v>
+      </c>
+      <c r="F107" s="18" t="s">
+        <v>378</v>
+      </c>
+      <c r="G107" s="18" t="s">
+        <v>379</v>
+      </c>
+      <c r="H107">
+        <v>460</v>
+      </c>
+      <c r="I107" s="7">
+        <v>1</v>
+      </c>
+      <c r="J107" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>kp2</v>
+      </c>
+      <c r="X107" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="108" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>490</v>
+      </c>
+      <c r="B108" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C108" s="18" t="s">
+        <v>582</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="E108" s="18" t="s">
+        <v>591</v>
+      </c>
+      <c r="F108" s="18" t="s">
+        <v>381</v>
+      </c>
+      <c r="G108" s="18" t="s">
+        <v>380</v>
+      </c>
+      <c r="H108">
+        <v>470</v>
+      </c>
+      <c r="I108" s="7">
+        <v>1</v>
+      </c>
+      <c r="J108" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>kp2</v>
+      </c>
+      <c r="X108" t="s">
+        <v>583</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding ART ststus dimension to dimendsion_item_sets config file
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF984974-5216-D14C-A4B3-7BD99DFBEBC2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E0C7AA-2D10-BA48-8ABF-D1C86AA49722}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2589" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2603" uniqueCount="603">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1813,13 +1813,46 @@
   </si>
   <si>
     <t>(TG not SW)</t>
+  </si>
+  <si>
+    <t>as</t>
+  </si>
+  <si>
+    <t>ART Status</t>
+  </si>
+  <si>
+    <t>M5w5H1KU40l</t>
+  </si>
+  <si>
+    <t>Already on ART</t>
+  </si>
+  <si>
+    <t>blnuJdt8f1Y</t>
+  </si>
+  <si>
+    <t>Life-long ART, Already</t>
+  </si>
+  <si>
+    <t>rSKP7Z85FX9</t>
+  </si>
+  <si>
+    <t>udcRwufEXFQ</t>
+  </si>
+  <si>
+    <t>Life-long ART, New</t>
+  </si>
+  <si>
+    <t>x9wEpHXMZ5Z</t>
+  </si>
+  <si>
+    <t>New on ART</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1877,6 +1910,12 @@
       <name val="Lucida Grande"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF881280"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1898,7 +1937,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1922,6 +1961,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2239,9 +2279,9 @@
   <dimension ref="A1:Z56"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7503,10 +7543,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
-  <dimension ref="A1:AD108"/>
+  <dimension ref="A1:AD112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109:XFD145"/>
+    <sheetView tabSelected="1" topLeftCell="G81" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="N110" sqref="N110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11768,6 +11808,67 @@
         <v>583</v>
       </c>
     </row>
+    <row r="109" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A109" s="16" t="s">
+        <v>594</v>
+      </c>
+      <c r="B109" s="16" t="s">
+        <v>593</v>
+      </c>
+      <c r="C109" s="16" t="s">
+        <v>596</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="E109" t="s">
+        <v>595</v>
+      </c>
+      <c r="F109" s="14" t="s">
+        <v>597</v>
+      </c>
+      <c r="G109" s="16" t="s">
+        <v>598</v>
+      </c>
+      <c r="H109">
+        <v>510</v>
+      </c>
+      <c r="I109" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="A110" s="16" t="s">
+        <v>594</v>
+      </c>
+      <c r="B110" s="16" t="s">
+        <v>593</v>
+      </c>
+      <c r="C110" s="16" t="s">
+        <v>601</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="E110" t="s">
+        <v>602</v>
+      </c>
+      <c r="F110" s="14" t="s">
+        <v>600</v>
+      </c>
+      <c r="G110" s="16" t="s">
+        <v>599</v>
+      </c>
+      <c r="H110">
+        <v>520</v>
+      </c>
+      <c r="I110" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="D112" s="19"/>
+    </row>
   </sheetData>
   <sortState ref="A4:W61">
     <sortCondition ref="H4:H61"/>

</xml_diff>

<commit_message>
added art status column to dimension item sets config file
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E0C7AA-2D10-BA48-8ABF-D1C86AA49722}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1A7790-6FAD-7046-919F-FC398B830DD1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2603" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2606" uniqueCount="605">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1846,6 +1846,12 @@
   </si>
   <si>
     <t>New on ART</t>
+  </si>
+  <si>
+    <t>as_already</t>
+  </si>
+  <si>
+    <t>as_new</t>
   </si>
 </sst>
 </file>
@@ -7543,10 +7549,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
-  <dimension ref="A1:AD112"/>
+  <dimension ref="A1:AE112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G81" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="N110" sqref="N110"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7564,7 +7570,7 @@
     <col min="19" max="19" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>389</v>
       </c>
@@ -7655,8 +7661,11 @@
       <c r="AD1" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" ht="18" x14ac:dyDescent="0.2">
+      <c r="AE1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>294</v>
       </c>
@@ -7700,7 +7709,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>294</v>
       </c>
@@ -7744,7 +7753,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>294</v>
       </c>
@@ -7786,7 +7795,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>294</v>
       </c>
@@ -7823,7 +7832,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>294</v>
       </c>
@@ -7856,7 +7865,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>294</v>
       </c>
@@ -7906,7 +7915,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>294</v>
       </c>
@@ -7942,7 +7951,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>294</v>
       </c>
@@ -7981,7 +7990,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>294</v>
       </c>
@@ -8028,7 +8037,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>294</v>
       </c>
@@ -8064,7 +8073,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>294</v>
       </c>
@@ -8116,7 +8125,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>294</v>
       </c>
@@ -8152,7 +8161,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>237</v>
       </c>
@@ -8195,7 +8204,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="15" spans="1:30" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>294</v>
       </c>
@@ -8231,7 +8240,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>237</v>
       </c>
@@ -10289,7 +10298,7 @@
         <v>1</v>
       </c>
       <c r="J66" s="6" t="str">
-        <f t="shared" ref="J66:J108" si="2">_xlfn.TEXTJOIN(";",1,K66:ZZ66)</f>
+        <f t="shared" ref="J66:J110" si="2">_xlfn.TEXTJOIN(";",1,K66:ZZ66)</f>
         <v>KnownNewResult</v>
       </c>
       <c r="AB66" t="s">
@@ -11376,7 +11385,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="97" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>490</v>
       </c>
@@ -11412,7 +11421,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="98" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>490</v>
       </c>
@@ -11448,7 +11457,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="99" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>490</v>
       </c>
@@ -11484,7 +11493,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="100" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>490</v>
       </c>
@@ -11520,7 +11529,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="101" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>490</v>
       </c>
@@ -11556,7 +11565,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="102" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>490</v>
       </c>
@@ -11592,7 +11601,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="103" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>490</v>
       </c>
@@ -11628,7 +11637,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="104" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>490</v>
       </c>
@@ -11664,7 +11673,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="105" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>490</v>
       </c>
@@ -11700,7 +11709,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="106" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>490</v>
       </c>
@@ -11736,7 +11745,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="107" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>490</v>
       </c>
@@ -11772,7 +11781,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="108" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>490</v>
       </c>
@@ -11808,7 +11817,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="109" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A109" s="16" t="s">
         <v>594</v>
       </c>
@@ -11836,8 +11845,15 @@
       <c r="I109" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="J109" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>as_already</v>
+      </c>
+      <c r="AE109" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="110" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A110" s="16" t="s">
         <v>594</v>
       </c>
@@ -11865,8 +11881,15 @@
       <c r="I110" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+      <c r="J110" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>as_new</v>
+      </c>
+      <c r="AE110" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="112" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="D112" s="19"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Dim_item_sets test status codes
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1A7790-6FAD-7046-919F-FC398B830DD1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB09DB16-4A53-5740-9179-FCE4043CA46F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2606" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2606" uniqueCount="607">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1464,9 +1464,6 @@
     <t>pElywX5bn06</t>
   </si>
   <si>
-    <t>KnownNewResult</t>
-  </si>
-  <si>
     <t>bDWsPYyXgWP</t>
   </si>
   <si>
@@ -1852,6 +1849,15 @@
   </si>
   <si>
     <t>as_new</t>
+  </si>
+  <si>
+    <t>tss_NewPos</t>
+  </si>
+  <si>
+    <t>tss_KnowPos</t>
+  </si>
+  <si>
+    <t>tss_NewNeg</t>
   </si>
 </sst>
 </file>
@@ -2287,7 +2293,7 @@
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7551,8 +7557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
   <dimension ref="A1:AE112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110"/>
+    <sheetView tabSelected="1" topLeftCell="F57" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J77" sqref="J77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7653,16 +7659,16 @@
         <v>470</v>
       </c>
       <c r="AB1" t="s">
-        <v>475</v>
+        <v>500</v>
       </c>
       <c r="AC1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="AD1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AE1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="18" x14ac:dyDescent="0.2">
@@ -10158,7 +10164,7 @@
         <v>tr_pos</v>
       </c>
       <c r="Y62" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="63" spans="1:28" ht="18" x14ac:dyDescent="0.25">
@@ -10194,30 +10200,30 @@
         <v>tr_neg</v>
       </c>
       <c r="Y63" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="64" spans="1:28" ht="19" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>475</v>
+      </c>
+      <c r="B64" s="16" t="s">
         <v>476</v>
       </c>
-      <c r="B64" s="16" t="s">
+      <c r="C64" s="14" t="s">
+        <v>478</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="E64" s="14" t="s">
         <v>477</v>
       </c>
-      <c r="C64" s="14" t="s">
-        <v>479</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="E64" s="14" t="s">
-        <v>478</v>
-      </c>
       <c r="F64" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="G64" s="1" t="s">
         <v>488</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>489</v>
       </c>
       <c r="H64">
         <v>10</v>
@@ -10227,33 +10233,33 @@
       </c>
       <c r="J64" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>KnownNewResult</v>
+        <v>tss_NewPos</v>
       </c>
       <c r="AB64" t="s">
-        <v>475</v>
+        <v>604</v>
       </c>
     </row>
     <row r="65" spans="1:30" ht="19" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>475</v>
+      </c>
+      <c r="B65" s="16" t="s">
         <v>476</v>
       </c>
-      <c r="B65" s="16" t="s">
-        <v>477</v>
-      </c>
       <c r="C65" s="16" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E65" s="14" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F65" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="G65" s="1" t="s">
         <v>484</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>485</v>
       </c>
       <c r="H65">
         <v>20</v>
@@ -10263,33 +10269,33 @@
       </c>
       <c r="J65" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>KnownNewResult</v>
+        <v>tss_KnowPos</v>
       </c>
       <c r="AB65" t="s">
-        <v>475</v>
+        <v>605</v>
       </c>
     </row>
     <row r="66" spans="1:30" ht="19" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>475</v>
+      </c>
+      <c r="B66" s="16" t="s">
         <v>476</v>
       </c>
-      <c r="B66" s="16" t="s">
-        <v>477</v>
-      </c>
       <c r="C66" s="16" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E66" s="16" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F66" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="G66" s="1" t="s">
         <v>486</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>487</v>
       </c>
       <c r="H66">
         <v>30</v>
@@ -10299,33 +10305,33 @@
       </c>
       <c r="J66" s="6" t="str">
         <f t="shared" ref="J66:J110" si="2">_xlfn.TEXTJOIN(";",1,K66:ZZ66)</f>
-        <v>KnownNewResult</v>
+        <v>tss_NewNeg</v>
       </c>
       <c r="AB66" t="s">
-        <v>475</v>
+        <v>606</v>
       </c>
     </row>
     <row r="67" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>489</v>
+      </c>
+      <c r="B67" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B67" s="16" t="s">
+      <c r="C67" s="17" t="s">
         <v>491</v>
       </c>
-      <c r="C67" s="17" t="s">
-        <v>492</v>
-      </c>
       <c r="D67" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="E67" s="16" t="s">
         <v>494</v>
       </c>
-      <c r="E67" s="16" t="s">
+      <c r="F67" s="16" t="s">
+        <v>494</v>
+      </c>
+      <c r="G67" s="16" t="s">
         <v>495</v>
-      </c>
-      <c r="F67" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="G67" s="16" t="s">
-        <v>496</v>
       </c>
       <c r="H67">
         <v>1</v>
@@ -10338,30 +10344,30 @@
         <v>vt_sv</v>
       </c>
       <c r="AC67" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="68" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>489</v>
+      </c>
+      <c r="B68" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B68" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C68" s="17" t="s">
+        <v>492</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="D68" s="2" t="s">
-        <v>494</v>
-      </c>
       <c r="E68" s="16" t="s">
+        <v>498</v>
+      </c>
+      <c r="F68" s="16" t="s">
+        <v>498</v>
+      </c>
+      <c r="G68" s="16" t="s">
         <v>499</v>
-      </c>
-      <c r="F68" s="16" t="s">
-        <v>499</v>
-      </c>
-      <c r="G68" s="16" t="s">
-        <v>500</v>
       </c>
       <c r="H68">
         <v>2</v>
@@ -10374,30 +10380,30 @@
         <v>vt_pe</v>
       </c>
       <c r="AC68" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="69" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>489</v>
+      </c>
+      <c r="B69" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B69" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C69" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E69" s="14" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F69" t="s">
+        <v>568</v>
+      </c>
+      <c r="G69" t="s">
         <v>569</v>
-      </c>
-      <c r="G69" t="s">
-        <v>570</v>
       </c>
       <c r="H69">
         <v>10</v>
@@ -10410,30 +10416,30 @@
         <v>st_da</v>
       </c>
       <c r="AD69" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="70" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>489</v>
+      </c>
+      <c r="B70" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B70" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C70" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E70" s="14" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F70" t="s">
+        <v>568</v>
+      </c>
+      <c r="G70" t="s">
         <v>569</v>
-      </c>
-      <c r="G70" t="s">
-        <v>570</v>
       </c>
       <c r="H70">
         <v>20</v>
@@ -10446,30 +10452,30 @@
         <v>st_da</v>
       </c>
       <c r="AD70" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="71" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>489</v>
+      </c>
+      <c r="B71" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B71" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C71" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E71" s="14" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F71" t="s">
+        <v>568</v>
+      </c>
+      <c r="G71" t="s">
         <v>569</v>
-      </c>
-      <c r="G71" t="s">
-        <v>570</v>
       </c>
       <c r="H71">
         <v>30</v>
@@ -10482,30 +10488,30 @@
         <v>st_da</v>
       </c>
       <c r="AD71" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="72" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>489</v>
+      </c>
+      <c r="B72" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B72" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C72" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E72" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F72" t="s">
+        <v>568</v>
+      </c>
+      <c r="G72" t="s">
         <v>569</v>
-      </c>
-      <c r="G72" t="s">
-        <v>570</v>
       </c>
       <c r="H72">
         <v>40</v>
@@ -10518,30 +10524,30 @@
         <v>st_da</v>
       </c>
       <c r="AD72" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="73" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>489</v>
+      </c>
+      <c r="B73" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B73" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C73" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E73" s="14" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F73" t="s">
+        <v>568</v>
+      </c>
+      <c r="G73" t="s">
         <v>569</v>
-      </c>
-      <c r="G73" t="s">
-        <v>570</v>
       </c>
       <c r="H73">
         <v>50</v>
@@ -10554,30 +10560,30 @@
         <v>st_da</v>
       </c>
       <c r="AD73" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="74" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>489</v>
+      </c>
+      <c r="B74" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B74" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C74" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E74" s="14" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F74" t="s">
+        <v>568</v>
+      </c>
+      <c r="G74" t="s">
         <v>569</v>
-      </c>
-      <c r="G74" t="s">
-        <v>570</v>
       </c>
       <c r="H74">
         <v>60</v>
@@ -10590,30 +10596,30 @@
         <v>st_da</v>
       </c>
       <c r="AD74" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="75" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>489</v>
+      </c>
+      <c r="B75" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B75" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C75" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E75" s="14" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F75" t="s">
+        <v>568</v>
+      </c>
+      <c r="G75" t="s">
         <v>569</v>
-      </c>
-      <c r="G75" t="s">
-        <v>570</v>
       </c>
       <c r="H75">
         <v>70</v>
@@ -10626,30 +10632,30 @@
         <v>st_da</v>
       </c>
       <c r="AD75" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="76" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>489</v>
+      </c>
+      <c r="B76" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B76" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C76" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E76" s="14" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F76" t="s">
+        <v>568</v>
+      </c>
+      <c r="G76" t="s">
         <v>569</v>
-      </c>
-      <c r="G76" t="s">
-        <v>570</v>
       </c>
       <c r="H76">
         <v>80</v>
@@ -10662,30 +10668,30 @@
         <v>st_da</v>
       </c>
       <c r="AD76" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="77" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>489</v>
+      </c>
+      <c r="B77" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B77" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C77" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E77" s="14" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F77" t="s">
+        <v>568</v>
+      </c>
+      <c r="G77" t="s">
         <v>569</v>
-      </c>
-      <c r="G77" t="s">
-        <v>570</v>
       </c>
       <c r="H77">
         <v>90</v>
@@ -10698,30 +10704,30 @@
         <v>st_da</v>
       </c>
       <c r="AD77" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="78" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>489</v>
+      </c>
+      <c r="B78" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B78" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C78" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E78" s="14" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F78" t="s">
+        <v>568</v>
+      </c>
+      <c r="G78" t="s">
         <v>569</v>
-      </c>
-      <c r="G78" t="s">
-        <v>570</v>
       </c>
       <c r="H78">
         <v>100</v>
@@ -10734,30 +10740,30 @@
         <v>st_da</v>
       </c>
       <c r="AD78" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="79" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>489</v>
+      </c>
+      <c r="B79" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B79" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C79" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E79" s="14" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F79" t="s">
+        <v>568</v>
+      </c>
+      <c r="G79" t="s">
         <v>569</v>
-      </c>
-      <c r="G79" t="s">
-        <v>570</v>
       </c>
       <c r="H79">
         <v>110</v>
@@ -10770,30 +10776,30 @@
         <v>st_da</v>
       </c>
       <c r="AD79" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="80" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>489</v>
+      </c>
+      <c r="B80" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B80" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C80" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E80" s="14" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F80" t="s">
+        <v>568</v>
+      </c>
+      <c r="G80" t="s">
         <v>569</v>
-      </c>
-      <c r="G80" t="s">
-        <v>570</v>
       </c>
       <c r="H80">
         <v>120</v>
@@ -10806,30 +10812,30 @@
         <v>st_da</v>
       </c>
       <c r="AD80" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="81" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>489</v>
+      </c>
+      <c r="B81" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B81" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C81" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E81" s="14" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F81" t="s">
+        <v>568</v>
+      </c>
+      <c r="G81" t="s">
         <v>569</v>
-      </c>
-      <c r="G81" t="s">
-        <v>570</v>
       </c>
       <c r="H81">
         <v>130</v>
@@ -10842,30 +10848,30 @@
         <v>st_da</v>
       </c>
       <c r="AD81" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="82" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>489</v>
+      </c>
+      <c r="B82" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B82" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C82" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E82" s="14" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F82" t="s">
+        <v>568</v>
+      </c>
+      <c r="G82" t="s">
         <v>569</v>
-      </c>
-      <c r="G82" t="s">
-        <v>570</v>
       </c>
       <c r="H82">
         <v>140</v>
@@ -10878,30 +10884,30 @@
         <v>st_da</v>
       </c>
       <c r="AD82" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="83" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>489</v>
+      </c>
+      <c r="B83" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B83" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C83" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E83" s="14" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F83" t="s">
+        <v>568</v>
+      </c>
+      <c r="G83" t="s">
         <v>569</v>
-      </c>
-      <c r="G83" t="s">
-        <v>570</v>
       </c>
       <c r="H83">
         <v>150</v>
@@ -10914,30 +10920,30 @@
         <v>st_da</v>
       </c>
       <c r="AD83" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="84" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>489</v>
+      </c>
+      <c r="B84" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B84" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C84" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E84" s="14" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F84" t="s">
+        <v>568</v>
+      </c>
+      <c r="G84" t="s">
         <v>569</v>
-      </c>
-      <c r="G84" t="s">
-        <v>570</v>
       </c>
       <c r="H84">
         <v>160</v>
@@ -10950,30 +10956,30 @@
         <v>st_da</v>
       </c>
       <c r="AD84" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="85" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>489</v>
+      </c>
+      <c r="B85" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B85" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C85" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E85" s="14" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F85" t="s">
+        <v>570</v>
+      </c>
+      <c r="G85" t="s">
         <v>571</v>
-      </c>
-      <c r="G85" t="s">
-        <v>572</v>
       </c>
       <c r="H85">
         <v>170</v>
@@ -10986,30 +10992,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD85" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="86" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>489</v>
+      </c>
+      <c r="B86" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B86" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C86" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E86" s="14" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F86" t="s">
+        <v>570</v>
+      </c>
+      <c r="G86" t="s">
         <v>571</v>
-      </c>
-      <c r="G86" t="s">
-        <v>572</v>
       </c>
       <c r="H86">
         <v>180</v>
@@ -11022,30 +11028,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD86" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="87" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>489</v>
+      </c>
+      <c r="B87" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B87" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C87" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E87" s="14" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F87" t="s">
+        <v>570</v>
+      </c>
+      <c r="G87" t="s">
         <v>571</v>
-      </c>
-      <c r="G87" t="s">
-        <v>572</v>
       </c>
       <c r="H87">
         <v>190</v>
@@ -11058,30 +11064,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD87" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="88" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>489</v>
+      </c>
+      <c r="B88" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B88" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C88" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E88" s="14" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F88" t="s">
+        <v>570</v>
+      </c>
+      <c r="G88" t="s">
         <v>571</v>
-      </c>
-      <c r="G88" t="s">
-        <v>572</v>
       </c>
       <c r="H88">
         <v>200</v>
@@ -11094,30 +11100,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD88" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="89" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>489</v>
+      </c>
+      <c r="B89" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B89" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C89" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E89" s="14" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F89" t="s">
+        <v>570</v>
+      </c>
+      <c r="G89" t="s">
         <v>571</v>
-      </c>
-      <c r="G89" t="s">
-        <v>572</v>
       </c>
       <c r="H89">
         <v>210</v>
@@ -11130,30 +11136,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD89" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="90" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>489</v>
+      </c>
+      <c r="B90" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B90" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C90" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E90" s="14" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F90" t="s">
+        <v>570</v>
+      </c>
+      <c r="G90" t="s">
         <v>571</v>
-      </c>
-      <c r="G90" t="s">
-        <v>572</v>
       </c>
       <c r="H90">
         <v>220</v>
@@ -11166,30 +11172,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD90" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="91" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>489</v>
+      </c>
+      <c r="B91" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B91" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C91" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E91" s="14" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F91" t="s">
+        <v>570</v>
+      </c>
+      <c r="G91" t="s">
         <v>571</v>
-      </c>
-      <c r="G91" t="s">
-        <v>572</v>
       </c>
       <c r="H91">
         <v>230</v>
@@ -11202,30 +11208,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD91" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="92" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>489</v>
+      </c>
+      <c r="B92" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B92" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C92" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E92" s="14" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F92" t="s">
+        <v>570</v>
+      </c>
+      <c r="G92" t="s">
         <v>571</v>
-      </c>
-      <c r="G92" t="s">
-        <v>572</v>
       </c>
       <c r="H92">
         <v>240</v>
@@ -11238,30 +11244,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD92" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="93" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>489</v>
+      </c>
+      <c r="B93" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B93" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C93" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E93" s="14" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F93" t="s">
+        <v>570</v>
+      </c>
+      <c r="G93" t="s">
         <v>571</v>
-      </c>
-      <c r="G93" t="s">
-        <v>572</v>
       </c>
       <c r="H93">
         <v>250</v>
@@ -11274,30 +11280,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD93" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="94" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>489</v>
+      </c>
+      <c r="B94" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B94" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C94" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E94" s="14" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F94" t="s">
+        <v>570</v>
+      </c>
+      <c r="G94" t="s">
         <v>571</v>
-      </c>
-      <c r="G94" t="s">
-        <v>572</v>
       </c>
       <c r="H94">
         <v>260</v>
@@ -11310,30 +11316,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD94" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="95" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>489</v>
+      </c>
+      <c r="B95" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B95" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C95" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E95" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F95" t="s">
+        <v>570</v>
+      </c>
+      <c r="G95" t="s">
         <v>571</v>
-      </c>
-      <c r="G95" t="s">
-        <v>572</v>
       </c>
       <c r="H95">
         <v>270</v>
@@ -11346,30 +11352,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD95" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="96" spans="1:30" ht="18" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>489</v>
+      </c>
+      <c r="B96" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B96" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C96" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E96" s="14" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F96" t="s">
+        <v>570</v>
+      </c>
+      <c r="G96" t="s">
         <v>571</v>
-      </c>
-      <c r="G96" t="s">
-        <v>572</v>
       </c>
       <c r="H96">
         <v>280</v>
@@ -11382,30 +11388,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD96" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="97" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>489</v>
+      </c>
+      <c r="B97" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B97" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C97" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E97" s="14" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F97" t="s">
+        <v>570</v>
+      </c>
+      <c r="G97" t="s">
         <v>571</v>
-      </c>
-      <c r="G97" t="s">
-        <v>572</v>
       </c>
       <c r="H97">
         <v>290</v>
@@ -11418,30 +11424,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD97" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="98" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>489</v>
+      </c>
+      <c r="B98" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B98" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C98" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E98" s="14" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F98" t="s">
+        <v>570</v>
+      </c>
+      <c r="G98" t="s">
         <v>571</v>
-      </c>
-      <c r="G98" t="s">
-        <v>572</v>
       </c>
       <c r="H98">
         <v>300</v>
@@ -11454,30 +11460,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD98" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="99" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>489</v>
+      </c>
+      <c r="B99" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B99" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C99" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E99" s="14" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F99" t="s">
+        <v>570</v>
+      </c>
+      <c r="G99" t="s">
         <v>571</v>
-      </c>
-      <c r="G99" t="s">
-        <v>572</v>
       </c>
       <c r="H99">
         <v>310</v>
@@ -11490,30 +11496,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD99" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="100" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>489</v>
+      </c>
+      <c r="B100" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B100" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C100" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E100" s="14" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F100" t="s">
+        <v>570</v>
+      </c>
+      <c r="G100" t="s">
         <v>571</v>
-      </c>
-      <c r="G100" t="s">
-        <v>572</v>
       </c>
       <c r="H100">
         <v>320</v>
@@ -11526,24 +11532,24 @@
         <v>st_ua</v>
       </c>
       <c r="AD100" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="101" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>489</v>
+      </c>
+      <c r="B101" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B101" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C101" s="18" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>386</v>
       </c>
       <c r="E101" s="18" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F101" s="18" t="s">
         <v>312</v>
@@ -11562,24 +11568,24 @@
         <v>kp2</v>
       </c>
       <c r="X101" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="102" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
+        <v>489</v>
+      </c>
+      <c r="B102" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B102" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C102" s="18" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>386</v>
       </c>
       <c r="E102" s="18" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F102" s="18" t="s">
         <v>372</v>
@@ -11598,24 +11604,24 @@
         <v>kp2</v>
       </c>
       <c r="X102" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="103" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
+        <v>489</v>
+      </c>
+      <c r="B103" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B103" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C103" s="18" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>386</v>
       </c>
       <c r="E103" s="18" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F103" s="18" t="s">
         <v>375</v>
@@ -11634,24 +11640,24 @@
         <v>kp2</v>
       </c>
       <c r="X103" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="104" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
+        <v>489</v>
+      </c>
+      <c r="B104" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B104" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C104" s="18" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>386</v>
       </c>
       <c r="E104" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F104" s="18" t="s">
         <v>377</v>
@@ -11670,24 +11676,24 @@
         <v>kp2</v>
       </c>
       <c r="X104" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="105" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
+        <v>489</v>
+      </c>
+      <c r="B105" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B105" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C105" s="18" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>386</v>
       </c>
       <c r="E105" s="18" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F105" s="18" t="s">
         <v>373</v>
@@ -11706,24 +11712,24 @@
         <v>kp2</v>
       </c>
       <c r="X105" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="106" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
+        <v>489</v>
+      </c>
+      <c r="B106" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B106" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C106" s="18" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>386</v>
       </c>
       <c r="E106" s="18" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F106" s="18" t="s">
         <v>382</v>
@@ -11742,24 +11748,24 @@
         <v>kp2</v>
       </c>
       <c r="X106" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="107" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
+        <v>489</v>
+      </c>
+      <c r="B107" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B107" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C107" s="18" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>386</v>
       </c>
       <c r="E107" s="18" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="F107" s="18" t="s">
         <v>378</v>
@@ -11778,24 +11784,24 @@
         <v>kp2</v>
       </c>
       <c r="X107" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="108" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
+        <v>489</v>
+      </c>
+      <c r="B108" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="B108" s="16" t="s">
-        <v>491</v>
-      </c>
       <c r="C108" s="18" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>386</v>
       </c>
       <c r="E108" s="18" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F108" s="18" t="s">
         <v>381</v>
@@ -11814,30 +11820,30 @@
         <v>kp2</v>
       </c>
       <c r="X108" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="109" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A109" s="16" t="s">
+        <v>593</v>
+      </c>
+      <c r="B109" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="C109" s="16" t="s">
+        <v>595</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="E109" t="s">
         <v>594</v>
       </c>
-      <c r="B109" s="16" t="s">
-        <v>593</v>
-      </c>
-      <c r="C109" s="16" t="s">
+      <c r="F109" s="14" t="s">
         <v>596</v>
       </c>
-      <c r="D109" s="2" t="s">
-        <v>592</v>
-      </c>
-      <c r="E109" t="s">
-        <v>595</v>
-      </c>
-      <c r="F109" s="14" t="s">
+      <c r="G109" s="16" t="s">
         <v>597</v>
-      </c>
-      <c r="G109" s="16" t="s">
-        <v>598</v>
       </c>
       <c r="H109">
         <v>510</v>
@@ -11850,30 +11856,30 @@
         <v>as_already</v>
       </c>
       <c r="AE109" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="110" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A110" s="16" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B110" s="16" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C110" s="16" t="s">
+        <v>600</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="E110" t="s">
         <v>601</v>
       </c>
-      <c r="D110" s="2" t="s">
-        <v>592</v>
-      </c>
-      <c r="E110" t="s">
-        <v>602</v>
-      </c>
       <c r="F110" s="14" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="G110" s="16" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="H110">
         <v>520</v>
@@ -11886,7 +11892,7 @@
         <v>as_new</v>
       </c>
       <c r="AE110" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="112" spans="1:31" ht="18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add prep new key pop items to dim_item_sets config file
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB09DB16-4A53-5740-9179-FCE4043CA46F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5374A7C5-4CDB-B043-BD5E-B54B3E75849E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2606" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2638" uniqueCount="614">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1858,13 +1858,34 @@
   </si>
   <si>
     <t>tss_NewNeg</t>
+  </si>
+  <si>
+    <t>RbB7UEptrN6</t>
+  </si>
+  <si>
+    <t>j8AfwCZj95X</t>
+  </si>
+  <si>
+    <t>GMK9eIdXAob</t>
+  </si>
+  <si>
+    <t>Other Key Populations</t>
+  </si>
+  <si>
+    <t>PmA9jG2I2PY</t>
+  </si>
+  <si>
+    <t>bQfzRTksp0Y</t>
+  </si>
+  <si>
+    <t>kp3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1922,12 +1943,6 @@
       <name val="Lucida Grande"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FF881280"/>
-      <name val="Courier New"/>
-      <family val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1949,7 +1964,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1973,7 +1988,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2291,9 +2305,9 @@
   <dimension ref="A1:Z56"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomLeft" activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7555,10 +7569,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
-  <dimension ref="A1:AE112"/>
+  <dimension ref="A1:AE114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F57" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J77" sqref="J77"/>
+    <sheetView tabSelected="1" topLeftCell="K95" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="W114" sqref="W114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10304,7 +10318,7 @@
         <v>1</v>
       </c>
       <c r="J66" s="6" t="str">
-        <f t="shared" ref="J66:J110" si="2">_xlfn.TEXTJOIN(";",1,K66:ZZ66)</f>
+        <f t="shared" ref="J66:J114" si="2">_xlfn.TEXTJOIN(";",1,K66:ZZ66)</f>
         <v>tss_NewNeg</v>
       </c>
       <c r="AB66" t="s">
@@ -11895,8 +11909,149 @@
         <v>603</v>
       </c>
     </row>
+    <row r="111" spans="1:31" ht="18" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>489</v>
+      </c>
+      <c r="B111" s="16" t="s">
+        <v>490</v>
+      </c>
+      <c r="C111" s="18" t="s">
+        <v>607</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="E111" s="18" t="s">
+        <v>319</v>
+      </c>
+      <c r="F111" s="18" t="s">
+        <v>319</v>
+      </c>
+      <c r="G111" s="18" t="s">
+        <v>318</v>
+      </c>
+      <c r="H111">
+        <v>610</v>
+      </c>
+      <c r="I111" s="7">
+        <v>1</v>
+      </c>
+      <c r="J111" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>kp3</v>
+      </c>
+      <c r="X111" t="s">
+        <v>613</v>
+      </c>
+    </row>
     <row r="112" spans="1:31" ht="18" x14ac:dyDescent="0.25">
-      <c r="D112" s="19"/>
+      <c r="A112" t="s">
+        <v>489</v>
+      </c>
+      <c r="B112" s="16" t="s">
+        <v>490</v>
+      </c>
+      <c r="C112" s="18" t="s">
+        <v>608</v>
+      </c>
+      <c r="D112" s="18" t="s">
+        <v>386</v>
+      </c>
+      <c r="E112" s="18" t="s">
+        <v>610</v>
+      </c>
+      <c r="F112" s="18" t="s">
+        <v>610</v>
+      </c>
+      <c r="G112" s="18" t="s">
+        <v>609</v>
+      </c>
+      <c r="H112">
+        <v>620</v>
+      </c>
+      <c r="I112" s="7">
+        <v>1</v>
+      </c>
+      <c r="J112" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>kp3</v>
+      </c>
+      <c r="X112" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="113" spans="1:24" ht="18" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>489</v>
+      </c>
+      <c r="B113" s="16" t="s">
+        <v>490</v>
+      </c>
+      <c r="C113" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="D113" s="18" t="s">
+        <v>386</v>
+      </c>
+      <c r="E113" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="F113" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="G113" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="H113">
+        <v>630</v>
+      </c>
+      <c r="I113" s="7">
+        <v>1</v>
+      </c>
+      <c r="J113" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>kp3</v>
+      </c>
+      <c r="X113" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="114" spans="1:24" ht="18" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>489</v>
+      </c>
+      <c r="B114" s="16" t="s">
+        <v>490</v>
+      </c>
+      <c r="C114" s="18" t="s">
+        <v>612</v>
+      </c>
+      <c r="D114" s="18" t="s">
+        <v>386</v>
+      </c>
+      <c r="E114" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="F114" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="G114" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="H114">
+        <v>640</v>
+      </c>
+      <c r="I114" s="7">
+        <v>1</v>
+      </c>
+      <c r="J114" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>kp3</v>
+      </c>
+      <c r="X114" t="s">
+        <v>613</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A4:W61">

</xml_diff>

<commit_message>
Add ti (test indication) column to dim_item_sets config file
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5374A7C5-4CDB-B043-BD5E-B54B3E75849E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDC3BD1-ED77-A342-B47D-D77A246F9B79}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2638" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2639" uniqueCount="615">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1879,6 +1879,9 @@
   </si>
   <si>
     <t>kp3</t>
+  </si>
+  <si>
+    <t>ti</t>
   </si>
 </sst>
 </file>
@@ -7569,10 +7572,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
-  <dimension ref="A1:AE114"/>
+  <dimension ref="A1:AF114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K95" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="W114" sqref="W114"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7590,7 +7593,7 @@
     <col min="19" max="19" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>389</v>
       </c>
@@ -7684,8 +7687,11 @@
       <c r="AE1" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="2" spans="1:31" ht="18" x14ac:dyDescent="0.2">
+      <c r="AF1" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>294</v>
       </c>
@@ -7729,7 +7735,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>294</v>
       </c>
@@ -7773,7 +7779,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>294</v>
       </c>
@@ -7815,7 +7821,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>294</v>
       </c>
@@ -7852,7 +7858,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>294</v>
       </c>
@@ -7885,7 +7891,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>294</v>
       </c>
@@ -7935,7 +7941,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>294</v>
       </c>
@@ -7971,7 +7977,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>294</v>
       </c>
@@ -8010,7 +8016,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>294</v>
       </c>
@@ -8057,7 +8063,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>294</v>
       </c>
@@ -8093,7 +8099,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>294</v>
       </c>
@@ -8145,7 +8151,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>294</v>
       </c>
@@ -8181,7 +8187,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>237</v>
       </c>
@@ -8224,7 +8230,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="15" spans="1:31" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:32" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>294</v>
       </c>
@@ -8260,7 +8266,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>237</v>
       </c>

</xml_diff>

<commit_message>
Addins rows to dim_item_sets config file for testindication = routine
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDC3BD1-ED77-A342-B47D-D77A246F9B79}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A8DBA3-0862-4745-B18E-C3FF89FB6D4F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2639" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2671" uniqueCount="626">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1882,6 +1882,39 @@
   </si>
   <si>
     <t>ti</t>
+  </si>
+  <si>
+    <t>&lt;15, Female, Routine, Positive</t>
+  </si>
+  <si>
+    <t>GeL5oP9wATo</t>
+  </si>
+  <si>
+    <t>15+, Female, Routine, Positive</t>
+  </si>
+  <si>
+    <t>v6YVL9IVWdw</t>
+  </si>
+  <si>
+    <t>&lt;15, Male, Routine, Positive</t>
+  </si>
+  <si>
+    <t>cvAG22BILFC</t>
+  </si>
+  <si>
+    <t>15+, Male, Routine, Positive</t>
+  </si>
+  <si>
+    <t>rtTEeMyntFT</t>
+  </si>
+  <si>
+    <t>ti_routine</t>
+  </si>
+  <si>
+    <t>Routine</t>
+  </si>
+  <si>
+    <t>rGptWqlhaVU</t>
   </si>
 </sst>
 </file>
@@ -7572,10 +7605,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
-  <dimension ref="A1:AF114"/>
+  <dimension ref="A1:AF118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="W98" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="X115" sqref="X115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10324,7 +10357,7 @@
         <v>1</v>
       </c>
       <c r="J66" s="6" t="str">
-        <f t="shared" ref="J66:J114" si="2">_xlfn.TEXTJOIN(";",1,K66:ZZ66)</f>
+        <f t="shared" ref="J66:J118" si="2">_xlfn.TEXTJOIN(";",1,K66:ZZ66)</f>
         <v>tss_NewNeg</v>
       </c>
       <c r="AB66" t="s">
@@ -11987,7 +12020,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="113" spans="1:24" ht="18" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:32" ht="18" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>489</v>
       </c>
@@ -12023,7 +12056,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="114" spans="1:24" ht="18" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:32" ht="18" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>489</v>
       </c>
@@ -12057,6 +12090,150 @@
       </c>
       <c r="X114" t="s">
         <v>613</v>
+      </c>
+    </row>
+    <row r="115" spans="1:32" ht="18" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>489</v>
+      </c>
+      <c r="B115" s="16" t="s">
+        <v>490</v>
+      </c>
+      <c r="C115" t="s">
+        <v>616</v>
+      </c>
+      <c r="D115" s="18" t="s">
+        <v>614</v>
+      </c>
+      <c r="E115" t="s">
+        <v>615</v>
+      </c>
+      <c r="F115" s="18" t="s">
+        <v>624</v>
+      </c>
+      <c r="G115" s="16" t="s">
+        <v>625</v>
+      </c>
+      <c r="H115">
+        <v>710</v>
+      </c>
+      <c r="I115" s="7">
+        <v>1</v>
+      </c>
+      <c r="J115" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>ti_routine</v>
+      </c>
+      <c r="AF115" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="116" spans="1:32" ht="18" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>489</v>
+      </c>
+      <c r="B116" s="16" t="s">
+        <v>490</v>
+      </c>
+      <c r="C116" t="s">
+        <v>618</v>
+      </c>
+      <c r="D116" s="18" t="s">
+        <v>614</v>
+      </c>
+      <c r="E116" t="s">
+        <v>617</v>
+      </c>
+      <c r="F116" s="18" t="s">
+        <v>624</v>
+      </c>
+      <c r="G116" s="16" t="s">
+        <v>625</v>
+      </c>
+      <c r="H116">
+        <v>720</v>
+      </c>
+      <c r="I116" s="7">
+        <v>1</v>
+      </c>
+      <c r="J116" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>ti_routine</v>
+      </c>
+      <c r="AF116" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="117" spans="1:32" ht="18" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>489</v>
+      </c>
+      <c r="B117" s="16" t="s">
+        <v>490</v>
+      </c>
+      <c r="C117" t="s">
+        <v>620</v>
+      </c>
+      <c r="D117" s="18" t="s">
+        <v>614</v>
+      </c>
+      <c r="E117" t="s">
+        <v>619</v>
+      </c>
+      <c r="F117" s="18" t="s">
+        <v>624</v>
+      </c>
+      <c r="G117" s="16" t="s">
+        <v>625</v>
+      </c>
+      <c r="H117">
+        <v>730</v>
+      </c>
+      <c r="I117" s="7">
+        <v>1</v>
+      </c>
+      <c r="J117" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>ti_routine</v>
+      </c>
+      <c r="AF117" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="118" spans="1:32" ht="18" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>489</v>
+      </c>
+      <c r="B118" s="16" t="s">
+        <v>490</v>
+      </c>
+      <c r="C118" t="s">
+        <v>622</v>
+      </c>
+      <c r="D118" s="18" t="s">
+        <v>614</v>
+      </c>
+      <c r="E118" t="s">
+        <v>621</v>
+      </c>
+      <c r="F118" s="18" t="s">
+        <v>624</v>
+      </c>
+      <c r="G118" s="16" t="s">
+        <v>625</v>
+      </c>
+      <c r="H118">
+        <v>740</v>
+      </c>
+      <c r="I118" s="7">
+        <v>1</v>
+      </c>
+      <c r="J118" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>ti_routine</v>
+      </c>
+      <c r="AF118" t="s">
+        <v>623</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add rows to dim_item_sets config file for HTS_INDEX test results
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A8DBA3-0862-4745-B18E-C3FF89FB6D4F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C236329-1C24-E348-9E71-F644251A6F36}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="33600" yWindow="0" windowWidth="25600" windowHeight="20480" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2671" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2687" uniqueCount="628">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1915,6 +1915,12 @@
   </si>
   <si>
     <t>rGptWqlhaVU</t>
+  </si>
+  <si>
+    <t>tr_pos2</t>
+  </si>
+  <si>
+    <t>tr_neg2</t>
   </si>
 </sst>
 </file>
@@ -7605,10 +7611,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
-  <dimension ref="A1:AF118"/>
+  <dimension ref="A1:AF120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W98" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="X115" sqref="X115"/>
+    <sheetView tabSelected="1" topLeftCell="F92" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K120" sqref="K120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10357,7 +10363,7 @@
         <v>1</v>
       </c>
       <c r="J66" s="6" t="str">
-        <f t="shared" ref="J66:J118" si="2">_xlfn.TEXTJOIN(";",1,K66:ZZ66)</f>
+        <f t="shared" ref="J66:J120" si="2">_xlfn.TEXTJOIN(";",1,K66:ZZ66)</f>
         <v>tss_NewNeg</v>
       </c>
       <c r="AB66" t="s">
@@ -12234,6 +12240,78 @@
       </c>
       <c r="AF118" t="s">
         <v>623</v>
+      </c>
+    </row>
+    <row r="119" spans="1:32" ht="19" x14ac:dyDescent="0.25">
+      <c r="A119" s="16" t="s">
+        <v>322</v>
+      </c>
+      <c r="B119" s="16" t="s">
+        <v>323</v>
+      </c>
+      <c r="C119" s="16" t="s">
+        <v>324</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="E119" s="16" t="s">
+        <v>325</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="H119">
+        <v>10</v>
+      </c>
+      <c r="I119" s="7">
+        <v>1</v>
+      </c>
+      <c r="J119" s="6" t="str">
+        <f>_xlfn.TEXTJOIN(";",1,K119:ZZ119)</f>
+        <v>tr_pos2</v>
+      </c>
+      <c r="Y119" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="120" spans="1:32" ht="19" x14ac:dyDescent="0.25">
+      <c r="A120" s="16" t="s">
+        <v>322</v>
+      </c>
+      <c r="B120" s="16" t="s">
+        <v>323</v>
+      </c>
+      <c r="C120" s="16" t="s">
+        <v>326</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="E120" s="16" t="s">
+        <v>327</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="G120" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="H120">
+        <v>20</v>
+      </c>
+      <c r="I120" s="7">
+        <v>1</v>
+      </c>
+      <c r="J120" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>tr_neg2</v>
+      </c>
+      <c r="Y120" t="s">
+        <v>627</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dim_item_sets config file change categoryOptionCombo to Category option combo for dimension name column
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C236329-1C24-E348-9E71-F644251A6F36}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8ED6A53-5B66-B444-920E-D97CDF5C2490}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="0" windowWidth="25600" windowHeight="20480" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1509,9 +1510,6 @@
     <t>co</t>
   </si>
   <si>
-    <t>categoryOptionCombo</t>
-  </si>
-  <si>
     <t>Cieg8r0FOGJ</t>
   </si>
   <si>
@@ -1921,6 +1919,9 @@
   </si>
   <si>
     <t>tr_neg2</t>
+  </si>
+  <si>
+    <t>Category option combo</t>
   </si>
 </sst>
 </file>
@@ -7613,8 +7614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
   <dimension ref="A1:AF120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F92" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K120" sqref="K120"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7715,19 +7716,19 @@
         <v>470</v>
       </c>
       <c r="AB1" t="s">
+        <v>499</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>492</v>
+      </c>
+      <c r="AD1" t="s">
         <v>500</v>
       </c>
-      <c r="AC1" t="s">
-        <v>493</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>501</v>
-      </c>
       <c r="AE1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="AF1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="18" x14ac:dyDescent="0.2">
@@ -10223,7 +10224,7 @@
         <v>tr_pos</v>
       </c>
       <c r="Y62" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="63" spans="1:28" ht="18" x14ac:dyDescent="0.25">
@@ -10259,7 +10260,7 @@
         <v>tr_neg</v>
       </c>
       <c r="Y63" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="64" spans="1:28" ht="19" x14ac:dyDescent="0.25">
@@ -10273,7 +10274,7 @@
         <v>478</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E64" s="14" t="s">
         <v>477</v>
@@ -10295,7 +10296,7 @@
         <v>tss_NewPos</v>
       </c>
       <c r="AB64" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="65" spans="1:30" ht="19" x14ac:dyDescent="0.25">
@@ -10309,7 +10310,7 @@
         <v>480</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E65" s="14" t="s">
         <v>479</v>
@@ -10331,7 +10332,7 @@
         <v>tss_KnowPos</v>
       </c>
       <c r="AB65" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="66" spans="1:30" ht="19" x14ac:dyDescent="0.25">
@@ -10345,7 +10346,7 @@
         <v>482</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E66" s="16" t="s">
         <v>481</v>
@@ -10367,7 +10368,7 @@
         <v>tss_NewNeg</v>
       </c>
       <c r="AB66" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="67" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -10375,22 +10376,22 @@
         <v>489</v>
       </c>
       <c r="B67" s="16" t="s">
+        <v>627</v>
+      </c>
+      <c r="C67" s="17" t="s">
         <v>490</v>
       </c>
-      <c r="C67" s="17" t="s">
-        <v>491</v>
-      </c>
       <c r="D67" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="E67" s="16" t="s">
         <v>493</v>
       </c>
-      <c r="E67" s="16" t="s">
+      <c r="F67" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="G67" s="16" t="s">
         <v>494</v>
-      </c>
-      <c r="F67" s="16" t="s">
-        <v>494</v>
-      </c>
-      <c r="G67" s="16" t="s">
-        <v>495</v>
       </c>
       <c r="H67">
         <v>1</v>
@@ -10403,7 +10404,7 @@
         <v>vt_sv</v>
       </c>
       <c r="AC67" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="68" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -10411,22 +10412,22 @@
         <v>489</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C68" s="17" t="s">
+        <v>491</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="D68" s="2" t="s">
-        <v>493</v>
-      </c>
       <c r="E68" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="F68" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="G68" s="16" t="s">
         <v>498</v>
-      </c>
-      <c r="F68" s="16" t="s">
-        <v>498</v>
-      </c>
-      <c r="G68" s="16" t="s">
-        <v>499</v>
       </c>
       <c r="H68">
         <v>2</v>
@@ -10439,7 +10440,7 @@
         <v>vt_pe</v>
       </c>
       <c r="AC68" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="69" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -10447,22 +10448,22 @@
         <v>489</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C69" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E69" s="14" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F69" t="s">
+        <v>567</v>
+      </c>
+      <c r="G69" t="s">
         <v>568</v>
-      </c>
-      <c r="G69" t="s">
-        <v>569</v>
       </c>
       <c r="H69">
         <v>10</v>
@@ -10475,7 +10476,7 @@
         <v>st_da</v>
       </c>
       <c r="AD69" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="70" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -10483,22 +10484,22 @@
         <v>489</v>
       </c>
       <c r="B70" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C70" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E70" s="14" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F70" t="s">
+        <v>567</v>
+      </c>
+      <c r="G70" t="s">
         <v>568</v>
-      </c>
-      <c r="G70" t="s">
-        <v>569</v>
       </c>
       <c r="H70">
         <v>20</v>
@@ -10511,7 +10512,7 @@
         <v>st_da</v>
       </c>
       <c r="AD70" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="71" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -10519,22 +10520,22 @@
         <v>489</v>
       </c>
       <c r="B71" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C71" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E71" s="14" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F71" t="s">
+        <v>567</v>
+      </c>
+      <c r="G71" t="s">
         <v>568</v>
-      </c>
-      <c r="G71" t="s">
-        <v>569</v>
       </c>
       <c r="H71">
         <v>30</v>
@@ -10547,7 +10548,7 @@
         <v>st_da</v>
       </c>
       <c r="AD71" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="72" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -10555,22 +10556,22 @@
         <v>489</v>
       </c>
       <c r="B72" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C72" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E72" s="14" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F72" t="s">
+        <v>567</v>
+      </c>
+      <c r="G72" t="s">
         <v>568</v>
-      </c>
-      <c r="G72" t="s">
-        <v>569</v>
       </c>
       <c r="H72">
         <v>40</v>
@@ -10583,7 +10584,7 @@
         <v>st_da</v>
       </c>
       <c r="AD72" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="73" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -10591,22 +10592,22 @@
         <v>489</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C73" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E73" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F73" t="s">
+        <v>567</v>
+      </c>
+      <c r="G73" t="s">
         <v>568</v>
-      </c>
-      <c r="G73" t="s">
-        <v>569</v>
       </c>
       <c r="H73">
         <v>50</v>
@@ -10619,7 +10620,7 @@
         <v>st_da</v>
       </c>
       <c r="AD73" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="74" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -10627,22 +10628,22 @@
         <v>489</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C74" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E74" s="14" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F74" t="s">
+        <v>567</v>
+      </c>
+      <c r="G74" t="s">
         <v>568</v>
-      </c>
-      <c r="G74" t="s">
-        <v>569</v>
       </c>
       <c r="H74">
         <v>60</v>
@@ -10655,7 +10656,7 @@
         <v>st_da</v>
       </c>
       <c r="AD74" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="75" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -10663,22 +10664,22 @@
         <v>489</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C75" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E75" s="14" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F75" t="s">
+        <v>567</v>
+      </c>
+      <c r="G75" t="s">
         <v>568</v>
-      </c>
-      <c r="G75" t="s">
-        <v>569</v>
       </c>
       <c r="H75">
         <v>70</v>
@@ -10691,7 +10692,7 @@
         <v>st_da</v>
       </c>
       <c r="AD75" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="76" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -10699,22 +10700,22 @@
         <v>489</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C76" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E76" s="14" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F76" t="s">
+        <v>567</v>
+      </c>
+      <c r="G76" t="s">
         <v>568</v>
-      </c>
-      <c r="G76" t="s">
-        <v>569</v>
       </c>
       <c r="H76">
         <v>80</v>
@@ -10727,7 +10728,7 @@
         <v>st_da</v>
       </c>
       <c r="AD76" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="77" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -10735,22 +10736,22 @@
         <v>489</v>
       </c>
       <c r="B77" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C77" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E77" s="14" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F77" t="s">
+        <v>567</v>
+      </c>
+      <c r="G77" t="s">
         <v>568</v>
-      </c>
-      <c r="G77" t="s">
-        <v>569</v>
       </c>
       <c r="H77">
         <v>90</v>
@@ -10763,7 +10764,7 @@
         <v>st_da</v>
       </c>
       <c r="AD77" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="78" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -10771,22 +10772,22 @@
         <v>489</v>
       </c>
       <c r="B78" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C78" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E78" s="14" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F78" t="s">
+        <v>567</v>
+      </c>
+      <c r="G78" t="s">
         <v>568</v>
-      </c>
-      <c r="G78" t="s">
-        <v>569</v>
       </c>
       <c r="H78">
         <v>100</v>
@@ -10799,7 +10800,7 @@
         <v>st_da</v>
       </c>
       <c r="AD78" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="79" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -10807,22 +10808,22 @@
         <v>489</v>
       </c>
       <c r="B79" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C79" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E79" s="14" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F79" t="s">
+        <v>567</v>
+      </c>
+      <c r="G79" t="s">
         <v>568</v>
-      </c>
-      <c r="G79" t="s">
-        <v>569</v>
       </c>
       <c r="H79">
         <v>110</v>
@@ -10835,7 +10836,7 @@
         <v>st_da</v>
       </c>
       <c r="AD79" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="80" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -10843,22 +10844,22 @@
         <v>489</v>
       </c>
       <c r="B80" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C80" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E80" s="14" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F80" t="s">
+        <v>567</v>
+      </c>
+      <c r="G80" t="s">
         <v>568</v>
-      </c>
-      <c r="G80" t="s">
-        <v>569</v>
       </c>
       <c r="H80">
         <v>120</v>
@@ -10871,7 +10872,7 @@
         <v>st_da</v>
       </c>
       <c r="AD80" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="81" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -10879,22 +10880,22 @@
         <v>489</v>
       </c>
       <c r="B81" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C81" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E81" s="14" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F81" t="s">
+        <v>567</v>
+      </c>
+      <c r="G81" t="s">
         <v>568</v>
-      </c>
-      <c r="G81" t="s">
-        <v>569</v>
       </c>
       <c r="H81">
         <v>130</v>
@@ -10907,7 +10908,7 @@
         <v>st_da</v>
       </c>
       <c r="AD81" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="82" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -10915,22 +10916,22 @@
         <v>489</v>
       </c>
       <c r="B82" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C82" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E82" s="14" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F82" t="s">
+        <v>567</v>
+      </c>
+      <c r="G82" t="s">
         <v>568</v>
-      </c>
-      <c r="G82" t="s">
-        <v>569</v>
       </c>
       <c r="H82">
         <v>140</v>
@@ -10943,7 +10944,7 @@
         <v>st_da</v>
       </c>
       <c r="AD82" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="83" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -10951,22 +10952,22 @@
         <v>489</v>
       </c>
       <c r="B83" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C83" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E83" s="14" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F83" t="s">
+        <v>567</v>
+      </c>
+      <c r="G83" t="s">
         <v>568</v>
-      </c>
-      <c r="G83" t="s">
-        <v>569</v>
       </c>
       <c r="H83">
         <v>150</v>
@@ -10979,7 +10980,7 @@
         <v>st_da</v>
       </c>
       <c r="AD83" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="84" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -10987,22 +10988,22 @@
         <v>489</v>
       </c>
       <c r="B84" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C84" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E84" s="14" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F84" t="s">
+        <v>567</v>
+      </c>
+      <c r="G84" t="s">
         <v>568</v>
-      </c>
-      <c r="G84" t="s">
-        <v>569</v>
       </c>
       <c r="H84">
         <v>160</v>
@@ -11015,7 +11016,7 @@
         <v>st_da</v>
       </c>
       <c r="AD84" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="85" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -11023,22 +11024,22 @@
         <v>489</v>
       </c>
       <c r="B85" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C85" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E85" s="14" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F85" t="s">
+        <v>569</v>
+      </c>
+      <c r="G85" t="s">
         <v>570</v>
-      </c>
-      <c r="G85" t="s">
-        <v>571</v>
       </c>
       <c r="H85">
         <v>170</v>
@@ -11051,7 +11052,7 @@
         <v>st_ua</v>
       </c>
       <c r="AD85" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="86" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -11059,22 +11060,22 @@
         <v>489</v>
       </c>
       <c r="B86" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C86" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E86" s="14" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F86" t="s">
+        <v>569</v>
+      </c>
+      <c r="G86" t="s">
         <v>570</v>
-      </c>
-      <c r="G86" t="s">
-        <v>571</v>
       </c>
       <c r="H86">
         <v>180</v>
@@ -11087,7 +11088,7 @@
         <v>st_ua</v>
       </c>
       <c r="AD86" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="87" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -11095,22 +11096,22 @@
         <v>489</v>
       </c>
       <c r="B87" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C87" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E87" s="14" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F87" t="s">
+        <v>569</v>
+      </c>
+      <c r="G87" t="s">
         <v>570</v>
-      </c>
-      <c r="G87" t="s">
-        <v>571</v>
       </c>
       <c r="H87">
         <v>190</v>
@@ -11123,7 +11124,7 @@
         <v>st_ua</v>
       </c>
       <c r="AD87" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="88" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -11131,22 +11132,22 @@
         <v>489</v>
       </c>
       <c r="B88" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C88" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E88" s="14" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F88" t="s">
+        <v>569</v>
+      </c>
+      <c r="G88" t="s">
         <v>570</v>
-      </c>
-      <c r="G88" t="s">
-        <v>571</v>
       </c>
       <c r="H88">
         <v>200</v>
@@ -11159,7 +11160,7 @@
         <v>st_ua</v>
       </c>
       <c r="AD88" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="89" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -11167,22 +11168,22 @@
         <v>489</v>
       </c>
       <c r="B89" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C89" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E89" s="14" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F89" t="s">
+        <v>569</v>
+      </c>
+      <c r="G89" t="s">
         <v>570</v>
-      </c>
-      <c r="G89" t="s">
-        <v>571</v>
       </c>
       <c r="H89">
         <v>210</v>
@@ -11195,7 +11196,7 @@
         <v>st_ua</v>
       </c>
       <c r="AD89" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="90" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -11203,22 +11204,22 @@
         <v>489</v>
       </c>
       <c r="B90" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C90" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E90" s="14" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F90" t="s">
+        <v>569</v>
+      </c>
+      <c r="G90" t="s">
         <v>570</v>
-      </c>
-      <c r="G90" t="s">
-        <v>571</v>
       </c>
       <c r="H90">
         <v>220</v>
@@ -11231,7 +11232,7 @@
         <v>st_ua</v>
       </c>
       <c r="AD90" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="91" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -11239,22 +11240,22 @@
         <v>489</v>
       </c>
       <c r="B91" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C91" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E91" s="14" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F91" t="s">
+        <v>569</v>
+      </c>
+      <c r="G91" t="s">
         <v>570</v>
-      </c>
-      <c r="G91" t="s">
-        <v>571</v>
       </c>
       <c r="H91">
         <v>230</v>
@@ -11267,7 +11268,7 @@
         <v>st_ua</v>
       </c>
       <c r="AD91" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="92" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -11275,22 +11276,22 @@
         <v>489</v>
       </c>
       <c r="B92" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C92" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E92" s="14" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F92" t="s">
+        <v>569</v>
+      </c>
+      <c r="G92" t="s">
         <v>570</v>
-      </c>
-      <c r="G92" t="s">
-        <v>571</v>
       </c>
       <c r="H92">
         <v>240</v>
@@ -11303,7 +11304,7 @@
         <v>st_ua</v>
       </c>
       <c r="AD92" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="93" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -11311,22 +11312,22 @@
         <v>489</v>
       </c>
       <c r="B93" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C93" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E93" s="14" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F93" t="s">
+        <v>569</v>
+      </c>
+      <c r="G93" t="s">
         <v>570</v>
-      </c>
-      <c r="G93" t="s">
-        <v>571</v>
       </c>
       <c r="H93">
         <v>250</v>
@@ -11339,7 +11340,7 @@
         <v>st_ua</v>
       </c>
       <c r="AD93" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="94" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -11347,22 +11348,22 @@
         <v>489</v>
       </c>
       <c r="B94" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C94" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E94" s="14" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F94" t="s">
+        <v>569</v>
+      </c>
+      <c r="G94" t="s">
         <v>570</v>
-      </c>
-      <c r="G94" t="s">
-        <v>571</v>
       </c>
       <c r="H94">
         <v>260</v>
@@ -11375,7 +11376,7 @@
         <v>st_ua</v>
       </c>
       <c r="AD94" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="95" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -11383,22 +11384,22 @@
         <v>489</v>
       </c>
       <c r="B95" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C95" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E95" s="14" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F95" t="s">
+        <v>569</v>
+      </c>
+      <c r="G95" t="s">
         <v>570</v>
-      </c>
-      <c r="G95" t="s">
-        <v>571</v>
       </c>
       <c r="H95">
         <v>270</v>
@@ -11411,7 +11412,7 @@
         <v>st_ua</v>
       </c>
       <c r="AD95" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="96" spans="1:30" ht="18" x14ac:dyDescent="0.25">
@@ -11419,22 +11420,22 @@
         <v>489</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C96" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E96" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F96" t="s">
+        <v>569</v>
+      </c>
+      <c r="G96" t="s">
         <v>570</v>
-      </c>
-      <c r="G96" t="s">
-        <v>571</v>
       </c>
       <c r="H96">
         <v>280</v>
@@ -11447,7 +11448,7 @@
         <v>st_ua</v>
       </c>
       <c r="AD96" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="97" spans="1:31" ht="18" x14ac:dyDescent="0.25">
@@ -11455,22 +11456,22 @@
         <v>489</v>
       </c>
       <c r="B97" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C97" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E97" s="14" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F97" t="s">
+        <v>569</v>
+      </c>
+      <c r="G97" t="s">
         <v>570</v>
-      </c>
-      <c r="G97" t="s">
-        <v>571</v>
       </c>
       <c r="H97">
         <v>290</v>
@@ -11483,7 +11484,7 @@
         <v>st_ua</v>
       </c>
       <c r="AD97" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="98" spans="1:31" ht="18" x14ac:dyDescent="0.25">
@@ -11491,22 +11492,22 @@
         <v>489</v>
       </c>
       <c r="B98" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C98" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E98" s="14" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F98" t="s">
+        <v>569</v>
+      </c>
+      <c r="G98" t="s">
         <v>570</v>
-      </c>
-      <c r="G98" t="s">
-        <v>571</v>
       </c>
       <c r="H98">
         <v>300</v>
@@ -11519,7 +11520,7 @@
         <v>st_ua</v>
       </c>
       <c r="AD98" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="99" spans="1:31" ht="18" x14ac:dyDescent="0.25">
@@ -11527,22 +11528,22 @@
         <v>489</v>
       </c>
       <c r="B99" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C99" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E99" s="14" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F99" t="s">
+        <v>569</v>
+      </c>
+      <c r="G99" t="s">
         <v>570</v>
-      </c>
-      <c r="G99" t="s">
-        <v>571</v>
       </c>
       <c r="H99">
         <v>310</v>
@@ -11555,7 +11556,7 @@
         <v>st_ua</v>
       </c>
       <c r="AD99" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="100" spans="1:31" ht="18" x14ac:dyDescent="0.25">
@@ -11563,22 +11564,22 @@
         <v>489</v>
       </c>
       <c r="B100" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C100" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E100" s="14" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F100" t="s">
+        <v>569</v>
+      </c>
+      <c r="G100" t="s">
         <v>570</v>
-      </c>
-      <c r="G100" t="s">
-        <v>571</v>
       </c>
       <c r="H100">
         <v>320</v>
@@ -11591,7 +11592,7 @@
         <v>st_ua</v>
       </c>
       <c r="AD100" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="101" spans="1:31" ht="18" x14ac:dyDescent="0.25">
@@ -11599,16 +11600,16 @@
         <v>489</v>
       </c>
       <c r="B101" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C101" s="18" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>386</v>
       </c>
       <c r="E101" s="18" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="F101" s="18" t="s">
         <v>312</v>
@@ -11627,7 +11628,7 @@
         <v>kp2</v>
       </c>
       <c r="X101" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="102" spans="1:31" ht="18" x14ac:dyDescent="0.25">
@@ -11635,16 +11636,16 @@
         <v>489</v>
       </c>
       <c r="B102" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C102" s="18" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>386</v>
       </c>
       <c r="E102" s="18" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F102" s="18" t="s">
         <v>372</v>
@@ -11663,7 +11664,7 @@
         <v>kp2</v>
       </c>
       <c r="X102" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="103" spans="1:31" ht="18" x14ac:dyDescent="0.25">
@@ -11671,16 +11672,16 @@
         <v>489</v>
       </c>
       <c r="B103" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C103" s="18" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>386</v>
       </c>
       <c r="E103" s="18" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F103" s="18" t="s">
         <v>375</v>
@@ -11699,7 +11700,7 @@
         <v>kp2</v>
       </c>
       <c r="X103" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="104" spans="1:31" ht="18" x14ac:dyDescent="0.25">
@@ -11707,16 +11708,16 @@
         <v>489</v>
       </c>
       <c r="B104" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C104" s="18" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>386</v>
       </c>
       <c r="E104" s="18" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F104" s="18" t="s">
         <v>377</v>
@@ -11735,7 +11736,7 @@
         <v>kp2</v>
       </c>
       <c r="X104" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="105" spans="1:31" ht="18" x14ac:dyDescent="0.25">
@@ -11743,16 +11744,16 @@
         <v>489</v>
       </c>
       <c r="B105" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C105" s="18" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>386</v>
       </c>
       <c r="E105" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F105" s="18" t="s">
         <v>373</v>
@@ -11771,7 +11772,7 @@
         <v>kp2</v>
       </c>
       <c r="X105" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="106" spans="1:31" ht="18" x14ac:dyDescent="0.25">
@@ -11779,16 +11780,16 @@
         <v>489</v>
       </c>
       <c r="B106" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C106" s="18" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>386</v>
       </c>
       <c r="E106" s="18" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F106" s="18" t="s">
         <v>382</v>
@@ -11807,7 +11808,7 @@
         <v>kp2</v>
       </c>
       <c r="X106" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="107" spans="1:31" ht="18" x14ac:dyDescent="0.25">
@@ -11815,16 +11816,16 @@
         <v>489</v>
       </c>
       <c r="B107" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C107" s="18" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>386</v>
       </c>
       <c r="E107" s="18" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F107" s="18" t="s">
         <v>378</v>
@@ -11843,7 +11844,7 @@
         <v>kp2</v>
       </c>
       <c r="X107" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="108" spans="1:31" ht="18" x14ac:dyDescent="0.25">
@@ -11851,16 +11852,16 @@
         <v>489</v>
       </c>
       <c r="B108" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C108" s="18" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>386</v>
       </c>
       <c r="E108" s="18" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="F108" s="18" t="s">
         <v>381</v>
@@ -11879,30 +11880,30 @@
         <v>kp2</v>
       </c>
       <c r="X108" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="109" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A109" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="B109" s="16" t="s">
+        <v>591</v>
+      </c>
+      <c r="C109" s="16" t="s">
+        <v>594</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="E109" t="s">
         <v>593</v>
       </c>
-      <c r="B109" s="16" t="s">
-        <v>592</v>
-      </c>
-      <c r="C109" s="16" t="s">
+      <c r="F109" s="14" t="s">
         <v>595</v>
       </c>
-      <c r="D109" s="2" t="s">
-        <v>591</v>
-      </c>
-      <c r="E109" t="s">
-        <v>594</v>
-      </c>
-      <c r="F109" s="14" t="s">
+      <c r="G109" s="16" t="s">
         <v>596</v>
-      </c>
-      <c r="G109" s="16" t="s">
-        <v>597</v>
       </c>
       <c r="H109">
         <v>510</v>
@@ -11915,30 +11916,30 @@
         <v>as_already</v>
       </c>
       <c r="AE109" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="110" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A110" s="16" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B110" s="16" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C110" s="16" t="s">
+        <v>599</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="E110" t="s">
         <v>600</v>
       </c>
-      <c r="D110" s="2" t="s">
-        <v>591</v>
-      </c>
-      <c r="E110" t="s">
-        <v>601</v>
-      </c>
       <c r="F110" s="14" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G110" s="16" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="H110">
         <v>520</v>
@@ -11951,7 +11952,7 @@
         <v>as_new</v>
       </c>
       <c r="AE110" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="111" spans="1:31" ht="18" x14ac:dyDescent="0.25">
@@ -11959,10 +11960,10 @@
         <v>489</v>
       </c>
       <c r="B111" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C111" s="18" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>386</v>
@@ -11987,7 +11988,7 @@
         <v>kp3</v>
       </c>
       <c r="X111" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="112" spans="1:31" ht="18" x14ac:dyDescent="0.25">
@@ -11995,22 +11996,22 @@
         <v>489</v>
       </c>
       <c r="B112" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C112" s="18" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D112" s="18" t="s">
         <v>386</v>
       </c>
       <c r="E112" s="18" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F112" s="18" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G112" s="18" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="H112">
         <v>620</v>
@@ -12023,7 +12024,7 @@
         <v>kp3</v>
       </c>
       <c r="X112" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="113" spans="1:32" ht="18" x14ac:dyDescent="0.25">
@@ -12031,10 +12032,10 @@
         <v>489</v>
       </c>
       <c r="B113" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C113" s="18" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D113" s="18" t="s">
         <v>386</v>
@@ -12059,7 +12060,7 @@
         <v>kp3</v>
       </c>
       <c r="X113" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="114" spans="1:32" ht="18" x14ac:dyDescent="0.25">
@@ -12067,10 +12068,10 @@
         <v>489</v>
       </c>
       <c r="B114" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C114" s="18" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D114" s="18" t="s">
         <v>386</v>
@@ -12095,7 +12096,7 @@
         <v>kp3</v>
       </c>
       <c r="X114" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="115" spans="1:32" ht="18" x14ac:dyDescent="0.25">
@@ -12103,22 +12104,22 @@
         <v>489</v>
       </c>
       <c r="B115" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C115" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D115" s="18" t="s">
+        <v>613</v>
+      </c>
+      <c r="E115" t="s">
         <v>614</v>
       </c>
-      <c r="E115" t="s">
-        <v>615</v>
-      </c>
       <c r="F115" s="18" t="s">
+        <v>623</v>
+      </c>
+      <c r="G115" s="16" t="s">
         <v>624</v>
-      </c>
-      <c r="G115" s="16" t="s">
-        <v>625</v>
       </c>
       <c r="H115">
         <v>710</v>
@@ -12131,7 +12132,7 @@
         <v>ti_routine</v>
       </c>
       <c r="AF115" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="116" spans="1:32" ht="18" x14ac:dyDescent="0.25">
@@ -12139,22 +12140,22 @@
         <v>489</v>
       </c>
       <c r="B116" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C116" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D116" s="18" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E116" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F116" s="18" t="s">
+        <v>623</v>
+      </c>
+      <c r="G116" s="16" t="s">
         <v>624</v>
-      </c>
-      <c r="G116" s="16" t="s">
-        <v>625</v>
       </c>
       <c r="H116">
         <v>720</v>
@@ -12167,7 +12168,7 @@
         <v>ti_routine</v>
       </c>
       <c r="AF116" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="117" spans="1:32" ht="18" x14ac:dyDescent="0.25">
@@ -12175,22 +12176,22 @@
         <v>489</v>
       </c>
       <c r="B117" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C117" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D117" s="18" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E117" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F117" s="18" t="s">
+        <v>623</v>
+      </c>
+      <c r="G117" s="16" t="s">
         <v>624</v>
-      </c>
-      <c r="G117" s="16" t="s">
-        <v>625</v>
       </c>
       <c r="H117">
         <v>730</v>
@@ -12203,7 +12204,7 @@
         <v>ti_routine</v>
       </c>
       <c r="AF117" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="118" spans="1:32" ht="18" x14ac:dyDescent="0.25">
@@ -12211,22 +12212,22 @@
         <v>489</v>
       </c>
       <c r="B118" s="16" t="s">
-        <v>490</v>
+        <v>627</v>
       </c>
       <c r="C118" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D118" s="18" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E118" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F118" s="18" t="s">
+        <v>623</v>
+      </c>
+      <c r="G118" s="16" t="s">
         <v>624</v>
-      </c>
-      <c r="G118" s="16" t="s">
-        <v>625</v>
       </c>
       <c r="H118">
         <v>740</v>
@@ -12239,7 +12240,7 @@
         <v>ti_routine</v>
       </c>
       <c r="AF118" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="119" spans="1:32" ht="19" x14ac:dyDescent="0.25">
@@ -12275,7 +12276,7 @@
         <v>tr_pos2</v>
       </c>
       <c r="Y119" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="120" spans="1:32" ht="19" x14ac:dyDescent="0.25">
@@ -12311,11 +12312,11 @@
         <v>tr_neg2</v>
       </c>
       <c r="Y120" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A4:W61">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:W61">
     <sortCondition ref="H4:H61"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
dim_item_sets add numbers after decimal place on weight column, ensure sets always sum to 1
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8ED6A53-5B66-B444-920E-D97CDF5C2490}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B717B3BC-09BD-3B49-9F66-5FCEB99D4DBA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data_required!$A$1:$Z$56</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">dimension_Item_sets!$A$1:$X$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">dimension_Item_sets!$A$1:$AF$120</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1928,6 +1928,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2007,7 +2010,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2031,6 +2034,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7614,8 +7619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
   <dimension ref="A1:AF120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A121" sqref="A121:XFD121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7627,6 +7632,7 @@
     <col min="5" max="5" width="52.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="49.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="19" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="41.83203125" customWidth="1"/>
     <col min="11" max="13" width="12.33203125" customWidth="1"/>
     <col min="14" max="18" width="10.83203125" customWidth="1"/>
@@ -7658,7 +7664,7 @@
       <c r="H1" t="s">
         <v>199</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="19" t="s">
         <v>292</v>
       </c>
       <c r="J1" t="s">
@@ -7756,7 +7762,7 @@
       <c r="H2">
         <v>3</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="19">
         <v>1</v>
       </c>
       <c r="J2" s="6" t="str">
@@ -7800,7 +7806,7 @@
       <c r="H3">
         <v>7</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="19">
         <v>1</v>
       </c>
       <c r="J3" s="6" t="str">
@@ -7844,7 +7850,7 @@
       <c r="H4" s="9">
         <v>10</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="20">
         <v>1</v>
       </c>
       <c r="J4" s="6" t="str">
@@ -7886,7 +7892,7 @@
       <c r="H5" s="9">
         <v>10</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="20">
         <v>0.25</v>
       </c>
       <c r="J5" s="6" t="str">
@@ -7923,7 +7929,7 @@
       <c r="H6" s="8">
         <v>10</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="19">
         <v>0.2</v>
       </c>
       <c r="J6" s="6" t="str">
@@ -7956,7 +7962,7 @@
       <c r="H7" s="9">
         <v>20</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="20">
         <v>0.5</v>
       </c>
       <c r="J7" s="6" t="str">
@@ -8006,7 +8012,7 @@
       <c r="H8" s="9">
         <v>20</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="20">
         <v>0.25</v>
       </c>
       <c r="J8" s="6" t="str">
@@ -8042,7 +8048,7 @@
       <c r="H9" s="8">
         <v>20</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="19">
         <v>1</v>
       </c>
       <c r="J9" s="6" t="str">
@@ -8081,7 +8087,7 @@
       <c r="H10" s="9">
         <v>30</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="20">
         <v>0.5</v>
       </c>
       <c r="J10" s="6" t="str">
@@ -8128,7 +8134,7 @@
       <c r="H11" s="9">
         <v>30</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="20">
         <v>0.25</v>
       </c>
       <c r="J11" s="6" t="str">
@@ -8164,7 +8170,7 @@
       <c r="H12" s="9">
         <v>40</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="20">
         <v>1</v>
       </c>
       <c r="J12" s="6" t="str">
@@ -8216,7 +8222,7 @@
       <c r="H13" s="9">
         <v>40</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="20">
         <v>0.25</v>
       </c>
       <c r="J13" s="6" t="str">
@@ -8252,9 +8258,8 @@
       <c r="H14" s="9">
         <v>40</v>
       </c>
-      <c r="I14" s="6">
-        <f>1/9</f>
-        <v>0.1111111111111111</v>
+      <c r="I14" s="19">
+        <v>0.1111</v>
       </c>
       <c r="J14" s="6" t="str">
         <f t="shared" si="0"/>
@@ -8295,7 +8300,7 @@
       <c r="H15" s="9">
         <v>45</v>
       </c>
-      <c r="I15" s="6">
+      <c r="I15" s="19">
         <v>1</v>
       </c>
       <c r="J15" s="6" t="str">
@@ -8331,7 +8336,7 @@
       <c r="H16" s="9">
         <v>45</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="19">
         <v>0.5</v>
       </c>
       <c r="J16" s="6" t="str">
@@ -8367,7 +8372,7 @@
       <c r="H17" s="9">
         <v>50</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="20">
         <v>1</v>
       </c>
       <c r="J17" s="6" t="str">
@@ -8403,7 +8408,7 @@
       <c r="H18" s="9">
         <v>60</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="19">
         <v>0.125</v>
       </c>
       <c r="J18" s="6" t="str">
@@ -8439,7 +8444,7 @@
       <c r="H19" s="9">
         <v>60</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="20">
         <v>1</v>
       </c>
       <c r="J19" s="6" t="str">
@@ -8490,9 +8495,8 @@
       <c r="H20" s="9">
         <v>60</v>
       </c>
-      <c r="I20" s="6">
-        <f>1/9</f>
-        <v>0.1111111111111111</v>
+      <c r="I20" s="19">
+        <v>0.1111</v>
       </c>
       <c r="J20" s="6" t="str">
         <f t="shared" si="0"/>
@@ -8533,7 +8537,7 @@
       <c r="H21" s="10">
         <v>65</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I21" s="19">
         <v>1</v>
       </c>
       <c r="J21" s="6" t="str">
@@ -8567,7 +8571,7 @@
       <c r="H22" s="9">
         <v>65</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="19">
         <v>0.5</v>
       </c>
       <c r="J22" s="6" t="str">
@@ -8609,7 +8613,7 @@
       <c r="H23" s="9">
         <v>70</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23" s="20">
         <v>1</v>
       </c>
       <c r="J23" s="6" t="str">
@@ -8650,7 +8654,7 @@
       <c r="H24" s="9">
         <v>80</v>
       </c>
-      <c r="I24" s="7">
+      <c r="I24" s="20">
         <v>0.125</v>
       </c>
       <c r="J24" s="6" t="str">
@@ -8686,7 +8690,7 @@
       <c r="H25" s="9">
         <v>80</v>
       </c>
-      <c r="I25" s="7">
+      <c r="I25" s="20">
         <v>1</v>
       </c>
       <c r="J25" s="6" t="str">
@@ -8737,9 +8741,8 @@
       <c r="H26" s="9">
         <v>80</v>
       </c>
-      <c r="I26" s="6">
-        <f>1/9</f>
-        <v>0.1111111111111111</v>
+      <c r="I26" s="19">
+        <v>0.1111</v>
       </c>
       <c r="J26" s="6" t="str">
         <f t="shared" si="0"/>
@@ -8780,7 +8783,7 @@
       <c r="H27" s="9">
         <v>90</v>
       </c>
-      <c r="I27" s="7">
+      <c r="I27" s="20">
         <v>0.125</v>
       </c>
       <c r="J27" s="6" t="str">
@@ -8816,7 +8819,7 @@
       <c r="H28" s="9">
         <v>90</v>
       </c>
-      <c r="I28" s="7">
+      <c r="I28" s="20">
         <v>1</v>
       </c>
       <c r="J28" s="6" t="str">
@@ -8869,7 +8872,7 @@
       <c r="H29" s="9">
         <v>90</v>
       </c>
-      <c r="I29" s="7">
+      <c r="I29" s="20">
         <v>0.2</v>
       </c>
       <c r="J29" s="6" t="str">
@@ -8905,9 +8908,8 @@
       <c r="H30" s="9">
         <v>90</v>
       </c>
-      <c r="I30" s="6">
-        <f>1/9</f>
-        <v>0.1111111111111111</v>
+      <c r="I30" s="19">
+        <v>0.1111</v>
       </c>
       <c r="J30" s="6" t="str">
         <f t="shared" si="0"/>
@@ -8948,7 +8950,7 @@
       <c r="H31" s="9">
         <v>100</v>
       </c>
-      <c r="I31" s="7">
+      <c r="I31" s="20">
         <v>1</v>
       </c>
       <c r="J31" s="6" t="str">
@@ -8984,7 +8986,7 @@
       <c r="H32" s="9">
         <v>110</v>
       </c>
-      <c r="I32" s="7">
+      <c r="I32" s="20">
         <v>0.125</v>
       </c>
       <c r="J32" s="6" t="str">
@@ -9020,7 +9022,7 @@
       <c r="H33" s="9">
         <v>110</v>
       </c>
-      <c r="I33" s="7">
+      <c r="I33" s="20">
         <v>0.2</v>
       </c>
       <c r="J33" s="6" t="str">
@@ -9056,7 +9058,7 @@
       <c r="H34" s="9">
         <v>110</v>
       </c>
-      <c r="I34" s="7">
+      <c r="I34" s="20">
         <v>1</v>
       </c>
       <c r="J34" s="6" t="str">
@@ -9109,9 +9111,8 @@
       <c r="H35" s="9">
         <v>110</v>
       </c>
-      <c r="I35" s="6">
-        <f>1/9</f>
-        <v>0.1111111111111111</v>
+      <c r="I35" s="19">
+        <v>0.11119999999999999</v>
       </c>
       <c r="J35" s="6" t="str">
         <f t="shared" si="1"/>
@@ -9152,7 +9153,7 @@
       <c r="H36" s="9">
         <v>120</v>
       </c>
-      <c r="I36" s="7">
+      <c r="I36" s="20">
         <v>0.125</v>
       </c>
       <c r="J36" s="6" t="str">
@@ -9188,7 +9189,7 @@
       <c r="H37" s="9">
         <v>120</v>
       </c>
-      <c r="I37" s="7">
+      <c r="I37" s="20">
         <v>0.2</v>
       </c>
       <c r="J37" s="6" t="str">
@@ -9224,7 +9225,7 @@
       <c r="H38" s="9">
         <v>120</v>
       </c>
-      <c r="I38" s="7">
+      <c r="I38" s="20">
         <v>1</v>
       </c>
       <c r="J38" s="6" t="str">
@@ -9275,9 +9276,8 @@
       <c r="H39" s="9">
         <v>120</v>
       </c>
-      <c r="I39" s="6">
-        <f>1/9</f>
-        <v>0.1111111111111111</v>
+      <c r="I39" s="19">
+        <v>0.1111</v>
       </c>
       <c r="J39" s="6" t="str">
         <f t="shared" si="1"/>
@@ -9318,7 +9318,7 @@
       <c r="H40" s="9">
         <v>130</v>
       </c>
-      <c r="I40" s="7">
+      <c r="I40" s="20">
         <v>0.125</v>
       </c>
       <c r="J40" s="6" t="str">
@@ -9354,7 +9354,7 @@
       <c r="H41" s="9">
         <v>130</v>
       </c>
-      <c r="I41" s="7">
+      <c r="I41" s="20">
         <v>0.2</v>
       </c>
       <c r="J41" s="6" t="str">
@@ -9390,7 +9390,7 @@
       <c r="H42" s="9">
         <v>130</v>
       </c>
-      <c r="I42" s="7">
+      <c r="I42" s="20">
         <v>0.5</v>
       </c>
       <c r="J42" s="6" t="str">
@@ -9441,9 +9441,8 @@
       <c r="H43" s="9">
         <v>130</v>
       </c>
-      <c r="I43" s="6">
-        <f>1/9</f>
-        <v>0.1111111111111111</v>
+      <c r="I43" s="19">
+        <v>0.1111</v>
       </c>
       <c r="J43" s="6" t="str">
         <f t="shared" si="1"/>
@@ -9484,7 +9483,7 @@
       <c r="H44" s="9">
         <v>140</v>
       </c>
-      <c r="I44" s="7">
+      <c r="I44" s="20">
         <v>0.125</v>
       </c>
       <c r="J44" s="6" t="str">
@@ -9520,7 +9519,7 @@
       <c r="H45" s="9">
         <v>140</v>
       </c>
-      <c r="I45" s="7">
+      <c r="I45" s="20">
         <v>0.2</v>
       </c>
       <c r="J45" s="6" t="str">
@@ -9556,7 +9555,7 @@
       <c r="H46" s="9">
         <v>140</v>
       </c>
-      <c r="I46" s="7">
+      <c r="I46" s="20">
         <v>0.5</v>
       </c>
       <c r="J46" s="6" t="str">
@@ -9607,9 +9606,8 @@
       <c r="H47" s="9">
         <v>140</v>
       </c>
-      <c r="I47" s="6">
-        <f>1/9</f>
-        <v>0.1111111111111111</v>
+      <c r="I47" s="19">
+        <v>0.1111</v>
       </c>
       <c r="J47" s="6" t="str">
         <f t="shared" si="1"/>
@@ -9650,7 +9648,7 @@
       <c r="H48" s="9">
         <v>150</v>
       </c>
-      <c r="I48" s="7">
+      <c r="I48" s="20">
         <v>0.125</v>
       </c>
       <c r="J48" s="6" t="str">
@@ -9686,7 +9684,7 @@
       <c r="H49" s="9">
         <v>150</v>
       </c>
-      <c r="I49" s="7">
+      <c r="I49" s="20">
         <v>1</v>
       </c>
       <c r="J49" s="6" t="str">
@@ -9737,9 +9735,8 @@
       <c r="H50" s="9">
         <v>150</v>
       </c>
-      <c r="I50" s="6">
-        <f>1/9</f>
-        <v>0.1111111111111111</v>
+      <c r="I50" s="19">
+        <v>0.1111</v>
       </c>
       <c r="J50" s="6" t="str">
         <f t="shared" si="1"/>
@@ -9780,7 +9777,7 @@
       <c r="H51" s="9">
         <v>201</v>
       </c>
-      <c r="I51" s="7">
+      <c r="I51" s="20">
         <v>1</v>
       </c>
       <c r="J51" s="6" t="str">
@@ -9822,7 +9819,7 @@
       <c r="H52">
         <v>201</v>
       </c>
-      <c r="I52" s="6">
+      <c r="I52" s="19">
         <v>0.5</v>
       </c>
       <c r="J52" s="6" t="str">
@@ -9864,7 +9861,7 @@
       <c r="H53" s="9">
         <v>201</v>
       </c>
-      <c r="I53" s="7">
+      <c r="I53" s="20">
         <v>0.5</v>
       </c>
       <c r="J53" s="6" t="str">
@@ -9909,7 +9906,7 @@
       <c r="H54" s="9">
         <v>202</v>
       </c>
-      <c r="I54" s="7">
+      <c r="I54" s="20">
         <v>1</v>
       </c>
       <c r="J54" s="6" t="str">
@@ -9953,7 +9950,7 @@
       <c r="H55" s="9">
         <v>202</v>
       </c>
-      <c r="I55" s="6">
+      <c r="I55" s="19">
         <v>0.5</v>
       </c>
       <c r="J55" s="6" t="str">
@@ -9995,7 +9992,7 @@
       <c r="H56" s="9">
         <v>202</v>
       </c>
-      <c r="I56" s="7">
+      <c r="I56" s="20">
         <v>0.5</v>
       </c>
       <c r="J56" s="6" t="str">
@@ -10036,7 +10033,7 @@
       <c r="H57">
         <v>300</v>
       </c>
-      <c r="I57" s="7">
+      <c r="I57" s="20">
         <v>1</v>
       </c>
       <c r="J57" s="6" t="str">
@@ -10072,7 +10069,7 @@
       <c r="H58">
         <v>310</v>
       </c>
-      <c r="I58" s="7">
+      <c r="I58" s="20">
         <v>1</v>
       </c>
       <c r="J58" s="6" t="str">
@@ -10108,7 +10105,7 @@
       <c r="H59">
         <v>320</v>
       </c>
-      <c r="I59" s="7">
+      <c r="I59" s="20">
         <v>1</v>
       </c>
       <c r="J59" s="6" t="str">
@@ -10144,7 +10141,7 @@
       <c r="H60" s="9">
         <v>330</v>
       </c>
-      <c r="I60" s="7">
+      <c r="I60" s="20">
         <v>1</v>
       </c>
       <c r="J60" s="6" t="str">
@@ -10180,7 +10177,7 @@
       <c r="H61">
         <v>340</v>
       </c>
-      <c r="I61" s="7">
+      <c r="I61" s="20">
         <v>1</v>
       </c>
       <c r="J61" s="6" t="str">
@@ -10216,7 +10213,7 @@
       <c r="H62">
         <v>10</v>
       </c>
-      <c r="I62" s="7">
+      <c r="I62" s="20">
         <v>1</v>
       </c>
       <c r="J62" s="6" t="str">
@@ -10252,7 +10249,7 @@
       <c r="H63">
         <v>20</v>
       </c>
-      <c r="I63" s="7">
+      <c r="I63" s="20">
         <v>1</v>
       </c>
       <c r="J63" s="6" t="str">
@@ -10288,7 +10285,7 @@
       <c r="H64">
         <v>10</v>
       </c>
-      <c r="I64" s="7">
+      <c r="I64" s="20">
         <v>1</v>
       </c>
       <c r="J64" s="6" t="str">
@@ -10324,7 +10321,7 @@
       <c r="H65">
         <v>20</v>
       </c>
-      <c r="I65" s="7">
+      <c r="I65" s="20">
         <v>1</v>
       </c>
       <c r="J65" s="6" t="str">
@@ -10360,7 +10357,7 @@
       <c r="H66">
         <v>30</v>
       </c>
-      <c r="I66" s="7">
+      <c r="I66" s="20">
         <v>1</v>
       </c>
       <c r="J66" s="6" t="str">
@@ -10396,7 +10393,7 @@
       <c r="H67">
         <v>1</v>
       </c>
-      <c r="I67" s="7">
+      <c r="I67" s="20">
         <v>1</v>
       </c>
       <c r="J67" s="6" t="str">
@@ -10432,7 +10429,7 @@
       <c r="H68">
         <v>2</v>
       </c>
-      <c r="I68" s="7">
+      <c r="I68" s="20">
         <v>1</v>
       </c>
       <c r="J68" s="6" t="str">
@@ -10468,7 +10465,7 @@
       <c r="H69">
         <v>10</v>
       </c>
-      <c r="I69" s="7">
+      <c r="I69" s="20">
         <v>1</v>
       </c>
       <c r="J69" s="6" t="str">
@@ -10504,7 +10501,7 @@
       <c r="H70">
         <v>20</v>
       </c>
-      <c r="I70" s="7">
+      <c r="I70" s="20">
         <v>1</v>
       </c>
       <c r="J70" s="6" t="str">
@@ -10540,7 +10537,7 @@
       <c r="H71">
         <v>30</v>
       </c>
-      <c r="I71" s="7">
+      <c r="I71" s="20">
         <v>1</v>
       </c>
       <c r="J71" s="6" t="str">
@@ -10576,7 +10573,7 @@
       <c r="H72">
         <v>40</v>
       </c>
-      <c r="I72" s="7">
+      <c r="I72" s="20">
         <v>1</v>
       </c>
       <c r="J72" s="6" t="str">
@@ -10612,7 +10609,7 @@
       <c r="H73">
         <v>50</v>
       </c>
-      <c r="I73" s="7">
+      <c r="I73" s="20">
         <v>1</v>
       </c>
       <c r="J73" s="6" t="str">
@@ -10648,7 +10645,7 @@
       <c r="H74">
         <v>60</v>
       </c>
-      <c r="I74" s="7">
+      <c r="I74" s="20">
         <v>1</v>
       </c>
       <c r="J74" s="6" t="str">
@@ -10684,7 +10681,7 @@
       <c r="H75">
         <v>70</v>
       </c>
-      <c r="I75" s="7">
+      <c r="I75" s="20">
         <v>1</v>
       </c>
       <c r="J75" s="6" t="str">
@@ -10720,7 +10717,7 @@
       <c r="H76">
         <v>80</v>
       </c>
-      <c r="I76" s="7">
+      <c r="I76" s="20">
         <v>1</v>
       </c>
       <c r="J76" s="6" t="str">
@@ -10756,7 +10753,7 @@
       <c r="H77">
         <v>90</v>
       </c>
-      <c r="I77" s="7">
+      <c r="I77" s="20">
         <v>1</v>
       </c>
       <c r="J77" s="6" t="str">
@@ -10792,7 +10789,7 @@
       <c r="H78">
         <v>100</v>
       </c>
-      <c r="I78" s="7">
+      <c r="I78" s="20">
         <v>1</v>
       </c>
       <c r="J78" s="6" t="str">
@@ -10828,7 +10825,7 @@
       <c r="H79">
         <v>110</v>
       </c>
-      <c r="I79" s="7">
+      <c r="I79" s="20">
         <v>1</v>
       </c>
       <c r="J79" s="6" t="str">
@@ -10864,7 +10861,7 @@
       <c r="H80">
         <v>120</v>
       </c>
-      <c r="I80" s="7">
+      <c r="I80" s="20">
         <v>1</v>
       </c>
       <c r="J80" s="6" t="str">
@@ -10900,7 +10897,7 @@
       <c r="H81">
         <v>130</v>
       </c>
-      <c r="I81" s="7">
+      <c r="I81" s="20">
         <v>1</v>
       </c>
       <c r="J81" s="6" t="str">
@@ -10936,7 +10933,7 @@
       <c r="H82">
         <v>140</v>
       </c>
-      <c r="I82" s="7">
+      <c r="I82" s="20">
         <v>1</v>
       </c>
       <c r="J82" s="6" t="str">
@@ -10972,7 +10969,7 @@
       <c r="H83">
         <v>150</v>
       </c>
-      <c r="I83" s="7">
+      <c r="I83" s="20">
         <v>1</v>
       </c>
       <c r="J83" s="6" t="str">
@@ -11008,7 +11005,7 @@
       <c r="H84">
         <v>160</v>
       </c>
-      <c r="I84" s="7">
+      <c r="I84" s="20">
         <v>1</v>
       </c>
       <c r="J84" s="6" t="str">
@@ -11044,7 +11041,7 @@
       <c r="H85">
         <v>170</v>
       </c>
-      <c r="I85" s="7">
+      <c r="I85" s="20">
         <v>1</v>
       </c>
       <c r="J85" s="6" t="str">
@@ -11080,7 +11077,7 @@
       <c r="H86">
         <v>180</v>
       </c>
-      <c r="I86" s="7">
+      <c r="I86" s="20">
         <v>1</v>
       </c>
       <c r="J86" s="6" t="str">
@@ -11116,7 +11113,7 @@
       <c r="H87">
         <v>190</v>
       </c>
-      <c r="I87" s="7">
+      <c r="I87" s="20">
         <v>1</v>
       </c>
       <c r="J87" s="6" t="str">
@@ -11152,7 +11149,7 @@
       <c r="H88">
         <v>200</v>
       </c>
-      <c r="I88" s="7">
+      <c r="I88" s="20">
         <v>1</v>
       </c>
       <c r="J88" s="6" t="str">
@@ -11188,7 +11185,7 @@
       <c r="H89">
         <v>210</v>
       </c>
-      <c r="I89" s="7">
+      <c r="I89" s="20">
         <v>1</v>
       </c>
       <c r="J89" s="6" t="str">
@@ -11224,7 +11221,7 @@
       <c r="H90">
         <v>220</v>
       </c>
-      <c r="I90" s="7">
+      <c r="I90" s="20">
         <v>1</v>
       </c>
       <c r="J90" s="6" t="str">
@@ -11260,7 +11257,7 @@
       <c r="H91">
         <v>230</v>
       </c>
-      <c r="I91" s="7">
+      <c r="I91" s="20">
         <v>1</v>
       </c>
       <c r="J91" s="6" t="str">
@@ -11296,7 +11293,7 @@
       <c r="H92">
         <v>240</v>
       </c>
-      <c r="I92" s="7">
+      <c r="I92" s="20">
         <v>1</v>
       </c>
       <c r="J92" s="6" t="str">
@@ -11332,7 +11329,7 @@
       <c r="H93">
         <v>250</v>
       </c>
-      <c r="I93" s="7">
+      <c r="I93" s="20">
         <v>1</v>
       </c>
       <c r="J93" s="6" t="str">
@@ -11368,7 +11365,7 @@
       <c r="H94">
         <v>260</v>
       </c>
-      <c r="I94" s="7">
+      <c r="I94" s="20">
         <v>1</v>
       </c>
       <c r="J94" s="6" t="str">
@@ -11404,7 +11401,7 @@
       <c r="H95">
         <v>270</v>
       </c>
-      <c r="I95" s="7">
+      <c r="I95" s="20">
         <v>1</v>
       </c>
       <c r="J95" s="6" t="str">
@@ -11440,7 +11437,7 @@
       <c r="H96">
         <v>280</v>
       </c>
-      <c r="I96" s="7">
+      <c r="I96" s="20">
         <v>1</v>
       </c>
       <c r="J96" s="6" t="str">
@@ -11476,7 +11473,7 @@
       <c r="H97">
         <v>290</v>
       </c>
-      <c r="I97" s="7">
+      <c r="I97" s="20">
         <v>1</v>
       </c>
       <c r="J97" s="6" t="str">
@@ -11512,7 +11509,7 @@
       <c r="H98">
         <v>300</v>
       </c>
-      <c r="I98" s="7">
+      <c r="I98" s="20">
         <v>1</v>
       </c>
       <c r="J98" s="6" t="str">
@@ -11548,7 +11545,7 @@
       <c r="H99">
         <v>310</v>
       </c>
-      <c r="I99" s="7">
+      <c r="I99" s="20">
         <v>1</v>
       </c>
       <c r="J99" s="6" t="str">
@@ -11584,7 +11581,7 @@
       <c r="H100">
         <v>320</v>
       </c>
-      <c r="I100" s="7">
+      <c r="I100" s="20">
         <v>1</v>
       </c>
       <c r="J100" s="6" t="str">
@@ -11620,7 +11617,7 @@
       <c r="H101">
         <v>400</v>
       </c>
-      <c r="I101" s="7">
+      <c r="I101" s="20">
         <v>1</v>
       </c>
       <c r="J101" s="6" t="str">
@@ -11656,7 +11653,7 @@
       <c r="H102">
         <v>410</v>
       </c>
-      <c r="I102" s="7">
+      <c r="I102" s="20">
         <v>1</v>
       </c>
       <c r="J102" s="6" t="str">
@@ -11692,7 +11689,7 @@
       <c r="H103">
         <v>420</v>
       </c>
-      <c r="I103" s="7">
+      <c r="I103" s="20">
         <v>1</v>
       </c>
       <c r="J103" s="6" t="str">
@@ -11728,7 +11725,7 @@
       <c r="H104">
         <v>430</v>
       </c>
-      <c r="I104" s="7">
+      <c r="I104" s="20">
         <v>1</v>
       </c>
       <c r="J104" s="6" t="str">
@@ -11764,7 +11761,7 @@
       <c r="H105">
         <v>440</v>
       </c>
-      <c r="I105" s="7">
+      <c r="I105" s="20">
         <v>1</v>
       </c>
       <c r="J105" s="6" t="str">
@@ -11800,7 +11797,7 @@
       <c r="H106">
         <v>450</v>
       </c>
-      <c r="I106" s="7">
+      <c r="I106" s="20">
         <v>1</v>
       </c>
       <c r="J106" s="6" t="str">
@@ -11836,7 +11833,7 @@
       <c r="H107">
         <v>460</v>
       </c>
-      <c r="I107" s="7">
+      <c r="I107" s="20">
         <v>1</v>
       </c>
       <c r="J107" s="6" t="str">
@@ -11872,7 +11869,7 @@
       <c r="H108">
         <v>470</v>
       </c>
-      <c r="I108" s="7">
+      <c r="I108" s="20">
         <v>1</v>
       </c>
       <c r="J108" s="6" t="str">
@@ -11908,7 +11905,7 @@
       <c r="H109">
         <v>510</v>
       </c>
-      <c r="I109" s="7">
+      <c r="I109" s="20">
         <v>1</v>
       </c>
       <c r="J109" s="6" t="str">
@@ -11944,7 +11941,7 @@
       <c r="H110">
         <v>520</v>
       </c>
-      <c r="I110" s="7">
+      <c r="I110" s="20">
         <v>1</v>
       </c>
       <c r="J110" s="6" t="str">
@@ -11980,7 +11977,7 @@
       <c r="H111">
         <v>610</v>
       </c>
-      <c r="I111" s="7">
+      <c r="I111" s="20">
         <v>1</v>
       </c>
       <c r="J111" s="6" t="str">
@@ -12016,7 +12013,7 @@
       <c r="H112">
         <v>620</v>
       </c>
-      <c r="I112" s="7">
+      <c r="I112" s="20">
         <v>1</v>
       </c>
       <c r="J112" s="6" t="str">
@@ -12052,7 +12049,7 @@
       <c r="H113">
         <v>630</v>
       </c>
-      <c r="I113" s="7">
+      <c r="I113" s="20">
         <v>1</v>
       </c>
       <c r="J113" s="6" t="str">
@@ -12088,7 +12085,7 @@
       <c r="H114">
         <v>640</v>
       </c>
-      <c r="I114" s="7">
+      <c r="I114" s="20">
         <v>1</v>
       </c>
       <c r="J114" s="6" t="str">
@@ -12124,7 +12121,7 @@
       <c r="H115">
         <v>710</v>
       </c>
-      <c r="I115" s="7">
+      <c r="I115" s="20">
         <v>1</v>
       </c>
       <c r="J115" s="6" t="str">
@@ -12160,7 +12157,7 @@
       <c r="H116">
         <v>720</v>
       </c>
-      <c r="I116" s="7">
+      <c r="I116" s="20">
         <v>1</v>
       </c>
       <c r="J116" s="6" t="str">
@@ -12196,7 +12193,7 @@
       <c r="H117">
         <v>730</v>
       </c>
-      <c r="I117" s="7">
+      <c r="I117" s="20">
         <v>1</v>
       </c>
       <c r="J117" s="6" t="str">
@@ -12232,7 +12229,7 @@
       <c r="H118">
         <v>740</v>
       </c>
-      <c r="I118" s="7">
+      <c r="I118" s="20">
         <v>1</v>
       </c>
       <c r="J118" s="6" t="str">
@@ -12268,7 +12265,7 @@
       <c r="H119">
         <v>10</v>
       </c>
-      <c r="I119" s="7">
+      <c r="I119" s="20">
         <v>1</v>
       </c>
       <c r="J119" s="6" t="str">
@@ -12304,7 +12301,7 @@
       <c r="H120">
         <v>20</v>
       </c>
-      <c r="I120" s="7">
+      <c r="I120" s="20">
         <v>1</v>
       </c>
       <c r="J120" s="6" t="str">
@@ -12316,6 +12313,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AF120" xr:uid="{F5070472-BD41-FC47-BC46-FB0AD4499DE3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:W61">
     <sortCondition ref="H4:H61"/>
   </sortState>

</xml_diff>

<commit_message>
Dim Item Sets add <15>15 age categoru
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B717B3BC-09BD-3B49-9F66-5FCEB99D4DBA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64898929-EC92-3F40-B3C6-096659C5B850}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2687" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2689" uniqueCount="629">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1922,6 +1922,9 @@
   </si>
   <si>
     <t>Category option combo</t>
+  </si>
+  <si>
+    <t>&lt;15/&gt;15</t>
   </si>
 </sst>
 </file>
@@ -2010,7 +2013,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2024,9 +2027,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3531,7 +3531,7 @@
       <c r="L15" t="s">
         <v>237</v>
       </c>
-      <c r="M15" s="14" t="s">
+      <c r="M15" s="13" t="s">
         <v>407</v>
       </c>
       <c r="N15" t="s">
@@ -3611,7 +3611,7 @@
       <c r="L16" t="s">
         <v>237</v>
       </c>
-      <c r="M16" s="14" t="s">
+      <c r="M16" s="13" t="s">
         <v>407</v>
       </c>
       <c r="N16" t="s">
@@ -3688,7 +3688,7 @@
       <c r="L17" t="s">
         <v>237</v>
       </c>
-      <c r="M17" s="14" t="s">
+      <c r="M17" s="13" t="s">
         <v>407</v>
       </c>
       <c r="N17" t="s">
@@ -3715,7 +3715,7 @@
       <c r="U17" t="s">
         <v>251</v>
       </c>
-      <c r="V17" s="14" t="s">
+      <c r="V17" s="13" t="s">
         <v>407</v>
       </c>
       <c r="W17" t="s">
@@ -3768,7 +3768,7 @@
       <c r="L18" t="s">
         <v>237</v>
       </c>
-      <c r="M18" s="14" t="s">
+      <c r="M18" s="13" t="s">
         <v>407</v>
       </c>
       <c r="N18" t="s">
@@ -3848,7 +3848,7 @@
       <c r="L19" t="s">
         <v>237</v>
       </c>
-      <c r="M19" s="14" t="s">
+      <c r="M19" s="13" t="s">
         <v>407</v>
       </c>
       <c r="N19" t="s">
@@ -3928,7 +3928,7 @@
       <c r="L20" t="s">
         <v>237</v>
       </c>
-      <c r="M20" s="14" t="s">
+      <c r="M20" s="13" t="s">
         <v>407</v>
       </c>
       <c r="N20" t="s">
@@ -4008,7 +4008,7 @@
       <c r="L21" t="s">
         <v>237</v>
       </c>
-      <c r="M21" s="14" t="s">
+      <c r="M21" s="13" t="s">
         <v>407</v>
       </c>
       <c r="N21" t="s">
@@ -4088,7 +4088,7 @@
       <c r="L22" t="s">
         <v>237</v>
       </c>
-      <c r="M22" s="14" t="s">
+      <c r="M22" s="13" t="s">
         <v>407</v>
       </c>
       <c r="N22" t="s">
@@ -4168,7 +4168,7 @@
       <c r="L23" t="s">
         <v>237</v>
       </c>
-      <c r="M23" s="14" t="s">
+      <c r="M23" s="13" t="s">
         <v>407</v>
       </c>
       <c r="N23" t="s">
@@ -4248,7 +4248,7 @@
       <c r="L24" t="s">
         <v>237</v>
       </c>
-      <c r="M24" s="14" t="s">
+      <c r="M24" s="13" t="s">
         <v>407</v>
       </c>
       <c r="N24" t="s">
@@ -4328,7 +4328,7 @@
       <c r="L25" t="s">
         <v>237</v>
       </c>
-      <c r="M25" s="14" t="s">
+      <c r="M25" s="13" t="s">
         <v>407</v>
       </c>
       <c r="N25" t="s">
@@ -4408,7 +4408,7 @@
       <c r="L26" t="s">
         <v>237</v>
       </c>
-      <c r="M26" s="14" t="s">
+      <c r="M26" s="13" t="s">
         <v>407</v>
       </c>
       <c r="N26" t="s">
@@ -4488,7 +4488,7 @@
       <c r="L27" t="s">
         <v>237</v>
       </c>
-      <c r="M27" s="14" t="s">
+      <c r="M27" s="13" t="s">
         <v>407</v>
       </c>
       <c r="N27" t="s">
@@ -4568,7 +4568,7 @@
       <c r="L28" t="s">
         <v>237</v>
       </c>
-      <c r="M28" s="14" t="s">
+      <c r="M28" s="13" t="s">
         <v>407</v>
       </c>
       <c r="N28" t="s">
@@ -4648,7 +4648,7 @@
       <c r="L29" t="s">
         <v>237</v>
       </c>
-      <c r="M29" s="14" t="s">
+      <c r="M29" s="13" t="s">
         <v>407</v>
       </c>
       <c r="N29" t="s">
@@ -4728,7 +4728,7 @@
       <c r="L30" t="s">
         <v>237</v>
       </c>
-      <c r="M30" s="14" t="s">
+      <c r="M30" s="13" t="s">
         <v>407</v>
       </c>
       <c r="N30" t="s">
@@ -4808,7 +4808,7 @@
       <c r="L31" t="s">
         <v>237</v>
       </c>
-      <c r="M31" s="14" t="s">
+      <c r="M31" s="13" t="s">
         <v>407</v>
       </c>
       <c r="N31" t="s">
@@ -4888,7 +4888,7 @@
       <c r="L32" t="s">
         <v>237</v>
       </c>
-      <c r="M32" s="14" t="s">
+      <c r="M32" s="13" t="s">
         <v>407</v>
       </c>
       <c r="N32" t="s">
@@ -4968,7 +4968,7 @@
       <c r="L33" t="s">
         <v>237</v>
       </c>
-      <c r="M33" s="14" t="s">
+      <c r="M33" s="13" t="s">
         <v>407</v>
       </c>
       <c r="N33" t="s">
@@ -5048,7 +5048,7 @@
       <c r="L34" t="s">
         <v>237</v>
       </c>
-      <c r="M34" s="14" t="s">
+      <c r="M34" s="13" t="s">
         <v>407</v>
       </c>
       <c r="N34" t="s">
@@ -5128,7 +5128,7 @@
       <c r="L35" t="s">
         <v>237</v>
       </c>
-      <c r="M35" s="14" t="s">
+      <c r="M35" s="13" t="s">
         <v>407</v>
       </c>
       <c r="N35" t="s">
@@ -5208,7 +5208,7 @@
       <c r="L36" t="s">
         <v>237</v>
       </c>
-      <c r="M36" s="14" t="s">
+      <c r="M36" s="13" t="s">
         <v>407</v>
       </c>
       <c r="N36" t="s">
@@ -5288,7 +5288,7 @@
       <c r="L37" t="s">
         <v>237</v>
       </c>
-      <c r="M37" s="14" t="s">
+      <c r="M37" s="13" t="s">
         <v>407</v>
       </c>
       <c r="N37" t="s">
@@ -5350,7 +5350,7 @@
       <c r="F38" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="G38" s="16" t="s">
+      <c r="G38" s="15" t="s">
         <v>422</v>
       </c>
       <c r="H38" t="s">
@@ -5430,7 +5430,7 @@
       <c r="F39" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="G39" s="16" t="s">
+      <c r="G39" s="15" t="s">
         <v>79</v>
       </c>
       <c r="H39" s="1" t="s">
@@ -5972,7 +5972,7 @@
       </c>
     </row>
     <row r="46" spans="1:26" ht="18" x14ac:dyDescent="0.2">
-      <c r="A46" s="15" t="s">
+      <c r="A46" s="14" t="s">
         <v>91</v>
       </c>
       <c r="B46" t="s">
@@ -6052,7 +6052,7 @@
       </c>
     </row>
     <row r="47" spans="1:26" ht="18" x14ac:dyDescent="0.2">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="14" t="s">
         <v>91</v>
       </c>
       <c r="B47" t="s">
@@ -6150,7 +6150,7 @@
       <c r="F48" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="G48" s="16" t="s">
+      <c r="G48" s="15" t="s">
         <v>423</v>
       </c>
       <c r="H48" t="s">
@@ -6230,7 +6230,7 @@
       <c r="F49" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="G49" s="16" t="s">
+      <c r="G49" s="15" t="s">
         <v>102</v>
       </c>
       <c r="H49" s="1" t="s">
@@ -7503,10 +7503,10 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="F37" s="14"/>
+      <c r="F37" s="13"/>
     </row>
     <row r="38" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="F38" s="14"/>
+      <c r="F38" s="13"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
@@ -7538,7 +7538,7 @@
       <c r="C40" t="s">
         <v>336</v>
       </c>
-      <c r="F40" s="14"/>
+      <c r="F40" s="13"/>
     </row>
     <row r="41" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -7550,7 +7550,7 @@
       <c r="C41">
         <v>485</v>
       </c>
-      <c r="F41" s="14"/>
+      <c r="F41" s="13"/>
     </row>
     <row r="42" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -7562,7 +7562,7 @@
       <c r="C42">
         <v>3101</v>
       </c>
-      <c r="F42" s="14"/>
+      <c r="F42" s="13"/>
     </row>
     <row r="43" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -7574,7 +7574,7 @@
       <c r="C43">
         <v>1784</v>
       </c>
-      <c r="F43" s="14"/>
+      <c r="F43" s="13"/>
     </row>
     <row r="44" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -7586,7 +7586,7 @@
       <c r="C44">
         <v>17684</v>
       </c>
-      <c r="F44" s="14"/>
+      <c r="F44" s="13"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
@@ -7617,10 +7617,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AF120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A121" sqref="A121:XFD121"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7632,7 +7633,7 @@
     <col min="5" max="5" width="52.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="49.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="18" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="41.83203125" customWidth="1"/>
     <col min="11" max="13" width="12.33203125" customWidth="1"/>
     <col min="14" max="18" width="10.83203125" customWidth="1"/>
@@ -7664,7 +7665,7 @@
       <c r="H1" t="s">
         <v>199</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="18" t="s">
         <v>292</v>
       </c>
       <c r="J1" t="s">
@@ -7737,7 +7738,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>294</v>
       </c>
@@ -7762,7 +7763,7 @@
       <c r="H2">
         <v>3</v>
       </c>
-      <c r="I2" s="19">
+      <c r="I2" s="18">
         <v>1</v>
       </c>
       <c r="J2" s="6" t="str">
@@ -7781,7 +7782,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="3" spans="1:32" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>294</v>
       </c>
@@ -7806,7 +7807,7 @@
       <c r="H3">
         <v>7</v>
       </c>
-      <c r="I3" s="19">
+      <c r="I3" s="18">
         <v>1</v>
       </c>
       <c r="J3" s="6" t="str">
@@ -7825,7 +7826,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>294</v>
       </c>
@@ -7850,7 +7851,7 @@
       <c r="H4" s="9">
         <v>10</v>
       </c>
-      <c r="I4" s="20">
+      <c r="I4" s="19">
         <v>1</v>
       </c>
       <c r="J4" s="6" t="str">
@@ -7867,7 +7868,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>294</v>
       </c>
@@ -7892,7 +7893,7 @@
       <c r="H5" s="9">
         <v>10</v>
       </c>
-      <c r="I5" s="20">
+      <c r="I5" s="19">
         <v>0.25</v>
       </c>
       <c r="J5" s="6" t="str">
@@ -7904,7 +7905,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>294</v>
       </c>
@@ -7929,7 +7930,7 @@
       <c r="H6" s="8">
         <v>10</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I6" s="18">
         <v>0.2</v>
       </c>
       <c r="J6" s="6" t="str">
@@ -7937,7 +7938,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>294</v>
       </c>
@@ -7962,7 +7963,7 @@
       <c r="H7" s="9">
         <v>20</v>
       </c>
-      <c r="I7" s="20">
+      <c r="I7" s="19">
         <v>0.5</v>
       </c>
       <c r="J7" s="6" t="str">
@@ -7987,7 +7988,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>294</v>
       </c>
@@ -8012,7 +8013,7 @@
       <c r="H8" s="9">
         <v>20</v>
       </c>
-      <c r="I8" s="20">
+      <c r="I8" s="19">
         <v>0.25</v>
       </c>
       <c r="J8" s="6" t="str">
@@ -8023,7 +8024,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>294</v>
       </c>
@@ -8048,7 +8049,7 @@
       <c r="H9" s="8">
         <v>20</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="18">
         <v>1</v>
       </c>
       <c r="J9" s="6" t="str">
@@ -8062,7 +8063,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>294</v>
       </c>
@@ -8087,7 +8088,7 @@
       <c r="H10" s="9">
         <v>30</v>
       </c>
-      <c r="I10" s="20">
+      <c r="I10" s="19">
         <v>0.5</v>
       </c>
       <c r="J10" s="6" t="str">
@@ -8109,7 +8110,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>294</v>
       </c>
@@ -8134,7 +8135,7 @@
       <c r="H11" s="9">
         <v>30</v>
       </c>
-      <c r="I11" s="20">
+      <c r="I11" s="19">
         <v>0.25</v>
       </c>
       <c r="J11" s="6" t="str">
@@ -8145,7 +8146,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>294</v>
       </c>
@@ -8170,7 +8171,7 @@
       <c r="H12" s="9">
         <v>40</v>
       </c>
-      <c r="I12" s="20">
+      <c r="I12" s="19">
         <v>1</v>
       </c>
       <c r="J12" s="6" t="str">
@@ -8197,7 +8198,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>294</v>
       </c>
@@ -8222,7 +8223,7 @@
       <c r="H13" s="9">
         <v>40</v>
       </c>
-      <c r="I13" s="20">
+      <c r="I13" s="19">
         <v>0.25</v>
       </c>
       <c r="J13" s="6" t="str">
@@ -8233,7 +8234,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>237</v>
       </c>
@@ -8258,7 +8259,7 @@
       <c r="H14" s="9">
         <v>40</v>
       </c>
-      <c r="I14" s="19">
+      <c r="I14" s="18">
         <v>0.1111</v>
       </c>
       <c r="J14" s="6" t="str">
@@ -8275,7 +8276,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="15" spans="1:32" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:32" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>294</v>
       </c>
@@ -8300,18 +8301,20 @@
       <c r="H15" s="9">
         <v>45</v>
       </c>
-      <c r="I15" s="19">
+      <c r="I15" s="18">
         <v>1</v>
       </c>
       <c r="J15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="P15" s="12"/>
+        <v>&lt;15/&gt;15</v>
+      </c>
+      <c r="P15" s="12" t="s">
+        <v>628</v>
+      </c>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>237</v>
       </c>
@@ -8336,7 +8339,7 @@
       <c r="H16" s="9">
         <v>45</v>
       </c>
-      <c r="I16" s="19">
+      <c r="I16" s="18">
         <v>0.5</v>
       </c>
       <c r="J16" s="6" t="str">
@@ -8347,7 +8350,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>294</v>
       </c>
@@ -8372,7 +8375,7 @@
       <c r="H17" s="9">
         <v>50</v>
       </c>
-      <c r="I17" s="20">
+      <c r="I17" s="19">
         <v>1</v>
       </c>
       <c r="J17" s="6" t="str">
@@ -8408,7 +8411,7 @@
       <c r="H18" s="9">
         <v>60</v>
       </c>
-      <c r="I18" s="19">
+      <c r="I18" s="18">
         <v>0.125</v>
       </c>
       <c r="J18" s="6" t="str">
@@ -8419,7 +8422,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>294</v>
       </c>
@@ -8444,7 +8447,7 @@
       <c r="H19" s="9">
         <v>60</v>
       </c>
-      <c r="I19" s="20">
+      <c r="I19" s="19">
         <v>1</v>
       </c>
       <c r="J19" s="6" t="str">
@@ -8470,7 +8473,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>237</v>
       </c>
@@ -8495,7 +8498,7 @@
       <c r="H20" s="9">
         <v>60</v>
       </c>
-      <c r="I20" s="19">
+      <c r="I20" s="18">
         <v>0.1111</v>
       </c>
       <c r="J20" s="6" t="str">
@@ -8537,16 +8540,18 @@
       <c r="H21" s="10">
         <v>65</v>
       </c>
-      <c r="I21" s="19">
+      <c r="I21" s="18">
         <v>1</v>
       </c>
       <c r="J21" s="6" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="P21" s="13"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+        <v>&lt;15/&gt;15</v>
+      </c>
+      <c r="P21" s="12" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>237</v>
       </c>
@@ -8571,7 +8576,7 @@
       <c r="H22" s="9">
         <v>65</v>
       </c>
-      <c r="I22" s="19">
+      <c r="I22" s="18">
         <v>0.5</v>
       </c>
       <c r="J22" s="6" t="str">
@@ -8588,7 +8593,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>294</v>
       </c>
@@ -8613,7 +8618,7 @@
       <c r="H23" s="9">
         <v>70</v>
       </c>
-      <c r="I23" s="20">
+      <c r="I23" s="19">
         <v>1</v>
       </c>
       <c r="J23" s="6" t="str">
@@ -8654,7 +8659,7 @@
       <c r="H24" s="9">
         <v>80</v>
       </c>
-      <c r="I24" s="20">
+      <c r="I24" s="19">
         <v>0.125</v>
       </c>
       <c r="J24" s="6" t="str">
@@ -8665,7 +8670,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>294</v>
       </c>
@@ -8690,7 +8695,7 @@
       <c r="H25" s="9">
         <v>80</v>
       </c>
-      <c r="I25" s="20">
+      <c r="I25" s="19">
         <v>1</v>
       </c>
       <c r="J25" s="6" t="str">
@@ -8716,7 +8721,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>237</v>
       </c>
@@ -8741,7 +8746,7 @@
       <c r="H26" s="9">
         <v>80</v>
       </c>
-      <c r="I26" s="19">
+      <c r="I26" s="18">
         <v>0.1111</v>
       </c>
       <c r="J26" s="6" t="str">
@@ -8783,7 +8788,7 @@
       <c r="H27" s="9">
         <v>90</v>
       </c>
-      <c r="I27" s="20">
+      <c r="I27" s="19">
         <v>0.125</v>
       </c>
       <c r="J27" s="6" t="str">
@@ -8794,7 +8799,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>294</v>
       </c>
@@ -8819,7 +8824,7 @@
       <c r="H28" s="9">
         <v>90</v>
       </c>
-      <c r="I28" s="20">
+      <c r="I28" s="19">
         <v>1</v>
       </c>
       <c r="J28" s="6" t="str">
@@ -8847,7 +8852,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>294</v>
       </c>
@@ -8872,7 +8877,7 @@
       <c r="H29" s="9">
         <v>90</v>
       </c>
-      <c r="I29" s="20">
+      <c r="I29" s="19">
         <v>0.2</v>
       </c>
       <c r="J29" s="6" t="str">
@@ -8883,7 +8888,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>237</v>
       </c>
@@ -8908,7 +8913,7 @@
       <c r="H30" s="9">
         <v>90</v>
       </c>
-      <c r="I30" s="19">
+      <c r="I30" s="18">
         <v>0.1111</v>
       </c>
       <c r="J30" s="6" t="str">
@@ -8925,7 +8930,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>294</v>
       </c>
@@ -8950,7 +8955,7 @@
       <c r="H31" s="9">
         <v>100</v>
       </c>
-      <c r="I31" s="20">
+      <c r="I31" s="19">
         <v>1</v>
       </c>
       <c r="J31" s="6" t="str">
@@ -8986,7 +8991,7 @@
       <c r="H32" s="9">
         <v>110</v>
       </c>
-      <c r="I32" s="20">
+      <c r="I32" s="19">
         <v>0.125</v>
       </c>
       <c r="J32" s="6" t="str">
@@ -8997,7 +9002,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>294</v>
       </c>
@@ -9022,7 +9027,7 @@
       <c r="H33" s="9">
         <v>110</v>
       </c>
-      <c r="I33" s="20">
+      <c r="I33" s="19">
         <v>0.2</v>
       </c>
       <c r="J33" s="6" t="str">
@@ -9033,7 +9038,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>294</v>
       </c>
@@ -9058,7 +9063,7 @@
       <c r="H34" s="9">
         <v>110</v>
       </c>
-      <c r="I34" s="20">
+      <c r="I34" s="19">
         <v>1</v>
       </c>
       <c r="J34" s="6" t="str">
@@ -9086,7 +9091,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>237</v>
       </c>
@@ -9111,7 +9116,7 @@
       <c r="H35" s="9">
         <v>110</v>
       </c>
-      <c r="I35" s="19">
+      <c r="I35" s="18">
         <v>0.11119999999999999</v>
       </c>
       <c r="J35" s="6" t="str">
@@ -9153,7 +9158,7 @@
       <c r="H36" s="9">
         <v>120</v>
       </c>
-      <c r="I36" s="20">
+      <c r="I36" s="19">
         <v>0.125</v>
       </c>
       <c r="J36" s="6" t="str">
@@ -9164,7 +9169,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>294</v>
       </c>
@@ -9189,7 +9194,7 @@
       <c r="H37" s="9">
         <v>120</v>
       </c>
-      <c r="I37" s="20">
+      <c r="I37" s="19">
         <v>0.2</v>
       </c>
       <c r="J37" s="6" t="str">
@@ -9200,7 +9205,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>294</v>
       </c>
@@ -9225,7 +9230,7 @@
       <c r="H38" s="9">
         <v>120</v>
       </c>
-      <c r="I38" s="20">
+      <c r="I38" s="19">
         <v>1</v>
       </c>
       <c r="J38" s="6" t="str">
@@ -9251,7 +9256,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>237</v>
       </c>
@@ -9276,7 +9281,7 @@
       <c r="H39" s="9">
         <v>120</v>
       </c>
-      <c r="I39" s="19">
+      <c r="I39" s="18">
         <v>0.1111</v>
       </c>
       <c r="J39" s="6" t="str">
@@ -9318,7 +9323,7 @@
       <c r="H40" s="9">
         <v>130</v>
       </c>
-      <c r="I40" s="20">
+      <c r="I40" s="19">
         <v>0.125</v>
       </c>
       <c r="J40" s="6" t="str">
@@ -9329,7 +9334,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>294</v>
       </c>
@@ -9354,7 +9359,7 @@
       <c r="H41" s="9">
         <v>130</v>
       </c>
-      <c r="I41" s="20">
+      <c r="I41" s="19">
         <v>0.2</v>
       </c>
       <c r="J41" s="6" t="str">
@@ -9365,7 +9370,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>294</v>
       </c>
@@ -9390,7 +9395,7 @@
       <c r="H42" s="9">
         <v>130</v>
       </c>
-      <c r="I42" s="20">
+      <c r="I42" s="19">
         <v>0.5</v>
       </c>
       <c r="J42" s="6" t="str">
@@ -9416,7 +9421,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>237</v>
       </c>
@@ -9441,7 +9446,7 @@
       <c r="H43" s="9">
         <v>130</v>
       </c>
-      <c r="I43" s="19">
+      <c r="I43" s="18">
         <v>0.1111</v>
       </c>
       <c r="J43" s="6" t="str">
@@ -9483,7 +9488,7 @@
       <c r="H44" s="9">
         <v>140</v>
       </c>
-      <c r="I44" s="20">
+      <c r="I44" s="19">
         <v>0.125</v>
       </c>
       <c r="J44" s="6" t="str">
@@ -9494,7 +9499,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>294</v>
       </c>
@@ -9519,7 +9524,7 @@
       <c r="H45" s="9">
         <v>140</v>
       </c>
-      <c r="I45" s="20">
+      <c r="I45" s="19">
         <v>0.2</v>
       </c>
       <c r="J45" s="6" t="str">
@@ -9530,7 +9535,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>294</v>
       </c>
@@ -9555,7 +9560,7 @@
       <c r="H46" s="9">
         <v>140</v>
       </c>
-      <c r="I46" s="20">
+      <c r="I46" s="19">
         <v>0.5</v>
       </c>
       <c r="J46" s="6" t="str">
@@ -9581,7 +9586,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>237</v>
       </c>
@@ -9606,7 +9611,7 @@
       <c r="H47" s="9">
         <v>140</v>
       </c>
-      <c r="I47" s="19">
+      <c r="I47" s="18">
         <v>0.1111</v>
       </c>
       <c r="J47" s="6" t="str">
@@ -9648,7 +9653,7 @@
       <c r="H48" s="9">
         <v>150</v>
       </c>
-      <c r="I48" s="20">
+      <c r="I48" s="19">
         <v>0.125</v>
       </c>
       <c r="J48" s="6" t="str">
@@ -9659,7 +9664,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>294</v>
       </c>
@@ -9684,7 +9689,7 @@
       <c r="H49" s="9">
         <v>150</v>
       </c>
-      <c r="I49" s="20">
+      <c r="I49" s="19">
         <v>1</v>
       </c>
       <c r="J49" s="6" t="str">
@@ -9710,7 +9715,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>237</v>
       </c>
@@ -9735,7 +9740,7 @@
       <c r="H50" s="9">
         <v>150</v>
       </c>
-      <c r="I50" s="19">
+      <c r="I50" s="18">
         <v>0.1111</v>
       </c>
       <c r="J50" s="6" t="str">
@@ -9752,7 +9757,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>295</v>
       </c>
@@ -9777,7 +9782,7 @@
       <c r="H51" s="9">
         <v>201</v>
       </c>
-      <c r="I51" s="20">
+      <c r="I51" s="19">
         <v>1</v>
       </c>
       <c r="J51" s="6" t="str">
@@ -9794,7 +9799,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>237</v>
       </c>
@@ -9819,7 +9824,7 @@
       <c r="H52">
         <v>201</v>
       </c>
-      <c r="I52" s="19">
+      <c r="I52" s="18">
         <v>0.5</v>
       </c>
       <c r="J52" s="6" t="str">
@@ -9836,7 +9841,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>295</v>
       </c>
@@ -9861,7 +9866,7 @@
       <c r="H53" s="9">
         <v>201</v>
       </c>
-      <c r="I53" s="20">
+      <c r="I53" s="19">
         <v>0.5</v>
       </c>
       <c r="J53" s="6" t="str">
@@ -9881,7 +9886,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>295</v>
       </c>
@@ -9906,7 +9911,7 @@
       <c r="H54" s="9">
         <v>202</v>
       </c>
-      <c r="I54" s="20">
+      <c r="I54" s="19">
         <v>1</v>
       </c>
       <c r="J54" s="6" t="str">
@@ -9925,7 +9930,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>237</v>
       </c>
@@ -9950,7 +9955,7 @@
       <c r="H55" s="9">
         <v>202</v>
       </c>
-      <c r="I55" s="19">
+      <c r="I55" s="18">
         <v>0.5</v>
       </c>
       <c r="J55" s="6" t="str">
@@ -9967,7 +9972,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>295</v>
       </c>
@@ -9992,7 +9997,7 @@
       <c r="H56" s="9">
         <v>202</v>
       </c>
-      <c r="I56" s="20">
+      <c r="I56" s="19">
         <v>0.5</v>
       </c>
       <c r="J56" s="6" t="str">
@@ -10008,11 +10013,11 @@
         <v>251</v>
       </c>
     </row>
-    <row r="57" spans="1:28" ht="18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>310</v>
       </c>
-      <c r="B57" s="14" t="s">
+      <c r="B57" s="13" t="s">
         <v>320</v>
       </c>
       <c r="C57" t="s">
@@ -10033,7 +10038,7 @@
       <c r="H57">
         <v>300</v>
       </c>
-      <c r="I57" s="20">
+      <c r="I57" s="19">
         <v>1</v>
       </c>
       <c r="J57" s="6" t="str">
@@ -10044,11 +10049,11 @@
         <v>321</v>
       </c>
     </row>
-    <row r="58" spans="1:28" ht="18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>310</v>
       </c>
-      <c r="B58" s="14" t="s">
+      <c r="B58" s="13" t="s">
         <v>320</v>
       </c>
       <c r="C58" t="s">
@@ -10069,7 +10074,7 @@
       <c r="H58">
         <v>310</v>
       </c>
-      <c r="I58" s="20">
+      <c r="I58" s="19">
         <v>1</v>
       </c>
       <c r="J58" s="6" t="str">
@@ -10080,11 +10085,11 @@
         <v>321</v>
       </c>
     </row>
-    <row r="59" spans="1:28" ht="18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>310</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B59" s="13" t="s">
         <v>320</v>
       </c>
       <c r="C59" t="s">
@@ -10105,7 +10110,7 @@
       <c r="H59">
         <v>320</v>
       </c>
-      <c r="I59" s="20">
+      <c r="I59" s="19">
         <v>1</v>
       </c>
       <c r="J59" s="6" t="str">
@@ -10116,11 +10121,11 @@
         <v>321</v>
       </c>
     </row>
-    <row r="60" spans="1:28" ht="18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>310</v>
       </c>
-      <c r="B60" s="14" t="s">
+      <c r="B60" s="13" t="s">
         <v>320</v>
       </c>
       <c r="C60" t="s">
@@ -10141,7 +10146,7 @@
       <c r="H60" s="9">
         <v>330</v>
       </c>
-      <c r="I60" s="20">
+      <c r="I60" s="19">
         <v>1</v>
       </c>
       <c r="J60" s="6" t="str">
@@ -10152,11 +10157,11 @@
         <v>321</v>
       </c>
     </row>
-    <row r="61" spans="1:28" ht="18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>310</v>
       </c>
-      <c r="B61" s="14" t="s">
+      <c r="B61" s="13" t="s">
         <v>320</v>
       </c>
       <c r="C61" t="s">
@@ -10177,7 +10182,7 @@
       <c r="H61">
         <v>340</v>
       </c>
-      <c r="I61" s="20">
+      <c r="I61" s="19">
         <v>1</v>
       </c>
       <c r="J61" s="6" t="str">
@@ -10188,32 +10193,32 @@
         <v>321</v>
       </c>
     </row>
-    <row r="62" spans="1:28" ht="18" x14ac:dyDescent="0.25">
-      <c r="A62" s="16" t="s">
+    <row r="62" spans="1:28" ht="18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="B62" s="16" t="s">
+      <c r="B62" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="C62" s="16" t="s">
+      <c r="C62" s="15" t="s">
         <v>324</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="E62" s="16" t="s">
+      <c r="E62" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="F62" s="16" t="s">
+      <c r="F62" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="G62" s="16" t="s">
+      <c r="G62" s="15" t="s">
         <v>324</v>
       </c>
       <c r="H62">
         <v>10</v>
       </c>
-      <c r="I62" s="20">
+      <c r="I62" s="19">
         <v>1</v>
       </c>
       <c r="J62" s="6" t="str">
@@ -10224,32 +10229,32 @@
         <v>571</v>
       </c>
     </row>
-    <row r="63" spans="1:28" ht="18" x14ac:dyDescent="0.25">
-      <c r="A63" s="16" t="s">
+    <row r="63" spans="1:28" ht="18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="B63" s="16" t="s">
+      <c r="B63" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="C63" s="16" t="s">
+      <c r="C63" s="15" t="s">
         <v>326</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="E63" s="16" t="s">
+      <c r="E63" s="15" t="s">
         <v>327</v>
       </c>
-      <c r="F63" s="16" t="s">
+      <c r="F63" s="15" t="s">
         <v>327</v>
       </c>
-      <c r="G63" s="16" t="s">
+      <c r="G63" s="15" t="s">
         <v>326</v>
       </c>
       <c r="H63">
         <v>20</v>
       </c>
-      <c r="I63" s="20">
+      <c r="I63" s="19">
         <v>1</v>
       </c>
       <c r="J63" s="6" t="str">
@@ -10260,20 +10265,20 @@
         <v>572</v>
       </c>
     </row>
-    <row r="64" spans="1:28" ht="19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>475</v>
       </c>
-      <c r="B64" s="16" t="s">
+      <c r="B64" s="15" t="s">
         <v>476</v>
       </c>
-      <c r="C64" s="14" t="s">
+      <c r="C64" s="13" t="s">
         <v>478</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="E64" s="14" t="s">
+      <c r="E64" s="13" t="s">
         <v>477</v>
       </c>
       <c r="F64" s="1" t="s">
@@ -10285,7 +10290,7 @@
       <c r="H64">
         <v>10</v>
       </c>
-      <c r="I64" s="20">
+      <c r="I64" s="19">
         <v>1</v>
       </c>
       <c r="J64" s="6" t="str">
@@ -10296,20 +10301,20 @@
         <v>603</v>
       </c>
     </row>
-    <row r="65" spans="1:30" ht="19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:30" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>475</v>
       </c>
-      <c r="B65" s="16" t="s">
+      <c r="B65" s="15" t="s">
         <v>476</v>
       </c>
-      <c r="C65" s="16" t="s">
+      <c r="C65" s="15" t="s">
         <v>480</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="E65" s="14" t="s">
+      <c r="E65" s="13" t="s">
         <v>479</v>
       </c>
       <c r="F65" s="1" t="s">
@@ -10321,7 +10326,7 @@
       <c r="H65">
         <v>20</v>
       </c>
-      <c r="I65" s="20">
+      <c r="I65" s="19">
         <v>1</v>
       </c>
       <c r="J65" s="6" t="str">
@@ -10332,20 +10337,20 @@
         <v>604</v>
       </c>
     </row>
-    <row r="66" spans="1:30" ht="19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:30" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>475</v>
       </c>
-      <c r="B66" s="16" t="s">
+      <c r="B66" s="15" t="s">
         <v>476</v>
       </c>
-      <c r="C66" s="16" t="s">
+      <c r="C66" s="15" t="s">
         <v>482</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="E66" s="16" t="s">
+      <c r="E66" s="15" t="s">
         <v>481</v>
       </c>
       <c r="F66" s="1" t="s">
@@ -10357,7 +10362,7 @@
       <c r="H66">
         <v>30</v>
       </c>
-      <c r="I66" s="20">
+      <c r="I66" s="19">
         <v>1</v>
       </c>
       <c r="J66" s="6" t="str">
@@ -10368,32 +10373,32 @@
         <v>605</v>
       </c>
     </row>
-    <row r="67" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>489</v>
       </c>
-      <c r="B67" s="16" t="s">
+      <c r="B67" s="15" t="s">
         <v>627</v>
       </c>
-      <c r="C67" s="17" t="s">
+      <c r="C67" s="16" t="s">
         <v>490</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="E67" s="16" t="s">
+      <c r="E67" s="15" t="s">
         <v>493</v>
       </c>
-      <c r="F67" s="16" t="s">
+      <c r="F67" s="15" t="s">
         <v>493</v>
       </c>
-      <c r="G67" s="16" t="s">
+      <c r="G67" s="15" t="s">
         <v>494</v>
       </c>
       <c r="H67">
         <v>1</v>
       </c>
-      <c r="I67" s="20">
+      <c r="I67" s="19">
         <v>1</v>
       </c>
       <c r="J67" s="6" t="str">
@@ -10404,32 +10409,32 @@
         <v>495</v>
       </c>
     </row>
-    <row r="68" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>489</v>
       </c>
-      <c r="B68" s="16" t="s">
+      <c r="B68" s="15" t="s">
         <v>627</v>
       </c>
-      <c r="C68" s="17" t="s">
+      <c r="C68" s="16" t="s">
         <v>491</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="E68" s="16" t="s">
+      <c r="E68" s="15" t="s">
         <v>497</v>
       </c>
-      <c r="F68" s="16" t="s">
+      <c r="F68" s="15" t="s">
         <v>497</v>
       </c>
-      <c r="G68" s="16" t="s">
+      <c r="G68" s="15" t="s">
         <v>498</v>
       </c>
       <c r="H68">
         <v>2</v>
       </c>
-      <c r="I68" s="20">
+      <c r="I68" s="19">
         <v>1</v>
       </c>
       <c r="J68" s="6" t="str">
@@ -10440,11 +10445,11 @@
         <v>496</v>
       </c>
     </row>
-    <row r="69" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>489</v>
       </c>
-      <c r="B69" s="16" t="s">
+      <c r="B69" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C69" t="s">
@@ -10453,7 +10458,7 @@
       <c r="D69" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E69" s="14" t="s">
+      <c r="E69" s="13" t="s">
         <v>502</v>
       </c>
       <c r="F69" t="s">
@@ -10465,7 +10470,7 @@
       <c r="H69">
         <v>10</v>
       </c>
-      <c r="I69" s="20">
+      <c r="I69" s="19">
         <v>1</v>
       </c>
       <c r="J69" s="6" t="str">
@@ -10476,11 +10481,11 @@
         <v>501</v>
       </c>
     </row>
-    <row r="70" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>489</v>
       </c>
-      <c r="B70" s="16" t="s">
+      <c r="B70" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C70" t="s">
@@ -10489,7 +10494,7 @@
       <c r="D70" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E70" s="14" t="s">
+      <c r="E70" s="13" t="s">
         <v>503</v>
       </c>
       <c r="F70" t="s">
@@ -10501,7 +10506,7 @@
       <c r="H70">
         <v>20</v>
       </c>
-      <c r="I70" s="20">
+      <c r="I70" s="19">
         <v>1</v>
       </c>
       <c r="J70" s="6" t="str">
@@ -10512,11 +10517,11 @@
         <v>501</v>
       </c>
     </row>
-    <row r="71" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>489</v>
       </c>
-      <c r="B71" s="16" t="s">
+      <c r="B71" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C71" t="s">
@@ -10525,7 +10530,7 @@
       <c r="D71" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E71" s="14" t="s">
+      <c r="E71" s="13" t="s">
         <v>504</v>
       </c>
       <c r="F71" t="s">
@@ -10537,7 +10542,7 @@
       <c r="H71">
         <v>30</v>
       </c>
-      <c r="I71" s="20">
+      <c r="I71" s="19">
         <v>1</v>
       </c>
       <c r="J71" s="6" t="str">
@@ -10548,11 +10553,11 @@
         <v>501</v>
       </c>
     </row>
-    <row r="72" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>489</v>
       </c>
-      <c r="B72" s="16" t="s">
+      <c r="B72" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C72" t="s">
@@ -10561,7 +10566,7 @@
       <c r="D72" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E72" s="14" t="s">
+      <c r="E72" s="13" t="s">
         <v>505</v>
       </c>
       <c r="F72" t="s">
@@ -10573,7 +10578,7 @@
       <c r="H72">
         <v>40</v>
       </c>
-      <c r="I72" s="20">
+      <c r="I72" s="19">
         <v>1</v>
       </c>
       <c r="J72" s="6" t="str">
@@ -10584,11 +10589,11 @@
         <v>501</v>
       </c>
     </row>
-    <row r="73" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>489</v>
       </c>
-      <c r="B73" s="16" t="s">
+      <c r="B73" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C73" t="s">
@@ -10597,7 +10602,7 @@
       <c r="D73" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E73" s="14" t="s">
+      <c r="E73" s="13" t="s">
         <v>506</v>
       </c>
       <c r="F73" t="s">
@@ -10609,7 +10614,7 @@
       <c r="H73">
         <v>50</v>
       </c>
-      <c r="I73" s="20">
+      <c r="I73" s="19">
         <v>1</v>
       </c>
       <c r="J73" s="6" t="str">
@@ -10620,11 +10625,11 @@
         <v>501</v>
       </c>
     </row>
-    <row r="74" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>489</v>
       </c>
-      <c r="B74" s="16" t="s">
+      <c r="B74" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C74" t="s">
@@ -10633,7 +10638,7 @@
       <c r="D74" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E74" s="14" t="s">
+      <c r="E74" s="13" t="s">
         <v>507</v>
       </c>
       <c r="F74" t="s">
@@ -10645,7 +10650,7 @@
       <c r="H74">
         <v>60</v>
       </c>
-      <c r="I74" s="20">
+      <c r="I74" s="19">
         <v>1</v>
       </c>
       <c r="J74" s="6" t="str">
@@ -10656,11 +10661,11 @@
         <v>501</v>
       </c>
     </row>
-    <row r="75" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>489</v>
       </c>
-      <c r="B75" s="16" t="s">
+      <c r="B75" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C75" t="s">
@@ -10669,7 +10674,7 @@
       <c r="D75" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E75" s="14" t="s">
+      <c r="E75" s="13" t="s">
         <v>508</v>
       </c>
       <c r="F75" t="s">
@@ -10681,7 +10686,7 @@
       <c r="H75">
         <v>70</v>
       </c>
-      <c r="I75" s="20">
+      <c r="I75" s="19">
         <v>1</v>
       </c>
       <c r="J75" s="6" t="str">
@@ -10692,11 +10697,11 @@
         <v>501</v>
       </c>
     </row>
-    <row r="76" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>489</v>
       </c>
-      <c r="B76" s="16" t="s">
+      <c r="B76" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C76" t="s">
@@ -10705,7 +10710,7 @@
       <c r="D76" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E76" s="14" t="s">
+      <c r="E76" s="13" t="s">
         <v>509</v>
       </c>
       <c r="F76" t="s">
@@ -10717,7 +10722,7 @@
       <c r="H76">
         <v>80</v>
       </c>
-      <c r="I76" s="20">
+      <c r="I76" s="19">
         <v>1</v>
       </c>
       <c r="J76" s="6" t="str">
@@ -10728,11 +10733,11 @@
         <v>501</v>
       </c>
     </row>
-    <row r="77" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>489</v>
       </c>
-      <c r="B77" s="16" t="s">
+      <c r="B77" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C77" t="s">
@@ -10741,7 +10746,7 @@
       <c r="D77" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E77" s="14" t="s">
+      <c r="E77" s="13" t="s">
         <v>510</v>
       </c>
       <c r="F77" t="s">
@@ -10753,7 +10758,7 @@
       <c r="H77">
         <v>90</v>
       </c>
-      <c r="I77" s="20">
+      <c r="I77" s="19">
         <v>1</v>
       </c>
       <c r="J77" s="6" t="str">
@@ -10764,11 +10769,11 @@
         <v>501</v>
       </c>
     </row>
-    <row r="78" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>489</v>
       </c>
-      <c r="B78" s="16" t="s">
+      <c r="B78" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C78" t="s">
@@ -10777,7 +10782,7 @@
       <c r="D78" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E78" s="14" t="s">
+      <c r="E78" s="13" t="s">
         <v>511</v>
       </c>
       <c r="F78" t="s">
@@ -10789,7 +10794,7 @@
       <c r="H78">
         <v>100</v>
       </c>
-      <c r="I78" s="20">
+      <c r="I78" s="19">
         <v>1</v>
       </c>
       <c r="J78" s="6" t="str">
@@ -10800,11 +10805,11 @@
         <v>501</v>
       </c>
     </row>
-    <row r="79" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>489</v>
       </c>
-      <c r="B79" s="16" t="s">
+      <c r="B79" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C79" t="s">
@@ -10813,7 +10818,7 @@
       <c r="D79" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E79" s="14" t="s">
+      <c r="E79" s="13" t="s">
         <v>512</v>
       </c>
       <c r="F79" t="s">
@@ -10825,7 +10830,7 @@
       <c r="H79">
         <v>110</v>
       </c>
-      <c r="I79" s="20">
+      <c r="I79" s="19">
         <v>1</v>
       </c>
       <c r="J79" s="6" t="str">
@@ -10836,11 +10841,11 @@
         <v>501</v>
       </c>
     </row>
-    <row r="80" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>489</v>
       </c>
-      <c r="B80" s="16" t="s">
+      <c r="B80" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C80" t="s">
@@ -10849,7 +10854,7 @@
       <c r="D80" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E80" s="14" t="s">
+      <c r="E80" s="13" t="s">
         <v>513</v>
       </c>
       <c r="F80" t="s">
@@ -10861,7 +10866,7 @@
       <c r="H80">
         <v>120</v>
       </c>
-      <c r="I80" s="20">
+      <c r="I80" s="19">
         <v>1</v>
       </c>
       <c r="J80" s="6" t="str">
@@ -10872,11 +10877,11 @@
         <v>501</v>
       </c>
     </row>
-    <row r="81" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>489</v>
       </c>
-      <c r="B81" s="16" t="s">
+      <c r="B81" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C81" t="s">
@@ -10885,7 +10890,7 @@
       <c r="D81" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E81" s="14" t="s">
+      <c r="E81" s="13" t="s">
         <v>514</v>
       </c>
       <c r="F81" t="s">
@@ -10897,7 +10902,7 @@
       <c r="H81">
         <v>130</v>
       </c>
-      <c r="I81" s="20">
+      <c r="I81" s="19">
         <v>1</v>
       </c>
       <c r="J81" s="6" t="str">
@@ -10908,11 +10913,11 @@
         <v>501</v>
       </c>
     </row>
-    <row r="82" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>489</v>
       </c>
-      <c r="B82" s="16" t="s">
+      <c r="B82" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C82" t="s">
@@ -10921,7 +10926,7 @@
       <c r="D82" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E82" s="14" t="s">
+      <c r="E82" s="13" t="s">
         <v>515</v>
       </c>
       <c r="F82" t="s">
@@ -10933,7 +10938,7 @@
       <c r="H82">
         <v>140</v>
       </c>
-      <c r="I82" s="20">
+      <c r="I82" s="19">
         <v>1</v>
       </c>
       <c r="J82" s="6" t="str">
@@ -10944,11 +10949,11 @@
         <v>501</v>
       </c>
     </row>
-    <row r="83" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>489</v>
       </c>
-      <c r="B83" s="16" t="s">
+      <c r="B83" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C83" t="s">
@@ -10957,7 +10962,7 @@
       <c r="D83" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E83" s="14" t="s">
+      <c r="E83" s="13" t="s">
         <v>516</v>
       </c>
       <c r="F83" t="s">
@@ -10969,7 +10974,7 @@
       <c r="H83">
         <v>150</v>
       </c>
-      <c r="I83" s="20">
+      <c r="I83" s="19">
         <v>1</v>
       </c>
       <c r="J83" s="6" t="str">
@@ -10980,11 +10985,11 @@
         <v>501</v>
       </c>
     </row>
-    <row r="84" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>489</v>
       </c>
-      <c r="B84" s="16" t="s">
+      <c r="B84" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C84" t="s">
@@ -10993,7 +10998,7 @@
       <c r="D84" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E84" s="14" t="s">
+      <c r="E84" s="13" t="s">
         <v>517</v>
       </c>
       <c r="F84" t="s">
@@ -11005,7 +11010,7 @@
       <c r="H84">
         <v>160</v>
       </c>
-      <c r="I84" s="20">
+      <c r="I84" s="19">
         <v>1</v>
       </c>
       <c r="J84" s="6" t="str">
@@ -11016,11 +11021,11 @@
         <v>501</v>
       </c>
     </row>
-    <row r="85" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>489</v>
       </c>
-      <c r="B85" s="16" t="s">
+      <c r="B85" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C85" t="s">
@@ -11029,7 +11034,7 @@
       <c r="D85" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E85" s="14" t="s">
+      <c r="E85" s="13" t="s">
         <v>534</v>
       </c>
       <c r="F85" t="s">
@@ -11041,7 +11046,7 @@
       <c r="H85">
         <v>170</v>
       </c>
-      <c r="I85" s="20">
+      <c r="I85" s="19">
         <v>1</v>
       </c>
       <c r="J85" s="6" t="str">
@@ -11052,11 +11057,11 @@
         <v>566</v>
       </c>
     </row>
-    <row r="86" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>489</v>
       </c>
-      <c r="B86" s="16" t="s">
+      <c r="B86" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C86" t="s">
@@ -11065,7 +11070,7 @@
       <c r="D86" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E86" s="14" t="s">
+      <c r="E86" s="13" t="s">
         <v>535</v>
       </c>
       <c r="F86" t="s">
@@ -11077,7 +11082,7 @@
       <c r="H86">
         <v>180</v>
       </c>
-      <c r="I86" s="20">
+      <c r="I86" s="19">
         <v>1</v>
       </c>
       <c r="J86" s="6" t="str">
@@ -11088,11 +11093,11 @@
         <v>566</v>
       </c>
     </row>
-    <row r="87" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>489</v>
       </c>
-      <c r="B87" s="16" t="s">
+      <c r="B87" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C87" t="s">
@@ -11101,7 +11106,7 @@
       <c r="D87" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E87" s="14" t="s">
+      <c r="E87" s="13" t="s">
         <v>536</v>
       </c>
       <c r="F87" t="s">
@@ -11113,7 +11118,7 @@
       <c r="H87">
         <v>190</v>
       </c>
-      <c r="I87" s="20">
+      <c r="I87" s="19">
         <v>1</v>
       </c>
       <c r="J87" s="6" t="str">
@@ -11124,11 +11129,11 @@
         <v>566</v>
       </c>
     </row>
-    <row r="88" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>489</v>
       </c>
-      <c r="B88" s="16" t="s">
+      <c r="B88" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C88" t="s">
@@ -11137,7 +11142,7 @@
       <c r="D88" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E88" s="14" t="s">
+      <c r="E88" s="13" t="s">
         <v>537</v>
       </c>
       <c r="F88" t="s">
@@ -11149,7 +11154,7 @@
       <c r="H88">
         <v>200</v>
       </c>
-      <c r="I88" s="20">
+      <c r="I88" s="19">
         <v>1</v>
       </c>
       <c r="J88" s="6" t="str">
@@ -11160,11 +11165,11 @@
         <v>566</v>
       </c>
     </row>
-    <row r="89" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>489</v>
       </c>
-      <c r="B89" s="16" t="s">
+      <c r="B89" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C89" t="s">
@@ -11173,7 +11178,7 @@
       <c r="D89" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E89" s="14" t="s">
+      <c r="E89" s="13" t="s">
         <v>538</v>
       </c>
       <c r="F89" t="s">
@@ -11185,7 +11190,7 @@
       <c r="H89">
         <v>210</v>
       </c>
-      <c r="I89" s="20">
+      <c r="I89" s="19">
         <v>1</v>
       </c>
       <c r="J89" s="6" t="str">
@@ -11196,11 +11201,11 @@
         <v>566</v>
       </c>
     </row>
-    <row r="90" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>489</v>
       </c>
-      <c r="B90" s="16" t="s">
+      <c r="B90" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C90" t="s">
@@ -11209,7 +11214,7 @@
       <c r="D90" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E90" s="14" t="s">
+      <c r="E90" s="13" t="s">
         <v>539</v>
       </c>
       <c r="F90" t="s">
@@ -11221,7 +11226,7 @@
       <c r="H90">
         <v>220</v>
       </c>
-      <c r="I90" s="20">
+      <c r="I90" s="19">
         <v>1</v>
       </c>
       <c r="J90" s="6" t="str">
@@ -11232,11 +11237,11 @@
         <v>566</v>
       </c>
     </row>
-    <row r="91" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>489</v>
       </c>
-      <c r="B91" s="16" t="s">
+      <c r="B91" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C91" t="s">
@@ -11245,7 +11250,7 @@
       <c r="D91" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E91" s="14" t="s">
+      <c r="E91" s="13" t="s">
         <v>540</v>
       </c>
       <c r="F91" t="s">
@@ -11257,7 +11262,7 @@
       <c r="H91">
         <v>230</v>
       </c>
-      <c r="I91" s="20">
+      <c r="I91" s="19">
         <v>1</v>
       </c>
       <c r="J91" s="6" t="str">
@@ -11268,11 +11273,11 @@
         <v>566</v>
       </c>
     </row>
-    <row r="92" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>489</v>
       </c>
-      <c r="B92" s="16" t="s">
+      <c r="B92" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C92" t="s">
@@ -11281,7 +11286,7 @@
       <c r="D92" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E92" s="14" t="s">
+      <c r="E92" s="13" t="s">
         <v>541</v>
       </c>
       <c r="F92" t="s">
@@ -11293,7 +11298,7 @@
       <c r="H92">
         <v>240</v>
       </c>
-      <c r="I92" s="20">
+      <c r="I92" s="19">
         <v>1</v>
       </c>
       <c r="J92" s="6" t="str">
@@ -11304,11 +11309,11 @@
         <v>566</v>
       </c>
     </row>
-    <row r="93" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>489</v>
       </c>
-      <c r="B93" s="16" t="s">
+      <c r="B93" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C93" t="s">
@@ -11317,7 +11322,7 @@
       <c r="D93" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E93" s="14" t="s">
+      <c r="E93" s="13" t="s">
         <v>542</v>
       </c>
       <c r="F93" t="s">
@@ -11329,7 +11334,7 @@
       <c r="H93">
         <v>250</v>
       </c>
-      <c r="I93" s="20">
+      <c r="I93" s="19">
         <v>1</v>
       </c>
       <c r="J93" s="6" t="str">
@@ -11340,11 +11345,11 @@
         <v>566</v>
       </c>
     </row>
-    <row r="94" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>489</v>
       </c>
-      <c r="B94" s="16" t="s">
+      <c r="B94" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C94" t="s">
@@ -11353,7 +11358,7 @@
       <c r="D94" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E94" s="14" t="s">
+      <c r="E94" s="13" t="s">
         <v>543</v>
       </c>
       <c r="F94" t="s">
@@ -11365,7 +11370,7 @@
       <c r="H94">
         <v>260</v>
       </c>
-      <c r="I94" s="20">
+      <c r="I94" s="19">
         <v>1</v>
       </c>
       <c r="J94" s="6" t="str">
@@ -11376,11 +11381,11 @@
         <v>566</v>
       </c>
     </row>
-    <row r="95" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>489</v>
       </c>
-      <c r="B95" s="16" t="s">
+      <c r="B95" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C95" t="s">
@@ -11389,7 +11394,7 @@
       <c r="D95" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E95" s="14" t="s">
+      <c r="E95" s="13" t="s">
         <v>544</v>
       </c>
       <c r="F95" t="s">
@@ -11401,7 +11406,7 @@
       <c r="H95">
         <v>270</v>
       </c>
-      <c r="I95" s="20">
+      <c r="I95" s="19">
         <v>1</v>
       </c>
       <c r="J95" s="6" t="str">
@@ -11412,11 +11417,11 @@
         <v>566</v>
       </c>
     </row>
-    <row r="96" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:30" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>489</v>
       </c>
-      <c r="B96" s="16" t="s">
+      <c r="B96" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C96" t="s">
@@ -11425,7 +11430,7 @@
       <c r="D96" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E96" s="14" t="s">
+      <c r="E96" s="13" t="s">
         <v>545</v>
       </c>
       <c r="F96" t="s">
@@ -11437,7 +11442,7 @@
       <c r="H96">
         <v>280</v>
       </c>
-      <c r="I96" s="20">
+      <c r="I96" s="19">
         <v>1</v>
       </c>
       <c r="J96" s="6" t="str">
@@ -11448,11 +11453,11 @@
         <v>566</v>
       </c>
     </row>
-    <row r="97" spans="1:31" ht="18" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:31" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>489</v>
       </c>
-      <c r="B97" s="16" t="s">
+      <c r="B97" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C97" t="s">
@@ -11461,7 +11466,7 @@
       <c r="D97" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E97" s="14" t="s">
+      <c r="E97" s="13" t="s">
         <v>546</v>
       </c>
       <c r="F97" t="s">
@@ -11473,7 +11478,7 @@
       <c r="H97">
         <v>290</v>
       </c>
-      <c r="I97" s="20">
+      <c r="I97" s="19">
         <v>1</v>
       </c>
       <c r="J97" s="6" t="str">
@@ -11484,11 +11489,11 @@
         <v>566</v>
       </c>
     </row>
-    <row r="98" spans="1:31" ht="18" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:31" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>489</v>
       </c>
-      <c r="B98" s="16" t="s">
+      <c r="B98" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C98" t="s">
@@ -11497,7 +11502,7 @@
       <c r="D98" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E98" s="14" t="s">
+      <c r="E98" s="13" t="s">
         <v>547</v>
       </c>
       <c r="F98" t="s">
@@ -11509,7 +11514,7 @@
       <c r="H98">
         <v>300</v>
       </c>
-      <c r="I98" s="20">
+      <c r="I98" s="19">
         <v>1</v>
       </c>
       <c r="J98" s="6" t="str">
@@ -11520,11 +11525,11 @@
         <v>566</v>
       </c>
     </row>
-    <row r="99" spans="1:31" ht="18" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:31" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>489</v>
       </c>
-      <c r="B99" s="16" t="s">
+      <c r="B99" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C99" t="s">
@@ -11533,7 +11538,7 @@
       <c r="D99" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E99" s="14" t="s">
+      <c r="E99" s="13" t="s">
         <v>548</v>
       </c>
       <c r="F99" t="s">
@@ -11545,7 +11550,7 @@
       <c r="H99">
         <v>310</v>
       </c>
-      <c r="I99" s="20">
+      <c r="I99" s="19">
         <v>1</v>
       </c>
       <c r="J99" s="6" t="str">
@@ -11556,11 +11561,11 @@
         <v>566</v>
       </c>
     </row>
-    <row r="100" spans="1:31" ht="18" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:31" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>489</v>
       </c>
-      <c r="B100" s="16" t="s">
+      <c r="B100" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C100" t="s">
@@ -11569,7 +11574,7 @@
       <c r="D100" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E100" s="14" t="s">
+      <c r="E100" s="13" t="s">
         <v>549</v>
       </c>
       <c r="F100" t="s">
@@ -11581,7 +11586,7 @@
       <c r="H100">
         <v>320</v>
       </c>
-      <c r="I100" s="20">
+      <c r="I100" s="19">
         <v>1</v>
       </c>
       <c r="J100" s="6" t="str">
@@ -11592,32 +11597,32 @@
         <v>566</v>
       </c>
     </row>
-    <row r="101" spans="1:31" ht="18" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:31" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>489</v>
       </c>
-      <c r="B101" s="16" t="s">
+      <c r="B101" s="15" t="s">
         <v>627</v>
       </c>
-      <c r="C101" s="18" t="s">
+      <c r="C101" s="17" t="s">
         <v>573</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="E101" s="18" t="s">
+      <c r="E101" s="17" t="s">
         <v>582</v>
       </c>
-      <c r="F101" s="18" t="s">
+      <c r="F101" s="17" t="s">
         <v>312</v>
       </c>
-      <c r="G101" s="18" t="s">
+      <c r="G101" s="17" t="s">
         <v>311</v>
       </c>
       <c r="H101">
         <v>400</v>
       </c>
-      <c r="I101" s="20">
+      <c r="I101" s="19">
         <v>1</v>
       </c>
       <c r="J101" s="6" t="str">
@@ -11628,32 +11633,32 @@
         <v>581</v>
       </c>
     </row>
-    <row r="102" spans="1:31" ht="18" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:31" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>489</v>
       </c>
-      <c r="B102" s="16" t="s">
+      <c r="B102" s="15" t="s">
         <v>627</v>
       </c>
-      <c r="C102" s="18" t="s">
+      <c r="C102" s="17" t="s">
         <v>574</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="E102" s="18" t="s">
+      <c r="E102" s="17" t="s">
         <v>583</v>
       </c>
-      <c r="F102" s="18" t="s">
+      <c r="F102" s="17" t="s">
         <v>372</v>
       </c>
-      <c r="G102" s="18" t="s">
+      <c r="G102" s="17" t="s">
         <v>370</v>
       </c>
       <c r="H102">
         <v>410</v>
       </c>
-      <c r="I102" s="20">
+      <c r="I102" s="19">
         <v>1</v>
       </c>
       <c r="J102" s="6" t="str">
@@ -11664,32 +11669,32 @@
         <v>581</v>
       </c>
     </row>
-    <row r="103" spans="1:31" ht="18" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:31" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>489</v>
       </c>
-      <c r="B103" s="16" t="s">
+      <c r="B103" s="15" t="s">
         <v>627</v>
       </c>
-      <c r="C103" s="18" t="s">
+      <c r="C103" s="17" t="s">
         <v>575</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="E103" s="18" t="s">
+      <c r="E103" s="17" t="s">
         <v>584</v>
       </c>
-      <c r="F103" s="18" t="s">
+      <c r="F103" s="17" t="s">
         <v>375</v>
       </c>
-      <c r="G103" s="18" t="s">
+      <c r="G103" s="17" t="s">
         <v>374</v>
       </c>
       <c r="H103">
         <v>420</v>
       </c>
-      <c r="I103" s="20">
+      <c r="I103" s="19">
         <v>1</v>
       </c>
       <c r="J103" s="6" t="str">
@@ -11700,32 +11705,32 @@
         <v>581</v>
       </c>
     </row>
-    <row r="104" spans="1:31" ht="18" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:31" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>489</v>
       </c>
-      <c r="B104" s="16" t="s">
+      <c r="B104" s="15" t="s">
         <v>627</v>
       </c>
-      <c r="C104" s="18" t="s">
+      <c r="C104" s="17" t="s">
         <v>576</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="E104" s="18" t="s">
+      <c r="E104" s="17" t="s">
         <v>585</v>
       </c>
-      <c r="F104" s="18" t="s">
+      <c r="F104" s="17" t="s">
         <v>377</v>
       </c>
-      <c r="G104" s="18" t="s">
+      <c r="G104" s="17" t="s">
         <v>376</v>
       </c>
       <c r="H104">
         <v>430</v>
       </c>
-      <c r="I104" s="20">
+      <c r="I104" s="19">
         <v>1</v>
       </c>
       <c r="J104" s="6" t="str">
@@ -11736,32 +11741,32 @@
         <v>581</v>
       </c>
     </row>
-    <row r="105" spans="1:31" ht="18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:31" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>489</v>
       </c>
-      <c r="B105" s="16" t="s">
+      <c r="B105" s="15" t="s">
         <v>627</v>
       </c>
-      <c r="C105" s="18" t="s">
+      <c r="C105" s="17" t="s">
         <v>577</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="E105" s="18" t="s">
+      <c r="E105" s="17" t="s">
         <v>586</v>
       </c>
-      <c r="F105" s="18" t="s">
+      <c r="F105" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="G105" s="18" t="s">
+      <c r="G105" s="17" t="s">
         <v>371</v>
       </c>
       <c r="H105">
         <v>440</v>
       </c>
-      <c r="I105" s="20">
+      <c r="I105" s="19">
         <v>1</v>
       </c>
       <c r="J105" s="6" t="str">
@@ -11772,32 +11777,32 @@
         <v>581</v>
       </c>
     </row>
-    <row r="106" spans="1:31" ht="18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:31" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>489</v>
       </c>
-      <c r="B106" s="16" t="s">
+      <c r="B106" s="15" t="s">
         <v>627</v>
       </c>
-      <c r="C106" s="18" t="s">
+      <c r="C106" s="17" t="s">
         <v>578</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="E106" s="18" t="s">
+      <c r="E106" s="17" t="s">
         <v>587</v>
       </c>
-      <c r="F106" s="18" t="s">
+      <c r="F106" s="17" t="s">
         <v>382</v>
       </c>
-      <c r="G106" s="18" t="s">
+      <c r="G106" s="17" t="s">
         <v>317</v>
       </c>
       <c r="H106">
         <v>450</v>
       </c>
-      <c r="I106" s="20">
+      <c r="I106" s="19">
         <v>1</v>
       </c>
       <c r="J106" s="6" t="str">
@@ -11808,32 +11813,32 @@
         <v>581</v>
       </c>
     </row>
-    <row r="107" spans="1:31" ht="18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:31" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>489</v>
       </c>
-      <c r="B107" s="16" t="s">
+      <c r="B107" s="15" t="s">
         <v>627</v>
       </c>
-      <c r="C107" s="18" t="s">
+      <c r="C107" s="17" t="s">
         <v>579</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="E107" s="18" t="s">
+      <c r="E107" s="17" t="s">
         <v>588</v>
       </c>
-      <c r="F107" s="18" t="s">
+      <c r="F107" s="17" t="s">
         <v>378</v>
       </c>
-      <c r="G107" s="18" t="s">
+      <c r="G107" s="17" t="s">
         <v>379</v>
       </c>
       <c r="H107">
         <v>460</v>
       </c>
-      <c r="I107" s="20">
+      <c r="I107" s="19">
         <v>1</v>
       </c>
       <c r="J107" s="6" t="str">
@@ -11844,32 +11849,32 @@
         <v>581</v>
       </c>
     </row>
-    <row r="108" spans="1:31" ht="18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:31" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>489</v>
       </c>
-      <c r="B108" s="16" t="s">
+      <c r="B108" s="15" t="s">
         <v>627</v>
       </c>
-      <c r="C108" s="18" t="s">
+      <c r="C108" s="17" t="s">
         <v>580</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="E108" s="18" t="s">
+      <c r="E108" s="17" t="s">
         <v>589</v>
       </c>
-      <c r="F108" s="18" t="s">
+      <c r="F108" s="17" t="s">
         <v>381</v>
       </c>
-      <c r="G108" s="18" t="s">
+      <c r="G108" s="17" t="s">
         <v>380</v>
       </c>
       <c r="H108">
         <v>470</v>
       </c>
-      <c r="I108" s="20">
+      <c r="I108" s="19">
         <v>1</v>
       </c>
       <c r="J108" s="6" t="str">
@@ -11880,14 +11885,14 @@
         <v>581</v>
       </c>
     </row>
-    <row r="109" spans="1:31" ht="18" x14ac:dyDescent="0.25">
-      <c r="A109" s="16" t="s">
+    <row r="109" spans="1:31" ht="18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="15" t="s">
         <v>592</v>
       </c>
-      <c r="B109" s="16" t="s">
+      <c r="B109" s="15" t="s">
         <v>591</v>
       </c>
-      <c r="C109" s="16" t="s">
+      <c r="C109" s="15" t="s">
         <v>594</v>
       </c>
       <c r="D109" s="2" t="s">
@@ -11896,16 +11901,16 @@
       <c r="E109" t="s">
         <v>593</v>
       </c>
-      <c r="F109" s="14" t="s">
+      <c r="F109" s="13" t="s">
         <v>595</v>
       </c>
-      <c r="G109" s="16" t="s">
+      <c r="G109" s="15" t="s">
         <v>596</v>
       </c>
       <c r="H109">
         <v>510</v>
       </c>
-      <c r="I109" s="20">
+      <c r="I109" s="19">
         <v>1</v>
       </c>
       <c r="J109" s="6" t="str">
@@ -11916,14 +11921,14 @@
         <v>601</v>
       </c>
     </row>
-    <row r="110" spans="1:31" ht="18" x14ac:dyDescent="0.25">
-      <c r="A110" s="16" t="s">
+    <row r="110" spans="1:31" ht="18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="15" t="s">
         <v>592</v>
       </c>
-      <c r="B110" s="16" t="s">
+      <c r="B110" s="15" t="s">
         <v>591</v>
       </c>
-      <c r="C110" s="16" t="s">
+      <c r="C110" s="15" t="s">
         <v>599</v>
       </c>
       <c r="D110" s="2" t="s">
@@ -11932,16 +11937,16 @@
       <c r="E110" t="s">
         <v>600</v>
       </c>
-      <c r="F110" s="14" t="s">
+      <c r="F110" s="13" t="s">
         <v>598</v>
       </c>
-      <c r="G110" s="16" t="s">
+      <c r="G110" s="15" t="s">
         <v>597</v>
       </c>
       <c r="H110">
         <v>520</v>
       </c>
-      <c r="I110" s="20">
+      <c r="I110" s="19">
         <v>1</v>
       </c>
       <c r="J110" s="6" t="str">
@@ -11952,32 +11957,32 @@
         <v>602</v>
       </c>
     </row>
-    <row r="111" spans="1:31" ht="18" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:31" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>489</v>
       </c>
-      <c r="B111" s="16" t="s">
+      <c r="B111" s="15" t="s">
         <v>627</v>
       </c>
-      <c r="C111" s="18" t="s">
+      <c r="C111" s="17" t="s">
         <v>606</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="E111" s="18" t="s">
+      <c r="E111" s="17" t="s">
         <v>319</v>
       </c>
-      <c r="F111" s="18" t="s">
+      <c r="F111" s="17" t="s">
         <v>319</v>
       </c>
-      <c r="G111" s="18" t="s">
+      <c r="G111" s="17" t="s">
         <v>318</v>
       </c>
       <c r="H111">
         <v>610</v>
       </c>
-      <c r="I111" s="20">
+      <c r="I111" s="19">
         <v>1</v>
       </c>
       <c r="J111" s="6" t="str">
@@ -11988,32 +11993,32 @@
         <v>612</v>
       </c>
     </row>
-    <row r="112" spans="1:31" ht="18" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:31" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>489</v>
       </c>
-      <c r="B112" s="16" t="s">
+      <c r="B112" s="15" t="s">
         <v>627</v>
       </c>
-      <c r="C112" s="18" t="s">
+      <c r="C112" s="17" t="s">
         <v>607</v>
       </c>
-      <c r="D112" s="18" t="s">
+      <c r="D112" s="17" t="s">
         <v>386</v>
       </c>
-      <c r="E112" s="18" t="s">
+      <c r="E112" s="17" t="s">
         <v>609</v>
       </c>
-      <c r="F112" s="18" t="s">
+      <c r="F112" s="17" t="s">
         <v>609</v>
       </c>
-      <c r="G112" s="18" t="s">
+      <c r="G112" s="17" t="s">
         <v>608</v>
       </c>
       <c r="H112">
         <v>620</v>
       </c>
-      <c r="I112" s="20">
+      <c r="I112" s="19">
         <v>1</v>
       </c>
       <c r="J112" s="6" t="str">
@@ -12024,32 +12029,32 @@
         <v>612</v>
       </c>
     </row>
-    <row r="113" spans="1:32" ht="18" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:32" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>489</v>
       </c>
-      <c r="B113" s="16" t="s">
+      <c r="B113" s="15" t="s">
         <v>627</v>
       </c>
-      <c r="C113" s="18" t="s">
+      <c r="C113" s="17" t="s">
         <v>610</v>
       </c>
-      <c r="D113" s="18" t="s">
+      <c r="D113" s="17" t="s">
         <v>386</v>
       </c>
-      <c r="E113" s="18" t="s">
+      <c r="E113" s="17" t="s">
         <v>314</v>
       </c>
-      <c r="F113" s="18" t="s">
+      <c r="F113" s="17" t="s">
         <v>314</v>
       </c>
-      <c r="G113" s="18" t="s">
+      <c r="G113" s="17" t="s">
         <v>313</v>
       </c>
       <c r="H113">
         <v>630</v>
       </c>
-      <c r="I113" s="20">
+      <c r="I113" s="19">
         <v>1</v>
       </c>
       <c r="J113" s="6" t="str">
@@ -12060,32 +12065,32 @@
         <v>612</v>
       </c>
     </row>
-    <row r="114" spans="1:32" ht="18" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:32" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>489</v>
       </c>
-      <c r="B114" s="16" t="s">
+      <c r="B114" s="15" t="s">
         <v>627</v>
       </c>
-      <c r="C114" s="18" t="s">
+      <c r="C114" s="17" t="s">
         <v>611</v>
       </c>
-      <c r="D114" s="18" t="s">
+      <c r="D114" s="17" t="s">
         <v>386</v>
       </c>
-      <c r="E114" s="18" t="s">
+      <c r="E114" s="17" t="s">
         <v>312</v>
       </c>
-      <c r="F114" s="18" t="s">
+      <c r="F114" s="17" t="s">
         <v>312</v>
       </c>
-      <c r="G114" s="18" t="s">
+      <c r="G114" s="17" t="s">
         <v>311</v>
       </c>
       <c r="H114">
         <v>640</v>
       </c>
-      <c r="I114" s="20">
+      <c r="I114" s="19">
         <v>1</v>
       </c>
       <c r="J114" s="6" t="str">
@@ -12096,32 +12101,32 @@
         <v>612</v>
       </c>
     </row>
-    <row r="115" spans="1:32" ht="18" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:32" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>489</v>
       </c>
-      <c r="B115" s="16" t="s">
+      <c r="B115" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C115" t="s">
         <v>615</v>
       </c>
-      <c r="D115" s="18" t="s">
+      <c r="D115" s="17" t="s">
         <v>613</v>
       </c>
       <c r="E115" t="s">
         <v>614</v>
       </c>
-      <c r="F115" s="18" t="s">
+      <c r="F115" s="17" t="s">
         <v>623</v>
       </c>
-      <c r="G115" s="16" t="s">
+      <c r="G115" s="15" t="s">
         <v>624</v>
       </c>
       <c r="H115">
         <v>710</v>
       </c>
-      <c r="I115" s="20">
+      <c r="I115" s="19">
         <v>1</v>
       </c>
       <c r="J115" s="6" t="str">
@@ -12132,32 +12137,32 @@
         <v>622</v>
       </c>
     </row>
-    <row r="116" spans="1:32" ht="18" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:32" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>489</v>
       </c>
-      <c r="B116" s="16" t="s">
+      <c r="B116" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C116" t="s">
         <v>617</v>
       </c>
-      <c r="D116" s="18" t="s">
+      <c r="D116" s="17" t="s">
         <v>613</v>
       </c>
       <c r="E116" t="s">
         <v>616</v>
       </c>
-      <c r="F116" s="18" t="s">
+      <c r="F116" s="17" t="s">
         <v>623</v>
       </c>
-      <c r="G116" s="16" t="s">
+      <c r="G116" s="15" t="s">
         <v>624</v>
       </c>
       <c r="H116">
         <v>720</v>
       </c>
-      <c r="I116" s="20">
+      <c r="I116" s="19">
         <v>1</v>
       </c>
       <c r="J116" s="6" t="str">
@@ -12168,32 +12173,32 @@
         <v>622</v>
       </c>
     </row>
-    <row r="117" spans="1:32" ht="18" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:32" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>489</v>
       </c>
-      <c r="B117" s="16" t="s">
+      <c r="B117" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C117" t="s">
         <v>619</v>
       </c>
-      <c r="D117" s="18" t="s">
+      <c r="D117" s="17" t="s">
         <v>613</v>
       </c>
       <c r="E117" t="s">
         <v>618</v>
       </c>
-      <c r="F117" s="18" t="s">
+      <c r="F117" s="17" t="s">
         <v>623</v>
       </c>
-      <c r="G117" s="16" t="s">
+      <c r="G117" s="15" t="s">
         <v>624</v>
       </c>
       <c r="H117">
         <v>730</v>
       </c>
-      <c r="I117" s="20">
+      <c r="I117" s="19">
         <v>1</v>
       </c>
       <c r="J117" s="6" t="str">
@@ -12204,32 +12209,32 @@
         <v>622</v>
       </c>
     </row>
-    <row r="118" spans="1:32" ht="18" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:32" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>489</v>
       </c>
-      <c r="B118" s="16" t="s">
+      <c r="B118" s="15" t="s">
         <v>627</v>
       </c>
       <c r="C118" t="s">
         <v>621</v>
       </c>
-      <c r="D118" s="18" t="s">
+      <c r="D118" s="17" t="s">
         <v>613</v>
       </c>
       <c r="E118" t="s">
         <v>620</v>
       </c>
-      <c r="F118" s="18" t="s">
+      <c r="F118" s="17" t="s">
         <v>623</v>
       </c>
-      <c r="G118" s="16" t="s">
+      <c r="G118" s="15" t="s">
         <v>624</v>
       </c>
       <c r="H118">
         <v>740</v>
       </c>
-      <c r="I118" s="20">
+      <c r="I118" s="19">
         <v>1</v>
       </c>
       <c r="J118" s="6" t="str">
@@ -12240,20 +12245,20 @@
         <v>622</v>
       </c>
     </row>
-    <row r="119" spans="1:32" ht="19" x14ac:dyDescent="0.25">
-      <c r="A119" s="16" t="s">
+    <row r="119" spans="1:32" ht="19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="B119" s="16" t="s">
+      <c r="B119" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="C119" s="16" t="s">
+      <c r="C119" s="15" t="s">
         <v>324</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="E119" s="16" t="s">
+      <c r="E119" s="15" t="s">
         <v>325</v>
       </c>
       <c r="F119" s="1" t="s">
@@ -12265,7 +12270,7 @@
       <c r="H119">
         <v>10</v>
       </c>
-      <c r="I119" s="20">
+      <c r="I119" s="19">
         <v>1</v>
       </c>
       <c r="J119" s="6" t="str">
@@ -12276,20 +12281,20 @@
         <v>625</v>
       </c>
     </row>
-    <row r="120" spans="1:32" ht="19" x14ac:dyDescent="0.25">
-      <c r="A120" s="16" t="s">
+    <row r="120" spans="1:32" ht="19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="B120" s="16" t="s">
+      <c r="B120" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="C120" s="16" t="s">
+      <c r="C120" s="15" t="s">
         <v>326</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="E120" s="16" t="s">
+      <c r="E120" s="15" t="s">
         <v>327</v>
       </c>
       <c r="F120" s="1" t="s">
@@ -12301,7 +12306,7 @@
       <c r="H120">
         <v>20</v>
       </c>
-      <c r="I120" s="20">
+      <c r="I120" s="19">
         <v>1</v>
       </c>
       <c r="J120" s="6" t="str">
@@ -12313,7 +12318,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AF120" xr:uid="{F5070472-BD41-FC47-BC46-FB0AD4499DE3}"/>
+  <autoFilter ref="A1:AF120" xr:uid="{F5070472-BD41-FC47-BC46-FB0AD4499DE3}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="15+ (Specific)"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:W61">
     <sortCondition ref="H4:H61"/>
   </sortState>

</xml_diff>

<commit_message>
.periods and $periods to pe_iso
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -868,7 +868,7 @@
     <t>data_pack_type</t>
   </si>
   <si>
-    <t>B.periods</t>
+    <t>B.pe_iso</t>
   </si>
   <si>
     <t>B.age_set</t>
@@ -880,7 +880,7 @@
     <t>B.dx_code</t>
   </si>
   <si>
-    <t>A.periods</t>
+    <t>A.pe_iso</t>
   </si>
   <si>
     <t>A.age_set</t>

</xml_diff>

<commit_message>
Data Required csv Add technical area, disagg type, nom or den columns
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE76798A-6011-A84D-BD29-CB114FA5C21F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2093BA-581F-1F4F-827F-B2EDA3E64FA6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data_required!$A$1:$Z$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data_required!$A$1:$AM$56</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">dimension_Item_sets!$A$1:$AF$120</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2689" uniqueCount="629">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2702" uniqueCount="642">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1925,6 +1925,45 @@
   </si>
   <si>
     <t>A.dx_code</t>
+  </si>
+  <si>
+    <t>B.kp_set</t>
+  </si>
+  <si>
+    <t>A.technical_area</t>
+  </si>
+  <si>
+    <t>A.technical_area_uid</t>
+  </si>
+  <si>
+    <t>A.num_or_den</t>
+  </si>
+  <si>
+    <t>A.num_or_den_uid</t>
+  </si>
+  <si>
+    <t>A.disagg_type</t>
+  </si>
+  <si>
+    <t>A.disagg_type_uid</t>
+  </si>
+  <si>
+    <t>B.technical_area</t>
+  </si>
+  <si>
+    <t>B.technical_area_uid</t>
+  </si>
+  <si>
+    <t>B.num_or_den</t>
+  </si>
+  <si>
+    <t>B.num_or_den_uid</t>
+  </si>
+  <si>
+    <t>B.disagg_type</t>
+  </si>
+  <si>
+    <t>B.disagg_type_uid</t>
   </si>
 </sst>
 </file>
@@ -2320,12 +2359,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
-  <dimension ref="A1:Z56"/>
+  <dimension ref="A1:AM56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2333,18 +2372,18 @@
     <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.83203125" customWidth="1"/>
     <col min="3" max="3" width="8.1640625" customWidth="1"/>
-    <col min="4" max="4" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="123.83203125" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
     <col min="7" max="7" width="68.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="14" width="17.33203125" customWidth="1"/>
-    <col min="15" max="15" width="53.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="46.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="20" width="17.33203125" customWidth="1"/>
+    <col min="21" max="21" width="53.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="46.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>274</v>
       </c>
@@ -2382,49 +2421,88 @@
         <v>283</v>
       </c>
       <c r="M1" t="s">
+        <v>630</v>
+      </c>
+      <c r="N1" t="s">
+        <v>631</v>
+      </c>
+      <c r="O1" t="s">
+        <v>632</v>
+      </c>
+      <c r="P1" t="s">
+        <v>633</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>634</v>
+      </c>
+      <c r="R1" t="s">
+        <v>635</v>
+      </c>
+      <c r="S1" t="s">
         <v>288</v>
       </c>
-      <c r="N1" t="s">
+      <c r="T1" t="s">
         <v>391</v>
       </c>
-      <c r="O1" t="s">
+      <c r="U1" t="s">
         <v>289</v>
       </c>
-      <c r="P1" t="s">
+      <c r="V1" t="s">
         <v>392</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="W1" t="s">
         <v>279</v>
       </c>
-      <c r="R1" t="s">
+      <c r="X1" t="s">
         <v>393</v>
       </c>
-      <c r="S1" t="s">
+      <c r="Y1" t="s">
         <v>276</v>
       </c>
-      <c r="T1" t="s">
+      <c r="Z1" t="s">
         <v>277</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AA1" t="s">
         <v>278</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AB1" t="s">
+        <v>629</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>636</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>637</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>638</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>639</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>640</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>641</v>
+      </c>
+      <c r="AI1" t="s">
         <v>429</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AJ1" t="s">
         <v>430</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AK1" t="s">
         <v>431</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AL1" t="s">
         <v>432</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AM1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2461,24 +2539,6 @@
       <c r="L2" t="s">
         <v>237</v>
       </c>
-      <c r="M2" t="s">
-        <v>237</v>
-      </c>
-      <c r="N2" t="s">
-        <v>237</v>
-      </c>
-      <c r="O2" t="s">
-        <v>237</v>
-      </c>
-      <c r="P2" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>237</v>
-      </c>
-      <c r="R2" t="s">
-        <v>237</v>
-      </c>
       <c r="S2" t="s">
         <v>237</v>
       </c>
@@ -2503,8 +2563,26 @@
       <c r="Z2" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2541,24 +2619,6 @@
       <c r="L3" t="s">
         <v>237</v>
       </c>
-      <c r="M3" t="s">
-        <v>237</v>
-      </c>
-      <c r="N3" t="s">
-        <v>237</v>
-      </c>
-      <c r="O3" t="s">
-        <v>237</v>
-      </c>
-      <c r="P3" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>237</v>
-      </c>
-      <c r="R3" t="s">
-        <v>237</v>
-      </c>
       <c r="S3" t="s">
         <v>237</v>
       </c>
@@ -2583,8 +2643,26 @@
       <c r="Z3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA3" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2621,24 +2699,6 @@
       <c r="L4" t="s">
         <v>237</v>
       </c>
-      <c r="M4" t="s">
-        <v>237</v>
-      </c>
-      <c r="N4" t="s">
-        <v>237</v>
-      </c>
-      <c r="O4" t="s">
-        <v>237</v>
-      </c>
-      <c r="P4" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>237</v>
-      </c>
-      <c r="R4" t="s">
-        <v>237</v>
-      </c>
       <c r="S4" t="s">
         <v>237</v>
       </c>
@@ -2663,8 +2723,26 @@
       <c r="Z4" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA4" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -2701,24 +2779,6 @@
       <c r="L5" t="s">
         <v>237</v>
       </c>
-      <c r="M5" t="s">
-        <v>237</v>
-      </c>
-      <c r="N5" t="s">
-        <v>237</v>
-      </c>
-      <c r="O5" t="s">
-        <v>237</v>
-      </c>
-      <c r="P5" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>237</v>
-      </c>
-      <c r="R5" t="s">
-        <v>237</v>
-      </c>
       <c r="S5" t="s">
         <v>237</v>
       </c>
@@ -2743,8 +2803,26 @@
       <c r="Z5" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2781,24 +2859,6 @@
       <c r="L6" t="s">
         <v>237</v>
       </c>
-      <c r="M6" t="s">
-        <v>237</v>
-      </c>
-      <c r="N6" t="s">
-        <v>237</v>
-      </c>
-      <c r="O6" t="s">
-        <v>237</v>
-      </c>
-      <c r="P6" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>237</v>
-      </c>
-      <c r="R6" t="s">
-        <v>237</v>
-      </c>
       <c r="S6" t="s">
         <v>237</v>
       </c>
@@ -2823,8 +2883,26 @@
       <c r="Z6" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA6" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -2861,24 +2939,6 @@
       <c r="L7" t="s">
         <v>237</v>
       </c>
-      <c r="M7" t="s">
-        <v>237</v>
-      </c>
-      <c r="N7" t="s">
-        <v>237</v>
-      </c>
-      <c r="O7" t="s">
-        <v>237</v>
-      </c>
-      <c r="P7" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>237</v>
-      </c>
-      <c r="R7" t="s">
-        <v>237</v>
-      </c>
       <c r="S7" t="s">
         <v>237</v>
       </c>
@@ -2903,8 +2963,26 @@
       <c r="Z7" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA7" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -2941,50 +3019,50 @@
       <c r="L8" t="s">
         <v>237</v>
       </c>
-      <c r="M8" t="s">
-        <v>237</v>
-      </c>
-      <c r="N8" t="s">
-        <v>237</v>
-      </c>
-      <c r="O8" t="s">
-        <v>237</v>
-      </c>
-      <c r="P8" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q8" t="s">
+      <c r="S8" t="s">
+        <v>237</v>
+      </c>
+      <c r="T8" t="s">
+        <v>237</v>
+      </c>
+      <c r="U8" t="s">
+        <v>237</v>
+      </c>
+      <c r="V8" t="s">
+        <v>237</v>
+      </c>
+      <c r="W8" t="s">
         <v>136</v>
       </c>
-      <c r="R8" t="s">
+      <c r="X8" t="s">
         <v>137</v>
       </c>
-      <c r="S8" t="s">
+      <c r="Y8" t="s">
         <v>233</v>
       </c>
-      <c r="T8" s="2" t="s">
+      <c r="Z8" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="U8" t="s">
+      <c r="AA8" t="s">
         <v>241</v>
       </c>
-      <c r="V8" t="s">
-        <v>237</v>
-      </c>
-      <c r="W8" t="s">
-        <v>237</v>
-      </c>
-      <c r="X8" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>237</v>
-      </c>
-      <c r="Z8" t="s">
+      <c r="AI8" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM8" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -3021,24 +3099,6 @@
       <c r="L9" t="s">
         <v>237</v>
       </c>
-      <c r="M9" t="s">
-        <v>237</v>
-      </c>
-      <c r="N9" t="s">
-        <v>237</v>
-      </c>
-      <c r="O9" t="s">
-        <v>237</v>
-      </c>
-      <c r="P9" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>237</v>
-      </c>
-      <c r="R9" t="s">
-        <v>237</v>
-      </c>
       <c r="S9" t="s">
         <v>237</v>
       </c>
@@ -3063,8 +3123,26 @@
       <c r="Z9" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA9" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -3101,24 +3179,6 @@
       <c r="L10" t="s">
         <v>237</v>
       </c>
-      <c r="M10" t="s">
-        <v>237</v>
-      </c>
-      <c r="N10" t="s">
-        <v>237</v>
-      </c>
-      <c r="O10" t="s">
-        <v>237</v>
-      </c>
-      <c r="P10" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>237</v>
-      </c>
-      <c r="R10" t="s">
-        <v>237</v>
-      </c>
       <c r="S10" t="s">
         <v>237</v>
       </c>
@@ -3143,8 +3203,26 @@
       <c r="Z10" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA10" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK10" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -3181,24 +3259,6 @@
       <c r="L11" t="s">
         <v>237</v>
       </c>
-      <c r="M11" t="s">
-        <v>237</v>
-      </c>
-      <c r="N11" t="s">
-        <v>237</v>
-      </c>
-      <c r="O11" t="s">
-        <v>237</v>
-      </c>
-      <c r="P11" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>237</v>
-      </c>
-      <c r="R11" t="s">
-        <v>237</v>
-      </c>
       <c r="S11" t="s">
         <v>237</v>
       </c>
@@ -3223,8 +3283,26 @@
       <c r="Z11" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA11" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -3261,24 +3339,6 @@
       <c r="L12" t="s">
         <v>237</v>
       </c>
-      <c r="M12" t="s">
-        <v>237</v>
-      </c>
-      <c r="N12" t="s">
-        <v>237</v>
-      </c>
-      <c r="O12" t="s">
-        <v>237</v>
-      </c>
-      <c r="P12" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>237</v>
-      </c>
-      <c r="R12" t="s">
-        <v>237</v>
-      </c>
       <c r="S12" t="s">
         <v>237</v>
       </c>
@@ -3303,8 +3363,26 @@
       <c r="Z12" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA12" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL12" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -3341,24 +3419,6 @@
       <c r="L13" t="s">
         <v>237</v>
       </c>
-      <c r="M13" t="s">
-        <v>237</v>
-      </c>
-      <c r="N13" t="s">
-        <v>237</v>
-      </c>
-      <c r="O13" t="s">
-        <v>237</v>
-      </c>
-      <c r="P13" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>237</v>
-      </c>
-      <c r="R13" t="s">
-        <v>237</v>
-      </c>
       <c r="S13" t="s">
         <v>237</v>
       </c>
@@ -3383,8 +3443,26 @@
       <c r="Z13" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA13" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM13" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -3421,24 +3499,6 @@
       <c r="L14" t="s">
         <v>237</v>
       </c>
-      <c r="M14" t="s">
-        <v>237</v>
-      </c>
-      <c r="N14" t="s">
-        <v>237</v>
-      </c>
-      <c r="O14" t="s">
-        <v>237</v>
-      </c>
-      <c r="P14" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>237</v>
-      </c>
-      <c r="R14" t="s">
-        <v>237</v>
-      </c>
       <c r="S14" t="s">
         <v>237</v>
       </c>
@@ -3463,8 +3523,26 @@
       <c r="Z14" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="15" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+      <c r="AA14" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -3501,36 +3579,18 @@
       <c r="L15" t="s">
         <v>237</v>
       </c>
-      <c r="M15" s="10" t="s">
+      <c r="S15" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="N15" t="s">
+      <c r="T15" t="s">
         <v>296</v>
       </c>
-      <c r="O15" t="s">
+      <c r="U15" t="s">
         <v>425</v>
       </c>
-      <c r="P15" t="s">
+      <c r="V15" t="s">
         <v>426</v>
       </c>
-      <c r="Q15" t="s">
-        <v>237</v>
-      </c>
-      <c r="R15" t="s">
-        <v>237</v>
-      </c>
-      <c r="S15" t="s">
-        <v>237</v>
-      </c>
-      <c r="T15" t="s">
-        <v>237</v>
-      </c>
-      <c r="U15" t="s">
-        <v>237</v>
-      </c>
-      <c r="V15" t="s">
-        <v>237</v>
-      </c>
       <c r="W15" t="s">
         <v>237</v>
       </c>
@@ -3543,8 +3603,26 @@
       <c r="Z15" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+      <c r="AA15" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL15" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM15" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -3581,36 +3659,18 @@
       <c r="L16" t="s">
         <v>237</v>
       </c>
-      <c r="M16" s="10" t="s">
+      <c r="S16" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="N16" t="s">
+      <c r="T16" t="s">
         <v>296</v>
       </c>
-      <c r="O16" t="s">
+      <c r="U16" t="s">
         <v>427</v>
       </c>
-      <c r="P16" t="s">
+      <c r="V16" t="s">
         <v>428</v>
       </c>
-      <c r="Q16" t="s">
-        <v>237</v>
-      </c>
-      <c r="R16" t="s">
-        <v>237</v>
-      </c>
-      <c r="S16" t="s">
-        <v>237</v>
-      </c>
-      <c r="T16" t="s">
-        <v>237</v>
-      </c>
-      <c r="U16" t="s">
-        <v>237</v>
-      </c>
-      <c r="V16" t="s">
-        <v>237</v>
-      </c>
       <c r="W16" t="s">
         <v>237</v>
       </c>
@@ -3623,8 +3683,26 @@
       <c r="Z16" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="17" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="AA16" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK16" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL16" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM16" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -3658,50 +3736,50 @@
       <c r="L17" t="s">
         <v>237</v>
       </c>
-      <c r="M17" s="10" t="s">
+      <c r="S17" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="N17" t="s">
+      <c r="T17" t="s">
         <v>296</v>
       </c>
-      <c r="O17" t="s">
+      <c r="U17" t="s">
         <v>425</v>
       </c>
-      <c r="P17" t="s">
+      <c r="V17" t="s">
         <v>426</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="W17" t="s">
         <v>419</v>
       </c>
-      <c r="R17" s="1" t="s">
+      <c r="X17" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="S17" t="s">
+      <c r="Y17" t="s">
         <v>233</v>
       </c>
-      <c r="T17" t="s">
+      <c r="Z17" t="s">
         <v>252</v>
       </c>
-      <c r="U17" t="s">
+      <c r="AA17" t="s">
         <v>251</v>
       </c>
-      <c r="V17" s="10" t="s">
+      <c r="AI17" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="W17" t="s">
+      <c r="AJ17" t="s">
         <v>296</v>
       </c>
-      <c r="X17" t="s">
+      <c r="AK17" t="s">
         <v>427</v>
       </c>
-      <c r="Y17" t="s">
+      <c r="AL17" t="s">
         <v>428</v>
       </c>
-      <c r="Z17" t="s">
+      <c r="AM17" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -3738,50 +3816,50 @@
       <c r="L18" t="s">
         <v>237</v>
       </c>
-      <c r="M18" s="10" t="s">
+      <c r="S18" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="N18" t="s">
+      <c r="T18" t="s">
         <v>296</v>
       </c>
-      <c r="O18" t="s">
+      <c r="U18" t="s">
         <v>435</v>
       </c>
-      <c r="P18" t="s">
+      <c r="V18" t="s">
         <v>253</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="W18" t="s">
         <v>419</v>
       </c>
-      <c r="R18" s="1" t="s">
+      <c r="X18" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="S18" t="s">
+      <c r="Y18" t="s">
         <v>233</v>
       </c>
-      <c r="T18" s="9" t="s">
+      <c r="Z18" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="U18" t="s">
+      <c r="AA18" t="s">
         <v>251</v>
       </c>
-      <c r="V18" t="s">
-        <v>237</v>
-      </c>
-      <c r="W18" t="s">
-        <v>237</v>
-      </c>
-      <c r="X18" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>237</v>
-      </c>
-      <c r="Z18" t="s">
+      <c r="AI18" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK18" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL18" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM18" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -3818,50 +3896,50 @@
       <c r="L19" t="s">
         <v>237</v>
       </c>
-      <c r="M19" s="10" t="s">
+      <c r="S19" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="N19" t="s">
+      <c r="T19" t="s">
         <v>296</v>
       </c>
-      <c r="O19" t="s">
+      <c r="U19" t="s">
         <v>436</v>
       </c>
-      <c r="P19" t="s">
+      <c r="V19" t="s">
         <v>261</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="W19" t="s">
         <v>419</v>
       </c>
-      <c r="R19" s="1" t="s">
+      <c r="X19" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="S19" t="s">
+      <c r="Y19" t="s">
         <v>233</v>
       </c>
-      <c r="T19" s="9" t="s">
+      <c r="Z19" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="U19" t="s">
+      <c r="AA19" t="s">
         <v>251</v>
       </c>
-      <c r="V19" t="s">
-        <v>237</v>
-      </c>
-      <c r="W19" t="s">
-        <v>237</v>
-      </c>
-      <c r="X19" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>237</v>
-      </c>
-      <c r="Z19" t="s">
+      <c r="AI19" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK19" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL19" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM19" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -3898,50 +3976,50 @@
       <c r="L20" t="s">
         <v>237</v>
       </c>
-      <c r="M20" s="10" t="s">
+      <c r="S20" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="N20" t="s">
+      <c r="T20" t="s">
         <v>296</v>
       </c>
-      <c r="O20" t="s">
+      <c r="U20" t="s">
         <v>437</v>
       </c>
-      <c r="P20" t="s">
+      <c r="V20" t="s">
         <v>268</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="W20" t="s">
         <v>419</v>
       </c>
-      <c r="R20" s="1" t="s">
+      <c r="X20" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="S20" t="s">
+      <c r="Y20" t="s">
         <v>233</v>
       </c>
-      <c r="T20" s="9" t="s">
+      <c r="Z20" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="U20" t="s">
+      <c r="AA20" t="s">
         <v>251</v>
       </c>
-      <c r="V20" t="s">
-        <v>237</v>
-      </c>
-      <c r="W20" t="s">
-        <v>237</v>
-      </c>
-      <c r="X20" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>237</v>
-      </c>
-      <c r="Z20" t="s">
+      <c r="AI20" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ20" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK20" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL20" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM20" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -3978,50 +4056,50 @@
       <c r="L21" t="s">
         <v>237</v>
       </c>
-      <c r="M21" s="10" t="s">
+      <c r="S21" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="N21" t="s">
+      <c r="T21" t="s">
         <v>296</v>
       </c>
-      <c r="O21" t="s">
+      <c r="U21" t="s">
         <v>438</v>
       </c>
-      <c r="P21" t="s">
+      <c r="V21" t="s">
         <v>263</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="W21" t="s">
         <v>419</v>
       </c>
-      <c r="R21" s="1" t="s">
+      <c r="X21" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="S21" t="s">
+      <c r="Y21" t="s">
         <v>233</v>
       </c>
-      <c r="T21" s="9" t="s">
+      <c r="Z21" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="U21" t="s">
+      <c r="AA21" t="s">
         <v>251</v>
       </c>
-      <c r="V21" t="s">
-        <v>237</v>
-      </c>
-      <c r="W21" t="s">
-        <v>237</v>
-      </c>
-      <c r="X21" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>237</v>
-      </c>
-      <c r="Z21" t="s">
+      <c r="AI21" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ21" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK21" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL21" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM21" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -4058,50 +4136,50 @@
       <c r="L22" t="s">
         <v>237</v>
       </c>
-      <c r="M22" s="10" t="s">
+      <c r="S22" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="N22" t="s">
+      <c r="T22" t="s">
         <v>296</v>
       </c>
-      <c r="O22" t="s">
+      <c r="U22" t="s">
         <v>439</v>
       </c>
-      <c r="P22" t="s">
+      <c r="V22" t="s">
         <v>264</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="W22" t="s">
         <v>419</v>
       </c>
-      <c r="R22" s="1" t="s">
+      <c r="X22" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="S22" t="s">
+      <c r="Y22" t="s">
         <v>233</v>
       </c>
-      <c r="T22" s="9" t="s">
+      <c r="Z22" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="U22" t="s">
+      <c r="AA22" t="s">
         <v>251</v>
       </c>
-      <c r="V22" t="s">
-        <v>237</v>
-      </c>
-      <c r="W22" t="s">
-        <v>237</v>
-      </c>
-      <c r="X22" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>237</v>
-      </c>
-      <c r="Z22" t="s">
+      <c r="AI22" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ22" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK22" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL22" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM22" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -4138,50 +4216,50 @@
       <c r="L23" t="s">
         <v>237</v>
       </c>
-      <c r="M23" s="10" t="s">
+      <c r="S23" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="N23" t="s">
+      <c r="T23" t="s">
         <v>296</v>
       </c>
-      <c r="O23" t="s">
+      <c r="U23" t="s">
         <v>440</v>
       </c>
-      <c r="P23" t="s">
+      <c r="V23" t="s">
         <v>265</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="W23" t="s">
         <v>419</v>
       </c>
-      <c r="R23" s="1" t="s">
+      <c r="X23" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="S23" t="s">
+      <c r="Y23" t="s">
         <v>233</v>
       </c>
-      <c r="T23" s="3" t="s">
+      <c r="Z23" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="U23" t="s">
+      <c r="AA23" t="s">
         <v>251</v>
       </c>
-      <c r="V23" t="s">
-        <v>237</v>
-      </c>
-      <c r="W23" t="s">
-        <v>237</v>
-      </c>
-      <c r="X23" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>237</v>
-      </c>
-      <c r="Z23" t="s">
+      <c r="AI23" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ23" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK23" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL23" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM23" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -4218,50 +4296,50 @@
       <c r="L24" t="s">
         <v>237</v>
       </c>
-      <c r="M24" s="10" t="s">
+      <c r="S24" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="N24" t="s">
+      <c r="T24" t="s">
         <v>296</v>
       </c>
-      <c r="O24" t="s">
+      <c r="U24" t="s">
         <v>441</v>
       </c>
-      <c r="P24" t="s">
+      <c r="V24" t="s">
         <v>266</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="W24" t="s">
         <v>419</v>
       </c>
-      <c r="R24" s="1" t="s">
+      <c r="X24" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="S24" t="s">
+      <c r="Y24" t="s">
         <v>233</v>
       </c>
-      <c r="T24" s="3" t="s">
+      <c r="Z24" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="U24" t="s">
+      <c r="AA24" t="s">
         <v>251</v>
       </c>
-      <c r="V24" t="s">
-        <v>237</v>
-      </c>
-      <c r="W24" t="s">
-        <v>237</v>
-      </c>
-      <c r="X24" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>237</v>
-      </c>
-      <c r="Z24" t="s">
+      <c r="AI24" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ24" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK24" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL24" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM24" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -4298,50 +4376,50 @@
       <c r="L25" t="s">
         <v>237</v>
       </c>
-      <c r="M25" s="10" t="s">
+      <c r="S25" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="N25" t="s">
+      <c r="T25" t="s">
         <v>296</v>
       </c>
-      <c r="O25" t="s">
+      <c r="U25" t="s">
         <v>442</v>
       </c>
-      <c r="P25" t="s">
+      <c r="V25" t="s">
         <v>267</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="W25" t="s">
         <v>419</v>
       </c>
-      <c r="R25" s="1" t="s">
+      <c r="X25" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="S25" t="s">
+      <c r="Y25" t="s">
         <v>233</v>
       </c>
-      <c r="T25" s="9" t="s">
+      <c r="Z25" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="U25" t="s">
+      <c r="AA25" t="s">
         <v>251</v>
       </c>
-      <c r="V25" t="s">
-        <v>237</v>
-      </c>
-      <c r="W25" t="s">
-        <v>237</v>
-      </c>
-      <c r="X25" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>237</v>
-      </c>
-      <c r="Z25" t="s">
+      <c r="AI25" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ25" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK25" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL25" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM25" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -4378,50 +4456,50 @@
       <c r="L26" t="s">
         <v>237</v>
       </c>
-      <c r="M26" s="10" t="s">
+      <c r="S26" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="N26" t="s">
+      <c r="T26" t="s">
         <v>296</v>
       </c>
-      <c r="O26" t="s">
+      <c r="U26" t="s">
         <v>443</v>
       </c>
-      <c r="P26" t="s">
+      <c r="V26" t="s">
         <v>262</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="W26" t="s">
         <v>419</v>
       </c>
-      <c r="R26" s="1" t="s">
+      <c r="X26" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="S26" t="s">
+      <c r="Y26" t="s">
         <v>233</v>
       </c>
-      <c r="T26" s="9" t="s">
+      <c r="Z26" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="U26" t="s">
+      <c r="AA26" t="s">
         <v>251</v>
       </c>
-      <c r="V26" t="s">
-        <v>237</v>
-      </c>
-      <c r="W26" t="s">
-        <v>237</v>
-      </c>
-      <c r="X26" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y26" t="s">
-        <v>237</v>
-      </c>
-      <c r="Z26" t="s">
+      <c r="AI26" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ26" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK26" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL26" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM26" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="27" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -4458,50 +4536,50 @@
       <c r="L27" t="s">
         <v>237</v>
       </c>
-      <c r="M27" s="10" t="s">
+      <c r="S27" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="N27" t="s">
+      <c r="T27" t="s">
         <v>296</v>
       </c>
-      <c r="O27" t="s">
+      <c r="U27" t="s">
         <v>444</v>
       </c>
-      <c r="P27" t="s">
+      <c r="V27" t="s">
         <v>269</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="W27" t="s">
         <v>419</v>
       </c>
-      <c r="R27" s="1" t="s">
+      <c r="X27" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="S27" t="s">
+      <c r="Y27" t="s">
         <v>233</v>
       </c>
-      <c r="T27" s="9" t="s">
+      <c r="Z27" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="U27" t="s">
+      <c r="AA27" t="s">
         <v>251</v>
       </c>
-      <c r="V27" t="s">
-        <v>237</v>
-      </c>
-      <c r="W27" t="s">
-        <v>237</v>
-      </c>
-      <c r="X27" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y27" t="s">
-        <v>237</v>
-      </c>
-      <c r="Z27" t="s">
+      <c r="AI27" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ27" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK27" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL27" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM27" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -4538,36 +4616,18 @@
       <c r="L28" t="s">
         <v>237</v>
       </c>
-      <c r="M28" s="10" t="s">
+      <c r="S28" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="N28" t="s">
+      <c r="T28" t="s">
         <v>296</v>
       </c>
-      <c r="O28" t="s">
+      <c r="U28" t="s">
         <v>435</v>
       </c>
-      <c r="P28" t="s">
+      <c r="V28" t="s">
         <v>253</v>
       </c>
-      <c r="Q28" t="s">
-        <v>237</v>
-      </c>
-      <c r="R28" t="s">
-        <v>237</v>
-      </c>
-      <c r="S28" t="s">
-        <v>237</v>
-      </c>
-      <c r="T28" t="s">
-        <v>237</v>
-      </c>
-      <c r="U28" t="s">
-        <v>237</v>
-      </c>
-      <c r="V28" t="s">
-        <v>237</v>
-      </c>
       <c r="W28" t="s">
         <v>237</v>
       </c>
@@ -4580,8 +4640,26 @@
       <c r="Z28" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="29" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="AA28" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI28" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ28" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK28" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL28" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:39" ht="19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -4618,36 +4696,18 @@
       <c r="L29" t="s">
         <v>237</v>
       </c>
-      <c r="M29" s="10" t="s">
+      <c r="S29" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="N29" t="s">
+      <c r="T29" t="s">
         <v>296</v>
       </c>
-      <c r="O29" t="s">
+      <c r="U29" t="s">
         <v>436</v>
       </c>
-      <c r="P29" t="s">
+      <c r="V29" t="s">
         <v>261</v>
       </c>
-      <c r="Q29" t="s">
-        <v>237</v>
-      </c>
-      <c r="R29" t="s">
-        <v>237</v>
-      </c>
-      <c r="S29" t="s">
-        <v>237</v>
-      </c>
-      <c r="T29" t="s">
-        <v>237</v>
-      </c>
-      <c r="U29" t="s">
-        <v>237</v>
-      </c>
-      <c r="V29" t="s">
-        <v>237</v>
-      </c>
       <c r="W29" t="s">
         <v>237</v>
       </c>
@@ -4660,8 +4720,26 @@
       <c r="Z29" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="30" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="AA29" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI29" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ29" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK29" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL29" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM29" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="30" spans="1:39" ht="19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -4698,36 +4776,18 @@
       <c r="L30" t="s">
         <v>237</v>
       </c>
-      <c r="M30" s="10" t="s">
+      <c r="S30" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="N30" t="s">
+      <c r="T30" t="s">
         <v>296</v>
       </c>
-      <c r="O30" t="s">
+      <c r="U30" t="s">
         <v>437</v>
       </c>
-      <c r="P30" t="s">
+      <c r="V30" t="s">
         <v>268</v>
       </c>
-      <c r="Q30" t="s">
-        <v>237</v>
-      </c>
-      <c r="R30" t="s">
-        <v>237</v>
-      </c>
-      <c r="S30" t="s">
-        <v>237</v>
-      </c>
-      <c r="T30" t="s">
-        <v>237</v>
-      </c>
-      <c r="U30" t="s">
-        <v>237</v>
-      </c>
-      <c r="V30" t="s">
-        <v>237</v>
-      </c>
       <c r="W30" t="s">
         <v>237</v>
       </c>
@@ -4740,8 +4800,26 @@
       <c r="Z30" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="31" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="AA30" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI30" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ30" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK30" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL30" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM30" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="31" spans="1:39" ht="19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -4778,36 +4856,18 @@
       <c r="L31" t="s">
         <v>237</v>
       </c>
-      <c r="M31" s="10" t="s">
+      <c r="S31" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="N31" t="s">
+      <c r="T31" t="s">
         <v>296</v>
       </c>
-      <c r="O31" t="s">
+      <c r="U31" t="s">
         <v>438</v>
       </c>
-      <c r="P31" t="s">
+      <c r="V31" t="s">
         <v>263</v>
       </c>
-      <c r="Q31" t="s">
-        <v>237</v>
-      </c>
-      <c r="R31" t="s">
-        <v>237</v>
-      </c>
-      <c r="S31" t="s">
-        <v>237</v>
-      </c>
-      <c r="T31" t="s">
-        <v>237</v>
-      </c>
-      <c r="U31" t="s">
-        <v>237</v>
-      </c>
-      <c r="V31" t="s">
-        <v>237</v>
-      </c>
       <c r="W31" t="s">
         <v>237</v>
       </c>
@@ -4820,8 +4880,26 @@
       <c r="Z31" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="32" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="AA31" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI31" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ31" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK31" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL31" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM31" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="32" spans="1:39" ht="19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -4858,36 +4936,18 @@
       <c r="L32" t="s">
         <v>237</v>
       </c>
-      <c r="M32" s="10" t="s">
+      <c r="S32" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="N32" t="s">
+      <c r="T32" t="s">
         <v>296</v>
       </c>
-      <c r="O32" t="s">
+      <c r="U32" t="s">
         <v>439</v>
       </c>
-      <c r="P32" t="s">
+      <c r="V32" t="s">
         <v>264</v>
       </c>
-      <c r="Q32" t="s">
-        <v>237</v>
-      </c>
-      <c r="R32" t="s">
-        <v>237</v>
-      </c>
-      <c r="S32" t="s">
-        <v>237</v>
-      </c>
-      <c r="T32" t="s">
-        <v>237</v>
-      </c>
-      <c r="U32" t="s">
-        <v>237</v>
-      </c>
-      <c r="V32" t="s">
-        <v>237</v>
-      </c>
       <c r="W32" t="s">
         <v>237</v>
       </c>
@@ -4900,8 +4960,26 @@
       <c r="Z32" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="33" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="AA32" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI32" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ32" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK32" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL32" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM32" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="33" spans="1:39" ht="19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -4938,36 +5016,18 @@
       <c r="L33" t="s">
         <v>237</v>
       </c>
-      <c r="M33" s="10" t="s">
+      <c r="S33" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="N33" t="s">
+      <c r="T33" t="s">
         <v>296</v>
       </c>
-      <c r="O33" t="s">
+      <c r="U33" t="s">
         <v>440</v>
       </c>
-      <c r="P33" t="s">
+      <c r="V33" t="s">
         <v>265</v>
       </c>
-      <c r="Q33" t="s">
-        <v>237</v>
-      </c>
-      <c r="R33" t="s">
-        <v>237</v>
-      </c>
-      <c r="S33" t="s">
-        <v>237</v>
-      </c>
-      <c r="T33" t="s">
-        <v>237</v>
-      </c>
-      <c r="U33" t="s">
-        <v>237</v>
-      </c>
-      <c r="V33" t="s">
-        <v>237</v>
-      </c>
       <c r="W33" t="s">
         <v>237</v>
       </c>
@@ -4980,8 +5040,26 @@
       <c r="Z33" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="34" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="AA33" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI33" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ33" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK33" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL33" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM33" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="34" spans="1:39" ht="19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -5018,36 +5096,18 @@
       <c r="L34" t="s">
         <v>237</v>
       </c>
-      <c r="M34" s="10" t="s">
+      <c r="S34" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="N34" t="s">
+      <c r="T34" t="s">
         <v>296</v>
       </c>
-      <c r="O34" t="s">
+      <c r="U34" t="s">
         <v>441</v>
       </c>
-      <c r="P34" t="s">
+      <c r="V34" t="s">
         <v>266</v>
       </c>
-      <c r="Q34" t="s">
-        <v>237</v>
-      </c>
-      <c r="R34" t="s">
-        <v>237</v>
-      </c>
-      <c r="S34" t="s">
-        <v>237</v>
-      </c>
-      <c r="T34" t="s">
-        <v>237</v>
-      </c>
-      <c r="U34" t="s">
-        <v>237</v>
-      </c>
-      <c r="V34" t="s">
-        <v>237</v>
-      </c>
       <c r="W34" t="s">
         <v>237</v>
       </c>
@@ -5060,8 +5120,26 @@
       <c r="Z34" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="35" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="AA34" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI34" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ34" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK34" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL34" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM34" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="35" spans="1:39" ht="19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -5098,36 +5176,18 @@
       <c r="L35" t="s">
         <v>237</v>
       </c>
-      <c r="M35" s="10" t="s">
+      <c r="S35" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="N35" t="s">
+      <c r="T35" t="s">
         <v>296</v>
       </c>
-      <c r="O35" t="s">
+      <c r="U35" t="s">
         <v>442</v>
       </c>
-      <c r="P35" t="s">
+      <c r="V35" t="s">
         <v>267</v>
       </c>
-      <c r="Q35" t="s">
-        <v>237</v>
-      </c>
-      <c r="R35" t="s">
-        <v>237</v>
-      </c>
-      <c r="S35" t="s">
-        <v>237</v>
-      </c>
-      <c r="T35" t="s">
-        <v>237</v>
-      </c>
-      <c r="U35" t="s">
-        <v>237</v>
-      </c>
-      <c r="V35" t="s">
-        <v>237</v>
-      </c>
       <c r="W35" t="s">
         <v>237</v>
       </c>
@@ -5140,8 +5200,26 @@
       <c r="Z35" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="36" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="AA35" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI35" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ35" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK35" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL35" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM35" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="36" spans="1:39" ht="19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -5178,36 +5256,18 @@
       <c r="L36" t="s">
         <v>237</v>
       </c>
-      <c r="M36" s="10" t="s">
+      <c r="S36" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="N36" t="s">
+      <c r="T36" t="s">
         <v>296</v>
       </c>
-      <c r="O36" t="s">
+      <c r="U36" t="s">
         <v>443</v>
       </c>
-      <c r="P36" t="s">
+      <c r="V36" t="s">
         <v>262</v>
       </c>
-      <c r="Q36" t="s">
-        <v>237</v>
-      </c>
-      <c r="R36" t="s">
-        <v>237</v>
-      </c>
-      <c r="S36" t="s">
-        <v>237</v>
-      </c>
-      <c r="T36" t="s">
-        <v>237</v>
-      </c>
-      <c r="U36" t="s">
-        <v>237</v>
-      </c>
-      <c r="V36" t="s">
-        <v>237</v>
-      </c>
       <c r="W36" t="s">
         <v>237</v>
       </c>
@@ -5220,8 +5280,26 @@
       <c r="Z36" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="37" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="AA36" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI36" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ36" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK36" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL36" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM36" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="37" spans="1:39" ht="19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -5258,36 +5336,18 @@
       <c r="L37" t="s">
         <v>237</v>
       </c>
-      <c r="M37" s="10" t="s">
+      <c r="S37" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="N37" t="s">
+      <c r="T37" t="s">
         <v>296</v>
       </c>
-      <c r="O37" t="s">
+      <c r="U37" t="s">
         <v>444</v>
       </c>
-      <c r="P37" t="s">
+      <c r="V37" t="s">
         <v>269</v>
       </c>
-      <c r="Q37" t="s">
-        <v>237</v>
-      </c>
-      <c r="R37" t="s">
-        <v>237</v>
-      </c>
-      <c r="S37" t="s">
-        <v>237</v>
-      </c>
-      <c r="T37" t="s">
-        <v>237</v>
-      </c>
-      <c r="U37" t="s">
-        <v>237</v>
-      </c>
-      <c r="V37" t="s">
-        <v>237</v>
-      </c>
       <c r="W37" t="s">
         <v>237</v>
       </c>
@@ -5300,8 +5360,26 @@
       <c r="Z37" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="38" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="AA37" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI37" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ37" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK37" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL37" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM37" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="38" spans="1:39" ht="19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -5338,24 +5416,6 @@
       <c r="L38" t="s">
         <v>237</v>
       </c>
-      <c r="M38" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="N38" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="O38" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="P38" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q38" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="R38" s="1" t="s">
-        <v>237</v>
-      </c>
       <c r="S38" s="1" t="s">
         <v>237</v>
       </c>
@@ -5365,23 +5425,48 @@
       <c r="U38" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="V38" t="s">
-        <v>237</v>
-      </c>
-      <c r="W38" t="s">
-        <v>237</v>
-      </c>
-      <c r="X38" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y38" t="s">
+      <c r="V38" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="W38" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="X38" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="Y38" s="1" t="s">
         <v>237</v>
       </c>
       <c r="Z38" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="39" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="AA38" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB38" s="1"/>
+      <c r="AC38" s="1"/>
+      <c r="AD38" s="1"/>
+      <c r="AE38" s="1"/>
+      <c r="AF38" s="1"/>
+      <c r="AG38" s="1"/>
+      <c r="AH38" s="1"/>
+      <c r="AI38" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ38" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK38" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL38" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM38" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="39" spans="1:39" ht="19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -5418,24 +5503,6 @@
       <c r="L39" t="s">
         <v>237</v>
       </c>
-      <c r="M39" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="N39" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="O39" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="P39" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q39" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="R39" s="1" t="s">
-        <v>237</v>
-      </c>
       <c r="S39" s="1" t="s">
         <v>237</v>
       </c>
@@ -5445,23 +5512,48 @@
       <c r="U39" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="V39" t="s">
-        <v>237</v>
-      </c>
-      <c r="W39" t="s">
-        <v>237</v>
-      </c>
-      <c r="X39" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y39" t="s">
+      <c r="V39" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="W39" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="X39" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="Y39" s="1" t="s">
         <v>237</v>
       </c>
       <c r="Z39" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="40" spans="1:26" ht="18" x14ac:dyDescent="0.2">
+      <c r="AA39" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB39" s="1"/>
+      <c r="AC39" s="1"/>
+      <c r="AD39" s="1"/>
+      <c r="AE39" s="1"/>
+      <c r="AF39" s="1"/>
+      <c r="AG39" s="1"/>
+      <c r="AH39" s="1"/>
+      <c r="AI39" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ39" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK39" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL39" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM39" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="40" spans="1:39" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>35</v>
       </c>
@@ -5498,50 +5590,50 @@
       <c r="L40" t="s">
         <v>237</v>
       </c>
-      <c r="M40" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="N40" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="O40" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="P40" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q40" t="s">
+      <c r="S40" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="T40" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="U40" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="V40" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="W40" t="s">
         <v>303</v>
       </c>
-      <c r="R40" t="s">
+      <c r="X40" t="s">
         <v>302</v>
       </c>
-      <c r="S40" s="1" t="s">
+      <c r="Y40" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="T40" s="9" t="s">
+      <c r="Z40" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="U40" t="s">
+      <c r="AA40" t="s">
         <v>241</v>
       </c>
-      <c r="V40" t="s">
-        <v>237</v>
-      </c>
-      <c r="W40" t="s">
-        <v>237</v>
-      </c>
-      <c r="X40" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y40" t="s">
-        <v>237</v>
-      </c>
-      <c r="Z40" t="s">
+      <c r="AI40" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ40" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK40" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL40" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM40" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="41" spans="1:26" ht="18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:39" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>82</v>
       </c>
@@ -5578,24 +5670,6 @@
       <c r="L41" t="s">
         <v>237</v>
       </c>
-      <c r="M41" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="N41" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="O41" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="P41" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q41" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="R41" s="1" t="s">
-        <v>237</v>
-      </c>
       <c r="S41" s="1" t="s">
         <v>237</v>
       </c>
@@ -5605,23 +5679,48 @@
       <c r="U41" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="V41" t="s">
-        <v>237</v>
-      </c>
-      <c r="W41" t="s">
-        <v>237</v>
-      </c>
-      <c r="X41" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y41" t="s">
+      <c r="V41" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="W41" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="X41" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="Y41" s="1" t="s">
         <v>237</v>
       </c>
       <c r="Z41" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="42" spans="1:26" ht="18" x14ac:dyDescent="0.2">
+      <c r="AA41" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB41" s="1"/>
+      <c r="AC41" s="1"/>
+      <c r="AD41" s="1"/>
+      <c r="AE41" s="1"/>
+      <c r="AF41" s="1"/>
+      <c r="AG41" s="1"/>
+      <c r="AH41" s="1"/>
+      <c r="AI41" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ41" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK41" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL41" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM41" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="42" spans="1:39" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>82</v>
       </c>
@@ -5658,24 +5757,6 @@
       <c r="L42" t="s">
         <v>237</v>
       </c>
-      <c r="M42" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="N42" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="O42" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="P42" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q42" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="R42" s="1" t="s">
-        <v>237</v>
-      </c>
       <c r="S42" s="1" t="s">
         <v>237</v>
       </c>
@@ -5685,23 +5766,48 @@
       <c r="U42" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="V42" t="s">
-        <v>237</v>
-      </c>
-      <c r="W42" t="s">
-        <v>237</v>
-      </c>
-      <c r="X42" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y42" t="s">
+      <c r="V42" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="W42" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="X42" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="Y42" s="1" t="s">
         <v>237</v>
       </c>
       <c r="Z42" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="43" spans="1:26" ht="18" x14ac:dyDescent="0.2">
+      <c r="AA42" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB42" s="1"/>
+      <c r="AC42" s="1"/>
+      <c r="AD42" s="1"/>
+      <c r="AE42" s="1"/>
+      <c r="AF42" s="1"/>
+      <c r="AG42" s="1"/>
+      <c r="AH42" s="1"/>
+      <c r="AI42" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ42" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK42" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL42" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM42" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="43" spans="1:39" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>87</v>
       </c>
@@ -5738,24 +5844,6 @@
       <c r="L43" t="s">
         <v>237</v>
       </c>
-      <c r="M43" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="N43" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="O43" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="P43" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q43" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="R43" s="1" t="s">
-        <v>237</v>
-      </c>
       <c r="S43" s="1" t="s">
         <v>237</v>
       </c>
@@ -5765,23 +5853,48 @@
       <c r="U43" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="V43" t="s">
-        <v>237</v>
-      </c>
-      <c r="W43" t="s">
-        <v>237</v>
-      </c>
-      <c r="X43" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y43" t="s">
+      <c r="V43" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="W43" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="X43" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="Y43" s="1" t="s">
         <v>237</v>
       </c>
       <c r="Z43" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="44" spans="1:26" ht="18" x14ac:dyDescent="0.2">
+      <c r="AA43" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB43" s="1"/>
+      <c r="AC43" s="1"/>
+      <c r="AD43" s="1"/>
+      <c r="AE43" s="1"/>
+      <c r="AF43" s="1"/>
+      <c r="AG43" s="1"/>
+      <c r="AH43" s="1"/>
+      <c r="AI43" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ43" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK43" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL43" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM43" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="44" spans="1:39" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>87</v>
       </c>
@@ -5818,50 +5931,50 @@
       <c r="L44" t="s">
         <v>237</v>
       </c>
-      <c r="M44" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="N44" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="O44" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="P44" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q44" t="s">
+      <c r="S44" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="T44" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="U44" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="V44" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="W44" t="s">
         <v>304</v>
       </c>
-      <c r="R44" t="s">
+      <c r="X44" t="s">
         <v>305</v>
       </c>
-      <c r="S44" s="1" t="s">
+      <c r="Y44" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="T44" t="s">
+      <c r="Z44" t="s">
         <v>401</v>
       </c>
-      <c r="U44" t="s">
+      <c r="AA44" t="s">
         <v>251</v>
       </c>
-      <c r="V44" t="s">
-        <v>237</v>
-      </c>
-      <c r="W44" t="s">
-        <v>237</v>
-      </c>
-      <c r="X44" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y44" t="s">
-        <v>237</v>
-      </c>
-      <c r="Z44" t="s">
+      <c r="AI44" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ44" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK44" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL44" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM44" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="45" spans="1:26" ht="18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:39" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>91</v>
       </c>
@@ -5898,24 +6011,6 @@
       <c r="L45" t="s">
         <v>237</v>
       </c>
-      <c r="M45" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="N45" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="O45" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="P45" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q45" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="R45" s="1" t="s">
-        <v>237</v>
-      </c>
       <c r="S45" s="1" t="s">
         <v>237</v>
       </c>
@@ -5925,23 +6020,48 @@
       <c r="U45" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="V45" t="s">
-        <v>237</v>
-      </c>
-      <c r="W45" t="s">
-        <v>237</v>
-      </c>
-      <c r="X45" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y45" t="s">
+      <c r="V45" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="W45" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="X45" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="Y45" s="1" t="s">
         <v>237</v>
       </c>
       <c r="Z45" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="46" spans="1:26" ht="18" x14ac:dyDescent="0.2">
+      <c r="AA45" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB45" s="1"/>
+      <c r="AC45" s="1"/>
+      <c r="AD45" s="1"/>
+      <c r="AE45" s="1"/>
+      <c r="AF45" s="1"/>
+      <c r="AG45" s="1"/>
+      <c r="AH45" s="1"/>
+      <c r="AI45" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ45" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK45" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL45" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM45" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="46" spans="1:39" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>91</v>
       </c>
@@ -5978,50 +6098,57 @@
       <c r="L46" t="s">
         <v>320</v>
       </c>
-      <c r="M46" s="1" t="s">
+      <c r="S46" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="N46" s="1" t="s">
+      <c r="T46" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="O46" t="s">
+      <c r="U46" t="s">
         <v>324</v>
       </c>
-      <c r="P46" t="s">
+      <c r="V46" t="s">
         <v>323</v>
       </c>
-      <c r="Q46" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="R46" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="S46" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="T46" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="U46" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="V46" t="s">
-        <v>237</v>
-      </c>
-      <c r="W46" t="s">
-        <v>237</v>
-      </c>
-      <c r="X46" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y46" t="s">
+      <c r="W46" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="X46" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="Y46" s="1" t="s">
         <v>237</v>
       </c>
       <c r="Z46" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="47" spans="1:26" ht="18" x14ac:dyDescent="0.2">
+      <c r="AA46" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB46" s="1"/>
+      <c r="AC46" s="1"/>
+      <c r="AD46" s="1"/>
+      <c r="AE46" s="1"/>
+      <c r="AF46" s="1"/>
+      <c r="AG46" s="1"/>
+      <c r="AH46" s="1"/>
+      <c r="AI46" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ46" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK46" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL46" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM46" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="47" spans="1:39" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
         <v>91</v>
       </c>
@@ -6058,50 +6185,57 @@
       <c r="L47" t="s">
         <v>320</v>
       </c>
-      <c r="M47" s="1" t="s">
+      <c r="S47" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="N47" s="1" t="s">
+      <c r="T47" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="O47" t="s">
+      <c r="U47" t="s">
         <v>326</v>
       </c>
-      <c r="P47" t="s">
+      <c r="V47" t="s">
         <v>325</v>
       </c>
-      <c r="Q47" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="R47" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="S47" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="T47" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="U47" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="V47" t="s">
-        <v>237</v>
-      </c>
-      <c r="W47" t="s">
-        <v>237</v>
-      </c>
-      <c r="X47" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y47" t="s">
+      <c r="W47" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="X47" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="Y47" s="1" t="s">
         <v>237</v>
       </c>
       <c r="Z47" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="48" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="AA47" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB47" s="1"/>
+      <c r="AC47" s="1"/>
+      <c r="AD47" s="1"/>
+      <c r="AE47" s="1"/>
+      <c r="AF47" s="1"/>
+      <c r="AG47" s="1"/>
+      <c r="AH47" s="1"/>
+      <c r="AI47" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ47" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK47" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL47" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM47" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="48" spans="1:39" ht="19" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>91</v>
       </c>
@@ -6138,24 +6272,6 @@
       <c r="L48" t="s">
         <v>320</v>
       </c>
-      <c r="M48" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="N48" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="O48" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="P48" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q48" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="R48" s="1" t="s">
-        <v>237</v>
-      </c>
       <c r="S48" s="1" t="s">
         <v>237</v>
       </c>
@@ -6165,23 +6281,48 @@
       <c r="U48" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="V48" t="s">
-        <v>237</v>
-      </c>
-      <c r="W48" t="s">
-        <v>237</v>
-      </c>
-      <c r="X48" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y48" t="s">
+      <c r="V48" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="W48" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="X48" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="Y48" s="1" t="s">
         <v>237</v>
       </c>
       <c r="Z48" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="49" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="AA48" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB48" s="1"/>
+      <c r="AC48" s="1"/>
+      <c r="AD48" s="1"/>
+      <c r="AE48" s="1"/>
+      <c r="AF48" s="1"/>
+      <c r="AG48" s="1"/>
+      <c r="AH48" s="1"/>
+      <c r="AI48" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ48" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK48" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL48" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM48" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="49" spans="1:39" ht="19" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>91</v>
       </c>
@@ -6218,24 +6359,6 @@
       <c r="L49" t="s">
         <v>320</v>
       </c>
-      <c r="M49" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="N49" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="O49" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="P49" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q49" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="R49" s="1" t="s">
-        <v>237</v>
-      </c>
       <c r="S49" s="1" t="s">
         <v>237</v>
       </c>
@@ -6245,23 +6368,48 @@
       <c r="U49" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="V49" t="s">
-        <v>237</v>
-      </c>
-      <c r="W49" t="s">
-        <v>237</v>
-      </c>
-      <c r="X49" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y49" t="s">
+      <c r="V49" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="W49" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="X49" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="Y49" s="1" t="s">
         <v>237</v>
       </c>
       <c r="Z49" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="50" spans="1:26" ht="18" x14ac:dyDescent="0.2">
+      <c r="AA49" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB49" s="1"/>
+      <c r="AC49" s="1"/>
+      <c r="AD49" s="1"/>
+      <c r="AE49" s="1"/>
+      <c r="AF49" s="1"/>
+      <c r="AG49" s="1"/>
+      <c r="AH49" s="1"/>
+      <c r="AI49" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ49" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK49" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL49" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM49" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="50" spans="1:39" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>91</v>
       </c>
@@ -6298,24 +6446,6 @@
       <c r="L50" t="s">
         <v>320</v>
       </c>
-      <c r="M50" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="N50" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="O50" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="P50" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q50" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="R50" s="1" t="s">
-        <v>237</v>
-      </c>
       <c r="S50" s="1" t="s">
         <v>237</v>
       </c>
@@ -6325,23 +6455,48 @@
       <c r="U50" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="V50" t="s">
-        <v>237</v>
-      </c>
-      <c r="W50" t="s">
-        <v>237</v>
-      </c>
-      <c r="X50" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y50" t="s">
+      <c r="V50" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="W50" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="X50" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="Y50" s="1" t="s">
         <v>237</v>
       </c>
       <c r="Z50" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="51" spans="1:26" ht="18" x14ac:dyDescent="0.2">
+      <c r="AA50" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB50" s="1"/>
+      <c r="AC50" s="1"/>
+      <c r="AD50" s="1"/>
+      <c r="AE50" s="1"/>
+      <c r="AF50" s="1"/>
+      <c r="AG50" s="1"/>
+      <c r="AH50" s="1"/>
+      <c r="AI50" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ50" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK50" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL50" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM50" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="51" spans="1:39" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>108</v>
       </c>
@@ -6378,24 +6533,6 @@
       <c r="L51" t="s">
         <v>237</v>
       </c>
-      <c r="M51" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="N51" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="O51" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="P51" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q51" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="R51" s="1" t="s">
-        <v>237</v>
-      </c>
       <c r="S51" s="1" t="s">
         <v>237</v>
       </c>
@@ -6405,23 +6542,48 @@
       <c r="U51" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="V51" t="s">
-        <v>237</v>
-      </c>
-      <c r="W51" t="s">
-        <v>237</v>
-      </c>
-      <c r="X51" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y51" t="s">
+      <c r="V51" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="W51" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="X51" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="Y51" s="1" t="s">
         <v>237</v>
       </c>
       <c r="Z51" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="52" spans="1:26" ht="18" x14ac:dyDescent="0.2">
+      <c r="AA51" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB51" s="1"/>
+      <c r="AC51" s="1"/>
+      <c r="AD51" s="1"/>
+      <c r="AE51" s="1"/>
+      <c r="AF51" s="1"/>
+      <c r="AG51" s="1"/>
+      <c r="AH51" s="1"/>
+      <c r="AI51" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ51" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK51" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL51" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM51" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="52" spans="1:39" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>108</v>
       </c>
@@ -6458,50 +6620,50 @@
       <c r="L52" t="s">
         <v>237</v>
       </c>
-      <c r="M52" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="N52" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="O52" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="P52" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q52" t="s">
+      <c r="S52" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="T52" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="U52" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="V52" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="W52" t="s">
         <v>306</v>
       </c>
-      <c r="R52" t="s">
+      <c r="X52" t="s">
         <v>307</v>
       </c>
-      <c r="S52" s="1" t="s">
+      <c r="Y52" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="T52" s="9" t="s">
+      <c r="Z52" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="U52" t="s">
+      <c r="AA52" t="s">
         <v>241</v>
       </c>
-      <c r="V52" t="s">
-        <v>237</v>
-      </c>
-      <c r="W52" t="s">
-        <v>237</v>
-      </c>
-      <c r="X52" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y52" t="s">
-        <v>237</v>
-      </c>
-      <c r="Z52" t="s">
+      <c r="AI52" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ52" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK52" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL52" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM52" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="53" spans="1:26" ht="18" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:39" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>112</v>
       </c>
@@ -6538,24 +6700,6 @@
       <c r="L53" t="s">
         <v>237</v>
       </c>
-      <c r="M53" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="N53" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="O53" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="P53" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q53" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="R53" s="1" t="s">
-        <v>237</v>
-      </c>
       <c r="S53" s="1" t="s">
         <v>237</v>
       </c>
@@ -6565,23 +6709,48 @@
       <c r="U53" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="V53" t="s">
-        <v>237</v>
-      </c>
-      <c r="W53" t="s">
-        <v>237</v>
-      </c>
-      <c r="X53" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y53" t="s">
+      <c r="V53" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="W53" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="X53" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="Y53" s="1" t="s">
         <v>237</v>
       </c>
       <c r="Z53" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="54" spans="1:26" ht="18" x14ac:dyDescent="0.2">
+      <c r="AA53" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB53" s="1"/>
+      <c r="AC53" s="1"/>
+      <c r="AD53" s="1"/>
+      <c r="AE53" s="1"/>
+      <c r="AF53" s="1"/>
+      <c r="AG53" s="1"/>
+      <c r="AH53" s="1"/>
+      <c r="AI53" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ53" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK53" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL53" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM53" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="54" spans="1:39" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>115</v>
       </c>
@@ -6618,24 +6787,6 @@
       <c r="L54" t="s">
         <v>237</v>
       </c>
-      <c r="M54" t="s">
-        <v>237</v>
-      </c>
-      <c r="N54" t="s">
-        <v>237</v>
-      </c>
-      <c r="O54" t="s">
-        <v>237</v>
-      </c>
-      <c r="P54" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q54" t="s">
-        <v>237</v>
-      </c>
-      <c r="R54" t="s">
-        <v>237</v>
-      </c>
       <c r="S54" t="s">
         <v>237</v>
       </c>
@@ -6660,8 +6811,26 @@
       <c r="Z54" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA54" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI54" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ54" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK54" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL54" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM54" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="55" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>115</v>
       </c>
@@ -6698,24 +6867,6 @@
       <c r="L55" t="s">
         <v>237</v>
       </c>
-      <c r="M55" t="s">
-        <v>237</v>
-      </c>
-      <c r="N55" t="s">
-        <v>237</v>
-      </c>
-      <c r="O55" t="s">
-        <v>237</v>
-      </c>
-      <c r="P55" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q55" t="s">
-        <v>237</v>
-      </c>
-      <c r="R55" t="s">
-        <v>237</v>
-      </c>
       <c r="S55" t="s">
         <v>237</v>
       </c>
@@ -6740,8 +6891,26 @@
       <c r="Z55" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="56" spans="1:26" ht="18" x14ac:dyDescent="0.2">
+      <c r="AA55" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI55" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ55" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK55" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL55" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM55" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="56" spans="1:39" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>115</v>
       </c>
@@ -6778,51 +6947,50 @@
       <c r="L56" t="s">
         <v>237</v>
       </c>
-      <c r="M56" t="s">
-        <v>237</v>
-      </c>
-      <c r="N56" t="s">
-        <v>237</v>
-      </c>
-      <c r="O56" t="s">
-        <v>237</v>
-      </c>
-      <c r="P56" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q56" s="1" t="s">
+      <c r="S56" t="s">
+        <v>237</v>
+      </c>
+      <c r="T56" t="s">
+        <v>237</v>
+      </c>
+      <c r="U56" t="s">
+        <v>237</v>
+      </c>
+      <c r="V56" t="s">
+        <v>237</v>
+      </c>
+      <c r="W56" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="R56" s="1" t="s">
+      <c r="X56" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="S56" s="1" t="s">
+      <c r="Y56" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="T56" t="s">
-        <v>237</v>
-      </c>
-      <c r="U56" t="s">
-        <v>237</v>
-      </c>
-      <c r="V56" t="s">
-        <v>237</v>
-      </c>
-      <c r="W56" t="s">
-        <v>237</v>
-      </c>
-      <c r="X56" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y56" t="s">
-        <v>237</v>
-      </c>
       <c r="Z56" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA56" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI56" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ56" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK56" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL56" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM56" t="s">
         <v>248</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z56" xr:uid="{DF301E54-0E7B-1E4E-9373-0F8968A635A9}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
data_required.csv add NA to new columns
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2093BA-581F-1F4F-827F-B2EDA3E64FA6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7BEB47-36FB-4B41-AC3B-ECC62B84E8A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2702" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3417" uniqueCount="642">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -2539,6 +2539,24 @@
       <c r="L2" t="s">
         <v>237</v>
       </c>
+      <c r="M2" t="s">
+        <v>237</v>
+      </c>
+      <c r="N2" t="s">
+        <v>237</v>
+      </c>
+      <c r="O2" t="s">
+        <v>237</v>
+      </c>
+      <c r="P2" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>237</v>
+      </c>
+      <c r="R2" t="s">
+        <v>237</v>
+      </c>
       <c r="S2" t="s">
         <v>237</v>
       </c>
@@ -2564,6 +2582,27 @@
         <v>237</v>
       </c>
       <c r="AA2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH2" t="s">
         <v>237</v>
       </c>
       <c r="AI2" t="s">
@@ -2619,6 +2658,24 @@
       <c r="L3" t="s">
         <v>237</v>
       </c>
+      <c r="M3" t="s">
+        <v>237</v>
+      </c>
+      <c r="N3" t="s">
+        <v>237</v>
+      </c>
+      <c r="O3" t="s">
+        <v>237</v>
+      </c>
+      <c r="P3" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>237</v>
+      </c>
+      <c r="R3" t="s">
+        <v>237</v>
+      </c>
       <c r="S3" t="s">
         <v>237</v>
       </c>
@@ -2644,6 +2701,27 @@
         <v>237</v>
       </c>
       <c r="AA3" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH3" t="s">
         <v>237</v>
       </c>
       <c r="AI3" t="s">
@@ -2699,6 +2777,24 @@
       <c r="L4" t="s">
         <v>237</v>
       </c>
+      <c r="M4" t="s">
+        <v>237</v>
+      </c>
+      <c r="N4" t="s">
+        <v>237</v>
+      </c>
+      <c r="O4" t="s">
+        <v>237</v>
+      </c>
+      <c r="P4" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>237</v>
+      </c>
+      <c r="R4" t="s">
+        <v>237</v>
+      </c>
       <c r="S4" t="s">
         <v>237</v>
       </c>
@@ -2724,6 +2820,27 @@
         <v>237</v>
       </c>
       <c r="AA4" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH4" t="s">
         <v>237</v>
       </c>
       <c r="AI4" t="s">
@@ -2779,6 +2896,24 @@
       <c r="L5" t="s">
         <v>237</v>
       </c>
+      <c r="M5" t="s">
+        <v>237</v>
+      </c>
+      <c r="N5" t="s">
+        <v>237</v>
+      </c>
+      <c r="O5" t="s">
+        <v>237</v>
+      </c>
+      <c r="P5" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>237</v>
+      </c>
+      <c r="R5" t="s">
+        <v>237</v>
+      </c>
       <c r="S5" t="s">
         <v>237</v>
       </c>
@@ -2804,6 +2939,27 @@
         <v>237</v>
       </c>
       <c r="AA5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH5" t="s">
         <v>237</v>
       </c>
       <c r="AI5" t="s">
@@ -2859,6 +3015,24 @@
       <c r="L6" t="s">
         <v>237</v>
       </c>
+      <c r="M6" t="s">
+        <v>237</v>
+      </c>
+      <c r="N6" t="s">
+        <v>237</v>
+      </c>
+      <c r="O6" t="s">
+        <v>237</v>
+      </c>
+      <c r="P6" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>237</v>
+      </c>
+      <c r="R6" t="s">
+        <v>237</v>
+      </c>
       <c r="S6" t="s">
         <v>237</v>
       </c>
@@ -2884,6 +3058,27 @@
         <v>237</v>
       </c>
       <c r="AA6" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH6" t="s">
         <v>237</v>
       </c>
       <c r="AI6" t="s">
@@ -2939,6 +3134,24 @@
       <c r="L7" t="s">
         <v>237</v>
       </c>
+      <c r="M7" t="s">
+        <v>237</v>
+      </c>
+      <c r="N7" t="s">
+        <v>237</v>
+      </c>
+      <c r="O7" t="s">
+        <v>237</v>
+      </c>
+      <c r="P7" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>237</v>
+      </c>
+      <c r="R7" t="s">
+        <v>237</v>
+      </c>
       <c r="S7" t="s">
         <v>237</v>
       </c>
@@ -2964,6 +3177,27 @@
         <v>237</v>
       </c>
       <c r="AA7" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH7" t="s">
         <v>237</v>
       </c>
       <c r="AI7" t="s">
@@ -3019,6 +3253,24 @@
       <c r="L8" t="s">
         <v>237</v>
       </c>
+      <c r="M8" t="s">
+        <v>237</v>
+      </c>
+      <c r="N8" t="s">
+        <v>237</v>
+      </c>
+      <c r="O8" t="s">
+        <v>237</v>
+      </c>
+      <c r="P8" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>237</v>
+      </c>
+      <c r="R8" t="s">
+        <v>237</v>
+      </c>
       <c r="S8" t="s">
         <v>237</v>
       </c>
@@ -3045,6 +3297,27 @@
       </c>
       <c r="AA8" t="s">
         <v>241</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>237</v>
       </c>
       <c r="AI8" t="s">
         <v>237</v>
@@ -3099,6 +3372,24 @@
       <c r="L9" t="s">
         <v>237</v>
       </c>
+      <c r="M9" t="s">
+        <v>237</v>
+      </c>
+      <c r="N9" t="s">
+        <v>237</v>
+      </c>
+      <c r="O9" t="s">
+        <v>237</v>
+      </c>
+      <c r="P9" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>237</v>
+      </c>
+      <c r="R9" t="s">
+        <v>237</v>
+      </c>
       <c r="S9" t="s">
         <v>237</v>
       </c>
@@ -3124,6 +3415,27 @@
         <v>237</v>
       </c>
       <c r="AA9" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH9" t="s">
         <v>237</v>
       </c>
       <c r="AI9" t="s">
@@ -3179,6 +3491,24 @@
       <c r="L10" t="s">
         <v>237</v>
       </c>
+      <c r="M10" t="s">
+        <v>237</v>
+      </c>
+      <c r="N10" t="s">
+        <v>237</v>
+      </c>
+      <c r="O10" t="s">
+        <v>237</v>
+      </c>
+      <c r="P10" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>237</v>
+      </c>
+      <c r="R10" t="s">
+        <v>237</v>
+      </c>
       <c r="S10" t="s">
         <v>237</v>
       </c>
@@ -3204,6 +3534,27 @@
         <v>237</v>
       </c>
       <c r="AA10" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH10" t="s">
         <v>237</v>
       </c>
       <c r="AI10" t="s">
@@ -3259,6 +3610,24 @@
       <c r="L11" t="s">
         <v>237</v>
       </c>
+      <c r="M11" t="s">
+        <v>237</v>
+      </c>
+      <c r="N11" t="s">
+        <v>237</v>
+      </c>
+      <c r="O11" t="s">
+        <v>237</v>
+      </c>
+      <c r="P11" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>237</v>
+      </c>
+      <c r="R11" t="s">
+        <v>237</v>
+      </c>
       <c r="S11" t="s">
         <v>237</v>
       </c>
@@ -3284,6 +3653,27 @@
         <v>237</v>
       </c>
       <c r="AA11" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH11" t="s">
         <v>237</v>
       </c>
       <c r="AI11" t="s">
@@ -3339,6 +3729,24 @@
       <c r="L12" t="s">
         <v>237</v>
       </c>
+      <c r="M12" t="s">
+        <v>237</v>
+      </c>
+      <c r="N12" t="s">
+        <v>237</v>
+      </c>
+      <c r="O12" t="s">
+        <v>237</v>
+      </c>
+      <c r="P12" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>237</v>
+      </c>
+      <c r="R12" t="s">
+        <v>237</v>
+      </c>
       <c r="S12" t="s">
         <v>237</v>
       </c>
@@ -3364,6 +3772,27 @@
         <v>237</v>
       </c>
       <c r="AA12" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH12" t="s">
         <v>237</v>
       </c>
       <c r="AI12" t="s">
@@ -3419,6 +3848,24 @@
       <c r="L13" t="s">
         <v>237</v>
       </c>
+      <c r="M13" t="s">
+        <v>237</v>
+      </c>
+      <c r="N13" t="s">
+        <v>237</v>
+      </c>
+      <c r="O13" t="s">
+        <v>237</v>
+      </c>
+      <c r="P13" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>237</v>
+      </c>
+      <c r="R13" t="s">
+        <v>237</v>
+      </c>
       <c r="S13" t="s">
         <v>237</v>
       </c>
@@ -3444,6 +3891,27 @@
         <v>237</v>
       </c>
       <c r="AA13" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH13" t="s">
         <v>237</v>
       </c>
       <c r="AI13" t="s">
@@ -3499,6 +3967,24 @@
       <c r="L14" t="s">
         <v>237</v>
       </c>
+      <c r="M14" t="s">
+        <v>237</v>
+      </c>
+      <c r="N14" t="s">
+        <v>237</v>
+      </c>
+      <c r="O14" t="s">
+        <v>237</v>
+      </c>
+      <c r="P14" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>237</v>
+      </c>
+      <c r="R14" t="s">
+        <v>237</v>
+      </c>
       <c r="S14" t="s">
         <v>237</v>
       </c>
@@ -3524,6 +4010,27 @@
         <v>237</v>
       </c>
       <c r="AA14" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH14" t="s">
         <v>237</v>
       </c>
       <c r="AI14" t="s">
@@ -3579,6 +4086,24 @@
       <c r="L15" t="s">
         <v>237</v>
       </c>
+      <c r="M15" t="s">
+        <v>237</v>
+      </c>
+      <c r="N15" t="s">
+        <v>237</v>
+      </c>
+      <c r="O15" t="s">
+        <v>237</v>
+      </c>
+      <c r="P15" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>237</v>
+      </c>
+      <c r="R15" t="s">
+        <v>237</v>
+      </c>
       <c r="S15" s="10" t="s">
         <v>406</v>
       </c>
@@ -3604,6 +4129,27 @@
         <v>237</v>
       </c>
       <c r="AA15" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH15" t="s">
         <v>237</v>
       </c>
       <c r="AI15" t="s">
@@ -3659,6 +4205,24 @@
       <c r="L16" t="s">
         <v>237</v>
       </c>
+      <c r="M16" t="s">
+        <v>237</v>
+      </c>
+      <c r="N16" t="s">
+        <v>237</v>
+      </c>
+      <c r="O16" t="s">
+        <v>237</v>
+      </c>
+      <c r="P16" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>237</v>
+      </c>
+      <c r="R16" t="s">
+        <v>237</v>
+      </c>
       <c r="S16" s="10" t="s">
         <v>406</v>
       </c>
@@ -3684,6 +4248,27 @@
         <v>237</v>
       </c>
       <c r="AA16" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH16" t="s">
         <v>237</v>
       </c>
       <c r="AI16" t="s">
@@ -3736,6 +4321,24 @@
       <c r="L17" t="s">
         <v>237</v>
       </c>
+      <c r="M17" t="s">
+        <v>237</v>
+      </c>
+      <c r="N17" t="s">
+        <v>237</v>
+      </c>
+      <c r="O17" t="s">
+        <v>237</v>
+      </c>
+      <c r="P17" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>237</v>
+      </c>
+      <c r="R17" t="s">
+        <v>237</v>
+      </c>
       <c r="S17" s="10" t="s">
         <v>406</v>
       </c>
@@ -3762,6 +4365,27 @@
       </c>
       <c r="AA17" t="s">
         <v>251</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>237</v>
       </c>
       <c r="AI17" s="10" t="s">
         <v>406</v>
@@ -3816,6 +4440,24 @@
       <c r="L18" t="s">
         <v>237</v>
       </c>
+      <c r="M18" t="s">
+        <v>237</v>
+      </c>
+      <c r="N18" t="s">
+        <v>237</v>
+      </c>
+      <c r="O18" t="s">
+        <v>237</v>
+      </c>
+      <c r="P18" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>237</v>
+      </c>
+      <c r="R18" t="s">
+        <v>237</v>
+      </c>
       <c r="S18" s="10" t="s">
         <v>406</v>
       </c>
@@ -3842,6 +4484,27 @@
       </c>
       <c r="AA18" t="s">
         <v>251</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>237</v>
       </c>
       <c r="AI18" t="s">
         <v>237</v>
@@ -3896,6 +4559,24 @@
       <c r="L19" t="s">
         <v>237</v>
       </c>
+      <c r="M19" t="s">
+        <v>237</v>
+      </c>
+      <c r="N19" t="s">
+        <v>237</v>
+      </c>
+      <c r="O19" t="s">
+        <v>237</v>
+      </c>
+      <c r="P19" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>237</v>
+      </c>
+      <c r="R19" t="s">
+        <v>237</v>
+      </c>
       <c r="S19" s="10" t="s">
         <v>406</v>
       </c>
@@ -3922,6 +4603,27 @@
       </c>
       <c r="AA19" t="s">
         <v>251</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>237</v>
       </c>
       <c r="AI19" t="s">
         <v>237</v>
@@ -3976,6 +4678,24 @@
       <c r="L20" t="s">
         <v>237</v>
       </c>
+      <c r="M20" t="s">
+        <v>237</v>
+      </c>
+      <c r="N20" t="s">
+        <v>237</v>
+      </c>
+      <c r="O20" t="s">
+        <v>237</v>
+      </c>
+      <c r="P20" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>237</v>
+      </c>
+      <c r="R20" t="s">
+        <v>237</v>
+      </c>
       <c r="S20" s="10" t="s">
         <v>406</v>
       </c>
@@ -4002,6 +4722,27 @@
       </c>
       <c r="AA20" t="s">
         <v>251</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>237</v>
       </c>
       <c r="AI20" t="s">
         <v>237</v>
@@ -4056,6 +4797,24 @@
       <c r="L21" t="s">
         <v>237</v>
       </c>
+      <c r="M21" t="s">
+        <v>237</v>
+      </c>
+      <c r="N21" t="s">
+        <v>237</v>
+      </c>
+      <c r="O21" t="s">
+        <v>237</v>
+      </c>
+      <c r="P21" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>237</v>
+      </c>
+      <c r="R21" t="s">
+        <v>237</v>
+      </c>
       <c r="S21" s="10" t="s">
         <v>406</v>
       </c>
@@ -4082,6 +4841,27 @@
       </c>
       <c r="AA21" t="s">
         <v>251</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>237</v>
       </c>
       <c r="AI21" t="s">
         <v>237</v>
@@ -4136,6 +4916,24 @@
       <c r="L22" t="s">
         <v>237</v>
       </c>
+      <c r="M22" t="s">
+        <v>237</v>
+      </c>
+      <c r="N22" t="s">
+        <v>237</v>
+      </c>
+      <c r="O22" t="s">
+        <v>237</v>
+      </c>
+      <c r="P22" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>237</v>
+      </c>
+      <c r="R22" t="s">
+        <v>237</v>
+      </c>
       <c r="S22" s="10" t="s">
         <v>406</v>
       </c>
@@ -4162,6 +4960,27 @@
       </c>
       <c r="AA22" t="s">
         <v>251</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>237</v>
       </c>
       <c r="AI22" t="s">
         <v>237</v>
@@ -4216,6 +5035,24 @@
       <c r="L23" t="s">
         <v>237</v>
       </c>
+      <c r="M23" t="s">
+        <v>237</v>
+      </c>
+      <c r="N23" t="s">
+        <v>237</v>
+      </c>
+      <c r="O23" t="s">
+        <v>237</v>
+      </c>
+      <c r="P23" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>237</v>
+      </c>
+      <c r="R23" t="s">
+        <v>237</v>
+      </c>
       <c r="S23" s="10" t="s">
         <v>406</v>
       </c>
@@ -4242,6 +5079,27 @@
       </c>
       <c r="AA23" t="s">
         <v>251</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG23" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH23" t="s">
+        <v>237</v>
       </c>
       <c r="AI23" t="s">
         <v>237</v>
@@ -4296,6 +5154,24 @@
       <c r="L24" t="s">
         <v>237</v>
       </c>
+      <c r="M24" t="s">
+        <v>237</v>
+      </c>
+      <c r="N24" t="s">
+        <v>237</v>
+      </c>
+      <c r="O24" t="s">
+        <v>237</v>
+      </c>
+      <c r="P24" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>237</v>
+      </c>
+      <c r="R24" t="s">
+        <v>237</v>
+      </c>
       <c r="S24" s="10" t="s">
         <v>406</v>
       </c>
@@ -4322,6 +5198,27 @@
       </c>
       <c r="AA24" t="s">
         <v>251</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF24" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG24" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH24" t="s">
+        <v>237</v>
       </c>
       <c r="AI24" t="s">
         <v>237</v>
@@ -4376,6 +5273,24 @@
       <c r="L25" t="s">
         <v>237</v>
       </c>
+      <c r="M25" t="s">
+        <v>237</v>
+      </c>
+      <c r="N25" t="s">
+        <v>237</v>
+      </c>
+      <c r="O25" t="s">
+        <v>237</v>
+      </c>
+      <c r="P25" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>237</v>
+      </c>
+      <c r="R25" t="s">
+        <v>237</v>
+      </c>
       <c r="S25" s="10" t="s">
         <v>406</v>
       </c>
@@ -4402,6 +5317,27 @@
       </c>
       <c r="AA25" t="s">
         <v>251</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF25" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG25" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH25" t="s">
+        <v>237</v>
       </c>
       <c r="AI25" t="s">
         <v>237</v>
@@ -4456,6 +5392,24 @@
       <c r="L26" t="s">
         <v>237</v>
       </c>
+      <c r="M26" t="s">
+        <v>237</v>
+      </c>
+      <c r="N26" t="s">
+        <v>237</v>
+      </c>
+      <c r="O26" t="s">
+        <v>237</v>
+      </c>
+      <c r="P26" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>237</v>
+      </c>
+      <c r="R26" t="s">
+        <v>237</v>
+      </c>
       <c r="S26" s="10" t="s">
         <v>406</v>
       </c>
@@ -4482,6 +5436,27 @@
       </c>
       <c r="AA26" t="s">
         <v>251</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF26" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG26" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH26" t="s">
+        <v>237</v>
       </c>
       <c r="AI26" t="s">
         <v>237</v>
@@ -4536,6 +5511,24 @@
       <c r="L27" t="s">
         <v>237</v>
       </c>
+      <c r="M27" t="s">
+        <v>237</v>
+      </c>
+      <c r="N27" t="s">
+        <v>237</v>
+      </c>
+      <c r="O27" t="s">
+        <v>237</v>
+      </c>
+      <c r="P27" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>237</v>
+      </c>
+      <c r="R27" t="s">
+        <v>237</v>
+      </c>
       <c r="S27" s="10" t="s">
         <v>406</v>
       </c>
@@ -4562,6 +5555,27 @@
       </c>
       <c r="AA27" t="s">
         <v>251</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF27" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG27" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH27" t="s">
+        <v>237</v>
       </c>
       <c r="AI27" t="s">
         <v>237</v>
@@ -4616,6 +5630,24 @@
       <c r="L28" t="s">
         <v>237</v>
       </c>
+      <c r="M28" t="s">
+        <v>237</v>
+      </c>
+      <c r="N28" t="s">
+        <v>237</v>
+      </c>
+      <c r="O28" t="s">
+        <v>237</v>
+      </c>
+      <c r="P28" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>237</v>
+      </c>
+      <c r="R28" t="s">
+        <v>237</v>
+      </c>
       <c r="S28" s="10" t="s">
         <v>406</v>
       </c>
@@ -4641,6 +5673,27 @@
         <v>237</v>
       </c>
       <c r="AA28" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF28" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG28" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH28" t="s">
         <v>237</v>
       </c>
       <c r="AI28" t="s">
@@ -4696,6 +5749,24 @@
       <c r="L29" t="s">
         <v>237</v>
       </c>
+      <c r="M29" t="s">
+        <v>237</v>
+      </c>
+      <c r="N29" t="s">
+        <v>237</v>
+      </c>
+      <c r="O29" t="s">
+        <v>237</v>
+      </c>
+      <c r="P29" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>237</v>
+      </c>
+      <c r="R29" t="s">
+        <v>237</v>
+      </c>
       <c r="S29" s="10" t="s">
         <v>406</v>
       </c>
@@ -4721,6 +5792,27 @@
         <v>237</v>
       </c>
       <c r="AA29" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF29" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG29" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH29" t="s">
         <v>237</v>
       </c>
       <c r="AI29" t="s">
@@ -4776,6 +5868,24 @@
       <c r="L30" t="s">
         <v>237</v>
       </c>
+      <c r="M30" t="s">
+        <v>237</v>
+      </c>
+      <c r="N30" t="s">
+        <v>237</v>
+      </c>
+      <c r="O30" t="s">
+        <v>237</v>
+      </c>
+      <c r="P30" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>237</v>
+      </c>
+      <c r="R30" t="s">
+        <v>237</v>
+      </c>
       <c r="S30" s="10" t="s">
         <v>406</v>
       </c>
@@ -4801,6 +5911,27 @@
         <v>237</v>
       </c>
       <c r="AA30" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG30" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH30" t="s">
         <v>237</v>
       </c>
       <c r="AI30" t="s">
@@ -4856,6 +5987,24 @@
       <c r="L31" t="s">
         <v>237</v>
       </c>
+      <c r="M31" t="s">
+        <v>237</v>
+      </c>
+      <c r="N31" t="s">
+        <v>237</v>
+      </c>
+      <c r="O31" t="s">
+        <v>237</v>
+      </c>
+      <c r="P31" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>237</v>
+      </c>
+      <c r="R31" t="s">
+        <v>237</v>
+      </c>
       <c r="S31" s="10" t="s">
         <v>406</v>
       </c>
@@ -4881,6 +6030,27 @@
         <v>237</v>
       </c>
       <c r="AA31" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF31" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG31" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH31" t="s">
         <v>237</v>
       </c>
       <c r="AI31" t="s">
@@ -4936,6 +6106,24 @@
       <c r="L32" t="s">
         <v>237</v>
       </c>
+      <c r="M32" t="s">
+        <v>237</v>
+      </c>
+      <c r="N32" t="s">
+        <v>237</v>
+      </c>
+      <c r="O32" t="s">
+        <v>237</v>
+      </c>
+      <c r="P32" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>237</v>
+      </c>
+      <c r="R32" t="s">
+        <v>237</v>
+      </c>
       <c r="S32" s="10" t="s">
         <v>406</v>
       </c>
@@ -4961,6 +6149,27 @@
         <v>237</v>
       </c>
       <c r="AA32" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD32" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF32" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG32" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH32" t="s">
         <v>237</v>
       </c>
       <c r="AI32" t="s">
@@ -5016,6 +6225,24 @@
       <c r="L33" t="s">
         <v>237</v>
       </c>
+      <c r="M33" t="s">
+        <v>237</v>
+      </c>
+      <c r="N33" t="s">
+        <v>237</v>
+      </c>
+      <c r="O33" t="s">
+        <v>237</v>
+      </c>
+      <c r="P33" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>237</v>
+      </c>
+      <c r="R33" t="s">
+        <v>237</v>
+      </c>
       <c r="S33" s="10" t="s">
         <v>406</v>
       </c>
@@ -5041,6 +6268,27 @@
         <v>237</v>
       </c>
       <c r="AA33" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF33" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG33" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH33" t="s">
         <v>237</v>
       </c>
       <c r="AI33" t="s">
@@ -5096,6 +6344,24 @@
       <c r="L34" t="s">
         <v>237</v>
       </c>
+      <c r="M34" t="s">
+        <v>237</v>
+      </c>
+      <c r="N34" t="s">
+        <v>237</v>
+      </c>
+      <c r="O34" t="s">
+        <v>237</v>
+      </c>
+      <c r="P34" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>237</v>
+      </c>
+      <c r="R34" t="s">
+        <v>237</v>
+      </c>
       <c r="S34" s="10" t="s">
         <v>406</v>
       </c>
@@ -5121,6 +6387,27 @@
         <v>237</v>
       </c>
       <c r="AA34" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC34" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD34" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF34" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG34" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH34" t="s">
         <v>237</v>
       </c>
       <c r="AI34" t="s">
@@ -5176,6 +6463,24 @@
       <c r="L35" t="s">
         <v>237</v>
       </c>
+      <c r="M35" t="s">
+        <v>237</v>
+      </c>
+      <c r="N35" t="s">
+        <v>237</v>
+      </c>
+      <c r="O35" t="s">
+        <v>237</v>
+      </c>
+      <c r="P35" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>237</v>
+      </c>
+      <c r="R35" t="s">
+        <v>237</v>
+      </c>
       <c r="S35" s="10" t="s">
         <v>406</v>
       </c>
@@ -5201,6 +6506,27 @@
         <v>237</v>
       </c>
       <c r="AA35" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC35" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD35" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE35" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF35" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG35" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH35" t="s">
         <v>237</v>
       </c>
       <c r="AI35" t="s">
@@ -5256,6 +6582,24 @@
       <c r="L36" t="s">
         <v>237</v>
       </c>
+      <c r="M36" t="s">
+        <v>237</v>
+      </c>
+      <c r="N36" t="s">
+        <v>237</v>
+      </c>
+      <c r="O36" t="s">
+        <v>237</v>
+      </c>
+      <c r="P36" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>237</v>
+      </c>
+      <c r="R36" t="s">
+        <v>237</v>
+      </c>
       <c r="S36" s="10" t="s">
         <v>406</v>
       </c>
@@ -5281,6 +6625,27 @@
         <v>237</v>
       </c>
       <c r="AA36" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC36" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD36" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE36" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF36" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG36" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH36" t="s">
         <v>237</v>
       </c>
       <c r="AI36" t="s">
@@ -5336,6 +6701,24 @@
       <c r="L37" t="s">
         <v>237</v>
       </c>
+      <c r="M37" t="s">
+        <v>237</v>
+      </c>
+      <c r="N37" t="s">
+        <v>237</v>
+      </c>
+      <c r="O37" t="s">
+        <v>237</v>
+      </c>
+      <c r="P37" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>237</v>
+      </c>
+      <c r="R37" t="s">
+        <v>237</v>
+      </c>
       <c r="S37" s="10" t="s">
         <v>406</v>
       </c>
@@ -5361,6 +6744,27 @@
         <v>237</v>
       </c>
       <c r="AA37" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD37" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE37" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF37" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG37" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH37" t="s">
         <v>237</v>
       </c>
       <c r="AI37" t="s">
@@ -5416,6 +6820,24 @@
       <c r="L38" t="s">
         <v>237</v>
       </c>
+      <c r="M38" t="s">
+        <v>237</v>
+      </c>
+      <c r="N38" t="s">
+        <v>237</v>
+      </c>
+      <c r="O38" t="s">
+        <v>237</v>
+      </c>
+      <c r="P38" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>237</v>
+      </c>
+      <c r="R38" t="s">
+        <v>237</v>
+      </c>
       <c r="S38" s="1" t="s">
         <v>237</v>
       </c>
@@ -5443,13 +6865,27 @@
       <c r="AA38" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AB38" s="1"/>
-      <c r="AC38" s="1"/>
-      <c r="AD38" s="1"/>
-      <c r="AE38" s="1"/>
-      <c r="AF38" s="1"/>
-      <c r="AG38" s="1"/>
-      <c r="AH38" s="1"/>
+      <c r="AB38" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC38" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD38" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE38" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF38" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG38" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH38" t="s">
+        <v>237</v>
+      </c>
       <c r="AI38" t="s">
         <v>237</v>
       </c>
@@ -5503,6 +6939,24 @@
       <c r="L39" t="s">
         <v>237</v>
       </c>
+      <c r="M39" t="s">
+        <v>237</v>
+      </c>
+      <c r="N39" t="s">
+        <v>237</v>
+      </c>
+      <c r="O39" t="s">
+        <v>237</v>
+      </c>
+      <c r="P39" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>237</v>
+      </c>
+      <c r="R39" t="s">
+        <v>237</v>
+      </c>
       <c r="S39" s="1" t="s">
         <v>237</v>
       </c>
@@ -5530,13 +6984,27 @@
       <c r="AA39" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AB39" s="1"/>
-      <c r="AC39" s="1"/>
-      <c r="AD39" s="1"/>
-      <c r="AE39" s="1"/>
-      <c r="AF39" s="1"/>
-      <c r="AG39" s="1"/>
-      <c r="AH39" s="1"/>
+      <c r="AB39" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC39" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD39" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE39" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF39" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG39" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH39" t="s">
+        <v>237</v>
+      </c>
       <c r="AI39" t="s">
         <v>237</v>
       </c>
@@ -5590,6 +7058,24 @@
       <c r="L40" t="s">
         <v>237</v>
       </c>
+      <c r="M40" t="s">
+        <v>237</v>
+      </c>
+      <c r="N40" t="s">
+        <v>237</v>
+      </c>
+      <c r="O40" t="s">
+        <v>237</v>
+      </c>
+      <c r="P40" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>237</v>
+      </c>
+      <c r="R40" t="s">
+        <v>237</v>
+      </c>
       <c r="S40" s="1" t="s">
         <v>237</v>
       </c>
@@ -5616,6 +7102,27 @@
       </c>
       <c r="AA40" t="s">
         <v>241</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC40" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD40" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE40" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF40" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG40" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH40" t="s">
+        <v>237</v>
       </c>
       <c r="AI40" t="s">
         <v>237</v>
@@ -5670,6 +7177,24 @@
       <c r="L41" t="s">
         <v>237</v>
       </c>
+      <c r="M41" t="s">
+        <v>237</v>
+      </c>
+      <c r="N41" t="s">
+        <v>237</v>
+      </c>
+      <c r="O41" t="s">
+        <v>237</v>
+      </c>
+      <c r="P41" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>237</v>
+      </c>
+      <c r="R41" t="s">
+        <v>237</v>
+      </c>
       <c r="S41" s="1" t="s">
         <v>237</v>
       </c>
@@ -5697,13 +7222,27 @@
       <c r="AA41" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AB41" s="1"/>
-      <c r="AC41" s="1"/>
-      <c r="AD41" s="1"/>
-      <c r="AE41" s="1"/>
-      <c r="AF41" s="1"/>
-      <c r="AG41" s="1"/>
-      <c r="AH41" s="1"/>
+      <c r="AB41" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC41" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD41" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE41" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF41" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG41" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH41" t="s">
+        <v>237</v>
+      </c>
       <c r="AI41" t="s">
         <v>237</v>
       </c>
@@ -5757,6 +7296,24 @@
       <c r="L42" t="s">
         <v>237</v>
       </c>
+      <c r="M42" t="s">
+        <v>237</v>
+      </c>
+      <c r="N42" t="s">
+        <v>237</v>
+      </c>
+      <c r="O42" t="s">
+        <v>237</v>
+      </c>
+      <c r="P42" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>237</v>
+      </c>
+      <c r="R42" t="s">
+        <v>237</v>
+      </c>
       <c r="S42" s="1" t="s">
         <v>237</v>
       </c>
@@ -5784,13 +7341,27 @@
       <c r="AA42" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AB42" s="1"/>
-      <c r="AC42" s="1"/>
-      <c r="AD42" s="1"/>
-      <c r="AE42" s="1"/>
-      <c r="AF42" s="1"/>
-      <c r="AG42" s="1"/>
-      <c r="AH42" s="1"/>
+      <c r="AB42" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC42" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD42" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE42" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF42" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG42" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH42" t="s">
+        <v>237</v>
+      </c>
       <c r="AI42" t="s">
         <v>237</v>
       </c>
@@ -5844,6 +7415,24 @@
       <c r="L43" t="s">
         <v>237</v>
       </c>
+      <c r="M43" t="s">
+        <v>237</v>
+      </c>
+      <c r="N43" t="s">
+        <v>237</v>
+      </c>
+      <c r="O43" t="s">
+        <v>237</v>
+      </c>
+      <c r="P43" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>237</v>
+      </c>
+      <c r="R43" t="s">
+        <v>237</v>
+      </c>
       <c r="S43" s="1" t="s">
         <v>237</v>
       </c>
@@ -5871,13 +7460,27 @@
       <c r="AA43" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AB43" s="1"/>
-      <c r="AC43" s="1"/>
-      <c r="AD43" s="1"/>
-      <c r="AE43" s="1"/>
-      <c r="AF43" s="1"/>
-      <c r="AG43" s="1"/>
-      <c r="AH43" s="1"/>
+      <c r="AB43" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC43" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD43" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF43" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG43" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH43" t="s">
+        <v>237</v>
+      </c>
       <c r="AI43" t="s">
         <v>237</v>
       </c>
@@ -5931,6 +7534,24 @@
       <c r="L44" t="s">
         <v>237</v>
       </c>
+      <c r="M44" t="s">
+        <v>237</v>
+      </c>
+      <c r="N44" t="s">
+        <v>237</v>
+      </c>
+      <c r="O44" t="s">
+        <v>237</v>
+      </c>
+      <c r="P44" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>237</v>
+      </c>
+      <c r="R44" t="s">
+        <v>237</v>
+      </c>
       <c r="S44" s="1" t="s">
         <v>237</v>
       </c>
@@ -5957,6 +7578,27 @@
       </c>
       <c r="AA44" t="s">
         <v>251</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC44" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD44" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE44" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF44" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG44" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH44" t="s">
+        <v>237</v>
       </c>
       <c r="AI44" t="s">
         <v>237</v>
@@ -6011,6 +7653,24 @@
       <c r="L45" t="s">
         <v>237</v>
       </c>
+      <c r="M45" t="s">
+        <v>237</v>
+      </c>
+      <c r="N45" t="s">
+        <v>237</v>
+      </c>
+      <c r="O45" t="s">
+        <v>237</v>
+      </c>
+      <c r="P45" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>237</v>
+      </c>
+      <c r="R45" t="s">
+        <v>237</v>
+      </c>
       <c r="S45" s="1" t="s">
         <v>237</v>
       </c>
@@ -6038,13 +7698,27 @@
       <c r="AA45" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AB45" s="1"/>
-      <c r="AC45" s="1"/>
-      <c r="AD45" s="1"/>
-      <c r="AE45" s="1"/>
-      <c r="AF45" s="1"/>
-      <c r="AG45" s="1"/>
-      <c r="AH45" s="1"/>
+      <c r="AB45" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC45" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD45" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE45" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF45" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG45" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH45" t="s">
+        <v>237</v>
+      </c>
       <c r="AI45" t="s">
         <v>237</v>
       </c>
@@ -6098,6 +7772,24 @@
       <c r="L46" t="s">
         <v>320</v>
       </c>
+      <c r="M46" t="s">
+        <v>237</v>
+      </c>
+      <c r="N46" t="s">
+        <v>237</v>
+      </c>
+      <c r="O46" t="s">
+        <v>237</v>
+      </c>
+      <c r="P46" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>237</v>
+      </c>
+      <c r="R46" t="s">
+        <v>237</v>
+      </c>
       <c r="S46" s="1" t="s">
         <v>322</v>
       </c>
@@ -6125,13 +7817,27 @@
       <c r="AA46" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AB46" s="1"/>
-      <c r="AC46" s="1"/>
-      <c r="AD46" s="1"/>
-      <c r="AE46" s="1"/>
-      <c r="AF46" s="1"/>
-      <c r="AG46" s="1"/>
-      <c r="AH46" s="1"/>
+      <c r="AB46" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC46" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD46" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE46" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF46" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG46" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH46" t="s">
+        <v>237</v>
+      </c>
       <c r="AI46" t="s">
         <v>237</v>
       </c>
@@ -6185,6 +7891,24 @@
       <c r="L47" t="s">
         <v>320</v>
       </c>
+      <c r="M47" t="s">
+        <v>237</v>
+      </c>
+      <c r="N47" t="s">
+        <v>237</v>
+      </c>
+      <c r="O47" t="s">
+        <v>237</v>
+      </c>
+      <c r="P47" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>237</v>
+      </c>
+      <c r="R47" t="s">
+        <v>237</v>
+      </c>
       <c r="S47" s="1" t="s">
         <v>322</v>
       </c>
@@ -6212,13 +7936,27 @@
       <c r="AA47" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AB47" s="1"/>
-      <c r="AC47" s="1"/>
-      <c r="AD47" s="1"/>
-      <c r="AE47" s="1"/>
-      <c r="AF47" s="1"/>
-      <c r="AG47" s="1"/>
-      <c r="AH47" s="1"/>
+      <c r="AB47" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC47" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD47" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE47" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF47" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG47" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH47" t="s">
+        <v>237</v>
+      </c>
       <c r="AI47" t="s">
         <v>237</v>
       </c>
@@ -6272,6 +8010,24 @@
       <c r="L48" t="s">
         <v>320</v>
       </c>
+      <c r="M48" t="s">
+        <v>237</v>
+      </c>
+      <c r="N48" t="s">
+        <v>237</v>
+      </c>
+      <c r="O48" t="s">
+        <v>237</v>
+      </c>
+      <c r="P48" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>237</v>
+      </c>
+      <c r="R48" t="s">
+        <v>237</v>
+      </c>
       <c r="S48" s="1" t="s">
         <v>237</v>
       </c>
@@ -6299,13 +8055,27 @@
       <c r="AA48" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AB48" s="1"/>
-      <c r="AC48" s="1"/>
-      <c r="AD48" s="1"/>
-      <c r="AE48" s="1"/>
-      <c r="AF48" s="1"/>
-      <c r="AG48" s="1"/>
-      <c r="AH48" s="1"/>
+      <c r="AB48" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC48" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD48" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE48" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF48" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG48" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH48" t="s">
+        <v>237</v>
+      </c>
       <c r="AI48" t="s">
         <v>237</v>
       </c>
@@ -6359,6 +8129,24 @@
       <c r="L49" t="s">
         <v>320</v>
       </c>
+      <c r="M49" t="s">
+        <v>237</v>
+      </c>
+      <c r="N49" t="s">
+        <v>237</v>
+      </c>
+      <c r="O49" t="s">
+        <v>237</v>
+      </c>
+      <c r="P49" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>237</v>
+      </c>
+      <c r="R49" t="s">
+        <v>237</v>
+      </c>
       <c r="S49" s="1" t="s">
         <v>237</v>
       </c>
@@ -6386,13 +8174,27 @@
       <c r="AA49" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AB49" s="1"/>
-      <c r="AC49" s="1"/>
-      <c r="AD49" s="1"/>
-      <c r="AE49" s="1"/>
-      <c r="AF49" s="1"/>
-      <c r="AG49" s="1"/>
-      <c r="AH49" s="1"/>
+      <c r="AB49" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC49" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD49" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE49" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF49" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG49" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH49" t="s">
+        <v>237</v>
+      </c>
       <c r="AI49" t="s">
         <v>237</v>
       </c>
@@ -6446,6 +8248,24 @@
       <c r="L50" t="s">
         <v>320</v>
       </c>
+      <c r="M50" t="s">
+        <v>237</v>
+      </c>
+      <c r="N50" t="s">
+        <v>237</v>
+      </c>
+      <c r="O50" t="s">
+        <v>237</v>
+      </c>
+      <c r="P50" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>237</v>
+      </c>
+      <c r="R50" t="s">
+        <v>237</v>
+      </c>
       <c r="S50" s="1" t="s">
         <v>237</v>
       </c>
@@ -6473,13 +8293,27 @@
       <c r="AA50" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AB50" s="1"/>
-      <c r="AC50" s="1"/>
-      <c r="AD50" s="1"/>
-      <c r="AE50" s="1"/>
-      <c r="AF50" s="1"/>
-      <c r="AG50" s="1"/>
-      <c r="AH50" s="1"/>
+      <c r="AB50" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC50" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD50" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE50" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF50" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG50" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH50" t="s">
+        <v>237</v>
+      </c>
       <c r="AI50" t="s">
         <v>237</v>
       </c>
@@ -6533,6 +8367,24 @@
       <c r="L51" t="s">
         <v>237</v>
       </c>
+      <c r="M51" t="s">
+        <v>237</v>
+      </c>
+      <c r="N51" t="s">
+        <v>237</v>
+      </c>
+      <c r="O51" t="s">
+        <v>237</v>
+      </c>
+      <c r="P51" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>237</v>
+      </c>
+      <c r="R51" t="s">
+        <v>237</v>
+      </c>
       <c r="S51" s="1" t="s">
         <v>237</v>
       </c>
@@ -6560,13 +8412,27 @@
       <c r="AA51" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AB51" s="1"/>
-      <c r="AC51" s="1"/>
-      <c r="AD51" s="1"/>
-      <c r="AE51" s="1"/>
-      <c r="AF51" s="1"/>
-      <c r="AG51" s="1"/>
-      <c r="AH51" s="1"/>
+      <c r="AB51" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC51" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD51" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE51" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF51" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG51" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH51" t="s">
+        <v>237</v>
+      </c>
       <c r="AI51" t="s">
         <v>237</v>
       </c>
@@ -6620,6 +8486,24 @@
       <c r="L52" t="s">
         <v>237</v>
       </c>
+      <c r="M52" t="s">
+        <v>237</v>
+      </c>
+      <c r="N52" t="s">
+        <v>237</v>
+      </c>
+      <c r="O52" t="s">
+        <v>237</v>
+      </c>
+      <c r="P52" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>237</v>
+      </c>
+      <c r="R52" t="s">
+        <v>237</v>
+      </c>
       <c r="S52" s="1" t="s">
         <v>237</v>
       </c>
@@ -6646,6 +8530,27 @@
       </c>
       <c r="AA52" t="s">
         <v>241</v>
+      </c>
+      <c r="AB52" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC52" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD52" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE52" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF52" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG52" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH52" t="s">
+        <v>237</v>
       </c>
       <c r="AI52" t="s">
         <v>237</v>
@@ -6700,6 +8605,24 @@
       <c r="L53" t="s">
         <v>237</v>
       </c>
+      <c r="M53" t="s">
+        <v>237</v>
+      </c>
+      <c r="N53" t="s">
+        <v>237</v>
+      </c>
+      <c r="O53" t="s">
+        <v>237</v>
+      </c>
+      <c r="P53" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>237</v>
+      </c>
+      <c r="R53" t="s">
+        <v>237</v>
+      </c>
       <c r="S53" s="1" t="s">
         <v>237</v>
       </c>
@@ -6727,13 +8650,27 @@
       <c r="AA53" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AB53" s="1"/>
-      <c r="AC53" s="1"/>
-      <c r="AD53" s="1"/>
-      <c r="AE53" s="1"/>
-      <c r="AF53" s="1"/>
-      <c r="AG53" s="1"/>
-      <c r="AH53" s="1"/>
+      <c r="AB53" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC53" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD53" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE53" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF53" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG53" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH53" t="s">
+        <v>237</v>
+      </c>
       <c r="AI53" t="s">
         <v>237</v>
       </c>
@@ -6787,6 +8724,24 @@
       <c r="L54" t="s">
         <v>237</v>
       </c>
+      <c r="M54" t="s">
+        <v>237</v>
+      </c>
+      <c r="N54" t="s">
+        <v>237</v>
+      </c>
+      <c r="O54" t="s">
+        <v>237</v>
+      </c>
+      <c r="P54" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>237</v>
+      </c>
+      <c r="R54" t="s">
+        <v>237</v>
+      </c>
       <c r="S54" t="s">
         <v>237</v>
       </c>
@@ -6812,6 +8767,27 @@
         <v>237</v>
       </c>
       <c r="AA54" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB54" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC54" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD54" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE54" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF54" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG54" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH54" t="s">
         <v>237</v>
       </c>
       <c r="AI54" t="s">
@@ -6867,6 +8843,24 @@
       <c r="L55" t="s">
         <v>237</v>
       </c>
+      <c r="M55" t="s">
+        <v>237</v>
+      </c>
+      <c r="N55" t="s">
+        <v>237</v>
+      </c>
+      <c r="O55" t="s">
+        <v>237</v>
+      </c>
+      <c r="P55" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>237</v>
+      </c>
+      <c r="R55" t="s">
+        <v>237</v>
+      </c>
       <c r="S55" t="s">
         <v>237</v>
       </c>
@@ -6892,6 +8886,27 @@
         <v>237</v>
       </c>
       <c r="AA55" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB55" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC55" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD55" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE55" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF55" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG55" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH55" t="s">
         <v>237</v>
       </c>
       <c r="AI55" t="s">
@@ -6947,6 +8962,24 @@
       <c r="L56" t="s">
         <v>237</v>
       </c>
+      <c r="M56" t="s">
+        <v>237</v>
+      </c>
+      <c r="N56" t="s">
+        <v>237</v>
+      </c>
+      <c r="O56" t="s">
+        <v>237</v>
+      </c>
+      <c r="P56" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>237</v>
+      </c>
+      <c r="R56" t="s">
+        <v>237</v>
+      </c>
       <c r="S56" t="s">
         <v>237</v>
       </c>
@@ -6972,6 +9005,27 @@
         <v>237</v>
       </c>
       <c r="AA56" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB56" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC56" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD56" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE56" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF56" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG56" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH56" t="s">
         <v>237</v>
       </c>
       <c r="AI56" t="s">

</xml_diff>

<commit_message>
data_required_csv add other_disagg_set columns
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7BEB47-36FB-4B41-AC3B-ECC62B84E8A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10648BF4-47A8-7E4D-A43D-A6DE45C129AF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data_required!$A$1:$AM$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data_required!$A$1:$AO$56</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">dimension_Item_sets!$A$1:$AF$120</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3417" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3529" uniqueCount="644">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1964,6 +1964,12 @@
   </si>
   <si>
     <t>B.disagg_type_uid</t>
+  </si>
+  <si>
+    <t>A.other_disagg_set</t>
+  </si>
+  <si>
+    <t>B.other_disagg_set</t>
   </si>
 </sst>
 </file>
@@ -2359,12 +2365,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
-  <dimension ref="A1:AM56"/>
+  <dimension ref="A1:AO56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="AD16" sqref="AD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2376,14 +2382,15 @@
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
     <col min="7" max="7" width="68.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="20" width="17.33203125" customWidth="1"/>
-    <col min="21" max="21" width="53.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="24" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="46.83203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="21" width="17.33203125" customWidth="1"/>
+    <col min="22" max="22" width="53.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="46.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>274</v>
       </c>
@@ -2421,88 +2428,94 @@
         <v>283</v>
       </c>
       <c r="M1" t="s">
+        <v>642</v>
+      </c>
+      <c r="N1" t="s">
         <v>630</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>631</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>632</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>633</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>634</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>635</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>288</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>391</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>289</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>392</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>279</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>393</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>276</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>277</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>278</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>629</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
+        <v>643</v>
+      </c>
+      <c r="AE1" t="s">
         <v>636</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>637</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>638</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>639</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>640</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>641</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>429</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>430</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>431</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>432</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2620,8 +2633,14 @@
       <c r="AM2" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2739,8 +2758,14 @@
       <c r="AM3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN3" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2858,8 +2883,14 @@
       <c r="AM4" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN4" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -2977,8 +3008,14 @@
       <c r="AM5" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -3096,8 +3133,14 @@
       <c r="AM6" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN6" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -3215,8 +3258,14 @@
       <c r="AM7" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN7" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -3284,23 +3333,23 @@
         <v>237</v>
       </c>
       <c r="W8" t="s">
+        <v>237</v>
+      </c>
+      <c r="X8" t="s">
         <v>136</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>137</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="Z8" t="s">
         <v>233</v>
       </c>
-      <c r="Z8" s="2" t="s">
+      <c r="AA8" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AB8" t="s">
         <v>241</v>
       </c>
-      <c r="AB8" t="s">
-        <v>237</v>
-      </c>
       <c r="AC8" t="s">
         <v>237</v>
       </c>
@@ -3332,10 +3381,16 @@
         <v>237</v>
       </c>
       <c r="AM8" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO8" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -3453,8 +3508,14 @@
       <c r="AM9" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN9" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -3572,8 +3633,14 @@
       <c r="AM10" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN10" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -3691,8 +3758,14 @@
       <c r="AM11" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN11" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -3810,8 +3883,14 @@
       <c r="AM12" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN12" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -3929,8 +4008,14 @@
       <c r="AM13" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN13" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO13" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -4048,8 +4133,14 @@
       <c r="AM14" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="15" spans="1:39" ht="18" x14ac:dyDescent="0.25">
+      <c r="AN14" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO14" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -4104,21 +4195,21 @@
       <c r="R15" t="s">
         <v>237</v>
       </c>
-      <c r="S15" s="10" t="s">
+      <c r="S15" t="s">
+        <v>237</v>
+      </c>
+      <c r="T15" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="T15" t="s">
+      <c r="U15" t="s">
         <v>296</v>
       </c>
-      <c r="U15" t="s">
+      <c r="V15" t="s">
         <v>425</v>
       </c>
-      <c r="V15" t="s">
+      <c r="W15" t="s">
         <v>426</v>
       </c>
-      <c r="W15" t="s">
-        <v>237</v>
-      </c>
       <c r="X15" t="s">
         <v>237</v>
       </c>
@@ -4167,8 +4258,14 @@
       <c r="AM15" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="16" spans="1:39" ht="18" x14ac:dyDescent="0.25">
+      <c r="AN15" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO15" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -4223,21 +4320,21 @@
       <c r="R16" t="s">
         <v>237</v>
       </c>
-      <c r="S16" s="10" t="s">
+      <c r="S16" t="s">
+        <v>237</v>
+      </c>
+      <c r="T16" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="T16" t="s">
+      <c r="U16" t="s">
         <v>296</v>
       </c>
-      <c r="U16" t="s">
+      <c r="V16" t="s">
         <v>427</v>
       </c>
-      <c r="V16" t="s">
+      <c r="W16" t="s">
         <v>428</v>
       </c>
-      <c r="W16" t="s">
-        <v>237</v>
-      </c>
       <c r="X16" t="s">
         <v>237</v>
       </c>
@@ -4286,8 +4383,14 @@
       <c r="AM16" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="17" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+      <c r="AN16" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO16" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -4339,36 +4442,36 @@
       <c r="R17" t="s">
         <v>237</v>
       </c>
-      <c r="S17" s="10" t="s">
+      <c r="S17" t="s">
+        <v>237</v>
+      </c>
+      <c r="T17" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="T17" t="s">
+      <c r="U17" t="s">
         <v>296</v>
       </c>
-      <c r="U17" t="s">
+      <c r="V17" t="s">
         <v>425</v>
       </c>
-      <c r="V17" t="s">
+      <c r="W17" t="s">
         <v>426</v>
       </c>
-      <c r="W17" t="s">
+      <c r="X17" t="s">
         <v>419</v>
       </c>
-      <c r="X17" s="1" t="s">
+      <c r="Y17" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="Y17" t="s">
+      <c r="Z17" t="s">
         <v>233</v>
       </c>
-      <c r="Z17" t="s">
+      <c r="AA17" t="s">
         <v>252</v>
       </c>
-      <c r="AA17" t="s">
+      <c r="AB17" t="s">
         <v>251</v>
       </c>
-      <c r="AB17" t="s">
-        <v>237</v>
-      </c>
       <c r="AC17" t="s">
         <v>237</v>
       </c>
@@ -4387,23 +4490,29 @@
       <c r="AH17" t="s">
         <v>237</v>
       </c>
-      <c r="AI17" s="10" t="s">
+      <c r="AI17" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK17" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="AJ17" t="s">
+      <c r="AL17" t="s">
         <v>296</v>
       </c>
-      <c r="AK17" t="s">
+      <c r="AM17" t="s">
         <v>427</v>
       </c>
-      <c r="AL17" t="s">
+      <c r="AN17" t="s">
         <v>428</v>
       </c>
-      <c r="AM17" t="s">
+      <c r="AO17" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="18" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -4458,36 +4567,36 @@
       <c r="R18" t="s">
         <v>237</v>
       </c>
-      <c r="S18" s="10" t="s">
+      <c r="S18" t="s">
+        <v>237</v>
+      </c>
+      <c r="T18" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="T18" t="s">
+      <c r="U18" t="s">
         <v>296</v>
       </c>
-      <c r="U18" t="s">
+      <c r="V18" t="s">
         <v>435</v>
       </c>
-      <c r="V18" t="s">
+      <c r="W18" t="s">
         <v>253</v>
       </c>
-      <c r="W18" t="s">
+      <c r="X18" t="s">
         <v>419</v>
       </c>
-      <c r="X18" s="1" t="s">
+      <c r="Y18" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="Y18" t="s">
+      <c r="Z18" t="s">
         <v>233</v>
       </c>
-      <c r="Z18" s="9" t="s">
+      <c r="AA18" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="AA18" t="s">
+      <c r="AB18" t="s">
         <v>251</v>
       </c>
-      <c r="AB18" t="s">
-        <v>237</v>
-      </c>
       <c r="AC18" t="s">
         <v>237</v>
       </c>
@@ -4519,10 +4628,16 @@
         <v>237</v>
       </c>
       <c r="AM18" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN18" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO18" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="19" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -4577,36 +4692,36 @@
       <c r="R19" t="s">
         <v>237</v>
       </c>
-      <c r="S19" s="10" t="s">
+      <c r="S19" t="s">
+        <v>237</v>
+      </c>
+      <c r="T19" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="T19" t="s">
+      <c r="U19" t="s">
         <v>296</v>
       </c>
-      <c r="U19" t="s">
+      <c r="V19" t="s">
         <v>436</v>
       </c>
-      <c r="V19" t="s">
+      <c r="W19" t="s">
         <v>261</v>
       </c>
-      <c r="W19" t="s">
+      <c r="X19" t="s">
         <v>419</v>
       </c>
-      <c r="X19" s="1" t="s">
+      <c r="Y19" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="Y19" t="s">
+      <c r="Z19" t="s">
         <v>233</v>
       </c>
-      <c r="Z19" s="9" t="s">
+      <c r="AA19" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="AA19" t="s">
+      <c r="AB19" t="s">
         <v>251</v>
       </c>
-      <c r="AB19" t="s">
-        <v>237</v>
-      </c>
       <c r="AC19" t="s">
         <v>237</v>
       </c>
@@ -4638,10 +4753,16 @@
         <v>237</v>
       </c>
       <c r="AM19" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN19" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO19" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="20" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -4696,36 +4817,36 @@
       <c r="R20" t="s">
         <v>237</v>
       </c>
-      <c r="S20" s="10" t="s">
+      <c r="S20" t="s">
+        <v>237</v>
+      </c>
+      <c r="T20" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="T20" t="s">
+      <c r="U20" t="s">
         <v>296</v>
       </c>
-      <c r="U20" t="s">
+      <c r="V20" t="s">
         <v>437</v>
       </c>
-      <c r="V20" t="s">
+      <c r="W20" t="s">
         <v>268</v>
       </c>
-      <c r="W20" t="s">
+      <c r="X20" t="s">
         <v>419</v>
       </c>
-      <c r="X20" s="1" t="s">
+      <c r="Y20" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="Y20" t="s">
+      <c r="Z20" t="s">
         <v>233</v>
       </c>
-      <c r="Z20" s="9" t="s">
+      <c r="AA20" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="AA20" t="s">
+      <c r="AB20" t="s">
         <v>251</v>
       </c>
-      <c r="AB20" t="s">
-        <v>237</v>
-      </c>
       <c r="AC20" t="s">
         <v>237</v>
       </c>
@@ -4757,10 +4878,16 @@
         <v>237</v>
       </c>
       <c r="AM20" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN20" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO20" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="21" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -4815,36 +4942,36 @@
       <c r="R21" t="s">
         <v>237</v>
       </c>
-      <c r="S21" s="10" t="s">
+      <c r="S21" t="s">
+        <v>237</v>
+      </c>
+      <c r="T21" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="T21" t="s">
+      <c r="U21" t="s">
         <v>296</v>
       </c>
-      <c r="U21" t="s">
+      <c r="V21" t="s">
         <v>438</v>
       </c>
-      <c r="V21" t="s">
+      <c r="W21" t="s">
         <v>263</v>
       </c>
-      <c r="W21" t="s">
+      <c r="X21" t="s">
         <v>419</v>
       </c>
-      <c r="X21" s="1" t="s">
+      <c r="Y21" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="Y21" t="s">
+      <c r="Z21" t="s">
         <v>233</v>
       </c>
-      <c r="Z21" s="9" t="s">
+      <c r="AA21" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="AA21" t="s">
+      <c r="AB21" t="s">
         <v>251</v>
       </c>
-      <c r="AB21" t="s">
-        <v>237</v>
-      </c>
       <c r="AC21" t="s">
         <v>237</v>
       </c>
@@ -4876,10 +5003,16 @@
         <v>237</v>
       </c>
       <c r="AM21" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN21" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO21" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="22" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -4934,36 +5067,36 @@
       <c r="R22" t="s">
         <v>237</v>
       </c>
-      <c r="S22" s="10" t="s">
+      <c r="S22" t="s">
+        <v>237</v>
+      </c>
+      <c r="T22" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="T22" t="s">
+      <c r="U22" t="s">
         <v>296</v>
       </c>
-      <c r="U22" t="s">
+      <c r="V22" t="s">
         <v>439</v>
       </c>
-      <c r="V22" t="s">
+      <c r="W22" t="s">
         <v>264</v>
       </c>
-      <c r="W22" t="s">
+      <c r="X22" t="s">
         <v>419</v>
       </c>
-      <c r="X22" s="1" t="s">
+      <c r="Y22" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="Y22" t="s">
+      <c r="Z22" t="s">
         <v>233</v>
       </c>
-      <c r="Z22" s="9" t="s">
+      <c r="AA22" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="AA22" t="s">
+      <c r="AB22" t="s">
         <v>251</v>
       </c>
-      <c r="AB22" t="s">
-        <v>237</v>
-      </c>
       <c r="AC22" t="s">
         <v>237</v>
       </c>
@@ -4995,10 +5128,16 @@
         <v>237</v>
       </c>
       <c r="AM22" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN22" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO22" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="23" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -5053,36 +5192,36 @@
       <c r="R23" t="s">
         <v>237</v>
       </c>
-      <c r="S23" s="10" t="s">
+      <c r="S23" t="s">
+        <v>237</v>
+      </c>
+      <c r="T23" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="T23" t="s">
+      <c r="U23" t="s">
         <v>296</v>
       </c>
-      <c r="U23" t="s">
+      <c r="V23" t="s">
         <v>440</v>
       </c>
-      <c r="V23" t="s">
+      <c r="W23" t="s">
         <v>265</v>
       </c>
-      <c r="W23" t="s">
+      <c r="X23" t="s">
         <v>419</v>
       </c>
-      <c r="X23" s="1" t="s">
+      <c r="Y23" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="Y23" t="s">
+      <c r="Z23" t="s">
         <v>233</v>
       </c>
-      <c r="Z23" s="3" t="s">
+      <c r="AA23" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="AA23" t="s">
+      <c r="AB23" t="s">
         <v>251</v>
       </c>
-      <c r="AB23" t="s">
-        <v>237</v>
-      </c>
       <c r="AC23" t="s">
         <v>237</v>
       </c>
@@ -5114,10 +5253,16 @@
         <v>237</v>
       </c>
       <c r="AM23" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN23" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO23" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="24" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -5172,36 +5317,36 @@
       <c r="R24" t="s">
         <v>237</v>
       </c>
-      <c r="S24" s="10" t="s">
+      <c r="S24" t="s">
+        <v>237</v>
+      </c>
+      <c r="T24" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="T24" t="s">
+      <c r="U24" t="s">
         <v>296</v>
       </c>
-      <c r="U24" t="s">
+      <c r="V24" t="s">
         <v>441</v>
       </c>
-      <c r="V24" t="s">
+      <c r="W24" t="s">
         <v>266</v>
       </c>
-      <c r="W24" t="s">
+      <c r="X24" t="s">
         <v>419</v>
       </c>
-      <c r="X24" s="1" t="s">
+      <c r="Y24" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="Y24" t="s">
+      <c r="Z24" t="s">
         <v>233</v>
       </c>
-      <c r="Z24" s="3" t="s">
+      <c r="AA24" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="AA24" t="s">
+      <c r="AB24" t="s">
         <v>251</v>
       </c>
-      <c r="AB24" t="s">
-        <v>237</v>
-      </c>
       <c r="AC24" t="s">
         <v>237</v>
       </c>
@@ -5233,10 +5378,16 @@
         <v>237</v>
       </c>
       <c r="AM24" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN24" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO24" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="25" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -5291,36 +5442,36 @@
       <c r="R25" t="s">
         <v>237</v>
       </c>
-      <c r="S25" s="10" t="s">
+      <c r="S25" t="s">
+        <v>237</v>
+      </c>
+      <c r="T25" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="T25" t="s">
+      <c r="U25" t="s">
         <v>296</v>
       </c>
-      <c r="U25" t="s">
+      <c r="V25" t="s">
         <v>442</v>
       </c>
-      <c r="V25" t="s">
+      <c r="W25" t="s">
         <v>267</v>
       </c>
-      <c r="W25" t="s">
+      <c r="X25" t="s">
         <v>419</v>
       </c>
-      <c r="X25" s="1" t="s">
+      <c r="Y25" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="Y25" t="s">
+      <c r="Z25" t="s">
         <v>233</v>
       </c>
-      <c r="Z25" s="9" t="s">
+      <c r="AA25" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="AA25" t="s">
+      <c r="AB25" t="s">
         <v>251</v>
       </c>
-      <c r="AB25" t="s">
-        <v>237</v>
-      </c>
       <c r="AC25" t="s">
         <v>237</v>
       </c>
@@ -5352,10 +5503,16 @@
         <v>237</v>
       </c>
       <c r="AM25" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN25" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO25" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="26" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -5410,36 +5567,36 @@
       <c r="R26" t="s">
         <v>237</v>
       </c>
-      <c r="S26" s="10" t="s">
+      <c r="S26" t="s">
+        <v>237</v>
+      </c>
+      <c r="T26" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="T26" t="s">
+      <c r="U26" t="s">
         <v>296</v>
       </c>
-      <c r="U26" t="s">
+      <c r="V26" t="s">
         <v>443</v>
       </c>
-      <c r="V26" t="s">
+      <c r="W26" t="s">
         <v>262</v>
       </c>
-      <c r="W26" t="s">
+      <c r="X26" t="s">
         <v>419</v>
       </c>
-      <c r="X26" s="1" t="s">
+      <c r="Y26" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="Y26" t="s">
+      <c r="Z26" t="s">
         <v>233</v>
       </c>
-      <c r="Z26" s="9" t="s">
+      <c r="AA26" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="AA26" t="s">
+      <c r="AB26" t="s">
         <v>251</v>
       </c>
-      <c r="AB26" t="s">
-        <v>237</v>
-      </c>
       <c r="AC26" t="s">
         <v>237</v>
       </c>
@@ -5471,10 +5628,16 @@
         <v>237</v>
       </c>
       <c r="AM26" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN26" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO26" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="27" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -5529,36 +5692,36 @@
       <c r="R27" t="s">
         <v>237</v>
       </c>
-      <c r="S27" s="10" t="s">
+      <c r="S27" t="s">
+        <v>237</v>
+      </c>
+      <c r="T27" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="T27" t="s">
+      <c r="U27" t="s">
         <v>296</v>
       </c>
-      <c r="U27" t="s">
+      <c r="V27" t="s">
         <v>444</v>
       </c>
-      <c r="V27" t="s">
+      <c r="W27" t="s">
         <v>269</v>
       </c>
-      <c r="W27" t="s">
+      <c r="X27" t="s">
         <v>419</v>
       </c>
-      <c r="X27" s="1" t="s">
+      <c r="Y27" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="Y27" t="s">
+      <c r="Z27" t="s">
         <v>233</v>
       </c>
-      <c r="Z27" s="9" t="s">
+      <c r="AA27" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="AA27" t="s">
+      <c r="AB27" t="s">
         <v>251</v>
       </c>
-      <c r="AB27" t="s">
-        <v>237</v>
-      </c>
       <c r="AC27" t="s">
         <v>237</v>
       </c>
@@ -5590,10 +5753,16 @@
         <v>237</v>
       </c>
       <c r="AM27" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN27" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO27" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="28" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -5648,21 +5817,21 @@
       <c r="R28" t="s">
         <v>237</v>
       </c>
-      <c r="S28" s="10" t="s">
+      <c r="S28" t="s">
+        <v>237</v>
+      </c>
+      <c r="T28" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="T28" t="s">
+      <c r="U28" t="s">
         <v>296</v>
       </c>
-      <c r="U28" t="s">
+      <c r="V28" t="s">
         <v>435</v>
       </c>
-      <c r="V28" t="s">
+      <c r="W28" t="s">
         <v>253</v>
       </c>
-      <c r="W28" t="s">
-        <v>237</v>
-      </c>
       <c r="X28" t="s">
         <v>237</v>
       </c>
@@ -5711,8 +5880,14 @@
       <c r="AM28" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="29" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+      <c r="AN28" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -5767,21 +5942,21 @@
       <c r="R29" t="s">
         <v>237</v>
       </c>
-      <c r="S29" s="10" t="s">
+      <c r="S29" t="s">
+        <v>237</v>
+      </c>
+      <c r="T29" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="T29" t="s">
+      <c r="U29" t="s">
         <v>296</v>
       </c>
-      <c r="U29" t="s">
+      <c r="V29" t="s">
         <v>436</v>
       </c>
-      <c r="V29" t="s">
+      <c r="W29" t="s">
         <v>261</v>
       </c>
-      <c r="W29" t="s">
-        <v>237</v>
-      </c>
       <c r="X29" t="s">
         <v>237</v>
       </c>
@@ -5830,8 +6005,14 @@
       <c r="AM29" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="30" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+      <c r="AN29" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO29" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="30" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -5886,21 +6067,21 @@
       <c r="R30" t="s">
         <v>237</v>
       </c>
-      <c r="S30" s="10" t="s">
+      <c r="S30" t="s">
+        <v>237</v>
+      </c>
+      <c r="T30" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="T30" t="s">
+      <c r="U30" t="s">
         <v>296</v>
       </c>
-      <c r="U30" t="s">
+      <c r="V30" t="s">
         <v>437</v>
       </c>
-      <c r="V30" t="s">
+      <c r="W30" t="s">
         <v>268</v>
       </c>
-      <c r="W30" t="s">
-        <v>237</v>
-      </c>
       <c r="X30" t="s">
         <v>237</v>
       </c>
@@ -5949,8 +6130,14 @@
       <c r="AM30" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="31" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+      <c r="AN30" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO30" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="31" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -6005,21 +6192,21 @@
       <c r="R31" t="s">
         <v>237</v>
       </c>
-      <c r="S31" s="10" t="s">
+      <c r="S31" t="s">
+        <v>237</v>
+      </c>
+      <c r="T31" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="T31" t="s">
+      <c r="U31" t="s">
         <v>296</v>
       </c>
-      <c r="U31" t="s">
+      <c r="V31" t="s">
         <v>438</v>
       </c>
-      <c r="V31" t="s">
+      <c r="W31" t="s">
         <v>263</v>
       </c>
-      <c r="W31" t="s">
-        <v>237</v>
-      </c>
       <c r="X31" t="s">
         <v>237</v>
       </c>
@@ -6068,8 +6255,14 @@
       <c r="AM31" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="32" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+      <c r="AN31" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO31" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="32" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -6124,21 +6317,21 @@
       <c r="R32" t="s">
         <v>237</v>
       </c>
-      <c r="S32" s="10" t="s">
+      <c r="S32" t="s">
+        <v>237</v>
+      </c>
+      <c r="T32" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="T32" t="s">
+      <c r="U32" t="s">
         <v>296</v>
       </c>
-      <c r="U32" t="s">
+      <c r="V32" t="s">
         <v>439</v>
       </c>
-      <c r="V32" t="s">
+      <c r="W32" t="s">
         <v>264</v>
       </c>
-      <c r="W32" t="s">
-        <v>237</v>
-      </c>
       <c r="X32" t="s">
         <v>237</v>
       </c>
@@ -6187,8 +6380,14 @@
       <c r="AM32" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="33" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+      <c r="AN32" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO32" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="33" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -6243,21 +6442,21 @@
       <c r="R33" t="s">
         <v>237</v>
       </c>
-      <c r="S33" s="10" t="s">
+      <c r="S33" t="s">
+        <v>237</v>
+      </c>
+      <c r="T33" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="T33" t="s">
+      <c r="U33" t="s">
         <v>296</v>
       </c>
-      <c r="U33" t="s">
+      <c r="V33" t="s">
         <v>440</v>
       </c>
-      <c r="V33" t="s">
+      <c r="W33" t="s">
         <v>265</v>
       </c>
-      <c r="W33" t="s">
-        <v>237</v>
-      </c>
       <c r="X33" t="s">
         <v>237</v>
       </c>
@@ -6306,8 +6505,14 @@
       <c r="AM33" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="34" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+      <c r="AN33" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO33" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="34" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -6362,21 +6567,21 @@
       <c r="R34" t="s">
         <v>237</v>
       </c>
-      <c r="S34" s="10" t="s">
+      <c r="S34" t="s">
+        <v>237</v>
+      </c>
+      <c r="T34" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="T34" t="s">
+      <c r="U34" t="s">
         <v>296</v>
       </c>
-      <c r="U34" t="s">
+      <c r="V34" t="s">
         <v>441</v>
       </c>
-      <c r="V34" t="s">
+      <c r="W34" t="s">
         <v>266</v>
       </c>
-      <c r="W34" t="s">
-        <v>237</v>
-      </c>
       <c r="X34" t="s">
         <v>237</v>
       </c>
@@ -6425,8 +6630,14 @@
       <c r="AM34" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="35" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+      <c r="AN34" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO34" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="35" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -6481,21 +6692,21 @@
       <c r="R35" t="s">
         <v>237</v>
       </c>
-      <c r="S35" s="10" t="s">
+      <c r="S35" t="s">
+        <v>237</v>
+      </c>
+      <c r="T35" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="T35" t="s">
+      <c r="U35" t="s">
         <v>296</v>
       </c>
-      <c r="U35" t="s">
+      <c r="V35" t="s">
         <v>442</v>
       </c>
-      <c r="V35" t="s">
+      <c r="W35" t="s">
         <v>267</v>
       </c>
-      <c r="W35" t="s">
-        <v>237</v>
-      </c>
       <c r="X35" t="s">
         <v>237</v>
       </c>
@@ -6544,8 +6755,14 @@
       <c r="AM35" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="36" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+      <c r="AN35" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO35" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="36" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -6600,21 +6817,21 @@
       <c r="R36" t="s">
         <v>237</v>
       </c>
-      <c r="S36" s="10" t="s">
+      <c r="S36" t="s">
+        <v>237</v>
+      </c>
+      <c r="T36" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="T36" t="s">
+      <c r="U36" t="s">
         <v>296</v>
       </c>
-      <c r="U36" t="s">
+      <c r="V36" t="s">
         <v>443</v>
       </c>
-      <c r="V36" t="s">
+      <c r="W36" t="s">
         <v>262</v>
       </c>
-      <c r="W36" t="s">
-        <v>237</v>
-      </c>
       <c r="X36" t="s">
         <v>237</v>
       </c>
@@ -6663,8 +6880,14 @@
       <c r="AM36" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="37" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+      <c r="AN36" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO36" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="37" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -6719,21 +6942,21 @@
       <c r="R37" t="s">
         <v>237</v>
       </c>
-      <c r="S37" s="10" t="s">
+      <c r="S37" t="s">
+        <v>237</v>
+      </c>
+      <c r="T37" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="T37" t="s">
+      <c r="U37" t="s">
         <v>296</v>
       </c>
-      <c r="U37" t="s">
+      <c r="V37" t="s">
         <v>444</v>
       </c>
-      <c r="V37" t="s">
+      <c r="W37" t="s">
         <v>269</v>
       </c>
-      <c r="W37" t="s">
-        <v>237</v>
-      </c>
       <c r="X37" t="s">
         <v>237</v>
       </c>
@@ -6782,8 +7005,14 @@
       <c r="AM37" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="38" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+      <c r="AN37" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO37" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="38" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -6838,7 +7067,7 @@
       <c r="R38" t="s">
         <v>237</v>
       </c>
-      <c r="S38" s="1" t="s">
+      <c r="S38" t="s">
         <v>237</v>
       </c>
       <c r="T38" s="1" t="s">
@@ -6865,7 +7094,7 @@
       <c r="AA38" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AB38" t="s">
+      <c r="AB38" s="1" t="s">
         <v>237</v>
       </c>
       <c r="AC38" t="s">
@@ -6898,11 +7127,17 @@
       <c r="AL38" t="s">
         <v>237</v>
       </c>
-      <c r="AM38" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="39" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+      <c r="AM38" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN38" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO38" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="39" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -6957,7 +7192,7 @@
       <c r="R39" t="s">
         <v>237</v>
       </c>
-      <c r="S39" s="1" t="s">
+      <c r="S39" t="s">
         <v>237</v>
       </c>
       <c r="T39" s="1" t="s">
@@ -6984,7 +7219,7 @@
       <c r="AA39" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AB39" t="s">
+      <c r="AB39" s="1" t="s">
         <v>237</v>
       </c>
       <c r="AC39" t="s">
@@ -7017,11 +7252,17 @@
       <c r="AL39" t="s">
         <v>237</v>
       </c>
-      <c r="AM39" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="40" spans="1:39" ht="18" x14ac:dyDescent="0.2">
+      <c r="AM39" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN39" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO39" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="40" spans="1:41" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>35</v>
       </c>
@@ -7076,7 +7317,7 @@
       <c r="R40" t="s">
         <v>237</v>
       </c>
-      <c r="S40" s="1" t="s">
+      <c r="S40" t="s">
         <v>237</v>
       </c>
       <c r="T40" s="1" t="s">
@@ -7088,24 +7329,24 @@
       <c r="V40" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="W40" t="s">
+      <c r="W40" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="X40" t="s">
         <v>303</v>
       </c>
-      <c r="X40" t="s">
+      <c r="Y40" t="s">
         <v>302</v>
       </c>
-      <c r="Y40" s="1" t="s">
+      <c r="Z40" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="Z40" s="9" t="s">
+      <c r="AA40" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="AA40" t="s">
+      <c r="AB40" t="s">
         <v>241</v>
       </c>
-      <c r="AB40" t="s">
-        <v>237</v>
-      </c>
       <c r="AC40" t="s">
         <v>237</v>
       </c>
@@ -7137,10 +7378,16 @@
         <v>237</v>
       </c>
       <c r="AM40" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN40" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO40" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="41" spans="1:39" ht="18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:41" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>82</v>
       </c>
@@ -7195,7 +7442,7 @@
       <c r="R41" t="s">
         <v>237</v>
       </c>
-      <c r="S41" s="1" t="s">
+      <c r="S41" t="s">
         <v>237</v>
       </c>
       <c r="T41" s="1" t="s">
@@ -7222,7 +7469,7 @@
       <c r="AA41" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AB41" t="s">
+      <c r="AB41" s="1" t="s">
         <v>237</v>
       </c>
       <c r="AC41" t="s">
@@ -7255,11 +7502,17 @@
       <c r="AL41" t="s">
         <v>237</v>
       </c>
-      <c r="AM41" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="42" spans="1:39" ht="18" x14ac:dyDescent="0.2">
+      <c r="AM41" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN41" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO41" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="42" spans="1:41" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>82</v>
       </c>
@@ -7314,7 +7567,7 @@
       <c r="R42" t="s">
         <v>237</v>
       </c>
-      <c r="S42" s="1" t="s">
+      <c r="S42" t="s">
         <v>237</v>
       </c>
       <c r="T42" s="1" t="s">
@@ -7341,7 +7594,7 @@
       <c r="AA42" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AB42" t="s">
+      <c r="AB42" s="1" t="s">
         <v>237</v>
       </c>
       <c r="AC42" t="s">
@@ -7374,11 +7627,17 @@
       <c r="AL42" t="s">
         <v>237</v>
       </c>
-      <c r="AM42" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="43" spans="1:39" ht="18" x14ac:dyDescent="0.2">
+      <c r="AM42" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN42" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO42" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="43" spans="1:41" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>87</v>
       </c>
@@ -7433,7 +7692,7 @@
       <c r="R43" t="s">
         <v>237</v>
       </c>
-      <c r="S43" s="1" t="s">
+      <c r="S43" t="s">
         <v>237</v>
       </c>
       <c r="T43" s="1" t="s">
@@ -7460,7 +7719,7 @@
       <c r="AA43" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AB43" t="s">
+      <c r="AB43" s="1" t="s">
         <v>237</v>
       </c>
       <c r="AC43" t="s">
@@ -7493,11 +7752,17 @@
       <c r="AL43" t="s">
         <v>237</v>
       </c>
-      <c r="AM43" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="44" spans="1:39" ht="18" x14ac:dyDescent="0.2">
+      <c r="AM43" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN43" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO43" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="44" spans="1:41" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>87</v>
       </c>
@@ -7552,7 +7817,7 @@
       <c r="R44" t="s">
         <v>237</v>
       </c>
-      <c r="S44" s="1" t="s">
+      <c r="S44" t="s">
         <v>237</v>
       </c>
       <c r="T44" s="1" t="s">
@@ -7564,24 +7829,24 @@
       <c r="V44" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="W44" t="s">
+      <c r="W44" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="X44" t="s">
         <v>304</v>
       </c>
-      <c r="X44" t="s">
+      <c r="Y44" t="s">
         <v>305</v>
       </c>
-      <c r="Y44" s="1" t="s">
+      <c r="Z44" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="Z44" t="s">
+      <c r="AA44" t="s">
         <v>401</v>
       </c>
-      <c r="AA44" t="s">
+      <c r="AB44" t="s">
         <v>251</v>
       </c>
-      <c r="AB44" t="s">
-        <v>237</v>
-      </c>
       <c r="AC44" t="s">
         <v>237</v>
       </c>
@@ -7613,10 +7878,16 @@
         <v>237</v>
       </c>
       <c r="AM44" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN44" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO44" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="45" spans="1:39" ht="18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:41" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>91</v>
       </c>
@@ -7671,7 +7942,7 @@
       <c r="R45" t="s">
         <v>237</v>
       </c>
-      <c r="S45" s="1" t="s">
+      <c r="S45" t="s">
         <v>237</v>
       </c>
       <c r="T45" s="1" t="s">
@@ -7698,7 +7969,7 @@
       <c r="AA45" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AB45" t="s">
+      <c r="AB45" s="1" t="s">
         <v>237</v>
       </c>
       <c r="AC45" t="s">
@@ -7731,11 +8002,17 @@
       <c r="AL45" t="s">
         <v>237</v>
       </c>
-      <c r="AM45" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="46" spans="1:39" ht="18" x14ac:dyDescent="0.2">
+      <c r="AM45" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN45" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO45" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="46" spans="1:41" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>91</v>
       </c>
@@ -7790,21 +8067,21 @@
       <c r="R46" t="s">
         <v>237</v>
       </c>
-      <c r="S46" s="1" t="s">
+      <c r="S46" t="s">
+        <v>237</v>
+      </c>
+      <c r="T46" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="T46" s="1" t="s">
+      <c r="U46" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="U46" t="s">
+      <c r="V46" t="s">
         <v>324</v>
       </c>
-      <c r="V46" t="s">
+      <c r="W46" t="s">
         <v>323</v>
       </c>
-      <c r="W46" s="1" t="s">
-        <v>237</v>
-      </c>
       <c r="X46" s="1" t="s">
         <v>237</v>
       </c>
@@ -7817,7 +8094,7 @@
       <c r="AA46" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AB46" t="s">
+      <c r="AB46" s="1" t="s">
         <v>237</v>
       </c>
       <c r="AC46" t="s">
@@ -7850,11 +8127,17 @@
       <c r="AL46" t="s">
         <v>237</v>
       </c>
-      <c r="AM46" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="47" spans="1:39" ht="18" x14ac:dyDescent="0.2">
+      <c r="AM46" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN46" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO46" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="47" spans="1:41" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
         <v>91</v>
       </c>
@@ -7909,21 +8192,21 @@
       <c r="R47" t="s">
         <v>237</v>
       </c>
-      <c r="S47" s="1" t="s">
+      <c r="S47" t="s">
+        <v>237</v>
+      </c>
+      <c r="T47" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="T47" s="1" t="s">
+      <c r="U47" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="U47" t="s">
+      <c r="V47" t="s">
         <v>326</v>
       </c>
-      <c r="V47" t="s">
+      <c r="W47" t="s">
         <v>325</v>
       </c>
-      <c r="W47" s="1" t="s">
-        <v>237</v>
-      </c>
       <c r="X47" s="1" t="s">
         <v>237</v>
       </c>
@@ -7936,7 +8219,7 @@
       <c r="AA47" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AB47" t="s">
+      <c r="AB47" s="1" t="s">
         <v>237</v>
       </c>
       <c r="AC47" t="s">
@@ -7969,11 +8252,17 @@
       <c r="AL47" t="s">
         <v>237</v>
       </c>
-      <c r="AM47" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="48" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+      <c r="AM47" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN47" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO47" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="48" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>91</v>
       </c>
@@ -8028,7 +8317,7 @@
       <c r="R48" t="s">
         <v>237</v>
       </c>
-      <c r="S48" s="1" t="s">
+      <c r="S48" t="s">
         <v>237</v>
       </c>
       <c r="T48" s="1" t="s">
@@ -8055,7 +8344,7 @@
       <c r="AA48" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AB48" t="s">
+      <c r="AB48" s="1" t="s">
         <v>237</v>
       </c>
       <c r="AC48" t="s">
@@ -8088,11 +8377,17 @@
       <c r="AL48" t="s">
         <v>237</v>
       </c>
-      <c r="AM48" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="49" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+      <c r="AM48" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN48" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO48" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="49" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>91</v>
       </c>
@@ -8147,7 +8442,7 @@
       <c r="R49" t="s">
         <v>237</v>
       </c>
-      <c r="S49" s="1" t="s">
+      <c r="S49" t="s">
         <v>237</v>
       </c>
       <c r="T49" s="1" t="s">
@@ -8174,7 +8469,7 @@
       <c r="AA49" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AB49" t="s">
+      <c r="AB49" s="1" t="s">
         <v>237</v>
       </c>
       <c r="AC49" t="s">
@@ -8207,11 +8502,17 @@
       <c r="AL49" t="s">
         <v>237</v>
       </c>
-      <c r="AM49" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="50" spans="1:39" ht="18" x14ac:dyDescent="0.2">
+      <c r="AM49" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN49" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO49" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="50" spans="1:41" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>91</v>
       </c>
@@ -8266,7 +8567,7 @@
       <c r="R50" t="s">
         <v>237</v>
       </c>
-      <c r="S50" s="1" t="s">
+      <c r="S50" t="s">
         <v>237</v>
       </c>
       <c r="T50" s="1" t="s">
@@ -8293,7 +8594,7 @@
       <c r="AA50" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AB50" t="s">
+      <c r="AB50" s="1" t="s">
         <v>237</v>
       </c>
       <c r="AC50" t="s">
@@ -8326,11 +8627,17 @@
       <c r="AL50" t="s">
         <v>237</v>
       </c>
-      <c r="AM50" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="51" spans="1:39" ht="18" x14ac:dyDescent="0.2">
+      <c r="AM50" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN50" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO50" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="51" spans="1:41" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>108</v>
       </c>
@@ -8385,7 +8692,7 @@
       <c r="R51" t="s">
         <v>237</v>
       </c>
-      <c r="S51" s="1" t="s">
+      <c r="S51" t="s">
         <v>237</v>
       </c>
       <c r="T51" s="1" t="s">
@@ -8412,7 +8719,7 @@
       <c r="AA51" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AB51" t="s">
+      <c r="AB51" s="1" t="s">
         <v>237</v>
       </c>
       <c r="AC51" t="s">
@@ -8445,11 +8752,17 @@
       <c r="AL51" t="s">
         <v>237</v>
       </c>
-      <c r="AM51" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="52" spans="1:39" ht="18" x14ac:dyDescent="0.2">
+      <c r="AM51" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN51" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO51" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="52" spans="1:41" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>108</v>
       </c>
@@ -8504,7 +8817,7 @@
       <c r="R52" t="s">
         <v>237</v>
       </c>
-      <c r="S52" s="1" t="s">
+      <c r="S52" t="s">
         <v>237</v>
       </c>
       <c r="T52" s="1" t="s">
@@ -8516,24 +8829,24 @@
       <c r="V52" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="W52" t="s">
+      <c r="W52" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="X52" t="s">
         <v>306</v>
       </c>
-      <c r="X52" t="s">
+      <c r="Y52" t="s">
         <v>307</v>
       </c>
-      <c r="Y52" s="1" t="s">
+      <c r="Z52" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="Z52" s="9" t="s">
+      <c r="AA52" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="AA52" t="s">
+      <c r="AB52" t="s">
         <v>241</v>
       </c>
-      <c r="AB52" t="s">
-        <v>237</v>
-      </c>
       <c r="AC52" t="s">
         <v>237</v>
       </c>
@@ -8565,10 +8878,16 @@
         <v>237</v>
       </c>
       <c r="AM52" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN52" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO52" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="53" spans="1:39" ht="18" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:41" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>112</v>
       </c>
@@ -8623,7 +8942,7 @@
       <c r="R53" t="s">
         <v>237</v>
       </c>
-      <c r="S53" s="1" t="s">
+      <c r="S53" t="s">
         <v>237</v>
       </c>
       <c r="T53" s="1" t="s">
@@ -8650,7 +8969,7 @@
       <c r="AA53" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AB53" t="s">
+      <c r="AB53" s="1" t="s">
         <v>237</v>
       </c>
       <c r="AC53" t="s">
@@ -8683,11 +9002,17 @@
       <c r="AL53" t="s">
         <v>237</v>
       </c>
-      <c r="AM53" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="54" spans="1:39" ht="18" x14ac:dyDescent="0.2">
+      <c r="AM53" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN53" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO53" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="54" spans="1:41" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>115</v>
       </c>
@@ -8805,8 +9130,14 @@
       <c r="AM54" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="55" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN54" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO54" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="55" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>115</v>
       </c>
@@ -8924,8 +9255,14 @@
       <c r="AM55" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="56" spans="1:39" ht="18" x14ac:dyDescent="0.2">
+      <c r="AN55" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO55" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="56" spans="1:41" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>115</v>
       </c>
@@ -8992,18 +9329,18 @@
       <c r="V56" t="s">
         <v>237</v>
       </c>
-      <c r="W56" s="1" t="s">
+      <c r="W56" t="s">
+        <v>237</v>
+      </c>
+      <c r="X56" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="X56" s="1" t="s">
+      <c r="Y56" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="Y56" s="1" t="s">
+      <c r="Z56" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="Z56" t="s">
-        <v>237</v>
-      </c>
       <c r="AA56" t="s">
         <v>237</v>
       </c>
@@ -9041,6 +9378,12 @@
         <v>237</v>
       </c>
       <c r="AM56" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN56" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO56" t="s">
         <v>248</v>
       </c>
     </row>

</xml_diff>

<commit_message>
dim_item_sets add hts modality items
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10648BF4-47A8-7E4D-A43D-A6DE45C129AF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91A24D4-8F7E-344D-B271-7EF73117DBC5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3529" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3613" uniqueCount="657">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1970,6 +1970,45 @@
   </si>
   <si>
     <t>B.other_disagg_set</t>
+  </si>
+  <si>
+    <t>other_disagg</t>
+  </si>
+  <si>
+    <t>CKTkg8dLlr8</t>
+  </si>
+  <si>
+    <t>CKTkg8dLlr9</t>
+  </si>
+  <si>
+    <t>CKTkg8dLlr10</t>
+  </si>
+  <si>
+    <t>CKTkg8dLlr11</t>
+  </si>
+  <si>
+    <t>CKTkg8dLlr12</t>
+  </si>
+  <si>
+    <t>CKTkg8dLlr13</t>
+  </si>
+  <si>
+    <t>CKTkg8dLlr14</t>
+  </si>
+  <si>
+    <t>CKTkg8dLlr15</t>
+  </si>
+  <si>
+    <t>CKTkg8dLlr16</t>
+  </si>
+  <si>
+    <t>CKTkg8dLlr17</t>
+  </si>
+  <si>
+    <t>CKTkg8dLlr18</t>
+  </si>
+  <si>
+    <t>QJZLPV5BcW</t>
   </si>
 </sst>
 </file>
@@ -1979,7 +2018,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2011,6 +2050,12 @@
       <color rgb="FF1A1AA6"/>
       <name val="Courier New"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2367,10 +2412,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
   <dimension ref="A1:AO56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="AF1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="AD16" sqref="AD16"/>
+      <selection pane="bottomLeft" activeCell="AM17" sqref="AM17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10152,10 +10197,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
-  <dimension ref="A1:AF120"/>
+  <dimension ref="A1:AF132"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A133" sqref="A133:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14807,7 +14852,7 @@
       <c r="I119" s="14">
         <v>1</v>
       </c>
-      <c r="J119" s="4" t="str">
+      <c r="J119" t="str">
         <f>_xlfn.TEXTJOIN(";",1,K119:ZZ119)</f>
         <v>tr_pos2</v>
       </c>
@@ -14843,12 +14888,360 @@
       <c r="I120" s="14">
         <v>1</v>
       </c>
-      <c r="J120" s="4" t="str">
+      <c r="J120" t="str">
         <f t="shared" si="2"/>
         <v>tr_neg2</v>
       </c>
       <c r="Y120" t="s">
         <v>623</v>
+      </c>
+    </row>
+    <row r="121" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>296</v>
+      </c>
+      <c r="B121" t="s">
+        <v>406</v>
+      </c>
+      <c r="C121" t="s">
+        <v>426</v>
+      </c>
+      <c r="D121" t="s">
+        <v>644</v>
+      </c>
+      <c r="E121" t="s">
+        <v>425</v>
+      </c>
+      <c r="F121" t="s">
+        <v>425</v>
+      </c>
+      <c r="G121" t="s">
+        <v>426</v>
+      </c>
+      <c r="H121">
+        <v>100</v>
+      </c>
+      <c r="I121" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>645</v>
+      </c>
+      <c r="B122" t="s">
+        <v>406</v>
+      </c>
+      <c r="C122" t="s">
+        <v>428</v>
+      </c>
+      <c r="D122" t="s">
+        <v>644</v>
+      </c>
+      <c r="E122" t="s">
+        <v>427</v>
+      </c>
+      <c r="F122" t="s">
+        <v>427</v>
+      </c>
+      <c r="G122" t="s">
+        <v>428</v>
+      </c>
+      <c r="H122">
+        <v>200</v>
+      </c>
+      <c r="I122" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>646</v>
+      </c>
+      <c r="B123" t="s">
+        <v>406</v>
+      </c>
+      <c r="C123" t="s">
+        <v>253</v>
+      </c>
+      <c r="D123" t="s">
+        <v>644</v>
+      </c>
+      <c r="E123" t="s">
+        <v>435</v>
+      </c>
+      <c r="F123" t="s">
+        <v>435</v>
+      </c>
+      <c r="G123" t="s">
+        <v>253</v>
+      </c>
+      <c r="H123">
+        <v>300</v>
+      </c>
+      <c r="I123" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>647</v>
+      </c>
+      <c r="B124" t="s">
+        <v>406</v>
+      </c>
+      <c r="C124" t="s">
+        <v>261</v>
+      </c>
+      <c r="D124" t="s">
+        <v>644</v>
+      </c>
+      <c r="E124" t="s">
+        <v>436</v>
+      </c>
+      <c r="F124" t="s">
+        <v>436</v>
+      </c>
+      <c r="G124" t="s">
+        <v>261</v>
+      </c>
+      <c r="H124">
+        <v>400</v>
+      </c>
+      <c r="I124" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>648</v>
+      </c>
+      <c r="B125" t="s">
+        <v>406</v>
+      </c>
+      <c r="C125" t="s">
+        <v>268</v>
+      </c>
+      <c r="D125" t="s">
+        <v>644</v>
+      </c>
+      <c r="E125" t="s">
+        <v>437</v>
+      </c>
+      <c r="F125" t="s">
+        <v>437</v>
+      </c>
+      <c r="G125" t="s">
+        <v>268</v>
+      </c>
+      <c r="H125">
+        <v>500</v>
+      </c>
+      <c r="I125" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>649</v>
+      </c>
+      <c r="B126" t="s">
+        <v>406</v>
+      </c>
+      <c r="C126" t="s">
+        <v>263</v>
+      </c>
+      <c r="D126" t="s">
+        <v>644</v>
+      </c>
+      <c r="E126" t="s">
+        <v>438</v>
+      </c>
+      <c r="F126" t="s">
+        <v>438</v>
+      </c>
+      <c r="G126" t="s">
+        <v>263</v>
+      </c>
+      <c r="H126">
+        <v>600</v>
+      </c>
+      <c r="I126" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>650</v>
+      </c>
+      <c r="B127" t="s">
+        <v>406</v>
+      </c>
+      <c r="C127" t="s">
+        <v>264</v>
+      </c>
+      <c r="D127" t="s">
+        <v>644</v>
+      </c>
+      <c r="E127" t="s">
+        <v>439</v>
+      </c>
+      <c r="F127" t="s">
+        <v>439</v>
+      </c>
+      <c r="G127" t="s">
+        <v>264</v>
+      </c>
+      <c r="H127">
+        <v>700</v>
+      </c>
+      <c r="I127" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>651</v>
+      </c>
+      <c r="B128" t="s">
+        <v>406</v>
+      </c>
+      <c r="C128" t="s">
+        <v>265</v>
+      </c>
+      <c r="D128" t="s">
+        <v>644</v>
+      </c>
+      <c r="E128" t="s">
+        <v>440</v>
+      </c>
+      <c r="F128" t="s">
+        <v>440</v>
+      </c>
+      <c r="G128" t="s">
+        <v>265</v>
+      </c>
+      <c r="H128">
+        <v>800</v>
+      </c>
+      <c r="I128" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>652</v>
+      </c>
+      <c r="B129" t="s">
+        <v>406</v>
+      </c>
+      <c r="C129" t="s">
+        <v>266</v>
+      </c>
+      <c r="D129" t="s">
+        <v>644</v>
+      </c>
+      <c r="E129" t="s">
+        <v>441</v>
+      </c>
+      <c r="F129" t="s">
+        <v>441</v>
+      </c>
+      <c r="G129" t="s">
+        <v>266</v>
+      </c>
+      <c r="H129">
+        <v>900</v>
+      </c>
+      <c r="I129" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>653</v>
+      </c>
+      <c r="B130" t="s">
+        <v>406</v>
+      </c>
+      <c r="C130" t="s">
+        <v>267</v>
+      </c>
+      <c r="D130" t="s">
+        <v>644</v>
+      </c>
+      <c r="E130" t="s">
+        <v>442</v>
+      </c>
+      <c r="F130" t="s">
+        <v>442</v>
+      </c>
+      <c r="G130" t="s">
+        <v>656</v>
+      </c>
+      <c r="H130">
+        <v>1000</v>
+      </c>
+      <c r="I130" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>654</v>
+      </c>
+      <c r="B131" t="s">
+        <v>406</v>
+      </c>
+      <c r="C131" t="s">
+        <v>262</v>
+      </c>
+      <c r="D131" t="s">
+        <v>644</v>
+      </c>
+      <c r="E131" t="s">
+        <v>443</v>
+      </c>
+      <c r="F131" t="s">
+        <v>443</v>
+      </c>
+      <c r="G131" t="s">
+        <v>267</v>
+      </c>
+      <c r="H131">
+        <v>1100</v>
+      </c>
+      <c r="I131" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>655</v>
+      </c>
+      <c r="B132" t="s">
+        <v>406</v>
+      </c>
+      <c r="C132" t="s">
+        <v>269</v>
+      </c>
+      <c r="D132" t="s">
+        <v>644</v>
+      </c>
+      <c r="E132" t="s">
+        <v>444</v>
+      </c>
+      <c r="F132" t="s">
+        <v>444</v>
+      </c>
+      <c r="G132" t="s">
+        <v>269</v>
+      </c>
+      <c r="H132">
+        <v>1200</v>
+      </c>
+      <c r="I132" s="14">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -14856,6 +15249,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:W61">
     <sortCondition ref="H4:H61"/>
   </sortState>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
dim_item_sets add model_sets for hts_mod
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91A24D4-8F7E-344D-B271-7EF73117DBC5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2533019B-757C-6047-AC8C-198A1DBBDA8A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3613" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3626" uniqueCount="670">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -2009,6 +2009,45 @@
   </si>
   <si>
     <t>QJZLPV5BcW</t>
+  </si>
+  <si>
+    <t>hts_mod</t>
+  </si>
+  <si>
+    <t>hts_mod_com_mob</t>
+  </si>
+  <si>
+    <t>hts_mod_com_ndx</t>
+  </si>
+  <si>
+    <t>hts_mod_fac_ndx</t>
+  </si>
+  <si>
+    <t>hts_mod_com_vct</t>
+  </si>
+  <si>
+    <t>hts_mod_com_otr</t>
+  </si>
+  <si>
+    <t>hts_mod_fac_ew</t>
+  </si>
+  <si>
+    <t>hts_mod_fac_inpat</t>
+  </si>
+  <si>
+    <t>hts_mod_fac_nut</t>
+  </si>
+  <si>
+    <t>hts_mod_fac_ped</t>
+  </si>
+  <si>
+    <t>hts_mod_fac_sti</t>
+  </si>
+  <si>
+    <t>hts_mod_fac_vct</t>
+  </si>
+  <si>
+    <t>hts_mod_fac_otr_pitc</t>
   </si>
 </sst>
 </file>
@@ -10197,10 +10236,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
-  <dimension ref="A1:AF132"/>
+  <dimension ref="A1:AG132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A133" sqref="A133:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="AG102" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="F1" sqref="F1"/>
+      <selection pane="topRight" activeCell="K1" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="AG121" sqref="AG121:AG124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10219,7 +10262,7 @@
     <col min="19" max="19" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>388</v>
       </c>
@@ -10316,8 +10359,11 @@
       <c r="AF1" t="s">
         <v>610</v>
       </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG1" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>293</v>
       </c>
@@ -10346,7 +10392,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="4" t="str">
-        <f t="shared" ref="J2:J33" si="0">_xlfn.TEXTJOIN(";",1,K2:ZZ2)</f>
+        <f>_xlfn.TEXTJOIN(";",1,K2:ZZ2)</f>
         <v>&lt;2mo</v>
       </c>
       <c r="K2" s="9"/>
@@ -10361,7 +10407,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>293</v>
       </c>
@@ -10390,7 +10436,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="J2:J33" si="0">_xlfn.TEXTJOIN(";",1,K3:ZZ3)</f>
         <v>2-12mo</v>
       </c>
       <c r="K3" s="9"/>
@@ -10405,7 +10451,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>293</v>
       </c>
@@ -10447,7 +10493,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>293</v>
       </c>
@@ -10484,7 +10530,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>293</v>
       </c>
@@ -10517,7 +10563,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>293</v>
       </c>
@@ -10567,7 +10613,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>293</v>
       </c>
@@ -10603,7 +10649,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>293</v>
       </c>
@@ -10642,7 +10688,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>293</v>
       </c>
@@ -10689,7 +10735,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>293</v>
       </c>
@@ -10725,7 +10771,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>293</v>
       </c>
@@ -10777,7 +10823,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>293</v>
       </c>
@@ -10813,7 +10859,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>237</v>
       </c>
@@ -10855,7 +10901,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="15" spans="1:32" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:33" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>293</v>
       </c>
@@ -10893,7 +10939,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>237</v>
       </c>
@@ -12945,7 +12991,7 @@
         <v>1</v>
       </c>
       <c r="J66" s="4" t="str">
-        <f t="shared" ref="J66:J120" si="2">_xlfn.TEXTJOIN(";",1,K66:ZZ66)</f>
+        <f t="shared" ref="J66:J129" si="2">_xlfn.TEXTJOIN(";",1,K66:ZZ66)</f>
         <v>tss_NewNeg</v>
       </c>
       <c r="AB66" t="s">
@@ -14608,7 +14654,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="113" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>486</v>
       </c>
@@ -14644,7 +14690,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="114" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>486</v>
       </c>
@@ -14680,7 +14726,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="115" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>486</v>
       </c>
@@ -14716,7 +14762,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="116" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>486</v>
       </c>
@@ -14752,7 +14798,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="117" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>486</v>
       </c>
@@ -14788,7 +14834,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="118" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>486</v>
       </c>
@@ -14824,7 +14870,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="119" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>321</v>
       </c>
@@ -14860,7 +14906,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="120" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>321</v>
       </c>
@@ -14896,7 +14942,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="121" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>296</v>
       </c>
@@ -14924,8 +14970,15 @@
       <c r="I121" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="J121" t="str">
+        <f t="shared" si="2"/>
+        <v>hts_mod_com_ndx</v>
+      </c>
+      <c r="AG121" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="122" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>645</v>
       </c>
@@ -14953,8 +15006,15 @@
       <c r="I122" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="J122" t="str">
+        <f t="shared" si="2"/>
+        <v>hts_mod_fac_ndx</v>
+      </c>
+      <c r="AG122" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="123" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>646</v>
       </c>
@@ -14982,8 +15042,15 @@
       <c r="I123" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="124" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="J123" t="str">
+        <f t="shared" si="2"/>
+        <v>hts_mod_com_mob</v>
+      </c>
+      <c r="AG123" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="124" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>647</v>
       </c>
@@ -15011,8 +15078,15 @@
       <c r="I124" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="J124" t="str">
+        <f t="shared" si="2"/>
+        <v>hts_mod_com_vct</v>
+      </c>
+      <c r="AG124" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="125" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>648</v>
       </c>
@@ -15040,8 +15114,15 @@
       <c r="I125" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="126" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="J125" t="str">
+        <f t="shared" si="2"/>
+        <v>hts_mod_com_otr</v>
+      </c>
+      <c r="AG125" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="126" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>649</v>
       </c>
@@ -15069,8 +15150,15 @@
       <c r="I126" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="127" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="J126" t="str">
+        <f t="shared" si="2"/>
+        <v>hts_mod_fac_ew</v>
+      </c>
+      <c r="AG126" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="127" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>650</v>
       </c>
@@ -15098,8 +15186,15 @@
       <c r="I127" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="128" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="J127" t="str">
+        <f t="shared" si="2"/>
+        <v>hts_mod_fac_inpat</v>
+      </c>
+      <c r="AG127" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="128" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>651</v>
       </c>
@@ -15127,8 +15222,15 @@
       <c r="I128" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J128" t="str">
+        <f t="shared" si="2"/>
+        <v>hts_mod_fac_nut</v>
+      </c>
+      <c r="AG128" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="129" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>652</v>
       </c>
@@ -15156,8 +15258,15 @@
       <c r="I129" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J129" t="str">
+        <f t="shared" si="2"/>
+        <v>hts_mod_fac_ped</v>
+      </c>
+      <c r="AG129" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="130" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>653</v>
       </c>
@@ -15185,8 +15294,15 @@
       <c r="I130" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J130" t="str">
+        <f t="shared" ref="J130:J132" si="3">_xlfn.TEXTJOIN(";",1,K130:ZZ130)</f>
+        <v>hts_mod_fac_sti</v>
+      </c>
+      <c r="AG130" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="131" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>654</v>
       </c>
@@ -15214,8 +15330,15 @@
       <c r="I131" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J131" t="str">
+        <f t="shared" si="3"/>
+        <v>hts_mod_fac_vct</v>
+      </c>
+      <c r="AG131" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="132" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>655</v>
       </c>
@@ -15242,6 +15365,13 @@
       </c>
       <c r="I132" s="14">
         <v>1</v>
+      </c>
+      <c r="J132" t="str">
+        <f t="shared" si="3"/>
+        <v>hts_mod_fac_otr_pitc</v>
+      </c>
+      <c r="AG132" t="s">
+        <v>669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dara_required.csv add hts_mod disagg sets
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2533019B-757C-6047-AC8C-198A1DBBDA8A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF9B4DE-EECE-6543-85E9-F70EBBFFA1E1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -2451,10 +2451,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
   <dimension ref="A1:AO56"/>
   <sheetViews>
-    <sheetView topLeftCell="AF1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="AM17" sqref="AM17"/>
+      <selection pane="bottomLeft" activeCell="V29" sqref="V29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2466,7 +2466,8 @@
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
     <col min="7" max="7" width="68.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="21" width="17.33203125" customWidth="1"/>
+    <col min="8" max="13" width="17.33203125" customWidth="1"/>
+    <col min="14" max="21" width="17.33203125" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="53.1640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="24" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="46.83203125" bestFit="1" customWidth="1"/>
@@ -4262,7 +4263,7 @@
         <v>237</v>
       </c>
       <c r="M15" t="s">
-        <v>237</v>
+        <v>659</v>
       </c>
       <c r="N15" t="s">
         <v>237</v>
@@ -4387,7 +4388,7 @@
         <v>237</v>
       </c>
       <c r="M16" t="s">
-        <v>237</v>
+        <v>660</v>
       </c>
       <c r="N16" t="s">
         <v>237</v>
@@ -4509,7 +4510,7 @@
         <v>237</v>
       </c>
       <c r="M17" t="s">
-        <v>237</v>
+        <v>659</v>
       </c>
       <c r="N17" t="s">
         <v>237</v>
@@ -4634,7 +4635,7 @@
         <v>237</v>
       </c>
       <c r="M18" t="s">
-        <v>237</v>
+        <v>658</v>
       </c>
       <c r="N18" t="s">
         <v>237</v>
@@ -4759,7 +4760,7 @@
         <v>237</v>
       </c>
       <c r="M19" t="s">
-        <v>237</v>
+        <v>661</v>
       </c>
       <c r="N19" t="s">
         <v>237</v>
@@ -4884,7 +4885,7 @@
         <v>237</v>
       </c>
       <c r="M20" t="s">
-        <v>237</v>
+        <v>662</v>
       </c>
       <c r="N20" t="s">
         <v>237</v>
@@ -5009,7 +5010,7 @@
         <v>237</v>
       </c>
       <c r="M21" t="s">
-        <v>237</v>
+        <v>663</v>
       </c>
       <c r="N21" t="s">
         <v>237</v>
@@ -5134,7 +5135,7 @@
         <v>237</v>
       </c>
       <c r="M22" t="s">
-        <v>237</v>
+        <v>664</v>
       </c>
       <c r="N22" t="s">
         <v>237</v>
@@ -5259,7 +5260,7 @@
         <v>237</v>
       </c>
       <c r="M23" t="s">
-        <v>237</v>
+        <v>665</v>
       </c>
       <c r="N23" t="s">
         <v>237</v>
@@ -5384,7 +5385,7 @@
         <v>237</v>
       </c>
       <c r="M24" t="s">
-        <v>237</v>
+        <v>666</v>
       </c>
       <c r="N24" t="s">
         <v>237</v>
@@ -5509,7 +5510,7 @@
         <v>237</v>
       </c>
       <c r="M25" t="s">
-        <v>237</v>
+        <v>667</v>
       </c>
       <c r="N25" t="s">
         <v>237</v>
@@ -5634,7 +5635,7 @@
         <v>237</v>
       </c>
       <c r="M26" t="s">
-        <v>237</v>
+        <v>668</v>
       </c>
       <c r="N26" t="s">
         <v>237</v>
@@ -5759,7 +5760,7 @@
         <v>237</v>
       </c>
       <c r="M27" t="s">
-        <v>237</v>
+        <v>669</v>
       </c>
       <c r="N27" t="s">
         <v>237</v>
@@ -5884,7 +5885,7 @@
         <v>237</v>
       </c>
       <c r="M28" t="s">
-        <v>237</v>
+        <v>658</v>
       </c>
       <c r="N28" t="s">
         <v>237</v>
@@ -6009,7 +6010,7 @@
         <v>237</v>
       </c>
       <c r="M29" t="s">
-        <v>237</v>
+        <v>661</v>
       </c>
       <c r="N29" t="s">
         <v>237</v>
@@ -6134,7 +6135,7 @@
         <v>237</v>
       </c>
       <c r="M30" t="s">
-        <v>237</v>
+        <v>662</v>
       </c>
       <c r="N30" t="s">
         <v>237</v>
@@ -6259,7 +6260,7 @@
         <v>237</v>
       </c>
       <c r="M31" t="s">
-        <v>237</v>
+        <v>663</v>
       </c>
       <c r="N31" t="s">
         <v>237</v>
@@ -6384,7 +6385,7 @@
         <v>237</v>
       </c>
       <c r="M32" t="s">
-        <v>237</v>
+        <v>664</v>
       </c>
       <c r="N32" t="s">
         <v>237</v>
@@ -6509,7 +6510,7 @@
         <v>237</v>
       </c>
       <c r="M33" t="s">
-        <v>237</v>
+        <v>665</v>
       </c>
       <c r="N33" t="s">
         <v>237</v>
@@ -6634,7 +6635,7 @@
         <v>237</v>
       </c>
       <c r="M34" t="s">
-        <v>237</v>
+        <v>666</v>
       </c>
       <c r="N34" t="s">
         <v>237</v>
@@ -6759,7 +6760,7 @@
         <v>237</v>
       </c>
       <c r="M35" t="s">
-        <v>237</v>
+        <v>667</v>
       </c>
       <c r="N35" t="s">
         <v>237</v>
@@ -6884,7 +6885,7 @@
         <v>237</v>
       </c>
       <c r="M36" t="s">
-        <v>237</v>
+        <v>668</v>
       </c>
       <c r="N36" t="s">
         <v>237</v>
@@ -7009,7 +7010,7 @@
         <v>237</v>
       </c>
       <c r="M37" t="s">
-        <v>237</v>
+        <v>669</v>
       </c>
       <c r="N37" t="s">
         <v>237</v>
@@ -10238,12 +10239,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
   <dimension ref="A1:AG132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="AG102" activePane="bottomRight" state="frozen"/>
+    <sheetView topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="AG101" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
-      <selection pane="bottomRight" activeCell="AG121" sqref="AG121:AG124"/>
+      <selection pane="bottomRight" activeCell="AG121" sqref="AG121:AG132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10436,7 +10437,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="4" t="str">
-        <f t="shared" ref="J2:J33" si="0">_xlfn.TEXTJOIN(";",1,K3:ZZ3)</f>
+        <f t="shared" ref="J3:J33" si="0">_xlfn.TEXTJOIN(";",1,K3:ZZ3)</f>
         <v>2-12mo</v>
       </c>
       <c r="K3" s="9"/>

</xml_diff>

<commit_message>
data required one more hts_mod disagg set
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF9B4DE-EECE-6543-85E9-F70EBBFFA1E1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52154360-5E54-604C-B5A9-9AD14949C725}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
@@ -2451,10 +2451,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
   <dimension ref="A1:AO56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="V29" sqref="V29"/>
+      <selection pane="bottomLeft" activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4561,7 +4561,7 @@
         <v>237</v>
       </c>
       <c r="AD17" t="s">
-        <v>237</v>
+        <v>660</v>
       </c>
       <c r="AE17" t="s">
         <v>237</v>

</xml_diff>

<commit_message>
data_required add other_disagg_set test results
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52154360-5E54-604C-B5A9-9AD14949C725}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA239FA6-084D-8C4B-B40C-4D225BB697D3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
@@ -2451,10 +2451,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
   <dimension ref="A1:AO56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="L17" sqref="L17"/>
+      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8135,7 +8135,7 @@
         <v>320</v>
       </c>
       <c r="M46" t="s">
-        <v>237</v>
+        <v>568</v>
       </c>
       <c r="N46" t="s">
         <v>237</v>
@@ -8260,7 +8260,7 @@
         <v>320</v>
       </c>
       <c r="M47" t="s">
-        <v>237</v>
+        <v>569</v>
       </c>
       <c r="N47" t="s">
         <v>237</v>
@@ -10239,12 +10239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
   <dimension ref="A1:AG132"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="AG101" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="F1" sqref="F1"/>
-      <selection pane="topRight" activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
-      <selection pane="bottomRight" activeCell="AG121" sqref="AG121:AG132"/>
+    <sheetView topLeftCell="K44" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="Y62" sqref="Y62:Y63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
data_required.csv add config rows for hard coded indicators
kp_prev, prep_new, and impatt.priority_snu
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA239FA6-084D-8C4B-B40C-4D225BB697D3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7573CF30-6594-B349-956C-1FDC692C789B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="33620" yWindow="460" windowWidth="25600" windowHeight="20020" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3626" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3743" uniqueCount="675">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -2048,6 +2048,21 @@
   </si>
   <si>
     <t>hts_mod_fac_otr_pitc</t>
+  </si>
+  <si>
+    <t>DE_GROUP-zhdJiWlPvCz</t>
+  </si>
+  <si>
+    <t>IMPATT.PRIORITY_SNU.19T</t>
+  </si>
+  <si>
+    <t>Prioritization</t>
+  </si>
+  <si>
+    <t>r4zbW3owX9n</t>
+  </si>
+  <si>
+    <t>2018Q4</t>
   </si>
 </sst>
 </file>
@@ -2057,7 +2072,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2096,6 +2111,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2117,7 +2138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -2135,6 +2156,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2449,12 +2471,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
-  <dimension ref="A1:AO56"/>
+  <dimension ref="A1:AO59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2466,7 +2488,8 @@
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
     <col min="7" max="7" width="68.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="17.33203125" customWidth="1"/>
     <col min="14" max="21" width="17.33203125" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="53.1640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="24" bestFit="1" customWidth="1"/>
@@ -9470,6 +9493,363 @@
       </c>
       <c r="AO56" t="s">
         <v>248</v>
+      </c>
+    </row>
+    <row r="57" spans="1:41" ht="18" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>91</v>
+      </c>
+      <c r="B57" t="s">
+        <v>106</v>
+      </c>
+      <c r="C57" t="s">
+        <v>2</v>
+      </c>
+      <c r="E57" t="s">
+        <v>4</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="H57" s="15" t="s">
+        <v>670</v>
+      </c>
+      <c r="I57" t="s">
+        <v>232</v>
+      </c>
+      <c r="J57" t="s">
+        <v>237</v>
+      </c>
+      <c r="K57" t="s">
+        <v>237</v>
+      </c>
+      <c r="L57" t="s">
+        <v>609</v>
+      </c>
+      <c r="M57" t="s">
+        <v>237</v>
+      </c>
+      <c r="N57" t="s">
+        <v>237</v>
+      </c>
+      <c r="O57" t="s">
+        <v>237</v>
+      </c>
+      <c r="P57" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>237</v>
+      </c>
+      <c r="R57" t="s">
+        <v>237</v>
+      </c>
+      <c r="S57" t="s">
+        <v>237</v>
+      </c>
+      <c r="T57" t="s">
+        <v>237</v>
+      </c>
+      <c r="U57" t="s">
+        <v>237</v>
+      </c>
+      <c r="V57" t="s">
+        <v>237</v>
+      </c>
+      <c r="W57" t="s">
+        <v>237</v>
+      </c>
+      <c r="X57" t="s">
+        <v>237</v>
+      </c>
+      <c r="Y57" t="s">
+        <v>237</v>
+      </c>
+      <c r="Z57" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA57" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB57" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC57" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD57" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE57" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF57" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG57" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH57" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI57" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ57" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK57" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL57" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM57" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN57" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO57" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="58" spans="1:41" ht="18" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>91</v>
+      </c>
+      <c r="B58" t="s">
+        <v>92</v>
+      </c>
+      <c r="C58" t="s">
+        <v>2</v>
+      </c>
+      <c r="E58" t="s">
+        <v>4</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="H58" s="15" t="s">
+        <v>670</v>
+      </c>
+      <c r="I58" t="s">
+        <v>232</v>
+      </c>
+      <c r="J58" t="s">
+        <v>237</v>
+      </c>
+      <c r="K58" t="s">
+        <v>237</v>
+      </c>
+      <c r="L58" t="s">
+        <v>578</v>
+      </c>
+      <c r="M58" t="s">
+        <v>237</v>
+      </c>
+      <c r="N58" t="s">
+        <v>237</v>
+      </c>
+      <c r="O58" t="s">
+        <v>237</v>
+      </c>
+      <c r="P58" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>237</v>
+      </c>
+      <c r="R58" t="s">
+        <v>237</v>
+      </c>
+      <c r="S58" t="s">
+        <v>237</v>
+      </c>
+      <c r="T58" t="s">
+        <v>237</v>
+      </c>
+      <c r="U58" t="s">
+        <v>237</v>
+      </c>
+      <c r="V58" t="s">
+        <v>237</v>
+      </c>
+      <c r="W58" t="s">
+        <v>237</v>
+      </c>
+      <c r="X58" t="s">
+        <v>237</v>
+      </c>
+      <c r="Y58" t="s">
+        <v>237</v>
+      </c>
+      <c r="Z58" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA58" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB58" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC58" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD58" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE58" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF58" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG58" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH58" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI58" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ58" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK58" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL58" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM58" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN58" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO58" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="59" spans="1:41" ht="18" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>672</v>
+      </c>
+      <c r="B59" t="s">
+        <v>671</v>
+      </c>
+      <c r="C59" t="s">
+        <v>2</v>
+      </c>
+      <c r="E59" t="s">
+        <v>4</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="H59" t="s">
+        <v>673</v>
+      </c>
+      <c r="I59" t="s">
+        <v>674</v>
+      </c>
+      <c r="J59" t="s">
+        <v>237</v>
+      </c>
+      <c r="K59" t="s">
+        <v>237</v>
+      </c>
+      <c r="L59" t="s">
+        <v>237</v>
+      </c>
+      <c r="M59" t="s">
+        <v>237</v>
+      </c>
+      <c r="N59" t="s">
+        <v>237</v>
+      </c>
+      <c r="O59" t="s">
+        <v>237</v>
+      </c>
+      <c r="P59" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>237</v>
+      </c>
+      <c r="R59" t="s">
+        <v>237</v>
+      </c>
+      <c r="S59" t="s">
+        <v>237</v>
+      </c>
+      <c r="T59" t="s">
+        <v>237</v>
+      </c>
+      <c r="U59" t="s">
+        <v>237</v>
+      </c>
+      <c r="V59" t="s">
+        <v>237</v>
+      </c>
+      <c r="W59" t="s">
+        <v>237</v>
+      </c>
+      <c r="X59" t="s">
+        <v>237</v>
+      </c>
+      <c r="Y59" t="s">
+        <v>237</v>
+      </c>
+      <c r="Z59" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA59" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB59" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC59" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD59" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE59" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF59" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG59" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH59" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI59" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ59" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK59" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL59" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM59" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN59" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO59" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -10239,8 +10619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
   <dimension ref="A1:AG132"/>
   <sheetViews>
-    <sheetView topLeftCell="K44" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="Y62" sqref="Y62:Y63"/>
+    <sheetView topLeftCell="C97" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Dimension Item Sets fix copy paste error in uid
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7573CF30-6594-B349-956C-1FDC692C789B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A97237E-28A3-504A-AAD0-C83FF076B752}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33620" yWindow="460" windowWidth="25600" windowHeight="20020" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3743" uniqueCount="675">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3743" uniqueCount="664">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1973,39 +1973,6 @@
   </si>
   <si>
     <t>other_disagg</t>
-  </si>
-  <si>
-    <t>CKTkg8dLlr8</t>
-  </si>
-  <si>
-    <t>CKTkg8dLlr9</t>
-  </si>
-  <si>
-    <t>CKTkg8dLlr10</t>
-  </si>
-  <si>
-    <t>CKTkg8dLlr11</t>
-  </si>
-  <si>
-    <t>CKTkg8dLlr12</t>
-  </si>
-  <si>
-    <t>CKTkg8dLlr13</t>
-  </si>
-  <si>
-    <t>CKTkg8dLlr14</t>
-  </si>
-  <si>
-    <t>CKTkg8dLlr15</t>
-  </si>
-  <si>
-    <t>CKTkg8dLlr16</t>
-  </si>
-  <si>
-    <t>CKTkg8dLlr17</t>
-  </si>
-  <si>
-    <t>CKTkg8dLlr18</t>
   </si>
   <si>
     <t>QJZLPV5BcW</t>
@@ -2473,8 +2440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
   <dimension ref="A1:AO59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
     </sheetView>
@@ -4286,7 +4253,7 @@
         <v>237</v>
       </c>
       <c r="M15" t="s">
-        <v>659</v>
+        <v>648</v>
       </c>
       <c r="N15" t="s">
         <v>237</v>
@@ -4411,7 +4378,7 @@
         <v>237</v>
       </c>
       <c r="M16" t="s">
-        <v>660</v>
+        <v>649</v>
       </c>
       <c r="N16" t="s">
         <v>237</v>
@@ -4533,7 +4500,7 @@
         <v>237</v>
       </c>
       <c r="M17" t="s">
-        <v>659</v>
+        <v>648</v>
       </c>
       <c r="N17" t="s">
         <v>237</v>
@@ -4584,7 +4551,7 @@
         <v>237</v>
       </c>
       <c r="AD17" t="s">
-        <v>660</v>
+        <v>649</v>
       </c>
       <c r="AE17" t="s">
         <v>237</v>
@@ -4658,7 +4625,7 @@
         <v>237</v>
       </c>
       <c r="M18" t="s">
-        <v>658</v>
+        <v>647</v>
       </c>
       <c r="N18" t="s">
         <v>237</v>
@@ -4783,7 +4750,7 @@
         <v>237</v>
       </c>
       <c r="M19" t="s">
-        <v>661</v>
+        <v>650</v>
       </c>
       <c r="N19" t="s">
         <v>237</v>
@@ -4908,7 +4875,7 @@
         <v>237</v>
       </c>
       <c r="M20" t="s">
-        <v>662</v>
+        <v>651</v>
       </c>
       <c r="N20" t="s">
         <v>237</v>
@@ -5033,7 +5000,7 @@
         <v>237</v>
       </c>
       <c r="M21" t="s">
-        <v>663</v>
+        <v>652</v>
       </c>
       <c r="N21" t="s">
         <v>237</v>
@@ -5158,7 +5125,7 @@
         <v>237</v>
       </c>
       <c r="M22" t="s">
-        <v>664</v>
+        <v>653</v>
       </c>
       <c r="N22" t="s">
         <v>237</v>
@@ -5283,7 +5250,7 @@
         <v>237</v>
       </c>
       <c r="M23" t="s">
-        <v>665</v>
+        <v>654</v>
       </c>
       <c r="N23" t="s">
         <v>237</v>
@@ -5408,7 +5375,7 @@
         <v>237</v>
       </c>
       <c r="M24" t="s">
-        <v>666</v>
+        <v>655</v>
       </c>
       <c r="N24" t="s">
         <v>237</v>
@@ -5533,7 +5500,7 @@
         <v>237</v>
       </c>
       <c r="M25" t="s">
-        <v>667</v>
+        <v>656</v>
       </c>
       <c r="N25" t="s">
         <v>237</v>
@@ -5658,7 +5625,7 @@
         <v>237</v>
       </c>
       <c r="M26" t="s">
-        <v>668</v>
+        <v>657</v>
       </c>
       <c r="N26" t="s">
         <v>237</v>
@@ -5783,7 +5750,7 @@
         <v>237</v>
       </c>
       <c r="M27" t="s">
-        <v>669</v>
+        <v>658</v>
       </c>
       <c r="N27" t="s">
         <v>237</v>
@@ -5908,7 +5875,7 @@
         <v>237</v>
       </c>
       <c r="M28" t="s">
-        <v>658</v>
+        <v>647</v>
       </c>
       <c r="N28" t="s">
         <v>237</v>
@@ -6033,7 +6000,7 @@
         <v>237</v>
       </c>
       <c r="M29" t="s">
-        <v>661</v>
+        <v>650</v>
       </c>
       <c r="N29" t="s">
         <v>237</v>
@@ -6158,7 +6125,7 @@
         <v>237</v>
       </c>
       <c r="M30" t="s">
-        <v>662</v>
+        <v>651</v>
       </c>
       <c r="N30" t="s">
         <v>237</v>
@@ -6283,7 +6250,7 @@
         <v>237</v>
       </c>
       <c r="M31" t="s">
-        <v>663</v>
+        <v>652</v>
       </c>
       <c r="N31" t="s">
         <v>237</v>
@@ -6408,7 +6375,7 @@
         <v>237</v>
       </c>
       <c r="M32" t="s">
-        <v>664</v>
+        <v>653</v>
       </c>
       <c r="N32" t="s">
         <v>237</v>
@@ -6533,7 +6500,7 @@
         <v>237</v>
       </c>
       <c r="M33" t="s">
-        <v>665</v>
+        <v>654</v>
       </c>
       <c r="N33" t="s">
         <v>237</v>
@@ -6658,7 +6625,7 @@
         <v>237</v>
       </c>
       <c r="M34" t="s">
-        <v>666</v>
+        <v>655</v>
       </c>
       <c r="N34" t="s">
         <v>237</v>
@@ -6783,7 +6750,7 @@
         <v>237</v>
       </c>
       <c r="M35" t="s">
-        <v>667</v>
+        <v>656</v>
       </c>
       <c r="N35" t="s">
         <v>237</v>
@@ -6908,7 +6875,7 @@
         <v>237</v>
       </c>
       <c r="M36" t="s">
-        <v>668</v>
+        <v>657</v>
       </c>
       <c r="N36" t="s">
         <v>237</v>
@@ -7033,7 +7000,7 @@
         <v>237</v>
       </c>
       <c r="M37" t="s">
-        <v>669</v>
+        <v>658</v>
       </c>
       <c r="N37" t="s">
         <v>237</v>
@@ -9512,7 +9479,7 @@
         <v>237</v>
       </c>
       <c r="H57" s="15" t="s">
-        <v>670</v>
+        <v>659</v>
       </c>
       <c r="I57" t="s">
         <v>232</v>
@@ -9631,7 +9598,7 @@
         <v>237</v>
       </c>
       <c r="H58" s="15" t="s">
-        <v>670</v>
+        <v>659</v>
       </c>
       <c r="I58" t="s">
         <v>232</v>
@@ -9735,10 +9702,10 @@
     </row>
     <row r="59" spans="1:41" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>672</v>
+        <v>661</v>
       </c>
       <c r="B59" t="s">
-        <v>671</v>
+        <v>660</v>
       </c>
       <c r="C59" t="s">
         <v>2</v>
@@ -9750,10 +9717,10 @@
         <v>237</v>
       </c>
       <c r="H59" t="s">
-        <v>673</v>
+        <v>662</v>
       </c>
       <c r="I59" t="s">
-        <v>674</v>
+        <v>663</v>
       </c>
       <c r="J59" t="s">
         <v>237</v>
@@ -10619,14 +10586,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
   <dimension ref="A1:AG132"/>
   <sheetViews>
-    <sheetView topLeftCell="C97" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C101" sqref="C101"/>
+    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C120" sqref="C120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.83203125" customWidth="1"/>
     <col min="5" max="5" width="52.33203125" bestFit="1" customWidth="1"/>
@@ -10737,7 +10704,7 @@
         <v>610</v>
       </c>
       <c r="AG1" t="s">
-        <v>657</v>
+        <v>646</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
@@ -15352,12 +15319,12 @@
         <v>hts_mod_com_ndx</v>
       </c>
       <c r="AG121" t="s">
-        <v>659</v>
+        <v>648</v>
       </c>
     </row>
     <row r="122" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>645</v>
+        <v>296</v>
       </c>
       <c r="B122" t="s">
         <v>406</v>
@@ -15388,12 +15355,12 @@
         <v>hts_mod_fac_ndx</v>
       </c>
       <c r="AG122" t="s">
-        <v>660</v>
+        <v>649</v>
       </c>
     </row>
     <row r="123" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>646</v>
+        <v>296</v>
       </c>
       <c r="B123" t="s">
         <v>406</v>
@@ -15424,12 +15391,12 @@
         <v>hts_mod_com_mob</v>
       </c>
       <c r="AG123" t="s">
-        <v>658</v>
+        <v>647</v>
       </c>
     </row>
     <row r="124" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>647</v>
+        <v>296</v>
       </c>
       <c r="B124" t="s">
         <v>406</v>
@@ -15460,12 +15427,12 @@
         <v>hts_mod_com_vct</v>
       </c>
       <c r="AG124" t="s">
-        <v>661</v>
+        <v>650</v>
       </c>
     </row>
     <row r="125" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>648</v>
+        <v>296</v>
       </c>
       <c r="B125" t="s">
         <v>406</v>
@@ -15496,12 +15463,12 @@
         <v>hts_mod_com_otr</v>
       </c>
       <c r="AG125" t="s">
-        <v>662</v>
+        <v>651</v>
       </c>
     </row>
     <row r="126" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>649</v>
+        <v>296</v>
       </c>
       <c r="B126" t="s">
         <v>406</v>
@@ -15532,12 +15499,12 @@
         <v>hts_mod_fac_ew</v>
       </c>
       <c r="AG126" t="s">
-        <v>663</v>
+        <v>652</v>
       </c>
     </row>
     <row r="127" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>650</v>
+        <v>296</v>
       </c>
       <c r="B127" t="s">
         <v>406</v>
@@ -15568,12 +15535,12 @@
         <v>hts_mod_fac_inpat</v>
       </c>
       <c r="AG127" t="s">
-        <v>664</v>
+        <v>653</v>
       </c>
     </row>
     <row r="128" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>651</v>
+        <v>296</v>
       </c>
       <c r="B128" t="s">
         <v>406</v>
@@ -15604,12 +15571,12 @@
         <v>hts_mod_fac_nut</v>
       </c>
       <c r="AG128" t="s">
-        <v>665</v>
+        <v>654</v>
       </c>
     </row>
     <row r="129" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>652</v>
+        <v>296</v>
       </c>
       <c r="B129" t="s">
         <v>406</v>
@@ -15640,12 +15607,12 @@
         <v>hts_mod_fac_ped</v>
       </c>
       <c r="AG129" t="s">
-        <v>666</v>
+        <v>655</v>
       </c>
     </row>
     <row r="130" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>653</v>
+        <v>296</v>
       </c>
       <c r="B130" t="s">
         <v>406</v>
@@ -15663,7 +15630,7 @@
         <v>442</v>
       </c>
       <c r="G130" t="s">
-        <v>656</v>
+        <v>645</v>
       </c>
       <c r="H130">
         <v>1000</v>
@@ -15676,12 +15643,12 @@
         <v>hts_mod_fac_sti</v>
       </c>
       <c r="AG130" t="s">
-        <v>667</v>
+        <v>656</v>
       </c>
     </row>
     <row r="131" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>654</v>
+        <v>296</v>
       </c>
       <c r="B131" t="s">
         <v>406</v>
@@ -15712,12 +15679,12 @@
         <v>hts_mod_fac_vct</v>
       </c>
       <c r="AG131" t="s">
-        <v>668</v>
+        <v>657</v>
       </c>
     </row>
     <row r="132" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>655</v>
+        <v>296</v>
       </c>
       <c r="B132" t="s">
         <v>406</v>
@@ -15748,7 +15715,7 @@
         <v>hts_mod_fac_otr_pitc</v>
       </c>
       <c r="AG132" t="s">
-        <v>669</v>
+        <v>658</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dimItemSets config file remove option values for data element group set dimension
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A97237E-28A3-504A-AAD0-C83FF076B752}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ABA1E61-DD04-3C49-8122-E8BD0FD56A9B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3743" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3743" uniqueCount="663">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1973,9 +1973,6 @@
   </si>
   <si>
     <t>other_disagg</t>
-  </si>
-  <si>
-    <t>QJZLPV5BcW</t>
   </si>
   <si>
     <t>hts_mod</t>
@@ -2440,10 +2437,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
   <dimension ref="A1:AO59"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="L1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
+      <selection pane="bottomLeft" activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4253,7 +4250,7 @@
         <v>237</v>
       </c>
       <c r="M15" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="N15" t="s">
         <v>237</v>
@@ -4378,7 +4375,7 @@
         <v>237</v>
       </c>
       <c r="M16" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="N16" t="s">
         <v>237</v>
@@ -4500,7 +4497,7 @@
         <v>237</v>
       </c>
       <c r="M17" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="N17" t="s">
         <v>237</v>
@@ -4551,7 +4548,7 @@
         <v>237</v>
       </c>
       <c r="AD17" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="AE17" t="s">
         <v>237</v>
@@ -4625,7 +4622,7 @@
         <v>237</v>
       </c>
       <c r="M18" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="N18" t="s">
         <v>237</v>
@@ -4750,7 +4747,7 @@
         <v>237</v>
       </c>
       <c r="M19" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="N19" t="s">
         <v>237</v>
@@ -4875,7 +4872,7 @@
         <v>237</v>
       </c>
       <c r="M20" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="N20" t="s">
         <v>237</v>
@@ -5000,7 +4997,7 @@
         <v>237</v>
       </c>
       <c r="M21" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="N21" t="s">
         <v>237</v>
@@ -5125,7 +5122,7 @@
         <v>237</v>
       </c>
       <c r="M22" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="N22" t="s">
         <v>237</v>
@@ -5250,7 +5247,7 @@
         <v>237</v>
       </c>
       <c r="M23" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="N23" t="s">
         <v>237</v>
@@ -5375,7 +5372,7 @@
         <v>237</v>
       </c>
       <c r="M24" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="N24" t="s">
         <v>237</v>
@@ -5500,7 +5497,7 @@
         <v>237</v>
       </c>
       <c r="M25" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="N25" t="s">
         <v>237</v>
@@ -5625,7 +5622,7 @@
         <v>237</v>
       </c>
       <c r="M26" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="N26" t="s">
         <v>237</v>
@@ -5750,7 +5747,7 @@
         <v>237</v>
       </c>
       <c r="M27" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="N27" t="s">
         <v>237</v>
@@ -5875,7 +5872,7 @@
         <v>237</v>
       </c>
       <c r="M28" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="N28" t="s">
         <v>237</v>
@@ -6000,7 +5997,7 @@
         <v>237</v>
       </c>
       <c r="M29" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="N29" t="s">
         <v>237</v>
@@ -6125,7 +6122,7 @@
         <v>237</v>
       </c>
       <c r="M30" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="N30" t="s">
         <v>237</v>
@@ -6250,7 +6247,7 @@
         <v>237</v>
       </c>
       <c r="M31" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="N31" t="s">
         <v>237</v>
@@ -6375,7 +6372,7 @@
         <v>237</v>
       </c>
       <c r="M32" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="N32" t="s">
         <v>237</v>
@@ -6500,7 +6497,7 @@
         <v>237</v>
       </c>
       <c r="M33" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="N33" t="s">
         <v>237</v>
@@ -6625,7 +6622,7 @@
         <v>237</v>
       </c>
       <c r="M34" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="N34" t="s">
         <v>237</v>
@@ -6750,7 +6747,7 @@
         <v>237</v>
       </c>
       <c r="M35" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="N35" t="s">
         <v>237</v>
@@ -6875,7 +6872,7 @@
         <v>237</v>
       </c>
       <c r="M36" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="N36" t="s">
         <v>237</v>
@@ -7000,7 +6997,7 @@
         <v>237</v>
       </c>
       <c r="M37" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="N37" t="s">
         <v>237</v>
@@ -9479,7 +9476,7 @@
         <v>237</v>
       </c>
       <c r="H57" s="15" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I57" t="s">
         <v>232</v>
@@ -9598,7 +9595,7 @@
         <v>237</v>
       </c>
       <c r="H58" s="15" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I58" t="s">
         <v>232</v>
@@ -9702,10 +9699,10 @@
     </row>
     <row r="59" spans="1:41" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B59" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C59" t="s">
         <v>2</v>
@@ -9717,10 +9714,10 @@
         <v>237</v>
       </c>
       <c r="H59" t="s">
+        <v>661</v>
+      </c>
+      <c r="I59" t="s">
         <v>662</v>
-      </c>
-      <c r="I59" t="s">
-        <v>663</v>
       </c>
       <c r="J59" t="s">
         <v>237</v>
@@ -10586,8 +10583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
   <dimension ref="A1:AG132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C120" sqref="C120"/>
+    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10704,7 +10701,7 @@
         <v>610</v>
       </c>
       <c r="AG1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
@@ -15303,10 +15300,10 @@
         <v>425</v>
       </c>
       <c r="F121" t="s">
-        <v>425</v>
+        <v>237</v>
       </c>
       <c r="G121" t="s">
-        <v>426</v>
+        <v>237</v>
       </c>
       <c r="H121">
         <v>100</v>
@@ -15319,7 +15316,7 @@
         <v>hts_mod_com_ndx</v>
       </c>
       <c r="AG121" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="122" spans="1:33" x14ac:dyDescent="0.2">
@@ -15339,10 +15336,10 @@
         <v>427</v>
       </c>
       <c r="F122" t="s">
-        <v>427</v>
+        <v>237</v>
       </c>
       <c r="G122" t="s">
-        <v>428</v>
+        <v>237</v>
       </c>
       <c r="H122">
         <v>200</v>
@@ -15355,7 +15352,7 @@
         <v>hts_mod_fac_ndx</v>
       </c>
       <c r="AG122" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="123" spans="1:33" x14ac:dyDescent="0.2">
@@ -15375,10 +15372,10 @@
         <v>435</v>
       </c>
       <c r="F123" t="s">
-        <v>435</v>
+        <v>237</v>
       </c>
       <c r="G123" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="H123">
         <v>300</v>
@@ -15391,7 +15388,7 @@
         <v>hts_mod_com_mob</v>
       </c>
       <c r="AG123" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="124" spans="1:33" x14ac:dyDescent="0.2">
@@ -15411,10 +15408,10 @@
         <v>436</v>
       </c>
       <c r="F124" t="s">
-        <v>436</v>
+        <v>237</v>
       </c>
       <c r="G124" t="s">
-        <v>261</v>
+        <v>237</v>
       </c>
       <c r="H124">
         <v>400</v>
@@ -15427,7 +15424,7 @@
         <v>hts_mod_com_vct</v>
       </c>
       <c r="AG124" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="125" spans="1:33" x14ac:dyDescent="0.2">
@@ -15447,10 +15444,10 @@
         <v>437</v>
       </c>
       <c r="F125" t="s">
-        <v>437</v>
+        <v>237</v>
       </c>
       <c r="G125" t="s">
-        <v>268</v>
+        <v>237</v>
       </c>
       <c r="H125">
         <v>500</v>
@@ -15463,7 +15460,7 @@
         <v>hts_mod_com_otr</v>
       </c>
       <c r="AG125" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="126" spans="1:33" x14ac:dyDescent="0.2">
@@ -15483,10 +15480,10 @@
         <v>438</v>
       </c>
       <c r="F126" t="s">
-        <v>438</v>
+        <v>237</v>
       </c>
       <c r="G126" t="s">
-        <v>263</v>
+        <v>237</v>
       </c>
       <c r="H126">
         <v>600</v>
@@ -15499,7 +15496,7 @@
         <v>hts_mod_fac_ew</v>
       </c>
       <c r="AG126" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="127" spans="1:33" x14ac:dyDescent="0.2">
@@ -15519,10 +15516,10 @@
         <v>439</v>
       </c>
       <c r="F127" t="s">
-        <v>439</v>
+        <v>237</v>
       </c>
       <c r="G127" t="s">
-        <v>264</v>
+        <v>237</v>
       </c>
       <c r="H127">
         <v>700</v>
@@ -15535,7 +15532,7 @@
         <v>hts_mod_fac_inpat</v>
       </c>
       <c r="AG127" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="128" spans="1:33" x14ac:dyDescent="0.2">
@@ -15555,10 +15552,10 @@
         <v>440</v>
       </c>
       <c r="F128" t="s">
-        <v>440</v>
+        <v>237</v>
       </c>
       <c r="G128" t="s">
-        <v>265</v>
+        <v>237</v>
       </c>
       <c r="H128">
         <v>800</v>
@@ -15571,7 +15568,7 @@
         <v>hts_mod_fac_nut</v>
       </c>
       <c r="AG128" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="129" spans="1:33" x14ac:dyDescent="0.2">
@@ -15591,10 +15588,10 @@
         <v>441</v>
       </c>
       <c r="F129" t="s">
-        <v>441</v>
+        <v>237</v>
       </c>
       <c r="G129" t="s">
-        <v>266</v>
+        <v>237</v>
       </c>
       <c r="H129">
         <v>900</v>
@@ -15607,7 +15604,7 @@
         <v>hts_mod_fac_ped</v>
       </c>
       <c r="AG129" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="130" spans="1:33" x14ac:dyDescent="0.2">
@@ -15627,10 +15624,10 @@
         <v>442</v>
       </c>
       <c r="F130" t="s">
-        <v>442</v>
+        <v>237</v>
       </c>
       <c r="G130" t="s">
-        <v>645</v>
+        <v>237</v>
       </c>
       <c r="H130">
         <v>1000</v>
@@ -15643,7 +15640,7 @@
         <v>hts_mod_fac_sti</v>
       </c>
       <c r="AG130" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="131" spans="1:33" x14ac:dyDescent="0.2">
@@ -15663,10 +15660,10 @@
         <v>443</v>
       </c>
       <c r="F131" t="s">
-        <v>443</v>
+        <v>237</v>
       </c>
       <c r="G131" t="s">
-        <v>267</v>
+        <v>237</v>
       </c>
       <c r="H131">
         <v>1100</v>
@@ -15679,7 +15676,7 @@
         <v>hts_mod_fac_vct</v>
       </c>
       <c r="AG131" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="132" spans="1:33" x14ac:dyDescent="0.2">
@@ -15699,10 +15696,10 @@
         <v>444</v>
       </c>
       <c r="F132" t="s">
-        <v>444</v>
+        <v>237</v>
       </c>
       <c r="G132" t="s">
-        <v>269</v>
+        <v>237</v>
       </c>
       <c r="H132">
         <v>1200</v>
@@ -15715,7 +15712,7 @@
         <v>hts_mod_fac_otr_pitc</v>
       </c>
       <c r="AG132" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data_required config file updating entries for kp_prev, prep_new and Impatt.priority
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ABA1E61-DD04-3C49-8122-E8BD0FD56A9B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280DE413-FEC7-AF4B-9B0B-4A1246BD9F10}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="34320" yWindow="460" windowWidth="25600" windowHeight="20020" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3743" uniqueCount="663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3749" uniqueCount="667">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -2014,9 +2014,6 @@
     <t>hts_mod_fac_otr_pitc</t>
   </si>
   <si>
-    <t>DE_GROUP-zhdJiWlPvCz</t>
-  </si>
-  <si>
     <t>IMPATT.PRIORITY_SNU.19T</t>
   </si>
   <si>
@@ -2027,6 +2024,21 @@
   </si>
   <si>
     <t>2018Q4</t>
+  </si>
+  <si>
+    <t>gdHE7Kk9Q1k</t>
+  </si>
+  <si>
+    <t>lXqlw8UxoqF</t>
+  </si>
+  <si>
+    <t>A+B</t>
+  </si>
+  <si>
+    <t>wDWUutgeEX8</t>
+  </si>
+  <si>
+    <t>VRgwEePUvdD</t>
   </si>
 </sst>
 </file>
@@ -2437,10 +2449,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
   <dimension ref="A1:AO59"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="M39" sqref="M39"/>
+      <selection pane="bottomLeft" activeCell="AT59" sqref="AT59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9469,14 +9481,20 @@
       <c r="C57" t="s">
         <v>2</v>
       </c>
+      <c r="D57" t="s">
+        <v>237</v>
+      </c>
       <c r="E57" t="s">
         <v>4</v>
       </c>
       <c r="F57" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="G57" s="1" t="s">
         <v>237</v>
       </c>
       <c r="H57" s="15" t="s">
-        <v>658</v>
+        <v>662</v>
       </c>
       <c r="I57" t="s">
         <v>232</v>
@@ -9527,10 +9545,10 @@
         <v>237</v>
       </c>
       <c r="Y57" t="s">
-        <v>237</v>
+        <v>663</v>
       </c>
       <c r="Z57" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="AA57" t="s">
         <v>237</v>
@@ -9539,7 +9557,7 @@
         <v>237</v>
       </c>
       <c r="AC57" t="s">
-        <v>237</v>
+        <v>609</v>
       </c>
       <c r="AD57" t="s">
         <v>237</v>
@@ -9575,7 +9593,7 @@
         <v>237</v>
       </c>
       <c r="AO57" t="s">
-        <v>237</v>
+        <v>664</v>
       </c>
     </row>
     <row r="58" spans="1:41" ht="18" x14ac:dyDescent="0.2">
@@ -9588,14 +9606,20 @@
       <c r="C58" t="s">
         <v>2</v>
       </c>
+      <c r="D58" t="s">
+        <v>237</v>
+      </c>
       <c r="E58" t="s">
         <v>4</v>
       </c>
       <c r="F58" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="G58" s="1" t="s">
         <v>237</v>
       </c>
       <c r="H58" s="15" t="s">
-        <v>658</v>
+        <v>665</v>
       </c>
       <c r="I58" t="s">
         <v>232</v>
@@ -9646,10 +9670,10 @@
         <v>237</v>
       </c>
       <c r="Y58" t="s">
-        <v>237</v>
+        <v>666</v>
       </c>
       <c r="Z58" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="AA58" t="s">
         <v>237</v>
@@ -9658,7 +9682,7 @@
         <v>237</v>
       </c>
       <c r="AC58" t="s">
-        <v>237</v>
+        <v>578</v>
       </c>
       <c r="AD58" t="s">
         <v>237</v>
@@ -9694,30 +9718,36 @@
         <v>237</v>
       </c>
       <c r="AO58" t="s">
-        <v>237</v>
+        <v>664</v>
       </c>
     </row>
     <row r="59" spans="1:41" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B59" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C59" t="s">
         <v>2</v>
       </c>
+      <c r="D59" t="s">
+        <v>237</v>
+      </c>
       <c r="E59" t="s">
         <v>4</v>
       </c>
       <c r="F59" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="G59" s="1" t="s">
         <v>237</v>
       </c>
       <c r="H59" t="s">
+        <v>660</v>
+      </c>
+      <c r="I59" t="s">
         <v>661</v>
-      </c>
-      <c r="I59" t="s">
-        <v>662</v>
       </c>
       <c r="J59" t="s">
         <v>237</v>
@@ -10583,7 +10613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
   <dimension ref="A1:AG132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A100" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
data_required config add columns to specify handling of NA values in calculations
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280DE413-FEC7-AF4B-9B0B-4A1246BD9F10}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582FECDD-DF97-9A4B-A3A8-5D0A5E9CAC57}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34320" yWindow="460" windowWidth="25600" windowHeight="20020" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3749" uniqueCount="667">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3863" uniqueCount="669">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -2039,6 +2039,12 @@
   </si>
   <si>
     <t>VRgwEePUvdD</t>
+  </si>
+  <si>
+    <t>A.value_na</t>
+  </si>
+  <si>
+    <t>B.value_na</t>
   </si>
 </sst>
 </file>
@@ -2447,12 +2453,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
-  <dimension ref="A1:AO59"/>
+  <dimension ref="A1:AQ59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="AT59" sqref="AT59"/>
+      <selection pane="bottomLeft" activeCell="AQ1" sqref="AQ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2474,7 +2480,7 @@
     <col min="30" max="30" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>274</v>
       </c>
@@ -2598,8 +2604,14 @@
       <c r="AO1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP1" t="s">
+        <v>667</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2723,8 +2735,14 @@
       <c r="AO2" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2848,8 +2866,14 @@
       <c r="AO3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP3" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2973,8 +2997,14 @@
       <c r="AO4" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP4" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -3098,8 +3128,14 @@
       <c r="AO5" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -3223,8 +3259,14 @@
       <c r="AO6" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP6" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -3348,8 +3390,14 @@
       <c r="AO7" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP7" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -3473,8 +3521,14 @@
       <c r="AO8" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP8" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -3598,8 +3652,14 @@
       <c r="AO9" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP9" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -3723,8 +3783,14 @@
       <c r="AO10" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP10" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -3848,8 +3914,14 @@
       <c r="AO11" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP11" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -3973,8 +4045,14 @@
       <c r="AO12" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP12" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -4098,8 +4176,14 @@
       <c r="AO13" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP13" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ13" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -4223,8 +4307,14 @@
       <c r="AO14" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="15" spans="1:41" ht="18" x14ac:dyDescent="0.25">
+      <c r="AP14" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ14" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:43" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -4348,8 +4438,14 @@
       <c r="AO15" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="16" spans="1:41" ht="18" x14ac:dyDescent="0.25">
+      <c r="AP15" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ15" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -4473,8 +4569,14 @@
       <c r="AO16" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="17" spans="1:41" ht="19" x14ac:dyDescent="0.25">
+      <c r="AP16" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ16" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -4595,8 +4697,14 @@
       <c r="AO17" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="18" spans="1:41" ht="19" x14ac:dyDescent="0.25">
+      <c r="AP17" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ17" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -4720,8 +4828,14 @@
       <c r="AO18" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="19" spans="1:41" ht="19" x14ac:dyDescent="0.25">
+      <c r="AP18" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ18" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -4845,8 +4959,14 @@
       <c r="AO19" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="20" spans="1:41" ht="19" x14ac:dyDescent="0.25">
+      <c r="AP19" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ19" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="20" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -4970,8 +5090,14 @@
       <c r="AO20" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="21" spans="1:41" ht="19" x14ac:dyDescent="0.25">
+      <c r="AP20" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ20" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -5095,8 +5221,14 @@
       <c r="AO21" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="22" spans="1:41" ht="19" x14ac:dyDescent="0.25">
+      <c r="AP21" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ21" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="22" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -5220,8 +5352,14 @@
       <c r="AO22" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="23" spans="1:41" ht="19" x14ac:dyDescent="0.25">
+      <c r="AP22" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ22" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -5345,8 +5483,14 @@
       <c r="AO23" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="24" spans="1:41" ht="19" x14ac:dyDescent="0.25">
+      <c r="AP23" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ23" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -5470,8 +5614,14 @@
       <c r="AO24" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="25" spans="1:41" ht="19" x14ac:dyDescent="0.25">
+      <c r="AP24" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ24" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -5595,8 +5745,14 @@
       <c r="AO25" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="26" spans="1:41" ht="19" x14ac:dyDescent="0.25">
+      <c r="AP25" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ25" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="26" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -5720,8 +5876,14 @@
       <c r="AO26" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="27" spans="1:41" ht="19" x14ac:dyDescent="0.25">
+      <c r="AP26" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ26" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="27" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -5845,8 +6007,14 @@
       <c r="AO27" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="28" spans="1:41" ht="19" x14ac:dyDescent="0.25">
+      <c r="AP27" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ27" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="28" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -5970,8 +6138,14 @@
       <c r="AO28" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="29" spans="1:41" ht="19" x14ac:dyDescent="0.25">
+      <c r="AP28" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -6095,8 +6269,14 @@
       <c r="AO29" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="30" spans="1:41" ht="19" x14ac:dyDescent="0.25">
+      <c r="AP29" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ29" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="30" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -6220,8 +6400,14 @@
       <c r="AO30" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="31" spans="1:41" ht="19" x14ac:dyDescent="0.25">
+      <c r="AP30" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ30" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="31" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -6345,8 +6531,14 @@
       <c r="AO31" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="32" spans="1:41" ht="19" x14ac:dyDescent="0.25">
+      <c r="AP31" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ31" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="32" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -6470,8 +6662,14 @@
       <c r="AO32" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="33" spans="1:41" ht="19" x14ac:dyDescent="0.25">
+      <c r="AP32" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ32" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="33" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -6595,8 +6793,14 @@
       <c r="AO33" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="34" spans="1:41" ht="19" x14ac:dyDescent="0.25">
+      <c r="AP33" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ33" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="34" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -6720,8 +6924,14 @@
       <c r="AO34" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="35" spans="1:41" ht="19" x14ac:dyDescent="0.25">
+      <c r="AP34" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ34" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="35" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -6845,8 +7055,14 @@
       <c r="AO35" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="36" spans="1:41" ht="19" x14ac:dyDescent="0.25">
+      <c r="AP35" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ35" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="36" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -6970,8 +7186,14 @@
       <c r="AO36" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="37" spans="1:41" ht="19" x14ac:dyDescent="0.25">
+      <c r="AP36" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ36" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="37" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -7095,8 +7317,14 @@
       <c r="AO37" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="38" spans="1:41" ht="19" x14ac:dyDescent="0.25">
+      <c r="AP37" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ37" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="38" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -7220,8 +7448,14 @@
       <c r="AO38" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="39" spans="1:41" ht="19" x14ac:dyDescent="0.25">
+      <c r="AP38" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ38" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="39" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -7345,8 +7579,14 @@
       <c r="AO39" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="40" spans="1:41" ht="18" x14ac:dyDescent="0.2">
+      <c r="AP39" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ39" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="40" spans="1:43" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>35</v>
       </c>
@@ -7470,8 +7710,14 @@
       <c r="AO40" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="41" spans="1:41" ht="18" x14ac:dyDescent="0.2">
+      <c r="AP40" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ40" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="41" spans="1:43" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>82</v>
       </c>
@@ -7595,8 +7841,14 @@
       <c r="AO41" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="42" spans="1:41" ht="18" x14ac:dyDescent="0.2">
+      <c r="AP41" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ41" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="42" spans="1:43" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>82</v>
       </c>
@@ -7720,8 +7972,14 @@
       <c r="AO42" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="43" spans="1:41" ht="18" x14ac:dyDescent="0.2">
+      <c r="AP42" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ42" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="43" spans="1:43" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>87</v>
       </c>
@@ -7845,8 +8103,14 @@
       <c r="AO43" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="44" spans="1:41" ht="18" x14ac:dyDescent="0.2">
+      <c r="AP43" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ43" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="44" spans="1:43" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>87</v>
       </c>
@@ -7970,8 +8234,14 @@
       <c r="AO44" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="45" spans="1:41" ht="18" x14ac:dyDescent="0.2">
+      <c r="AP44" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ44" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="45" spans="1:43" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>91</v>
       </c>
@@ -8095,8 +8365,14 @@
       <c r="AO45" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="46" spans="1:41" ht="18" x14ac:dyDescent="0.2">
+      <c r="AP45" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ45" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="46" spans="1:43" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>91</v>
       </c>
@@ -8220,8 +8496,14 @@
       <c r="AO46" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="47" spans="1:41" ht="18" x14ac:dyDescent="0.2">
+      <c r="AP46" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ46" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="47" spans="1:43" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
         <v>91</v>
       </c>
@@ -8345,8 +8627,14 @@
       <c r="AO47" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="48" spans="1:41" ht="19" x14ac:dyDescent="0.25">
+      <c r="AP47" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ47" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="48" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>91</v>
       </c>
@@ -8470,8 +8758,14 @@
       <c r="AO48" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="49" spans="1:41" ht="19" x14ac:dyDescent="0.25">
+      <c r="AP48" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ48" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="49" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>91</v>
       </c>
@@ -8595,8 +8889,14 @@
       <c r="AO49" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="50" spans="1:41" ht="18" x14ac:dyDescent="0.2">
+      <c r="AP49" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ49" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="50" spans="1:43" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>91</v>
       </c>
@@ -8720,8 +9020,14 @@
       <c r="AO50" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="51" spans="1:41" ht="18" x14ac:dyDescent="0.2">
+      <c r="AP50" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ50" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="51" spans="1:43" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>108</v>
       </c>
@@ -8845,8 +9151,14 @@
       <c r="AO51" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="52" spans="1:41" ht="18" x14ac:dyDescent="0.2">
+      <c r="AP51" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ51" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="52" spans="1:43" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>108</v>
       </c>
@@ -8970,8 +9282,14 @@
       <c r="AO52" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="53" spans="1:41" ht="18" x14ac:dyDescent="0.2">
+      <c r="AP52" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ52" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="53" spans="1:43" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>112</v>
       </c>
@@ -9095,8 +9413,14 @@
       <c r="AO53" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="54" spans="1:41" ht="18" x14ac:dyDescent="0.2">
+      <c r="AP53" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ53" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="54" spans="1:43" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>115</v>
       </c>
@@ -9220,8 +9544,14 @@
       <c r="AO54" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="55" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP54" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ54" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="55" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>115</v>
       </c>
@@ -9345,8 +9675,14 @@
       <c r="AO55" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="56" spans="1:41" ht="18" x14ac:dyDescent="0.2">
+      <c r="AP55" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ55" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="56" spans="1:43" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>115</v>
       </c>
@@ -9470,8 +9806,14 @@
       <c r="AO56" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="57" spans="1:41" ht="18" x14ac:dyDescent="0.2">
+      <c r="AP56" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ56" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="57" spans="1:43" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>91</v>
       </c>
@@ -9595,8 +9937,14 @@
       <c r="AO57" t="s">
         <v>664</v>
       </c>
-    </row>
-    <row r="58" spans="1:41" ht="18" x14ac:dyDescent="0.2">
+      <c r="AP57">
+        <v>0</v>
+      </c>
+      <c r="AQ57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:43" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>91</v>
       </c>
@@ -9720,8 +10068,14 @@
       <c r="AO58" t="s">
         <v>664</v>
       </c>
-    </row>
-    <row r="59" spans="1:41" ht="18" x14ac:dyDescent="0.2">
+      <c r="AP58">
+        <v>0</v>
+      </c>
+      <c r="AQ58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:43" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>659</v>
       </c>
@@ -9843,6 +10197,12 @@
         <v>237</v>
       </c>
       <c r="AO59" t="s">
+        <v>237</v>
+      </c>
+      <c r="AP59" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ59" t="s">
         <v>237</v>
       </c>
     </row>

</xml_diff>

<commit_message>
data_required config file change how NA are handled for compPosShare
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582FECDD-DF97-9A4B-A3A8-5D0A5E9CAC57}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945EF99E-E117-C444-ACDD-B5D82D19DCA6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3863" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3861" uniqueCount="669">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -2455,10 +2455,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
   <dimension ref="A1:AQ59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="AQ1" sqref="AQ1"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4697,11 +4698,11 @@
       <c r="AO17" t="s">
         <v>434</v>
       </c>
-      <c r="AP17" t="s">
-        <v>237</v>
-      </c>
-      <c r="AQ17" t="s">
-        <v>237</v>
+      <c r="AP17">
+        <v>0</v>
+      </c>
+      <c r="AQ17">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:43" ht="19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
data_required update comPosShare full formula
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945EF99E-E117-C444-ACDD-B5D82D19DCA6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68602CE-6EFD-1941-9427-574B512E793F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3861" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3862" uniqueCount="670">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -2045,6 +2045,9 @@
   </si>
   <si>
     <t>B.value_na</t>
+  </si>
+  <si>
+    <t>=([HTS_TST.N.IndexMod/Age/Sex/Result.18R.Positive])%/%([HTS_TST.N.Index/Age/Sex/Result.18R.Positive]+[HTS_TST.N.IndexMod/Age/Sex/Result.18R.Positive])</t>
   </si>
 </sst>
 </file>
@@ -2456,10 +2459,10 @@
   <dimension ref="A1:AQ59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4586,6 +4589,9 @@
       </c>
       <c r="C17" t="s">
         <v>6</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>669</v>
       </c>
       <c r="E17" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
data_required 2018Oct to 2019Oct for A.pe_iso
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64045369-6823-0E44-B94D-EBE7B0F33E4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9475FE6C-F17E-424F-A413-FCD8083E7702}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3862" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3862" uniqueCount="671">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -2048,6 +2048,9 @@
   </si>
   <si>
     <t>[PMTCT_HEI_POS.N.Age/HIVStatus.18R.&lt;= 2 months]%/%[PMTCT_EID.N.Age.18R.&lt;= 2 months]</t>
+  </si>
+  <si>
+    <t>2019Oct</t>
   </si>
 </sst>
 </file>
@@ -2459,10 +2462,10 @@
   <dimension ref="A1:AQ59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D53" sqref="D53"/>
+      <selection pane="bottomRight" activeCell="Z57" sqref="Z57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2641,7 +2644,7 @@
         <v>81</v>
       </c>
       <c r="I2" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="J2" t="s">
         <v>185</v>
@@ -3296,7 +3299,7 @@
         <v>86</v>
       </c>
       <c r="I7" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>241</v>
@@ -3427,7 +3430,7 @@
         <v>86</v>
       </c>
       <c r="I8" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>241</v>
@@ -3820,7 +3823,7 @@
         <v>91</v>
       </c>
       <c r="I11" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="J11" t="s">
         <v>185</v>
@@ -4213,7 +4216,7 @@
         <v>94</v>
       </c>
       <c r="I14" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="J14" t="s">
         <v>201</v>
@@ -7357,7 +7360,7 @@
         <v>98</v>
       </c>
       <c r="I38" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="J38" t="s">
         <v>185</v>
@@ -7488,7 +7491,7 @@
         <v>109</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="J39" t="s">
         <v>185</v>
@@ -7619,7 +7622,7 @@
         <v>248</v>
       </c>
       <c r="I40" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="J40" t="s">
         <v>185</v>
@@ -8012,7 +8015,7 @@
         <v>102</v>
       </c>
       <c r="I43" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="J43" t="s">
         <v>348</v>
@@ -8143,7 +8146,7 @@
         <v>102</v>
       </c>
       <c r="I44" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="J44" t="s">
         <v>348</v>
@@ -8274,7 +8277,7 @@
         <v>104</v>
       </c>
       <c r="I45" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="J45" t="s">
         <v>188</v>
@@ -8405,7 +8408,7 @@
         <v>106</v>
       </c>
       <c r="I46" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="J46" t="s">
         <v>188</v>
@@ -8536,7 +8539,7 @@
         <v>106</v>
       </c>
       <c r="I47" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="J47" t="s">
         <v>188</v>
@@ -8667,7 +8670,7 @@
         <v>108</v>
       </c>
       <c r="I48" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="J48" t="s">
         <v>188</v>
@@ -8798,7 +8801,7 @@
         <v>99</v>
       </c>
       <c r="I49" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="J49" t="s">
         <v>188</v>
@@ -8929,7 +8932,7 @@
         <v>110</v>
       </c>
       <c r="I50" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="J50" t="s">
         <v>188</v>
@@ -9060,7 +9063,7 @@
         <v>112</v>
       </c>
       <c r="I51" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="J51" t="s">
         <v>185</v>
@@ -9191,7 +9194,7 @@
         <v>112</v>
       </c>
       <c r="I52" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="J52" t="s">
         <v>185</v>
@@ -9322,7 +9325,7 @@
         <v>113</v>
       </c>
       <c r="I53" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="J53" t="s">
         <v>223</v>
@@ -9453,7 +9456,7 @@
         <v>115</v>
       </c>
       <c r="I54" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="J54" t="s">
         <v>188</v>
@@ -9584,7 +9587,7 @@
         <v>117</v>
       </c>
       <c r="I55" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="J55" t="s">
         <v>188</v>
@@ -9715,7 +9718,7 @@
         <v>345</v>
       </c>
       <c r="I56" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="J56" t="s">
         <v>188</v>
@@ -9846,7 +9849,7 @@
         <v>609</v>
       </c>
       <c r="I57" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="J57" t="s">
         <v>188</v>
@@ -9977,7 +9980,7 @@
         <v>612</v>
       </c>
       <c r="I58" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="J58" t="s">
         <v>188</v>

</xml_diff>

<commit_message>
data_required 2017Oct to 2018Oct for A.pe_iso
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9475FE6C-F17E-424F-A413-FCD8083E7702}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFD8B8F-FDA3-E145-9426-DB5B26CABDDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
@@ -2462,10 +2462,10 @@
   <dimension ref="A1:AQ59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z57" sqref="Z57"/>
+      <selection pane="bottomRight" activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2775,7 +2775,7 @@
         <v>82</v>
       </c>
       <c r="I3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J3" t="s">
         <v>185</v>
@@ -2906,7 +2906,7 @@
         <v>83</v>
       </c>
       <c r="I4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J4" t="s">
         <v>185</v>
@@ -3037,7 +3037,7 @@
         <v>84</v>
       </c>
       <c r="I5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J5" t="s">
         <v>188</v>
@@ -3168,7 +3168,7 @@
         <v>85</v>
       </c>
       <c r="I6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J6" t="s">
         <v>188</v>
@@ -3561,7 +3561,7 @@
         <v>89</v>
       </c>
       <c r="I9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>241</v>
@@ -3692,7 +3692,7 @@
         <v>90</v>
       </c>
       <c r="I10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>241</v>
@@ -3954,7 +3954,7 @@
         <v>92</v>
       </c>
       <c r="I12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J12" t="s">
         <v>237</v>
@@ -4085,7 +4085,7 @@
         <v>93</v>
       </c>
       <c r="I13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J13" t="s">
         <v>237</v>
@@ -4347,7 +4347,7 @@
         <v>95</v>
       </c>
       <c r="I15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J15" t="s">
         <v>203</v>
@@ -4478,7 +4478,7 @@
         <v>95</v>
       </c>
       <c r="I16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J16" t="s">
         <v>203</v>
@@ -4609,7 +4609,7 @@
         <v>96</v>
       </c>
       <c r="I17" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J17" t="s">
         <v>203</v>
@@ -4740,7 +4740,7 @@
         <v>96</v>
       </c>
       <c r="I18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J18" t="s">
         <v>203</v>
@@ -4871,7 +4871,7 @@
         <v>96</v>
       </c>
       <c r="I19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J19" t="s">
         <v>203</v>
@@ -5002,7 +5002,7 @@
         <v>96</v>
       </c>
       <c r="I20" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J20" t="s">
         <v>203</v>
@@ -5133,7 +5133,7 @@
         <v>96</v>
       </c>
       <c r="I21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J21" t="s">
         <v>203</v>
@@ -5264,7 +5264,7 @@
         <v>96</v>
       </c>
       <c r="I22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J22" t="s">
         <v>203</v>
@@ -5395,7 +5395,7 @@
         <v>96</v>
       </c>
       <c r="I23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>134</v>
@@ -5526,7 +5526,7 @@
         <v>96</v>
       </c>
       <c r="I24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>134</v>
@@ -5657,7 +5657,7 @@
         <v>96</v>
       </c>
       <c r="I25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J25" t="s">
         <v>203</v>
@@ -5788,7 +5788,7 @@
         <v>96</v>
       </c>
       <c r="I26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J26" t="s">
         <v>203</v>
@@ -5919,7 +5919,7 @@
         <v>96</v>
       </c>
       <c r="I27" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J27" t="s">
         <v>203</v>
@@ -6050,7 +6050,7 @@
         <v>97</v>
       </c>
       <c r="I28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J28" t="s">
         <v>203</v>
@@ -6181,7 +6181,7 @@
         <v>97</v>
       </c>
       <c r="I29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J29" t="s">
         <v>203</v>
@@ -6312,7 +6312,7 @@
         <v>97</v>
       </c>
       <c r="I30" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J30" t="s">
         <v>203</v>
@@ -6443,7 +6443,7 @@
         <v>97</v>
       </c>
       <c r="I31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J31" t="s">
         <v>203</v>
@@ -6574,7 +6574,7 @@
         <v>97</v>
       </c>
       <c r="I32" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J32" t="s">
         <v>203</v>
@@ -6705,7 +6705,7 @@
         <v>97</v>
       </c>
       <c r="I33" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>134</v>
@@ -6836,7 +6836,7 @@
         <v>97</v>
       </c>
       <c r="I34" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>134</v>
@@ -6967,7 +6967,7 @@
         <v>97</v>
       </c>
       <c r="I35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J35" t="s">
         <v>203</v>
@@ -7098,7 +7098,7 @@
         <v>97</v>
       </c>
       <c r="I36" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J36" t="s">
         <v>203</v>
@@ -7229,7 +7229,7 @@
         <v>97</v>
       </c>
       <c r="I37" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J37" t="s">
         <v>203</v>
@@ -7753,7 +7753,7 @@
         <v>100</v>
       </c>
       <c r="I41" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J41" t="s">
         <v>238</v>
@@ -7884,7 +7884,7 @@
         <v>101</v>
       </c>
       <c r="I42" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J42" t="s">
         <v>238</v>

</xml_diff>

<commit_message>
data_required 2018Oct to 2019Oct for B.pe_iso
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFD8B8F-FDA3-E145-9426-DB5B26CABDDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D9A929-A893-4E4D-BB5E-898D7309D3DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
@@ -2462,10 +2462,10 @@
   <dimension ref="A1:AQ59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z8" sqref="Z8"/>
+      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2478,8 +2478,7 @@
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
     <col min="7" max="7" width="68.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="17.33203125" customWidth="1"/>
-    <col min="14" max="21" width="17.33203125" hidden="1" customWidth="1"/>
+    <col min="9" max="21" width="17.33203125" customWidth="1"/>
     <col min="22" max="22" width="53.1640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="24" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="46.83203125" bestFit="1" customWidth="1"/>
@@ -9900,7 +9899,7 @@
         <v>610</v>
       </c>
       <c r="Z57" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="AA57" t="s">
         <v>188</v>
@@ -10031,7 +10030,7 @@
         <v>613</v>
       </c>
       <c r="Z58" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="AA58" t="s">
         <v>188</v>

</xml_diff>

<commit_message>
data_required HTS_TST_POS indicator uid update
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FE7B1D-05D8-F148-92B6-38D317FB65CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB668CB-D7CF-3C4A-AE06-EA7CB4D61B2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="34320" yWindow="460" windowWidth="33600" windowHeight="20020" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -1135,9 +1135,6 @@
     <t>HTS_TST.N.Pos</t>
   </si>
   <si>
-    <t>HTS_TST.N.yield</t>
-  </si>
-  <si>
     <t>HTS_SELF.N.Age/Sex/SelfTest.19T.Directly_Assisted</t>
   </si>
   <si>
@@ -2048,6 +2045,9 @@
   </si>
   <si>
     <t>IQJhBffoYIJ</t>
+  </si>
+  <si>
+    <t>joBC2hxzpGN</t>
   </si>
 </sst>
 </file>
@@ -2459,10 +2459,10 @@
   <dimension ref="A1:AQ59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="W14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H28" sqref="H28"/>
+      <selection pane="bottomRight" activeCell="Y17" sqref="Y17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2503,7 +2503,7 @@
         <v>340</v>
       </c>
       <c r="G1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H1" t="s">
         <v>336</v>
@@ -2521,25 +2521,25 @@
         <v>232</v>
       </c>
       <c r="M1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="N1" t="s">
+        <v>574</v>
+      </c>
+      <c r="O1" t="s">
         <v>575</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>576</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>577</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>578</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>579</v>
-      </c>
-      <c r="S1" t="s">
-        <v>580</v>
       </c>
       <c r="T1" t="s">
         <v>237</v>
@@ -2569,49 +2569,49 @@
         <v>227</v>
       </c>
       <c r="AC1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="AD1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="AE1" t="s">
+        <v>580</v>
+      </c>
+      <c r="AF1" t="s">
         <v>581</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>582</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>583</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>584</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>585</v>
       </c>
-      <c r="AJ1" t="s">
-        <v>586</v>
-      </c>
       <c r="AK1" t="s">
+        <v>373</v>
+      </c>
+      <c r="AL1" t="s">
         <v>374</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>375</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>376</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>377</v>
       </c>
       <c r="AO1" t="s">
         <v>196</v>
       </c>
       <c r="AP1" t="s">
+        <v>611</v>
+      </c>
+      <c r="AQ1" t="s">
         <v>612</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.2">
@@ -2625,7 +2625,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -2640,7 +2640,7 @@
         <v>81</v>
       </c>
       <c r="I2" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J2" t="s">
         <v>183</v>
@@ -2756,7 +2756,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
@@ -2887,7 +2887,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
@@ -3018,7 +3018,7 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
@@ -3149,7 +3149,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -3280,7 +3280,7 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="E7" t="s">
         <v>3</v>
@@ -3295,7 +3295,7 @@
         <v>86</v>
       </c>
       <c r="I7" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>239</v>
@@ -3411,7 +3411,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
@@ -3426,7 +3426,7 @@
         <v>86</v>
       </c>
       <c r="I8" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>239</v>
@@ -3542,7 +3542,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
@@ -3673,7 +3673,7 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
@@ -3804,7 +3804,7 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="E11" t="s">
         <v>3</v>
@@ -3819,7 +3819,7 @@
         <v>91</v>
       </c>
       <c r="I11" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J11" t="s">
         <v>183</v>
@@ -3935,7 +3935,7 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E12" t="s">
         <v>6</v>
@@ -4066,7 +4066,7 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
@@ -4197,7 +4197,7 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="E14" t="s">
         <v>3</v>
@@ -4212,7 +4212,7 @@
         <v>94</v>
       </c>
       <c r="I14" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J14" t="s">
         <v>199</v>
@@ -4322,13 +4322,13 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
@@ -4337,7 +4337,7 @@
         <v>187</v>
       </c>
       <c r="G15" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H15" t="s">
         <v>95</v>
@@ -4355,7 +4355,7 @@
         <v>186</v>
       </c>
       <c r="M15" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="N15" t="s">
         <v>186</v>
@@ -4382,10 +4382,10 @@
         <v>245</v>
       </c>
       <c r="V15" t="s">
+        <v>369</v>
+      </c>
+      <c r="W15" t="s">
         <v>370</v>
-      </c>
-      <c r="W15" t="s">
-        <v>371</v>
       </c>
       <c r="X15" t="s">
         <v>186</v>
@@ -4453,13 +4453,13 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="E16" t="s">
         <v>6</v>
@@ -4468,7 +4468,7 @@
         <v>187</v>
       </c>
       <c r="G16" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H16" t="s">
         <v>95</v>
@@ -4486,7 +4486,7 @@
         <v>186</v>
       </c>
       <c r="M16" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="N16" t="s">
         <v>186</v>
@@ -4513,10 +4513,10 @@
         <v>245</v>
       </c>
       <c r="V16" t="s">
+        <v>371</v>
+      </c>
+      <c r="W16" t="s">
         <v>372</v>
-      </c>
-      <c r="W16" t="s">
-        <v>373</v>
       </c>
       <c r="X16" t="s">
         <v>186</v>
@@ -4584,13 +4584,13 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E17" t="s">
         <v>6</v>
@@ -4599,10 +4599,10 @@
         <v>185</v>
       </c>
       <c r="G17" t="s">
-        <v>364</v>
+        <v>186</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>96</v>
+        <v>669</v>
       </c>
       <c r="I17" t="s">
         <v>182</v>
@@ -4617,7 +4617,7 @@
         <v>186</v>
       </c>
       <c r="M17" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="N17" t="s">
         <v>186</v>
@@ -4644,10 +4644,10 @@
         <v>245</v>
       </c>
       <c r="V17" t="s">
+        <v>369</v>
+      </c>
+      <c r="W17" t="s">
         <v>370</v>
-      </c>
-      <c r="W17" t="s">
-        <v>371</v>
       </c>
       <c r="X17" t="s">
         <v>364</v>
@@ -4668,7 +4668,7 @@
         <v>186</v>
       </c>
       <c r="AD17" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="AE17" t="s">
         <v>186</v>
@@ -4695,13 +4695,13 @@
         <v>245</v>
       </c>
       <c r="AM17" t="s">
+        <v>371</v>
+      </c>
+      <c r="AN17" t="s">
         <v>372</v>
       </c>
-      <c r="AN17" t="s">
-        <v>373</v>
-      </c>
       <c r="AO17" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AP17">
         <v>0</v>
@@ -4721,7 +4721,7 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E18" t="s">
         <v>6</v>
@@ -4730,10 +4730,10 @@
         <v>185</v>
       </c>
       <c r="G18" t="s">
-        <v>364</v>
+        <v>186</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>96</v>
+        <v>669</v>
       </c>
       <c r="I18" t="s">
         <v>182</v>
@@ -4748,7 +4748,7 @@
         <v>186</v>
       </c>
       <c r="M18" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="N18" t="s">
         <v>186</v>
@@ -4775,7 +4775,7 @@
         <v>245</v>
       </c>
       <c r="V18" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="W18" t="s">
         <v>202</v>
@@ -4852,7 +4852,7 @@
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="E19" t="s">
         <v>6</v>
@@ -4861,10 +4861,10 @@
         <v>185</v>
       </c>
       <c r="G19" t="s">
-        <v>364</v>
+        <v>186</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>96</v>
+        <v>669</v>
       </c>
       <c r="I19" t="s">
         <v>182</v>
@@ -4879,7 +4879,7 @@
         <v>186</v>
       </c>
       <c r="M19" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="N19" t="s">
         <v>186</v>
@@ -4906,7 +4906,7 @@
         <v>245</v>
       </c>
       <c r="V19" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="W19" t="s">
         <v>210</v>
@@ -4983,7 +4983,7 @@
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="E20" t="s">
         <v>6</v>
@@ -4992,10 +4992,10 @@
         <v>185</v>
       </c>
       <c r="G20" t="s">
-        <v>364</v>
+        <v>186</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>96</v>
+        <v>669</v>
       </c>
       <c r="I20" t="s">
         <v>182</v>
@@ -5010,7 +5010,7 @@
         <v>186</v>
       </c>
       <c r="M20" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="N20" t="s">
         <v>186</v>
@@ -5037,7 +5037,7 @@
         <v>245</v>
       </c>
       <c r="V20" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="W20" t="s">
         <v>217</v>
@@ -5114,7 +5114,7 @@
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E21" t="s">
         <v>6</v>
@@ -5123,10 +5123,10 @@
         <v>185</v>
       </c>
       <c r="G21" t="s">
-        <v>364</v>
+        <v>186</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>96</v>
+        <v>669</v>
       </c>
       <c r="I21" t="s">
         <v>182</v>
@@ -5141,7 +5141,7 @@
         <v>186</v>
       </c>
       <c r="M21" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="N21" t="s">
         <v>186</v>
@@ -5168,7 +5168,7 @@
         <v>245</v>
       </c>
       <c r="V21" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="W21" t="s">
         <v>212</v>
@@ -5245,7 +5245,7 @@
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E22" t="s">
         <v>6</v>
@@ -5254,10 +5254,10 @@
         <v>185</v>
       </c>
       <c r="G22" t="s">
-        <v>364</v>
+        <v>186</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>96</v>
+        <v>669</v>
       </c>
       <c r="I22" t="s">
         <v>182</v>
@@ -5272,7 +5272,7 @@
         <v>186</v>
       </c>
       <c r="M22" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="N22" t="s">
         <v>186</v>
@@ -5299,7 +5299,7 @@
         <v>245</v>
       </c>
       <c r="V22" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="W22" t="s">
         <v>213</v>
@@ -5376,7 +5376,7 @@
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="E23" t="s">
         <v>6</v>
@@ -5385,10 +5385,10 @@
         <v>185</v>
       </c>
       <c r="G23" t="s">
-        <v>364</v>
+        <v>186</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>96</v>
+        <v>669</v>
       </c>
       <c r="I23" t="s">
         <v>182</v>
@@ -5403,7 +5403,7 @@
         <v>186</v>
       </c>
       <c r="M23" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="N23" t="s">
         <v>186</v>
@@ -5430,7 +5430,7 @@
         <v>245</v>
       </c>
       <c r="V23" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="W23" t="s">
         <v>214</v>
@@ -5507,7 +5507,7 @@
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E24" t="s">
         <v>6</v>
@@ -5516,10 +5516,10 @@
         <v>185</v>
       </c>
       <c r="G24" t="s">
-        <v>364</v>
+        <v>186</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>96</v>
+        <v>669</v>
       </c>
       <c r="I24" t="s">
         <v>182</v>
@@ -5534,7 +5534,7 @@
         <v>186</v>
       </c>
       <c r="M24" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="N24" t="s">
         <v>186</v>
@@ -5561,7 +5561,7 @@
         <v>245</v>
       </c>
       <c r="V24" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="W24" t="s">
         <v>215</v>
@@ -5638,7 +5638,7 @@
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="E25" t="s">
         <v>6</v>
@@ -5647,10 +5647,10 @@
         <v>185</v>
       </c>
       <c r="G25" t="s">
-        <v>364</v>
+        <v>186</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>96</v>
+        <v>669</v>
       </c>
       <c r="I25" t="s">
         <v>182</v>
@@ -5665,7 +5665,7 @@
         <v>186</v>
       </c>
       <c r="M25" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="N25" t="s">
         <v>186</v>
@@ -5692,7 +5692,7 @@
         <v>245</v>
       </c>
       <c r="V25" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="W25" t="s">
         <v>216</v>
@@ -5769,7 +5769,7 @@
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="E26" t="s">
         <v>6</v>
@@ -5778,10 +5778,10 @@
         <v>185</v>
       </c>
       <c r="G26" t="s">
-        <v>364</v>
+        <v>186</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>96</v>
+        <v>669</v>
       </c>
       <c r="I26" t="s">
         <v>182</v>
@@ -5796,7 +5796,7 @@
         <v>186</v>
       </c>
       <c r="M26" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="N26" t="s">
         <v>186</v>
@@ -5823,7 +5823,7 @@
         <v>245</v>
       </c>
       <c r="V26" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="W26" t="s">
         <v>211</v>
@@ -5900,7 +5900,7 @@
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="E27" t="s">
         <v>6</v>
@@ -5909,10 +5909,10 @@
         <v>185</v>
       </c>
       <c r="G27" t="s">
-        <v>364</v>
+        <v>186</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>96</v>
+        <v>669</v>
       </c>
       <c r="I27" t="s">
         <v>182</v>
@@ -5927,7 +5927,7 @@
         <v>186</v>
       </c>
       <c r="M27" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="N27" t="s">
         <v>186</v>
@@ -5954,7 +5954,7 @@
         <v>245</v>
       </c>
       <c r="V27" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="W27" t="s">
         <v>218</v>
@@ -6031,7 +6031,7 @@
         <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="E28" t="s">
         <v>6</v>
@@ -6040,10 +6040,10 @@
         <v>187</v>
       </c>
       <c r="G28" t="s">
-        <v>365</v>
+        <v>186</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I28" t="s">
         <v>182</v>
@@ -6058,7 +6058,7 @@
         <v>186</v>
       </c>
       <c r="M28" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="N28" t="s">
         <v>186</v>
@@ -6085,7 +6085,7 @@
         <v>245</v>
       </c>
       <c r="V28" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="W28" t="s">
         <v>202</v>
@@ -6162,7 +6162,7 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="E29" t="s">
         <v>6</v>
@@ -6171,10 +6171,10 @@
         <v>187</v>
       </c>
       <c r="G29" t="s">
-        <v>365</v>
+        <v>186</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I29" t="s">
         <v>182</v>
@@ -6189,7 +6189,7 @@
         <v>186</v>
       </c>
       <c r="M29" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="N29" t="s">
         <v>186</v>
@@ -6216,7 +6216,7 @@
         <v>245</v>
       </c>
       <c r="V29" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="W29" t="s">
         <v>210</v>
@@ -6293,7 +6293,7 @@
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="E30" t="s">
         <v>6</v>
@@ -6302,10 +6302,10 @@
         <v>187</v>
       </c>
       <c r="G30" t="s">
-        <v>365</v>
+        <v>186</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I30" t="s">
         <v>182</v>
@@ -6320,7 +6320,7 @@
         <v>186</v>
       </c>
       <c r="M30" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="N30" t="s">
         <v>186</v>
@@ -6347,7 +6347,7 @@
         <v>245</v>
       </c>
       <c r="V30" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="W30" t="s">
         <v>217</v>
@@ -6424,7 +6424,7 @@
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E31" t="s">
         <v>6</v>
@@ -6433,10 +6433,10 @@
         <v>187</v>
       </c>
       <c r="G31" t="s">
-        <v>365</v>
+        <v>186</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I31" t="s">
         <v>182</v>
@@ -6451,7 +6451,7 @@
         <v>186</v>
       </c>
       <c r="M31" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="N31" t="s">
         <v>186</v>
@@ -6478,7 +6478,7 @@
         <v>245</v>
       </c>
       <c r="V31" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="W31" t="s">
         <v>212</v>
@@ -6555,7 +6555,7 @@
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E32" t="s">
         <v>6</v>
@@ -6564,10 +6564,10 @@
         <v>187</v>
       </c>
       <c r="G32" t="s">
-        <v>365</v>
+        <v>186</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I32" t="s">
         <v>182</v>
@@ -6582,7 +6582,7 @@
         <v>186</v>
       </c>
       <c r="M32" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="N32" t="s">
         <v>186</v>
@@ -6609,7 +6609,7 @@
         <v>245</v>
       </c>
       <c r="V32" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="W32" t="s">
         <v>213</v>
@@ -6686,7 +6686,7 @@
         <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E33" t="s">
         <v>6</v>
@@ -6695,10 +6695,10 @@
         <v>187</v>
       </c>
       <c r="G33" t="s">
-        <v>365</v>
+        <v>186</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I33" t="s">
         <v>182</v>
@@ -6713,7 +6713,7 @@
         <v>186</v>
       </c>
       <c r="M33" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="N33" t="s">
         <v>186</v>
@@ -6740,7 +6740,7 @@
         <v>245</v>
       </c>
       <c r="V33" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="W33" t="s">
         <v>214</v>
@@ -6817,7 +6817,7 @@
         <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E34" t="s">
         <v>6</v>
@@ -6826,10 +6826,10 @@
         <v>187</v>
       </c>
       <c r="G34" t="s">
-        <v>365</v>
+        <v>186</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I34" t="s">
         <v>182</v>
@@ -6844,7 +6844,7 @@
         <v>186</v>
       </c>
       <c r="M34" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="N34" t="s">
         <v>186</v>
@@ -6871,7 +6871,7 @@
         <v>245</v>
       </c>
       <c r="V34" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="W34" t="s">
         <v>215</v>
@@ -6948,7 +6948,7 @@
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E35" t="s">
         <v>6</v>
@@ -6957,10 +6957,10 @@
         <v>187</v>
       </c>
       <c r="G35" t="s">
-        <v>365</v>
+        <v>186</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I35" t="s">
         <v>182</v>
@@ -6975,7 +6975,7 @@
         <v>186</v>
       </c>
       <c r="M35" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="N35" t="s">
         <v>186</v>
@@ -7002,7 +7002,7 @@
         <v>245</v>
       </c>
       <c r="V35" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="W35" t="s">
         <v>216</v>
@@ -7079,7 +7079,7 @@
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="E36" t="s">
         <v>6</v>
@@ -7088,10 +7088,10 @@
         <v>187</v>
       </c>
       <c r="G36" t="s">
-        <v>365</v>
+        <v>186</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I36" t="s">
         <v>182</v>
@@ -7106,7 +7106,7 @@
         <v>186</v>
       </c>
       <c r="M36" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="N36" t="s">
         <v>186</v>
@@ -7133,7 +7133,7 @@
         <v>245</v>
       </c>
       <c r="V36" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="W36" t="s">
         <v>211</v>
@@ -7210,7 +7210,7 @@
         <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="E37" t="s">
         <v>6</v>
@@ -7219,10 +7219,10 @@
         <v>187</v>
       </c>
       <c r="G37" t="s">
-        <v>365</v>
+        <v>186</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I37" t="s">
         <v>182</v>
@@ -7237,7 +7237,7 @@
         <v>186</v>
       </c>
       <c r="M37" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="N37" t="s">
         <v>186</v>
@@ -7264,7 +7264,7 @@
         <v>245</v>
       </c>
       <c r="V37" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="W37" t="s">
         <v>218</v>
@@ -7341,7 +7341,7 @@
         <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E38" t="s">
         <v>3</v>
@@ -7350,13 +7350,13 @@
         <v>185</v>
       </c>
       <c r="G38" s="12" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H38" t="s">
         <v>97</v>
       </c>
       <c r="I38" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J38" t="s">
         <v>183</v>
@@ -7472,7 +7472,7 @@
         <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E39" t="s">
         <v>3</v>
@@ -7487,7 +7487,7 @@
         <v>108</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J39" t="s">
         <v>183</v>
@@ -7603,7 +7603,7 @@
         <v>5</v>
       </c>
       <c r="D40" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E40" t="s">
         <v>6</v>
@@ -7618,7 +7618,7 @@
         <v>246</v>
       </c>
       <c r="I40" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J40" t="s">
         <v>183</v>
@@ -7734,7 +7734,7 @@
         <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="E41" t="s">
         <v>6</v>
@@ -7865,7 +7865,7 @@
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="E42" t="s">
         <v>6</v>
@@ -7996,7 +7996,7 @@
         <v>2</v>
       </c>
       <c r="D43" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E43" t="s">
         <v>3</v>
@@ -8011,7 +8011,7 @@
         <v>101</v>
       </c>
       <c r="I43" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J43" t="s">
         <v>346</v>
@@ -8127,7 +8127,7 @@
         <v>5</v>
       </c>
       <c r="D44" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="E44" t="s">
         <v>6</v>
@@ -8142,7 +8142,7 @@
         <v>101</v>
       </c>
       <c r="I44" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J44" t="s">
         <v>346</v>
@@ -8258,7 +8258,7 @@
         <v>2</v>
       </c>
       <c r="D45" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="E45" t="s">
         <v>3</v>
@@ -8273,7 +8273,7 @@
         <v>103</v>
       </c>
       <c r="I45" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J45" t="s">
         <v>186</v>
@@ -8389,7 +8389,7 @@
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E46" t="s">
         <v>3</v>
@@ -8404,7 +8404,7 @@
         <v>105</v>
       </c>
       <c r="I46" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J46" t="s">
         <v>186</v>
@@ -8416,7 +8416,7 @@
         <v>266</v>
       </c>
       <c r="M46" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="N46" t="s">
         <v>186</v>
@@ -8520,7 +8520,7 @@
         <v>2</v>
       </c>
       <c r="D47" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="E47" t="s">
         <v>3</v>
@@ -8535,7 +8535,7 @@
         <v>105</v>
       </c>
       <c r="I47" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J47" t="s">
         <v>186</v>
@@ -8547,7 +8547,7 @@
         <v>266</v>
       </c>
       <c r="M47" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="N47" t="s">
         <v>186</v>
@@ -8651,7 +8651,7 @@
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E48" t="s">
         <v>3</v>
@@ -8660,13 +8660,13 @@
         <v>185</v>
       </c>
       <c r="G48" s="12" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H48" t="s">
         <v>107</v>
       </c>
       <c r="I48" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J48" t="s">
         <v>186</v>
@@ -8782,7 +8782,7 @@
         <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="E49" t="s">
         <v>3</v>
@@ -8797,7 +8797,7 @@
         <v>98</v>
       </c>
       <c r="I49" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J49" t="s">
         <v>186</v>
@@ -8913,7 +8913,7 @@
         <v>2</v>
       </c>
       <c r="D50" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E50" t="s">
         <v>3</v>
@@ -8928,7 +8928,7 @@
         <v>109</v>
       </c>
       <c r="I50" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J50" t="s">
         <v>186</v>
@@ -9044,7 +9044,7 @@
         <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E51" t="s">
         <v>3</v>
@@ -9059,7 +9059,7 @@
         <v>111</v>
       </c>
       <c r="I51" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J51" t="s">
         <v>183</v>
@@ -9175,7 +9175,7 @@
         <v>5</v>
       </c>
       <c r="D52" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E52" t="s">
         <v>6</v>
@@ -9190,7 +9190,7 @@
         <v>111</v>
       </c>
       <c r="I52" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J52" t="s">
         <v>183</v>
@@ -9306,7 +9306,7 @@
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E53" t="s">
         <v>3</v>
@@ -9321,7 +9321,7 @@
         <v>112</v>
       </c>
       <c r="I53" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J53" t="s">
         <v>221</v>
@@ -9437,7 +9437,7 @@
         <v>2</v>
       </c>
       <c r="D54" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="E54" t="s">
         <v>3</v>
@@ -9452,7 +9452,7 @@
         <v>114</v>
       </c>
       <c r="I54" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J54" t="s">
         <v>186</v>
@@ -9568,7 +9568,7 @@
         <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E55" t="s">
         <v>3</v>
@@ -9583,7 +9583,7 @@
         <v>116</v>
       </c>
       <c r="I55" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J55" t="s">
         <v>186</v>
@@ -9699,7 +9699,7 @@
         <v>5</v>
       </c>
       <c r="D56" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E56" t="s">
         <v>6</v>
@@ -9714,7 +9714,7 @@
         <v>343</v>
       </c>
       <c r="I56" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J56" t="s">
         <v>186</v>
@@ -9842,106 +9842,106 @@
         <v>186</v>
       </c>
       <c r="H57" s="15" t="s">
+        <v>606</v>
+      </c>
+      <c r="I57" t="s">
+        <v>667</v>
+      </c>
+      <c r="J57" t="s">
+        <v>186</v>
+      </c>
+      <c r="K57" t="s">
+        <v>186</v>
+      </c>
+      <c r="L57" t="s">
+        <v>553</v>
+      </c>
+      <c r="M57" t="s">
+        <v>186</v>
+      </c>
+      <c r="N57" t="s">
+        <v>186</v>
+      </c>
+      <c r="O57" t="s">
+        <v>186</v>
+      </c>
+      <c r="P57" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>186</v>
+      </c>
+      <c r="R57" t="s">
+        <v>186</v>
+      </c>
+      <c r="S57" t="s">
+        <v>186</v>
+      </c>
+      <c r="T57" t="s">
+        <v>186</v>
+      </c>
+      <c r="U57" t="s">
+        <v>186</v>
+      </c>
+      <c r="V57" t="s">
+        <v>186</v>
+      </c>
+      <c r="W57" t="s">
+        <v>186</v>
+      </c>
+      <c r="X57" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y57" t="s">
         <v>607</v>
       </c>
-      <c r="I57" t="s">
-        <v>668</v>
-      </c>
-      <c r="J57" t="s">
-        <v>186</v>
-      </c>
-      <c r="K57" t="s">
-        <v>186</v>
-      </c>
-      <c r="L57" t="s">
-        <v>554</v>
-      </c>
-      <c r="M57" t="s">
-        <v>186</v>
-      </c>
-      <c r="N57" t="s">
-        <v>186</v>
-      </c>
-      <c r="O57" t="s">
-        <v>186</v>
-      </c>
-      <c r="P57" t="s">
-        <v>186</v>
-      </c>
-      <c r="Q57" t="s">
-        <v>186</v>
-      </c>
-      <c r="R57" t="s">
-        <v>186</v>
-      </c>
-      <c r="S57" t="s">
-        <v>186</v>
-      </c>
-      <c r="T57" t="s">
-        <v>186</v>
-      </c>
-      <c r="U57" t="s">
-        <v>186</v>
-      </c>
-      <c r="V57" t="s">
-        <v>186</v>
-      </c>
-      <c r="W57" t="s">
-        <v>186</v>
-      </c>
-      <c r="X57" t="s">
-        <v>186</v>
-      </c>
-      <c r="Y57" t="s">
+      <c r="Z57" t="s">
+        <v>667</v>
+      </c>
+      <c r="AA57" t="s">
+        <v>186</v>
+      </c>
+      <c r="AB57" t="s">
+        <v>186</v>
+      </c>
+      <c r="AC57" t="s">
+        <v>553</v>
+      </c>
+      <c r="AD57" t="s">
+        <v>186</v>
+      </c>
+      <c r="AE57" t="s">
+        <v>186</v>
+      </c>
+      <c r="AF57" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG57" t="s">
+        <v>186</v>
+      </c>
+      <c r="AH57" t="s">
+        <v>186</v>
+      </c>
+      <c r="AI57" t="s">
+        <v>186</v>
+      </c>
+      <c r="AJ57" t="s">
+        <v>186</v>
+      </c>
+      <c r="AK57" t="s">
+        <v>186</v>
+      </c>
+      <c r="AL57" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM57" t="s">
+        <v>186</v>
+      </c>
+      <c r="AN57" t="s">
+        <v>186</v>
+      </c>
+      <c r="AO57" t="s">
         <v>608</v>
-      </c>
-      <c r="Z57" t="s">
-        <v>668</v>
-      </c>
-      <c r="AA57" t="s">
-        <v>186</v>
-      </c>
-      <c r="AB57" t="s">
-        <v>186</v>
-      </c>
-      <c r="AC57" t="s">
-        <v>554</v>
-      </c>
-      <c r="AD57" t="s">
-        <v>186</v>
-      </c>
-      <c r="AE57" t="s">
-        <v>186</v>
-      </c>
-      <c r="AF57" t="s">
-        <v>186</v>
-      </c>
-      <c r="AG57" t="s">
-        <v>186</v>
-      </c>
-      <c r="AH57" t="s">
-        <v>186</v>
-      </c>
-      <c r="AI57" t="s">
-        <v>186</v>
-      </c>
-      <c r="AJ57" t="s">
-        <v>186</v>
-      </c>
-      <c r="AK57" t="s">
-        <v>186</v>
-      </c>
-      <c r="AL57" t="s">
-        <v>186</v>
-      </c>
-      <c r="AM57" t="s">
-        <v>186</v>
-      </c>
-      <c r="AN57" t="s">
-        <v>186</v>
-      </c>
-      <c r="AO57" t="s">
-        <v>609</v>
       </c>
       <c r="AP57">
         <v>0</v>
@@ -9973,61 +9973,61 @@
         <v>186</v>
       </c>
       <c r="H58" s="15" t="s">
+        <v>609</v>
+      </c>
+      <c r="I58" t="s">
+        <v>667</v>
+      </c>
+      <c r="J58" t="s">
+        <v>186</v>
+      </c>
+      <c r="K58" t="s">
+        <v>186</v>
+      </c>
+      <c r="L58" t="s">
+        <v>522</v>
+      </c>
+      <c r="M58" t="s">
+        <v>186</v>
+      </c>
+      <c r="N58" t="s">
+        <v>186</v>
+      </c>
+      <c r="O58" t="s">
+        <v>186</v>
+      </c>
+      <c r="P58" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>186</v>
+      </c>
+      <c r="R58" t="s">
+        <v>186</v>
+      </c>
+      <c r="S58" t="s">
+        <v>186</v>
+      </c>
+      <c r="T58" t="s">
+        <v>186</v>
+      </c>
+      <c r="U58" t="s">
+        <v>186</v>
+      </c>
+      <c r="V58" t="s">
+        <v>186</v>
+      </c>
+      <c r="W58" t="s">
+        <v>186</v>
+      </c>
+      <c r="X58" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y58" t="s">
         <v>610</v>
       </c>
-      <c r="I58" t="s">
-        <v>668</v>
-      </c>
-      <c r="J58" t="s">
-        <v>186</v>
-      </c>
-      <c r="K58" t="s">
-        <v>186</v>
-      </c>
-      <c r="L58" t="s">
-        <v>523</v>
-      </c>
-      <c r="M58" t="s">
-        <v>186</v>
-      </c>
-      <c r="N58" t="s">
-        <v>186</v>
-      </c>
-      <c r="O58" t="s">
-        <v>186</v>
-      </c>
-      <c r="P58" t="s">
-        <v>186</v>
-      </c>
-      <c r="Q58" t="s">
-        <v>186</v>
-      </c>
-      <c r="R58" t="s">
-        <v>186</v>
-      </c>
-      <c r="S58" t="s">
-        <v>186</v>
-      </c>
-      <c r="T58" t="s">
-        <v>186</v>
-      </c>
-      <c r="U58" t="s">
-        <v>186</v>
-      </c>
-      <c r="V58" t="s">
-        <v>186</v>
-      </c>
-      <c r="W58" t="s">
-        <v>186</v>
-      </c>
-      <c r="X58" t="s">
-        <v>186</v>
-      </c>
-      <c r="Y58" t="s">
-        <v>611</v>
-      </c>
       <c r="Z58" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="AA58" t="s">
         <v>186</v>
@@ -10036,7 +10036,7 @@
         <v>186</v>
       </c>
       <c r="AC58" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="AD58" t="s">
         <v>186</v>
@@ -10072,7 +10072,7 @@
         <v>186</v>
       </c>
       <c r="AO58" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AP58">
         <v>0</v>
@@ -10083,10 +10083,10 @@
     </row>
     <row r="59" spans="1:43" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B59" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C59" t="s">
         <v>2</v>
@@ -10104,10 +10104,10 @@
         <v>186</v>
       </c>
       <c r="H59" t="s">
+        <v>604</v>
+      </c>
+      <c r="I59" t="s">
         <v>605</v>
-      </c>
-      <c r="I59" t="s">
-        <v>606</v>
       </c>
       <c r="J59" t="s">
         <v>186</v>
@@ -11073,31 +11073,31 @@
         <v>331</v>
       </c>
       <c r="Y1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Z1" t="s">
+        <v>412</v>
+      </c>
+      <c r="AA1" t="s">
         <v>413</v>
       </c>
-      <c r="AA1" t="s">
-        <v>414</v>
-      </c>
       <c r="AB1" t="s">
+        <v>440</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>433</v>
+      </c>
+      <c r="AD1" t="s">
         <v>441</v>
       </c>
-      <c r="AC1" t="s">
-        <v>434</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>442</v>
-      </c>
       <c r="AE1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AF1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="AG1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
@@ -11108,19 +11108,19 @@
         <v>350</v>
       </c>
       <c r="C2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D2" t="s">
         <v>330</v>
       </c>
       <c r="E2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F2" t="s">
+        <v>570</v>
+      </c>
+      <c r="G2" t="s">
         <v>571</v>
-      </c>
-      <c r="G2" t="s">
-        <v>572</v>
       </c>
       <c r="H2">
         <v>3</v>
@@ -11141,7 +11141,7 @@
       <c r="R2" s="9"/>
       <c r="T2" s="9"/>
       <c r="Z2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
@@ -11152,19 +11152,19 @@
         <v>350</v>
       </c>
       <c r="C3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D3" t="s">
         <v>330</v>
       </c>
       <c r="E3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F3" t="s">
+        <v>414</v>
+      </c>
+      <c r="G3" t="s">
         <v>415</v>
-      </c>
-      <c r="G3" t="s">
-        <v>416</v>
       </c>
       <c r="H3">
         <v>7</v>
@@ -11185,7 +11185,7 @@
       <c r="R3" s="9"/>
       <c r="T3" s="9"/>
       <c r="AA3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.2">
@@ -11202,7 +11202,7 @@
         <v>330</v>
       </c>
       <c r="E4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F4" t="s">
         <v>135</v>
@@ -11244,7 +11244,7 @@
         <v>330</v>
       </c>
       <c r="E5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F5" t="s">
         <v>135</v>
@@ -11281,7 +11281,7 @@
         <v>330</v>
       </c>
       <c r="E6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F6" t="s">
         <v>135</v>
@@ -11314,7 +11314,7 @@
         <v>330</v>
       </c>
       <c r="E7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F7" t="s">
         <v>133</v>
@@ -11364,7 +11364,7 @@
         <v>330</v>
       </c>
       <c r="E8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F8" t="s">
         <v>133</v>
@@ -11400,7 +11400,7 @@
         <v>330</v>
       </c>
       <c r="E9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F9" t="s">
         <v>133</v>
@@ -11439,7 +11439,7 @@
         <v>330</v>
       </c>
       <c r="E10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F10" t="s">
         <v>134</v>
@@ -11486,7 +11486,7 @@
         <v>330</v>
       </c>
       <c r="E11" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F11" t="s">
         <v>134</v>
@@ -11522,7 +11522,7 @@
         <v>330</v>
       </c>
       <c r="E12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F12" t="s">
         <v>142</v>
@@ -11574,7 +11574,7 @@
         <v>330</v>
       </c>
       <c r="E13" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F13" t="s">
         <v>142</v>
@@ -11652,7 +11652,7 @@
         <v>330</v>
       </c>
       <c r="E15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F15" t="s">
         <v>146</v>
@@ -11671,7 +11671,7 @@
         <v>&lt;15/&gt;15</v>
       </c>
       <c r="P15" s="9" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -11726,7 +11726,7 @@
         <v>330</v>
       </c>
       <c r="E17" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F17" t="s">
         <v>143</v>
@@ -11762,7 +11762,7 @@
         <v>330</v>
       </c>
       <c r="E18" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F18" t="s">
         <v>144</v>
@@ -11798,7 +11798,7 @@
         <v>330</v>
       </c>
       <c r="E19" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F19" t="s">
         <v>144</v>
@@ -11891,7 +11891,7 @@
         <v>330</v>
       </c>
       <c r="E21" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F21" t="s">
         <v>147</v>
@@ -11910,7 +11910,7 @@
         <v>&lt;15/&gt;15</v>
       </c>
       <c r="P21" s="9" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
@@ -11969,7 +11969,7 @@
         <v>330</v>
       </c>
       <c r="E23" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F23" t="s">
         <v>347</v>
@@ -12010,7 +12010,7 @@
         <v>330</v>
       </c>
       <c r="E24" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F24" t="s">
         <v>145</v>
@@ -12046,7 +12046,7 @@
         <v>330</v>
       </c>
       <c r="E25" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F25" t="s">
         <v>145</v>
@@ -12139,7 +12139,7 @@
         <v>330</v>
       </c>
       <c r="E27" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F27" t="s">
         <v>136</v>
@@ -12175,7 +12175,7 @@
         <v>330</v>
       </c>
       <c r="E28" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F28" t="s">
         <v>136</v>
@@ -12228,7 +12228,7 @@
         <v>330</v>
       </c>
       <c r="E29" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F29" t="s">
         <v>136</v>
@@ -12306,7 +12306,7 @@
         <v>330</v>
       </c>
       <c r="E31" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F31" t="s">
         <v>347</v>
@@ -12342,7 +12342,7 @@
         <v>330</v>
       </c>
       <c r="E32" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F32" t="s">
         <v>137</v>
@@ -12378,7 +12378,7 @@
         <v>330</v>
       </c>
       <c r="E33" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F33" t="s">
         <v>137</v>
@@ -12414,7 +12414,7 @@
         <v>330</v>
       </c>
       <c r="E34" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F34" t="s">
         <v>137</v>
@@ -12509,7 +12509,7 @@
         <v>330</v>
       </c>
       <c r="E36" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F36" t="s">
         <v>138</v>
@@ -12545,7 +12545,7 @@
         <v>330</v>
       </c>
       <c r="E37" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F37" t="s">
         <v>138</v>
@@ -12581,7 +12581,7 @@
         <v>330</v>
       </c>
       <c r="E38" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F38" t="s">
         <v>138</v>
@@ -12674,7 +12674,7 @@
         <v>330</v>
       </c>
       <c r="E40" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F40" t="s">
         <v>139</v>
@@ -12710,7 +12710,7 @@
         <v>330</v>
       </c>
       <c r="E41" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F41" t="s">
         <v>139</v>
@@ -12746,7 +12746,7 @@
         <v>330</v>
       </c>
       <c r="E42" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F42" t="s">
         <v>139</v>
@@ -12839,7 +12839,7 @@
         <v>330</v>
       </c>
       <c r="E44" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F44" t="s">
         <v>140</v>
@@ -12875,7 +12875,7 @@
         <v>330</v>
       </c>
       <c r="E45" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F45" t="s">
         <v>140</v>
@@ -12911,7 +12911,7 @@
         <v>330</v>
       </c>
       <c r="E46" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F46" t="s">
         <v>140</v>
@@ -13004,7 +13004,7 @@
         <v>330</v>
       </c>
       <c r="E48" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F48" t="s">
         <v>141</v>
@@ -13040,7 +13040,7 @@
         <v>330</v>
       </c>
       <c r="E49" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F49" t="s">
         <v>141</v>
@@ -13566,7 +13566,7 @@
         <v>269</v>
       </c>
       <c r="D62" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E62" t="s">
         <v>270</v>
@@ -13588,7 +13588,7 @@
         <v>tr_pos</v>
       </c>
       <c r="Y62" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="63" spans="1:28" x14ac:dyDescent="0.2">
@@ -13602,7 +13602,7 @@
         <v>271</v>
       </c>
       <c r="D63" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E63" t="s">
         <v>272</v>
@@ -13624,30 +13624,30 @@
         <v>tr_neg</v>
       </c>
       <c r="Y63" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="64" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>416</v>
+      </c>
+      <c r="B64" t="s">
         <v>417</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
+        <v>419</v>
+      </c>
+      <c r="D64" t="s">
+        <v>440</v>
+      </c>
+      <c r="E64" t="s">
         <v>418</v>
       </c>
-      <c r="C64" t="s">
-        <v>420</v>
-      </c>
-      <c r="D64" t="s">
-        <v>441</v>
-      </c>
-      <c r="E64" t="s">
-        <v>419</v>
-      </c>
       <c r="F64" t="s">
+        <v>428</v>
+      </c>
+      <c r="G64" t="s">
         <v>429</v>
-      </c>
-      <c r="G64" t="s">
-        <v>430</v>
       </c>
       <c r="H64">
         <v>10</v>
@@ -13660,30 +13660,30 @@
         <v>tss_NewPos</v>
       </c>
       <c r="AB64" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="65" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>416</v>
+      </c>
+      <c r="B65" t="s">
         <v>417</v>
       </c>
-      <c r="B65" t="s">
-        <v>418</v>
-      </c>
       <c r="C65" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D65" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E65" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F65" t="s">
+        <v>424</v>
+      </c>
+      <c r="G65" t="s">
         <v>425</v>
-      </c>
-      <c r="G65" t="s">
-        <v>426</v>
       </c>
       <c r="H65">
         <v>20</v>
@@ -13696,30 +13696,30 @@
         <v>tss_KnowPos</v>
       </c>
       <c r="AB65" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="66" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>416</v>
+      </c>
+      <c r="B66" t="s">
         <v>417</v>
       </c>
-      <c r="B66" t="s">
-        <v>418</v>
-      </c>
       <c r="C66" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D66" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E66" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F66" t="s">
+        <v>426</v>
+      </c>
+      <c r="G66" t="s">
         <v>427</v>
-      </c>
-      <c r="G66" t="s">
-        <v>428</v>
       </c>
       <c r="H66">
         <v>30</v>
@@ -13732,30 +13732,30 @@
         <v>tss_NewNeg</v>
       </c>
       <c r="AB66" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="67" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>430</v>
+      </c>
+      <c r="B67" t="s">
+        <v>568</v>
+      </c>
+      <c r="C67" t="s">
         <v>431</v>
       </c>
-      <c r="B67" t="s">
-        <v>569</v>
-      </c>
-      <c r="C67" t="s">
-        <v>432</v>
-      </c>
       <c r="D67" t="s">
+        <v>433</v>
+      </c>
+      <c r="E67" t="s">
         <v>434</v>
       </c>
-      <c r="E67" t="s">
+      <c r="F67" t="s">
+        <v>434</v>
+      </c>
+      <c r="G67" t="s">
         <v>435</v>
-      </c>
-      <c r="F67" t="s">
-        <v>435</v>
-      </c>
-      <c r="G67" t="s">
-        <v>436</v>
       </c>
       <c r="H67">
         <v>1</v>
@@ -13768,30 +13768,30 @@
         <v>vt_sv</v>
       </c>
       <c r="AC67" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="68" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B68" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C68" t="s">
+        <v>432</v>
+      </c>
+      <c r="D68" t="s">
         <v>433</v>
       </c>
-      <c r="D68" t="s">
-        <v>434</v>
-      </c>
       <c r="E68" t="s">
+        <v>438</v>
+      </c>
+      <c r="F68" t="s">
+        <v>438</v>
+      </c>
+      <c r="G68" t="s">
         <v>439</v>
-      </c>
-      <c r="F68" t="s">
-        <v>439</v>
-      </c>
-      <c r="G68" t="s">
-        <v>440</v>
       </c>
       <c r="H68">
         <v>2</v>
@@ -13804,30 +13804,30 @@
         <v>vt_pe</v>
       </c>
       <c r="AC68" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="69" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B69" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C69" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D69" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E69" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F69" t="s">
+        <v>508</v>
+      </c>
+      <c r="G69" t="s">
         <v>509</v>
-      </c>
-      <c r="G69" t="s">
-        <v>510</v>
       </c>
       <c r="H69">
         <v>10</v>
@@ -13840,30 +13840,30 @@
         <v>st_da</v>
       </c>
       <c r="AD69" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="70" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B70" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C70" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D70" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E70" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F70" t="s">
+        <v>508</v>
+      </c>
+      <c r="G70" t="s">
         <v>509</v>
-      </c>
-      <c r="G70" t="s">
-        <v>510</v>
       </c>
       <c r="H70">
         <v>20</v>
@@ -13876,30 +13876,30 @@
         <v>st_da</v>
       </c>
       <c r="AD70" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="71" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B71" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C71" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D71" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E71" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F71" t="s">
+        <v>508</v>
+      </c>
+      <c r="G71" t="s">
         <v>509</v>
-      </c>
-      <c r="G71" t="s">
-        <v>510</v>
       </c>
       <c r="H71">
         <v>30</v>
@@ -13912,30 +13912,30 @@
         <v>st_da</v>
       </c>
       <c r="AD71" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="72" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B72" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C72" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D72" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E72" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F72" t="s">
+        <v>508</v>
+      </c>
+      <c r="G72" t="s">
         <v>509</v>
-      </c>
-      <c r="G72" t="s">
-        <v>510</v>
       </c>
       <c r="H72">
         <v>40</v>
@@ -13948,30 +13948,30 @@
         <v>st_da</v>
       </c>
       <c r="AD72" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="73" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B73" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C73" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D73" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E73" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F73" t="s">
+        <v>508</v>
+      </c>
+      <c r="G73" t="s">
         <v>509</v>
-      </c>
-      <c r="G73" t="s">
-        <v>510</v>
       </c>
       <c r="H73">
         <v>50</v>
@@ -13984,30 +13984,30 @@
         <v>st_da</v>
       </c>
       <c r="AD73" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="74" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B74" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C74" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D74" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E74" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F74" t="s">
+        <v>508</v>
+      </c>
+      <c r="G74" t="s">
         <v>509</v>
-      </c>
-      <c r="G74" t="s">
-        <v>510</v>
       </c>
       <c r="H74">
         <v>60</v>
@@ -14020,30 +14020,30 @@
         <v>st_da</v>
       </c>
       <c r="AD74" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="75" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B75" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C75" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D75" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E75" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F75" t="s">
+        <v>508</v>
+      </c>
+      <c r="G75" t="s">
         <v>509</v>
-      </c>
-      <c r="G75" t="s">
-        <v>510</v>
       </c>
       <c r="H75">
         <v>70</v>
@@ -14056,30 +14056,30 @@
         <v>st_da</v>
       </c>
       <c r="AD75" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="76" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B76" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C76" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D76" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E76" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F76" t="s">
+        <v>508</v>
+      </c>
+      <c r="G76" t="s">
         <v>509</v>
-      </c>
-      <c r="G76" t="s">
-        <v>510</v>
       </c>
       <c r="H76">
         <v>80</v>
@@ -14092,30 +14092,30 @@
         <v>st_da</v>
       </c>
       <c r="AD76" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="77" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B77" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C77" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D77" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E77" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F77" t="s">
+        <v>508</v>
+      </c>
+      <c r="G77" t="s">
         <v>509</v>
-      </c>
-      <c r="G77" t="s">
-        <v>510</v>
       </c>
       <c r="H77">
         <v>90</v>
@@ -14128,30 +14128,30 @@
         <v>st_da</v>
       </c>
       <c r="AD77" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="78" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B78" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C78" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D78" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E78" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F78" t="s">
+        <v>508</v>
+      </c>
+      <c r="G78" t="s">
         <v>509</v>
-      </c>
-      <c r="G78" t="s">
-        <v>510</v>
       </c>
       <c r="H78">
         <v>100</v>
@@ -14164,30 +14164,30 @@
         <v>st_da</v>
       </c>
       <c r="AD78" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="79" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B79" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C79" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D79" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E79" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F79" t="s">
+        <v>508</v>
+      </c>
+      <c r="G79" t="s">
         <v>509</v>
-      </c>
-      <c r="G79" t="s">
-        <v>510</v>
       </c>
       <c r="H79">
         <v>110</v>
@@ -14200,30 +14200,30 @@
         <v>st_da</v>
       </c>
       <c r="AD79" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="80" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B80" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C80" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D80" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E80" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F80" t="s">
+        <v>508</v>
+      </c>
+      <c r="G80" t="s">
         <v>509</v>
-      </c>
-      <c r="G80" t="s">
-        <v>510</v>
       </c>
       <c r="H80">
         <v>120</v>
@@ -14236,30 +14236,30 @@
         <v>st_da</v>
       </c>
       <c r="AD80" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="81" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B81" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C81" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D81" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E81" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F81" t="s">
+        <v>508</v>
+      </c>
+      <c r="G81" t="s">
         <v>509</v>
-      </c>
-      <c r="G81" t="s">
-        <v>510</v>
       </c>
       <c r="H81">
         <v>130</v>
@@ -14272,30 +14272,30 @@
         <v>st_da</v>
       </c>
       <c r="AD81" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="82" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B82" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C82" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D82" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E82" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F82" t="s">
+        <v>508</v>
+      </c>
+      <c r="G82" t="s">
         <v>509</v>
-      </c>
-      <c r="G82" t="s">
-        <v>510</v>
       </c>
       <c r="H82">
         <v>140</v>
@@ -14308,30 +14308,30 @@
         <v>st_da</v>
       </c>
       <c r="AD82" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="83" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B83" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C83" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D83" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E83" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F83" t="s">
+        <v>508</v>
+      </c>
+      <c r="G83" t="s">
         <v>509</v>
-      </c>
-      <c r="G83" t="s">
-        <v>510</v>
       </c>
       <c r="H83">
         <v>150</v>
@@ -14344,30 +14344,30 @@
         <v>st_da</v>
       </c>
       <c r="AD83" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="84" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B84" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C84" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D84" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E84" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F84" t="s">
+        <v>508</v>
+      </c>
+      <c r="G84" t="s">
         <v>509</v>
-      </c>
-      <c r="G84" t="s">
-        <v>510</v>
       </c>
       <c r="H84">
         <v>160</v>
@@ -14380,30 +14380,30 @@
         <v>st_da</v>
       </c>
       <c r="AD84" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="85" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B85" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C85" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D85" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E85" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F85" t="s">
+        <v>510</v>
+      </c>
+      <c r="G85" t="s">
         <v>511</v>
-      </c>
-      <c r="G85" t="s">
-        <v>512</v>
       </c>
       <c r="H85">
         <v>170</v>
@@ -14416,30 +14416,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD85" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="86" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B86" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C86" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D86" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E86" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F86" t="s">
+        <v>510</v>
+      </c>
+      <c r="G86" t="s">
         <v>511</v>
-      </c>
-      <c r="G86" t="s">
-        <v>512</v>
       </c>
       <c r="H86">
         <v>180</v>
@@ -14452,30 +14452,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD86" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="87" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B87" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C87" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D87" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E87" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F87" t="s">
+        <v>510</v>
+      </c>
+      <c r="G87" t="s">
         <v>511</v>
-      </c>
-      <c r="G87" t="s">
-        <v>512</v>
       </c>
       <c r="H87">
         <v>190</v>
@@ -14488,30 +14488,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD87" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="88" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B88" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C88" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D88" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E88" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F88" t="s">
+        <v>510</v>
+      </c>
+      <c r="G88" t="s">
         <v>511</v>
-      </c>
-      <c r="G88" t="s">
-        <v>512</v>
       </c>
       <c r="H88">
         <v>200</v>
@@ -14524,30 +14524,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD88" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="89" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B89" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C89" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D89" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E89" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F89" t="s">
+        <v>510</v>
+      </c>
+      <c r="G89" t="s">
         <v>511</v>
-      </c>
-      <c r="G89" t="s">
-        <v>512</v>
       </c>
       <c r="H89">
         <v>210</v>
@@ -14560,30 +14560,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD89" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="90" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B90" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C90" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D90" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E90" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F90" t="s">
+        <v>510</v>
+      </c>
+      <c r="G90" t="s">
         <v>511</v>
-      </c>
-      <c r="G90" t="s">
-        <v>512</v>
       </c>
       <c r="H90">
         <v>220</v>
@@ -14596,30 +14596,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD90" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="91" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B91" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C91" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D91" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E91" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F91" t="s">
+        <v>510</v>
+      </c>
+      <c r="G91" t="s">
         <v>511</v>
-      </c>
-      <c r="G91" t="s">
-        <v>512</v>
       </c>
       <c r="H91">
         <v>230</v>
@@ -14632,30 +14632,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD91" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="92" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B92" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C92" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D92" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E92" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F92" t="s">
+        <v>510</v>
+      </c>
+      <c r="G92" t="s">
         <v>511</v>
-      </c>
-      <c r="G92" t="s">
-        <v>512</v>
       </c>
       <c r="H92">
         <v>240</v>
@@ -14668,30 +14668,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD92" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="93" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B93" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C93" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D93" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E93" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F93" t="s">
+        <v>510</v>
+      </c>
+      <c r="G93" t="s">
         <v>511</v>
-      </c>
-      <c r="G93" t="s">
-        <v>512</v>
       </c>
       <c r="H93">
         <v>250</v>
@@ -14704,30 +14704,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD93" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="94" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B94" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C94" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D94" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E94" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F94" t="s">
+        <v>510</v>
+      </c>
+      <c r="G94" t="s">
         <v>511</v>
-      </c>
-      <c r="G94" t="s">
-        <v>512</v>
       </c>
       <c r="H94">
         <v>260</v>
@@ -14740,30 +14740,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD94" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="95" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B95" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C95" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D95" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E95" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F95" t="s">
+        <v>510</v>
+      </c>
+      <c r="G95" t="s">
         <v>511</v>
-      </c>
-      <c r="G95" t="s">
-        <v>512</v>
       </c>
       <c r="H95">
         <v>270</v>
@@ -14776,30 +14776,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD95" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="96" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B96" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C96" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D96" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E96" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F96" t="s">
+        <v>510</v>
+      </c>
+      <c r="G96" t="s">
         <v>511</v>
-      </c>
-      <c r="G96" t="s">
-        <v>512</v>
       </c>
       <c r="H96">
         <v>280</v>
@@ -14812,30 +14812,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD96" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="97" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B97" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C97" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D97" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E97" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F97" t="s">
+        <v>510</v>
+      </c>
+      <c r="G97" t="s">
         <v>511</v>
-      </c>
-      <c r="G97" t="s">
-        <v>512</v>
       </c>
       <c r="H97">
         <v>290</v>
@@ -14848,30 +14848,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD97" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="98" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B98" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C98" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D98" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E98" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F98" t="s">
+        <v>510</v>
+      </c>
+      <c r="G98" t="s">
         <v>511</v>
-      </c>
-      <c r="G98" t="s">
-        <v>512</v>
       </c>
       <c r="H98">
         <v>300</v>
@@ -14884,30 +14884,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD98" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="99" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B99" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C99" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D99" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E99" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F99" t="s">
+        <v>510</v>
+      </c>
+      <c r="G99" t="s">
         <v>511</v>
-      </c>
-      <c r="G99" t="s">
-        <v>512</v>
       </c>
       <c r="H99">
         <v>310</v>
@@ -14920,30 +14920,30 @@
         <v>st_ua</v>
       </c>
       <c r="AD99" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="100" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B100" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C100" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D100" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E100" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F100" t="s">
+        <v>510</v>
+      </c>
+      <c r="G100" t="s">
         <v>511</v>
-      </c>
-      <c r="G100" t="s">
-        <v>512</v>
       </c>
       <c r="H100">
         <v>320</v>
@@ -14956,24 +14956,24 @@
         <v>st_ua</v>
       </c>
       <c r="AD100" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="101" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B101" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C101" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D101" t="s">
         <v>331</v>
       </c>
       <c r="E101" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F101" t="s">
         <v>257</v>
@@ -14992,24 +14992,24 @@
         <v>kp2</v>
       </c>
       <c r="X101" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="102" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B102" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C102" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D102" t="s">
         <v>331</v>
       </c>
       <c r="E102" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F102" t="s">
         <v>317</v>
@@ -15028,24 +15028,24 @@
         <v>kp2</v>
       </c>
       <c r="X102" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="103" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B103" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C103" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D103" t="s">
         <v>331</v>
       </c>
       <c r="E103" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="F103" t="s">
         <v>320</v>
@@ -15064,24 +15064,24 @@
         <v>kp2</v>
       </c>
       <c r="X103" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="104" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B104" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C104" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D104" t="s">
         <v>331</v>
       </c>
       <c r="E104" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F104" t="s">
         <v>322</v>
@@ -15100,24 +15100,24 @@
         <v>kp2</v>
       </c>
       <c r="X104" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="105" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B105" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C105" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D105" t="s">
         <v>331</v>
       </c>
       <c r="E105" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F105" t="s">
         <v>318</v>
@@ -15136,24 +15136,24 @@
         <v>kp2</v>
       </c>
       <c r="X105" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="106" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B106" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C106" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D106" t="s">
         <v>331</v>
       </c>
       <c r="E106" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="F106" t="s">
         <v>327</v>
@@ -15172,24 +15172,24 @@
         <v>kp2</v>
       </c>
       <c r="X106" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="107" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B107" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C107" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D107" t="s">
         <v>331</v>
       </c>
       <c r="E107" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F107" t="s">
         <v>323</v>
@@ -15208,24 +15208,24 @@
         <v>kp2</v>
       </c>
       <c r="X107" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="108" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B108" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C108" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D108" t="s">
         <v>331</v>
       </c>
       <c r="E108" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F108" t="s">
         <v>326</v>
@@ -15244,30 +15244,30 @@
         <v>kp2</v>
       </c>
       <c r="X108" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="109" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>533</v>
+      </c>
+      <c r="B109" t="s">
+        <v>532</v>
+      </c>
+      <c r="C109" t="s">
+        <v>535</v>
+      </c>
+      <c r="D109" t="s">
+        <v>531</v>
+      </c>
+      <c r="E109" t="s">
         <v>534</v>
       </c>
-      <c r="B109" t="s">
-        <v>533</v>
-      </c>
-      <c r="C109" t="s">
+      <c r="F109" t="s">
         <v>536</v>
       </c>
-      <c r="D109" t="s">
-        <v>532</v>
-      </c>
-      <c r="E109" t="s">
-        <v>535</v>
-      </c>
-      <c r="F109" t="s">
+      <c r="G109" t="s">
         <v>537</v>
-      </c>
-      <c r="G109" t="s">
-        <v>538</v>
       </c>
       <c r="H109">
         <v>510</v>
@@ -15280,30 +15280,30 @@
         <v>as_already</v>
       </c>
       <c r="AE109" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="110" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B110" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C110" t="s">
+        <v>540</v>
+      </c>
+      <c r="D110" t="s">
+        <v>531</v>
+      </c>
+      <c r="E110" t="s">
         <v>541</v>
       </c>
-      <c r="D110" t="s">
-        <v>532</v>
-      </c>
-      <c r="E110" t="s">
-        <v>542</v>
-      </c>
       <c r="F110" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="G110" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H110">
         <v>520</v>
@@ -15316,18 +15316,18 @@
         <v>as_new</v>
       </c>
       <c r="AE110" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="111" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B111" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C111" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D111" t="s">
         <v>331</v>
@@ -15352,30 +15352,30 @@
         <v>kp3</v>
       </c>
       <c r="X111" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="112" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B112" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C112" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D112" t="s">
         <v>331</v>
       </c>
       <c r="E112" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F112" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="G112" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H112">
         <v>620</v>
@@ -15388,18 +15388,18 @@
         <v>kp3</v>
       </c>
       <c r="X112" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="113" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B113" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C113" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D113" t="s">
         <v>331</v>
@@ -15424,18 +15424,18 @@
         <v>kp3</v>
       </c>
       <c r="X113" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="114" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B114" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C114" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D114" t="s">
         <v>331</v>
@@ -15460,30 +15460,30 @@
         <v>kp3</v>
       </c>
       <c r="X114" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="115" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B115" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C115" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D115" t="s">
+        <v>554</v>
+      </c>
+      <c r="E115" t="s">
         <v>555</v>
       </c>
-      <c r="E115" t="s">
-        <v>556</v>
-      </c>
       <c r="F115" t="s">
+        <v>564</v>
+      </c>
+      <c r="G115" t="s">
         <v>565</v>
-      </c>
-      <c r="G115" t="s">
-        <v>566</v>
       </c>
       <c r="H115">
         <v>710</v>
@@ -15496,30 +15496,30 @@
         <v>ti_routine</v>
       </c>
       <c r="AF115" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="116" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B116" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C116" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D116" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E116" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F116" t="s">
+        <v>564</v>
+      </c>
+      <c r="G116" t="s">
         <v>565</v>
-      </c>
-      <c r="G116" t="s">
-        <v>566</v>
       </c>
       <c r="H116">
         <v>720</v>
@@ -15532,30 +15532,30 @@
         <v>ti_routine</v>
       </c>
       <c r="AF116" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="117" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B117" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C117" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D117" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E117" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F117" t="s">
+        <v>564</v>
+      </c>
+      <c r="G117" t="s">
         <v>565</v>
-      </c>
-      <c r="G117" t="s">
-        <v>566</v>
       </c>
       <c r="H117">
         <v>730</v>
@@ -15568,30 +15568,30 @@
         <v>ti_routine</v>
       </c>
       <c r="AF117" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="118" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B118" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C118" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D118" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E118" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F118" t="s">
+        <v>564</v>
+      </c>
+      <c r="G118" t="s">
         <v>565</v>
-      </c>
-      <c r="G118" t="s">
-        <v>566</v>
       </c>
       <c r="H118">
         <v>740</v>
@@ -15604,7 +15604,7 @@
         <v>ti_routine</v>
       </c>
       <c r="AF118" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="119" spans="1:33" x14ac:dyDescent="0.2">
@@ -15618,16 +15618,16 @@
         <v>269</v>
       </c>
       <c r="D119" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E119" t="s">
         <v>270</v>
       </c>
       <c r="F119" t="s">
+        <v>428</v>
+      </c>
+      <c r="G119" t="s">
         <v>429</v>
-      </c>
-      <c r="G119" t="s">
-        <v>430</v>
       </c>
       <c r="H119">
         <v>10</v>
@@ -15640,7 +15640,7 @@
         <v>tr_pos2</v>
       </c>
       <c r="Y119" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="120" spans="1:33" x14ac:dyDescent="0.2">
@@ -15654,16 +15654,16 @@
         <v>271</v>
       </c>
       <c r="D120" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E120" t="s">
         <v>272</v>
       </c>
       <c r="F120" t="s">
+        <v>426</v>
+      </c>
+      <c r="G120" t="s">
         <v>427</v>
-      </c>
-      <c r="G120" t="s">
-        <v>428</v>
       </c>
       <c r="H120">
         <v>20</v>
@@ -15676,7 +15676,7 @@
         <v>tr_neg2</v>
       </c>
       <c r="Y120" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="121" spans="1:33" x14ac:dyDescent="0.2">
@@ -15687,13 +15687,13 @@
         <v>351</v>
       </c>
       <c r="C121" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D121" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E121" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F121" t="s">
         <v>186</v>
@@ -15712,7 +15712,7 @@
         <v>hts_mod_com_ndx</v>
       </c>
       <c r="AG121" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="122" spans="1:33" x14ac:dyDescent="0.2">
@@ -15723,13 +15723,13 @@
         <v>351</v>
       </c>
       <c r="C122" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D122" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E122" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F122" t="s">
         <v>186</v>
@@ -15748,7 +15748,7 @@
         <v>hts_mod_fac_ndx</v>
       </c>
       <c r="AG122" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="123" spans="1:33" x14ac:dyDescent="0.2">
@@ -15762,10 +15762,10 @@
         <v>202</v>
       </c>
       <c r="D123" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E123" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F123" t="s">
         <v>186</v>
@@ -15784,7 +15784,7 @@
         <v>hts_mod_com_mob</v>
       </c>
       <c r="AG123" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="124" spans="1:33" x14ac:dyDescent="0.2">
@@ -15798,10 +15798,10 @@
         <v>210</v>
       </c>
       <c r="D124" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E124" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F124" t="s">
         <v>186</v>
@@ -15820,7 +15820,7 @@
         <v>hts_mod_com_vct</v>
       </c>
       <c r="AG124" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="125" spans="1:33" x14ac:dyDescent="0.2">
@@ -15834,10 +15834,10 @@
         <v>217</v>
       </c>
       <c r="D125" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E125" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F125" t="s">
         <v>186</v>
@@ -15856,7 +15856,7 @@
         <v>hts_mod_com_otr</v>
       </c>
       <c r="AG125" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="126" spans="1:33" x14ac:dyDescent="0.2">
@@ -15870,10 +15870,10 @@
         <v>212</v>
       </c>
       <c r="D126" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E126" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F126" t="s">
         <v>186</v>
@@ -15892,7 +15892,7 @@
         <v>hts_mod_fac_ew</v>
       </c>
       <c r="AG126" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="127" spans="1:33" x14ac:dyDescent="0.2">
@@ -15906,10 +15906,10 @@
         <v>213</v>
       </c>
       <c r="D127" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E127" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F127" t="s">
         <v>186</v>
@@ -15928,7 +15928,7 @@
         <v>hts_mod_fac_inpat</v>
       </c>
       <c r="AG127" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="128" spans="1:33" x14ac:dyDescent="0.2">
@@ -15942,10 +15942,10 @@
         <v>214</v>
       </c>
       <c r="D128" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E128" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F128" t="s">
         <v>186</v>
@@ -15964,7 +15964,7 @@
         <v>hts_mod_fac_nut</v>
       </c>
       <c r="AG128" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="129" spans="1:33" x14ac:dyDescent="0.2">
@@ -15978,10 +15978,10 @@
         <v>215</v>
       </c>
       <c r="D129" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E129" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F129" t="s">
         <v>186</v>
@@ -16000,7 +16000,7 @@
         <v>hts_mod_fac_ped</v>
       </c>
       <c r="AG129" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="130" spans="1:33" x14ac:dyDescent="0.2">
@@ -16014,10 +16014,10 @@
         <v>216</v>
       </c>
       <c r="D130" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E130" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F130" t="s">
         <v>186</v>
@@ -16036,7 +16036,7 @@
         <v>hts_mod_fac_sti</v>
       </c>
       <c r="AG130" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="131" spans="1:33" x14ac:dyDescent="0.2">
@@ -16050,10 +16050,10 @@
         <v>211</v>
       </c>
       <c r="D131" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E131" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F131" t="s">
         <v>186</v>
@@ -16072,7 +16072,7 @@
         <v>hts_mod_fac_vct</v>
       </c>
       <c r="AG131" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="132" spans="1:33" x14ac:dyDescent="0.2">
@@ -16086,10 +16086,10 @@
         <v>218</v>
       </c>
       <c r="D132" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E132" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F132" t="s">
         <v>186</v>
@@ -16108,7 +16108,7 @@
         <v>hts_mod_fac_otr_pitc</v>
       </c>
       <c r="AG132" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data required vmmc_yield changed to standard yield indicator
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5947CA-BDA6-E44A-BCAA-915F2A59C98B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C6D836-5815-9C45-B3F5-79EB7EB4C9E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="35320" yWindow="460" windowWidth="33600" windowHeight="20020" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3401" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3401" uniqueCount="670">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1880,12 +1880,6 @@
   </si>
   <si>
     <t>joBC2hxzpGN</t>
-  </si>
-  <si>
-    <t>Byon9M4BJsS</t>
-  </si>
-  <si>
-    <t>VMMC_CIRC.N.yield.19R</t>
   </si>
   <si>
     <t>VMMC_CIRC.N.indeterminateRate.19R</t>
@@ -2465,10 +2459,10 @@
   <dimension ref="A1:AI57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomRight" activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2846,7 +2840,7 @@
         <v>173</v>
       </c>
       <c r="M4" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="N4" t="s">
         <v>173</v>
@@ -3488,7 +3482,7 @@
         <v>173</v>
       </c>
       <c r="M10" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="N10" t="s">
         <v>173</v>
@@ -3664,7 +3658,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:35" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -3684,10 +3678,10 @@
         <v>174</v>
       </c>
       <c r="G12" t="s">
-        <v>615</v>
-      </c>
-      <c r="H12" t="s">
-        <v>614</v>
+        <v>173</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>612</v>
       </c>
       <c r="I12" t="s">
         <v>169</v>
@@ -3702,7 +3696,7 @@
         <v>173</v>
       </c>
       <c r="M12" t="s">
-        <v>173</v>
+        <v>665</v>
       </c>
       <c r="N12" t="s">
         <v>173</v>
@@ -3791,10 +3785,10 @@
         <v>174</v>
       </c>
       <c r="G13" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="H13" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="I13" t="s">
         <v>169</v>
@@ -6787,10 +6781,10 @@
         <v>174</v>
       </c>
       <c r="G41" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="I41" t="s">
         <v>169</v>
@@ -6894,10 +6888,10 @@
         <v>174</v>
       </c>
       <c r="G42" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="I42" t="s">
         <v>169</v>
@@ -7001,10 +6995,10 @@
         <v>172</v>
       </c>
       <c r="G43" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="H43" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="I43" t="s">
         <v>611</v>
@@ -7108,10 +7102,10 @@
         <v>172</v>
       </c>
       <c r="G44" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="H44" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="I44" t="s">
         <v>611</v>
@@ -7147,10 +7141,10 @@
         <v>173</v>
       </c>
       <c r="T44" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="U44" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="V44" s="1" t="s">
         <v>169</v>
@@ -8181,7 +8175,7 @@
         <v>173</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="I54" t="s">
         <v>611</v>
@@ -9353,7 +9347,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
   <dimension ref="A1:AG140"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView topLeftCell="F118" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J138" sqref="J138"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9681,13 +9677,13 @@
         <v>318</v>
       </c>
       <c r="C7" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="D7" t="s">
         <v>302</v>
       </c>
       <c r="E7" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F7" t="s">
         <v>120</v>
@@ -9856,13 +9852,13 @@
         <v>318</v>
       </c>
       <c r="C11" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="D11" t="s">
         <v>302</v>
       </c>
       <c r="E11" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="F11" t="s">
         <v>121</v>
@@ -10433,13 +10429,13 @@
         <v>318</v>
       </c>
       <c r="C25" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="D25" t="s">
         <v>302</v>
       </c>
       <c r="E25" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="F25" t="s">
         <v>315</v>
@@ -11179,13 +11175,13 @@
         <v>318</v>
       </c>
       <c r="C43" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="D43" t="s">
         <v>302</v>
       </c>
       <c r="E43" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="F43" t="s">
         <v>126</v>
@@ -11395,13 +11391,13 @@
         <v>318</v>
       </c>
       <c r="C48" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="D48" t="s">
         <v>302</v>
       </c>
       <c r="E48" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="F48" t="s">
         <v>127</v>
@@ -14294,19 +14290,19 @@
     </row>
     <row r="126" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B126" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C126" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D126" t="s">
         <v>534</v>
       </c>
       <c r="E126" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="F126" t="s">
         <v>173</v>
@@ -14330,19 +14326,19 @@
     </row>
     <row r="127" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B127" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C127" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="D127" t="s">
         <v>534</v>
       </c>
       <c r="E127" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="F127" t="s">
         <v>173</v>
@@ -14366,19 +14362,19 @@
     </row>
     <row r="128" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B128" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C128" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="D128" t="s">
         <v>534</v>
       </c>
       <c r="E128" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="F128" t="s">
         <v>173</v>
@@ -14402,19 +14398,19 @@
     </row>
     <row r="129" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B129" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C129" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="D129" t="s">
         <v>534</v>
       </c>
       <c r="E129" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="F129" t="s">
         <v>173</v>
@@ -14438,19 +14434,19 @@
     </row>
     <row r="130" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B130" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C130" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D130" t="s">
         <v>534</v>
       </c>
       <c r="E130" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="F130" t="s">
         <v>173</v>
@@ -14474,19 +14470,19 @@
     </row>
     <row r="131" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B131" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C131" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D131" t="s">
         <v>534</v>
       </c>
       <c r="E131" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="F131" t="s">
         <v>173</v>
@@ -14510,19 +14506,19 @@
     </row>
     <row r="132" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B132" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C132" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="D132" t="s">
         <v>534</v>
       </c>
       <c r="E132" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="F132" t="s">
         <v>173</v>
@@ -14546,19 +14542,19 @@
     </row>
     <row r="133" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B133" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C133" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="D133" t="s">
         <v>534</v>
       </c>
       <c r="E133" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="F133" t="s">
         <v>173</v>
@@ -14582,19 +14578,19 @@
     </row>
     <row r="134" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B134" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C134" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D134" t="s">
         <v>534</v>
       </c>
       <c r="E134" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="F134" t="s">
         <v>173</v>
@@ -14618,19 +14614,19 @@
     </row>
     <row r="135" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B135" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C135" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="D135" t="s">
         <v>534</v>
       </c>
       <c r="E135" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="F135" t="s">
         <v>173</v>
@@ -14654,19 +14650,19 @@
     </row>
     <row r="136" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B136" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C136" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="D136" t="s">
         <v>534</v>
       </c>
       <c r="E136" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="F136" t="s">
         <v>173</v>
@@ -14690,19 +14686,19 @@
     </row>
     <row r="137" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B137" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C137" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="D137" t="s">
         <v>534</v>
       </c>
       <c r="E137" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="F137" t="s">
         <v>173</v>
@@ -14726,19 +14722,19 @@
     </row>
     <row r="138" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B138" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C138" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="D138" t="s">
         <v>534</v>
       </c>
       <c r="E138" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="F138" t="s">
         <v>173</v>
@@ -14757,24 +14753,24 @@
         <v>hts_mod_fac_vmmc</v>
       </c>
       <c r="AG138" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
     </row>
     <row r="139" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B139" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C139" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="D139" t="s">
         <v>534</v>
       </c>
       <c r="E139" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="F139" t="s">
         <v>173</v>
@@ -14793,24 +14789,24 @@
         <v>hts_mod_fac_anc_1</v>
       </c>
       <c r="AG139" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="140" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B140" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C140" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="D140" t="s">
         <v>534</v>
       </c>
       <c r="E140" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="F140" t="s">
         <v>173</v>
@@ -14829,7 +14825,7 @@
         <v>hts_mod_fac_tb</v>
       </c>
       <c r="AG140" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data required updatet tb_stat age set
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95AE0D6-B5B2-084E-8B86-7CB2D16A9E61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480DA512-E5C3-3F45-86E0-929A364A3725}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
@@ -2477,10 +2477,10 @@
   <dimension ref="A1:AI57"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A39" sqref="A39"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3383,8 +3383,8 @@
       <c r="I9" t="s">
         <v>167</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>212</v>
+      <c r="J9" t="s">
+        <v>184</v>
       </c>
       <c r="K9" t="s">
         <v>175</v>
@@ -9365,7 +9365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
   <dimension ref="A1:AG142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R103" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="AK142" sqref="AK142"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update tb_stat age sets
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480DA512-E5C3-3F45-86E0-929A364A3725}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FA6085-1732-334D-A119-7D14D6B096A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="2" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -2476,11 +2476,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
   <dimension ref="A1:AI57"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3169,8 +3169,8 @@
       <c r="I7" t="s">
         <v>608</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>212</v>
+      <c r="J7" t="s">
+        <v>184</v>
       </c>
       <c r="K7" t="s">
         <v>175</v>
@@ -3276,8 +3276,8 @@
       <c r="I8" t="s">
         <v>608</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>212</v>
+      <c r="J8" t="s">
+        <v>184</v>
       </c>
       <c r="K8" t="s">
         <v>175</v>
@@ -3315,8 +3315,8 @@
       <c r="V8" t="s">
         <v>167</v>
       </c>
-      <c r="W8" s="2" t="s">
-        <v>212</v>
+      <c r="W8" t="s">
+        <v>184</v>
       </c>
       <c r="X8" t="s">
         <v>175</v>
@@ -9365,9 +9365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
   <dimension ref="A1:AG142"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AK142" sqref="AK142"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
data required update ped and nut hts_tst sex dimension
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721ECFC6-3A1B-7241-BFF4-4CCFEC93F4CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AEF29A9-5A47-4548-9816-954D61C81519}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data_required!$A$1:$AG$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data_required!$A$1:$AI$57</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">dimension_Item_sets!$A$1:$AF$142</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -2480,10 +2480,10 @@
   <dimension ref="A1:AI57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5957,8 +5957,8 @@
       <c r="J33" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="K33" s="1" t="s">
-        <v>194</v>
+      <c r="K33" t="s">
+        <v>184</v>
       </c>
       <c r="L33" t="s">
         <v>170</v>
@@ -6064,8 +6064,8 @@
       <c r="J34" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="K34" s="1" t="s">
-        <v>194</v>
+      <c r="K34" t="s">
+        <v>184</v>
       </c>
       <c r="L34" t="s">
         <v>170</v>
@@ -8602,6 +8602,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AI57" xr:uid="{6F439630-CB66-7E4E-9544-3F25521DB3EB}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9369,8 +9370,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AG142"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9691,7 +9692,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>214</v>
       </c>
@@ -9741,7 +9742,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="8" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>214</v>
       </c>
@@ -9827,7 +9828,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="10" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>214</v>
       </c>
@@ -10164,7 +10165,7 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>170</v>
       </c>
@@ -10401,7 +10402,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>170</v>
       </c>
@@ -14932,10 +14933,10 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AF142" xr:uid="{F5070472-BD41-FC47-BC46-FB0AD4499DE3}">
-    <filterColumn colId="18">
-      <filters>
-        <filter val="missing_age_2"/>
-      </filters>
+    <filterColumn colId="16">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:W66">

</xml_diff>

<commit_message>
data required tb_tx_prev replace missing age and missing sex dimensions.
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AEF29A9-5A47-4548-9816-954D61C81519}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D7A9B5-B984-3243-9AA9-B0D4B32D1604}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -2480,10 +2480,10 @@
   <dimension ref="A1:AI57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D42" sqref="D42"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6810,11 +6810,11 @@
       <c r="I41" t="s">
         <v>166</v>
       </c>
-      <c r="J41" t="s">
-        <v>210</v>
+      <c r="J41" s="9" t="s">
+        <v>511</v>
       </c>
       <c r="K41" t="s">
-        <v>208</v>
+        <v>174</v>
       </c>
       <c r="L41" t="s">
         <v>170</v>
@@ -6917,11 +6917,11 @@
       <c r="I42" t="s">
         <v>166</v>
       </c>
-      <c r="J42" t="s">
-        <v>210</v>
+      <c r="J42" s="9" t="s">
+        <v>511</v>
       </c>
       <c r="K42" t="s">
-        <v>208</v>
+        <v>174</v>
       </c>
       <c r="L42" t="s">
         <v>170</v>
@@ -9370,8 +9370,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AG142"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView topLeftCell="K1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AB145" sqref="AB145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9692,7 +9692,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>214</v>
       </c>
@@ -9742,7 +9742,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>214</v>
       </c>
@@ -9828,7 +9828,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>214</v>
       </c>
@@ -10127,7 +10127,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>214</v>
       </c>
@@ -10366,7 +10366,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>214</v>
       </c>
@@ -14933,10 +14933,10 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AF142" xr:uid="{F5070472-BD41-FC47-BC46-FB0AD4499DE3}">
-    <filterColumn colId="16">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
+    <filterColumn colId="15">
+      <filters>
+        <filter val="&lt;15/&gt;15"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:W66">

</xml_diff>

<commit_message>
data_required prep_new key pop update to use indicator and v3 keypops
last year uses keypopabr
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D7A9B5-B984-3243-9AA9-B0D4B32D1604}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF07C4F9-A786-1D48-B0EE-4115143E8FD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3417" uniqueCount="677">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3419" uniqueCount="675">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1682,12 +1682,6 @@
   </si>
   <si>
     <t>2018Q4</t>
-  </si>
-  <si>
-    <t>gdHE7Kk9Q1k</t>
-  </si>
-  <si>
-    <t>lXqlw8UxoqF</t>
   </si>
   <si>
     <t>A+B</t>
@@ -2480,10 +2474,10 @@
   <dimension ref="A1:AI57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AB23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2603,10 +2597,10 @@
         <v>180</v>
       </c>
       <c r="AH1" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="AI1" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">
@@ -2620,7 +2614,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -2635,7 +2629,7 @@
         <v>79</v>
       </c>
       <c r="I2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="J2" t="s">
         <v>167</v>
@@ -2727,7 +2721,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
@@ -2834,7 +2828,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
@@ -2846,7 +2840,7 @@
         <v>170</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="I4" t="s">
         <v>166</v>
@@ -2861,7 +2855,7 @@
         <v>170</v>
       </c>
       <c r="M4" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="N4" t="s">
         <v>170</v>
@@ -2941,7 +2935,7 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
@@ -3048,7 +3042,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -3155,7 +3149,7 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="E7" t="s">
         <v>3</v>
@@ -3170,7 +3164,7 @@
         <v>83</v>
       </c>
       <c r="I7" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="J7" t="s">
         <v>183</v>
@@ -3262,7 +3256,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
@@ -3277,7 +3271,7 @@
         <v>83</v>
       </c>
       <c r="I8" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="J8" t="s">
         <v>183</v>
@@ -3369,7 +3363,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
@@ -3476,7 +3470,7 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
@@ -3488,7 +3482,7 @@
         <v>170</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="I10" t="s">
         <v>166</v>
@@ -3503,7 +3497,7 @@
         <v>170</v>
       </c>
       <c r="M10" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="N10" t="s">
         <v>170</v>
@@ -3583,7 +3577,7 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="E11" t="s">
         <v>3</v>
@@ -3592,13 +3586,13 @@
         <v>169</v>
       </c>
       <c r="G11" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="H11" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="I11" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="J11" t="s">
         <v>167</v>
@@ -3690,7 +3684,7 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="E12" t="s">
         <v>6</v>
@@ -3702,7 +3696,7 @@
         <v>170</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="I12" t="s">
         <v>166</v>
@@ -3717,7 +3711,7 @@
         <v>170</v>
       </c>
       <c r="M12" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="N12" t="s">
         <v>170</v>
@@ -3797,7 +3791,7 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
@@ -3806,10 +3800,10 @@
         <v>171</v>
       </c>
       <c r="G13" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="H13" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="I13" t="s">
         <v>166</v>
@@ -3904,7 +3898,7 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="E14" t="s">
         <v>3</v>
@@ -3919,7 +3913,7 @@
         <v>87</v>
       </c>
       <c r="I14" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="J14" t="s">
         <v>183</v>
@@ -4011,7 +4005,7 @@
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
@@ -4023,7 +4017,7 @@
         <v>170</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="I15" t="s">
         <v>166</v>
@@ -4118,7 +4112,7 @@
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="E16" t="s">
         <v>6</v>
@@ -4130,7 +4124,7 @@
         <v>170</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="I16" t="s">
         <v>166</v>
@@ -4225,7 +4219,7 @@
         <v>5</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="E17" t="s">
         <v>6</v>
@@ -4237,7 +4231,7 @@
         <v>170</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="I17" t="s">
         <v>166</v>
@@ -4276,7 +4270,7 @@
         <v>170</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="V17" t="s">
         <v>166</v>
@@ -4332,7 +4326,7 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="E18" t="s">
         <v>6</v>
@@ -4344,7 +4338,7 @@
         <v>170</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="I18" t="s">
         <v>166</v>
@@ -4383,7 +4377,7 @@
         <v>170</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="V18" t="s">
         <v>166</v>
@@ -4439,7 +4433,7 @@
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="E19" t="s">
         <v>6</v>
@@ -4451,7 +4445,7 @@
         <v>170</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="I19" t="s">
         <v>166</v>
@@ -4490,7 +4484,7 @@
         <v>170</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="V19" t="s">
         <v>166</v>
@@ -4546,7 +4540,7 @@
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="E20" t="s">
         <v>6</v>
@@ -4558,7 +4552,7 @@
         <v>170</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="I20" t="s">
         <v>166</v>
@@ -4597,7 +4591,7 @@
         <v>170</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="V20" t="s">
         <v>166</v>
@@ -4653,7 +4647,7 @@
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="E21" t="s">
         <v>6</v>
@@ -4665,7 +4659,7 @@
         <v>170</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="I21" t="s">
         <v>166</v>
@@ -4704,7 +4698,7 @@
         <v>170</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="V21" t="s">
         <v>166</v>
@@ -4760,7 +4754,7 @@
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E22" t="s">
         <v>6</v>
@@ -4772,7 +4766,7 @@
         <v>170</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="I22" t="s">
         <v>166</v>
@@ -4811,7 +4805,7 @@
         <v>170</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="V22" t="s">
         <v>166</v>
@@ -4867,7 +4861,7 @@
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="E23" t="s">
         <v>6</v>
@@ -4879,7 +4873,7 @@
         <v>170</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="I23" t="s">
         <v>166</v>
@@ -4918,7 +4912,7 @@
         <v>170</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="V23" t="s">
         <v>166</v>
@@ -4974,7 +4968,7 @@
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="E24" t="s">
         <v>6</v>
@@ -4986,7 +4980,7 @@
         <v>170</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="I24" t="s">
         <v>166</v>
@@ -5025,7 +5019,7 @@
         <v>170</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="V24" t="s">
         <v>166</v>
@@ -5081,7 +5075,7 @@
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="E25" t="s">
         <v>6</v>
@@ -5093,7 +5087,7 @@
         <v>170</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="I25" t="s">
         <v>166</v>
@@ -5132,7 +5126,7 @@
         <v>170</v>
       </c>
       <c r="U25" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="V25" t="s">
         <v>166</v>
@@ -5188,7 +5182,7 @@
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E26" t="s">
         <v>6</v>
@@ -5200,7 +5194,7 @@
         <v>170</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="I26" t="s">
         <v>166</v>
@@ -5239,7 +5233,7 @@
         <v>170</v>
       </c>
       <c r="U26" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="V26" t="s">
         <v>166</v>
@@ -5295,7 +5289,7 @@
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="E27" t="s">
         <v>6</v>
@@ -5307,7 +5301,7 @@
         <v>170</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="I27" t="s">
         <v>166</v>
@@ -5346,7 +5340,7 @@
         <v>170</v>
       </c>
       <c r="U27" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="V27" t="s">
         <v>166</v>
@@ -5402,7 +5396,7 @@
         <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="E28" t="s">
         <v>6</v>
@@ -5414,7 +5408,7 @@
         <v>170</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="I28" t="s">
         <v>166</v>
@@ -5509,7 +5503,7 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="E29" t="s">
         <v>6</v>
@@ -5521,7 +5515,7 @@
         <v>170</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="I29" t="s">
         <v>166</v>
@@ -5616,7 +5610,7 @@
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="E30" t="s">
         <v>6</v>
@@ -5628,7 +5622,7 @@
         <v>170</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="I30" t="s">
         <v>166</v>
@@ -5723,7 +5717,7 @@
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="E31" t="s">
         <v>6</v>
@@ -5735,7 +5729,7 @@
         <v>170</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="I31" t="s">
         <v>166</v>
@@ -5830,7 +5824,7 @@
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="E32" t="s">
         <v>6</v>
@@ -5842,7 +5836,7 @@
         <v>170</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="I32" t="s">
         <v>166</v>
@@ -5937,7 +5931,7 @@
         <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="E33" t="s">
         <v>6</v>
@@ -5949,7 +5943,7 @@
         <v>170</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="I33" t="s">
         <v>166</v>
@@ -6044,7 +6038,7 @@
         <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="E34" t="s">
         <v>6</v>
@@ -6056,7 +6050,7 @@
         <v>170</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="I34" t="s">
         <v>166</v>
@@ -6151,7 +6145,7 @@
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="E35" t="s">
         <v>6</v>
@@ -6163,7 +6157,7 @@
         <v>170</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="I35" t="s">
         <v>166</v>
@@ -6258,7 +6252,7 @@
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E36" t="s">
         <v>6</v>
@@ -6270,7 +6264,7 @@
         <v>170</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="I36" t="s">
         <v>166</v>
@@ -6365,7 +6359,7 @@
         <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="E37" t="s">
         <v>6</v>
@@ -6377,7 +6371,7 @@
         <v>170</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="I37" t="s">
         <v>166</v>
@@ -6472,7 +6466,7 @@
         <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="E38" t="s">
         <v>3</v>
@@ -6484,10 +6478,10 @@
         <v>170</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="I38" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="J38" t="s">
         <v>167</v>
@@ -6579,7 +6573,7 @@
         <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="E39" t="s">
         <v>3</v>
@@ -6591,16 +6585,16 @@
         <v>170</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="J39" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="K39" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="L39" t="s">
         <v>170</v>
@@ -6686,7 +6680,7 @@
         <v>5</v>
       </c>
       <c r="D40" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E40" t="s">
         <v>6</v>
@@ -6701,7 +6695,7 @@
         <v>217</v>
       </c>
       <c r="I40" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="J40" t="s">
         <v>167</v>
@@ -6793,7 +6787,7 @@
         <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="E41" t="s">
         <v>6</v>
@@ -6802,10 +6796,10 @@
         <v>171</v>
       </c>
       <c r="G41" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="I41" t="s">
         <v>166</v>
@@ -6900,7 +6894,7 @@
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="E42" t="s">
         <v>6</v>
@@ -6909,10 +6903,10 @@
         <v>171</v>
       </c>
       <c r="G42" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="I42" t="s">
         <v>166</v>
@@ -7007,7 +7001,7 @@
         <v>2</v>
       </c>
       <c r="D43" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="E43" t="s">
         <v>3</v>
@@ -7016,13 +7010,13 @@
         <v>169</v>
       </c>
       <c r="G43" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="H43" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="I43" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="J43" t="s">
         <v>311</v>
@@ -7114,7 +7108,7 @@
         <v>5</v>
       </c>
       <c r="D44" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E44" t="s">
         <v>6</v>
@@ -7123,13 +7117,13 @@
         <v>169</v>
       </c>
       <c r="G44" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="H44" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="I44" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="J44" t="s">
         <v>311</v>
@@ -7162,10 +7156,10 @@
         <v>170</v>
       </c>
       <c r="T44" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="U44" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="V44" s="1" t="s">
         <v>166</v>
@@ -7221,7 +7215,7 @@
         <v>2</v>
       </c>
       <c r="D45" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="E45" t="s">
         <v>3</v>
@@ -7236,7 +7230,7 @@
         <v>89</v>
       </c>
       <c r="I45" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="J45" t="s">
         <v>170</v>
@@ -7328,7 +7322,7 @@
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="E46" t="s">
         <v>3</v>
@@ -7343,7 +7337,7 @@
         <v>91</v>
       </c>
       <c r="I46" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="J46" t="s">
         <v>170</v>
@@ -7435,7 +7429,7 @@
         <v>2</v>
       </c>
       <c r="D47" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="E47" t="s">
         <v>3</v>
@@ -7450,7 +7444,7 @@
         <v>91</v>
       </c>
       <c r="I47" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="J47" t="s">
         <v>170</v>
@@ -7542,7 +7536,7 @@
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E48" t="s">
         <v>3</v>
@@ -7557,7 +7551,7 @@
         <v>93</v>
       </c>
       <c r="I48" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="J48" t="s">
         <v>170</v>
@@ -7649,7 +7643,7 @@
         <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="E49" t="s">
         <v>3</v>
@@ -7664,7 +7658,7 @@
         <v>95</v>
       </c>
       <c r="I49" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="J49" t="s">
         <v>167</v>
@@ -7756,7 +7750,7 @@
         <v>5</v>
       </c>
       <c r="D50" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="E50" t="s">
         <v>6</v>
@@ -7771,7 +7765,7 @@
         <v>95</v>
       </c>
       <c r="I50" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="J50" t="s">
         <v>167</v>
@@ -7863,7 +7857,7 @@
         <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="E51" t="s">
         <v>3</v>
@@ -7878,7 +7872,7 @@
         <v>96</v>
       </c>
       <c r="I51" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="J51" t="s">
         <v>195</v>
@@ -7970,7 +7964,7 @@
         <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E52" t="s">
         <v>3</v>
@@ -7985,7 +7979,7 @@
         <v>98</v>
       </c>
       <c r="I52" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="J52" t="s">
         <v>170</v>
@@ -8077,7 +8071,7 @@
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="E53" t="s">
         <v>3</v>
@@ -8092,7 +8086,7 @@
         <v>100</v>
       </c>
       <c r="I53" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="J53" t="s">
         <v>170</v>
@@ -8184,7 +8178,7 @@
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="E54" t="s">
         <v>6</v>
@@ -8196,10 +8190,10 @@
         <v>170</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="I54" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="J54" t="s">
         <v>170</v>
@@ -8300,13 +8294,13 @@
         <v>169</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>170</v>
+        <v>59</v>
       </c>
       <c r="H55" s="15" t="s">
-        <v>548</v>
+        <v>94</v>
       </c>
       <c r="I55" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="J55" t="s">
         <v>170</v>
@@ -8315,7 +8309,7 @@
         <v>170</v>
       </c>
       <c r="L55" t="s">
-        <v>495</v>
+        <v>235</v>
       </c>
       <c r="M55" t="s">
         <v>170</v>
@@ -8342,10 +8336,10 @@
         <v>170</v>
       </c>
       <c r="U55" t="s">
-        <v>549</v>
+        <v>170</v>
       </c>
       <c r="V55" t="s">
-        <v>607</v>
+        <v>170</v>
       </c>
       <c r="W55" t="s">
         <v>170</v>
@@ -8354,7 +8348,7 @@
         <v>170</v>
       </c>
       <c r="Y55" t="s">
-        <v>495</v>
+        <v>170</v>
       </c>
       <c r="Z55" t="s">
         <v>170</v>
@@ -8378,13 +8372,13 @@
         <v>170</v>
       </c>
       <c r="AG55" t="s">
-        <v>550</v>
-      </c>
-      <c r="AH55">
-        <v>0</v>
-      </c>
-      <c r="AI55">
-        <v>0</v>
+        <v>170</v>
+      </c>
+      <c r="AH55" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI55" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="56" spans="1:35" ht="18" x14ac:dyDescent="0.2">
@@ -8410,10 +8404,10 @@
         <v>170</v>
       </c>
       <c r="H56" s="15" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="I56" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="J56" t="s">
         <v>170</v>
@@ -8449,10 +8443,10 @@
         <v>170</v>
       </c>
       <c r="U56" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="V56" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="W56" t="s">
         <v>170</v>
@@ -8485,7 +8479,7 @@
         <v>170</v>
       </c>
       <c r="AG56" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="AH56">
         <v>0</v>
@@ -8611,8 +8605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D15FCD2F-A9CC-CD4F-8AF1-79C36D527EBB}">
   <dimension ref="A1:AF46"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:B46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9370,8 +9364,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AG142"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AB145" sqref="AB145"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9700,13 +9694,13 @@
         <v>315</v>
       </c>
       <c r="C7" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="D7" t="s">
         <v>299</v>
       </c>
       <c r="E7" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="F7" t="s">
         <v>117</v>
@@ -9875,13 +9869,13 @@
         <v>315</v>
       </c>
       <c r="C11" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="D11" t="s">
         <v>299</v>
       </c>
       <c r="E11" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="F11" t="s">
         <v>118</v>
@@ -10127,7 +10121,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>214</v>
       </c>
@@ -10366,7 +10360,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>214</v>
       </c>
@@ -10452,13 +10446,13 @@
         <v>315</v>
       </c>
       <c r="C25" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="D25" t="s">
         <v>299</v>
       </c>
       <c r="E25" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="F25" t="s">
         <v>312</v>
@@ -11198,13 +11192,13 @@
         <v>315</v>
       </c>
       <c r="C43" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="D43" t="s">
         <v>299</v>
       </c>
       <c r="E43" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F43" t="s">
         <v>123</v>
@@ -11414,13 +11408,13 @@
         <v>315</v>
       </c>
       <c r="C48" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="D48" t="s">
         <v>299</v>
       </c>
       <c r="E48" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="F48" t="s">
         <v>124</v>
@@ -12007,7 +12001,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="62" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>224</v>
       </c>
@@ -12043,7 +12037,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="63" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>224</v>
       </c>
@@ -12079,7 +12073,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="64" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>224</v>
       </c>
@@ -12115,7 +12109,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="65" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>224</v>
       </c>
@@ -12151,7 +12145,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="66" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>224</v>
       </c>
@@ -13591,7 +13585,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="106" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>372</v>
       </c>
@@ -13627,7 +13621,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="107" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>372</v>
       </c>
@@ -13663,7 +13657,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="108" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>372</v>
       </c>
@@ -13699,7 +13693,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="109" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>372</v>
       </c>
@@ -13735,7 +13729,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="110" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>372</v>
       </c>
@@ -13771,7 +13765,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="111" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>372</v>
       </c>
@@ -13807,7 +13801,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="112" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>372</v>
       </c>
@@ -13843,7 +13837,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="113" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>372</v>
       </c>
@@ -13951,7 +13945,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="116" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>372</v>
       </c>
@@ -13987,7 +13981,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="117" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>372</v>
       </c>
@@ -14023,7 +14017,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="118" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>372</v>
       </c>
@@ -14059,7 +14053,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="119" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>372</v>
       </c>
@@ -14313,19 +14307,19 @@
     </row>
     <row r="126" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B126" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C126" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="D126" t="s">
         <v>530</v>
       </c>
       <c r="E126" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="F126" t="s">
         <v>170</v>
@@ -14349,19 +14343,19 @@
     </row>
     <row r="127" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B127" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C127" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="D127" t="s">
         <v>530</v>
       </c>
       <c r="E127" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="F127" t="s">
         <v>170</v>
@@ -14385,19 +14379,19 @@
     </row>
     <row r="128" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B128" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C128" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="D128" t="s">
         <v>530</v>
       </c>
       <c r="E128" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="F128" t="s">
         <v>170</v>
@@ -14421,19 +14415,19 @@
     </row>
     <row r="129" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B129" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C129" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D129" t="s">
         <v>530</v>
       </c>
       <c r="E129" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="F129" t="s">
         <v>170</v>
@@ -14457,19 +14451,19 @@
     </row>
     <row r="130" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B130" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C130" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="D130" t="s">
         <v>530</v>
       </c>
       <c r="E130" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="F130" t="s">
         <v>170</v>
@@ -14493,19 +14487,19 @@
     </row>
     <row r="131" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B131" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C131" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="D131" t="s">
         <v>530</v>
       </c>
       <c r="E131" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="F131" t="s">
         <v>170</v>
@@ -14529,19 +14523,19 @@
     </row>
     <row r="132" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B132" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C132" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="D132" t="s">
         <v>530</v>
       </c>
       <c r="E132" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="F132" t="s">
         <v>170</v>
@@ -14565,19 +14559,19 @@
     </row>
     <row r="133" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B133" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C133" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D133" t="s">
         <v>530</v>
       </c>
       <c r="E133" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="F133" t="s">
         <v>170</v>
@@ -14601,19 +14595,19 @@
     </row>
     <row r="134" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B134" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C134" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D134" t="s">
         <v>530</v>
       </c>
       <c r="E134" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="F134" t="s">
         <v>170</v>
@@ -14637,19 +14631,19 @@
     </row>
     <row r="135" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B135" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C135" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="D135" t="s">
         <v>530</v>
       </c>
       <c r="E135" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="F135" t="s">
         <v>170</v>
@@ -14673,19 +14667,19 @@
     </row>
     <row r="136" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B136" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C136" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="D136" t="s">
         <v>530</v>
       </c>
       <c r="E136" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="F136" t="s">
         <v>170</v>
@@ -14709,19 +14703,19 @@
     </row>
     <row r="137" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B137" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C137" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D137" t="s">
         <v>530</v>
       </c>
       <c r="E137" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="F137" t="s">
         <v>170</v>
@@ -14745,19 +14739,19 @@
     </row>
     <row r="138" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B138" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C138" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="D138" t="s">
         <v>530</v>
       </c>
       <c r="E138" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="F138" t="s">
         <v>170</v>
@@ -14776,24 +14770,24 @@
         <v>hts_mod_fac_vmmc</v>
       </c>
       <c r="AG138" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="139" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B139" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C139" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="D139" t="s">
         <v>530</v>
       </c>
       <c r="E139" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="F139" t="s">
         <v>170</v>
@@ -14812,24 +14806,24 @@
         <v>hts_mod_fac_anc_1</v>
       </c>
       <c r="AG139" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="140" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B140" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C140" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="D140" t="s">
         <v>530</v>
       </c>
       <c r="E140" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="F140" t="s">
         <v>170</v>
@@ -14848,7 +14842,7 @@
         <v>hts_mod_fac_tb</v>
       </c>
       <c r="AG140" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="141" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
@@ -14859,19 +14853,19 @@
         <v>315</v>
       </c>
       <c r="C141" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="D141" t="s">
         <v>299</v>
       </c>
       <c r="E141" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F141" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="G141" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="H141">
         <v>3</v>
@@ -14892,7 +14886,7 @@
       <c r="R141" s="9"/>
       <c r="T141" s="9"/>
       <c r="AG141" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="142" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
@@ -14912,10 +14906,10 @@
         <v>154</v>
       </c>
       <c r="F142" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="G142" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="H142">
         <v>3</v>
@@ -14928,15 +14922,15 @@
         <v>U_sex</v>
       </c>
       <c r="AG142" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:AF142" xr:uid="{F5070472-BD41-FC47-BC46-FB0AD4499DE3}">
-    <filterColumn colId="15">
-      <filters>
-        <filter val="&lt;15/&gt;15"/>
-      </filters>
+    <filterColumn colId="23">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:W66">

</xml_diff>

<commit_message>
data_required add A.dx_name column
not all indicators have a code so I want to validate by name
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF07C4F9-A786-1D48-B0EE-4115143E8FD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E14C5D-4B43-D749-B049-E30785E73EB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data_required!$A$1:$AI$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data_required!$A$1:$AJ$57</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">dimension_Item_sets!$A$1:$AF$142</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3419" uniqueCount="675">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3476" uniqueCount="702">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -2063,6 +2063,87 @@
   </si>
   <si>
     <t>DvmJZSv0zxL</t>
+  </si>
+  <si>
+    <t>A.dx_name</t>
+  </si>
+  <si>
+    <t>PMTCT_STAT (D, DSD+TA, Age/Sex) TARGET</t>
+  </si>
+  <si>
+    <t>PMTCT_STAT Percentage at Entry Known Positive (DSD+TA, Age/Sex/Known)</t>
+  </si>
+  <si>
+    <t>FY19 Results Analytic Indicators: HTS_TST Yeild (HTS_TST_POS/HTS_TST)</t>
+  </si>
+  <si>
+    <t>PMTCT_HEI_POS (DSD+TA, &lt;= 2 months/Positive) Yield</t>
+  </si>
+  <si>
+    <t>PMTCT_HEI_POS (DSD+TA, 2 - 12 months/Positive) Yield</t>
+  </si>
+  <si>
+    <t>TB_STAT (DSD+TA, Age Aggregated/Sex) TARGETS</t>
+  </si>
+  <si>
+    <t>TB_STAT Percentage With already known status</t>
+  </si>
+  <si>
+    <t>VMMC_CIRC (DSD+TA, Age/Sex/HIVStatus) TARGET</t>
+  </si>
+  <si>
+    <t>VMMC_CIRC Indeterminate Rate (N, HIVStatus) FY19R</t>
+  </si>
+  <si>
+    <t>TX_CURR (DSD+TA, Age/Sex/HIVStatus) TARGET</t>
+  </si>
+  <si>
+    <t>FY19 Results Analytic Indicators: HTS_TST_POS (Age/Sex)</t>
+  </si>
+  <si>
+    <t>COP19 Targets HTS_SELF Directly Assisted</t>
+  </si>
+  <si>
+    <t>COP19 Targets HTS_SELF Unassisted</t>
+  </si>
+  <si>
+    <t>HTS_SELF (N, DSD+TA, Age/Sex/HIVSelfTest) TARGET</t>
+  </si>
+  <si>
+    <t>TX_TB Yield New ART  (D, DSD+TA, Age/Sex/TBScreen/NewExistingART/HIVStatus)</t>
+  </si>
+  <si>
+    <t>TX_TB Yield Already On ART (D, DSD+TA, Age/Sex/TBScreen/NewExistingART/HIVStatus)</t>
+  </si>
+  <si>
+    <t>OVC_SERV (DSD+TA, Age/Sex/ProgramStatus) TARGET</t>
+  </si>
+  <si>
+    <t>KP_MAT (DSD+TA, Sex) TARGET</t>
+  </si>
+  <si>
+    <t>HTS_TST (DSD+TA, KeyPop/Result) TARGET</t>
+  </si>
+  <si>
+    <t>TX_NEW (DSD+TA, KeyPop/HIVStatus) TARGET</t>
+  </si>
+  <si>
+    <t>PP_PREV (DSD+TA, Age/Sex) TARGET</t>
+  </si>
+  <si>
+    <t>PrEP_NEW (DSD+TA, Age/Sex) TARGET</t>
+  </si>
+  <si>
+    <t>GEND_GBV (DSD+TA, Physical Violence) TARGET</t>
+  </si>
+  <si>
+    <t>GEND_GBV (DSD+TA, Sexual Violence) TARGET</t>
+  </si>
+  <si>
+    <t>COP19 Targets GEND_GBV</t>
+  </si>
+  <si>
+    <t>PrEP_NEW (DSD+TA, KeyPopAbr) TARGET</t>
   </si>
 </sst>
 </file>
@@ -2471,13 +2552,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
-  <dimension ref="A1:AI57"/>
+  <dimension ref="A1:AJ57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AB23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A26" sqref="A26"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2488,15 +2569,15 @@
     <col min="4" max="4" width="255.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
-    <col min="7" max="7" width="68.33203125" customWidth="1"/>
-    <col min="8" max="8" width="22.83203125" customWidth="1"/>
-    <col min="9" max="19" width="17.33203125" customWidth="1"/>
-    <col min="20" max="20" width="46.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="68.33203125" customWidth="1"/>
+    <col min="9" max="9" width="22.83203125" customWidth="1"/>
+    <col min="10" max="20" width="17.33203125" customWidth="1"/>
+    <col min="21" max="21" width="46.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>197</v>
       </c>
@@ -2519,91 +2600,94 @@
         <v>514</v>
       </c>
       <c r="H1" t="s">
+        <v>675</v>
+      </c>
+      <c r="I1" t="s">
         <v>305</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>203</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>204</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>205</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>206</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>528</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>516</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>517</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>518</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>519</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>520</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>521</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>202</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>306</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>199</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>200</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>201</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>515</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>529</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>522</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>523</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>524</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>525</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>526</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>527</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>180</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>551</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2626,20 +2710,20 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
+        <v>676</v>
+      </c>
+      <c r="I2" t="s">
         <v>79</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>605</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>167</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>168</v>
       </c>
-      <c r="L2" t="s">
-        <v>170</v>
-      </c>
       <c r="M2" t="s">
         <v>170</v>
       </c>
@@ -2709,8 +2793,11 @@
       <c r="AI2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AJ2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2733,20 +2820,20 @@
         <v>4</v>
       </c>
       <c r="H3" t="s">
+        <v>677</v>
+      </c>
+      <c r="I3" t="s">
         <v>80</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>166</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>167</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>168</v>
       </c>
-      <c r="L3" t="s">
-        <v>170</v>
-      </c>
       <c r="M3" t="s">
         <v>170</v>
       </c>
@@ -2816,8 +2903,11 @@
       <c r="AI3" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="4" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2839,27 +2929,27 @@
       <c r="G4" t="s">
         <v>170</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" t="s">
+        <v>678</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>166</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>167</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>168</v>
       </c>
-      <c r="L4" t="s">
-        <v>170</v>
-      </c>
       <c r="M4" t="s">
+        <v>170</v>
+      </c>
+      <c r="N4" t="s">
         <v>660</v>
       </c>
-      <c r="N4" t="s">
-        <v>170</v>
-      </c>
       <c r="O4" t="s">
         <v>170</v>
       </c>
@@ -2923,8 +3013,11 @@
       <c r="AI4" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AJ4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2947,14 +3040,14 @@
         <v>9</v>
       </c>
       <c r="H5" t="s">
+        <v>679</v>
+      </c>
+      <c r="I5" t="s">
         <v>81</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>166</v>
       </c>
-      <c r="J5" t="s">
-        <v>170</v>
-      </c>
       <c r="K5" t="s">
         <v>170</v>
       </c>
@@ -3030,8 +3123,11 @@
       <c r="AI5" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AJ5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -3054,14 +3150,14 @@
         <v>10</v>
       </c>
       <c r="H6" t="s">
+        <v>680</v>
+      </c>
+      <c r="I6" t="s">
         <v>82</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>166</v>
       </c>
-      <c r="J6" t="s">
-        <v>170</v>
-      </c>
       <c r="K6" t="s">
         <v>170</v>
       </c>
@@ -3137,8 +3233,11 @@
       <c r="AI6" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AJ6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -3161,20 +3260,20 @@
         <v>12</v>
       </c>
       <c r="H7" t="s">
+        <v>681</v>
+      </c>
+      <c r="I7" t="s">
         <v>83</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>605</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>183</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>174</v>
       </c>
-      <c r="L7" t="s">
-        <v>170</v>
-      </c>
       <c r="M7" t="s">
         <v>170</v>
       </c>
@@ -3244,8 +3343,11 @@
       <c r="AI7" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AJ7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -3268,20 +3370,20 @@
         <v>12</v>
       </c>
       <c r="H8" t="s">
+        <v>681</v>
+      </c>
+      <c r="I8" t="s">
         <v>83</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>605</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>183</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>174</v>
       </c>
-      <c r="L8" t="s">
-        <v>170</v>
-      </c>
       <c r="M8" t="s">
         <v>170</v>
       </c>
@@ -3304,23 +3406,23 @@
         <v>170</v>
       </c>
       <c r="T8" t="s">
+        <v>170</v>
+      </c>
+      <c r="U8" t="s">
         <v>84</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>85</v>
       </c>
-      <c r="V8" t="s">
+      <c r="W8" t="s">
         <v>166</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>183</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>174</v>
       </c>
-      <c r="Y8" t="s">
-        <v>170</v>
-      </c>
       <c r="Z8" t="s">
         <v>170</v>
       </c>
@@ -3343,16 +3445,19 @@
         <v>170</v>
       </c>
       <c r="AG8" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH8" t="s">
         <v>181</v>
       </c>
-      <c r="AH8" t="s">
-        <v>170</v>
-      </c>
       <c r="AI8" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AJ8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -3375,20 +3480,20 @@
         <v>14</v>
       </c>
       <c r="H9" t="s">
+        <v>682</v>
+      </c>
+      <c r="I9" t="s">
         <v>86</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>166</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>183</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>174</v>
       </c>
-      <c r="L9" t="s">
-        <v>170</v>
-      </c>
       <c r="M9" t="s">
         <v>170</v>
       </c>
@@ -3458,8 +3563,11 @@
       <c r="AI9" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="10" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -3481,27 +3589,27 @@
       <c r="G10" t="s">
         <v>170</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" t="s">
+        <v>678</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>166</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>183</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>174</v>
       </c>
-      <c r="L10" t="s">
-        <v>170</v>
-      </c>
       <c r="M10" t="s">
+        <v>170</v>
+      </c>
+      <c r="N10" t="s">
         <v>663</v>
       </c>
-      <c r="N10" t="s">
-        <v>170</v>
-      </c>
       <c r="O10" t="s">
         <v>170</v>
       </c>
@@ -3565,8 +3673,11 @@
       <c r="AI10" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AJ10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -3589,20 +3700,20 @@
         <v>673</v>
       </c>
       <c r="H11" t="s">
+        <v>683</v>
+      </c>
+      <c r="I11" t="s">
         <v>674</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>605</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>167</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>182</v>
       </c>
-      <c r="L11" t="s">
-        <v>170</v>
-      </c>
       <c r="M11" t="s">
         <v>170</v>
       </c>
@@ -3672,8 +3783,11 @@
       <c r="AI11" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="12" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -3695,27 +3809,27 @@
       <c r="G12" t="s">
         <v>170</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" t="s">
+        <v>678</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>166</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>167</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>182</v>
       </c>
-      <c r="L12" t="s">
-        <v>170</v>
-      </c>
       <c r="M12" t="s">
+        <v>170</v>
+      </c>
+      <c r="N12" t="s">
         <v>659</v>
       </c>
-      <c r="N12" t="s">
-        <v>170</v>
-      </c>
       <c r="O12" t="s">
         <v>170</v>
       </c>
@@ -3779,8 +3893,11 @@
       <c r="AI12" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AJ12" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -3803,20 +3920,20 @@
         <v>608</v>
       </c>
       <c r="H13" t="s">
+        <v>684</v>
+      </c>
+      <c r="I13" t="s">
         <v>609</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>166</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>167</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>182</v>
       </c>
-      <c r="L13" t="s">
-        <v>170</v>
-      </c>
       <c r="M13" t="s">
         <v>170</v>
       </c>
@@ -3886,8 +4003,11 @@
       <c r="AI13" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AJ13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -3910,20 +4030,20 @@
         <v>21</v>
       </c>
       <c r="H14" t="s">
+        <v>685</v>
+      </c>
+      <c r="I14" t="s">
         <v>87</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>605</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>183</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>184</v>
       </c>
-      <c r="L14" t="s">
-        <v>170</v>
-      </c>
       <c r="M14" t="s">
         <v>170</v>
       </c>
@@ -3993,8 +4113,11 @@
       <c r="AI14" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="15" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -4016,27 +4139,27 @@
       <c r="G15" t="s">
         <v>170</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" t="s">
+        <v>678</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>166</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>185</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>184</v>
       </c>
-      <c r="L15" t="s">
-        <v>170</v>
-      </c>
       <c r="M15" t="s">
+        <v>170</v>
+      </c>
+      <c r="N15" t="s">
         <v>533</v>
       </c>
-      <c r="N15" t="s">
-        <v>170</v>
-      </c>
       <c r="O15" t="s">
         <v>170</v>
       </c>
@@ -4100,8 +4223,11 @@
       <c r="AI15" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="16" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ15" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -4123,27 +4249,27 @@
       <c r="G16" t="s">
         <v>170</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" t="s">
+        <v>678</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>166</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>185</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>184</v>
       </c>
-      <c r="L16" t="s">
-        <v>170</v>
-      </c>
       <c r="M16" t="s">
+        <v>170</v>
+      </c>
+      <c r="N16" t="s">
         <v>534</v>
       </c>
-      <c r="N16" t="s">
-        <v>170</v>
-      </c>
       <c r="O16" t="s">
         <v>170</v>
       </c>
@@ -4207,8 +4333,11 @@
       <c r="AI16" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="17" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -4230,27 +4359,27 @@
       <c r="G17" t="s">
         <v>170</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" t="s">
+        <v>686</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>166</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>185</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>184</v>
       </c>
-      <c r="L17" t="s">
-        <v>170</v>
-      </c>
       <c r="M17" t="s">
+        <v>170</v>
+      </c>
+      <c r="N17" t="s">
         <v>533</v>
       </c>
-      <c r="N17" t="s">
-        <v>170</v>
-      </c>
       <c r="O17" t="s">
         <v>170</v>
       </c>
@@ -4269,27 +4398,27 @@
       <c r="T17" t="s">
         <v>170</v>
       </c>
-      <c r="U17" s="1" t="s">
+      <c r="U17" t="s">
+        <v>170</v>
+      </c>
+      <c r="V17" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="V17" t="s">
+      <c r="W17" t="s">
         <v>166</v>
       </c>
-      <c r="W17" t="s">
+      <c r="X17" t="s">
         <v>185</v>
       </c>
-      <c r="X17" t="s">
+      <c r="Y17" t="s">
         <v>184</v>
       </c>
-      <c r="Y17" t="s">
-        <v>170</v>
-      </c>
       <c r="Z17" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA17" t="s">
         <v>534</v>
       </c>
-      <c r="AA17" t="s">
-        <v>170</v>
-      </c>
       <c r="AB17" t="s">
         <v>170</v>
       </c>
@@ -4306,16 +4435,19 @@
         <v>170</v>
       </c>
       <c r="AG17" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH17" t="s">
         <v>331</v>
-      </c>
-      <c r="AH17">
-        <v>0</v>
       </c>
       <c r="AI17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -4337,27 +4469,27 @@
       <c r="G18" t="s">
         <v>170</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" t="s">
+        <v>686</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>166</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>185</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>184</v>
       </c>
-      <c r="L18" t="s">
-        <v>170</v>
-      </c>
       <c r="M18" t="s">
+        <v>170</v>
+      </c>
+      <c r="N18" t="s">
         <v>532</v>
       </c>
-      <c r="N18" t="s">
-        <v>170</v>
-      </c>
       <c r="O18" t="s">
         <v>170</v>
       </c>
@@ -4376,21 +4508,21 @@
       <c r="T18" t="s">
         <v>170</v>
       </c>
-      <c r="U18" s="1" t="s">
+      <c r="U18" t="s">
+        <v>170</v>
+      </c>
+      <c r="V18" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="V18" t="s">
+      <c r="W18" t="s">
         <v>166</v>
       </c>
-      <c r="W18" s="9" t="s">
+      <c r="X18" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="X18" t="s">
+      <c r="Y18" t="s">
         <v>184</v>
       </c>
-      <c r="Y18" t="s">
-        <v>170</v>
-      </c>
       <c r="Z18" t="s">
         <v>170</v>
       </c>
@@ -4413,16 +4545,19 @@
         <v>170</v>
       </c>
       <c r="AG18" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH18" t="s">
         <v>192</v>
       </c>
-      <c r="AH18" t="s">
-        <v>170</v>
-      </c>
       <c r="AI18" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="19" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -4444,27 +4579,27 @@
       <c r="G19" t="s">
         <v>170</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" t="s">
+        <v>686</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>166</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>185</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>184</v>
       </c>
-      <c r="L19" t="s">
-        <v>170</v>
-      </c>
       <c r="M19" t="s">
+        <v>170</v>
+      </c>
+      <c r="N19" t="s">
         <v>535</v>
       </c>
-      <c r="N19" t="s">
-        <v>170</v>
-      </c>
       <c r="O19" t="s">
         <v>170</v>
       </c>
@@ -4483,21 +4618,21 @@
       <c r="T19" t="s">
         <v>170</v>
       </c>
-      <c r="U19" s="1" t="s">
+      <c r="U19" t="s">
+        <v>170</v>
+      </c>
+      <c r="V19" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="V19" t="s">
+      <c r="W19" t="s">
         <v>166</v>
       </c>
-      <c r="W19" s="9" t="s">
+      <c r="X19" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="X19" t="s">
+      <c r="Y19" t="s">
         <v>184</v>
       </c>
-      <c r="Y19" t="s">
-        <v>170</v>
-      </c>
       <c r="Z19" t="s">
         <v>170</v>
       </c>
@@ -4520,16 +4655,19 @@
         <v>170</v>
       </c>
       <c r="AG19" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH19" t="s">
         <v>192</v>
       </c>
-      <c r="AH19" t="s">
-        <v>170</v>
-      </c>
       <c r="AI19" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="20" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ19" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -4551,27 +4689,27 @@
       <c r="G20" t="s">
         <v>170</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" t="s">
+        <v>686</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>166</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>185</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>184</v>
       </c>
-      <c r="L20" t="s">
-        <v>170</v>
-      </c>
       <c r="M20" t="s">
+        <v>170</v>
+      </c>
+      <c r="N20" t="s">
         <v>536</v>
       </c>
-      <c r="N20" t="s">
-        <v>170</v>
-      </c>
       <c r="O20" t="s">
         <v>170</v>
       </c>
@@ -4590,21 +4728,21 @@
       <c r="T20" t="s">
         <v>170</v>
       </c>
-      <c r="U20" s="1" t="s">
+      <c r="U20" t="s">
+        <v>170</v>
+      </c>
+      <c r="V20" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="V20" t="s">
+      <c r="W20" t="s">
         <v>166</v>
       </c>
-      <c r="W20" s="9" t="s">
+      <c r="X20" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="X20" t="s">
+      <c r="Y20" t="s">
         <v>184</v>
       </c>
-      <c r="Y20" t="s">
-        <v>170</v>
-      </c>
       <c r="Z20" t="s">
         <v>170</v>
       </c>
@@ -4627,16 +4765,19 @@
         <v>170</v>
       </c>
       <c r="AG20" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH20" t="s">
         <v>192</v>
       </c>
-      <c r="AH20" t="s">
-        <v>170</v>
-      </c>
       <c r="AI20" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="21" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ20" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -4658,27 +4799,27 @@
       <c r="G21" t="s">
         <v>170</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H21" t="s">
+        <v>686</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>166</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>185</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>184</v>
       </c>
-      <c r="L21" t="s">
-        <v>170</v>
-      </c>
       <c r="M21" t="s">
+        <v>170</v>
+      </c>
+      <c r="N21" t="s">
         <v>537</v>
       </c>
-      <c r="N21" t="s">
-        <v>170</v>
-      </c>
       <c r="O21" t="s">
         <v>170</v>
       </c>
@@ -4697,21 +4838,21 @@
       <c r="T21" t="s">
         <v>170</v>
       </c>
-      <c r="U21" s="1" t="s">
+      <c r="U21" t="s">
+        <v>170</v>
+      </c>
+      <c r="V21" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="V21" t="s">
+      <c r="W21" t="s">
         <v>166</v>
       </c>
-      <c r="W21" s="9" t="s">
+      <c r="X21" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="X21" t="s">
+      <c r="Y21" t="s">
         <v>184</v>
       </c>
-      <c r="Y21" t="s">
-        <v>170</v>
-      </c>
       <c r="Z21" t="s">
         <v>170</v>
       </c>
@@ -4734,16 +4875,19 @@
         <v>170</v>
       </c>
       <c r="AG21" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH21" t="s">
         <v>192</v>
       </c>
-      <c r="AH21" t="s">
-        <v>170</v>
-      </c>
       <c r="AI21" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="22" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ21" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -4765,27 +4909,27 @@
       <c r="G22" t="s">
         <v>170</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H22" t="s">
+        <v>686</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>166</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>185</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>184</v>
       </c>
-      <c r="L22" t="s">
-        <v>170</v>
-      </c>
       <c r="M22" t="s">
+        <v>170</v>
+      </c>
+      <c r="N22" t="s">
         <v>538</v>
       </c>
-      <c r="N22" t="s">
-        <v>170</v>
-      </c>
       <c r="O22" t="s">
         <v>170</v>
       </c>
@@ -4804,21 +4948,21 @@
       <c r="T22" t="s">
         <v>170</v>
       </c>
-      <c r="U22" s="1" t="s">
+      <c r="U22" t="s">
+        <v>170</v>
+      </c>
+      <c r="V22" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="V22" t="s">
+      <c r="W22" t="s">
         <v>166</v>
       </c>
-      <c r="W22" s="9" t="s">
+      <c r="X22" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="X22" t="s">
+      <c r="Y22" t="s">
         <v>184</v>
       </c>
-      <c r="Y22" t="s">
-        <v>170</v>
-      </c>
       <c r="Z22" t="s">
         <v>170</v>
       </c>
@@ -4841,16 +4985,19 @@
         <v>170</v>
       </c>
       <c r="AG22" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH22" t="s">
         <v>192</v>
       </c>
-      <c r="AH22" t="s">
-        <v>170</v>
-      </c>
       <c r="AI22" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="23" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ22" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -4872,27 +5019,27 @@
       <c r="G23" t="s">
         <v>170</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="H23" t="s">
+        <v>686</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>166</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="K23" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>184</v>
       </c>
-      <c r="L23" t="s">
-        <v>170</v>
-      </c>
       <c r="M23" t="s">
+        <v>170</v>
+      </c>
+      <c r="N23" t="s">
         <v>539</v>
       </c>
-      <c r="N23" t="s">
-        <v>170</v>
-      </c>
       <c r="O23" t="s">
         <v>170</v>
       </c>
@@ -4911,21 +5058,21 @@
       <c r="T23" t="s">
         <v>170</v>
       </c>
-      <c r="U23" s="1" t="s">
+      <c r="U23" t="s">
+        <v>170</v>
+      </c>
+      <c r="V23" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="V23" t="s">
+      <c r="W23" t="s">
         <v>166</v>
       </c>
-      <c r="W23" s="3" t="s">
+      <c r="X23" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="X23" t="s">
+      <c r="Y23" t="s">
         <v>184</v>
       </c>
-      <c r="Y23" t="s">
-        <v>170</v>
-      </c>
       <c r="Z23" t="s">
         <v>170</v>
       </c>
@@ -4948,16 +5095,19 @@
         <v>170</v>
       </c>
       <c r="AG23" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH23" t="s">
         <v>192</v>
       </c>
-      <c r="AH23" t="s">
-        <v>170</v>
-      </c>
       <c r="AI23" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="24" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ23" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -4979,27 +5129,27 @@
       <c r="G24" t="s">
         <v>170</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H24" t="s">
+        <v>686</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>166</v>
       </c>
-      <c r="J24" s="3" t="s">
+      <c r="K24" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>184</v>
       </c>
-      <c r="L24" t="s">
-        <v>170</v>
-      </c>
       <c r="M24" t="s">
+        <v>170</v>
+      </c>
+      <c r="N24" t="s">
         <v>540</v>
       </c>
-      <c r="N24" t="s">
-        <v>170</v>
-      </c>
       <c r="O24" t="s">
         <v>170</v>
       </c>
@@ -5018,21 +5168,21 @@
       <c r="T24" t="s">
         <v>170</v>
       </c>
-      <c r="U24" s="1" t="s">
+      <c r="U24" t="s">
+        <v>170</v>
+      </c>
+      <c r="V24" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="V24" t="s">
+      <c r="W24" t="s">
         <v>166</v>
       </c>
-      <c r="W24" s="3" t="s">
+      <c r="X24" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="X24" t="s">
+      <c r="Y24" t="s">
         <v>184</v>
       </c>
-      <c r="Y24" t="s">
-        <v>170</v>
-      </c>
       <c r="Z24" t="s">
         <v>170</v>
       </c>
@@ -5055,16 +5205,19 @@
         <v>170</v>
       </c>
       <c r="AG24" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH24" t="s">
         <v>192</v>
       </c>
-      <c r="AH24" t="s">
-        <v>170</v>
-      </c>
       <c r="AI24" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="25" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ24" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -5086,27 +5239,27 @@
       <c r="G25" t="s">
         <v>170</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H25" t="s">
+        <v>686</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>166</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>185</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>184</v>
       </c>
-      <c r="L25" t="s">
-        <v>170</v>
-      </c>
       <c r="M25" t="s">
+        <v>170</v>
+      </c>
+      <c r="N25" t="s">
         <v>541</v>
       </c>
-      <c r="N25" t="s">
-        <v>170</v>
-      </c>
       <c r="O25" t="s">
         <v>170</v>
       </c>
@@ -5125,21 +5278,21 @@
       <c r="T25" t="s">
         <v>170</v>
       </c>
-      <c r="U25" s="1" t="s">
+      <c r="U25" t="s">
+        <v>170</v>
+      </c>
+      <c r="V25" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="V25" t="s">
+      <c r="W25" t="s">
         <v>166</v>
       </c>
-      <c r="W25" s="9" t="s">
+      <c r="X25" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="X25" t="s">
+      <c r="Y25" t="s">
         <v>184</v>
       </c>
-      <c r="Y25" t="s">
-        <v>170</v>
-      </c>
       <c r="Z25" t="s">
         <v>170</v>
       </c>
@@ -5162,16 +5315,19 @@
         <v>170</v>
       </c>
       <c r="AG25" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH25" t="s">
         <v>192</v>
       </c>
-      <c r="AH25" t="s">
-        <v>170</v>
-      </c>
       <c r="AI25" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="26" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ25" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -5193,27 +5349,27 @@
       <c r="G26" t="s">
         <v>170</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="H26" t="s">
+        <v>686</v>
+      </c>
+      <c r="I26" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>166</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>185</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>184</v>
       </c>
-      <c r="L26" t="s">
-        <v>170</v>
-      </c>
       <c r="M26" t="s">
+        <v>170</v>
+      </c>
+      <c r="N26" t="s">
         <v>542</v>
       </c>
-      <c r="N26" t="s">
-        <v>170</v>
-      </c>
       <c r="O26" t="s">
         <v>170</v>
       </c>
@@ -5232,21 +5388,21 @@
       <c r="T26" t="s">
         <v>170</v>
       </c>
-      <c r="U26" s="1" t="s">
+      <c r="U26" t="s">
+        <v>170</v>
+      </c>
+      <c r="V26" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="V26" t="s">
+      <c r="W26" t="s">
         <v>166</v>
       </c>
-      <c r="W26" s="9" t="s">
+      <c r="X26" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="X26" t="s">
+      <c r="Y26" t="s">
         <v>184</v>
       </c>
-      <c r="Y26" t="s">
-        <v>170</v>
-      </c>
       <c r="Z26" t="s">
         <v>170</v>
       </c>
@@ -5269,16 +5425,19 @@
         <v>170</v>
       </c>
       <c r="AG26" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH26" t="s">
         <v>192</v>
       </c>
-      <c r="AH26" t="s">
-        <v>170</v>
-      </c>
       <c r="AI26" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="27" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -5300,27 +5459,27 @@
       <c r="G27" t="s">
         <v>170</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="H27" t="s">
+        <v>686</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>166</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>185</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>184</v>
       </c>
-      <c r="L27" t="s">
-        <v>170</v>
-      </c>
       <c r="M27" t="s">
+        <v>170</v>
+      </c>
+      <c r="N27" t="s">
         <v>543</v>
       </c>
-      <c r="N27" t="s">
-        <v>170</v>
-      </c>
       <c r="O27" t="s">
         <v>170</v>
       </c>
@@ -5339,21 +5498,21 @@
       <c r="T27" t="s">
         <v>170</v>
       </c>
-      <c r="U27" s="1" t="s">
+      <c r="U27" t="s">
+        <v>170</v>
+      </c>
+      <c r="V27" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="V27" t="s">
+      <c r="W27" t="s">
         <v>166</v>
       </c>
-      <c r="W27" s="9" t="s">
+      <c r="X27" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="X27" t="s">
+      <c r="Y27" t="s">
         <v>184</v>
       </c>
-      <c r="Y27" t="s">
-        <v>170</v>
-      </c>
       <c r="Z27" t="s">
         <v>170</v>
       </c>
@@ -5376,16 +5535,19 @@
         <v>170</v>
       </c>
       <c r="AG27" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH27" t="s">
         <v>192</v>
       </c>
-      <c r="AH27" t="s">
-        <v>170</v>
-      </c>
       <c r="AI27" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="28" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ27" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -5407,27 +5569,27 @@
       <c r="G28" t="s">
         <v>170</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="H28" t="s">
+        <v>678</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>166</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>185</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>184</v>
       </c>
-      <c r="L28" t="s">
-        <v>170</v>
-      </c>
       <c r="M28" t="s">
+        <v>170</v>
+      </c>
+      <c r="N28" t="s">
         <v>532</v>
       </c>
-      <c r="N28" t="s">
-        <v>170</v>
-      </c>
       <c r="O28" t="s">
         <v>170</v>
       </c>
@@ -5491,8 +5653,11 @@
       <c r="AI28" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="29" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ28" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -5514,27 +5679,27 @@
       <c r="G29" t="s">
         <v>170</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="H29" t="s">
+        <v>678</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>166</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>185</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>184</v>
       </c>
-      <c r="L29" t="s">
-        <v>170</v>
-      </c>
       <c r="M29" t="s">
+        <v>170</v>
+      </c>
+      <c r="N29" t="s">
         <v>535</v>
       </c>
-      <c r="N29" t="s">
-        <v>170</v>
-      </c>
       <c r="O29" t="s">
         <v>170</v>
       </c>
@@ -5598,8 +5763,11 @@
       <c r="AI29" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="30" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ29" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="30" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -5621,27 +5789,27 @@
       <c r="G30" t="s">
         <v>170</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="H30" t="s">
+        <v>678</v>
+      </c>
+      <c r="I30" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>166</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>185</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>184</v>
       </c>
-      <c r="L30" t="s">
-        <v>170</v>
-      </c>
       <c r="M30" t="s">
+        <v>170</v>
+      </c>
+      <c r="N30" t="s">
         <v>536</v>
       </c>
-      <c r="N30" t="s">
-        <v>170</v>
-      </c>
       <c r="O30" t="s">
         <v>170</v>
       </c>
@@ -5705,8 +5873,11 @@
       <c r="AI30" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="31" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ30" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="31" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -5728,27 +5899,27 @@
       <c r="G31" t="s">
         <v>170</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="H31" t="s">
+        <v>678</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>166</v>
       </c>
-      <c r="J31" t="s">
+      <c r="K31" t="s">
         <v>185</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
         <v>184</v>
       </c>
-      <c r="L31" t="s">
-        <v>170</v>
-      </c>
       <c r="M31" t="s">
+        <v>170</v>
+      </c>
+      <c r="N31" t="s">
         <v>537</v>
       </c>
-      <c r="N31" t="s">
-        <v>170</v>
-      </c>
       <c r="O31" t="s">
         <v>170</v>
       </c>
@@ -5812,8 +5983,11 @@
       <c r="AI31" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="32" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ31" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -5835,27 +6009,27 @@
       <c r="G32" t="s">
         <v>170</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="H32" t="s">
+        <v>678</v>
+      </c>
+      <c r="I32" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>166</v>
       </c>
-      <c r="J32" t="s">
+      <c r="K32" t="s">
         <v>185</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
         <v>184</v>
       </c>
-      <c r="L32" t="s">
-        <v>170</v>
-      </c>
       <c r="M32" t="s">
+        <v>170</v>
+      </c>
+      <c r="N32" t="s">
         <v>538</v>
       </c>
-      <c r="N32" t="s">
-        <v>170</v>
-      </c>
       <c r="O32" t="s">
         <v>170</v>
       </c>
@@ -5919,8 +6093,11 @@
       <c r="AI32" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="33" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ32" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="33" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -5942,27 +6119,27 @@
       <c r="G33" t="s">
         <v>170</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="H33" t="s">
+        <v>678</v>
+      </c>
+      <c r="I33" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>166</v>
       </c>
-      <c r="J33" s="3" t="s">
+      <c r="K33" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>184</v>
       </c>
-      <c r="L33" t="s">
-        <v>170</v>
-      </c>
       <c r="M33" t="s">
+        <v>170</v>
+      </c>
+      <c r="N33" t="s">
         <v>539</v>
       </c>
-      <c r="N33" t="s">
-        <v>170</v>
-      </c>
       <c r="O33" t="s">
         <v>170</v>
       </c>
@@ -6026,8 +6203,11 @@
       <c r="AI33" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="34" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ33" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="34" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -6049,27 +6229,27 @@
       <c r="G34" t="s">
         <v>170</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="H34" t="s">
+        <v>678</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>166</v>
       </c>
-      <c r="J34" s="3" t="s">
+      <c r="K34" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
         <v>184</v>
       </c>
-      <c r="L34" t="s">
-        <v>170</v>
-      </c>
       <c r="M34" t="s">
+        <v>170</v>
+      </c>
+      <c r="N34" t="s">
         <v>540</v>
       </c>
-      <c r="N34" t="s">
-        <v>170</v>
-      </c>
       <c r="O34" t="s">
         <v>170</v>
       </c>
@@ -6133,8 +6313,11 @@
       <c r="AI34" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="35" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ34" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="35" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -6156,27 +6339,27 @@
       <c r="G35" t="s">
         <v>170</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="H35" t="s">
+        <v>678</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="I35" t="s">
+      <c r="J35" t="s">
         <v>166</v>
       </c>
-      <c r="J35" t="s">
+      <c r="K35" t="s">
         <v>185</v>
       </c>
-      <c r="K35" t="s">
+      <c r="L35" t="s">
         <v>184</v>
       </c>
-      <c r="L35" t="s">
-        <v>170</v>
-      </c>
       <c r="M35" t="s">
+        <v>170</v>
+      </c>
+      <c r="N35" t="s">
         <v>541</v>
       </c>
-      <c r="N35" t="s">
-        <v>170</v>
-      </c>
       <c r="O35" t="s">
         <v>170</v>
       </c>
@@ -6240,8 +6423,11 @@
       <c r="AI35" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="36" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ35" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="36" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -6263,27 +6449,27 @@
       <c r="G36" t="s">
         <v>170</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="H36" t="s">
+        <v>678</v>
+      </c>
+      <c r="I36" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>166</v>
       </c>
-      <c r="J36" t="s">
+      <c r="K36" t="s">
         <v>185</v>
       </c>
-      <c r="K36" t="s">
+      <c r="L36" t="s">
         <v>184</v>
       </c>
-      <c r="L36" t="s">
-        <v>170</v>
-      </c>
       <c r="M36" t="s">
+        <v>170</v>
+      </c>
+      <c r="N36" t="s">
         <v>542</v>
       </c>
-      <c r="N36" t="s">
-        <v>170</v>
-      </c>
       <c r="O36" t="s">
         <v>170</v>
       </c>
@@ -6347,8 +6533,11 @@
       <c r="AI36" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="37" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ36" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="37" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -6370,27 +6559,27 @@
       <c r="G37" t="s">
         <v>170</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="H37" t="s">
+        <v>678</v>
+      </c>
+      <c r="I37" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
         <v>166</v>
       </c>
-      <c r="J37" t="s">
+      <c r="K37" t="s">
         <v>185</v>
       </c>
-      <c r="K37" t="s">
+      <c r="L37" t="s">
         <v>184</v>
       </c>
-      <c r="L37" t="s">
-        <v>170</v>
-      </c>
       <c r="M37" t="s">
+        <v>170</v>
+      </c>
+      <c r="N37" t="s">
         <v>543</v>
       </c>
-      <c r="N37" t="s">
-        <v>170</v>
-      </c>
       <c r="O37" t="s">
         <v>170</v>
       </c>
@@ -6454,8 +6643,11 @@
       <c r="AI37" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="38" spans="1:35" ht="19" x14ac:dyDescent="0.25">
+      <c r="AJ37" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="38" spans="1:36" ht="19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -6477,21 +6669,21 @@
       <c r="G38" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="H38" t="s">
+        <v>687</v>
+      </c>
+      <c r="I38" s="1" t="s">
         <v>664</v>
       </c>
-      <c r="I38" t="s">
+      <c r="J38" t="s">
         <v>605</v>
       </c>
-      <c r="J38" t="s">
+      <c r="K38" t="s">
         <v>167</v>
       </c>
-      <c r="K38" t="s">
+      <c r="L38" t="s">
         <v>174</v>
       </c>
-      <c r="L38" t="s">
-        <v>170</v>
-      </c>
       <c r="M38" t="s">
         <v>170</v>
       </c>
@@ -6513,7 +6705,7 @@
       <c r="S38" t="s">
         <v>170</v>
       </c>
-      <c r="T38" s="1" t="s">
+      <c r="T38" t="s">
         <v>170</v>
       </c>
       <c r="U38" s="1" t="s">
@@ -6528,7 +6720,7 @@
       <c r="X38" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="Y38" t="s">
+      <c r="Y38" s="1" t="s">
         <v>170</v>
       </c>
       <c r="Z38" t="s">
@@ -6552,17 +6744,20 @@
       <c r="AF38" t="s">
         <v>170</v>
       </c>
-      <c r="AG38" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH38" t="s">
+      <c r="AG38" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH38" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AI38" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="39" spans="1:35" ht="19" x14ac:dyDescent="0.25">
+      <c r="AJ38" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="1:36" ht="19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>22</v>
       </c>
@@ -6584,21 +6779,21 @@
       <c r="G39" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="H39" t="s">
+        <v>688</v>
+      </c>
+      <c r="I39" s="1" t="s">
         <v>665</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="J39" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="J39" t="s">
+      <c r="K39" t="s">
         <v>666</v>
       </c>
-      <c r="K39" t="s">
+      <c r="L39" t="s">
         <v>670</v>
       </c>
-      <c r="L39" t="s">
-        <v>170</v>
-      </c>
       <c r="M39" t="s">
         <v>170</v>
       </c>
@@ -6620,7 +6815,7 @@
       <c r="S39" t="s">
         <v>170</v>
       </c>
-      <c r="T39" s="1" t="s">
+      <c r="T39" t="s">
         <v>170</v>
       </c>
       <c r="U39" s="1" t="s">
@@ -6635,7 +6830,7 @@
       <c r="X39" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="Y39" t="s">
+      <c r="Y39" s="1" t="s">
         <v>170</v>
       </c>
       <c r="Z39" t="s">
@@ -6659,17 +6854,20 @@
       <c r="AF39" t="s">
         <v>170</v>
       </c>
-      <c r="AG39" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH39" t="s">
+      <c r="AG39" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH39" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AI39" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="40" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ39" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="40" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -6692,20 +6890,20 @@
         <v>218</v>
       </c>
       <c r="H40" t="s">
+        <v>689</v>
+      </c>
+      <c r="I40" t="s">
         <v>217</v>
       </c>
-      <c r="I40" t="s">
+      <c r="J40" t="s">
         <v>605</v>
       </c>
-      <c r="J40" t="s">
+      <c r="K40" t="s">
         <v>167</v>
       </c>
-      <c r="K40" t="s">
+      <c r="L40" t="s">
         <v>174</v>
       </c>
-      <c r="L40" t="s">
-        <v>170</v>
-      </c>
       <c r="M40" t="s">
         <v>170</v>
       </c>
@@ -6728,23 +6926,23 @@
         <v>170</v>
       </c>
       <c r="T40" t="s">
+        <v>170</v>
+      </c>
+      <c r="U40" t="s">
         <v>220</v>
       </c>
-      <c r="U40" t="s">
+      <c r="V40" t="s">
         <v>219</v>
       </c>
-      <c r="V40" s="1" t="s">
+      <c r="W40" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="W40" s="9" t="s">
+      <c r="X40" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="X40" t="s">
+      <c r="Y40" t="s">
         <v>174</v>
       </c>
-      <c r="Y40" t="s">
-        <v>170</v>
-      </c>
       <c r="Z40" t="s">
         <v>170</v>
       </c>
@@ -6767,16 +6965,19 @@
         <v>170</v>
       </c>
       <c r="AG40" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH40" t="s">
         <v>181</v>
       </c>
-      <c r="AH40" t="s">
-        <v>170</v>
-      </c>
       <c r="AI40" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="41" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ40" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="41" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -6798,21 +6999,21 @@
       <c r="G41" t="s">
         <v>616</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="H41" t="s">
+        <v>690</v>
+      </c>
+      <c r="I41" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="I41" t="s">
+      <c r="J41" t="s">
         <v>166</v>
       </c>
-      <c r="J41" s="9" t="s">
+      <c r="K41" s="9" t="s">
         <v>511</v>
       </c>
-      <c r="K41" t="s">
+      <c r="L41" t="s">
         <v>174</v>
       </c>
-      <c r="L41" t="s">
-        <v>170</v>
-      </c>
       <c r="M41" t="s">
         <v>170</v>
       </c>
@@ -6834,7 +7035,7 @@
       <c r="S41" t="s">
         <v>170</v>
       </c>
-      <c r="T41" s="1" t="s">
+      <c r="T41" t="s">
         <v>170</v>
       </c>
       <c r="U41" s="1" t="s">
@@ -6849,7 +7050,7 @@
       <c r="X41" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="Y41" t="s">
+      <c r="Y41" s="1" t="s">
         <v>170</v>
       </c>
       <c r="Z41" t="s">
@@ -6873,17 +7074,20 @@
       <c r="AF41" t="s">
         <v>170</v>
       </c>
-      <c r="AG41" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH41" t="s">
+      <c r="AG41" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH41" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AI41" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="42" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ41" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -6905,21 +7109,21 @@
       <c r="G42" t="s">
         <v>617</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="H42" t="s">
+        <v>691</v>
+      </c>
+      <c r="I42" s="1" t="s">
         <v>618</v>
       </c>
-      <c r="I42" t="s">
+      <c r="J42" t="s">
         <v>166</v>
       </c>
-      <c r="J42" s="9" t="s">
+      <c r="K42" s="9" t="s">
         <v>511</v>
       </c>
-      <c r="K42" t="s">
+      <c r="L42" t="s">
         <v>174</v>
       </c>
-      <c r="L42" t="s">
-        <v>170</v>
-      </c>
       <c r="M42" t="s">
         <v>170</v>
       </c>
@@ -6941,7 +7145,7 @@
       <c r="S42" t="s">
         <v>170</v>
       </c>
-      <c r="T42" s="1" t="s">
+      <c r="T42" t="s">
         <v>170</v>
       </c>
       <c r="U42" s="1" t="s">
@@ -6956,7 +7160,7 @@
       <c r="X42" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="Y42" t="s">
+      <c r="Y42" s="1" t="s">
         <v>170</v>
       </c>
       <c r="Z42" t="s">
@@ -6980,17 +7184,20 @@
       <c r="AF42" t="s">
         <v>170</v>
       </c>
-      <c r="AG42" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH42" t="s">
+      <c r="AG42" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH42" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AI42" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="43" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ42" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="43" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -7013,20 +7220,20 @@
         <v>612</v>
       </c>
       <c r="H43" t="s">
+        <v>692</v>
+      </c>
+      <c r="I43" t="s">
         <v>613</v>
       </c>
-      <c r="I43" t="s">
+      <c r="J43" t="s">
         <v>605</v>
       </c>
-      <c r="J43" t="s">
+      <c r="K43" t="s">
         <v>311</v>
       </c>
-      <c r="K43" t="s">
+      <c r="L43" t="s">
         <v>184</v>
       </c>
-      <c r="L43" t="s">
-        <v>170</v>
-      </c>
       <c r="M43" t="s">
         <v>170</v>
       </c>
@@ -7048,7 +7255,7 @@
       <c r="S43" t="s">
         <v>170</v>
       </c>
-      <c r="T43" s="1" t="s">
+      <c r="T43" t="s">
         <v>170</v>
       </c>
       <c r="U43" s="1" t="s">
@@ -7063,7 +7270,7 @@
       <c r="X43" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="Y43" t="s">
+      <c r="Y43" s="1" t="s">
         <v>170</v>
       </c>
       <c r="Z43" t="s">
@@ -7087,17 +7294,20 @@
       <c r="AF43" t="s">
         <v>170</v>
       </c>
-      <c r="AG43" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH43" t="s">
+      <c r="AG43" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH43" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AI43" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="44" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ43" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="44" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -7120,20 +7330,20 @@
         <v>612</v>
       </c>
       <c r="H44" t="s">
+        <v>692</v>
+      </c>
+      <c r="I44" t="s">
         <v>613</v>
       </c>
-      <c r="I44" t="s">
+      <c r="J44" t="s">
         <v>605</v>
       </c>
-      <c r="J44" t="s">
+      <c r="K44" t="s">
         <v>311</v>
       </c>
-      <c r="K44" t="s">
+      <c r="L44" t="s">
         <v>184</v>
       </c>
-      <c r="L44" t="s">
-        <v>170</v>
-      </c>
       <c r="M44" t="s">
         <v>170</v>
       </c>
@@ -7156,23 +7366,23 @@
         <v>170</v>
       </c>
       <c r="T44" t="s">
+        <v>170</v>
+      </c>
+      <c r="U44" t="s">
         <v>610</v>
       </c>
-      <c r="U44" t="s">
+      <c r="V44" t="s">
         <v>611</v>
       </c>
-      <c r="V44" s="1" t="s">
+      <c r="W44" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="W44" t="s">
+      <c r="X44" t="s">
         <v>311</v>
       </c>
-      <c r="X44" t="s">
+      <c r="Y44" t="s">
         <v>184</v>
       </c>
-      <c r="Y44" t="s">
-        <v>170</v>
-      </c>
       <c r="Z44" t="s">
         <v>170</v>
       </c>
@@ -7195,16 +7405,19 @@
         <v>170</v>
       </c>
       <c r="AG44" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH44" t="s">
         <v>181</v>
       </c>
-      <c r="AH44" t="s">
-        <v>170</v>
-      </c>
       <c r="AI44" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="45" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ44" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="45" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -7227,20 +7440,20 @@
         <v>55</v>
       </c>
       <c r="H45" t="s">
+        <v>693</v>
+      </c>
+      <c r="I45" t="s">
         <v>89</v>
       </c>
-      <c r="I45" t="s">
+      <c r="J45" t="s">
         <v>605</v>
       </c>
-      <c r="J45" t="s">
-        <v>170</v>
-      </c>
       <c r="K45" t="s">
+        <v>170</v>
+      </c>
+      <c r="L45" t="s">
         <v>174</v>
       </c>
-      <c r="L45" t="s">
-        <v>170</v>
-      </c>
       <c r="M45" t="s">
         <v>170</v>
       </c>
@@ -7262,7 +7475,7 @@
       <c r="S45" t="s">
         <v>170</v>
       </c>
-      <c r="T45" s="1" t="s">
+      <c r="T45" t="s">
         <v>170</v>
       </c>
       <c r="U45" s="1" t="s">
@@ -7277,7 +7490,7 @@
       <c r="X45" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="Y45" t="s">
+      <c r="Y45" s="1" t="s">
         <v>170</v>
       </c>
       <c r="Z45" t="s">
@@ -7301,17 +7514,20 @@
       <c r="AF45" t="s">
         <v>170</v>
       </c>
-      <c r="AG45" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH45" t="s">
+      <c r="AG45" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH45" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AI45" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="46" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ45" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="46" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>52</v>
       </c>
@@ -7334,26 +7550,26 @@
         <v>90</v>
       </c>
       <c r="H46" t="s">
+        <v>694</v>
+      </c>
+      <c r="I46" t="s">
         <v>91</v>
       </c>
-      <c r="I46" t="s">
+      <c r="J46" t="s">
         <v>605</v>
       </c>
-      <c r="J46" t="s">
-        <v>170</v>
-      </c>
       <c r="K46" t="s">
         <v>170</v>
       </c>
       <c r="L46" t="s">
+        <v>170</v>
+      </c>
+      <c r="M46" t="s">
         <v>235</v>
       </c>
-      <c r="M46" t="s">
+      <c r="N46" t="s">
         <v>454</v>
       </c>
-      <c r="N46" t="s">
-        <v>170</v>
-      </c>
       <c r="O46" t="s">
         <v>170</v>
       </c>
@@ -7369,7 +7585,7 @@
       <c r="S46" t="s">
         <v>170</v>
       </c>
-      <c r="T46" s="1" t="s">
+      <c r="T46" t="s">
         <v>170</v>
       </c>
       <c r="U46" s="1" t="s">
@@ -7384,7 +7600,7 @@
       <c r="X46" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="Y46" t="s">
+      <c r="Y46" s="1" t="s">
         <v>170</v>
       </c>
       <c r="Z46" t="s">
@@ -7408,17 +7624,20 @@
       <c r="AF46" t="s">
         <v>170</v>
       </c>
-      <c r="AG46" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH46" t="s">
+      <c r="AG46" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH46" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AI46" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="47" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ46" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="47" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
         <v>52</v>
       </c>
@@ -7441,26 +7660,26 @@
         <v>90</v>
       </c>
       <c r="H47" t="s">
+        <v>694</v>
+      </c>
+      <c r="I47" t="s">
         <v>91</v>
       </c>
-      <c r="I47" t="s">
+      <c r="J47" t="s">
         <v>605</v>
       </c>
-      <c r="J47" t="s">
-        <v>170</v>
-      </c>
       <c r="K47" t="s">
         <v>170</v>
       </c>
       <c r="L47" t="s">
+        <v>170</v>
+      </c>
+      <c r="M47" t="s">
         <v>235</v>
       </c>
-      <c r="M47" t="s">
+      <c r="N47" t="s">
         <v>455</v>
       </c>
-      <c r="N47" t="s">
-        <v>170</v>
-      </c>
       <c r="O47" t="s">
         <v>170</v>
       </c>
@@ -7476,7 +7695,7 @@
       <c r="S47" t="s">
         <v>170</v>
       </c>
-      <c r="T47" s="1" t="s">
+      <c r="T47" t="s">
         <v>170</v>
       </c>
       <c r="U47" s="1" t="s">
@@ -7491,7 +7710,7 @@
       <c r="X47" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="Y47" t="s">
+      <c r="Y47" s="1" t="s">
         <v>170</v>
       </c>
       <c r="Z47" t="s">
@@ -7515,17 +7734,20 @@
       <c r="AF47" t="s">
         <v>170</v>
       </c>
-      <c r="AG47" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH47" t="s">
+      <c r="AG47" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH47" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AI47" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="48" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ47" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="48" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -7548,23 +7770,23 @@
         <v>58</v>
       </c>
       <c r="H48" t="s">
+        <v>695</v>
+      </c>
+      <c r="I48" t="s">
         <v>93</v>
       </c>
-      <c r="I48" t="s">
+      <c r="J48" t="s">
         <v>605</v>
       </c>
-      <c r="J48" t="s">
-        <v>170</v>
-      </c>
       <c r="K48" t="s">
         <v>170</v>
       </c>
       <c r="L48" t="s">
+        <v>170</v>
+      </c>
+      <c r="M48" t="s">
         <v>235</v>
       </c>
-      <c r="M48" t="s">
-        <v>170</v>
-      </c>
       <c r="N48" t="s">
         <v>170</v>
       </c>
@@ -7583,7 +7805,7 @@
       <c r="S48" t="s">
         <v>170</v>
       </c>
-      <c r="T48" s="1" t="s">
+      <c r="T48" t="s">
         <v>170</v>
       </c>
       <c r="U48" s="1" t="s">
@@ -7598,7 +7820,7 @@
       <c r="X48" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="Y48" t="s">
+      <c r="Y48" s="1" t="s">
         <v>170</v>
       </c>
       <c r="Z48" t="s">
@@ -7622,17 +7844,20 @@
       <c r="AF48" t="s">
         <v>170</v>
       </c>
-      <c r="AG48" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH48" t="s">
+      <c r="AG48" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH48" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AI48" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="49" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ48" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="49" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>61</v>
       </c>
@@ -7655,20 +7880,20 @@
         <v>62</v>
       </c>
       <c r="H49" t="s">
+        <v>696</v>
+      </c>
+      <c r="I49" t="s">
         <v>95</v>
       </c>
-      <c r="I49" t="s">
+      <c r="J49" t="s">
         <v>605</v>
       </c>
-      <c r="J49" t="s">
+      <c r="K49" t="s">
         <v>167</v>
       </c>
-      <c r="K49" t="s">
+      <c r="L49" t="s">
         <v>174</v>
       </c>
-      <c r="L49" t="s">
-        <v>170</v>
-      </c>
       <c r="M49" t="s">
         <v>170</v>
       </c>
@@ -7690,7 +7915,7 @@
       <c r="S49" t="s">
         <v>170</v>
       </c>
-      <c r="T49" s="1" t="s">
+      <c r="T49" t="s">
         <v>170</v>
       </c>
       <c r="U49" s="1" t="s">
@@ -7705,7 +7930,7 @@
       <c r="X49" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="Y49" t="s">
+      <c r="Y49" s="1" t="s">
         <v>170</v>
       </c>
       <c r="Z49" t="s">
@@ -7729,17 +7954,20 @@
       <c r="AF49" t="s">
         <v>170</v>
       </c>
-      <c r="AG49" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH49" t="s">
+      <c r="AG49" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH49" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AI49" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="50" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ49" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="50" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>61</v>
       </c>
@@ -7762,20 +7990,20 @@
         <v>62</v>
       </c>
       <c r="H50" t="s">
+        <v>696</v>
+      </c>
+      <c r="I50" t="s">
         <v>95</v>
       </c>
-      <c r="I50" t="s">
+      <c r="J50" t="s">
         <v>605</v>
       </c>
-      <c r="J50" t="s">
+      <c r="K50" t="s">
         <v>167</v>
       </c>
-      <c r="K50" t="s">
+      <c r="L50" t="s">
         <v>174</v>
       </c>
-      <c r="L50" t="s">
-        <v>170</v>
-      </c>
       <c r="M50" t="s">
         <v>170</v>
       </c>
@@ -7798,23 +8026,23 @@
         <v>170</v>
       </c>
       <c r="T50" t="s">
+        <v>170</v>
+      </c>
+      <c r="U50" t="s">
         <v>221</v>
       </c>
-      <c r="U50" t="s">
+      <c r="V50" t="s">
         <v>222</v>
       </c>
-      <c r="V50" s="1" t="s">
+      <c r="W50" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="W50" s="9" t="s">
+      <c r="X50" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="X50" t="s">
+      <c r="Y50" t="s">
         <v>174</v>
       </c>
-      <c r="Y50" t="s">
-        <v>170</v>
-      </c>
       <c r="Z50" t="s">
         <v>170</v>
       </c>
@@ -7837,16 +8065,19 @@
         <v>170</v>
       </c>
       <c r="AG50" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH50" t="s">
         <v>181</v>
       </c>
-      <c r="AH50" t="s">
-        <v>170</v>
-      </c>
       <c r="AI50" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="51" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ50" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="51" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>64</v>
       </c>
@@ -7869,20 +8100,20 @@
         <v>65</v>
       </c>
       <c r="H51" t="s">
+        <v>697</v>
+      </c>
+      <c r="I51" t="s">
         <v>96</v>
       </c>
-      <c r="I51" t="s">
+      <c r="J51" t="s">
         <v>605</v>
       </c>
-      <c r="J51" t="s">
+      <c r="K51" t="s">
         <v>195</v>
       </c>
-      <c r="K51" t="s">
+      <c r="L51" t="s">
         <v>174</v>
       </c>
-      <c r="L51" t="s">
-        <v>170</v>
-      </c>
       <c r="M51" t="s">
         <v>170</v>
       </c>
@@ -7904,7 +8135,7 @@
       <c r="S51" t="s">
         <v>170</v>
       </c>
-      <c r="T51" s="1" t="s">
+      <c r="T51" t="s">
         <v>170</v>
       </c>
       <c r="U51" s="1" t="s">
@@ -7919,7 +8150,7 @@
       <c r="X51" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="Y51" t="s">
+      <c r="Y51" s="1" t="s">
         <v>170</v>
       </c>
       <c r="Z51" t="s">
@@ -7943,17 +8174,20 @@
       <c r="AF51" t="s">
         <v>170</v>
       </c>
-      <c r="AG51" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH51" t="s">
+      <c r="AG51" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH51" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AI51" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="52" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ51" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="52" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>66</v>
       </c>
@@ -7976,14 +8210,14 @@
         <v>97</v>
       </c>
       <c r="H52" t="s">
+        <v>698</v>
+      </c>
+      <c r="I52" t="s">
         <v>98</v>
       </c>
-      <c r="I52" t="s">
+      <c r="J52" t="s">
         <v>605</v>
       </c>
-      <c r="J52" t="s">
-        <v>170</v>
-      </c>
       <c r="K52" t="s">
         <v>170</v>
       </c>
@@ -8059,8 +8293,11 @@
       <c r="AI52" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AJ52" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="53" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>66</v>
       </c>
@@ -8083,14 +8320,14 @@
         <v>99</v>
       </c>
       <c r="H53" t="s">
+        <v>699</v>
+      </c>
+      <c r="I53" t="s">
         <v>100</v>
       </c>
-      <c r="I53" t="s">
+      <c r="J53" t="s">
         <v>605</v>
       </c>
-      <c r="J53" t="s">
-        <v>170</v>
-      </c>
       <c r="K53" t="s">
         <v>170</v>
       </c>
@@ -8166,8 +8403,11 @@
       <c r="AI53" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="54" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ53" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="54" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>66</v>
       </c>
@@ -8189,15 +8429,15 @@
       <c r="G54" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="H54" s="1" t="s">
+      <c r="H54" t="s">
+        <v>700</v>
+      </c>
+      <c r="I54" s="1" t="s">
         <v>614</v>
       </c>
-      <c r="I54" t="s">
+      <c r="J54" t="s">
         <v>605</v>
       </c>
-      <c r="J54" t="s">
-        <v>170</v>
-      </c>
       <c r="K54" t="s">
         <v>170</v>
       </c>
@@ -8225,18 +8465,18 @@
       <c r="S54" t="s">
         <v>170</v>
       </c>
-      <c r="T54" s="1" t="s">
+      <c r="T54" t="s">
+        <v>170</v>
+      </c>
+      <c r="U54" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="U54" s="1" t="s">
+      <c r="V54" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="V54" s="1" t="s">
+      <c r="W54" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="W54" t="s">
-        <v>170</v>
-      </c>
       <c r="X54" t="s">
         <v>170</v>
       </c>
@@ -8265,16 +8505,19 @@
         <v>170</v>
       </c>
       <c r="AG54" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH54" t="s">
         <v>181</v>
       </c>
-      <c r="AH54" t="s">
-        <v>170</v>
-      </c>
       <c r="AI54" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="55" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ54" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="55" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -8296,24 +8539,24 @@
       <c r="G55" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H55" s="15" t="s">
+      <c r="H55" t="s">
+        <v>701</v>
+      </c>
+      <c r="I55" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="I55" t="s">
+      <c r="J55" t="s">
         <v>605</v>
       </c>
-      <c r="J55" t="s">
-        <v>170</v>
-      </c>
       <c r="K55" t="s">
         <v>170</v>
       </c>
       <c r="L55" t="s">
+        <v>170</v>
+      </c>
+      <c r="M55" t="s">
         <v>235</v>
       </c>
-      <c r="M55" t="s">
-        <v>170</v>
-      </c>
       <c r="N55" t="s">
         <v>170</v>
       </c>
@@ -8380,8 +8623,11 @@
       <c r="AI55" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="56" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ55" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="56" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>52</v>
       </c>
@@ -8403,24 +8649,24 @@
       <c r="G56" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="H56" s="15" t="s">
+      <c r="H56" t="s">
+        <v>170</v>
+      </c>
+      <c r="I56" s="15" t="s">
         <v>549</v>
       </c>
-      <c r="I56" t="s">
+      <c r="J56" t="s">
         <v>605</v>
       </c>
-      <c r="J56" t="s">
-        <v>170</v>
-      </c>
       <c r="K56" t="s">
         <v>170</v>
       </c>
       <c r="L56" t="s">
+        <v>170</v>
+      </c>
+      <c r="M56" t="s">
         <v>464</v>
       </c>
-      <c r="M56" t="s">
-        <v>170</v>
-      </c>
       <c r="N56" t="s">
         <v>170</v>
       </c>
@@ -8443,23 +8689,23 @@
         <v>170</v>
       </c>
       <c r="U56" t="s">
+        <v>170</v>
+      </c>
+      <c r="V56" t="s">
         <v>550</v>
       </c>
-      <c r="V56" t="s">
+      <c r="W56" t="s">
         <v>605</v>
       </c>
-      <c r="W56" t="s">
-        <v>170</v>
-      </c>
       <c r="X56" t="s">
         <v>170</v>
       </c>
       <c r="Y56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z56" t="s">
         <v>464</v>
       </c>
-      <c r="Z56" t="s">
-        <v>170</v>
-      </c>
       <c r="AA56" t="s">
         <v>170</v>
       </c>
@@ -8479,16 +8725,19 @@
         <v>170</v>
       </c>
       <c r="AG56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH56" t="s">
         <v>548</v>
-      </c>
-      <c r="AH56">
-        <v>0</v>
       </c>
       <c r="AI56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:35" ht="18" x14ac:dyDescent="0.2">
+      <c r="AJ56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:36" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>545</v>
       </c>
@@ -8511,14 +8760,14 @@
         <v>170</v>
       </c>
       <c r="H57" t="s">
+        <v>170</v>
+      </c>
+      <c r="I57" t="s">
         <v>546</v>
       </c>
-      <c r="I57" t="s">
+      <c r="J57" t="s">
         <v>547</v>
       </c>
-      <c r="J57" t="s">
-        <v>170</v>
-      </c>
       <c r="K57" t="s">
         <v>170</v>
       </c>
@@ -8594,9 +8843,12 @@
       <c r="AI57" t="s">
         <v>170</v>
       </c>
+      <c r="AJ57" t="s">
+        <v>170</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AI57" xr:uid="{6F439630-CB66-7E4E-9544-3F25521DB3EB}"/>
+  <autoFilter ref="A1:AJ57" xr:uid="{6F439630-CB66-7E4E-9544-3F25521DB3EB}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
data_required add B.dx_name column
again fror documentation and validation purposes
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E14C5D-4B43-D749-B049-E30785E73EB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652ED7D3-57A0-684B-AAC5-3E68DE2FD61F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data_required!$A$1:$AJ$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data_required!$A$1:$AK$57</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">dimension_Item_sets!$A$1:$AF$142</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3476" uniqueCount="702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3533" uniqueCount="708">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -2144,6 +2144,24 @@
   </si>
   <si>
     <t>PrEP_NEW (DSD+TA, KeyPopAbr) TARGET</t>
+  </si>
+  <si>
+    <t>B.dx_name</t>
+  </si>
+  <si>
+    <t>TB_STAT (D, DSD+TA, , Age Aggregated/Sex)</t>
+  </si>
+  <si>
+    <t>HTS_SELF (N, DSD+TA, Age/Sex/HIVSelfTest)</t>
+  </si>
+  <si>
+    <t>OVC_SERV (DSD+TA, Age/Sex/ProgramStatus)</t>
+  </si>
+  <si>
+    <t>PP_PREV (DSD+TA, Age/Sex)</t>
+  </si>
+  <si>
+    <t>GEND_GBV (DSD+TA, Age/Sex/ViolenceType)</t>
   </si>
 </sst>
 </file>
@@ -2552,13 +2570,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
-  <dimension ref="A1:AJ57"/>
+  <dimension ref="A1:AK57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="R31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomRight" activeCell="V37" sqref="V37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2573,11 +2591,12 @@
     <col min="9" max="9" width="22.83203125" customWidth="1"/>
     <col min="10" max="20" width="17.33203125" customWidth="1"/>
     <col min="21" max="21" width="46.83203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="46.83203125" customWidth="1"/>
+    <col min="23" max="23" width="16" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>197</v>
       </c>
@@ -2642,52 +2661,55 @@
         <v>202</v>
       </c>
       <c r="V1" t="s">
+        <v>702</v>
+      </c>
+      <c r="W1" t="s">
         <v>306</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>199</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>200</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>201</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>515</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>529</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>522</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>523</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>524</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>525</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>526</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>527</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>180</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>551</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2796,8 +2818,11 @@
       <c r="AJ2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2906,8 +2931,11 @@
       <c r="AJ3" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="4" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -3016,8 +3044,11 @@
       <c r="AJ4" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3126,8 +3157,11 @@
       <c r="AJ5" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -3236,8 +3270,11 @@
       <c r="AJ6" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -3346,8 +3383,11 @@
       <c r="AJ7" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -3412,20 +3452,20 @@
         <v>84</v>
       </c>
       <c r="V8" t="s">
+        <v>703</v>
+      </c>
+      <c r="W8" t="s">
         <v>85</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>166</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>183</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="Z8" t="s">
         <v>174</v>
       </c>
-      <c r="Z8" t="s">
-        <v>170</v>
-      </c>
       <c r="AA8" t="s">
         <v>170</v>
       </c>
@@ -3448,16 +3488,19 @@
         <v>170</v>
       </c>
       <c r="AH8" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI8" t="s">
         <v>181</v>
       </c>
-      <c r="AI8" t="s">
-        <v>170</v>
-      </c>
       <c r="AJ8" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -3566,8 +3609,11 @@
       <c r="AJ9" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="10" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -3676,8 +3722,11 @@
       <c r="AJ10" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -3786,8 +3835,11 @@
       <c r="AJ11" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="12" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -3896,8 +3948,11 @@
       <c r="AJ12" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK12" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -4006,8 +4061,11 @@
       <c r="AJ13" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -4116,8 +4174,11 @@
       <c r="AJ14" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="15" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -4226,8 +4287,11 @@
       <c r="AJ15" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="16" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK15" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -4336,8 +4400,11 @@
       <c r="AJ16" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="17" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -4401,27 +4468,27 @@
       <c r="U17" t="s">
         <v>170</v>
       </c>
-      <c r="V17" s="1" t="s">
+      <c r="V17" t="s">
+        <v>686</v>
+      </c>
+      <c r="W17" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="W17" t="s">
+      <c r="X17" t="s">
         <v>166</v>
       </c>
-      <c r="X17" t="s">
+      <c r="Y17" t="s">
         <v>185</v>
       </c>
-      <c r="Y17" t="s">
+      <c r="Z17" t="s">
         <v>184</v>
       </c>
-      <c r="Z17" t="s">
-        <v>170</v>
-      </c>
       <c r="AA17" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB17" t="s">
         <v>534</v>
       </c>
-      <c r="AB17" t="s">
-        <v>170</v>
-      </c>
       <c r="AC17" t="s">
         <v>170</v>
       </c>
@@ -4438,16 +4505,19 @@
         <v>170</v>
       </c>
       <c r="AH17" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI17" t="s">
         <v>331</v>
-      </c>
-      <c r="AI17">
-        <v>0</v>
       </c>
       <c r="AJ17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -4511,21 +4581,21 @@
       <c r="U18" t="s">
         <v>170</v>
       </c>
-      <c r="V18" s="1" t="s">
+      <c r="V18" t="s">
+        <v>686</v>
+      </c>
+      <c r="W18" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="W18" t="s">
+      <c r="X18" t="s">
         <v>166</v>
       </c>
-      <c r="X18" s="9" t="s">
+      <c r="Y18" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="Y18" t="s">
+      <c r="Z18" t="s">
         <v>184</v>
       </c>
-      <c r="Z18" t="s">
-        <v>170</v>
-      </c>
       <c r="AA18" t="s">
         <v>170</v>
       </c>
@@ -4548,16 +4618,19 @@
         <v>170</v>
       </c>
       <c r="AH18" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI18" t="s">
         <v>192</v>
       </c>
-      <c r="AI18" t="s">
-        <v>170</v>
-      </c>
       <c r="AJ18" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="19" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -4621,21 +4694,21 @@
       <c r="U19" t="s">
         <v>170</v>
       </c>
-      <c r="V19" s="1" t="s">
+      <c r="V19" t="s">
+        <v>686</v>
+      </c>
+      <c r="W19" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="W19" t="s">
+      <c r="X19" t="s">
         <v>166</v>
       </c>
-      <c r="X19" s="9" t="s">
+      <c r="Y19" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="Y19" t="s">
+      <c r="Z19" t="s">
         <v>184</v>
       </c>
-      <c r="Z19" t="s">
-        <v>170</v>
-      </c>
       <c r="AA19" t="s">
         <v>170</v>
       </c>
@@ -4658,16 +4731,19 @@
         <v>170</v>
       </c>
       <c r="AH19" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI19" t="s">
         <v>192</v>
       </c>
-      <c r="AI19" t="s">
-        <v>170</v>
-      </c>
       <c r="AJ19" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="20" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK19" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -4731,21 +4807,21 @@
       <c r="U20" t="s">
         <v>170</v>
       </c>
-      <c r="V20" s="1" t="s">
+      <c r="V20" t="s">
+        <v>686</v>
+      </c>
+      <c r="W20" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="W20" t="s">
+      <c r="X20" t="s">
         <v>166</v>
       </c>
-      <c r="X20" s="9" t="s">
+      <c r="Y20" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="Y20" t="s">
+      <c r="Z20" t="s">
         <v>184</v>
       </c>
-      <c r="Z20" t="s">
-        <v>170</v>
-      </c>
       <c r="AA20" t="s">
         <v>170</v>
       </c>
@@ -4768,16 +4844,19 @@
         <v>170</v>
       </c>
       <c r="AH20" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI20" t="s">
         <v>192</v>
       </c>
-      <c r="AI20" t="s">
-        <v>170</v>
-      </c>
       <c r="AJ20" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="21" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK20" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -4841,21 +4920,21 @@
       <c r="U21" t="s">
         <v>170</v>
       </c>
-      <c r="V21" s="1" t="s">
+      <c r="V21" t="s">
+        <v>686</v>
+      </c>
+      <c r="W21" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="W21" t="s">
+      <c r="X21" t="s">
         <v>166</v>
       </c>
-      <c r="X21" s="9" t="s">
+      <c r="Y21" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="Y21" t="s">
+      <c r="Z21" t="s">
         <v>184</v>
       </c>
-      <c r="Z21" t="s">
-        <v>170</v>
-      </c>
       <c r="AA21" t="s">
         <v>170</v>
       </c>
@@ -4878,16 +4957,19 @@
         <v>170</v>
       </c>
       <c r="AH21" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI21" t="s">
         <v>192</v>
       </c>
-      <c r="AI21" t="s">
-        <v>170</v>
-      </c>
       <c r="AJ21" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="22" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK21" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -4951,21 +5033,21 @@
       <c r="U22" t="s">
         <v>170</v>
       </c>
-      <c r="V22" s="1" t="s">
+      <c r="V22" t="s">
+        <v>686</v>
+      </c>
+      <c r="W22" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="W22" t="s">
+      <c r="X22" t="s">
         <v>166</v>
       </c>
-      <c r="X22" s="9" t="s">
+      <c r="Y22" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="Y22" t="s">
+      <c r="Z22" t="s">
         <v>184</v>
       </c>
-      <c r="Z22" t="s">
-        <v>170</v>
-      </c>
       <c r="AA22" t="s">
         <v>170</v>
       </c>
@@ -4988,16 +5070,19 @@
         <v>170</v>
       </c>
       <c r="AH22" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI22" t="s">
         <v>192</v>
       </c>
-      <c r="AI22" t="s">
-        <v>170</v>
-      </c>
       <c r="AJ22" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="23" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK22" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -5061,21 +5146,21 @@
       <c r="U23" t="s">
         <v>170</v>
       </c>
-      <c r="V23" s="1" t="s">
+      <c r="V23" t="s">
+        <v>686</v>
+      </c>
+      <c r="W23" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="W23" t="s">
+      <c r="X23" t="s">
         <v>166</v>
       </c>
-      <c r="X23" s="3" t="s">
+      <c r="Y23" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="Y23" t="s">
+      <c r="Z23" t="s">
         <v>184</v>
       </c>
-      <c r="Z23" t="s">
-        <v>170</v>
-      </c>
       <c r="AA23" t="s">
         <v>170</v>
       </c>
@@ -5098,16 +5183,19 @@
         <v>170</v>
       </c>
       <c r="AH23" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI23" t="s">
         <v>192</v>
       </c>
-      <c r="AI23" t="s">
-        <v>170</v>
-      </c>
       <c r="AJ23" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="24" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK23" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -5171,21 +5259,21 @@
       <c r="U24" t="s">
         <v>170</v>
       </c>
-      <c r="V24" s="1" t="s">
+      <c r="V24" t="s">
+        <v>686</v>
+      </c>
+      <c r="W24" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="W24" t="s">
+      <c r="X24" t="s">
         <v>166</v>
       </c>
-      <c r="X24" s="3" t="s">
+      <c r="Y24" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="Y24" t="s">
+      <c r="Z24" t="s">
         <v>184</v>
       </c>
-      <c r="Z24" t="s">
-        <v>170</v>
-      </c>
       <c r="AA24" t="s">
         <v>170</v>
       </c>
@@ -5208,16 +5296,19 @@
         <v>170</v>
       </c>
       <c r="AH24" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI24" t="s">
         <v>192</v>
       </c>
-      <c r="AI24" t="s">
-        <v>170</v>
-      </c>
       <c r="AJ24" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="25" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK24" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -5281,21 +5372,21 @@
       <c r="U25" t="s">
         <v>170</v>
       </c>
-      <c r="V25" s="1" t="s">
+      <c r="V25" t="s">
+        <v>686</v>
+      </c>
+      <c r="W25" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="W25" t="s">
+      <c r="X25" t="s">
         <v>166</v>
       </c>
-      <c r="X25" s="9" t="s">
+      <c r="Y25" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="Y25" t="s">
+      <c r="Z25" t="s">
         <v>184</v>
       </c>
-      <c r="Z25" t="s">
-        <v>170</v>
-      </c>
       <c r="AA25" t="s">
         <v>170</v>
       </c>
@@ -5318,16 +5409,19 @@
         <v>170</v>
       </c>
       <c r="AH25" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI25" t="s">
         <v>192</v>
       </c>
-      <c r="AI25" t="s">
-        <v>170</v>
-      </c>
       <c r="AJ25" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="26" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK25" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="26" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -5391,21 +5485,21 @@
       <c r="U26" t="s">
         <v>170</v>
       </c>
-      <c r="V26" s="1" t="s">
+      <c r="V26" t="s">
+        <v>686</v>
+      </c>
+      <c r="W26" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="W26" t="s">
+      <c r="X26" t="s">
         <v>166</v>
       </c>
-      <c r="X26" s="9" t="s">
+      <c r="Y26" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="Y26" t="s">
+      <c r="Z26" t="s">
         <v>184</v>
       </c>
-      <c r="Z26" t="s">
-        <v>170</v>
-      </c>
       <c r="AA26" t="s">
         <v>170</v>
       </c>
@@ -5428,16 +5522,19 @@
         <v>170</v>
       </c>
       <c r="AH26" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI26" t="s">
         <v>192</v>
       </c>
-      <c r="AI26" t="s">
-        <v>170</v>
-      </c>
       <c r="AJ26" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="27" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -5501,21 +5598,21 @@
       <c r="U27" t="s">
         <v>170</v>
       </c>
-      <c r="V27" s="1" t="s">
+      <c r="V27" t="s">
+        <v>686</v>
+      </c>
+      <c r="W27" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="W27" t="s">
+      <c r="X27" t="s">
         <v>166</v>
       </c>
-      <c r="X27" s="9" t="s">
+      <c r="Y27" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="Y27" t="s">
+      <c r="Z27" t="s">
         <v>184</v>
       </c>
-      <c r="Z27" t="s">
-        <v>170</v>
-      </c>
       <c r="AA27" t="s">
         <v>170</v>
       </c>
@@ -5538,16 +5635,19 @@
         <v>170</v>
       </c>
       <c r="AH27" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI27" t="s">
         <v>192</v>
       </c>
-      <c r="AI27" t="s">
-        <v>170</v>
-      </c>
       <c r="AJ27" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="28" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK27" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -5656,8 +5756,11 @@
       <c r="AJ28" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="29" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK28" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -5766,8 +5869,11 @@
       <c r="AJ29" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="30" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK29" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="30" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -5876,8 +5982,11 @@
       <c r="AJ30" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="31" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK30" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="31" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -5986,8 +6095,11 @@
       <c r="AJ31" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="32" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK31" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -6096,8 +6208,11 @@
       <c r="AJ32" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="33" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK32" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="33" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -6206,8 +6321,11 @@
       <c r="AJ33" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="34" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK33" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="34" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -6316,8 +6434,11 @@
       <c r="AJ34" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="35" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK34" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="35" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -6426,8 +6547,11 @@
       <c r="AJ35" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="36" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK35" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="36" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -6536,8 +6660,11 @@
       <c r="AJ36" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="37" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK36" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="37" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -6646,8 +6773,11 @@
       <c r="AJ37" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="38" spans="1:36" ht="19" x14ac:dyDescent="0.25">
+      <c r="AK37" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="38" spans="1:37" ht="19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -6711,7 +6841,7 @@
       <c r="U38" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="V38" s="1" t="s">
+      <c r="V38" t="s">
         <v>170</v>
       </c>
       <c r="W38" s="1" t="s">
@@ -6723,7 +6853,7 @@
       <c r="Y38" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="Z38" t="s">
+      <c r="Z38" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AA38" t="s">
@@ -6747,17 +6877,20 @@
       <c r="AG38" t="s">
         <v>170</v>
       </c>
-      <c r="AH38" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AI38" t="s">
+      <c r="AH38" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI38" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AJ38" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="39" spans="1:36" ht="19" x14ac:dyDescent="0.25">
+      <c r="AK38" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="1:37" ht="19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>22</v>
       </c>
@@ -6821,7 +6954,7 @@
       <c r="U39" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="V39" s="1" t="s">
+      <c r="V39" t="s">
         <v>170</v>
       </c>
       <c r="W39" s="1" t="s">
@@ -6833,7 +6966,7 @@
       <c r="Y39" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="Z39" t="s">
+      <c r="Z39" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AA39" t="s">
@@ -6857,17 +6990,20 @@
       <c r="AG39" t="s">
         <v>170</v>
       </c>
-      <c r="AH39" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AI39" t="s">
+      <c r="AH39" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI39" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AJ39" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="40" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK39" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="40" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -6932,20 +7068,20 @@
         <v>220</v>
       </c>
       <c r="V40" t="s">
+        <v>704</v>
+      </c>
+      <c r="W40" t="s">
         <v>219</v>
       </c>
-      <c r="W40" s="1" t="s">
+      <c r="X40" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="X40" s="9" t="s">
+      <c r="Y40" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="Y40" t="s">
+      <c r="Z40" t="s">
         <v>174</v>
       </c>
-      <c r="Z40" t="s">
-        <v>170</v>
-      </c>
       <c r="AA40" t="s">
         <v>170</v>
       </c>
@@ -6968,16 +7104,19 @@
         <v>170</v>
       </c>
       <c r="AH40" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI40" t="s">
         <v>181</v>
       </c>
-      <c r="AI40" t="s">
-        <v>170</v>
-      </c>
       <c r="AJ40" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="41" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK40" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="41" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -7041,7 +7180,7 @@
       <c r="U41" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="V41" s="1" t="s">
+      <c r="V41" t="s">
         <v>170</v>
       </c>
       <c r="W41" s="1" t="s">
@@ -7053,7 +7192,7 @@
       <c r="Y41" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="Z41" t="s">
+      <c r="Z41" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AA41" t="s">
@@ -7077,17 +7216,20 @@
       <c r="AG41" t="s">
         <v>170</v>
       </c>
-      <c r="AH41" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AI41" t="s">
+      <c r="AH41" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI41" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AJ41" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="42" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK41" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -7151,7 +7293,7 @@
       <c r="U42" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="V42" s="1" t="s">
+      <c r="V42" t="s">
         <v>170</v>
       </c>
       <c r="W42" s="1" t="s">
@@ -7163,7 +7305,7 @@
       <c r="Y42" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="Z42" t="s">
+      <c r="Z42" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AA42" t="s">
@@ -7187,17 +7329,20 @@
       <c r="AG42" t="s">
         <v>170</v>
       </c>
-      <c r="AH42" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AI42" t="s">
+      <c r="AH42" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI42" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AJ42" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="43" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK42" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="43" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -7261,7 +7406,7 @@
       <c r="U43" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="V43" s="1" t="s">
+      <c r="V43" t="s">
         <v>170</v>
       </c>
       <c r="W43" s="1" t="s">
@@ -7273,7 +7418,7 @@
       <c r="Y43" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="Z43" t="s">
+      <c r="Z43" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AA43" t="s">
@@ -7297,17 +7442,20 @@
       <c r="AG43" t="s">
         <v>170</v>
       </c>
-      <c r="AH43" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AI43" t="s">
+      <c r="AH43" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI43" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AJ43" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="44" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK43" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="44" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -7372,20 +7520,20 @@
         <v>610</v>
       </c>
       <c r="V44" t="s">
+        <v>705</v>
+      </c>
+      <c r="W44" t="s">
         <v>611</v>
       </c>
-      <c r="W44" s="1" t="s">
+      <c r="X44" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="X44" t="s">
+      <c r="Y44" t="s">
         <v>311</v>
       </c>
-      <c r="Y44" t="s">
+      <c r="Z44" t="s">
         <v>184</v>
       </c>
-      <c r="Z44" t="s">
-        <v>170</v>
-      </c>
       <c r="AA44" t="s">
         <v>170</v>
       </c>
@@ -7408,16 +7556,19 @@
         <v>170</v>
       </c>
       <c r="AH44" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI44" t="s">
         <v>181</v>
       </c>
-      <c r="AI44" t="s">
-        <v>170</v>
-      </c>
       <c r="AJ44" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="45" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK44" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="45" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -7481,7 +7632,7 @@
       <c r="U45" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="V45" s="1" t="s">
+      <c r="V45" t="s">
         <v>170</v>
       </c>
       <c r="W45" s="1" t="s">
@@ -7493,7 +7644,7 @@
       <c r="Y45" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="Z45" t="s">
+      <c r="Z45" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AA45" t="s">
@@ -7517,17 +7668,20 @@
       <c r="AG45" t="s">
         <v>170</v>
       </c>
-      <c r="AH45" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AI45" t="s">
+      <c r="AH45" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI45" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AJ45" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="46" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK45" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="46" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>52</v>
       </c>
@@ -7591,7 +7745,7 @@
       <c r="U46" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="V46" s="1" t="s">
+      <c r="V46" t="s">
         <v>170</v>
       </c>
       <c r="W46" s="1" t="s">
@@ -7603,7 +7757,7 @@
       <c r="Y46" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="Z46" t="s">
+      <c r="Z46" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AA46" t="s">
@@ -7627,17 +7781,20 @@
       <c r="AG46" t="s">
         <v>170</v>
       </c>
-      <c r="AH46" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AI46" t="s">
+      <c r="AH46" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI46" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AJ46" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="47" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK46" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="47" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
         <v>52</v>
       </c>
@@ -7701,7 +7858,7 @@
       <c r="U47" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="V47" s="1" t="s">
+      <c r="V47" t="s">
         <v>170</v>
       </c>
       <c r="W47" s="1" t="s">
@@ -7713,7 +7870,7 @@
       <c r="Y47" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="Z47" t="s">
+      <c r="Z47" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AA47" t="s">
@@ -7737,17 +7894,20 @@
       <c r="AG47" t="s">
         <v>170</v>
       </c>
-      <c r="AH47" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AI47" t="s">
+      <c r="AH47" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI47" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AJ47" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="48" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK47" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="48" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -7811,7 +7971,7 @@
       <c r="U48" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="V48" s="1" t="s">
+      <c r="V48" t="s">
         <v>170</v>
       </c>
       <c r="W48" s="1" t="s">
@@ -7823,7 +7983,7 @@
       <c r="Y48" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="Z48" t="s">
+      <c r="Z48" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AA48" t="s">
@@ -7847,17 +8007,20 @@
       <c r="AG48" t="s">
         <v>170</v>
       </c>
-      <c r="AH48" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AI48" t="s">
+      <c r="AH48" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI48" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AJ48" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="49" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK48" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="49" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>61</v>
       </c>
@@ -7921,7 +8084,7 @@
       <c r="U49" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="V49" s="1" t="s">
+      <c r="V49" t="s">
         <v>170</v>
       </c>
       <c r="W49" s="1" t="s">
@@ -7933,7 +8096,7 @@
       <c r="Y49" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="Z49" t="s">
+      <c r="Z49" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AA49" t="s">
@@ -7957,17 +8120,20 @@
       <c r="AG49" t="s">
         <v>170</v>
       </c>
-      <c r="AH49" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AI49" t="s">
+      <c r="AH49" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI49" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AJ49" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="50" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK49" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="50" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>61</v>
       </c>
@@ -8032,20 +8198,20 @@
         <v>221</v>
       </c>
       <c r="V50" t="s">
+        <v>706</v>
+      </c>
+      <c r="W50" t="s">
         <v>222</v>
       </c>
-      <c r="W50" s="1" t="s">
+      <c r="X50" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="X50" s="9" t="s">
+      <c r="Y50" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="Y50" t="s">
+      <c r="Z50" t="s">
         <v>174</v>
       </c>
-      <c r="Z50" t="s">
-        <v>170</v>
-      </c>
       <c r="AA50" t="s">
         <v>170</v>
       </c>
@@ -8068,16 +8234,19 @@
         <v>170</v>
       </c>
       <c r="AH50" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI50" t="s">
         <v>181</v>
       </c>
-      <c r="AI50" t="s">
-        <v>170</v>
-      </c>
       <c r="AJ50" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="51" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK50" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="51" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>64</v>
       </c>
@@ -8141,7 +8310,7 @@
       <c r="U51" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="V51" s="1" t="s">
+      <c r="V51" t="s">
         <v>170</v>
       </c>
       <c r="W51" s="1" t="s">
@@ -8153,7 +8322,7 @@
       <c r="Y51" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="Z51" t="s">
+      <c r="Z51" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AA51" t="s">
@@ -8177,17 +8346,20 @@
       <c r="AG51" t="s">
         <v>170</v>
       </c>
-      <c r="AH51" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AI51" t="s">
+      <c r="AH51" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI51" s="1" t="s">
         <v>170</v>
       </c>
       <c r="AJ51" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="52" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK51" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="52" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>66</v>
       </c>
@@ -8296,8 +8468,11 @@
       <c r="AJ52" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK52" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="53" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>66</v>
       </c>
@@ -8406,8 +8581,11 @@
       <c r="AJ53" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="54" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK53" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="54" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>66</v>
       </c>
@@ -8471,15 +8649,15 @@
       <c r="U54" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="V54" s="1" t="s">
+      <c r="V54" t="s">
+        <v>707</v>
+      </c>
+      <c r="W54" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="W54" s="1" t="s">
+      <c r="X54" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="X54" t="s">
-        <v>170</v>
-      </c>
       <c r="Y54" t="s">
         <v>170</v>
       </c>
@@ -8508,16 +8686,19 @@
         <v>170</v>
       </c>
       <c r="AH54" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI54" t="s">
         <v>181</v>
       </c>
-      <c r="AI54" t="s">
-        <v>170</v>
-      </c>
       <c r="AJ54" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="55" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK54" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="55" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -8626,8 +8807,11 @@
       <c r="AJ55" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="56" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK55" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="56" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>52</v>
       </c>
@@ -8692,23 +8876,23 @@
         <v>170</v>
       </c>
       <c r="V56" t="s">
+        <v>170</v>
+      </c>
+      <c r="W56" t="s">
         <v>550</v>
       </c>
-      <c r="W56" t="s">
+      <c r="X56" t="s">
         <v>605</v>
       </c>
-      <c r="X56" t="s">
-        <v>170</v>
-      </c>
       <c r="Y56" t="s">
         <v>170</v>
       </c>
       <c r="Z56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA56" t="s">
         <v>464</v>
       </c>
-      <c r="AA56" t="s">
-        <v>170</v>
-      </c>
       <c r="AB56" t="s">
         <v>170</v>
       </c>
@@ -8728,16 +8912,19 @@
         <v>170</v>
       </c>
       <c r="AH56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI56" t="s">
         <v>548</v>
-      </c>
-      <c r="AI56">
-        <v>0</v>
       </c>
       <c r="AJ56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:36" ht="18" x14ac:dyDescent="0.2">
+      <c r="AK56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:37" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>545</v>
       </c>
@@ -8846,9 +9033,12 @@
       <c r="AJ57" t="s">
         <v>170</v>
       </c>
+      <c r="AK57" t="s">
+        <v>170</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AJ57" xr:uid="{6F439630-CB66-7E4E-9544-3F25521DB3EB}"/>
+  <autoFilter ref="A1:AK57" xr:uid="{6F439630-CB66-7E4E-9544-3F25521DB3EB}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
data required update year for impatt prioritization
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652ED7D3-57A0-684B-AAC5-3E68DE2FD61F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D507C452-13C4-7146-BBDA-EEE372B8732C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
@@ -1681,9 +1681,6 @@
     <t>r4zbW3owX9n</t>
   </si>
   <si>
-    <t>2018Q4</t>
-  </si>
-  <si>
     <t>A+B</t>
   </si>
   <si>
@@ -2162,6 +2159,9 @@
   </si>
   <si>
     <t>GEND_GBV (DSD+TA, Age/Sex/ViolenceType)</t>
+  </si>
+  <si>
+    <t>2019Q4</t>
   </si>
 </sst>
 </file>
@@ -2573,10 +2573,10 @@
   <dimension ref="A1:AK57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="R31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V37" sqref="V37"/>
+      <selection pane="bottomRight" activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2619,7 +2619,7 @@
         <v>514</v>
       </c>
       <c r="H1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="I1" t="s">
         <v>305</v>
@@ -2661,7 +2661,7 @@
         <v>202</v>
       </c>
       <c r="V1" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="W1" t="s">
         <v>306</v>
@@ -2703,10 +2703,10 @@
         <v>180</v>
       </c>
       <c r="AJ1" t="s">
+        <v>550</v>
+      </c>
+      <c r="AK1" t="s">
         <v>551</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
@@ -2720,7 +2720,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -2732,13 +2732,13 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I2" t="s">
         <v>79</v>
       </c>
       <c r="J2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="K2" t="s">
         <v>167</v>
@@ -2833,7 +2833,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
@@ -2845,7 +2845,7 @@
         <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="I3" t="s">
         <v>80</v>
@@ -2946,7 +2946,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
@@ -2958,10 +2958,10 @@
         <v>170</v>
       </c>
       <c r="H4" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="J4" t="s">
         <v>166</v>
@@ -2976,7 +2976,7 @@
         <v>170</v>
       </c>
       <c r="N4" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="O4" t="s">
         <v>170</v>
@@ -3059,7 +3059,7 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
@@ -3071,7 +3071,7 @@
         <v>9</v>
       </c>
       <c r="H5" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="I5" t="s">
         <v>81</v>
@@ -3172,7 +3172,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -3184,7 +3184,7 @@
         <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="I6" t="s">
         <v>82</v>
@@ -3285,7 +3285,7 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E7" t="s">
         <v>3</v>
@@ -3297,13 +3297,13 @@
         <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I7" t="s">
         <v>83</v>
       </c>
       <c r="J7" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="K7" t="s">
         <v>183</v>
@@ -3398,7 +3398,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
@@ -3410,13 +3410,13 @@
         <v>12</v>
       </c>
       <c r="H8" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I8" t="s">
         <v>83</v>
       </c>
       <c r="J8" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="K8" t="s">
         <v>183</v>
@@ -3452,7 +3452,7 @@
         <v>84</v>
       </c>
       <c r="V8" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="W8" t="s">
         <v>85</v>
@@ -3511,7 +3511,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
@@ -3523,7 +3523,7 @@
         <v>14</v>
       </c>
       <c r="H9" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="I9" t="s">
         <v>86</v>
@@ -3624,7 +3624,7 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
@@ -3636,10 +3636,10 @@
         <v>170</v>
       </c>
       <c r="H10" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="J10" t="s">
         <v>166</v>
@@ -3654,7 +3654,7 @@
         <v>170</v>
       </c>
       <c r="N10" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="O10" t="s">
         <v>170</v>
@@ -3737,7 +3737,7 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="E11" t="s">
         <v>3</v>
@@ -3746,16 +3746,16 @@
         <v>169</v>
       </c>
       <c r="G11" t="s">
+        <v>672</v>
+      </c>
+      <c r="H11" t="s">
+        <v>682</v>
+      </c>
+      <c r="I11" t="s">
         <v>673</v>
       </c>
-      <c r="H11" t="s">
-        <v>683</v>
-      </c>
-      <c r="I11" t="s">
-        <v>674</v>
-      </c>
       <c r="J11" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="K11" t="s">
         <v>167</v>
@@ -3850,7 +3850,7 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="E12" t="s">
         <v>6</v>
@@ -3862,10 +3862,10 @@
         <v>170</v>
       </c>
       <c r="H12" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="J12" t="s">
         <v>166</v>
@@ -3880,7 +3880,7 @@
         <v>170</v>
       </c>
       <c r="N12" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="O12" t="s">
         <v>170</v>
@@ -3963,7 +3963,7 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
@@ -3972,13 +3972,13 @@
         <v>171</v>
       </c>
       <c r="G13" t="s">
+        <v>607</v>
+      </c>
+      <c r="H13" t="s">
+        <v>683</v>
+      </c>
+      <c r="I13" t="s">
         <v>608</v>
-      </c>
-      <c r="H13" t="s">
-        <v>684</v>
-      </c>
-      <c r="I13" t="s">
-        <v>609</v>
       </c>
       <c r="J13" t="s">
         <v>166</v>
@@ -4076,7 +4076,7 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="E14" t="s">
         <v>3</v>
@@ -4088,13 +4088,13 @@
         <v>21</v>
       </c>
       <c r="H14" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="I14" t="s">
         <v>87</v>
       </c>
       <c r="J14" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="K14" t="s">
         <v>183</v>
@@ -4189,7 +4189,7 @@
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
@@ -4201,10 +4201,10 @@
         <v>170</v>
       </c>
       <c r="H15" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="J15" t="s">
         <v>166</v>
@@ -4302,7 +4302,7 @@
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="E16" t="s">
         <v>6</v>
@@ -4314,10 +4314,10 @@
         <v>170</v>
       </c>
       <c r="H16" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="J16" t="s">
         <v>166</v>
@@ -4415,7 +4415,7 @@
         <v>5</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="E17" t="s">
         <v>6</v>
@@ -4427,10 +4427,10 @@
         <v>170</v>
       </c>
       <c r="H17" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="J17" t="s">
         <v>166</v>
@@ -4469,10 +4469,10 @@
         <v>170</v>
       </c>
       <c r="V17" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="X17" t="s">
         <v>166</v>
@@ -4528,7 +4528,7 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="E18" t="s">
         <v>6</v>
@@ -4540,10 +4540,10 @@
         <v>170</v>
       </c>
       <c r="H18" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="J18" t="s">
         <v>166</v>
@@ -4582,10 +4582,10 @@
         <v>170</v>
       </c>
       <c r="V18" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="X18" t="s">
         <v>166</v>
@@ -4641,7 +4641,7 @@
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E19" t="s">
         <v>6</v>
@@ -4653,10 +4653,10 @@
         <v>170</v>
       </c>
       <c r="H19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="J19" t="s">
         <v>166</v>
@@ -4695,10 +4695,10 @@
         <v>170</v>
       </c>
       <c r="V19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="X19" t="s">
         <v>166</v>
@@ -4754,7 +4754,7 @@
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E20" t="s">
         <v>6</v>
@@ -4766,10 +4766,10 @@
         <v>170</v>
       </c>
       <c r="H20" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="J20" t="s">
         <v>166</v>
@@ -4808,10 +4808,10 @@
         <v>170</v>
       </c>
       <c r="V20" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="X20" t="s">
         <v>166</v>
@@ -4867,7 +4867,7 @@
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E21" t="s">
         <v>6</v>
@@ -4879,10 +4879,10 @@
         <v>170</v>
       </c>
       <c r="H21" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="J21" t="s">
         <v>166</v>
@@ -4921,10 +4921,10 @@
         <v>170</v>
       </c>
       <c r="V21" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="W21" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="X21" t="s">
         <v>166</v>
@@ -4980,7 +4980,7 @@
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E22" t="s">
         <v>6</v>
@@ -4992,10 +4992,10 @@
         <v>170</v>
       </c>
       <c r="H22" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="J22" t="s">
         <v>166</v>
@@ -5034,10 +5034,10 @@
         <v>170</v>
       </c>
       <c r="V22" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="X22" t="s">
         <v>166</v>
@@ -5093,7 +5093,7 @@
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E23" t="s">
         <v>6</v>
@@ -5105,10 +5105,10 @@
         <v>170</v>
       </c>
       <c r="H23" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="J23" t="s">
         <v>166</v>
@@ -5147,10 +5147,10 @@
         <v>170</v>
       </c>
       <c r="V23" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="W23" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="X23" t="s">
         <v>166</v>
@@ -5206,7 +5206,7 @@
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E24" t="s">
         <v>6</v>
@@ -5218,10 +5218,10 @@
         <v>170</v>
       </c>
       <c r="H24" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="J24" t="s">
         <v>166</v>
@@ -5260,10 +5260,10 @@
         <v>170</v>
       </c>
       <c r="V24" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="W24" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="X24" t="s">
         <v>166</v>
@@ -5319,7 +5319,7 @@
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E25" t="s">
         <v>6</v>
@@ -5331,10 +5331,10 @@
         <v>170</v>
       </c>
       <c r="H25" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="J25" t="s">
         <v>166</v>
@@ -5373,10 +5373,10 @@
         <v>170</v>
       </c>
       <c r="V25" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="W25" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="X25" t="s">
         <v>166</v>
@@ -5432,7 +5432,7 @@
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E26" t="s">
         <v>6</v>
@@ -5444,10 +5444,10 @@
         <v>170</v>
       </c>
       <c r="H26" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="J26" t="s">
         <v>166</v>
@@ -5486,10 +5486,10 @@
         <v>170</v>
       </c>
       <c r="V26" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="W26" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="X26" t="s">
         <v>166</v>
@@ -5545,7 +5545,7 @@
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E27" t="s">
         <v>6</v>
@@ -5557,10 +5557,10 @@
         <v>170</v>
       </c>
       <c r="H27" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="J27" t="s">
         <v>166</v>
@@ -5599,10 +5599,10 @@
         <v>170</v>
       </c>
       <c r="V27" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="W27" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="X27" t="s">
         <v>166</v>
@@ -5658,7 +5658,7 @@
         <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E28" t="s">
         <v>6</v>
@@ -5670,10 +5670,10 @@
         <v>170</v>
       </c>
       <c r="H28" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="J28" t="s">
         <v>166</v>
@@ -5771,7 +5771,7 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E29" t="s">
         <v>6</v>
@@ -5783,10 +5783,10 @@
         <v>170</v>
       </c>
       <c r="H29" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="J29" t="s">
         <v>166</v>
@@ -5884,7 +5884,7 @@
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="E30" t="s">
         <v>6</v>
@@ -5896,10 +5896,10 @@
         <v>170</v>
       </c>
       <c r="H30" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="J30" t="s">
         <v>166</v>
@@ -5997,7 +5997,7 @@
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E31" t="s">
         <v>6</v>
@@ -6009,10 +6009,10 @@
         <v>170</v>
       </c>
       <c r="H31" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="J31" t="s">
         <v>166</v>
@@ -6110,7 +6110,7 @@
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E32" t="s">
         <v>6</v>
@@ -6122,10 +6122,10 @@
         <v>170</v>
       </c>
       <c r="H32" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="J32" t="s">
         <v>166</v>
@@ -6223,7 +6223,7 @@
         <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E33" t="s">
         <v>6</v>
@@ -6235,10 +6235,10 @@
         <v>170</v>
       </c>
       <c r="H33" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="J33" t="s">
         <v>166</v>
@@ -6336,7 +6336,7 @@
         <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E34" t="s">
         <v>6</v>
@@ -6348,10 +6348,10 @@
         <v>170</v>
       </c>
       <c r="H34" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="J34" t="s">
         <v>166</v>
@@ -6449,7 +6449,7 @@
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E35" t="s">
         <v>6</v>
@@ -6461,10 +6461,10 @@
         <v>170</v>
       </c>
       <c r="H35" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="J35" t="s">
         <v>166</v>
@@ -6562,7 +6562,7 @@
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E36" t="s">
         <v>6</v>
@@ -6574,10 +6574,10 @@
         <v>170</v>
       </c>
       <c r="H36" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="J36" t="s">
         <v>166</v>
@@ -6675,7 +6675,7 @@
         <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="E37" t="s">
         <v>6</v>
@@ -6687,10 +6687,10 @@
         <v>170</v>
       </c>
       <c r="H37" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="J37" t="s">
         <v>166</v>
@@ -6788,7 +6788,7 @@
         <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="E38" t="s">
         <v>3</v>
@@ -6800,13 +6800,13 @@
         <v>170</v>
       </c>
       <c r="H38" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="J38" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="K38" t="s">
         <v>167</v>
@@ -6901,7 +6901,7 @@
         <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="E39" t="s">
         <v>3</v>
@@ -6913,19 +6913,19 @@
         <v>170</v>
       </c>
       <c r="H39" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="I39" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="K39" t="s">
         <v>665</v>
       </c>
-      <c r="J39" s="1" t="s">
-        <v>605</v>
-      </c>
-      <c r="K39" t="s">
-        <v>666</v>
-      </c>
       <c r="L39" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="M39" t="s">
         <v>170</v>
@@ -7014,7 +7014,7 @@
         <v>5</v>
       </c>
       <c r="D40" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E40" t="s">
         <v>6</v>
@@ -7026,13 +7026,13 @@
         <v>218</v>
       </c>
       <c r="H40" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="I40" t="s">
         <v>217</v>
       </c>
       <c r="J40" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="K40" t="s">
         <v>167</v>
@@ -7068,7 +7068,7 @@
         <v>220</v>
       </c>
       <c r="V40" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="W40" t="s">
         <v>219</v>
@@ -7127,7 +7127,7 @@
         <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="E41" t="s">
         <v>6</v>
@@ -7136,13 +7136,13 @@
         <v>171</v>
       </c>
       <c r="G41" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="H41" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="J41" t="s">
         <v>166</v>
@@ -7240,7 +7240,7 @@
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E42" t="s">
         <v>6</v>
@@ -7249,13 +7249,13 @@
         <v>171</v>
       </c>
       <c r="G42" t="s">
+        <v>616</v>
+      </c>
+      <c r="H42" t="s">
+        <v>690</v>
+      </c>
+      <c r="I42" s="1" t="s">
         <v>617</v>
-      </c>
-      <c r="H42" t="s">
-        <v>691</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>618</v>
       </c>
       <c r="J42" t="s">
         <v>166</v>
@@ -7353,7 +7353,7 @@
         <v>2</v>
       </c>
       <c r="D43" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E43" t="s">
         <v>3</v>
@@ -7362,16 +7362,16 @@
         <v>169</v>
       </c>
       <c r="G43" t="s">
+        <v>611</v>
+      </c>
+      <c r="H43" t="s">
+        <v>691</v>
+      </c>
+      <c r="I43" t="s">
         <v>612</v>
       </c>
-      <c r="H43" t="s">
-        <v>692</v>
-      </c>
-      <c r="I43" t="s">
-        <v>613</v>
-      </c>
       <c r="J43" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="K43" t="s">
         <v>311</v>
@@ -7466,7 +7466,7 @@
         <v>5</v>
       </c>
       <c r="D44" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E44" t="s">
         <v>6</v>
@@ -7475,16 +7475,16 @@
         <v>169</v>
       </c>
       <c r="G44" t="s">
+        <v>611</v>
+      </c>
+      <c r="H44" t="s">
+        <v>691</v>
+      </c>
+      <c r="I44" t="s">
         <v>612</v>
       </c>
-      <c r="H44" t="s">
-        <v>692</v>
-      </c>
-      <c r="I44" t="s">
-        <v>613</v>
-      </c>
       <c r="J44" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="K44" t="s">
         <v>311</v>
@@ -7517,13 +7517,13 @@
         <v>170</v>
       </c>
       <c r="U44" t="s">
+        <v>609</v>
+      </c>
+      <c r="V44" t="s">
+        <v>704</v>
+      </c>
+      <c r="W44" t="s">
         <v>610</v>
-      </c>
-      <c r="V44" t="s">
-        <v>705</v>
-      </c>
-      <c r="W44" t="s">
-        <v>611</v>
       </c>
       <c r="X44" s="1" t="s">
         <v>166</v>
@@ -7579,7 +7579,7 @@
         <v>2</v>
       </c>
       <c r="D45" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E45" t="s">
         <v>3</v>
@@ -7591,13 +7591,13 @@
         <v>55</v>
       </c>
       <c r="H45" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="I45" t="s">
         <v>89</v>
       </c>
       <c r="J45" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="K45" t="s">
         <v>170</v>
@@ -7692,7 +7692,7 @@
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E46" t="s">
         <v>3</v>
@@ -7704,13 +7704,13 @@
         <v>90</v>
       </c>
       <c r="H46" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="I46" t="s">
         <v>91</v>
       </c>
       <c r="J46" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="K46" t="s">
         <v>170</v>
@@ -7805,7 +7805,7 @@
         <v>2</v>
       </c>
       <c r="D47" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E47" t="s">
         <v>3</v>
@@ -7817,13 +7817,13 @@
         <v>90</v>
       </c>
       <c r="H47" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="I47" t="s">
         <v>91</v>
       </c>
       <c r="J47" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="K47" t="s">
         <v>170</v>
@@ -7918,7 +7918,7 @@
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E48" t="s">
         <v>3</v>
@@ -7930,13 +7930,13 @@
         <v>58</v>
       </c>
       <c r="H48" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="I48" t="s">
         <v>93</v>
       </c>
       <c r="J48" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="K48" t="s">
         <v>170</v>
@@ -8031,7 +8031,7 @@
         <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E49" t="s">
         <v>3</v>
@@ -8043,13 +8043,13 @@
         <v>62</v>
       </c>
       <c r="H49" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="I49" t="s">
         <v>95</v>
       </c>
       <c r="J49" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="K49" t="s">
         <v>167</v>
@@ -8144,7 +8144,7 @@
         <v>5</v>
       </c>
       <c r="D50" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E50" t="s">
         <v>6</v>
@@ -8156,13 +8156,13 @@
         <v>62</v>
       </c>
       <c r="H50" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="I50" t="s">
         <v>95</v>
       </c>
       <c r="J50" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="K50" t="s">
         <v>167</v>
@@ -8198,7 +8198,7 @@
         <v>221</v>
       </c>
       <c r="V50" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="W50" t="s">
         <v>222</v>
@@ -8257,7 +8257,7 @@
         <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E51" t="s">
         <v>3</v>
@@ -8269,13 +8269,13 @@
         <v>65</v>
       </c>
       <c r="H51" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="I51" t="s">
         <v>96</v>
       </c>
       <c r="J51" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="K51" t="s">
         <v>195</v>
@@ -8370,7 +8370,7 @@
         <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="E52" t="s">
         <v>3</v>
@@ -8382,13 +8382,13 @@
         <v>97</v>
       </c>
       <c r="H52" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="I52" t="s">
         <v>98</v>
       </c>
       <c r="J52" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="K52" t="s">
         <v>170</v>
@@ -8483,7 +8483,7 @@
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E53" t="s">
         <v>3</v>
@@ -8495,13 +8495,13 @@
         <v>99</v>
       </c>
       <c r="H53" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I53" t="s">
         <v>100</v>
       </c>
       <c r="J53" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="K53" t="s">
         <v>170</v>
@@ -8596,7 +8596,7 @@
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E54" t="s">
         <v>6</v>
@@ -8608,13 +8608,13 @@
         <v>170</v>
       </c>
       <c r="H54" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="J54" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="K54" t="s">
         <v>170</v>
@@ -8650,7 +8650,7 @@
         <v>309</v>
       </c>
       <c r="V54" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="W54" s="1" t="s">
         <v>310</v>
@@ -8721,13 +8721,13 @@
         <v>59</v>
       </c>
       <c r="H55" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="I55" s="15" t="s">
         <v>94</v>
       </c>
       <c r="J55" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="K55" t="s">
         <v>170</v>
@@ -8837,10 +8837,10 @@
         <v>170</v>
       </c>
       <c r="I56" s="15" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="J56" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="K56" t="s">
         <v>170</v>
@@ -8879,10 +8879,10 @@
         <v>170</v>
       </c>
       <c r="W56" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="X56" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="Y56" t="s">
         <v>170</v>
@@ -8915,7 +8915,7 @@
         <v>170</v>
       </c>
       <c r="AI56" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AJ56">
         <v>0</v>
@@ -8953,7 +8953,7 @@
         <v>546</v>
       </c>
       <c r="J57" t="s">
-        <v>547</v>
+        <v>707</v>
       </c>
       <c r="K57" t="s">
         <v>170</v>
@@ -10136,13 +10136,13 @@
         <v>315</v>
       </c>
       <c r="C7" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D7" t="s">
         <v>299</v>
       </c>
       <c r="E7" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="F7" t="s">
         <v>117</v>
@@ -10311,13 +10311,13 @@
         <v>315</v>
       </c>
       <c r="C11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D11" t="s">
         <v>299</v>
       </c>
       <c r="E11" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="F11" t="s">
         <v>118</v>
@@ -10888,13 +10888,13 @@
         <v>315</v>
       </c>
       <c r="C25" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D25" t="s">
         <v>299</v>
       </c>
       <c r="E25" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="F25" t="s">
         <v>312</v>
@@ -11634,13 +11634,13 @@
         <v>315</v>
       </c>
       <c r="C43" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="D43" t="s">
         <v>299</v>
       </c>
       <c r="E43" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F43" t="s">
         <v>123</v>
@@ -11850,13 +11850,13 @@
         <v>315</v>
       </c>
       <c r="C48" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D48" t="s">
         <v>299</v>
       </c>
       <c r="E48" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F48" t="s">
         <v>124</v>
@@ -14749,19 +14749,19 @@
     </row>
     <row r="126" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
+        <v>656</v>
+      </c>
+      <c r="B126" t="s">
         <v>657</v>
       </c>
-      <c r="B126" t="s">
-        <v>658</v>
-      </c>
       <c r="C126" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D126" t="s">
         <v>530</v>
       </c>
       <c r="E126" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="F126" t="s">
         <v>170</v>
@@ -14785,19 +14785,19 @@
     </row>
     <row r="127" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
+        <v>656</v>
+      </c>
+      <c r="B127" t="s">
         <v>657</v>
       </c>
-      <c r="B127" t="s">
-        <v>658</v>
-      </c>
       <c r="C127" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D127" t="s">
         <v>530</v>
       </c>
       <c r="E127" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F127" t="s">
         <v>170</v>
@@ -14821,19 +14821,19 @@
     </row>
     <row r="128" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
+        <v>656</v>
+      </c>
+      <c r="B128" t="s">
         <v>657</v>
       </c>
-      <c r="B128" t="s">
-        <v>658</v>
-      </c>
       <c r="C128" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D128" t="s">
         <v>530</v>
       </c>
       <c r="E128" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="F128" t="s">
         <v>170</v>
@@ -14857,19 +14857,19 @@
     </row>
     <row r="129" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
+        <v>656</v>
+      </c>
+      <c r="B129" t="s">
         <v>657</v>
       </c>
-      <c r="B129" t="s">
-        <v>658</v>
-      </c>
       <c r="C129" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D129" t="s">
         <v>530</v>
       </c>
       <c r="E129" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F129" t="s">
         <v>170</v>
@@ -14893,19 +14893,19 @@
     </row>
     <row r="130" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
+        <v>656</v>
+      </c>
+      <c r="B130" t="s">
         <v>657</v>
       </c>
-      <c r="B130" t="s">
-        <v>658</v>
-      </c>
       <c r="C130" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D130" t="s">
         <v>530</v>
       </c>
       <c r="E130" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="F130" t="s">
         <v>170</v>
@@ -14929,19 +14929,19 @@
     </row>
     <row r="131" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
+        <v>656</v>
+      </c>
+      <c r="B131" t="s">
         <v>657</v>
       </c>
-      <c r="B131" t="s">
-        <v>658</v>
-      </c>
       <c r="C131" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D131" t="s">
         <v>530</v>
       </c>
       <c r="E131" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="F131" t="s">
         <v>170</v>
@@ -14965,19 +14965,19 @@
     </row>
     <row r="132" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
+        <v>656</v>
+      </c>
+      <c r="B132" t="s">
         <v>657</v>
       </c>
-      <c r="B132" t="s">
-        <v>658</v>
-      </c>
       <c r="C132" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D132" t="s">
         <v>530</v>
       </c>
       <c r="E132" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="F132" t="s">
         <v>170</v>
@@ -15001,19 +15001,19 @@
     </row>
     <row r="133" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
+        <v>656</v>
+      </c>
+      <c r="B133" t="s">
         <v>657</v>
       </c>
-      <c r="B133" t="s">
-        <v>658</v>
-      </c>
       <c r="C133" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D133" t="s">
         <v>530</v>
       </c>
       <c r="E133" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="F133" t="s">
         <v>170</v>
@@ -15037,19 +15037,19 @@
     </row>
     <row r="134" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
+        <v>656</v>
+      </c>
+      <c r="B134" t="s">
         <v>657</v>
       </c>
-      <c r="B134" t="s">
-        <v>658</v>
-      </c>
       <c r="C134" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D134" t="s">
         <v>530</v>
       </c>
       <c r="E134" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="F134" t="s">
         <v>170</v>
@@ -15073,19 +15073,19 @@
     </row>
     <row r="135" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
+        <v>656</v>
+      </c>
+      <c r="B135" t="s">
         <v>657</v>
       </c>
-      <c r="B135" t="s">
-        <v>658</v>
-      </c>
       <c r="C135" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D135" t="s">
         <v>530</v>
       </c>
       <c r="E135" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="F135" t="s">
         <v>170</v>
@@ -15109,19 +15109,19 @@
     </row>
     <row r="136" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
+        <v>656</v>
+      </c>
+      <c r="B136" t="s">
         <v>657</v>
       </c>
-      <c r="B136" t="s">
-        <v>658</v>
-      </c>
       <c r="C136" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D136" t="s">
         <v>530</v>
       </c>
       <c r="E136" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="F136" t="s">
         <v>170</v>
@@ -15145,19 +15145,19 @@
     </row>
     <row r="137" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
+        <v>656</v>
+      </c>
+      <c r="B137" t="s">
         <v>657</v>
       </c>
-      <c r="B137" t="s">
-        <v>658</v>
-      </c>
       <c r="C137" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="D137" t="s">
         <v>530</v>
       </c>
       <c r="E137" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="F137" t="s">
         <v>170</v>
@@ -15181,19 +15181,19 @@
     </row>
     <row r="138" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
+        <v>656</v>
+      </c>
+      <c r="B138" t="s">
         <v>657</v>
       </c>
-      <c r="B138" t="s">
-        <v>658</v>
-      </c>
       <c r="C138" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D138" t="s">
         <v>530</v>
       </c>
       <c r="E138" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="F138" t="s">
         <v>170</v>
@@ -15212,24 +15212,24 @@
         <v>hts_mod_fac_vmmc</v>
       </c>
       <c r="AG138" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="139" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
+        <v>656</v>
+      </c>
+      <c r="B139" t="s">
         <v>657</v>
       </c>
-      <c r="B139" t="s">
-        <v>658</v>
-      </c>
       <c r="C139" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D139" t="s">
         <v>530</v>
       </c>
       <c r="E139" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="F139" t="s">
         <v>170</v>
@@ -15248,24 +15248,24 @@
         <v>hts_mod_fac_anc_1</v>
       </c>
       <c r="AG139" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="140" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
+        <v>656</v>
+      </c>
+      <c r="B140" t="s">
         <v>657</v>
       </c>
-      <c r="B140" t="s">
-        <v>658</v>
-      </c>
       <c r="C140" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D140" t="s">
         <v>530</v>
       </c>
       <c r="E140" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="F140" t="s">
         <v>170</v>
@@ -15284,7 +15284,7 @@
         <v>hts_mod_fac_tb</v>
       </c>
       <c r="AG140" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="141" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
@@ -15295,19 +15295,19 @@
         <v>315</v>
       </c>
       <c r="C141" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D141" t="s">
         <v>299</v>
       </c>
       <c r="E141" t="s">
+        <v>667</v>
+      </c>
+      <c r="F141" t="s">
+        <v>667</v>
+      </c>
+      <c r="G141" t="s">
         <v>668</v>
-      </c>
-      <c r="F141" t="s">
-        <v>668</v>
-      </c>
-      <c r="G141" t="s">
-        <v>669</v>
       </c>
       <c r="H141">
         <v>3</v>
@@ -15328,7 +15328,7 @@
       <c r="R141" s="9"/>
       <c r="T141" s="9"/>
       <c r="AG141" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="142" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
@@ -15348,10 +15348,10 @@
         <v>154</v>
       </c>
       <c r="F142" t="s">
+        <v>670</v>
+      </c>
+      <c r="G142" t="s">
         <v>671</v>
-      </c>
-      <c r="G142" t="s">
-        <v>672</v>
       </c>
       <c r="H142">
         <v>3</v>
@@ -15364,7 +15364,7 @@
         <v>U_sex</v>
       </c>
       <c r="AG142" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data required update one datapack code
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE8A32F-B161-074A-A1D8-40CAE84070FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95AD9B39-8114-1842-9813-DF58EF30365E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
@@ -1919,9 +1919,6 @@
     <t>GEND_GBV.N.ViolenceServiceType.T_1.physEmot</t>
   </si>
   <si>
-    <t>GEND_GBV.N.ViolenceServiceType.T_1.Sexual_Violence__Post_Rape_Care</t>
-  </si>
-  <si>
     <t>PrEP_NEW.N.KeyPopAbr.T_1</t>
   </si>
   <si>
@@ -1986,6 +1983,9 @@
   </si>
   <si>
     <t>HTS_SELF.N.Age/Sex/HIVSelfTest.R</t>
+  </si>
+  <si>
+    <t>GEND_GBV.N.ViolenceServiceType.T_1.Sexual</t>
   </si>
 </sst>
 </file>
@@ -2414,7 +2414,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B61" sqref="B61"/>
+      <selection pane="bottomRight" activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6620,13 +6620,13 @@
         <v>21</v>
       </c>
       <c r="B38" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
       </c>
       <c r="D38" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="E38" t="s">
         <v>6</v>
@@ -6656,7 +6656,7 @@
         <v>143</v>
       </c>
       <c r="N38" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="O38" t="s">
         <v>143</v>
@@ -8315,13 +8315,13 @@
         <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C53" t="s">
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E53" t="s">
         <v>3</v>
@@ -8330,13 +8330,13 @@
         <v>142</v>
       </c>
       <c r="G53" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="H53" t="s">
         <v>642</v>
       </c>
-      <c r="H53" t="s">
+      <c r="I53" t="s">
         <v>643</v>
-      </c>
-      <c r="I53" t="s">
-        <v>644</v>
       </c>
       <c r="J53" t="s">
         <v>509</v>
@@ -8541,7 +8541,7 @@
         <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>627</v>
+        <v>649</v>
       </c>
       <c r="C55" t="s">
         <v>2</v>
@@ -8767,7 +8767,7 @@
         <v>48</v>
       </c>
       <c r="B57" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C57" t="s">
         <v>2</v>
@@ -8880,7 +8880,7 @@
         <v>48</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C58" t="s">
         <v>2</v>
@@ -8895,13 +8895,13 @@
         <v>142</v>
       </c>
       <c r="G58" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="H58" t="s">
+        <v>644</v>
+      </c>
+      <c r="I58" s="14" t="s">
         <v>647</v>
-      </c>
-      <c r="H58" t="s">
-        <v>645</v>
-      </c>
-      <c r="I58" s="14" t="s">
-        <v>648</v>
       </c>
       <c r="J58" t="s">
         <v>509</v>
@@ -8993,7 +8993,7 @@
         <v>48</v>
       </c>
       <c r="B59" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C59" t="s">
         <v>2</v>
@@ -9106,7 +9106,7 @@
         <v>450</v>
       </c>
       <c r="B60" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C60" t="s">
         <v>2</v>
@@ -9219,13 +9219,13 @@
         <v>21</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C61" t="s">
         <v>5</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E61" t="s">
         <v>6</v>
@@ -9279,10 +9279,10 @@
         <v>143</v>
       </c>
       <c r="V61" t="s">
+        <v>632</v>
+      </c>
+      <c r="W61" t="s">
         <v>633</v>
-      </c>
-      <c r="W61" t="s">
-        <v>634</v>
       </c>
       <c r="X61" s="1" t="s">
         <v>139</v>
@@ -9332,13 +9332,13 @@
         <v>21</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C62" t="s">
         <v>2</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E62" t="s">
         <v>3</v>
@@ -14939,13 +14939,13 @@
         <v>562</v>
       </c>
       <c r="C141" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D141" t="s">
         <v>436</v>
       </c>
       <c r="E141" s="17" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="F141" t="s">
         <v>143</v>
@@ -14964,7 +14964,7 @@
         <v>hts_mod_fac_post_anc_1</v>
       </c>
       <c r="AG141" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="142" spans="1:33" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
data required change / to _ in codes
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95AD9B39-8114-1842-9813-DF58EF30365E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A14091-50BA-C942-BDDD-3E82E99D6A61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="33600" yWindow="0" windowWidth="25600" windowHeight="20480" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3535" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3535" uniqueCount="651">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1877,45 +1877,9 @@
     <t>2019Q4</t>
   </si>
   <si>
-    <t>PMTCT_STAT.D.Age/Sex.T_1</t>
-  </si>
-  <si>
-    <t>TB_STAT.D.Age/Sex.T_1</t>
-  </si>
-  <si>
-    <t>VMMC_CIRC.N.Age/Sex.T_1</t>
-  </si>
-  <si>
-    <t>TX_CURR.N.Age/Sex/HIVStatus.T_1</t>
-  </si>
-  <si>
-    <t>HTS_SELF.N.Age/Sex/HIVSelfTest.T_1.Directly_Assisted</t>
-  </si>
-  <si>
-    <t>HTS_SELF.N.Age/Sex/HIVSelfTest.T_1.Unassisted</t>
-  </si>
-  <si>
-    <t>OVC_SERV.N.Age/Sex.T_1</t>
-  </si>
-  <si>
     <t>KP_MAT.N.Sex.T_1</t>
   </si>
   <si>
-    <t>HTS_TST.N.KeyPop/Result.T_1.Positive</t>
-  </si>
-  <si>
-    <t>HTS_TST.N.KeyPop/Result.T_1.Negative</t>
-  </si>
-  <si>
-    <t>TX_NEW.N.KeyPop/HIVStatus.T_1</t>
-  </si>
-  <si>
-    <t>PP_PREV.N.Age/Sex.T_1</t>
-  </si>
-  <si>
-    <t>PrEP_NEW.N.Age/Sex.T_1</t>
-  </si>
-  <si>
     <t>GEND_GBV.N.ViolenceServiceType.T_1.physEmot</t>
   </si>
   <si>
@@ -1955,9 +1919,6 @@
     <t>qdFQQc5dCbH</t>
   </si>
   <si>
-    <t>PrEP_CURR.N.Age/Sex.T_1</t>
-  </si>
-  <si>
     <t>[PrEP_CURR.N.Age/Sex.T]</t>
   </si>
   <si>
@@ -1986,6 +1947,48 @@
   </si>
   <si>
     <t>GEND_GBV.N.ViolenceServiceType.T_1.Sexual</t>
+  </si>
+  <si>
+    <t>PMTCT_STAT.D.Age_Sex.T_1</t>
+  </si>
+  <si>
+    <t>TB_STAT.D.Age_Sex.T_1</t>
+  </si>
+  <si>
+    <t>VMMC_CIRC.N.Age_Sex.T_1</t>
+  </si>
+  <si>
+    <t>TX_CURR.N.Age_Sex_HIVStatus.T_1</t>
+  </si>
+  <si>
+    <t>HTS_SELF.N.Age_Sex_HIVSelfTest.T_1.Directly_Assisted</t>
+  </si>
+  <si>
+    <t>HTS_SELF.N.Age_Sex_HIVSelfTest.T_1.Unassisted</t>
+  </si>
+  <si>
+    <t>OVC_SERV.N.Age_Sex.T_1</t>
+  </si>
+  <si>
+    <t>HTS_TST.N.KeyPop_Result.T_1.Positive</t>
+  </si>
+  <si>
+    <t>HTS_TST.N.KeyPop_Result.T_1.Negative</t>
+  </si>
+  <si>
+    <t>TX_NEW.N.KeyPop_HIVStatus.T_1</t>
+  </si>
+  <si>
+    <t>PP_PREV.N.Age_Sex.T_1</t>
+  </si>
+  <si>
+    <t>PrEP_NEW.N.Age_Sex.T_1</t>
+  </si>
+  <si>
+    <t>PrEP_CURR.N.Age_Sex.T_1</t>
+  </si>
+  <si>
+    <t>HTS_SELF.N.Age_Sex_HIVSelfTest.R</t>
   </si>
 </sst>
 </file>
@@ -2411,10 +2414,10 @@
   <dimension ref="A1:AK62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B52" sqref="B52"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2552,7 +2555,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>613</v>
+        <v>637</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -3117,7 +3120,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>614</v>
+        <v>638</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -3569,7 +3572,7 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>615</v>
+        <v>639</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -3908,7 +3911,7 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>616</v>
+        <v>640</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
@@ -6620,13 +6623,13 @@
         <v>21</v>
       </c>
       <c r="B38" t="s">
-        <v>634</v>
+        <v>622</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
       </c>
       <c r="D38" t="s">
-        <v>635</v>
+        <v>623</v>
       </c>
       <c r="E38" t="s">
         <v>6</v>
@@ -6656,7 +6659,7 @@
         <v>143</v>
       </c>
       <c r="N38" t="s">
-        <v>637</v>
+        <v>625</v>
       </c>
       <c r="O38" t="s">
         <v>143</v>
@@ -6733,7 +6736,7 @@
         <v>21</v>
       </c>
       <c r="B39" t="s">
-        <v>617</v>
+        <v>641</v>
       </c>
       <c r="C39" t="s">
         <v>2</v>
@@ -6846,7 +6849,7 @@
         <v>21</v>
       </c>
       <c r="B40" t="s">
-        <v>618</v>
+        <v>642</v>
       </c>
       <c r="C40" t="s">
         <v>2</v>
@@ -7298,7 +7301,7 @@
         <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>619</v>
+        <v>643</v>
       </c>
       <c r="C44" t="s">
         <v>2</v>
@@ -7524,7 +7527,7 @@
         <v>48</v>
       </c>
       <c r="B46" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="C46" t="s">
         <v>2</v>
@@ -7637,7 +7640,7 @@
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>621</v>
+        <v>644</v>
       </c>
       <c r="C47" t="s">
         <v>2</v>
@@ -7750,7 +7753,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>622</v>
+        <v>645</v>
       </c>
       <c r="C48" t="s">
         <v>2</v>
@@ -7863,7 +7866,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>623</v>
+        <v>646</v>
       </c>
       <c r="C49" t="s">
         <v>2</v>
@@ -7976,7 +7979,7 @@
         <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>624</v>
+        <v>647</v>
       </c>
       <c r="C50" t="s">
         <v>2</v>
@@ -8202,7 +8205,7 @@
         <v>55</v>
       </c>
       <c r="B52" t="s">
-        <v>625</v>
+        <v>648</v>
       </c>
       <c r="C52" t="s">
         <v>2</v>
@@ -8315,13 +8318,13 @@
         <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>639</v>
+        <v>649</v>
       </c>
       <c r="C53" t="s">
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>640</v>
+        <v>627</v>
       </c>
       <c r="E53" t="s">
         <v>3</v>
@@ -8330,13 +8333,13 @@
         <v>142</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>641</v>
+        <v>628</v>
       </c>
       <c r="H53" t="s">
-        <v>642</v>
+        <v>629</v>
       </c>
       <c r="I53" t="s">
-        <v>643</v>
+        <v>630</v>
       </c>
       <c r="J53" t="s">
         <v>509</v>
@@ -8428,7 +8431,7 @@
         <v>57</v>
       </c>
       <c r="B54" t="s">
-        <v>626</v>
+        <v>614</v>
       </c>
       <c r="C54" t="s">
         <v>2</v>
@@ -8541,7 +8544,7 @@
         <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>649</v>
+        <v>636</v>
       </c>
       <c r="C55" t="s">
         <v>2</v>
@@ -8767,7 +8770,7 @@
         <v>48</v>
       </c>
       <c r="B57" t="s">
-        <v>627</v>
+        <v>615</v>
       </c>
       <c r="C57" t="s">
         <v>2</v>
@@ -8880,7 +8883,7 @@
         <v>48</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>645</v>
+        <v>632</v>
       </c>
       <c r="C58" t="s">
         <v>2</v>
@@ -8895,13 +8898,13 @@
         <v>142</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>646</v>
+        <v>633</v>
       </c>
       <c r="H58" t="s">
-        <v>644</v>
+        <v>631</v>
       </c>
       <c r="I58" s="14" t="s">
-        <v>647</v>
+        <v>634</v>
       </c>
       <c r="J58" t="s">
         <v>509</v>
@@ -8993,7 +8996,7 @@
         <v>48</v>
       </c>
       <c r="B59" t="s">
-        <v>628</v>
+        <v>616</v>
       </c>
       <c r="C59" t="s">
         <v>2</v>
@@ -9106,7 +9109,7 @@
         <v>450</v>
       </c>
       <c r="B60" t="s">
-        <v>629</v>
+        <v>617</v>
       </c>
       <c r="C60" t="s">
         <v>2</v>
@@ -9219,13 +9222,13 @@
         <v>21</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>630</v>
+        <v>618</v>
       </c>
       <c r="C61" t="s">
         <v>5</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>631</v>
+        <v>619</v>
       </c>
       <c r="E61" t="s">
         <v>6</v>
@@ -9279,10 +9282,10 @@
         <v>143</v>
       </c>
       <c r="V61" t="s">
-        <v>632</v>
+        <v>620</v>
       </c>
       <c r="W61" t="s">
-        <v>633</v>
+        <v>621</v>
       </c>
       <c r="X61" s="1" t="s">
         <v>139</v>
@@ -9332,13 +9335,13 @@
         <v>21</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="C62" t="s">
         <v>2</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>648</v>
+        <v>635</v>
       </c>
       <c r="E62" t="s">
         <v>3</v>
@@ -14939,13 +14942,13 @@
         <v>562</v>
       </c>
       <c r="C141" t="s">
-        <v>638</v>
+        <v>626</v>
       </c>
       <c r="D141" t="s">
         <v>436</v>
       </c>
       <c r="E141" s="17" t="s">
-        <v>636</v>
+        <v>624</v>
       </c>
       <c r="F141" t="s">
         <v>143</v>
@@ -14964,7 +14967,7 @@
         <v>hts_mod_fac_post_anc_1</v>
       </c>
       <c r="AG141" t="s">
-        <v>637</v>
+        <v>625</v>
       </c>
     </row>
     <row r="142" spans="1:33" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
data required update formulas with T_1 or R
correspnding to FY agnostic naming
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A14091-50BA-C942-BDDD-3E82E99D6A61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F73281-FE72-694C-BAF1-E4685ACC7C91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="0" windowWidth="25600" windowHeight="20480" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -1409,162 +1409,6 @@
     <t>B.value_na</t>
   </si>
   <si>
-    <t>[@PMTCT_STAT.D.Age/Sex.19T]</t>
-  </si>
-  <si>
-    <t>[@PMTCT_STAT.N.Age/Sex/KnownNewResult.18R.Known_at_Entry_Positive]%/%[@PMTCT_STAT.N.Age/Sex/KnownNewResult.18R]</t>
-  </si>
-  <si>
-    <t>[@PMTCT_STAT.N.Age/Sex/KnownNewResult.18R.Newly_Identified_Positive]%/%([@PMTCT_STAT.N.Age/Sex/KnownNewResult.18R.Newly_Identified_Positive]+[@PMTCT_STAT.N.Age/Sex/KnownNewResult.18R.Newly_Identified_Negative])</t>
-  </si>
-  <si>
-    <t>[PMTCT_HEI_POS.N.Age/HIVStatus.18R.2 - 12 months]%/%[PMTCT_EID.N.Age.18R.2 - 12 months]</t>
-  </si>
-  <si>
-    <t>[TB_STAT.D.Age/Sex.19T]</t>
-  </si>
-  <si>
-    <t>([TB_STAT.D.Age/Sex.19T]-[TB_STAT.D.Age/Sex.18R])%/%[TB_STAT.D.Age/Sex.18R]</t>
-  </si>
-  <si>
-    <t>[TB_STAT.N.Age Agg/Sex/KnownNewPosNeg.18R.Known_at_Entry_Positive]%/%[TB_STAT.N.Age Agg/Sex/KnownNewPosNeg.18R]</t>
-  </si>
-  <si>
-    <t>[TB_STAT.N.Age Agg/Sex/KnownNewPosNeg.18R.Newly_Identified_Positive]%/%([TB_STAT.N.Age Agg/Sex/KnownNewPosNeg.18R.Newly_Identified_Positive]+[TB_STAT.N.Age Agg/Sex/KnownNewPosNeg.18R.Newly_Identified_Negative])</t>
-  </si>
-  <si>
-    <t>[VMMC_CIRC.N.Age/Sex.19T]</t>
-  </si>
-  <si>
-    <t>[VMMC_CIRC.N.HIVStatus/Sex.18R.Positive]%/%([VMMC_CIRC.N.HIVStatus/Sex.18R.Positive]+[VMMC_CIRC.N.HIVStatus/Sex.18R.Negative])</t>
-  </si>
-  <si>
-    <t>[VMMC_CIRC.N.HIVStatus/Sex.18R.Unknown]%/%[VMMC_CIRC.N.HIVStatus/Sex.18R]</t>
-  </si>
-  <si>
-    <t>[TX_CURR.N.Age/Sex/HIVStatus.19T]</t>
-  </si>
-  <si>
-    <t>([HTS_TST.N.Index/Age/Sex/Result.18R.Positive]+[HTS_TST.N.IndexMod/Age/Sex/Result.18R.Positive])%/%([HTS_TST.N.Index/Age/Sex/Result.18R.Positive]+[HTS_TST.N.IndexMod/Age/Sex/Result.18R.Positive]+[HTS_TST.N.Index/Age/Sex/Result.18R.Negative]+[HTS_TST.N.IndexMod/Age/Sex/Result.18R.Negative])</t>
-  </si>
-  <si>
-    <t>([HTS_TST.N.IndexMod/Age/Sex/Result.18R.Positive])%/%([HTS_TST.N.Index/Age/Sex/Result.18R.Positive]+[HTS_TST.N.IndexMod/Age/Sex/Result.18R.Positive])</t>
-  </si>
-  <si>
-    <t>[HTS_TST.N.MobileMod/Age/Sex/Result.18R.Positive]%/%[HTS_TST_POS.N.???.18R]</t>
-  </si>
-  <si>
-    <t>[HTS_TST.N.VCTMod/Age/Sex/Result.18R.Positive]%/%[HTS_TST_POS.N.???.18R]</t>
-  </si>
-  <si>
-    <t>[HTS_TST.N.OtherMod/Age/Sex/Result.18R.Positive]%/%[HTS_TST_POS.N.???.18R]</t>
-  </si>
-  <si>
-    <t>[HTS_TST.N.Emergency Ward/Age/Sex/Result.18R.Positive]%/%[HTS_TST_POS.N.???.18R]</t>
-  </si>
-  <si>
-    <t>[HTS_TST.N.Inpat/Age/Sex/Result.18R.Positive]%/%[HTS_TST_POS.N.???.18R]</t>
-  </si>
-  <si>
-    <t>[HTS_TST.N.Malnutrition/Age/Sex/Result.18R.Positive]%/%[HTS_TST_POS.N.???.18R]</t>
-  </si>
-  <si>
-    <t>[HTS_TST.N.Pediatric/Age/Sex/Result.18R.Positive]%/%[HTS_TST_POS.N.???.18R]</t>
-  </si>
-  <si>
-    <t>[HTS_TST.N.STI Clinic/Age/Sex/Result.18R.Positive]%/%[HTS_TST_POS.N.???.18R]</t>
-  </si>
-  <si>
-    <t>[HTS_TST.N.VCT/Age/Sex/Result.18R.Positive]%/%[HTS_TST_POS.N.???.18R]</t>
-  </si>
-  <si>
-    <t>[HTS_TST.N.OtherPITC/Age/Sex/Result.18R.Positive]%/%[HTS_TST_POS.N.???.18R]</t>
-  </si>
-  <si>
-    <t>[HTS_TST.N.MobileMod/Age/Sex/Result.18R.Positive]%/%([HTS_TST.N.MobileMod/Age/Sex/Result.18R.Positive]+[HTS_TST.N.MobileMod/Age/Sex/Result.18R.Negative])</t>
-  </si>
-  <si>
-    <t>[HTS_TST.N.VCTMod/Age/Sex/Result.18R.Positive]%/%([HTS_TST.N.VCTMod/Age/Sex/Result.18R.Positive]+[HTS_TST.N.VCTMod/Age/Sex/Result.18R.Negative])</t>
-  </si>
-  <si>
-    <t>[HTS_TST.N.OtherMod/Age/Sex/Result.18R.Positive]%/%([HTS_TST.N.OtherMod/Age/Sex/Result.18R.Positive]+[HTS_TST.N.OtherMod/Age/Sex/Result.18R.Negative])</t>
-  </si>
-  <si>
-    <t>[HTS_TST.N.Emergency Ward/Age/Sex/Result.18R.Positive]%/%([HTS_TST.N.Emergency Ward/Age/Sex/Result.18R.Positive]+[HTS_TST.N.Emergency Ward/Age/Sex/Result.18R.Negative])</t>
-  </si>
-  <si>
-    <t>[HTS_TST.N.Inpat/Age/Sex/Result.18R.Positive]%/%([HTS_TST.N.Inpat/Age/Sex/Result.18R.Positive]+[HTS_TST.N.Inpat/Age/Sex/Result.18R.Negative])</t>
-  </si>
-  <si>
-    <t>[HTS_TST.N.Malnutrition/Age/Sex/Result.18R.Positive]%/%([HTS_TST.N.Malnutrition/Age/Sex/Result.18R.Positive]+[HTS_TST.N.Malnutrition/Age/Sex/Result.18R.Negative])</t>
-  </si>
-  <si>
-    <t>[HTS_TST.N.Pediatric/Age/Sex/Result.18R.Positive]%/%([HTS_TST.N.Pediatric/Age/Sex/Result.18R.Positive]+[HTS_TST.N.Pediatric/Age/Sex/Result.18R.Negative])</t>
-  </si>
-  <si>
-    <t>[HTS_TST.N.STI Clinic/Age/Sex/Result.18R.Positive]%/%([HTS_TST.N.STI Clinic/Age/Sex/Result.18R.Positive]+[HTS_TST.N.STI Clinic/Age/Sex/Result.18R.Negative])</t>
-  </si>
-  <si>
-    <t>[HTS_TST.N.VCT/Age/Sex/Result.18R.Positive]%/%([HTS_TST.N.VCT/Age/Sex/Result.18R.Positive]+[HTS_TST.N.VCT/Age/Sex/Result.18R.Negative])</t>
-  </si>
-  <si>
-    <t>[HTS_TST.N.OtherPITC/Age/Sex/Result.18R.Positive]%/%([HTS_TST.N.OtherPITC/Age/Sex/Result.18R.Positive]+[HTS_TST.N.OtherPITC/Age/Sex/Result.18R.Negative])</t>
-  </si>
-  <si>
-    <t>[HTS_SELF.N.Age/Sex/HIVSelfTest.19T.Directly_Assisted]</t>
-  </si>
-  <si>
-    <t>[HTS_SELF.N.Age/Sex/HIVSelfTest.19T.Unassisted]</t>
-  </si>
-  <si>
-    <t>([HTS_SELF.N.Age/Sex/HIVSelfTest.19T]-[HTS_SELF.N.Age/Sex/HIVSelfTest.18R])%/%[HTS_SELF.N.Age/Sex/HIVSelfTest.18R]</t>
-  </si>
-  <si>
-    <t>[TX_TB.D.TBScreen/NewExistingART/HIVStatus.18R.Life-long ART/New/TB Screen - Positive/Positive]%/%([TX_TB.D.TBScreen/NewExistingART/HIVStatus.18R.Life-long ART/New/TB Screen - Positive/Positive]+[TX_TB.D.TBScreen/NewExistingART/HIVStatus.18R.Life-long ART/New/TB Screen - Negative/Positive])</t>
-  </si>
-  <si>
-    <t>[TX_TB.D.TBScreen/NewExistingART/HIVStatus.18R.Life-long ART/Already/TB Screen - Positive/Positive]%/%([TX_TB.D.TBScreen/NewExistingART/HIVStatus.18R.Life-long ART/Already/TB Screen - Positive/Positive]+[TX_TB.D.TBScreen/NewExistingART/HIVStatus.18R.Life-long ART/Already/TB Screen - Negative/Positive])</t>
-  </si>
-  <si>
-    <t>[OVC_SERV.N.Age/Sex.19T]</t>
-  </si>
-  <si>
-    <t>([OVC_SERV.N.Age/Sex.19T]-[OVC_SERV.N.Age/Sex.18R])%/%[OVC_SERV.N.Age/Sex.18R]</t>
-  </si>
-  <si>
-    <t>[KP_MAT.N.Sex.19T]</t>
-  </si>
-  <si>
-    <t>[HTS_TST.N.KeyPop/Result.19T.Positive]</t>
-  </si>
-  <si>
-    <t>[HTS_TST.N.KeyPop/Result.19T.Negative]</t>
-  </si>
-  <si>
-    <t>[TX_NEW.N.KeyPop/HIVStatus.19T]</t>
-  </si>
-  <si>
-    <t>[PP_PREV.N.Age/Sex.19T]</t>
-  </si>
-  <si>
-    <t>([PP_PREV.N.Age/Sex.19T]-[PP_PREV.N.Age/Sex.18R])%/%[PP_PREV.N.Age/Sex.18R]</t>
-  </si>
-  <si>
-    <t>[PrEP_NEW.N.Age/Sex.19T]</t>
-  </si>
-  <si>
-    <t>[GEND_GBV.N.ViolenceServiceType.19T.Physical_and_or_Emotional_Violence]</t>
-  </si>
-  <si>
-    <t>[GEND_GBV.N.ViolenceServiceType.19T.Sexual_Violence__Post_Rape_Care_]</t>
-  </si>
-  <si>
-    <t>([GEND_GBV.N.Age/Sex/ViolenceType.19T]-[GEND_GBV.N.Age/Sex/ViolenceType.18R])%/%[GEND_GBV.N.Age/Sex/ViolenceType.18R]</t>
-  </si>
-  <si>
-    <t>[PMTCT_HEI_POS.N.Age/HIVStatus.18R.&lt;= 2 months]%/%[PMTCT_EID.N.Age.18R.&lt;= 2 months]</t>
-  </si>
-  <si>
     <t>2019Oct</t>
   </si>
   <si>
@@ -1907,9 +1751,6 @@
     <t>HTS_TST_PMTCTPostANC1.N.yield</t>
   </si>
   <si>
-    <t>[HTS_TST.N.PMTCTPostANC1/Age/Sex/Result.18R.Positive]%/%([HTS_TST.N.PMTCTPostANC1/Age/Sex/Result.18R.Positive]+[HTS_TST.N.PMTCTPostANC1/Age/Sex/Result.18R.Negative])</t>
-  </si>
-  <si>
     <t>Facility - PMTCT Post ANC1 FY19R/FY20T</t>
   </si>
   <si>
@@ -1919,9 +1760,6 @@
     <t>qdFQQc5dCbH</t>
   </si>
   <si>
-    <t>[PrEP_CURR.N.Age/Sex.T]</t>
-  </si>
-  <si>
     <t>PrEP_CURR.N.Age/Sex.T</t>
   </si>
   <si>
@@ -1989,6 +1827,168 @@
   </si>
   <si>
     <t>HTS_SELF.N.Age_Sex_HIVSelfTest.R</t>
+  </si>
+  <si>
+    <t>[PrEP_CURR.N.Age/Sex.T_1]</t>
+  </si>
+  <si>
+    <t>[@PMTCT_STAT.D.Age/Sex.T_1]</t>
+  </si>
+  <si>
+    <t>[TB_STAT.D.Age/Sex.T_1]</t>
+  </si>
+  <si>
+    <t>[VMMC_CIRC.N.Age/Sex.T_1]</t>
+  </si>
+  <si>
+    <t>[TX_CURR.N.Age/Sex/HIVStatus.T_1]</t>
+  </si>
+  <si>
+    <t>[HTS_SELF.N.Age/Sex/HIVSelfTest.T_1.Directly_Assisted]</t>
+  </si>
+  <si>
+    <t>[HTS_SELF.N.Age/Sex/HIVSelfTest.T_1.Unassisted]</t>
+  </si>
+  <si>
+    <t>[OVC_SERV.N.Age/Sex.T_1]</t>
+  </si>
+  <si>
+    <t>[KP_MAT.N.Sex.T_1]</t>
+  </si>
+  <si>
+    <t>[HTS_TST.N.KeyPop/Result.T_1.Positive]</t>
+  </si>
+  <si>
+    <t>[HTS_TST.N.KeyPop/Result.T_1.Negative]</t>
+  </si>
+  <si>
+    <t>[TX_NEW.N.KeyPop/HIVStatus.T_1]</t>
+  </si>
+  <si>
+    <t>[PP_PREV.N.Age/Sex.T_1]</t>
+  </si>
+  <si>
+    <t>[PrEP_NEW.N.Age/Sex.T_1]</t>
+  </si>
+  <si>
+    <t>[GEND_GBV.N.ViolenceServiceType.T_1.Physical_and_or_Emotional_Violence]</t>
+  </si>
+  <si>
+    <t>[GEND_GBV.N.ViolenceServiceType.T_1.Sexual_Violence__Post_Rape_Care_]</t>
+  </si>
+  <si>
+    <t>[@PMTCT_STAT.N.Age/Sex/KnownNewResult.R.Known_at_Entry_Positive]%/%[@PMTCT_STAT.N.Age/Sex/KnownNewResult.R]</t>
+  </si>
+  <si>
+    <t>[@PMTCT_STAT.N.Age/Sex/KnownNewResult.R.Newly_Identified_Positive]%/%([@PMTCT_STAT.N.Age/Sex/KnownNewResult.R.Newly_Identified_Positive]+[@PMTCT_STAT.N.Age/Sex/KnownNewResult.R.Newly_Identified_Negative])</t>
+  </si>
+  <si>
+    <t>[PMTCT_HEI_POS.N.Age/HIVStatus.R.&lt;= 2 months]%/%[PMTCT_EID.N.Age.R.&lt;= 2 months]</t>
+  </si>
+  <si>
+    <t>[PMTCT_HEI_POS.N.Age/HIVStatus.R.2 - 12 months]%/%[PMTCT_EID.N.Age.R.2 - 12 months]</t>
+  </si>
+  <si>
+    <t>([TB_STAT.D.Age/Sex.T_1]-[TB_STAT.D.Age/Sex.R])%/%[TB_STAT.D.Age/Sex.R]</t>
+  </si>
+  <si>
+    <t>[TB_STAT.N.Age Agg/Sex/KnownNewPosNeg.R.Known_at_Entry_Positive]%/%[TB_STAT.N.Age Agg/Sex/KnownNewPosNeg.R]</t>
+  </si>
+  <si>
+    <t>[TB_STAT.N.Age Agg/Sex/KnownNewPosNeg.R.Newly_Identified_Positive]%/%([TB_STAT.N.Age Agg/Sex/KnownNewPosNeg.R.Newly_Identified_Positive]+[TB_STAT.N.Age Agg/Sex/KnownNewPosNeg.R.Newly_Identified_Negative])</t>
+  </si>
+  <si>
+    <t>[VMMC_CIRC.N.HIVStatus/Sex.R.Positive]%/%([VMMC_CIRC.N.HIVStatus/Sex.R.Positive]+[VMMC_CIRC.N.HIVStatus/Sex.R.Negative])</t>
+  </si>
+  <si>
+    <t>[VMMC_CIRC.N.HIVStatus/Sex.R.Unknown]%/%[VMMC_CIRC.N.HIVStatus/Sex.R]</t>
+  </si>
+  <si>
+    <t>([HTS_TST.N.Index/Age/Sex/Result.R.Positive]+[HTS_TST.N.IndexMod/Age/Sex/Result.R.Positive])%/%([HTS_TST.N.Index/Age/Sex/Result.R.Positive]+[HTS_TST.N.IndexMod/Age/Sex/Result.R.Positive]+[HTS_TST.N.Index/Age/Sex/Result.R.Negative]+[HTS_TST.N.IndexMod/Age/Sex/Result.R.Negative])</t>
+  </si>
+  <si>
+    <t>([HTS_TST.N.IndexMod/Age/Sex/Result.R.Positive])%/%([HTS_TST.N.Index/Age/Sex/Result.R.Positive]+[HTS_TST.N.IndexMod/Age/Sex/Result.R.Positive])</t>
+  </si>
+  <si>
+    <t>[HTS_TST.N.MobileMod/Age/Sex/Result.R.Positive]%/%[HTS_TST_POS.N.???.R]</t>
+  </si>
+  <si>
+    <t>[HTS_TST.N.VCTMod/Age/Sex/Result.R.Positive]%/%[HTS_TST_POS.N.???.R]</t>
+  </si>
+  <si>
+    <t>[HTS_TST.N.OtherMod/Age/Sex/Result.R.Positive]%/%[HTS_TST_POS.N.???.R]</t>
+  </si>
+  <si>
+    <t>[HTS_TST.N.Emergency Ward/Age/Sex/Result.R.Positive]%/%[HTS_TST_POS.N.???.R]</t>
+  </si>
+  <si>
+    <t>[HTS_TST.N.Inpat/Age/Sex/Result.R.Positive]%/%[HTS_TST_POS.N.???.R]</t>
+  </si>
+  <si>
+    <t>[HTS_TST.N.Malnutrition/Age/Sex/Result.R.Positive]%/%[HTS_TST_POS.N.???.R]</t>
+  </si>
+  <si>
+    <t>[HTS_TST.N.Pediatric/Age/Sex/Result.R.Positive]%/%[HTS_TST_POS.N.???.R]</t>
+  </si>
+  <si>
+    <t>[HTS_TST.N.STI Clinic/Age/Sex/Result.R.Positive]%/%[HTS_TST_POS.N.???.R]</t>
+  </si>
+  <si>
+    <t>[HTS_TST.N.VCT/Age/Sex/Result.R.Positive]%/%[HTS_TST_POS.N.???.R]</t>
+  </si>
+  <si>
+    <t>[HTS_TST.N.OtherPITC/Age/Sex/Result.R.Positive]%/%[HTS_TST_POS.N.???.R]</t>
+  </si>
+  <si>
+    <t>[HTS_TST.N.MobileMod/Age/Sex/Result.R.Positive]%/%([HTS_TST.N.MobileMod/Age/Sex/Result.R.Positive]+[HTS_TST.N.MobileMod/Age/Sex/Result.R.Negative])</t>
+  </si>
+  <si>
+    <t>[HTS_TST.N.VCTMod/Age/Sex/Result.R.Positive]%/%([HTS_TST.N.VCTMod/Age/Sex/Result.R.Positive]+[HTS_TST.N.VCTMod/Age/Sex/Result.R.Negative])</t>
+  </si>
+  <si>
+    <t>[HTS_TST.N.OtherMod/Age/Sex/Result.R.Positive]%/%([HTS_TST.N.OtherMod/Age/Sex/Result.R.Positive]+[HTS_TST.N.OtherMod/Age/Sex/Result.R.Negative])</t>
+  </si>
+  <si>
+    <t>[HTS_TST.N.Emergency Ward/Age/Sex/Result.R.Positive]%/%([HTS_TST.N.Emergency Ward/Age/Sex/Result.R.Positive]+[HTS_TST.N.Emergency Ward/Age/Sex/Result.R.Negative])</t>
+  </si>
+  <si>
+    <t>[HTS_TST.N.Inpat/Age/Sex/Result.R.Positive]%/%([HTS_TST.N.Inpat/Age/Sex/Result.R.Positive]+[HTS_TST.N.Inpat/Age/Sex/Result.R.Negative])</t>
+  </si>
+  <si>
+    <t>[HTS_TST.N.Malnutrition/Age/Sex/Result.R.Positive]%/%([HTS_TST.N.Malnutrition/Age/Sex/Result.R.Positive]+[HTS_TST.N.Malnutrition/Age/Sex/Result.R.Negative])</t>
+  </si>
+  <si>
+    <t>[HTS_TST.N.Pediatric/Age/Sex/Result.R.Positive]%/%([HTS_TST.N.Pediatric/Age/Sex/Result.R.Positive]+[HTS_TST.N.Pediatric/Age/Sex/Result.R.Negative])</t>
+  </si>
+  <si>
+    <t>[HTS_TST.N.STI Clinic/Age/Sex/Result.R.Positive]%/%([HTS_TST.N.STI Clinic/Age/Sex/Result.R.Positive]+[HTS_TST.N.STI Clinic/Age/Sex/Result.R.Negative])</t>
+  </si>
+  <si>
+    <t>[HTS_TST.N.VCT/Age/Sex/Result.R.Positive]%/%([HTS_TST.N.VCT/Age/Sex/Result.R.Positive]+[HTS_TST.N.VCT/Age/Sex/Result.R.Negative])</t>
+  </si>
+  <si>
+    <t>[HTS_TST.N.OtherPITC/Age/Sex/Result.R.Positive]%/%([HTS_TST.N.OtherPITC/Age/Sex/Result.R.Positive]+[HTS_TST.N.OtherPITC/Age/Sex/Result.R.Negative])</t>
+  </si>
+  <si>
+    <t>[HTS_TST.N.PMTCTPostANC1/Age/Sex/Result.R.Positive]%/%([HTS_TST.N.PMTCTPostANC1/Age/Sex/Result.R.Positive]+[HTS_TST.N.PMTCTPostANC1/Age/Sex/Result.R.Negative])</t>
+  </si>
+  <si>
+    <t>([HTS_SELF.N.Age/Sex/HIVSelfTest.T_1]-[HTS_SELF.N.Age/Sex/HIVSelfTest.R])%/%[HTS_SELF.N.Age/Sex/HIVSelfTest.R]</t>
+  </si>
+  <si>
+    <t>[TX_TB.D.TBScreen/NewExistingART/HIVStatus.R.Life-long ART/New/TB Screen - Positive/Positive]%/%([TX_TB.D.TBScreen/NewExistingART/HIVStatus.R.Life-long ART/New/TB Screen - Positive/Positive]+[TX_TB.D.TBScreen/NewExistingART/HIVStatus.R.Life-long ART/New/TB Screen - Negative/Positive])</t>
+  </si>
+  <si>
+    <t>[TX_TB.D.TBScreen/NewExistingART/HIVStatus.R.Life-long ART/Already/TB Screen - Positive/Positive]%/%([TX_TB.D.TBScreen/NewExistingART/HIVStatus.R.Life-long ART/Already/TB Screen - Positive/Positive]+[TX_TB.D.TBScreen/NewExistingART/HIVStatus.R.Life-long ART/Already/TB Screen - Negative/Positive])</t>
+  </si>
+  <si>
+    <t>([OVC_SERV.N.Age/Sex.T_1]-[OVC_SERV.N.Age/Sex.R])%/%[OVC_SERV.N.Age/Sex.R]</t>
+  </si>
+  <si>
+    <t>([PP_PREV.N.Age/Sex.T_1]-[PP_PREV.N.Age/Sex.R])%/%[PP_PREV.N.Age/Sex.R]</t>
+  </si>
+  <si>
+    <t>([GEND_GBV.N.Age/Sex/ViolenceType.T_1]-[GEND_GBV.N.Age/Sex/ViolenceType.R])%/%[GEND_GBV.N.Age/Sex/ViolenceType.R]</t>
   </si>
 </sst>
 </file>
@@ -2414,10 +2414,10 @@
   <dimension ref="A1:AK62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2460,7 +2460,7 @@
         <v>420</v>
       </c>
       <c r="H1" t="s">
-        <v>579</v>
+        <v>527</v>
       </c>
       <c r="I1" t="s">
         <v>223</v>
@@ -2502,7 +2502,7 @@
         <v>162</v>
       </c>
       <c r="V1" t="s">
-        <v>606</v>
+        <v>554</v>
       </c>
       <c r="W1" t="s">
         <v>224</v>
@@ -2555,13 +2555,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>637</v>
+        <v>583</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>457</v>
+        <v>598</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -2573,13 +2573,13 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>580</v>
+        <v>528</v>
       </c>
       <c r="I2" t="s">
         <v>61</v>
       </c>
       <c r="J2" t="s">
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="K2" t="s">
         <v>140</v>
@@ -2674,7 +2674,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>458</v>
+        <v>613</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
@@ -2686,7 +2686,7 @@
         <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>581</v>
+        <v>529</v>
       </c>
       <c r="I3" t="s">
         <v>62</v>
@@ -2787,7 +2787,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>459</v>
+        <v>614</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
@@ -2799,10 +2799,10 @@
         <v>143</v>
       </c>
       <c r="H4" t="s">
-        <v>582</v>
+        <v>530</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>510</v>
+        <v>458</v>
       </c>
       <c r="J4" t="s">
         <v>139</v>
@@ -2817,7 +2817,7 @@
         <v>143</v>
       </c>
       <c r="N4" t="s">
-        <v>564</v>
+        <v>512</v>
       </c>
       <c r="O4" t="s">
         <v>143</v>
@@ -2900,7 +2900,7 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>508</v>
+        <v>615</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
@@ -2912,7 +2912,7 @@
         <v>9</v>
       </c>
       <c r="H5" t="s">
-        <v>583</v>
+        <v>531</v>
       </c>
       <c r="I5" t="s">
         <v>63</v>
@@ -3013,7 +3013,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>460</v>
+        <v>616</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -3025,7 +3025,7 @@
         <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>584</v>
+        <v>532</v>
       </c>
       <c r="I6" t="s">
         <v>64</v>
@@ -3120,13 +3120,13 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>638</v>
+        <v>584</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>461</v>
+        <v>599</v>
       </c>
       <c r="E7" t="s">
         <v>3</v>
@@ -3138,13 +3138,13 @@
         <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>585</v>
+        <v>533</v>
       </c>
       <c r="I7" t="s">
         <v>65</v>
       </c>
       <c r="J7" t="s">
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="K7" t="s">
         <v>149</v>
@@ -3239,7 +3239,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>462</v>
+        <v>617</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
@@ -3251,13 +3251,13 @@
         <v>12</v>
       </c>
       <c r="H8" t="s">
-        <v>585</v>
+        <v>533</v>
       </c>
       <c r="I8" t="s">
         <v>65</v>
       </c>
       <c r="J8" t="s">
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="K8" t="s">
         <v>149</v>
@@ -3293,7 +3293,7 @@
         <v>66</v>
       </c>
       <c r="V8" t="s">
-        <v>607</v>
+        <v>555</v>
       </c>
       <c r="W8" t="s">
         <v>67</v>
@@ -3352,7 +3352,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>463</v>
+        <v>618</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
@@ -3364,7 +3364,7 @@
         <v>14</v>
       </c>
       <c r="H9" t="s">
-        <v>586</v>
+        <v>534</v>
       </c>
       <c r="I9" t="s">
         <v>68</v>
@@ -3465,7 +3465,7 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>464</v>
+        <v>619</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
@@ -3477,10 +3477,10 @@
         <v>143</v>
       </c>
       <c r="H10" t="s">
-        <v>582</v>
+        <v>530</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>510</v>
+        <v>458</v>
       </c>
       <c r="J10" t="s">
         <v>139</v>
@@ -3495,7 +3495,7 @@
         <v>143</v>
       </c>
       <c r="N10" t="s">
-        <v>567</v>
+        <v>515</v>
       </c>
       <c r="O10" t="s">
         <v>143</v>
@@ -3572,13 +3572,13 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>639</v>
+        <v>585</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>465</v>
+        <v>600</v>
       </c>
       <c r="E11" t="s">
         <v>3</v>
@@ -3587,16 +3587,16 @@
         <v>142</v>
       </c>
       <c r="G11" t="s">
-        <v>577</v>
+        <v>525</v>
       </c>
       <c r="H11" t="s">
-        <v>587</v>
+        <v>535</v>
       </c>
       <c r="I11" t="s">
-        <v>578</v>
+        <v>526</v>
       </c>
       <c r="J11" t="s">
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="K11" t="s">
         <v>140</v>
@@ -3691,7 +3691,7 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>466</v>
+        <v>620</v>
       </c>
       <c r="E12" t="s">
         <v>6</v>
@@ -3703,10 +3703,10 @@
         <v>143</v>
       </c>
       <c r="H12" t="s">
-        <v>582</v>
+        <v>530</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>510</v>
+        <v>458</v>
       </c>
       <c r="J12" t="s">
         <v>139</v>
@@ -3721,7 +3721,7 @@
         <v>143</v>
       </c>
       <c r="N12" t="s">
-        <v>563</v>
+        <v>511</v>
       </c>
       <c r="O12" t="s">
         <v>143</v>
@@ -3804,7 +3804,7 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>467</v>
+        <v>621</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
@@ -3813,13 +3813,13 @@
         <v>144</v>
       </c>
       <c r="G13" t="s">
-        <v>512</v>
+        <v>460</v>
       </c>
       <c r="H13" t="s">
-        <v>588</v>
+        <v>536</v>
       </c>
       <c r="I13" t="s">
-        <v>513</v>
+        <v>461</v>
       </c>
       <c r="J13" t="s">
         <v>139</v>
@@ -3911,13 +3911,13 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>640</v>
+        <v>586</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>468</v>
+        <v>601</v>
       </c>
       <c r="E14" t="s">
         <v>3</v>
@@ -3929,13 +3929,13 @@
         <v>20</v>
       </c>
       <c r="H14" t="s">
-        <v>589</v>
+        <v>537</v>
       </c>
       <c r="I14" t="s">
         <v>69</v>
       </c>
       <c r="J14" t="s">
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="K14" t="s">
         <v>149</v>
@@ -4030,7 +4030,7 @@
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>469</v>
+        <v>622</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
@@ -4042,10 +4042,10 @@
         <v>143</v>
       </c>
       <c r="H15" t="s">
-        <v>582</v>
+        <v>530</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>510</v>
+        <v>458</v>
       </c>
       <c r="J15" t="s">
         <v>139</v>
@@ -4143,7 +4143,7 @@
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>469</v>
+        <v>622</v>
       </c>
       <c r="E16" t="s">
         <v>6</v>
@@ -4155,10 +4155,10 @@
         <v>143</v>
       </c>
       <c r="H16" t="s">
-        <v>582</v>
+        <v>530</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>510</v>
+        <v>458</v>
       </c>
       <c r="J16" t="s">
         <v>139</v>
@@ -4256,7 +4256,7 @@
         <v>5</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>470</v>
+        <v>623</v>
       </c>
       <c r="E17" t="s">
         <v>6</v>
@@ -4268,10 +4268,10 @@
         <v>143</v>
       </c>
       <c r="H17" t="s">
-        <v>590</v>
+        <v>538</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>511</v>
+        <v>459</v>
       </c>
       <c r="J17" t="s">
         <v>139</v>
@@ -4310,10 +4310,10 @@
         <v>143</v>
       </c>
       <c r="V17" t="s">
-        <v>590</v>
+        <v>538</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>511</v>
+        <v>459</v>
       </c>
       <c r="X17" t="s">
         <v>139</v>
@@ -4369,7 +4369,7 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>471</v>
+        <v>624</v>
       </c>
       <c r="E18" t="s">
         <v>6</v>
@@ -4381,10 +4381,10 @@
         <v>143</v>
       </c>
       <c r="H18" t="s">
-        <v>590</v>
+        <v>538</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>511</v>
+        <v>459</v>
       </c>
       <c r="J18" t="s">
         <v>139</v>
@@ -4423,10 +4423,10 @@
         <v>143</v>
       </c>
       <c r="V18" t="s">
-        <v>590</v>
+        <v>538</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>511</v>
+        <v>459</v>
       </c>
       <c r="X18" t="s">
         <v>139</v>
@@ -4482,7 +4482,7 @@
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>472</v>
+        <v>625</v>
       </c>
       <c r="E19" t="s">
         <v>6</v>
@@ -4494,10 +4494,10 @@
         <v>143</v>
       </c>
       <c r="H19" t="s">
-        <v>590</v>
+        <v>538</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>511</v>
+        <v>459</v>
       </c>
       <c r="J19" t="s">
         <v>139</v>
@@ -4536,10 +4536,10 @@
         <v>143</v>
       </c>
       <c r="V19" t="s">
-        <v>590</v>
+        <v>538</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>511</v>
+        <v>459</v>
       </c>
       <c r="X19" t="s">
         <v>139</v>
@@ -4595,7 +4595,7 @@
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>473</v>
+        <v>626</v>
       </c>
       <c r="E20" t="s">
         <v>6</v>
@@ -4607,10 +4607,10 @@
         <v>143</v>
       </c>
       <c r="H20" t="s">
-        <v>590</v>
+        <v>538</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>511</v>
+        <v>459</v>
       </c>
       <c r="J20" t="s">
         <v>139</v>
@@ -4649,10 +4649,10 @@
         <v>143</v>
       </c>
       <c r="V20" t="s">
-        <v>590</v>
+        <v>538</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>511</v>
+        <v>459</v>
       </c>
       <c r="X20" t="s">
         <v>139</v>
@@ -4708,7 +4708,7 @@
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>474</v>
+        <v>627</v>
       </c>
       <c r="E21" t="s">
         <v>6</v>
@@ -4720,10 +4720,10 @@
         <v>143</v>
       </c>
       <c r="H21" t="s">
-        <v>590</v>
+        <v>538</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>511</v>
+        <v>459</v>
       </c>
       <c r="J21" t="s">
         <v>139</v>
@@ -4762,10 +4762,10 @@
         <v>143</v>
       </c>
       <c r="V21" t="s">
-        <v>590</v>
+        <v>538</v>
       </c>
       <c r="W21" s="1" t="s">
-        <v>511</v>
+        <v>459</v>
       </c>
       <c r="X21" t="s">
         <v>139</v>
@@ -4821,7 +4821,7 @@
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>475</v>
+        <v>628</v>
       </c>
       <c r="E22" t="s">
         <v>6</v>
@@ -4833,10 +4833,10 @@
         <v>143</v>
       </c>
       <c r="H22" t="s">
-        <v>590</v>
+        <v>538</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>511</v>
+        <v>459</v>
       </c>
       <c r="J22" t="s">
         <v>139</v>
@@ -4875,10 +4875,10 @@
         <v>143</v>
       </c>
       <c r="V22" t="s">
-        <v>590</v>
+        <v>538</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>511</v>
+        <v>459</v>
       </c>
       <c r="X22" t="s">
         <v>139</v>
@@ -4934,7 +4934,7 @@
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>476</v>
+        <v>629</v>
       </c>
       <c r="E23" t="s">
         <v>6</v>
@@ -4946,10 +4946,10 @@
         <v>143</v>
       </c>
       <c r="H23" t="s">
-        <v>590</v>
+        <v>538</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>511</v>
+        <v>459</v>
       </c>
       <c r="J23" t="s">
         <v>139</v>
@@ -4988,10 +4988,10 @@
         <v>143</v>
       </c>
       <c r="V23" t="s">
-        <v>590</v>
+        <v>538</v>
       </c>
       <c r="W23" s="1" t="s">
-        <v>511</v>
+        <v>459</v>
       </c>
       <c r="X23" t="s">
         <v>139</v>
@@ -5047,7 +5047,7 @@
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>477</v>
+        <v>630</v>
       </c>
       <c r="E24" t="s">
         <v>6</v>
@@ -5059,10 +5059,10 @@
         <v>143</v>
       </c>
       <c r="H24" t="s">
-        <v>590</v>
+        <v>538</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>511</v>
+        <v>459</v>
       </c>
       <c r="J24" t="s">
         <v>139</v>
@@ -5101,10 +5101,10 @@
         <v>143</v>
       </c>
       <c r="V24" t="s">
-        <v>590</v>
+        <v>538</v>
       </c>
       <c r="W24" s="1" t="s">
-        <v>511</v>
+        <v>459</v>
       </c>
       <c r="X24" t="s">
         <v>139</v>
@@ -5160,7 +5160,7 @@
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>478</v>
+        <v>631</v>
       </c>
       <c r="E25" t="s">
         <v>6</v>
@@ -5172,10 +5172,10 @@
         <v>143</v>
       </c>
       <c r="H25" t="s">
-        <v>590</v>
+        <v>538</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>511</v>
+        <v>459</v>
       </c>
       <c r="J25" t="s">
         <v>139</v>
@@ -5214,10 +5214,10 @@
         <v>143</v>
       </c>
       <c r="V25" t="s">
-        <v>590</v>
+        <v>538</v>
       </c>
       <c r="W25" s="1" t="s">
-        <v>511</v>
+        <v>459</v>
       </c>
       <c r="X25" t="s">
         <v>139</v>
@@ -5273,7 +5273,7 @@
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>479</v>
+        <v>632</v>
       </c>
       <c r="E26" t="s">
         <v>6</v>
@@ -5285,10 +5285,10 @@
         <v>143</v>
       </c>
       <c r="H26" t="s">
-        <v>590</v>
+        <v>538</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>511</v>
+        <v>459</v>
       </c>
       <c r="J26" t="s">
         <v>139</v>
@@ -5327,10 +5327,10 @@
         <v>143</v>
       </c>
       <c r="V26" t="s">
-        <v>590</v>
+        <v>538</v>
       </c>
       <c r="W26" s="1" t="s">
-        <v>511</v>
+        <v>459</v>
       </c>
       <c r="X26" t="s">
         <v>139</v>
@@ -5386,7 +5386,7 @@
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>480</v>
+        <v>633</v>
       </c>
       <c r="E27" t="s">
         <v>6</v>
@@ -5398,10 +5398,10 @@
         <v>143</v>
       </c>
       <c r="H27" t="s">
-        <v>590</v>
+        <v>538</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>511</v>
+        <v>459</v>
       </c>
       <c r="J27" t="s">
         <v>139</v>
@@ -5440,10 +5440,10 @@
         <v>143</v>
       </c>
       <c r="V27" t="s">
-        <v>590</v>
+        <v>538</v>
       </c>
       <c r="W27" s="1" t="s">
-        <v>511</v>
+        <v>459</v>
       </c>
       <c r="X27" t="s">
         <v>139</v>
@@ -5499,7 +5499,7 @@
         <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>481</v>
+        <v>634</v>
       </c>
       <c r="E28" t="s">
         <v>6</v>
@@ -5511,10 +5511,10 @@
         <v>143</v>
       </c>
       <c r="H28" t="s">
-        <v>582</v>
+        <v>530</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>510</v>
+        <v>458</v>
       </c>
       <c r="J28" t="s">
         <v>139</v>
@@ -5612,7 +5612,7 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>482</v>
+        <v>635</v>
       </c>
       <c r="E29" t="s">
         <v>6</v>
@@ -5624,10 +5624,10 @@
         <v>143</v>
       </c>
       <c r="H29" t="s">
-        <v>582</v>
+        <v>530</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>510</v>
+        <v>458</v>
       </c>
       <c r="J29" t="s">
         <v>139</v>
@@ -5725,7 +5725,7 @@
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>483</v>
+        <v>636</v>
       </c>
       <c r="E30" t="s">
         <v>6</v>
@@ -5737,10 +5737,10 @@
         <v>143</v>
       </c>
       <c r="H30" t="s">
-        <v>582</v>
+        <v>530</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>510</v>
+        <v>458</v>
       </c>
       <c r="J30" t="s">
         <v>139</v>
@@ -5838,7 +5838,7 @@
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>484</v>
+        <v>637</v>
       </c>
       <c r="E31" t="s">
         <v>6</v>
@@ -5850,10 +5850,10 @@
         <v>143</v>
       </c>
       <c r="H31" t="s">
-        <v>582</v>
+        <v>530</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>510</v>
+        <v>458</v>
       </c>
       <c r="J31" t="s">
         <v>139</v>
@@ -5951,7 +5951,7 @@
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>485</v>
+        <v>638</v>
       </c>
       <c r="E32" t="s">
         <v>6</v>
@@ -5963,10 +5963,10 @@
         <v>143</v>
       </c>
       <c r="H32" t="s">
-        <v>582</v>
+        <v>530</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>510</v>
+        <v>458</v>
       </c>
       <c r="J32" t="s">
         <v>139</v>
@@ -6064,7 +6064,7 @@
         <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>486</v>
+        <v>639</v>
       </c>
       <c r="E33" t="s">
         <v>6</v>
@@ -6076,10 +6076,10 @@
         <v>143</v>
       </c>
       <c r="H33" t="s">
-        <v>582</v>
+        <v>530</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>510</v>
+        <v>458</v>
       </c>
       <c r="J33" t="s">
         <v>139</v>
@@ -6177,7 +6177,7 @@
         <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>487</v>
+        <v>640</v>
       </c>
       <c r="E34" t="s">
         <v>6</v>
@@ -6189,10 +6189,10 @@
         <v>143</v>
       </c>
       <c r="H34" t="s">
-        <v>582</v>
+        <v>530</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>510</v>
+        <v>458</v>
       </c>
       <c r="J34" t="s">
         <v>139</v>
@@ -6290,7 +6290,7 @@
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>488</v>
+        <v>641</v>
       </c>
       <c r="E35" t="s">
         <v>6</v>
@@ -6302,10 +6302,10 @@
         <v>143</v>
       </c>
       <c r="H35" t="s">
-        <v>582</v>
+        <v>530</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>510</v>
+        <v>458</v>
       </c>
       <c r="J35" t="s">
         <v>139</v>
@@ -6403,7 +6403,7 @@
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>489</v>
+        <v>642</v>
       </c>
       <c r="E36" t="s">
         <v>6</v>
@@ -6415,10 +6415,10 @@
         <v>143</v>
       </c>
       <c r="H36" t="s">
-        <v>582</v>
+        <v>530</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>510</v>
+        <v>458</v>
       </c>
       <c r="J36" t="s">
         <v>139</v>
@@ -6516,7 +6516,7 @@
         <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>490</v>
+        <v>643</v>
       </c>
       <c r="E37" t="s">
         <v>6</v>
@@ -6528,10 +6528,10 @@
         <v>143</v>
       </c>
       <c r="H37" t="s">
-        <v>582</v>
+        <v>530</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>510</v>
+        <v>458</v>
       </c>
       <c r="J37" t="s">
         <v>139</v>
@@ -6623,13 +6623,13 @@
         <v>21</v>
       </c>
       <c r="B38" t="s">
-        <v>622</v>
+        <v>570</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
       </c>
       <c r="D38" t="s">
-        <v>623</v>
+        <v>644</v>
       </c>
       <c r="E38" t="s">
         <v>6</v>
@@ -6641,10 +6641,10 @@
         <v>143</v>
       </c>
       <c r="H38" t="s">
-        <v>582</v>
+        <v>530</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>510</v>
+        <v>458</v>
       </c>
       <c r="J38" t="s">
         <v>139</v>
@@ -6659,7 +6659,7 @@
         <v>143</v>
       </c>
       <c r="N38" t="s">
-        <v>625</v>
+        <v>572</v>
       </c>
       <c r="O38" t="s">
         <v>143</v>
@@ -6736,13 +6736,13 @@
         <v>21</v>
       </c>
       <c r="B39" t="s">
-        <v>641</v>
+        <v>587</v>
       </c>
       <c r="C39" t="s">
         <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>491</v>
+        <v>602</v>
       </c>
       <c r="E39" t="s">
         <v>3</v>
@@ -6754,13 +6754,13 @@
         <v>143</v>
       </c>
       <c r="H39" t="s">
-        <v>591</v>
+        <v>539</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>568</v>
+        <v>516</v>
       </c>
       <c r="J39" t="s">
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="K39" t="s">
         <v>140</v>
@@ -6849,13 +6849,13 @@
         <v>21</v>
       </c>
       <c r="B40" t="s">
-        <v>642</v>
+        <v>588</v>
       </c>
       <c r="C40" t="s">
         <v>2</v>
       </c>
       <c r="D40" t="s">
-        <v>492</v>
+        <v>603</v>
       </c>
       <c r="E40" t="s">
         <v>3</v>
@@ -6867,19 +6867,19 @@
         <v>143</v>
       </c>
       <c r="H40" t="s">
-        <v>592</v>
+        <v>540</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>569</v>
+        <v>517</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="K40" t="s">
-        <v>570</v>
+        <v>518</v>
       </c>
       <c r="L40" t="s">
-        <v>574</v>
+        <v>522</v>
       </c>
       <c r="M40" t="s">
         <v>143</v>
@@ -6968,7 +6968,7 @@
         <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>493</v>
+        <v>645</v>
       </c>
       <c r="E41" t="s">
         <v>6</v>
@@ -6980,13 +6980,13 @@
         <v>178</v>
       </c>
       <c r="H41" t="s">
-        <v>593</v>
+        <v>541</v>
       </c>
       <c r="I41" t="s">
         <v>177</v>
       </c>
       <c r="J41" t="s">
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="K41" t="s">
         <v>140</v>
@@ -7022,7 +7022,7 @@
         <v>180</v>
       </c>
       <c r="V41" t="s">
-        <v>608</v>
+        <v>556</v>
       </c>
       <c r="W41" t="s">
         <v>179</v>
@@ -7081,7 +7081,7 @@
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>494</v>
+        <v>646</v>
       </c>
       <c r="E42" t="s">
         <v>6</v>
@@ -7090,13 +7090,13 @@
         <v>144</v>
       </c>
       <c r="G42" t="s">
-        <v>520</v>
+        <v>468</v>
       </c>
       <c r="H42" t="s">
-        <v>594</v>
+        <v>542</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>519</v>
+        <v>467</v>
       </c>
       <c r="J42" t="s">
         <v>139</v>
@@ -7194,7 +7194,7 @@
         <v>5</v>
       </c>
       <c r="D43" t="s">
-        <v>495</v>
+        <v>647</v>
       </c>
       <c r="E43" t="s">
         <v>6</v>
@@ -7203,13 +7203,13 @@
         <v>144</v>
       </c>
       <c r="G43" t="s">
-        <v>521</v>
+        <v>469</v>
       </c>
       <c r="H43" t="s">
-        <v>595</v>
+        <v>543</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>522</v>
+        <v>470</v>
       </c>
       <c r="J43" t="s">
         <v>139</v>
@@ -7301,13 +7301,13 @@
         <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>643</v>
+        <v>589</v>
       </c>
       <c r="C44" t="s">
         <v>2</v>
       </c>
       <c r="D44" t="s">
-        <v>496</v>
+        <v>604</v>
       </c>
       <c r="E44" t="s">
         <v>3</v>
@@ -7316,16 +7316,16 @@
         <v>142</v>
       </c>
       <c r="G44" t="s">
-        <v>516</v>
+        <v>464</v>
       </c>
       <c r="H44" t="s">
-        <v>596</v>
+        <v>544</v>
       </c>
       <c r="I44" t="s">
-        <v>517</v>
+        <v>465</v>
       </c>
       <c r="J44" t="s">
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="K44" t="s">
         <v>229</v>
@@ -7420,7 +7420,7 @@
         <v>5</v>
       </c>
       <c r="D45" t="s">
-        <v>497</v>
+        <v>648</v>
       </c>
       <c r="E45" t="s">
         <v>6</v>
@@ -7429,16 +7429,16 @@
         <v>142</v>
       </c>
       <c r="G45" t="s">
-        <v>516</v>
+        <v>464</v>
       </c>
       <c r="H45" t="s">
-        <v>596</v>
+        <v>544</v>
       </c>
       <c r="I45" t="s">
-        <v>517</v>
+        <v>465</v>
       </c>
       <c r="J45" t="s">
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="K45" t="s">
         <v>229</v>
@@ -7471,13 +7471,13 @@
         <v>143</v>
       </c>
       <c r="U45" t="s">
-        <v>514</v>
+        <v>462</v>
       </c>
       <c r="V45" t="s">
-        <v>609</v>
+        <v>557</v>
       </c>
       <c r="W45" t="s">
-        <v>515</v>
+        <v>463</v>
       </c>
       <c r="X45" s="1" t="s">
         <v>139</v>
@@ -7527,13 +7527,13 @@
         <v>48</v>
       </c>
       <c r="B46" t="s">
-        <v>613</v>
+        <v>561</v>
       </c>
       <c r="C46" t="s">
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>498</v>
+        <v>605</v>
       </c>
       <c r="E46" t="s">
         <v>3</v>
@@ -7545,13 +7545,13 @@
         <v>49</v>
       </c>
       <c r="H46" t="s">
-        <v>597</v>
+        <v>545</v>
       </c>
       <c r="I46" t="s">
         <v>70</v>
       </c>
       <c r="J46" t="s">
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="K46" t="s">
         <v>143</v>
@@ -7640,13 +7640,13 @@
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>644</v>
+        <v>590</v>
       </c>
       <c r="C47" t="s">
         <v>2</v>
       </c>
       <c r="D47" t="s">
-        <v>499</v>
+        <v>606</v>
       </c>
       <c r="E47" t="s">
         <v>3</v>
@@ -7658,13 +7658,13 @@
         <v>71</v>
       </c>
       <c r="H47" t="s">
-        <v>598</v>
+        <v>546</v>
       </c>
       <c r="I47" t="s">
         <v>72</v>
       </c>
       <c r="J47" t="s">
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="K47" t="s">
         <v>143</v>
@@ -7753,13 +7753,13 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>645</v>
+        <v>591</v>
       </c>
       <c r="C48" t="s">
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>500</v>
+        <v>607</v>
       </c>
       <c r="E48" t="s">
         <v>3</v>
@@ -7771,13 +7771,13 @@
         <v>71</v>
       </c>
       <c r="H48" t="s">
-        <v>598</v>
+        <v>546</v>
       </c>
       <c r="I48" t="s">
         <v>72</v>
       </c>
       <c r="J48" t="s">
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="K48" t="s">
         <v>143</v>
@@ -7866,13 +7866,13 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>646</v>
+        <v>592</v>
       </c>
       <c r="C49" t="s">
         <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>501</v>
+        <v>608</v>
       </c>
       <c r="E49" t="s">
         <v>3</v>
@@ -7884,13 +7884,13 @@
         <v>50</v>
       </c>
       <c r="H49" t="s">
-        <v>599</v>
+        <v>547</v>
       </c>
       <c r="I49" t="s">
         <v>73</v>
       </c>
       <c r="J49" t="s">
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="K49" t="s">
         <v>143</v>
@@ -7979,13 +7979,13 @@
         <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>647</v>
+        <v>593</v>
       </c>
       <c r="C50" t="s">
         <v>2</v>
       </c>
       <c r="D50" t="s">
-        <v>502</v>
+        <v>609</v>
       </c>
       <c r="E50" t="s">
         <v>3</v>
@@ -7997,13 +7997,13 @@
         <v>53</v>
       </c>
       <c r="H50" t="s">
-        <v>600</v>
+        <v>548</v>
       </c>
       <c r="I50" t="s">
         <v>75</v>
       </c>
       <c r="J50" t="s">
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="K50" t="s">
         <v>140</v>
@@ -8098,7 +8098,7 @@
         <v>5</v>
       </c>
       <c r="D51" t="s">
-        <v>503</v>
+        <v>649</v>
       </c>
       <c r="E51" t="s">
         <v>6</v>
@@ -8110,13 +8110,13 @@
         <v>53</v>
       </c>
       <c r="H51" t="s">
-        <v>600</v>
+        <v>548</v>
       </c>
       <c r="I51" t="s">
         <v>75</v>
       </c>
       <c r="J51" t="s">
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="K51" t="s">
         <v>140</v>
@@ -8152,7 +8152,7 @@
         <v>181</v>
       </c>
       <c r="V51" t="s">
-        <v>610</v>
+        <v>558</v>
       </c>
       <c r="W51" t="s">
         <v>182</v>
@@ -8205,13 +8205,13 @@
         <v>55</v>
       </c>
       <c r="B52" t="s">
-        <v>648</v>
+        <v>594</v>
       </c>
       <c r="C52" t="s">
         <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>504</v>
+        <v>610</v>
       </c>
       <c r="E52" t="s">
         <v>3</v>
@@ -8223,13 +8223,13 @@
         <v>56</v>
       </c>
       <c r="H52" t="s">
-        <v>601</v>
+        <v>549</v>
       </c>
       <c r="I52" t="s">
         <v>76</v>
       </c>
       <c r="J52" t="s">
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="K52" t="s">
         <v>155</v>
@@ -8318,13 +8318,13 @@
         <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>649</v>
+        <v>595</v>
       </c>
       <c r="C53" t="s">
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>627</v>
+        <v>597</v>
       </c>
       <c r="E53" t="s">
         <v>3</v>
@@ -8333,16 +8333,16 @@
         <v>142</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>628</v>
+        <v>574</v>
       </c>
       <c r="H53" t="s">
-        <v>629</v>
+        <v>575</v>
       </c>
       <c r="I53" t="s">
-        <v>630</v>
+        <v>576</v>
       </c>
       <c r="J53" t="s">
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="K53" t="s">
         <v>155</v>
@@ -8431,13 +8431,13 @@
         <v>57</v>
       </c>
       <c r="B54" t="s">
-        <v>614</v>
+        <v>562</v>
       </c>
       <c r="C54" t="s">
         <v>2</v>
       </c>
       <c r="D54" t="s">
-        <v>505</v>
+        <v>611</v>
       </c>
       <c r="E54" t="s">
         <v>3</v>
@@ -8449,13 +8449,13 @@
         <v>77</v>
       </c>
       <c r="H54" t="s">
-        <v>602</v>
+        <v>550</v>
       </c>
       <c r="I54" t="s">
         <v>78</v>
       </c>
       <c r="J54" t="s">
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="K54" t="s">
         <v>143</v>
@@ -8544,13 +8544,13 @@
         <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>636</v>
+        <v>582</v>
       </c>
       <c r="C55" t="s">
         <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>506</v>
+        <v>612</v>
       </c>
       <c r="E55" t="s">
         <v>3</v>
@@ -8562,13 +8562,13 @@
         <v>79</v>
       </c>
       <c r="H55" t="s">
-        <v>603</v>
+        <v>551</v>
       </c>
       <c r="I55" t="s">
         <v>80</v>
       </c>
       <c r="J55" t="s">
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="K55" t="s">
         <v>143</v>
@@ -8663,7 +8663,7 @@
         <v>5</v>
       </c>
       <c r="D56" t="s">
-        <v>507</v>
+        <v>650</v>
       </c>
       <c r="E56" t="s">
         <v>6</v>
@@ -8675,13 +8675,13 @@
         <v>143</v>
       </c>
       <c r="H56" t="s">
-        <v>604</v>
+        <v>552</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>518</v>
+        <v>466</v>
       </c>
       <c r="J56" t="s">
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="K56" t="s">
         <v>143</v>
@@ -8717,7 +8717,7 @@
         <v>227</v>
       </c>
       <c r="V56" t="s">
-        <v>611</v>
+        <v>559</v>
       </c>
       <c r="W56" s="1" t="s">
         <v>228</v>
@@ -8770,7 +8770,7 @@
         <v>48</v>
       </c>
       <c r="B57" t="s">
-        <v>615</v>
+        <v>563</v>
       </c>
       <c r="C57" t="s">
         <v>2</v>
@@ -8788,13 +8788,13 @@
         <v>51</v>
       </c>
       <c r="H57" t="s">
-        <v>605</v>
+        <v>553</v>
       </c>
       <c r="I57" s="14" t="s">
         <v>74</v>
       </c>
       <c r="J57" t="s">
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="K57" t="s">
         <v>143</v>
@@ -8883,7 +8883,7 @@
         <v>48</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>632</v>
+        <v>578</v>
       </c>
       <c r="C58" t="s">
         <v>2</v>
@@ -8898,16 +8898,16 @@
         <v>142</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>633</v>
+        <v>579</v>
       </c>
       <c r="H58" t="s">
-        <v>631</v>
+        <v>577</v>
       </c>
       <c r="I58" s="14" t="s">
-        <v>634</v>
+        <v>580</v>
       </c>
       <c r="J58" t="s">
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="K58" t="s">
         <v>143</v>
@@ -8996,7 +8996,7 @@
         <v>48</v>
       </c>
       <c r="B59" t="s">
-        <v>616</v>
+        <v>564</v>
       </c>
       <c r="C59" t="s">
         <v>2</v>
@@ -9020,7 +9020,7 @@
         <v>453</v>
       </c>
       <c r="J59" t="s">
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="K59" t="s">
         <v>143</v>
@@ -9062,7 +9062,7 @@
         <v>454</v>
       </c>
       <c r="X59" t="s">
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="Y59" t="s">
         <v>143</v>
@@ -9109,7 +9109,7 @@
         <v>450</v>
       </c>
       <c r="B60" t="s">
-        <v>617</v>
+        <v>565</v>
       </c>
       <c r="C60" t="s">
         <v>2</v>
@@ -9133,7 +9133,7 @@
         <v>451</v>
       </c>
       <c r="J60" t="s">
-        <v>612</v>
+        <v>560</v>
       </c>
       <c r="K60" t="s">
         <v>143</v>
@@ -9222,13 +9222,13 @@
         <v>21</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>618</v>
+        <v>566</v>
       </c>
       <c r="C61" t="s">
         <v>5</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>619</v>
+        <v>567</v>
       </c>
       <c r="E61" t="s">
         <v>6</v>
@@ -9240,13 +9240,13 @@
         <v>143</v>
       </c>
       <c r="H61" t="s">
-        <v>591</v>
+        <v>539</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>568</v>
+        <v>516</v>
       </c>
       <c r="J61" t="s">
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="K61" t="s">
         <v>140</v>
@@ -9282,10 +9282,10 @@
         <v>143</v>
       </c>
       <c r="V61" t="s">
-        <v>620</v>
+        <v>568</v>
       </c>
       <c r="W61" t="s">
-        <v>621</v>
+        <v>569</v>
       </c>
       <c r="X61" s="1" t="s">
         <v>139</v>
@@ -9335,13 +9335,13 @@
         <v>21</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>650</v>
+        <v>596</v>
       </c>
       <c r="C62" t="s">
         <v>2</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>635</v>
+        <v>581</v>
       </c>
       <c r="E62" t="s">
         <v>3</v>
@@ -9353,7 +9353,7 @@
         <v>180</v>
       </c>
       <c r="H62" t="s">
-        <v>608</v>
+        <v>556</v>
       </c>
       <c r="I62" t="s">
         <v>179</v>
@@ -9783,13 +9783,13 @@
         <v>233</v>
       </c>
       <c r="C7" t="s">
-        <v>523</v>
+        <v>471</v>
       </c>
       <c r="D7" t="s">
         <v>217</v>
       </c>
       <c r="E7" t="s">
-        <v>524</v>
+        <v>472</v>
       </c>
       <c r="F7" t="s">
         <v>97</v>
@@ -9958,13 +9958,13 @@
         <v>233</v>
       </c>
       <c r="C11" t="s">
-        <v>525</v>
+        <v>473</v>
       </c>
       <c r="D11" t="s">
         <v>217</v>
       </c>
       <c r="E11" t="s">
-        <v>526</v>
+        <v>474</v>
       </c>
       <c r="F11" t="s">
         <v>98</v>
@@ -10535,13 +10535,13 @@
         <v>233</v>
       </c>
       <c r="C25" t="s">
-        <v>527</v>
+        <v>475</v>
       </c>
       <c r="D25" t="s">
         <v>217</v>
       </c>
       <c r="E25" t="s">
-        <v>528</v>
+        <v>476</v>
       </c>
       <c r="F25" t="s">
         <v>230</v>
@@ -11281,13 +11281,13 @@
         <v>233</v>
       </c>
       <c r="C43" t="s">
-        <v>529</v>
+        <v>477</v>
       </c>
       <c r="D43" t="s">
         <v>217</v>
       </c>
       <c r="E43" t="s">
-        <v>530</v>
+        <v>478</v>
       </c>
       <c r="F43" t="s">
         <v>103</v>
@@ -11497,13 +11497,13 @@
         <v>233</v>
       </c>
       <c r="C48" t="s">
-        <v>531</v>
+        <v>479</v>
       </c>
       <c r="D48" t="s">
         <v>217</v>
       </c>
       <c r="E48" t="s">
-        <v>532</v>
+        <v>480</v>
       </c>
       <c r="F48" t="s">
         <v>104</v>
@@ -14396,19 +14396,19 @@
     </row>
     <row r="126" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>561</v>
+        <v>509</v>
       </c>
       <c r="B126" t="s">
-        <v>562</v>
+        <v>510</v>
       </c>
       <c r="C126" t="s">
-        <v>533</v>
+        <v>481</v>
       </c>
       <c r="D126" t="s">
         <v>436</v>
       </c>
       <c r="E126" t="s">
-        <v>534</v>
+        <v>482</v>
       </c>
       <c r="F126" t="s">
         <v>143</v>
@@ -14432,19 +14432,19 @@
     </row>
     <row r="127" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>561</v>
+        <v>509</v>
       </c>
       <c r="B127" t="s">
-        <v>562</v>
+        <v>510</v>
       </c>
       <c r="C127" t="s">
-        <v>535</v>
+        <v>483</v>
       </c>
       <c r="D127" t="s">
         <v>436</v>
       </c>
       <c r="E127" t="s">
-        <v>536</v>
+        <v>484</v>
       </c>
       <c r="F127" t="s">
         <v>143</v>
@@ -14468,19 +14468,19 @@
     </row>
     <row r="128" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>561</v>
+        <v>509</v>
       </c>
       <c r="B128" t="s">
-        <v>562</v>
+        <v>510</v>
       </c>
       <c r="C128" t="s">
-        <v>537</v>
+        <v>485</v>
       </c>
       <c r="D128" t="s">
         <v>436</v>
       </c>
       <c r="E128" t="s">
-        <v>538</v>
+        <v>486</v>
       </c>
       <c r="F128" t="s">
         <v>143</v>
@@ -14504,19 +14504,19 @@
     </row>
     <row r="129" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>561</v>
+        <v>509</v>
       </c>
       <c r="B129" t="s">
-        <v>562</v>
+        <v>510</v>
       </c>
       <c r="C129" t="s">
-        <v>539</v>
+        <v>487</v>
       </c>
       <c r="D129" t="s">
         <v>436</v>
       </c>
       <c r="E129" t="s">
-        <v>540</v>
+        <v>488</v>
       </c>
       <c r="F129" t="s">
         <v>143</v>
@@ -14540,19 +14540,19 @@
     </row>
     <row r="130" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>561</v>
+        <v>509</v>
       </c>
       <c r="B130" t="s">
-        <v>562</v>
+        <v>510</v>
       </c>
       <c r="C130" t="s">
-        <v>541</v>
+        <v>489</v>
       </c>
       <c r="D130" t="s">
         <v>436</v>
       </c>
       <c r="E130" t="s">
-        <v>542</v>
+        <v>490</v>
       </c>
       <c r="F130" t="s">
         <v>143</v>
@@ -14576,19 +14576,19 @@
     </row>
     <row r="131" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>561</v>
+        <v>509</v>
       </c>
       <c r="B131" t="s">
-        <v>562</v>
+        <v>510</v>
       </c>
       <c r="C131" t="s">
-        <v>543</v>
+        <v>491</v>
       </c>
       <c r="D131" t="s">
         <v>436</v>
       </c>
       <c r="E131" t="s">
-        <v>544</v>
+        <v>492</v>
       </c>
       <c r="F131" t="s">
         <v>143</v>
@@ -14612,19 +14612,19 @@
     </row>
     <row r="132" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>561</v>
+        <v>509</v>
       </c>
       <c r="B132" t="s">
-        <v>562</v>
+        <v>510</v>
       </c>
       <c r="C132" t="s">
-        <v>545</v>
+        <v>493</v>
       </c>
       <c r="D132" t="s">
         <v>436</v>
       </c>
       <c r="E132" t="s">
-        <v>546</v>
+        <v>494</v>
       </c>
       <c r="F132" t="s">
         <v>143</v>
@@ -14648,19 +14648,19 @@
     </row>
     <row r="133" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>561</v>
+        <v>509</v>
       </c>
       <c r="B133" t="s">
-        <v>562</v>
+        <v>510</v>
       </c>
       <c r="C133" t="s">
-        <v>547</v>
+        <v>495</v>
       </c>
       <c r="D133" t="s">
         <v>436</v>
       </c>
       <c r="E133" t="s">
-        <v>548</v>
+        <v>496</v>
       </c>
       <c r="F133" t="s">
         <v>143</v>
@@ -14684,19 +14684,19 @@
     </row>
     <row r="134" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>561</v>
+        <v>509</v>
       </c>
       <c r="B134" t="s">
-        <v>562</v>
+        <v>510</v>
       </c>
       <c r="C134" t="s">
-        <v>549</v>
+        <v>497</v>
       </c>
       <c r="D134" t="s">
         <v>436</v>
       </c>
       <c r="E134" t="s">
-        <v>550</v>
+        <v>498</v>
       </c>
       <c r="F134" t="s">
         <v>143</v>
@@ -14720,19 +14720,19 @@
     </row>
     <row r="135" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>561</v>
+        <v>509</v>
       </c>
       <c r="B135" t="s">
-        <v>562</v>
+        <v>510</v>
       </c>
       <c r="C135" t="s">
-        <v>551</v>
+        <v>499</v>
       </c>
       <c r="D135" t="s">
         <v>436</v>
       </c>
       <c r="E135" t="s">
-        <v>552</v>
+        <v>500</v>
       </c>
       <c r="F135" t="s">
         <v>143</v>
@@ -14756,19 +14756,19 @@
     </row>
     <row r="136" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>561</v>
+        <v>509</v>
       </c>
       <c r="B136" t="s">
-        <v>562</v>
+        <v>510</v>
       </c>
       <c r="C136" t="s">
-        <v>553</v>
+        <v>501</v>
       </c>
       <c r="D136" t="s">
         <v>436</v>
       </c>
       <c r="E136" t="s">
-        <v>554</v>
+        <v>502</v>
       </c>
       <c r="F136" t="s">
         <v>143</v>
@@ -14792,19 +14792,19 @@
     </row>
     <row r="137" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>561</v>
+        <v>509</v>
       </c>
       <c r="B137" t="s">
-        <v>562</v>
+        <v>510</v>
       </c>
       <c r="C137" t="s">
-        <v>555</v>
+        <v>503</v>
       </c>
       <c r="D137" t="s">
         <v>436</v>
       </c>
       <c r="E137" t="s">
-        <v>556</v>
+        <v>504</v>
       </c>
       <c r="F137" t="s">
         <v>143</v>
@@ -14828,19 +14828,19 @@
     </row>
     <row r="138" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>561</v>
+        <v>509</v>
       </c>
       <c r="B138" t="s">
-        <v>562</v>
+        <v>510</v>
       </c>
       <c r="C138" t="s">
-        <v>557</v>
+        <v>505</v>
       </c>
       <c r="D138" t="s">
         <v>436</v>
       </c>
       <c r="E138" t="s">
-        <v>558</v>
+        <v>506</v>
       </c>
       <c r="F138" t="s">
         <v>143</v>
@@ -14859,24 +14859,24 @@
         <v>hts_mod_fac_vmmc</v>
       </c>
       <c r="AG138" t="s">
-        <v>563</v>
+        <v>511</v>
       </c>
     </row>
     <row r="139" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>561</v>
+        <v>509</v>
       </c>
       <c r="B139" t="s">
-        <v>562</v>
+        <v>510</v>
       </c>
       <c r="C139" t="s">
-        <v>559</v>
+        <v>507</v>
       </c>
       <c r="D139" t="s">
         <v>436</v>
       </c>
       <c r="E139" t="s">
-        <v>560</v>
+        <v>508</v>
       </c>
       <c r="F139" t="s">
         <v>143</v>
@@ -14895,24 +14895,24 @@
         <v>hts_mod_fac_anc_1</v>
       </c>
       <c r="AG139" t="s">
-        <v>564</v>
+        <v>512</v>
       </c>
     </row>
     <row r="140" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>561</v>
+        <v>509</v>
       </c>
       <c r="B140" t="s">
-        <v>562</v>
+        <v>510</v>
       </c>
       <c r="C140" t="s">
-        <v>566</v>
+        <v>514</v>
       </c>
       <c r="D140" t="s">
         <v>436</v>
       </c>
       <c r="E140" t="s">
-        <v>565</v>
+        <v>513</v>
       </c>
       <c r="F140" t="s">
         <v>143</v>
@@ -14931,24 +14931,24 @@
         <v>hts_mod_fac_tb</v>
       </c>
       <c r="AG140" t="s">
-        <v>567</v>
+        <v>515</v>
       </c>
     </row>
     <row r="141" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>561</v>
+        <v>509</v>
       </c>
       <c r="B141" t="s">
-        <v>562</v>
+        <v>510</v>
       </c>
       <c r="C141" t="s">
-        <v>626</v>
+        <v>573</v>
       </c>
       <c r="D141" t="s">
         <v>436</v>
       </c>
       <c r="E141" s="17" t="s">
-        <v>624</v>
+        <v>571</v>
       </c>
       <c r="F141" t="s">
         <v>143</v>
@@ -14967,7 +14967,7 @@
         <v>hts_mod_fac_post_anc_1</v>
       </c>
       <c r="AG141" t="s">
-        <v>625</v>
+        <v>572</v>
       </c>
     </row>
     <row r="142" spans="1:33" x14ac:dyDescent="0.2">
@@ -14978,19 +14978,19 @@
         <v>233</v>
       </c>
       <c r="C142" t="s">
-        <v>571</v>
+        <v>519</v>
       </c>
       <c r="D142" t="s">
         <v>217</v>
       </c>
       <c r="E142" t="s">
-        <v>572</v>
+        <v>520</v>
       </c>
       <c r="F142" t="s">
-        <v>572</v>
+        <v>520</v>
       </c>
       <c r="G142" t="s">
-        <v>573</v>
+        <v>521</v>
       </c>
       <c r="H142">
         <v>3</v>
@@ -15011,7 +15011,7 @@
       <c r="R142" s="9"/>
       <c r="T142" s="9"/>
       <c r="AG142" t="s">
-        <v>570</v>
+        <v>518</v>
       </c>
     </row>
     <row r="143" spans="1:33" x14ac:dyDescent="0.2">
@@ -15031,10 +15031,10 @@
         <v>134</v>
       </c>
       <c r="F143" t="s">
-        <v>575</v>
+        <v>523</v>
       </c>
       <c r="G143" t="s">
-        <v>576</v>
+        <v>524</v>
       </c>
       <c r="H143">
         <v>3</v>
@@ -15047,7 +15047,7 @@
         <v>U_sex</v>
       </c>
       <c r="AG143" t="s">
-        <v>574</v>
+        <v>522</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data required full formula updates
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F73281-FE72-694C-BAF1-E4685ACC7C91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7ADF88E-317D-124A-BD8F-B8907AA8CECC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="7780" yWindow="2020" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3535" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3535" uniqueCount="654">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1739,9 +1739,6 @@
     <t>HTS_SELF.N.directlyAssistedGrowth</t>
   </si>
   <si>
-    <t>(T_1 - R) / R</t>
-  </si>
-  <si>
     <t>FY19 Results HTS_SELF (N, Age/Sex/HIVSelfTest): Directly Assisted</t>
   </si>
   <si>
@@ -1832,9 +1829,6 @@
     <t>[PrEP_CURR.N.Age/Sex.T_1]</t>
   </si>
   <si>
-    <t>[@PMTCT_STAT.D.Age/Sex.T_1]</t>
-  </si>
-  <si>
     <t>[TB_STAT.D.Age/Sex.T_1]</t>
   </si>
   <si>
@@ -1850,9 +1844,6 @@
     <t>[HTS_SELF.N.Age/Sex/HIVSelfTest.T_1.Unassisted]</t>
   </si>
   <si>
-    <t>[OVC_SERV.N.Age/Sex.T_1]</t>
-  </si>
-  <si>
     <t>[KP_MAT.N.Sex.T_1]</t>
   </si>
   <si>
@@ -1874,15 +1865,6 @@
     <t>[GEND_GBV.N.ViolenceServiceType.T_1.Physical_and_or_Emotional_Violence]</t>
   </si>
   <si>
-    <t>[GEND_GBV.N.ViolenceServiceType.T_1.Sexual_Violence__Post_Rape_Care_]</t>
-  </si>
-  <si>
-    <t>[@PMTCT_STAT.N.Age/Sex/KnownNewResult.R.Known_at_Entry_Positive]%/%[@PMTCT_STAT.N.Age/Sex/KnownNewResult.R]</t>
-  </si>
-  <si>
-    <t>[@PMTCT_STAT.N.Age/Sex/KnownNewResult.R.Newly_Identified_Positive]%/%([@PMTCT_STAT.N.Age/Sex/KnownNewResult.R.Newly_Identified_Positive]+[@PMTCT_STAT.N.Age/Sex/KnownNewResult.R.Newly_Identified_Negative])</t>
-  </si>
-  <si>
     <t>[PMTCT_HEI_POS.N.Age/HIVStatus.R.&lt;= 2 months]%/%[PMTCT_EID.N.Age.R.&lt;= 2 months]</t>
   </si>
   <si>
@@ -1901,9 +1883,6 @@
     <t>[VMMC_CIRC.N.HIVStatus/Sex.R.Positive]%/%([VMMC_CIRC.N.HIVStatus/Sex.R.Positive]+[VMMC_CIRC.N.HIVStatus/Sex.R.Negative])</t>
   </si>
   <si>
-    <t>[VMMC_CIRC.N.HIVStatus/Sex.R.Unknown]%/%[VMMC_CIRC.N.HIVStatus/Sex.R]</t>
-  </si>
-  <si>
     <t>([HTS_TST.N.Index/Age/Sex/Result.R.Positive]+[HTS_TST.N.IndexMod/Age/Sex/Result.R.Positive])%/%([HTS_TST.N.Index/Age/Sex/Result.R.Positive]+[HTS_TST.N.IndexMod/Age/Sex/Result.R.Positive]+[HTS_TST.N.Index/Age/Sex/Result.R.Negative]+[HTS_TST.N.IndexMod/Age/Sex/Result.R.Negative])</t>
   </si>
   <si>
@@ -1976,19 +1955,49 @@
     <t>([HTS_SELF.N.Age/Sex/HIVSelfTest.T_1]-[HTS_SELF.N.Age/Sex/HIVSelfTest.R])%/%[HTS_SELF.N.Age/Sex/HIVSelfTest.R]</t>
   </si>
   <si>
-    <t>[TX_TB.D.TBScreen/NewExistingART/HIVStatus.R.Life-long ART/New/TB Screen - Positive/Positive]%/%([TX_TB.D.TBScreen/NewExistingART/HIVStatus.R.Life-long ART/New/TB Screen - Positive/Positive]+[TX_TB.D.TBScreen/NewExistingART/HIVStatus.R.Life-long ART/New/TB Screen - Negative/Positive])</t>
-  </si>
-  <si>
-    <t>[TX_TB.D.TBScreen/NewExistingART/HIVStatus.R.Life-long ART/Already/TB Screen - Positive/Positive]%/%([TX_TB.D.TBScreen/NewExistingART/HIVStatus.R.Life-long ART/Already/TB Screen - Positive/Positive]+[TX_TB.D.TBScreen/NewExistingART/HIVStatus.R.Life-long ART/Already/TB Screen - Negative/Positive])</t>
-  </si>
-  <si>
-    <t>([OVC_SERV.N.Age/Sex.T_1]-[OVC_SERV.N.Age/Sex.R])%/%[OVC_SERV.N.Age/Sex.R]</t>
-  </si>
-  <si>
     <t>([PP_PREV.N.Age/Sex.T_1]-[PP_PREV.N.Age/Sex.R])%/%[PP_PREV.N.Age/Sex.R]</t>
   </si>
   <si>
     <t>([GEND_GBV.N.Age/Sex/ViolenceType.T_1]-[GEND_GBV.N.Age/Sex/ViolenceType.R])%/%[GEND_GBV.N.Age/Sex/ViolenceType.R]</t>
+  </si>
+  <si>
+    <t>[VMMC_CIRC.N.Age/Sex/HIVStatus.R.Unknown]%/%[VMMC_CIRC.N.Age/Sex/HIVStatus.R]</t>
+  </si>
+  <si>
+    <t>([OVC_SERV.N.Age/Sex/ProgramStatus.T_1]-[OVC_SERV.N.Age/Sex/ProgramStatus.R])%/%[OVC_SERV.N.Age/Sex/ProgramStatus.R]</t>
+  </si>
+  <si>
+    <t>[OVC_SERV.N.Age/Sex/ProgramStatus.T_1]</t>
+  </si>
+  <si>
+    <t>[TX_TB.D.Age/Sex/TBScreen/NewExistingART/HIVStatus.R.Life-long ART/New/TB Screen - Positive/Positive]%/%([TX_TB.D.Age/Sex/TBScreen/NewExistingART/HIVStatus.R.Life-long ART/New/TB Screen - Positive/Positive]+[TX_TB.D.Age/Sex/TBScreen/NewExistingART/HIVStatus.R.Life-long ART/New/TB Screen - Negative/Positive])</t>
+  </si>
+  <si>
+    <t>[TX_TB.D.Age/Sex/TBScreen/NewExistingART/HIVStatus.R.Life-long ART/Already/TB Screen - Positive/Positive]%/%([TX_TB.D.Age/Sex/TBScreen/NewExistingART/HIVStatus.R.Life-long ART/Already/TB Screen - Positive/Positive]+[TX_TB.D.Age/Sex/TBScreen/NewExistingART/HIVStatus.R.Life-long ART/Already/TB Screen - Negative/Positive])</t>
+  </si>
+  <si>
+    <t>[PMTCT_STAT.D.Age/Sex.T_1]</t>
+  </si>
+  <si>
+    <t>[PMTCT_STAT.N.Age/Sex/KnownNewResult.R.Known_at_Entry_Positive]%/%[PMTCT_STAT.N.Age/Sex/KnownNewResult.R]</t>
+  </si>
+  <si>
+    <t>[PMTCT_STAT.N.Age/Sex/KnownNewResult.R.Newly_Identified_Positive]%/%([PMTCT_STAT.N.Age/Sex/KnownNewResult.R.Newly_Identified_Positive]+[PMTCT_STAT.N.Age/Sex/KnownNewResult.R.Newly_Identified_Negative])</t>
+  </si>
+  <si>
+    <t>[GEND_GBV.N.ViolenceServiceType.T_1.Sexual_Violence_Post_Rape_Care]</t>
+  </si>
+  <si>
+    <t>[PrEP_NEW.N.KeyPop.T_1]</t>
+  </si>
+  <si>
+    <t>[PrEP_CURR.N.KeyPop.T_1]</t>
+  </si>
+  <si>
+    <t>[IMPATT.PRIORITY_SNU.T_1]</t>
+  </si>
+  <si>
+    <t>([HTS_SELF (N, Age/Sex/HIVSelfTest).T_1] - [HTS_SELF (N, Age/Sex/HIVSelfTest).R]) / [HTS_SELF (N, Age/Sex/HIVSelfTest).R]</t>
   </si>
 </sst>
 </file>
@@ -1998,7 +2007,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2055,6 +2064,12 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2076,7 +2091,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -2097,6 +2112,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2414,10 +2430,10 @@
   <dimension ref="A1:AK62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G62" sqref="G62"/>
+      <selection pane="bottomRight" activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2555,13 +2571,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>598</v>
+        <v>646</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -2674,7 +2690,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>613</v>
+        <v>647</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
@@ -2787,7 +2803,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>614</v>
+        <v>648</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
@@ -2900,7 +2916,7 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
@@ -3013,7 +3029,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -3120,13 +3136,13 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E7" t="s">
         <v>3</v>
@@ -3239,7 +3255,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
@@ -3352,7 +3368,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
@@ -3465,7 +3481,7 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
@@ -3572,13 +3588,13 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="E11" t="s">
         <v>3</v>
@@ -3691,7 +3707,7 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="E12" t="s">
         <v>6</v>
@@ -3804,7 +3820,7 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>621</v>
+        <v>641</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
@@ -3911,13 +3927,13 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="E14" t="s">
         <v>3</v>
@@ -4030,7 +4046,7 @@
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>622</v>
+        <v>615</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
@@ -4143,7 +4159,7 @@
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>622</v>
+        <v>615</v>
       </c>
       <c r="E16" t="s">
         <v>6</v>
@@ -4256,7 +4272,7 @@
         <v>5</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>623</v>
+        <v>616</v>
       </c>
       <c r="E17" t="s">
         <v>6</v>
@@ -4369,7 +4385,7 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>624</v>
+        <v>617</v>
       </c>
       <c r="E18" t="s">
         <v>6</v>
@@ -4482,7 +4498,7 @@
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>625</v>
+        <v>618</v>
       </c>
       <c r="E19" t="s">
         <v>6</v>
@@ -4595,7 +4611,7 @@
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>626</v>
+        <v>619</v>
       </c>
       <c r="E20" t="s">
         <v>6</v>
@@ -4708,7 +4724,7 @@
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>627</v>
+        <v>620</v>
       </c>
       <c r="E21" t="s">
         <v>6</v>
@@ -4821,7 +4837,7 @@
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>628</v>
+        <v>621</v>
       </c>
       <c r="E22" t="s">
         <v>6</v>
@@ -4934,7 +4950,7 @@
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>629</v>
+        <v>622</v>
       </c>
       <c r="E23" t="s">
         <v>6</v>
@@ -5047,7 +5063,7 @@
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>630</v>
+        <v>623</v>
       </c>
       <c r="E24" t="s">
         <v>6</v>
@@ -5160,7 +5176,7 @@
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
       <c r="E25" t="s">
         <v>6</v>
@@ -5273,7 +5289,7 @@
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>632</v>
+        <v>625</v>
       </c>
       <c r="E26" t="s">
         <v>6</v>
@@ -5386,7 +5402,7 @@
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>633</v>
+        <v>626</v>
       </c>
       <c r="E27" t="s">
         <v>6</v>
@@ -5499,7 +5515,7 @@
         <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>634</v>
+        <v>627</v>
       </c>
       <c r="E28" t="s">
         <v>6</v>
@@ -5612,7 +5628,7 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>635</v>
+        <v>628</v>
       </c>
       <c r="E29" t="s">
         <v>6</v>
@@ -5725,7 +5741,7 @@
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>636</v>
+        <v>629</v>
       </c>
       <c r="E30" t="s">
         <v>6</v>
@@ -5838,7 +5854,7 @@
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>637</v>
+        <v>630</v>
       </c>
       <c r="E31" t="s">
         <v>6</v>
@@ -5951,7 +5967,7 @@
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>638</v>
+        <v>631</v>
       </c>
       <c r="E32" t="s">
         <v>6</v>
@@ -6064,7 +6080,7 @@
         <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>639</v>
+        <v>632</v>
       </c>
       <c r="E33" t="s">
         <v>6</v>
@@ -6177,7 +6193,7 @@
         <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>640</v>
+        <v>633</v>
       </c>
       <c r="E34" t="s">
         <v>6</v>
@@ -6290,7 +6306,7 @@
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>641</v>
+        <v>634</v>
       </c>
       <c r="E35" t="s">
         <v>6</v>
@@ -6403,7 +6419,7 @@
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>642</v>
+        <v>635</v>
       </c>
       <c r="E36" t="s">
         <v>6</v>
@@ -6516,7 +6532,7 @@
         <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>643</v>
+        <v>636</v>
       </c>
       <c r="E37" t="s">
         <v>6</v>
@@ -6623,13 +6639,13 @@
         <v>21</v>
       </c>
       <c r="B38" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
       </c>
       <c r="D38" t="s">
-        <v>644</v>
+        <v>637</v>
       </c>
       <c r="E38" t="s">
         <v>6</v>
@@ -6659,7 +6675,7 @@
         <v>143</v>
       </c>
       <c r="N38" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="O38" t="s">
         <v>143</v>
@@ -6736,13 +6752,13 @@
         <v>21</v>
       </c>
       <c r="B39" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C39" t="s">
         <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="E39" t="s">
         <v>3</v>
@@ -6849,13 +6865,13 @@
         <v>21</v>
       </c>
       <c r="B40" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C40" t="s">
         <v>2</v>
       </c>
       <c r="D40" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E40" t="s">
         <v>3</v>
@@ -6968,7 +6984,7 @@
         <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>645</v>
+        <v>638</v>
       </c>
       <c r="E41" t="s">
         <v>6</v>
@@ -7081,7 +7097,7 @@
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="E42" t="s">
         <v>6</v>
@@ -7194,7 +7210,7 @@
         <v>5</v>
       </c>
       <c r="D43" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="E43" t="s">
         <v>6</v>
@@ -7301,13 +7317,13 @@
         <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C44" t="s">
         <v>2</v>
       </c>
       <c r="D44" t="s">
-        <v>604</v>
+        <v>643</v>
       </c>
       <c r="E44" t="s">
         <v>3</v>
@@ -7420,7 +7436,7 @@
         <v>5</v>
       </c>
       <c r="D45" t="s">
-        <v>648</v>
+        <v>642</v>
       </c>
       <c r="E45" t="s">
         <v>6</v>
@@ -7533,7 +7549,7 @@
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="E46" t="s">
         <v>3</v>
@@ -7640,13 +7656,13 @@
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C47" t="s">
         <v>2</v>
       </c>
       <c r="D47" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="E47" t="s">
         <v>3</v>
@@ -7753,13 +7769,13 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C48" t="s">
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="E48" t="s">
         <v>3</v>
@@ -7866,13 +7882,13 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C49" t="s">
         <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="E49" t="s">
         <v>3</v>
@@ -7979,13 +7995,13 @@
         <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C50" t="s">
         <v>2</v>
       </c>
       <c r="D50" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="E50" t="s">
         <v>3</v>
@@ -8098,7 +8114,7 @@
         <v>5</v>
       </c>
       <c r="D51" t="s">
-        <v>649</v>
+        <v>639</v>
       </c>
       <c r="E51" t="s">
         <v>6</v>
@@ -8205,13 +8221,13 @@
         <v>55</v>
       </c>
       <c r="B52" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C52" t="s">
         <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="E52" t="s">
         <v>3</v>
@@ -8318,13 +8334,13 @@
         <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C53" t="s">
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E53" t="s">
         <v>3</v>
@@ -8333,13 +8349,13 @@
         <v>142</v>
       </c>
       <c r="G53" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="H53" t="s">
         <v>574</v>
       </c>
-      <c r="H53" t="s">
+      <c r="I53" t="s">
         <v>575</v>
-      </c>
-      <c r="I53" t="s">
-        <v>576</v>
       </c>
       <c r="J53" t="s">
         <v>457</v>
@@ -8437,7 +8453,7 @@
         <v>2</v>
       </c>
       <c r="D54" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="E54" t="s">
         <v>3</v>
@@ -8544,13 +8560,13 @@
         <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C55" t="s">
         <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>612</v>
+        <v>649</v>
       </c>
       <c r="E55" t="s">
         <v>3</v>
@@ -8663,7 +8679,7 @@
         <v>5</v>
       </c>
       <c r="D56" t="s">
-        <v>650</v>
+        <v>640</v>
       </c>
       <c r="E56" t="s">
         <v>6</v>
@@ -8765,7 +8781,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="57" spans="1:37" ht="18" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:37" ht="20" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>48</v>
       </c>
@@ -8775,8 +8791,8 @@
       <c r="C57" t="s">
         <v>2</v>
       </c>
-      <c r="D57" t="s">
-        <v>143</v>
+      <c r="D57" s="18" t="s">
+        <v>650</v>
       </c>
       <c r="E57" t="s">
         <v>3</v>
@@ -8883,13 +8899,13 @@
         <v>48</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C58" t="s">
         <v>2</v>
       </c>
       <c r="D58" t="s">
-        <v>143</v>
+        <v>651</v>
       </c>
       <c r="E58" t="s">
         <v>3</v>
@@ -8898,13 +8914,13 @@
         <v>142</v>
       </c>
       <c r="G58" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="H58" t="s">
+        <v>576</v>
+      </c>
+      <c r="I58" s="14" t="s">
         <v>579</v>
-      </c>
-      <c r="H58" t="s">
-        <v>577</v>
-      </c>
-      <c r="I58" s="14" t="s">
-        <v>580</v>
       </c>
       <c r="J58" t="s">
         <v>457</v>
@@ -9115,7 +9131,7 @@
         <v>2</v>
       </c>
       <c r="D60" t="s">
-        <v>143</v>
+        <v>652</v>
       </c>
       <c r="E60" t="s">
         <v>3</v>
@@ -9228,7 +9244,7 @@
         <v>5</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>567</v>
+        <v>653</v>
       </c>
       <c r="E61" t="s">
         <v>6</v>
@@ -9282,10 +9298,10 @@
         <v>143</v>
       </c>
       <c r="V61" t="s">
+        <v>567</v>
+      </c>
+      <c r="W61" t="s">
         <v>568</v>
-      </c>
-      <c r="W61" t="s">
-        <v>569</v>
       </c>
       <c r="X61" s="1" t="s">
         <v>139</v>
@@ -9335,13 +9351,13 @@
         <v>21</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C62" t="s">
         <v>2</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E62" t="s">
         <v>3</v>
@@ -14942,13 +14958,13 @@
         <v>510</v>
       </c>
       <c r="C141" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D141" t="s">
         <v>436</v>
       </c>
       <c r="E141" s="17" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F141" t="s">
         <v>143</v>
@@ -14967,7 +14983,7 @@
         <v>hts_mod_fac_post_anc_1</v>
       </c>
       <c r="AG141" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="142" spans="1:33" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
data required change F/M/U to f/m
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7ADF88E-317D-124A-BD8F-B8907AA8CECC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427126F9-9728-6E40-8D83-1EA447E18253}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7780" yWindow="2020" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -2430,10 +2430,10 @@
   <dimension ref="A1:AK62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="T17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A61" sqref="A61"/>
+      <selection pane="bottomRight" activeCell="Z17" sqref="Z17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3957,7 +3957,7 @@
         <v>149</v>
       </c>
       <c r="L14" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M14" t="s">
         <v>143</v>
@@ -4070,7 +4070,7 @@
         <v>151</v>
       </c>
       <c r="L15" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M15" t="s">
         <v>143</v>
@@ -4183,7 +4183,7 @@
         <v>151</v>
       </c>
       <c r="L16" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M16" t="s">
         <v>143</v>
@@ -4296,7 +4296,7 @@
         <v>151</v>
       </c>
       <c r="L17" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M17" t="s">
         <v>143</v>
@@ -4409,7 +4409,7 @@
         <v>151</v>
       </c>
       <c r="L18" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M18" t="s">
         <v>143</v>
@@ -4522,7 +4522,7 @@
         <v>151</v>
       </c>
       <c r="L19" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M19" t="s">
         <v>143</v>
@@ -4635,7 +4635,7 @@
         <v>151</v>
       </c>
       <c r="L20" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M20" t="s">
         <v>143</v>
@@ -4748,7 +4748,7 @@
         <v>151</v>
       </c>
       <c r="L21" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M21" t="s">
         <v>143</v>
@@ -4861,7 +4861,7 @@
         <v>151</v>
       </c>
       <c r="L22" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M22" t="s">
         <v>143</v>
@@ -4974,7 +4974,7 @@
         <v>97</v>
       </c>
       <c r="L23" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M23" t="s">
         <v>143</v>
@@ -5087,7 +5087,7 @@
         <v>97</v>
       </c>
       <c r="L24" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M24" t="s">
         <v>143</v>
@@ -5200,7 +5200,7 @@
         <v>151</v>
       </c>
       <c r="L25" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M25" t="s">
         <v>143</v>
@@ -5313,7 +5313,7 @@
         <v>151</v>
       </c>
       <c r="L26" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M26" t="s">
         <v>143</v>
@@ -5426,7 +5426,7 @@
         <v>151</v>
       </c>
       <c r="L27" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M27" t="s">
         <v>143</v>
@@ -5539,7 +5539,7 @@
         <v>151</v>
       </c>
       <c r="L28" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M28" t="s">
         <v>143</v>
@@ -5652,7 +5652,7 @@
         <v>151</v>
       </c>
       <c r="L29" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M29" t="s">
         <v>143</v>
@@ -5765,7 +5765,7 @@
         <v>151</v>
       </c>
       <c r="L30" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M30" t="s">
         <v>143</v>
@@ -5878,7 +5878,7 @@
         <v>151</v>
       </c>
       <c r="L31" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M31" t="s">
         <v>143</v>
@@ -5991,7 +5991,7 @@
         <v>151</v>
       </c>
       <c r="L32" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M32" t="s">
         <v>143</v>
@@ -6104,7 +6104,7 @@
         <v>97</v>
       </c>
       <c r="L33" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M33" t="s">
         <v>143</v>
@@ -6217,7 +6217,7 @@
         <v>97</v>
       </c>
       <c r="L34" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M34" t="s">
         <v>143</v>
@@ -6330,7 +6330,7 @@
         <v>151</v>
       </c>
       <c r="L35" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M35" t="s">
         <v>143</v>
@@ -6443,7 +6443,7 @@
         <v>151</v>
       </c>
       <c r="L36" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M36" t="s">
         <v>143</v>
@@ -6556,7 +6556,7 @@
         <v>151</v>
       </c>
       <c r="L37" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M37" t="s">
         <v>143</v>
@@ -7347,7 +7347,7 @@
         <v>229</v>
       </c>
       <c r="L44" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M44" t="s">
         <v>143</v>
@@ -7460,7 +7460,7 @@
         <v>229</v>
       </c>
       <c r="L45" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M45" t="s">
         <v>143</v>
@@ -9469,8 +9469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
   <dimension ref="A1:AG143"/>
   <sheetViews>
-    <sheetView topLeftCell="G109" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="W141" sqref="W141"/>
+    <sheetView topLeftCell="A39" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
dim_item_sets add new age category
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC11E5F-C7D9-6D44-89A0-C96E403C91DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB66851-892D-4045-8626-025E593D4C8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="14700" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data_required!$A$1:$AK$60</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">dimension_Item_sets!$A$1:$AF$143</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">dimension_Item_sets!$A$1:$AG$143</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3535" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3564" uniqueCount="655">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1998,6 +1998,9 @@
   </si>
   <si>
     <t>([HTS_SELF (N, Age/Sex/HIVSelfTest).T_1] - [HTS_SELF (N, Age/Sex/HIVSelfTest).R]) / [HTS_SELF (N, Age/Sex/HIVSelfTest).R]</t>
+  </si>
+  <si>
+    <t>&lt;1-50+.&lt;15/&gt;15.d</t>
   </si>
 </sst>
 </file>
@@ -2429,7 +2432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
   <dimension ref="A1:AK62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="J34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -9467,10 +9470,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
-  <dimension ref="A1:AG143"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:AH143"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9488,9 +9492,10 @@
     <col min="11" max="13" width="12.33203125" customWidth="1"/>
     <col min="14" max="18" width="10.83203125" customWidth="1"/>
     <col min="19" max="19" width="13.5" customWidth="1"/>
+    <col min="21" max="21" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>221</v>
       </c>
@@ -9551,47 +9556,50 @@
       <c r="T1" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="9" t="s">
+        <v>654</v>
+      </c>
+      <c r="V1" t="s">
         <v>216</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>145</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>150</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>218</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>255</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>260</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>261</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>288</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>281</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>289</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>379</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>402</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>174</v>
       </c>
@@ -9620,7 +9628,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="4" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K2:ZZ2)</f>
+        <f>_xlfn.TEXTJOIN(";",1,K2:AAA2)</f>
         <v>&lt;2mo</v>
       </c>
       <c r="K2" s="9"/>
@@ -9631,11 +9639,12 @@
       <c r="Q2" s="9"/>
       <c r="R2" s="9"/>
       <c r="T2" s="9"/>
-      <c r="Z2" t="s">
+      <c r="U2" s="9"/>
+      <c r="AA2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>174</v>
       </c>
@@ -9664,7 +9673,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="4" t="str">
-        <f t="shared" ref="J3:J36" si="0">_xlfn.TEXTJOIN(";",1,K3:ZZ3)</f>
+        <f t="shared" ref="J3:J36" si="0">_xlfn.TEXTJOIN(";",1,K3:AAA3)</f>
         <v>2-12mo</v>
       </c>
       <c r="K3" s="9"/>
@@ -9675,11 +9684,12 @@
       <c r="Q3" s="9"/>
       <c r="R3" s="9"/>
       <c r="T3" s="9"/>
-      <c r="AA3" t="s">
+      <c r="U3" s="9"/>
+      <c r="AB3" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>174</v>
       </c>
@@ -9709,7 +9719,7 @@
       </c>
       <c r="J4" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;1-50+;&lt;1-18+</v>
+        <v>&lt;1-50+;&lt;1-18+;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>149</v>
@@ -9720,8 +9730,11 @@
       <c r="O4" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="U4" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>174</v>
       </c>
@@ -9751,14 +9764,17 @@
       </c>
       <c r="J5" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;15/&gt;15.d</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="O5" s="9"/>
       <c r="P5" s="9" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="U5" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>174</v>
       </c>
@@ -9791,7 +9807,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>174</v>
       </c>
@@ -9821,7 +9837,7 @@
       </c>
       <c r="J7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;&lt;1-18+;1-4;1-50+/&lt;5</v>
+        <v>&lt;1-50+;1-50+;&lt;1-18+;1-4;1-50+/&lt;5;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="K7" s="9" t="s">
         <v>149</v>
@@ -9840,8 +9856,11 @@
       <c r="R7" s="9" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="U7" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>174</v>
       </c>
@@ -9871,7 +9890,7 @@
       </c>
       <c r="J8" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;&lt;1-18+;1-4;1-50+/&lt;5</v>
+        <v>&lt;1-50+;1-50+;&lt;1-18+;1-4;1-50+/&lt;5;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="K8" s="9" t="s">
         <v>149</v>
@@ -9890,8 +9909,11 @@
       <c r="R8" s="9" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="U8" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>174</v>
       </c>
@@ -9921,13 +9943,16 @@
       </c>
       <c r="J9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;15/&gt;15.d</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="P9" s="9" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="U9" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>174</v>
       </c>
@@ -9966,7 +9991,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>174</v>
       </c>
@@ -9996,7 +10021,7 @@
       </c>
       <c r="J11" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;&lt;1-18+;1-50+/&lt;5</v>
+        <v>&lt;1-50+;1-50+;&lt;1-18+;1-50+/&lt;5;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="K11" s="9" t="s">
         <v>149</v>
@@ -10012,8 +10037,11 @@
       <c r="R11" s="9" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="U11" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>174</v>
       </c>
@@ -10043,7 +10071,7 @@
       </c>
       <c r="J12" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;&lt;1-18+;1-50+/&lt;5</v>
+        <v>&lt;1-50+;1-50+;&lt;1-18+;1-50+/&lt;5;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="K12" s="9" t="s">
         <v>149</v>
@@ -10059,8 +10087,11 @@
       <c r="R12" s="9" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="U12" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>174</v>
       </c>
@@ -10090,13 +10121,16 @@
       </c>
       <c r="J13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;15/&gt;15.d</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="P13" s="9" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="U13" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>174</v>
       </c>
@@ -10126,7 +10160,7 @@
       </c>
       <c r="J14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;10-50+;&lt;1-18+;1-50+/&lt;5;10-50+.all</v>
+        <v>&lt;1-50+;1-50+;10-50+;&lt;1-18+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="K14" s="9" t="s">
         <v>149</v>
@@ -10147,8 +10181,11 @@
       <c r="T14" s="9" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="U14" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>174</v>
       </c>
@@ -10178,13 +10215,16 @@
       </c>
       <c r="J15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;15/&gt;15.d</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="P15" s="9" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="U15" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>143</v>
       </c>
@@ -10226,7 +10266,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>174</v>
       </c>
@@ -10264,7 +10304,7 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>143</v>
       </c>
@@ -10300,7 +10340,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>174</v>
       </c>
@@ -10336,7 +10376,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>174</v>
       </c>
@@ -10366,13 +10406,16 @@
       </c>
       <c r="J20" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;15/&gt;15.d</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="P20" s="9" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U20" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>174</v>
       </c>
@@ -10402,7 +10445,7 @@
       </c>
       <c r="J21" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all</v>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="K21" s="9" t="s">
         <v>149</v>
@@ -10422,8 +10465,11 @@
       <c r="T21" s="9" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U21" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>143</v>
       </c>
@@ -10465,7 +10511,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>174</v>
       </c>
@@ -10501,7 +10547,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>143</v>
       </c>
@@ -10543,7 +10589,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>174</v>
       </c>
@@ -10572,7 +10618,7 @@
         <v>1</v>
       </c>
       <c r="J25" s="4" t="str">
-        <f t="shared" ref="J25" si="1">_xlfn.TEXTJOIN(";",1,K25:ZZ25)</f>
+        <f t="shared" ref="J25" si="1">_xlfn.TEXTJOIN(";",1,K25:AAA25)</f>
         <v>&lt;1-18+</v>
       </c>
       <c r="K25" s="5"/>
@@ -10584,7 +10630,7 @@
       </c>
       <c r="P25" s="5"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>174</v>
       </c>
@@ -10625,7 +10671,7 @@
       </c>
       <c r="P26" s="5"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>174</v>
       </c>
@@ -10655,13 +10701,16 @@
       </c>
       <c r="J27" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;15/&gt;15.d</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="P27" s="9" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U27" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>174</v>
       </c>
@@ -10691,7 +10740,7 @@
       </c>
       <c r="J28" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all</v>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="K28" s="9" t="s">
         <v>149</v>
@@ -10711,8 +10760,11 @@
       <c r="T28" s="9" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U28" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>143</v>
       </c>
@@ -10754,7 +10806,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>174</v>
       </c>
@@ -10784,13 +10836,16 @@
       </c>
       <c r="J30" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;15/&gt;15.d</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="P30" s="9" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U30" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>174</v>
       </c>
@@ -10820,7 +10875,7 @@
       </c>
       <c r="J31" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all</v>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="K31" s="9" t="s">
         <v>149</v>
@@ -10842,8 +10897,11 @@
       <c r="T31" s="9" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U31" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>174</v>
       </c>
@@ -10879,7 +10937,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>143</v>
       </c>
@@ -10921,7 +10979,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>174</v>
       </c>
@@ -10957,7 +11015,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>174</v>
       </c>
@@ -10987,13 +11045,16 @@
       </c>
       <c r="J35" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;15/&gt;15.d</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="P35" s="9" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U35" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>174</v>
       </c>
@@ -11029,7 +11090,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>174</v>
       </c>
@@ -11058,8 +11119,8 @@
         <v>1</v>
       </c>
       <c r="J37" s="4" t="str">
-        <f t="shared" ref="J37:J70" si="2">_xlfn.TEXTJOIN(";",1,K37:ZZ37)</f>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all</v>
+        <f t="shared" ref="J37:J70" si="2">_xlfn.TEXTJOIN(";",1,K37:AAA37)</f>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="K37" s="9" t="s">
         <v>149</v>
@@ -11081,8 +11142,11 @@
       <c r="T37" s="9" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U37" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>143</v>
       </c>
@@ -11124,7 +11188,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>174</v>
       </c>
@@ -11154,13 +11218,16 @@
       </c>
       <c r="J39" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;15/&gt;15.d</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="P39" s="9" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U39" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>174</v>
       </c>
@@ -11196,7 +11263,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>174</v>
       </c>
@@ -11226,7 +11293,7 @@
       </c>
       <c r="J41" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all</v>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="K41" s="9" t="s">
         <v>149</v>
@@ -11246,8 +11313,11 @@
       <c r="T41" s="9" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U41" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>143</v>
       </c>
@@ -11289,7 +11359,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>174</v>
       </c>
@@ -11318,8 +11388,8 @@
         <v>1</v>
       </c>
       <c r="J43" s="4" t="str">
-        <f t="shared" ref="J43" si="3">_xlfn.TEXTJOIN(";",1,K43:ZZ43)</f>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all</v>
+        <f t="shared" ref="J43" si="3">_xlfn.TEXTJOIN(";",1,K43:AAA43)</f>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="K43" s="9" t="s">
         <v>149</v>
@@ -11339,8 +11409,11 @@
       <c r="T43" s="9" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U43" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>174</v>
       </c>
@@ -11370,13 +11443,16 @@
       </c>
       <c r="J44" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;15/&gt;15.d</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="P44" s="9" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U44" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>174</v>
       </c>
@@ -11412,7 +11488,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>174</v>
       </c>
@@ -11442,7 +11518,7 @@
       </c>
       <c r="J46" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all</v>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="K46" s="9" t="s">
         <v>149</v>
@@ -11462,8 +11538,11 @@
       <c r="T46" s="9" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U46" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>143</v>
       </c>
@@ -11505,7 +11584,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>174</v>
       </c>
@@ -11534,8 +11613,8 @@
         <v>1</v>
       </c>
       <c r="J48" s="4" t="str">
-        <f t="shared" ref="J48" si="4">_xlfn.TEXTJOIN(";",1,K48:ZZ48)</f>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all</v>
+        <f t="shared" ref="J48" si="4">_xlfn.TEXTJOIN(";",1,K48:AAA48)</f>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="K48" s="9" t="s">
         <v>149</v>
@@ -11555,8 +11634,11 @@
       <c r="T48" s="9" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U48" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>174</v>
       </c>
@@ -11586,13 +11668,16 @@
       </c>
       <c r="J49" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;15/&gt;15.d</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="P49" s="9" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U49" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>174</v>
       </c>
@@ -11628,7 +11713,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>174</v>
       </c>
@@ -11658,7 +11743,7 @@
       </c>
       <c r="J51" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all</v>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="K51" s="9" t="s">
         <v>149</v>
@@ -11678,8 +11763,11 @@
       <c r="T51" s="9" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U51" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>143</v>
       </c>
@@ -11721,7 +11809,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>174</v>
       </c>
@@ -11751,13 +11839,16 @@
       </c>
       <c r="J53" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;15/&gt;15.d</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="P53" s="9" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U53" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>174</v>
       </c>
@@ -11787,7 +11878,7 @@
       </c>
       <c r="J54" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all</v>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d</v>
       </c>
       <c r="K54" s="9" t="s">
         <v>149</v>
@@ -11807,8 +11898,11 @@
       <c r="T54" s="9" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U54" s="9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>143</v>
       </c>
@@ -11850,7 +11944,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>175</v>
       </c>
@@ -11882,17 +11976,17 @@
         <f t="shared" si="2"/>
         <v>F;F/M;F/M/U</v>
       </c>
-      <c r="U56" t="s">
+      <c r="V56" t="s">
         <v>141</v>
       </c>
-      <c r="V56" t="s">
+      <c r="W56" t="s">
         <v>145</v>
       </c>
-      <c r="W56" t="s">
+      <c r="X56" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>143</v>
       </c>
@@ -11934,7 +12028,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>175</v>
       </c>
@@ -11972,14 +12066,14 @@
       <c r="N58" s="5"/>
       <c r="O58" s="5"/>
       <c r="P58" s="5"/>
-      <c r="U58" t="s">
+      <c r="V58" t="s">
         <v>154</v>
       </c>
-      <c r="W58" t="s">
+      <c r="X58" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>175</v>
       </c>
@@ -12013,17 +12107,18 @@
       </c>
       <c r="S59" s="5"/>
       <c r="T59" s="5"/>
-      <c r="U59" t="s">
+      <c r="U59" s="5"/>
+      <c r="V59" t="s">
         <v>148</v>
       </c>
-      <c r="V59" t="s">
+      <c r="W59" t="s">
         <v>145</v>
       </c>
-      <c r="W59" t="s">
+      <c r="X59" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>143</v>
       </c>
@@ -12065,7 +12160,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>175</v>
       </c>
@@ -12099,14 +12194,15 @@
       </c>
       <c r="S61" s="5"/>
       <c r="T61" s="5"/>
-      <c r="U61" t="s">
+      <c r="U61" s="5"/>
+      <c r="V61" t="s">
         <v>154</v>
       </c>
-      <c r="W61" t="s">
+      <c r="X61" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>184</v>
       </c>
@@ -12138,11 +12234,11 @@
         <f t="shared" si="2"/>
         <v>kp1</v>
       </c>
-      <c r="X62" t="s">
+      <c r="Y62" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>184</v>
       </c>
@@ -12174,11 +12270,11 @@
         <f t="shared" si="2"/>
         <v>kp1</v>
       </c>
-      <c r="X63" t="s">
+      <c r="Y63" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>184</v>
       </c>
@@ -12210,11 +12306,11 @@
         <f t="shared" si="2"/>
         <v>kp1</v>
       </c>
-      <c r="X64" t="s">
+      <c r="Y64" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="65" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>184</v>
       </c>
@@ -12246,11 +12342,11 @@
         <f t="shared" si="2"/>
         <v>kp1</v>
       </c>
-      <c r="X65" t="s">
+      <c r="Y65" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="66" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>184</v>
       </c>
@@ -12282,11 +12378,11 @@
         <f t="shared" si="2"/>
         <v>kp1</v>
       </c>
-      <c r="X66" t="s">
+      <c r="Y66" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="67" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>196</v>
       </c>
@@ -12318,11 +12414,11 @@
         <f t="shared" si="2"/>
         <v>tr_pos</v>
       </c>
-      <c r="Y67" t="s">
+      <c r="Z67" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="68" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>196</v>
       </c>
@@ -12354,11 +12450,11 @@
         <f t="shared" si="2"/>
         <v>tr_neg</v>
       </c>
-      <c r="Y68" t="s">
+      <c r="Z68" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="69" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>264</v>
       </c>
@@ -12390,11 +12486,11 @@
         <f t="shared" si="2"/>
         <v>tss_NewPos</v>
       </c>
-      <c r="AB69" t="s">
+      <c r="AC69" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="70" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>264</v>
       </c>
@@ -12426,11 +12522,11 @@
         <f t="shared" si="2"/>
         <v>tss_KnowPos</v>
       </c>
-      <c r="AB70" t="s">
+      <c r="AC70" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="71" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>264</v>
       </c>
@@ -12459,14 +12555,14 @@
         <v>1</v>
       </c>
       <c r="J71" s="4" t="str">
-        <f t="shared" ref="J71:J134" si="5">_xlfn.TEXTJOIN(";",1,K71:ZZ71)</f>
+        <f t="shared" ref="J71:J134" si="5">_xlfn.TEXTJOIN(";",1,K71:AAA71)</f>
         <v>tss_NewNeg</v>
       </c>
-      <c r="AB71" t="s">
+      <c r="AC71" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="72" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>278</v>
       </c>
@@ -12498,11 +12594,11 @@
         <f t="shared" si="5"/>
         <v>vt_sv</v>
       </c>
-      <c r="AC72" t="s">
+      <c r="AD72" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="73" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>278</v>
       </c>
@@ -12534,11 +12630,11 @@
         <f t="shared" si="5"/>
         <v>vt_pe</v>
       </c>
-      <c r="AC73" t="s">
+      <c r="AD73" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="74" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>278</v>
       </c>
@@ -12570,11 +12666,11 @@
         <f t="shared" si="5"/>
         <v>st_da</v>
       </c>
-      <c r="AD74" t="s">
+      <c r="AE74" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="75" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>278</v>
       </c>
@@ -12606,11 +12702,11 @@
         <f t="shared" si="5"/>
         <v>st_da</v>
       </c>
-      <c r="AD75" t="s">
+      <c r="AE75" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="76" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>278</v>
       </c>
@@ -12642,11 +12738,11 @@
         <f t="shared" si="5"/>
         <v>st_da</v>
       </c>
-      <c r="AD76" t="s">
+      <c r="AE76" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="77" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>278</v>
       </c>
@@ -12678,11 +12774,11 @@
         <f t="shared" si="5"/>
         <v>st_da</v>
       </c>
-      <c r="AD77" t="s">
+      <c r="AE77" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="78" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>278</v>
       </c>
@@ -12714,11 +12810,11 @@
         <f t="shared" si="5"/>
         <v>st_da</v>
       </c>
-      <c r="AD78" t="s">
+      <c r="AE78" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="79" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>278</v>
       </c>
@@ -12750,11 +12846,11 @@
         <f t="shared" si="5"/>
         <v>st_da</v>
       </c>
-      <c r="AD79" t="s">
+      <c r="AE79" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="80" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>278</v>
       </c>
@@ -12786,11 +12882,11 @@
         <f t="shared" si="5"/>
         <v>st_da</v>
       </c>
-      <c r="AD80" t="s">
+      <c r="AE80" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="81" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>278</v>
       </c>
@@ -12822,11 +12918,11 @@
         <f t="shared" si="5"/>
         <v>st_da</v>
       </c>
-      <c r="AD81" t="s">
+      <c r="AE81" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="82" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>278</v>
       </c>
@@ -12858,11 +12954,11 @@
         <f t="shared" si="5"/>
         <v>st_da</v>
       </c>
-      <c r="AD82" t="s">
+      <c r="AE82" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="83" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>278</v>
       </c>
@@ -12894,11 +12990,11 @@
         <f t="shared" si="5"/>
         <v>st_da</v>
       </c>
-      <c r="AD83" t="s">
+      <c r="AE83" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="84" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>278</v>
       </c>
@@ -12930,11 +13026,11 @@
         <f t="shared" si="5"/>
         <v>st_da</v>
       </c>
-      <c r="AD84" t="s">
+      <c r="AE84" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="85" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>278</v>
       </c>
@@ -12966,11 +13062,11 @@
         <f t="shared" si="5"/>
         <v>st_da</v>
       </c>
-      <c r="AD85" t="s">
+      <c r="AE85" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="86" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>278</v>
       </c>
@@ -13002,11 +13098,11 @@
         <f t="shared" si="5"/>
         <v>st_da</v>
       </c>
-      <c r="AD86" t="s">
+      <c r="AE86" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="87" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>278</v>
       </c>
@@ -13038,11 +13134,11 @@
         <f t="shared" si="5"/>
         <v>st_da</v>
       </c>
-      <c r="AD87" t="s">
+      <c r="AE87" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="88" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>278</v>
       </c>
@@ -13074,11 +13170,11 @@
         <f t="shared" si="5"/>
         <v>st_da</v>
       </c>
-      <c r="AD88" t="s">
+      <c r="AE88" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="89" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>278</v>
       </c>
@@ -13110,11 +13206,11 @@
         <f t="shared" si="5"/>
         <v>st_da</v>
       </c>
-      <c r="AD89" t="s">
+      <c r="AE89" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="90" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>278</v>
       </c>
@@ -13146,11 +13242,11 @@
         <f t="shared" si="5"/>
         <v>st_ua</v>
       </c>
-      <c r="AD90" t="s">
+      <c r="AE90" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="91" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>278</v>
       </c>
@@ -13182,11 +13278,11 @@
         <f t="shared" si="5"/>
         <v>st_ua</v>
       </c>
-      <c r="AD91" t="s">
+      <c r="AE91" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="92" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>278</v>
       </c>
@@ -13218,11 +13314,11 @@
         <f t="shared" si="5"/>
         <v>st_ua</v>
       </c>
-      <c r="AD92" t="s">
+      <c r="AE92" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="93" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>278</v>
       </c>
@@ -13254,11 +13350,11 @@
         <f t="shared" si="5"/>
         <v>st_ua</v>
       </c>
-      <c r="AD93" t="s">
+      <c r="AE93" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="94" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>278</v>
       </c>
@@ -13290,11 +13386,11 @@
         <f t="shared" si="5"/>
         <v>st_ua</v>
       </c>
-      <c r="AD94" t="s">
+      <c r="AE94" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="95" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>278</v>
       </c>
@@ -13326,11 +13422,11 @@
         <f t="shared" si="5"/>
         <v>st_ua</v>
       </c>
-      <c r="AD95" t="s">
+      <c r="AE95" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="96" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>278</v>
       </c>
@@ -13362,11 +13458,11 @@
         <f t="shared" si="5"/>
         <v>st_ua</v>
       </c>
-      <c r="AD96" t="s">
+      <c r="AE96" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="97" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>278</v>
       </c>
@@ -13398,11 +13494,11 @@
         <f t="shared" si="5"/>
         <v>st_ua</v>
       </c>
-      <c r="AD97" t="s">
+      <c r="AE97" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="98" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>278</v>
       </c>
@@ -13434,11 +13530,11 @@
         <f t="shared" si="5"/>
         <v>st_ua</v>
       </c>
-      <c r="AD98" t="s">
+      <c r="AE98" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="99" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>278</v>
       </c>
@@ -13470,11 +13566,11 @@
         <f t="shared" si="5"/>
         <v>st_ua</v>
       </c>
-      <c r="AD99" t="s">
+      <c r="AE99" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="100" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>278</v>
       </c>
@@ -13506,11 +13602,11 @@
         <f t="shared" si="5"/>
         <v>st_ua</v>
       </c>
-      <c r="AD100" t="s">
+      <c r="AE100" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="101" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>278</v>
       </c>
@@ -13542,11 +13638,11 @@
         <f t="shared" si="5"/>
         <v>st_ua</v>
       </c>
-      <c r="AD101" t="s">
+      <c r="AE101" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="102" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>278</v>
       </c>
@@ -13578,11 +13674,11 @@
         <f t="shared" si="5"/>
         <v>st_ua</v>
       </c>
-      <c r="AD102" t="s">
+      <c r="AE102" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="103" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>278</v>
       </c>
@@ -13614,11 +13710,11 @@
         <f t="shared" si="5"/>
         <v>st_ua</v>
       </c>
-      <c r="AD103" t="s">
+      <c r="AE103" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="104" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>278</v>
       </c>
@@ -13650,11 +13746,11 @@
         <f t="shared" si="5"/>
         <v>st_ua</v>
       </c>
-      <c r="AD104" t="s">
+      <c r="AE104" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="105" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>278</v>
       </c>
@@ -13686,11 +13782,11 @@
         <f t="shared" si="5"/>
         <v>st_ua</v>
       </c>
-      <c r="AD105" t="s">
+      <c r="AE105" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="106" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>278</v>
       </c>
@@ -13722,11 +13818,11 @@
         <f t="shared" si="5"/>
         <v>kp2</v>
       </c>
-      <c r="X106" t="s">
+      <c r="Y106" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="107" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>278</v>
       </c>
@@ -13758,11 +13854,11 @@
         <f t="shared" si="5"/>
         <v>kp2</v>
       </c>
-      <c r="X107" t="s">
+      <c r="Y107" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="108" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>278</v>
       </c>
@@ -13794,11 +13890,11 @@
         <f t="shared" si="5"/>
         <v>kp2</v>
       </c>
-      <c r="X108" t="s">
+      <c r="Y108" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="109" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>278</v>
       </c>
@@ -13830,11 +13926,11 @@
         <f t="shared" si="5"/>
         <v>kp2</v>
       </c>
-      <c r="X109" t="s">
+      <c r="Y109" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="110" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>278</v>
       </c>
@@ -13866,11 +13962,11 @@
         <f t="shared" si="5"/>
         <v>kp2</v>
       </c>
-      <c r="X110" t="s">
+      <c r="Y110" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="111" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>278</v>
       </c>
@@ -13902,11 +13998,11 @@
         <f t="shared" si="5"/>
         <v>kp2</v>
       </c>
-      <c r="X111" t="s">
+      <c r="Y111" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="112" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>278</v>
       </c>
@@ -13938,11 +14034,11 @@
         <f t="shared" si="5"/>
         <v>kp2</v>
       </c>
-      <c r="X112" t="s">
+      <c r="Y112" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="113" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>278</v>
       </c>
@@ -13974,11 +14070,11 @@
         <f t="shared" si="5"/>
         <v>kp2</v>
       </c>
-      <c r="X113" t="s">
+      <c r="Y113" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="114" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>381</v>
       </c>
@@ -14010,11 +14106,11 @@
         <f t="shared" si="5"/>
         <v>as_already</v>
       </c>
-      <c r="AE114" t="s">
+      <c r="AF114" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="115" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>381</v>
       </c>
@@ -14046,11 +14142,11 @@
         <f t="shared" si="5"/>
         <v>as_new</v>
       </c>
-      <c r="AE115" t="s">
+      <c r="AF115" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="116" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>278</v>
       </c>
@@ -14082,11 +14178,11 @@
         <f t="shared" si="5"/>
         <v>kp3</v>
       </c>
-      <c r="X116" t="s">
+      <c r="Y116" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="117" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>278</v>
       </c>
@@ -14118,11 +14214,11 @@
         <f t="shared" si="5"/>
         <v>kp3</v>
       </c>
-      <c r="X117" t="s">
+      <c r="Y117" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="118" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>278</v>
       </c>
@@ -14154,11 +14250,11 @@
         <f t="shared" si="5"/>
         <v>kp3</v>
       </c>
-      <c r="X118" t="s">
+      <c r="Y118" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="119" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>278</v>
       </c>
@@ -14190,11 +14286,11 @@
         <f t="shared" si="5"/>
         <v>kp3</v>
       </c>
-      <c r="X119" t="s">
+      <c r="Y119" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="120" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>278</v>
       </c>
@@ -14226,11 +14322,11 @@
         <f t="shared" si="5"/>
         <v>ti_routine</v>
       </c>
-      <c r="AF120" t="s">
+      <c r="AG120" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="121" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>278</v>
       </c>
@@ -14262,11 +14358,11 @@
         <f t="shared" si="5"/>
         <v>ti_routine</v>
       </c>
-      <c r="AF121" t="s">
+      <c r="AG121" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="122" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>278</v>
       </c>
@@ -14298,11 +14394,11 @@
         <f t="shared" si="5"/>
         <v>ti_routine</v>
       </c>
-      <c r="AF122" t="s">
+      <c r="AG122" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="123" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>278</v>
       </c>
@@ -14334,11 +14430,11 @@
         <f t="shared" si="5"/>
         <v>ti_routine</v>
       </c>
-      <c r="AF123" t="s">
+      <c r="AG123" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="124" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>196</v>
       </c>
@@ -14367,14 +14463,14 @@
         <v>1</v>
       </c>
       <c r="J124" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K124:ZZ124)</f>
+        <f>_xlfn.TEXTJOIN(";",1,K124:AAA124)</f>
         <v>tr_pos2</v>
       </c>
-      <c r="Y124" t="s">
+      <c r="Z124" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="125" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>196</v>
       </c>
@@ -14406,11 +14502,11 @@
         <f t="shared" si="5"/>
         <v>tr_neg2</v>
       </c>
-      <c r="Y125" t="s">
+      <c r="Z125" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="126" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>509</v>
       </c>
@@ -14439,14 +14535,14 @@
         <v>1</v>
       </c>
       <c r="J126" t="str">
-        <f t="shared" ref="J126:J132" si="6">_xlfn.TEXTJOIN(";",1,K126:ZZ126)</f>
+        <f t="shared" ref="J126:J132" si="6">_xlfn.TEXTJOIN(";",1,K126:AAA126)</f>
         <v>hts_mod_com_ndx</v>
       </c>
-      <c r="AG126" t="s">
+      <c r="AH126" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="127" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>509</v>
       </c>
@@ -14478,11 +14574,11 @@
         <f t="shared" si="6"/>
         <v>hts_mod_fac_ndx</v>
       </c>
-      <c r="AG127" t="s">
+      <c r="AH127" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="128" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>509</v>
       </c>
@@ -14514,11 +14610,11 @@
         <f t="shared" si="6"/>
         <v>hts_mod_com_mob</v>
       </c>
-      <c r="AG128" t="s">
+      <c r="AH128" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="129" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>509</v>
       </c>
@@ -14550,11 +14646,11 @@
         <f t="shared" si="6"/>
         <v>hts_mod_com_vct</v>
       </c>
-      <c r="AG129" t="s">
+      <c r="AH129" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="130" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>509</v>
       </c>
@@ -14586,11 +14682,11 @@
         <f t="shared" si="6"/>
         <v>hts_mod_com_otr</v>
       </c>
-      <c r="AG130" t="s">
+      <c r="AH130" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="131" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>509</v>
       </c>
@@ -14622,11 +14718,11 @@
         <f t="shared" si="6"/>
         <v>hts_mod_fac_ew</v>
       </c>
-      <c r="AG131" t="s">
+      <c r="AH131" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="132" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>509</v>
       </c>
@@ -14658,11 +14754,11 @@
         <f t="shared" si="6"/>
         <v>hts_mod_fac_inpat</v>
       </c>
-      <c r="AG132" t="s">
+      <c r="AH132" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="133" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>509</v>
       </c>
@@ -14694,11 +14790,11 @@
         <f t="shared" si="5"/>
         <v>hts_mod_fac_nut</v>
       </c>
-      <c r="AG133" t="s">
+      <c r="AH133" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="134" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>509</v>
       </c>
@@ -14730,11 +14826,11 @@
         <f t="shared" si="5"/>
         <v>hts_mod_fac_ped</v>
       </c>
-      <c r="AG134" t="s">
+      <c r="AH134" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="135" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>509</v>
       </c>
@@ -14763,14 +14859,14 @@
         <v>1</v>
       </c>
       <c r="J135" t="str">
-        <f t="shared" ref="J135:J140" si="7">_xlfn.TEXTJOIN(";",1,K135:ZZ135)</f>
+        <f t="shared" ref="J135:J140" si="7">_xlfn.TEXTJOIN(";",1,K135:AAA135)</f>
         <v>hts_mod_fac_sti</v>
       </c>
-      <c r="AG135" t="s">
+      <c r="AH135" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="136" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>509</v>
       </c>
@@ -14802,11 +14898,11 @@
         <f t="shared" si="7"/>
         <v>hts_mod_fac_vct</v>
       </c>
-      <c r="AG136" t="s">
+      <c r="AH136" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="137" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>509</v>
       </c>
@@ -14838,11 +14934,11 @@
         <f t="shared" si="7"/>
         <v>hts_mod_fac_otr_pitc</v>
       </c>
-      <c r="AG137" t="s">
+      <c r="AH137" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="138" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>509</v>
       </c>
@@ -14874,11 +14970,11 @@
         <f t="shared" si="7"/>
         <v>hts_mod_fac_vmmc</v>
       </c>
-      <c r="AG138" t="s">
+      <c r="AH138" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="139" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>509</v>
       </c>
@@ -14910,11 +15006,11 @@
         <f t="shared" si="7"/>
         <v>hts_mod_fac_anc_1</v>
       </c>
-      <c r="AG139" t="s">
+      <c r="AH139" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="140" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>509</v>
       </c>
@@ -14946,11 +15042,11 @@
         <f t="shared" si="7"/>
         <v>hts_mod_fac_tb</v>
       </c>
-      <c r="AG140" t="s">
+      <c r="AH140" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="141" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>509</v>
       </c>
@@ -14979,14 +15075,14 @@
         <v>1</v>
       </c>
       <c r="J141" t="str">
-        <f t="shared" ref="J141" si="8">_xlfn.TEXTJOIN(";",1,K141:ZZ141)</f>
+        <f t="shared" ref="J141" si="8">_xlfn.TEXTJOIN(";",1,K141:AAA141)</f>
         <v>hts_mod_fac_post_anc_1</v>
       </c>
-      <c r="AG141" t="s">
+      <c r="AH141" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="142" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>174</v>
       </c>
@@ -15015,7 +15111,7 @@
         <v>1</v>
       </c>
       <c r="J142" s="4" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K142:ZZ142)</f>
+        <f>_xlfn.TEXTJOIN(";",1,K142:AAA142)</f>
         <v>U_age</v>
       </c>
       <c r="K142" s="9"/>
@@ -15026,11 +15122,12 @@
       <c r="Q142" s="9"/>
       <c r="R142" s="9"/>
       <c r="T142" s="9"/>
-      <c r="AG142" t="s">
+      <c r="U142" s="9"/>
+      <c r="AH142" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="143" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>175</v>
       </c>
@@ -15059,16 +15156,22 @@
         <v>1</v>
       </c>
       <c r="J143" s="4" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K143:ZZ143)</f>
+        <f>_xlfn.TEXTJOIN(";",1,K143:AAA143)</f>
         <v>U_sex</v>
       </c>
-      <c r="AG143" t="s">
+      <c r="AH143" t="s">
         <v>522</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AF143" xr:uid="{F5070472-BD41-FC47-BC46-FB0AD4499DE3}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:W66">
+  <autoFilter ref="A1:AG143" xr:uid="{F5070472-BD41-FC47-BC46-FB0AD4499DE3}">
+    <filterColumn colId="10">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:X66">
     <sortCondition ref="H4:H66"/>
   </sortState>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
dim item sets add unknown age dimension for <1-50+.<15/>15.d.u
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB66851-892D-4045-8626-025E593D4C8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B386756-DF89-8148-97EB-A25369B81656}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14700" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3564" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3671" uniqueCount="659">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -2000,7 +2000,19 @@
     <t>([HTS_SELF (N, Age/Sex/HIVSelfTest).T_1] - [HTS_SELF (N, Age/Sex/HIVSelfTest).R]) / [HTS_SELF (N, Age/Sex/HIVSelfTest).R]</t>
   </si>
   <si>
-    <t>&lt;1-50+.&lt;15/&gt;15.d</t>
+    <t>TX_CURR.N.Age_Sex_HIVStatus.R</t>
+  </si>
+  <si>
+    <t>VqlLJRUf0BK</t>
+  </si>
+  <si>
+    <t>TX_CURR (DSD+TA, Age/Sex/HIVStatus)</t>
+  </si>
+  <si>
+    <t>2019Q3</t>
+  </si>
+  <si>
+    <t>&lt;1-50+.&lt;15/&gt;15.d.u</t>
   </si>
 </sst>
 </file>
@@ -2430,13 +2442,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
-  <dimension ref="A1:AK62"/>
+  <dimension ref="A1:AK63"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L47" sqref="L47"/>
+      <selection pane="bottomRight" activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9462,6 +9474,41 @@
         <v>143</v>
       </c>
     </row>
+    <row r="63" spans="1:37" ht="18" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>19</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>654</v>
+      </c>
+      <c r="C63" t="s">
+        <v>2</v>
+      </c>
+      <c r="D63" s="15" t="s">
+        <v>654</v>
+      </c>
+      <c r="E63" t="s">
+        <v>3</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H63" s="16" t="s">
+        <v>656</v>
+      </c>
+      <c r="I63" s="16" t="s">
+        <v>655</v>
+      </c>
+      <c r="J63" t="s">
+        <v>657</v>
+      </c>
+      <c r="K63" s="9" t="s">
+        <v>658</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AK60" xr:uid="{6F439630-CB66-7E4E-9544-3F25521DB3EB}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9470,11 +9517,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:AH143"/>
+  <dimension ref="A1:AH155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AH13" sqref="AH13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9557,7 +9603,7 @@
         <v>183</v>
       </c>
       <c r="U1" s="9" t="s">
-        <v>654</v>
+        <v>658</v>
       </c>
       <c r="V1" t="s">
         <v>216</v>
@@ -9599,7 +9645,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="2" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>174</v>
       </c>
@@ -9644,7 +9690,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="3" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>174</v>
       </c>
@@ -9719,7 +9765,7 @@
       </c>
       <c r="J4" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;1-50+;&lt;1-18+;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;1-50+;&lt;1-18+;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>149</v>
@@ -9731,10 +9777,10 @@
         <v>229</v>
       </c>
       <c r="U4" s="9" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>174</v>
       </c>
@@ -9764,17 +9810,17 @@
       </c>
       <c r="J5" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="O5" s="9"/>
       <c r="P5" s="9" t="s">
         <v>171</v>
       </c>
       <c r="U5" s="9" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>174</v>
       </c>
@@ -9837,7 +9883,7 @@
       </c>
       <c r="J7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;&lt;1-18+;1-4;1-50+/&lt;5;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;1-50+;1-50+;&lt;1-18+;1-4;1-50+/&lt;5;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K7" s="9" t="s">
         <v>149</v>
@@ -9857,7 +9903,7 @@
         <v>226</v>
       </c>
       <c r="U7" s="9" t="s">
-        <v>654</v>
+        <v>658</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.2">
@@ -9890,7 +9936,7 @@
       </c>
       <c r="J8" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;&lt;1-18+;1-4;1-50+/&lt;5;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;1-50+;1-50+;&lt;1-18+;1-4;1-50+/&lt;5;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K8" s="9" t="s">
         <v>149</v>
@@ -9910,10 +9956,10 @@
         <v>226</v>
       </c>
       <c r="U8" s="9" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="9" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>174</v>
       </c>
@@ -9943,16 +9989,16 @@
       </c>
       <c r="J9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="P9" s="9" t="s">
         <v>171</v>
       </c>
       <c r="U9" s="9" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="10" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>174</v>
       </c>
@@ -10021,7 +10067,7 @@
       </c>
       <c r="J11" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;&lt;1-18+;1-50+/&lt;5;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;1-50+;1-50+;&lt;1-18+;1-50+/&lt;5;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K11" s="9" t="s">
         <v>149</v>
@@ -10038,7 +10084,7 @@
         <v>226</v>
       </c>
       <c r="U11" s="9" t="s">
-        <v>654</v>
+        <v>658</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.2">
@@ -10071,7 +10117,7 @@
       </c>
       <c r="J12" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;&lt;1-18+;1-50+/&lt;5;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;1-50+;1-50+;&lt;1-18+;1-50+/&lt;5;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K12" s="9" t="s">
         <v>149</v>
@@ -10088,10 +10134,10 @@
         <v>226</v>
       </c>
       <c r="U12" s="9" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="13" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>174</v>
       </c>
@@ -10121,13 +10167,13 @@
       </c>
       <c r="J13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="P13" s="9" t="s">
         <v>171</v>
       </c>
       <c r="U13" s="9" t="s">
-        <v>654</v>
+        <v>658</v>
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.2">
@@ -10160,7 +10206,7 @@
       </c>
       <c r="J14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;10-50+;&lt;1-18+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;1-50+;1-50+;10-50+;&lt;1-18+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K14" s="9" t="s">
         <v>149</v>
@@ -10182,10 +10228,10 @@
         <v>183</v>
       </c>
       <c r="U14" s="9" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="15" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>174</v>
       </c>
@@ -10215,16 +10261,16 @@
       </c>
       <c r="J15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="P15" s="9" t="s">
         <v>171</v>
       </c>
       <c r="U15" s="9" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="16" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>143</v>
       </c>
@@ -10266,7 +10312,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>174</v>
       </c>
@@ -10304,7 +10350,7 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>143</v>
       </c>
@@ -10340,7 +10386,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>174</v>
       </c>
@@ -10376,7 +10422,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="20" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>174</v>
       </c>
@@ -10406,13 +10452,13 @@
       </c>
       <c r="J20" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="P20" s="9" t="s">
         <v>171</v>
       </c>
       <c r="U20" s="9" t="s">
-        <v>654</v>
+        <v>658</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.2">
@@ -10445,7 +10491,7 @@
       </c>
       <c r="J21" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K21" s="9" t="s">
         <v>149</v>
@@ -10466,10 +10512,10 @@
         <v>183</v>
       </c>
       <c r="U21" s="9" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>143</v>
       </c>
@@ -10511,7 +10557,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>174</v>
       </c>
@@ -10547,7 +10593,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="24" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>143</v>
       </c>
@@ -10589,7 +10635,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="25" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>174</v>
       </c>
@@ -10630,7 +10676,7 @@
       </c>
       <c r="P25" s="5"/>
     </row>
-    <row r="26" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>174</v>
       </c>
@@ -10671,7 +10717,7 @@
       </c>
       <c r="P26" s="5"/>
     </row>
-    <row r="27" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>174</v>
       </c>
@@ -10701,13 +10747,13 @@
       </c>
       <c r="J27" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="P27" s="9" t="s">
         <v>171</v>
       </c>
       <c r="U27" s="9" t="s">
-        <v>654</v>
+        <v>658</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.2">
@@ -10740,7 +10786,7 @@
       </c>
       <c r="J28" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K28" s="9" t="s">
         <v>149</v>
@@ -10761,10 +10807,10 @@
         <v>183</v>
       </c>
       <c r="U28" s="9" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>143</v>
       </c>
@@ -10806,7 +10852,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>174</v>
       </c>
@@ -10836,13 +10882,13 @@
       </c>
       <c r="J30" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="P30" s="9" t="s">
         <v>171</v>
       </c>
       <c r="U30" s="9" t="s">
-        <v>654</v>
+        <v>658</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.2">
@@ -10875,7 +10921,7 @@
       </c>
       <c r="J31" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K31" s="9" t="s">
         <v>149</v>
@@ -10898,10 +10944,10 @@
         <v>183</v>
       </c>
       <c r="U31" s="9" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>174</v>
       </c>
@@ -10937,7 +10983,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="33" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>143</v>
       </c>
@@ -10979,7 +11025,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="34" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>174</v>
       </c>
@@ -11015,7 +11061,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="35" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>174</v>
       </c>
@@ -11045,16 +11091,16 @@
       </c>
       <c r="J35" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="P35" s="9" t="s">
         <v>171</v>
       </c>
       <c r="U35" s="9" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>174</v>
       </c>
@@ -11120,7 +11166,7 @@
       </c>
       <c r="J37" s="4" t="str">
         <f t="shared" ref="J37:J70" si="2">_xlfn.TEXTJOIN(";",1,K37:AAA37)</f>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K37" s="9" t="s">
         <v>149</v>
@@ -11143,10 +11189,10 @@
         <v>183</v>
       </c>
       <c r="U37" s="9" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>143</v>
       </c>
@@ -11188,7 +11234,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="39" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>174</v>
       </c>
@@ -11218,16 +11264,16 @@
       </c>
       <c r="J39" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="P39" s="9" t="s">
         <v>171</v>
       </c>
       <c r="U39" s="9" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>174</v>
       </c>
@@ -11293,7 +11339,7 @@
       </c>
       <c r="J41" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K41" s="9" t="s">
         <v>149</v>
@@ -11314,10 +11360,10 @@
         <v>183</v>
       </c>
       <c r="U41" s="9" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>143</v>
       </c>
@@ -11389,7 +11435,7 @@
       </c>
       <c r="J43" s="4" t="str">
         <f t="shared" ref="J43" si="3">_xlfn.TEXTJOIN(";",1,K43:AAA43)</f>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K43" s="9" t="s">
         <v>149</v>
@@ -11410,10 +11456,10 @@
         <v>183</v>
       </c>
       <c r="U43" s="9" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>174</v>
       </c>
@@ -11443,16 +11489,16 @@
       </c>
       <c r="J44" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="P44" s="9" t="s">
         <v>171</v>
       </c>
       <c r="U44" s="9" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>174</v>
       </c>
@@ -11518,7 +11564,7 @@
       </c>
       <c r="J46" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K46" s="9" t="s">
         <v>149</v>
@@ -11539,10 +11585,10 @@
         <v>183</v>
       </c>
       <c r="U46" s="9" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>143</v>
       </c>
@@ -11614,7 +11660,7 @@
       </c>
       <c r="J48" s="4" t="str">
         <f t="shared" ref="J48" si="4">_xlfn.TEXTJOIN(";",1,K48:AAA48)</f>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K48" s="9" t="s">
         <v>149</v>
@@ -11635,10 +11681,10 @@
         <v>183</v>
       </c>
       <c r="U48" s="9" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="49" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>174</v>
       </c>
@@ -11668,16 +11714,16 @@
       </c>
       <c r="J49" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="P49" s="9" t="s">
         <v>171</v>
       </c>
       <c r="U49" s="9" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="50" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>174</v>
       </c>
@@ -11743,7 +11789,7 @@
       </c>
       <c r="J51" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K51" s="9" t="s">
         <v>149</v>
@@ -11764,10 +11810,10 @@
         <v>183</v>
       </c>
       <c r="U51" s="9" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="52" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>143</v>
       </c>
@@ -11809,7 +11855,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="53" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>174</v>
       </c>
@@ -11839,13 +11885,13 @@
       </c>
       <c r="J53" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="P53" s="9" t="s">
         <v>171</v>
       </c>
       <c r="U53" s="9" t="s">
-        <v>654</v>
+        <v>658</v>
       </c>
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.2">
@@ -11878,7 +11924,7 @@
       </c>
       <c r="J54" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d</v>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K54" s="9" t="s">
         <v>149</v>
@@ -11899,10 +11945,10 @@
         <v>183</v>
       </c>
       <c r="U54" s="9" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="55" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>143</v>
       </c>
@@ -11944,7 +11990,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="56" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>175</v>
       </c>
@@ -11986,7 +12032,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="57" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>143</v>
       </c>
@@ -12028,7 +12074,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="58" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>175</v>
       </c>
@@ -12073,7 +12119,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="59" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>175</v>
       </c>
@@ -12118,7 +12164,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="60" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>143</v>
       </c>
@@ -12160,7 +12206,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="61" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>175</v>
       </c>
@@ -12202,7 +12248,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="62" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>184</v>
       </c>
@@ -12238,7 +12284,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="63" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>184</v>
       </c>
@@ -12274,7 +12320,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="64" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>184</v>
       </c>
@@ -12310,7 +12356,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="65" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>184</v>
       </c>
@@ -12346,7 +12392,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="66" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>184</v>
       </c>
@@ -12382,7 +12428,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="67" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>196</v>
       </c>
@@ -12418,7 +12464,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="68" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>196</v>
       </c>
@@ -12454,7 +12500,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="69" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>264</v>
       </c>
@@ -12490,7 +12536,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="70" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>264</v>
       </c>
@@ -12526,7 +12572,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="71" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>264</v>
       </c>
@@ -12562,7 +12608,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="72" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>278</v>
       </c>
@@ -12598,7 +12644,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="73" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>278</v>
       </c>
@@ -12634,7 +12680,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="74" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>278</v>
       </c>
@@ -12670,7 +12716,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="75" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>278</v>
       </c>
@@ -12706,7 +12752,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="76" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>278</v>
       </c>
@@ -12742,7 +12788,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="77" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>278</v>
       </c>
@@ -12778,7 +12824,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="78" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>278</v>
       </c>
@@ -12814,7 +12860,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="79" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>278</v>
       </c>
@@ -12850,7 +12896,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="80" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>278</v>
       </c>
@@ -12886,7 +12932,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="81" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>278</v>
       </c>
@@ -12922,7 +12968,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="82" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>278</v>
       </c>
@@ -12958,7 +13004,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="83" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>278</v>
       </c>
@@ -12994,7 +13040,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="84" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>278</v>
       </c>
@@ -13030,7 +13076,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="85" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>278</v>
       </c>
@@ -13066,7 +13112,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="86" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>278</v>
       </c>
@@ -13102,7 +13148,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="87" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>278</v>
       </c>
@@ -13138,7 +13184,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="88" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>278</v>
       </c>
@@ -13174,7 +13220,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="89" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>278</v>
       </c>
@@ -13210,7 +13256,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="90" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>278</v>
       </c>
@@ -13246,7 +13292,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="91" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>278</v>
       </c>
@@ -13282,7 +13328,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="92" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>278</v>
       </c>
@@ -13318,7 +13364,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="93" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>278</v>
       </c>
@@ -13354,7 +13400,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="94" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>278</v>
       </c>
@@ -13390,7 +13436,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="95" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>278</v>
       </c>
@@ -13426,7 +13472,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="96" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>278</v>
       </c>
@@ -13462,7 +13508,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="97" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>278</v>
       </c>
@@ -13498,7 +13544,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="98" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>278</v>
       </c>
@@ -13534,7 +13580,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="99" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>278</v>
       </c>
@@ -13570,7 +13616,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="100" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>278</v>
       </c>
@@ -13606,7 +13652,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="101" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>278</v>
       </c>
@@ -13642,7 +13688,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="102" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>278</v>
       </c>
@@ -13678,7 +13724,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="103" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>278</v>
       </c>
@@ -13714,7 +13760,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="104" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>278</v>
       </c>
@@ -13750,7 +13796,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="105" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>278</v>
       </c>
@@ -13786,7 +13832,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="106" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>278</v>
       </c>
@@ -13822,7 +13868,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="107" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>278</v>
       </c>
@@ -13858,7 +13904,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="108" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>278</v>
       </c>
@@ -13894,7 +13940,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="109" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>278</v>
       </c>
@@ -13930,7 +13976,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="110" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>278</v>
       </c>
@@ -13966,7 +14012,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="111" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>278</v>
       </c>
@@ -14002,7 +14048,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="112" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>278</v>
       </c>
@@ -14038,7 +14084,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="113" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>278</v>
       </c>
@@ -14074,7 +14120,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="114" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>381</v>
       </c>
@@ -14110,7 +14156,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="115" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>381</v>
       </c>
@@ -14146,7 +14192,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="116" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>278</v>
       </c>
@@ -14182,7 +14228,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="117" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>278</v>
       </c>
@@ -14218,7 +14264,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="118" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>278</v>
       </c>
@@ -14254,7 +14300,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="119" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>278</v>
       </c>
@@ -14290,7 +14336,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="120" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>278</v>
       </c>
@@ -14326,7 +14372,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="121" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>278</v>
       </c>
@@ -14362,7 +14408,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="122" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>278</v>
       </c>
@@ -14398,7 +14444,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="123" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>278</v>
       </c>
@@ -14434,7 +14480,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="124" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>196</v>
       </c>
@@ -14470,7 +14516,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="125" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>196</v>
       </c>
@@ -14506,7 +14552,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="126" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>509</v>
       </c>
@@ -14542,7 +14588,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="127" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>509</v>
       </c>
@@ -14578,7 +14624,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="128" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>509</v>
       </c>
@@ -14614,7 +14660,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="129" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>509</v>
       </c>
@@ -14650,7 +14696,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="130" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>509</v>
       </c>
@@ -14686,7 +14732,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="131" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>509</v>
       </c>
@@ -14722,7 +14768,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="132" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>509</v>
       </c>
@@ -14758,7 +14804,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="133" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>509</v>
       </c>
@@ -14794,7 +14840,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="134" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>509</v>
       </c>
@@ -14830,7 +14876,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="135" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>509</v>
       </c>
@@ -14866,7 +14912,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="136" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>509</v>
       </c>
@@ -14902,7 +14948,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="137" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>509</v>
       </c>
@@ -14938,7 +14984,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="138" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>509</v>
       </c>
@@ -14974,7 +15020,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="139" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>509</v>
       </c>
@@ -15010,7 +15056,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="140" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>509</v>
       </c>
@@ -15046,7 +15092,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="141" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>509</v>
       </c>
@@ -15082,7 +15128,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="142" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>174</v>
       </c>
@@ -15127,7 +15173,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="143" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>175</v>
       </c>
@@ -15163,14 +15209,440 @@
         <v>522</v>
       </c>
     </row>
+    <row r="144" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>174</v>
+      </c>
+      <c r="B144" t="s">
+        <v>233</v>
+      </c>
+      <c r="C144" t="s">
+        <v>519</v>
+      </c>
+      <c r="D144" t="s">
+        <v>217</v>
+      </c>
+      <c r="E144" t="s">
+        <v>520</v>
+      </c>
+      <c r="F144" t="s">
+        <v>99</v>
+      </c>
+      <c r="G144" t="s">
+        <v>114</v>
+      </c>
+      <c r="H144" s="7">
+        <v>10</v>
+      </c>
+      <c r="I144" s="13">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="J144" s="4" t="str">
+        <f t="shared" ref="J144:J155" si="9">_xlfn.TEXTJOIN(";",1,K144:AAA144)</f>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
+      </c>
+      <c r="U144" s="9" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="145" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>174</v>
+      </c>
+      <c r="B145" t="s">
+        <v>233</v>
+      </c>
+      <c r="C145" t="s">
+        <v>519</v>
+      </c>
+      <c r="D145" t="s">
+        <v>217</v>
+      </c>
+      <c r="E145" t="s">
+        <v>520</v>
+      </c>
+      <c r="F145" t="s">
+        <v>97</v>
+      </c>
+      <c r="G145" t="s">
+        <v>117</v>
+      </c>
+      <c r="H145" s="6">
+        <v>15</v>
+      </c>
+      <c r="I145" s="13">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="J145" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
+      </c>
+      <c r="U145" s="9" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="146" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>174</v>
+      </c>
+      <c r="B146" t="s">
+        <v>233</v>
+      </c>
+      <c r="C146" t="s">
+        <v>519</v>
+      </c>
+      <c r="D146" t="s">
+        <v>217</v>
+      </c>
+      <c r="E146" t="s">
+        <v>520</v>
+      </c>
+      <c r="F146" t="s">
+        <v>98</v>
+      </c>
+      <c r="G146" t="s">
+        <v>127</v>
+      </c>
+      <c r="H146" s="7">
+        <v>30</v>
+      </c>
+      <c r="I146" s="13">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="J146" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
+      </c>
+      <c r="U146" s="9" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="147" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>174</v>
+      </c>
+      <c r="B147" t="s">
+        <v>233</v>
+      </c>
+      <c r="C147" t="s">
+        <v>519</v>
+      </c>
+      <c r="D147" t="s">
+        <v>217</v>
+      </c>
+      <c r="E147" t="s">
+        <v>520</v>
+      </c>
+      <c r="F147" t="s">
+        <v>106</v>
+      </c>
+      <c r="G147" t="s">
+        <v>118</v>
+      </c>
+      <c r="H147" s="7">
+        <v>40</v>
+      </c>
+      <c r="I147" s="13">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="J147" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
+      </c>
+      <c r="U147" s="9" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="148" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>174</v>
+      </c>
+      <c r="B148" t="s">
+        <v>233</v>
+      </c>
+      <c r="C148" t="s">
+        <v>519</v>
+      </c>
+      <c r="D148" t="s">
+        <v>217</v>
+      </c>
+      <c r="E148" t="s">
+        <v>520</v>
+      </c>
+      <c r="F148" t="s">
+        <v>108</v>
+      </c>
+      <c r="G148" t="s">
+        <v>120</v>
+      </c>
+      <c r="H148" s="7">
+        <v>60</v>
+      </c>
+      <c r="I148" s="13">
+        <v>8.3400000000000002E-2</v>
+      </c>
+      <c r="J148" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
+      </c>
+      <c r="U148" s="9" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="149" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>174</v>
+      </c>
+      <c r="B149" t="s">
+        <v>233</v>
+      </c>
+      <c r="C149" t="s">
+        <v>519</v>
+      </c>
+      <c r="D149" t="s">
+        <v>217</v>
+      </c>
+      <c r="E149" t="s">
+        <v>520</v>
+      </c>
+      <c r="F149" t="s">
+        <v>109</v>
+      </c>
+      <c r="G149" t="s">
+        <v>121</v>
+      </c>
+      <c r="H149" s="7">
+        <v>80</v>
+      </c>
+      <c r="I149" s="13">
+        <v>8.3400000000000002E-2</v>
+      </c>
+      <c r="J149" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
+      </c>
+      <c r="U149" s="9" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="150" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>174</v>
+      </c>
+      <c r="B150" t="s">
+        <v>233</v>
+      </c>
+      <c r="C150" t="s">
+        <v>519</v>
+      </c>
+      <c r="D150" t="s">
+        <v>217</v>
+      </c>
+      <c r="E150" t="s">
+        <v>520</v>
+      </c>
+      <c r="F150" t="s">
+        <v>100</v>
+      </c>
+      <c r="G150" t="s">
+        <v>122</v>
+      </c>
+      <c r="H150" s="7">
+        <v>90</v>
+      </c>
+      <c r="I150" s="13">
+        <v>8.3400000000000002E-2</v>
+      </c>
+      <c r="J150" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
+      </c>
+      <c r="U150" s="9" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="151" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>174</v>
+      </c>
+      <c r="B151" t="s">
+        <v>233</v>
+      </c>
+      <c r="C151" t="s">
+        <v>519</v>
+      </c>
+      <c r="D151" t="s">
+        <v>217</v>
+      </c>
+      <c r="E151" t="s">
+        <v>520</v>
+      </c>
+      <c r="F151" t="s">
+        <v>101</v>
+      </c>
+      <c r="G151" t="s">
+        <v>123</v>
+      </c>
+      <c r="H151" s="7">
+        <v>110</v>
+      </c>
+      <c r="I151" s="13">
+        <v>8.3400000000000002E-2</v>
+      </c>
+      <c r="J151" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
+      </c>
+      <c r="U151" s="9" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="152" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>174</v>
+      </c>
+      <c r="B152" t="s">
+        <v>233</v>
+      </c>
+      <c r="C152" t="s">
+        <v>519</v>
+      </c>
+      <c r="D152" t="s">
+        <v>217</v>
+      </c>
+      <c r="E152" t="s">
+        <v>520</v>
+      </c>
+      <c r="F152" t="s">
+        <v>102</v>
+      </c>
+      <c r="G152" t="s">
+        <v>124</v>
+      </c>
+      <c r="H152" s="7">
+        <v>120</v>
+      </c>
+      <c r="I152" s="13">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="J152" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
+      </c>
+      <c r="U152" s="9" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="153" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>174</v>
+      </c>
+      <c r="B153" t="s">
+        <v>233</v>
+      </c>
+      <c r="C153" t="s">
+        <v>519</v>
+      </c>
+      <c r="D153" t="s">
+        <v>217</v>
+      </c>
+      <c r="E153" t="s">
+        <v>520</v>
+      </c>
+      <c r="F153" t="s">
+        <v>103</v>
+      </c>
+      <c r="G153" t="s">
+        <v>125</v>
+      </c>
+      <c r="H153" s="7">
+        <v>130</v>
+      </c>
+      <c r="I153" s="13">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="J153" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
+      </c>
+      <c r="U153" s="9" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="154" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>174</v>
+      </c>
+      <c r="B154" t="s">
+        <v>233</v>
+      </c>
+      <c r="C154" t="s">
+        <v>519</v>
+      </c>
+      <c r="D154" t="s">
+        <v>217</v>
+      </c>
+      <c r="E154" t="s">
+        <v>520</v>
+      </c>
+      <c r="F154" t="s">
+        <v>104</v>
+      </c>
+      <c r="G154" t="s">
+        <v>126</v>
+      </c>
+      <c r="H154" s="7">
+        <v>140</v>
+      </c>
+      <c r="I154" s="13">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="J154" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
+      </c>
+      <c r="U154" s="9" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="155" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>174</v>
+      </c>
+      <c r="B155" t="s">
+        <v>233</v>
+      </c>
+      <c r="C155" t="s">
+        <v>519</v>
+      </c>
+      <c r="D155" t="s">
+        <v>217</v>
+      </c>
+      <c r="E155" t="s">
+        <v>520</v>
+      </c>
+      <c r="F155" t="s">
+        <v>105</v>
+      </c>
+      <c r="G155" t="s">
+        <v>116</v>
+      </c>
+      <c r="H155" s="7">
+        <v>150</v>
+      </c>
+      <c r="I155" s="13">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="J155" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
+      </c>
+      <c r="U155" s="9" t="s">
+        <v>658</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AG143" xr:uid="{F5070472-BD41-FC47-BC46-FB0AD4499DE3}">
-    <filterColumn colId="10">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AG143" xr:uid="{F5070472-BD41-FC47-BC46-FB0AD4499DE3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:X66">
     <sortCondition ref="H4:H66"/>
   </sortState>

</xml_diff>

<commit_message>
data required adding TX_CURR AND TX_NEW results
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B386756-DF89-8148-97EB-A25369B81656}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626D366E-EDCC-974E-9E89-CC583E1F1FDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3671" uniqueCount="659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3734" uniqueCount="662">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -2013,6 +2013,15 @@
   </si>
   <si>
     <t>&lt;1-50+.&lt;15/&gt;15.d.u</t>
+  </si>
+  <si>
+    <t>TX_NEW.N.Age_Sex_HIVStatus.R</t>
+  </si>
+  <si>
+    <t>TX_NEW (DSD+TA, Age/Sex/HIV Status)</t>
+  </si>
+  <si>
+    <t>sPLZOoumW9X</t>
   </si>
 </sst>
 </file>
@@ -2442,13 +2451,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
-  <dimension ref="A1:AK63"/>
+  <dimension ref="A1:AK65"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G35" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="AE35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H64" sqref="H64"/>
+      <selection pane="bottomRight" activeCell="AR64" sqref="AR64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9508,6 +9517,200 @@
       <c r="K63" s="9" t="s">
         <v>658</v>
       </c>
+      <c r="L63" t="s">
+        <v>145</v>
+      </c>
+      <c r="M63" t="s">
+        <v>143</v>
+      </c>
+      <c r="N63" t="s">
+        <v>143</v>
+      </c>
+      <c r="O63" t="s">
+        <v>143</v>
+      </c>
+      <c r="P63" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>143</v>
+      </c>
+      <c r="R63" t="s">
+        <v>143</v>
+      </c>
+      <c r="S63" t="s">
+        <v>143</v>
+      </c>
+      <c r="T63" t="s">
+        <v>143</v>
+      </c>
+      <c r="U63" t="s">
+        <v>143</v>
+      </c>
+      <c r="V63" t="s">
+        <v>143</v>
+      </c>
+      <c r="W63" t="s">
+        <v>143</v>
+      </c>
+      <c r="X63" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y63" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z63" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA63" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB63" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC63" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD63" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE63" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF63" t="s">
+        <v>143</v>
+      </c>
+      <c r="AG63" t="s">
+        <v>143</v>
+      </c>
+      <c r="AH63" t="s">
+        <v>143</v>
+      </c>
+      <c r="AI63" t="s">
+        <v>143</v>
+      </c>
+      <c r="AJ63" t="s">
+        <v>143</v>
+      </c>
+      <c r="AK63" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="64" spans="1:37" ht="18" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>19</v>
+      </c>
+      <c r="B64" s="15" t="s">
+        <v>659</v>
+      </c>
+      <c r="C64" t="s">
+        <v>2</v>
+      </c>
+      <c r="D64" s="16" t="s">
+        <v>660</v>
+      </c>
+      <c r="E64" t="s">
+        <v>3</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H64" s="16" t="s">
+        <v>660</v>
+      </c>
+      <c r="I64" s="16" t="s">
+        <v>661</v>
+      </c>
+      <c r="J64" t="s">
+        <v>139</v>
+      </c>
+      <c r="K64" s="9" t="s">
+        <v>658</v>
+      </c>
+      <c r="L64" t="s">
+        <v>145</v>
+      </c>
+      <c r="M64" t="s">
+        <v>143</v>
+      </c>
+      <c r="N64" t="s">
+        <v>143</v>
+      </c>
+      <c r="O64" t="s">
+        <v>143</v>
+      </c>
+      <c r="P64" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>143</v>
+      </c>
+      <c r="R64" t="s">
+        <v>143</v>
+      </c>
+      <c r="S64" t="s">
+        <v>143</v>
+      </c>
+      <c r="T64" t="s">
+        <v>143</v>
+      </c>
+      <c r="U64" t="s">
+        <v>143</v>
+      </c>
+      <c r="V64" t="s">
+        <v>143</v>
+      </c>
+      <c r="W64" t="s">
+        <v>143</v>
+      </c>
+      <c r="X64" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y64" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z64" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA64" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB64" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC64" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD64" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE64" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF64" t="s">
+        <v>143</v>
+      </c>
+      <c r="AG64" t="s">
+        <v>143</v>
+      </c>
+      <c r="AH64" t="s">
+        <v>143</v>
+      </c>
+      <c r="AI64" t="s">
+        <v>143</v>
+      </c>
+      <c r="AJ64" t="s">
+        <v>143</v>
+      </c>
+      <c r="AK64" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="B65" s="16"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AK60" xr:uid="{6F439630-CB66-7E4E-9544-3F25521DB3EB}"/>
@@ -9519,8 +9722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
   <dimension ref="A1:AH155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AH13" sqref="AH13"/>
+    <sheetView topLeftCell="B4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
data_required dim_item_sets add new indicators
https://github.com/pepfar-datim/COP-Target-Setting/issues/566
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626D366E-EDCC-974E-9E89-CC583E1F1FDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C6CA49-61CC-0D4B-8084-D7581BD94C6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3734" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3952" uniqueCount="680">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -2022,6 +2022,212 @@
   </si>
   <si>
     <t>sPLZOoumW9X</t>
+  </si>
+  <si>
+    <t>TX_NEW.N.Age_Sex_HIVStatus.T_1</t>
+  </si>
+  <si>
+    <t>UDW0CSk6bHz</t>
+  </si>
+  <si>
+    <t>TX_NEW (DSD+TA, Age/Sex/HIV Status) TARGET</t>
+  </si>
+  <si>
+    <t>TB_STAT.N.Age_Sex_KnownNewPosNeg.T_1.NewPos</t>
+  </si>
+  <si>
+    <t>TB_STAT (N, DSD+TA, Age/Sex/KnownNewPosNeg) TARGET</t>
+  </si>
+  <si>
+    <t>iu2PV9NpeSd</t>
+  </si>
+  <si>
+    <t>TX_NEW.N.TBRate</t>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>TB_ART, Numerator, New on ART, finer age/sex, FY19 Results</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>] / [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>TX_NEW, finer age/sex, FY19 Results</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t>TB_ART (N, DSD+TA, Age/Sex/NewExistingArt/HIVStatus)</t>
+  </si>
+  <si>
+    <t>TJjb1v6zbUH</t>
+  </si>
+  <si>
+    <t>TX_NEW.N.PMTCTRate</t>
+  </si>
+  <si>
+    <t>TX_NEW.N.PostANC1Rate</t>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>PMTCT_ART, Numerator, New on ART, finer age/sex, FY19 Results</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>] / [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>TX_NEW, finer age/sex, FY19 Results</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>HTS_TST (PMTCT Post ANC1), Positives, finer age/sex, FY19 Results</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>] / [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>TX_NEW, finer age/sex, FY19 Results</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t>TX_NEW.N.VMMCRate</t>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>VMMC_CIRC, Positives, finer age/sex, FY19 Results</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>] / [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>TX_NEW, finer age/sex, FY19 Results</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t>vWBWKmRWFAC</t>
+  </si>
+  <si>
+    <t>FY19 Results Analytic Indicators: PMTCT_ART (NewExistingART)</t>
   </si>
 </sst>
 </file>
@@ -2451,13 +2657,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
-  <dimension ref="A1:AK65"/>
+  <dimension ref="A1:AK70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AE35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AE43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AR64" sqref="AR64"/>
+      <selection pane="bottomRight" activeCell="AR68" sqref="AR68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9709,8 +9915,683 @@
         <v>143</v>
       </c>
     </row>
-    <row r="65" spans="2:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="B65" s="16"/>
+    <row r="65" spans="1:37" ht="19" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>19</v>
+      </c>
+      <c r="B65" s="15" t="s">
+        <v>662</v>
+      </c>
+      <c r="C65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>664</v>
+      </c>
+      <c r="E65" t="s">
+        <v>3</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H65" s="11" t="s">
+        <v>664</v>
+      </c>
+      <c r="I65" s="16" t="s">
+        <v>663</v>
+      </c>
+      <c r="J65" t="s">
+        <v>457</v>
+      </c>
+      <c r="K65" t="s">
+        <v>149</v>
+      </c>
+      <c r="L65" t="s">
+        <v>145</v>
+      </c>
+      <c r="M65" t="s">
+        <v>143</v>
+      </c>
+      <c r="N65" t="s">
+        <v>143</v>
+      </c>
+      <c r="O65" t="s">
+        <v>143</v>
+      </c>
+      <c r="P65" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>143</v>
+      </c>
+      <c r="R65" t="s">
+        <v>143</v>
+      </c>
+      <c r="S65" t="s">
+        <v>143</v>
+      </c>
+      <c r="T65" t="s">
+        <v>143</v>
+      </c>
+      <c r="U65" t="s">
+        <v>143</v>
+      </c>
+      <c r="V65" t="s">
+        <v>143</v>
+      </c>
+      <c r="W65" t="s">
+        <v>143</v>
+      </c>
+      <c r="X65" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y65" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z65" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA65" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB65" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC65" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD65" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE65" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF65" t="s">
+        <v>143</v>
+      </c>
+      <c r="AG65" t="s">
+        <v>143</v>
+      </c>
+      <c r="AH65" t="s">
+        <v>143</v>
+      </c>
+      <c r="AI65" t="s">
+        <v>143</v>
+      </c>
+      <c r="AJ65" t="s">
+        <v>143</v>
+      </c>
+      <c r="AK65" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="66" spans="1:37" ht="18" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>19</v>
+      </c>
+      <c r="B66" s="15" t="s">
+        <v>665</v>
+      </c>
+      <c r="C66" t="s">
+        <v>2</v>
+      </c>
+      <c r="D66" s="15" t="s">
+        <v>665</v>
+      </c>
+      <c r="E66" t="s">
+        <v>3</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H66" t="s">
+        <v>666</v>
+      </c>
+      <c r="I66" t="s">
+        <v>667</v>
+      </c>
+      <c r="J66" t="s">
+        <v>457</v>
+      </c>
+      <c r="K66" t="s">
+        <v>149</v>
+      </c>
+      <c r="L66" t="s">
+        <v>145</v>
+      </c>
+      <c r="M66" t="s">
+        <v>143</v>
+      </c>
+      <c r="N66" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="O66" t="s">
+        <v>143</v>
+      </c>
+      <c r="P66" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>143</v>
+      </c>
+      <c r="R66" t="s">
+        <v>143</v>
+      </c>
+      <c r="S66" t="s">
+        <v>143</v>
+      </c>
+      <c r="T66" t="s">
+        <v>143</v>
+      </c>
+      <c r="U66" t="s">
+        <v>143</v>
+      </c>
+      <c r="V66" t="s">
+        <v>143</v>
+      </c>
+      <c r="W66" t="s">
+        <v>143</v>
+      </c>
+      <c r="X66" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y66" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z66" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA66" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB66" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC66" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD66" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE66" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF66" t="s">
+        <v>143</v>
+      </c>
+      <c r="AG66" t="s">
+        <v>143</v>
+      </c>
+      <c r="AH66" t="s">
+        <v>143</v>
+      </c>
+      <c r="AI66" t="s">
+        <v>143</v>
+      </c>
+      <c r="AJ66" t="s">
+        <v>143</v>
+      </c>
+      <c r="AK66" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="67" spans="1:37" ht="18" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>19</v>
+      </c>
+      <c r="B67" s="15" t="s">
+        <v>668</v>
+      </c>
+      <c r="C67" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" s="16" t="s">
+        <v>669</v>
+      </c>
+      <c r="E67" t="s">
+        <v>6</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H67" t="s">
+        <v>670</v>
+      </c>
+      <c r="I67" t="s">
+        <v>671</v>
+      </c>
+      <c r="J67" t="s">
+        <v>139</v>
+      </c>
+      <c r="K67" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="L67" t="s">
+        <v>145</v>
+      </c>
+      <c r="M67" t="s">
+        <v>143</v>
+      </c>
+      <c r="N67" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="O67" t="s">
+        <v>143</v>
+      </c>
+      <c r="P67" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>143</v>
+      </c>
+      <c r="R67" t="s">
+        <v>143</v>
+      </c>
+      <c r="S67" t="s">
+        <v>143</v>
+      </c>
+      <c r="T67" t="s">
+        <v>143</v>
+      </c>
+      <c r="U67" t="s">
+        <v>143</v>
+      </c>
+      <c r="V67" s="16" t="s">
+        <v>660</v>
+      </c>
+      <c r="W67" s="16" t="s">
+        <v>661</v>
+      </c>
+      <c r="X67" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y67" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z67" t="s">
+        <v>145</v>
+      </c>
+      <c r="AA67" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB67" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC67" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD67" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE67" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF67" t="s">
+        <v>143</v>
+      </c>
+      <c r="AG67" t="s">
+        <v>143</v>
+      </c>
+      <c r="AH67" t="s">
+        <v>143</v>
+      </c>
+      <c r="AI67" t="s">
+        <v>152</v>
+      </c>
+      <c r="AJ67">
+        <v>0</v>
+      </c>
+      <c r="AK67" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="68" spans="1:37" ht="18" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>19</v>
+      </c>
+      <c r="B68" s="15" t="s">
+        <v>672</v>
+      </c>
+      <c r="C68" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" s="16" t="s">
+        <v>674</v>
+      </c>
+      <c r="E68" t="s">
+        <v>6</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H68" t="s">
+        <v>679</v>
+      </c>
+      <c r="I68" t="s">
+        <v>678</v>
+      </c>
+      <c r="J68" t="s">
+        <v>139</v>
+      </c>
+      <c r="K68" t="s">
+        <v>140</v>
+      </c>
+      <c r="L68" t="s">
+        <v>141</v>
+      </c>
+      <c r="M68" t="s">
+        <v>143</v>
+      </c>
+      <c r="N68" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="O68" t="s">
+        <v>143</v>
+      </c>
+      <c r="P68" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>143</v>
+      </c>
+      <c r="R68" t="s">
+        <v>143</v>
+      </c>
+      <c r="S68" t="s">
+        <v>143</v>
+      </c>
+      <c r="T68" t="s">
+        <v>143</v>
+      </c>
+      <c r="U68" t="s">
+        <v>143</v>
+      </c>
+      <c r="V68" s="16" t="s">
+        <v>660</v>
+      </c>
+      <c r="W68" s="16" t="s">
+        <v>661</v>
+      </c>
+      <c r="X68" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y68" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z68" t="s">
+        <v>141</v>
+      </c>
+      <c r="AA68" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB68" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC68" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD68" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE68" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF68" t="s">
+        <v>143</v>
+      </c>
+      <c r="AG68" t="s">
+        <v>143</v>
+      </c>
+      <c r="AH68" t="s">
+        <v>143</v>
+      </c>
+      <c r="AI68" t="s">
+        <v>152</v>
+      </c>
+      <c r="AJ68">
+        <v>0</v>
+      </c>
+      <c r="AK68" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="69" spans="1:37" ht="18" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>19</v>
+      </c>
+      <c r="B69" s="15" t="s">
+        <v>673</v>
+      </c>
+      <c r="C69" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" s="16" t="s">
+        <v>675</v>
+      </c>
+      <c r="E69" t="s">
+        <v>6</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H69" t="s">
+        <v>538</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="J69" t="s">
+        <v>139</v>
+      </c>
+      <c r="K69" t="s">
+        <v>140</v>
+      </c>
+      <c r="L69" t="s">
+        <v>141</v>
+      </c>
+      <c r="M69" t="s">
+        <v>143</v>
+      </c>
+      <c r="N69" t="s">
+        <v>571</v>
+      </c>
+      <c r="O69" t="s">
+        <v>143</v>
+      </c>
+      <c r="P69" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>143</v>
+      </c>
+      <c r="R69" t="s">
+        <v>143</v>
+      </c>
+      <c r="S69" t="s">
+        <v>143</v>
+      </c>
+      <c r="T69" t="s">
+        <v>143</v>
+      </c>
+      <c r="U69" t="s">
+        <v>143</v>
+      </c>
+      <c r="V69" s="16" t="s">
+        <v>660</v>
+      </c>
+      <c r="W69" s="16" t="s">
+        <v>661</v>
+      </c>
+      <c r="X69" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y69" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z69" t="s">
+        <v>141</v>
+      </c>
+      <c r="AA69" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB69" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC69" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD69" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE69" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF69" t="s">
+        <v>143</v>
+      </c>
+      <c r="AG69" t="s">
+        <v>143</v>
+      </c>
+      <c r="AH69" t="s">
+        <v>143</v>
+      </c>
+      <c r="AI69" t="s">
+        <v>152</v>
+      </c>
+      <c r="AJ69">
+        <v>0</v>
+      </c>
+      <c r="AK69" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="70" spans="1:37" ht="18" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>19</v>
+      </c>
+      <c r="B70" s="15" t="s">
+        <v>676</v>
+      </c>
+      <c r="C70" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" s="16" t="s">
+        <v>677</v>
+      </c>
+      <c r="E70" t="s">
+        <v>6</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H70" t="s">
+        <v>538</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="J70" t="s">
+        <v>139</v>
+      </c>
+      <c r="K70" t="s">
+        <v>140</v>
+      </c>
+      <c r="L70" t="s">
+        <v>148</v>
+      </c>
+      <c r="M70" t="s">
+        <v>143</v>
+      </c>
+      <c r="N70" t="s">
+        <v>511</v>
+      </c>
+      <c r="O70" t="s">
+        <v>143</v>
+      </c>
+      <c r="P70" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>143</v>
+      </c>
+      <c r="R70" t="s">
+        <v>143</v>
+      </c>
+      <c r="S70" t="s">
+        <v>143</v>
+      </c>
+      <c r="T70" t="s">
+        <v>143</v>
+      </c>
+      <c r="U70" t="s">
+        <v>143</v>
+      </c>
+      <c r="V70" s="16" t="s">
+        <v>660</v>
+      </c>
+      <c r="W70" s="16" t="s">
+        <v>661</v>
+      </c>
+      <c r="X70" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y70" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z70" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA70" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB70" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC70" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD70" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE70" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF70" t="s">
+        <v>143</v>
+      </c>
+      <c r="AG70" t="s">
+        <v>143</v>
+      </c>
+      <c r="AH70" t="s">
+        <v>143</v>
+      </c>
+      <c r="AI70" t="s">
+        <v>152</v>
+      </c>
+      <c r="AJ70">
+        <v>0</v>
+      </c>
+      <c r="AK70" t="s">
+        <v>143</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:AK60" xr:uid="{6F439630-CB66-7E4E-9544-3F25521DB3EB}"/>
@@ -9722,8 +10603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
   <dimension ref="A1:AH155"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="C94" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J115" sqref="J115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
data_required add tb_prev (N) indicators
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C6CA49-61CC-0D4B-8084-D7581BD94C6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B76DBA4-8FD8-514B-8649-062B72F0589C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3952" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4026" uniqueCount="686">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -2228,6 +2228,24 @@
   </si>
   <si>
     <t>FY19 Results Analytic Indicators: PMTCT_ART (NewExistingART)</t>
+  </si>
+  <si>
+    <t>bQhs5uRiSni</t>
+  </si>
+  <si>
+    <t>TB_PREV (N, DSD+TA, Age/TherapyType/NewExistingArt/HIVStatus) TARGET</t>
+  </si>
+  <si>
+    <t>TB_PREV.N.Age_NewExistingArt_HIVStatus.T_1.New</t>
+  </si>
+  <si>
+    <t>TB_PREV.N.Age_NewExistingArt_HIVStatus.T_1.Already</t>
+  </si>
+  <si>
+    <t>TB_PREV (N, DSD+TA, Age/TherapyType/NewExistingArt/HIVStatus) TARGET New on art</t>
+  </si>
+  <si>
+    <t>TB_PREV (N, DSD+TA, Age/TherapyType/NewExistingArt/HIVStatus) TARGET already on art</t>
   </si>
 </sst>
 </file>
@@ -2657,19 +2675,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
-  <dimension ref="A1:AK70"/>
+  <dimension ref="A1:AK72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AE43" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AR68" sqref="AR68"/>
+      <selection pane="bottomRight" activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.83203125" customWidth="1"/>
+    <col min="2" max="2" width="61" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.1640625" customWidth="1"/>
     <col min="4" max="4" width="255.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
@@ -10593,6 +10611,232 @@
         <v>143</v>
       </c>
     </row>
+    <row r="71" spans="1:37" ht="18" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>43</v>
+      </c>
+      <c r="B71" s="15" t="s">
+        <v>682</v>
+      </c>
+      <c r="C71" t="s">
+        <v>2</v>
+      </c>
+      <c r="D71" t="s">
+        <v>684</v>
+      </c>
+      <c r="E71" t="s">
+        <v>3</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H71" t="s">
+        <v>681</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="J71" t="s">
+        <v>457</v>
+      </c>
+      <c r="K71" s="9" t="s">
+        <v>417</v>
+      </c>
+      <c r="L71" t="s">
+        <v>145</v>
+      </c>
+      <c r="M71" t="s">
+        <v>143</v>
+      </c>
+      <c r="N71" t="s">
+        <v>391</v>
+      </c>
+      <c r="O71" t="s">
+        <v>143</v>
+      </c>
+      <c r="P71" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>143</v>
+      </c>
+      <c r="R71" t="s">
+        <v>143</v>
+      </c>
+      <c r="S71" t="s">
+        <v>143</v>
+      </c>
+      <c r="T71" t="s">
+        <v>143</v>
+      </c>
+      <c r="U71" t="s">
+        <v>143</v>
+      </c>
+      <c r="V71" t="s">
+        <v>143</v>
+      </c>
+      <c r="W71" t="s">
+        <v>143</v>
+      </c>
+      <c r="X71" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y71" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z71" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA71" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB71" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC71" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD71" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE71" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF71" t="s">
+        <v>143</v>
+      </c>
+      <c r="AG71" t="s">
+        <v>143</v>
+      </c>
+      <c r="AH71" t="s">
+        <v>143</v>
+      </c>
+      <c r="AI71" t="s">
+        <v>143</v>
+      </c>
+      <c r="AJ71" t="s">
+        <v>143</v>
+      </c>
+      <c r="AK71" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="72" spans="1:37" ht="18" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>43</v>
+      </c>
+      <c r="B72" s="15" t="s">
+        <v>683</v>
+      </c>
+      <c r="C72" t="s">
+        <v>2</v>
+      </c>
+      <c r="D72" t="s">
+        <v>685</v>
+      </c>
+      <c r="E72" t="s">
+        <v>3</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H72" t="s">
+        <v>681</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="J72" t="s">
+        <v>457</v>
+      </c>
+      <c r="K72" s="9" t="s">
+        <v>417</v>
+      </c>
+      <c r="L72" t="s">
+        <v>145</v>
+      </c>
+      <c r="M72" t="s">
+        <v>143</v>
+      </c>
+      <c r="N72" t="s">
+        <v>390</v>
+      </c>
+      <c r="O72" t="s">
+        <v>143</v>
+      </c>
+      <c r="P72" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>143</v>
+      </c>
+      <c r="R72" t="s">
+        <v>143</v>
+      </c>
+      <c r="S72" t="s">
+        <v>143</v>
+      </c>
+      <c r="T72" t="s">
+        <v>143</v>
+      </c>
+      <c r="U72" t="s">
+        <v>143</v>
+      </c>
+      <c r="V72" t="s">
+        <v>143</v>
+      </c>
+      <c r="W72" t="s">
+        <v>143</v>
+      </c>
+      <c r="X72" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y72" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z72" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA72" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB72" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC72" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD72" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE72" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF72" t="s">
+        <v>143</v>
+      </c>
+      <c r="AG72" t="s">
+        <v>143</v>
+      </c>
+      <c r="AH72" t="s">
+        <v>143</v>
+      </c>
+      <c r="AI72" t="s">
+        <v>143</v>
+      </c>
+      <c r="AJ72" t="s">
+        <v>143</v>
+      </c>
+      <c r="AK72" t="s">
+        <v>143</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AK60" xr:uid="{6F439630-CB66-7E4E-9544-3F25521DB3EB}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10603,8 +10847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
   <dimension ref="A1:AH155"/>
   <sheetViews>
-    <sheetView topLeftCell="C94" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J115" sqref="J115"/>
+    <sheetView topLeftCell="A95" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
data required and dim item sets modify tx rates
Changed to distribute TX_NEW to fine age bands. see https://github.com/pepfar-datim/COP-Target-Setting/issues/491
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B76DBA4-8FD8-514B-8649-062B72F0589C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D7AEAC-863E-414A-B3B2-BDBF6B7D3214}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data_required!$A$1:$AK$60</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">dimension_Item_sets!$A$1:$AG$143</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">dimension_Item_sets!$A$1:$AH$155</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4026" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4056" uniqueCount="687">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -2246,6 +2246,9 @@
   </si>
   <si>
     <t>TB_PREV (N, DSD+TA, Age/TherapyType/NewExistingArt/HIVStatus) TARGET already on art</t>
+  </si>
+  <si>
+    <t>10-50+.&lt;15/&gt;15.d.u</t>
   </si>
 </sst>
 </file>
@@ -2339,7 +2342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -2361,6 +2364,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2678,10 +2684,10 @@
   <dimension ref="A1:AK72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C57" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="S57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B59" sqref="B59"/>
+      <selection pane="bottomRight" activeCell="W70" sqref="W70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10233,7 +10239,7 @@
         <v>139</v>
       </c>
       <c r="Y67" s="9" t="s">
-        <v>149</v>
+        <v>658</v>
       </c>
       <c r="Z67" t="s">
         <v>145</v>
@@ -10345,8 +10351,8 @@
       <c r="X68" t="s">
         <v>139</v>
       </c>
-      <c r="Y68" s="9" t="s">
-        <v>140</v>
+      <c r="Y68" s="19" t="s">
+        <v>686</v>
       </c>
       <c r="Z68" t="s">
         <v>141</v>
@@ -10458,8 +10464,8 @@
       <c r="X69" t="s">
         <v>139</v>
       </c>
-      <c r="Y69" s="9" t="s">
-        <v>140</v>
+      <c r="Y69" s="19" t="s">
+        <v>686</v>
       </c>
       <c r="Z69" t="s">
         <v>141</v>
@@ -10571,8 +10577,8 @@
       <c r="X70" t="s">
         <v>139</v>
       </c>
-      <c r="Y70" s="9" t="s">
-        <v>140</v>
+      <c r="Y70" s="19" t="s">
+        <v>686</v>
       </c>
       <c r="Z70" t="s">
         <v>148</v>
@@ -10845,19 +10851,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
-  <dimension ref="A1:AH155"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:AI155"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="6" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="V43" sqref="V43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
     <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.83203125" customWidth="1"/>
-    <col min="5" max="5" width="52.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.1640625" customWidth="1"/>
     <col min="6" max="6" width="49.5" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" customWidth="1"/>
@@ -10866,10 +10874,10 @@
     <col min="11" max="13" width="12.33203125" customWidth="1"/>
     <col min="14" max="18" width="10.83203125" customWidth="1"/>
     <col min="19" max="19" width="13.5" customWidth="1"/>
-    <col min="21" max="21" width="19.6640625" customWidth="1"/>
+    <col min="21" max="22" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>221</v>
       </c>
@@ -10933,47 +10941,50 @@
       <c r="U1" s="9" t="s">
         <v>658</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="19" t="s">
+        <v>686</v>
+      </c>
+      <c r="W1" t="s">
         <v>216</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>145</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>150</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>218</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>255</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>260</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>261</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>288</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>281</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>289</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>379</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>402</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>174</v>
       </c>
@@ -11002,7 +11013,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="4" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K2:AAA2)</f>
+        <f t="shared" ref="J2:J33" si="0">_xlfn.TEXTJOIN(";",1,K2:AAB2)</f>
         <v>&lt;2mo</v>
       </c>
       <c r="K2" s="9"/>
@@ -11014,11 +11025,12 @@
       <c r="R2" s="9"/>
       <c r="T2" s="9"/>
       <c r="U2" s="9"/>
-      <c r="AA2" t="s">
+      <c r="V2" s="9"/>
+      <c r="AB2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>174</v>
       </c>
@@ -11047,7 +11059,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="4" t="str">
-        <f t="shared" ref="J3:J36" si="0">_xlfn.TEXTJOIN(";",1,K3:AAA3)</f>
+        <f t="shared" si="0"/>
         <v>2-12mo</v>
       </c>
       <c r="K3" s="9"/>
@@ -11059,11 +11071,12 @@
       <c r="R3" s="9"/>
       <c r="T3" s="9"/>
       <c r="U3" s="9"/>
-      <c r="AB3" t="s">
+      <c r="V3" s="9"/>
+      <c r="AC3" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>174</v>
       </c>
@@ -11107,8 +11120,9 @@
       <c r="U4" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="V4" s="9"/>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>174</v>
       </c>
@@ -11147,8 +11161,9 @@
       <c r="U5" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="V5" s="9"/>
+    </row>
+    <row r="6" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>174</v>
       </c>
@@ -11181,7 +11196,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>174</v>
       </c>
@@ -11233,8 +11248,9 @@
       <c r="U7" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="V7" s="9"/>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>174</v>
       </c>
@@ -11286,8 +11302,9 @@
       <c r="U8" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="V8" s="9"/>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>174</v>
       </c>
@@ -11325,8 +11342,9 @@
       <c r="U9" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="V9" s="9"/>
+    </row>
+    <row r="10" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>174</v>
       </c>
@@ -11365,7 +11383,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>174</v>
       </c>
@@ -11414,8 +11432,9 @@
       <c r="U11" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="V11" s="9"/>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>174</v>
       </c>
@@ -11464,8 +11483,9 @@
       <c r="U12" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="V12" s="9"/>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>174</v>
       </c>
@@ -11503,8 +11523,9 @@
       <c r="U13" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="V13" s="9"/>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>174</v>
       </c>
@@ -11534,7 +11555,7 @@
       </c>
       <c r="J14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;10-50+;&lt;1-18+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <v>&lt;1-50+;1-50+;10-50+;&lt;1-18+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K14" s="9" t="s">
         <v>149</v>
@@ -11558,8 +11579,11 @@
       <c r="U14" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="V14" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>174</v>
       </c>
@@ -11589,7 +11613,7 @@
       </c>
       <c r="J15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="P15" s="9" t="s">
         <v>171</v>
@@ -11597,8 +11621,11 @@
       <c r="U15" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="V15" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>143</v>
       </c>
@@ -11640,7 +11667,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>174</v>
       </c>
@@ -11678,7 +11705,7 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>143</v>
       </c>
@@ -11714,7 +11741,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>174</v>
       </c>
@@ -11750,7 +11777,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>174</v>
       </c>
@@ -11780,7 +11807,7 @@
       </c>
       <c r="J20" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="P20" s="9" t="s">
         <v>171</v>
@@ -11788,8 +11815,11 @@
       <c r="U20" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V20" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>174</v>
       </c>
@@ -11819,7 +11849,7 @@
       </c>
       <c r="J21" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K21" s="9" t="s">
         <v>149</v>
@@ -11842,8 +11872,11 @@
       <c r="U21" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V21" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>143</v>
       </c>
@@ -11885,7 +11918,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>174</v>
       </c>
@@ -11921,7 +11954,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>143</v>
       </c>
@@ -11963,7 +11996,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>174</v>
       </c>
@@ -11992,7 +12025,7 @@
         <v>1</v>
       </c>
       <c r="J25" s="4" t="str">
-        <f t="shared" ref="J25" si="1">_xlfn.TEXTJOIN(";",1,K25:AAA25)</f>
+        <f t="shared" si="0"/>
         <v>&lt;1-18+</v>
       </c>
       <c r="K25" s="5"/>
@@ -12004,7 +12037,7 @@
       </c>
       <c r="P25" s="5"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>174</v>
       </c>
@@ -12045,7 +12078,7 @@
       </c>
       <c r="P26" s="5"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>174</v>
       </c>
@@ -12075,7 +12108,7 @@
       </c>
       <c r="J27" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="P27" s="9" t="s">
         <v>171</v>
@@ -12083,8 +12116,11 @@
       <c r="U27" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V27" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>174</v>
       </c>
@@ -12114,7 +12150,7 @@
       </c>
       <c r="J28" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K28" s="9" t="s">
         <v>149</v>
@@ -12137,8 +12173,11 @@
       <c r="U28" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V28" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>143</v>
       </c>
@@ -12180,7 +12219,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>174</v>
       </c>
@@ -12210,7 +12249,7 @@
       </c>
       <c r="J30" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="P30" s="9" t="s">
         <v>171</v>
@@ -12218,8 +12257,11 @@
       <c r="U30" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V30" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>174</v>
       </c>
@@ -12249,7 +12291,7 @@
       </c>
       <c r="J31" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K31" s="9" t="s">
         <v>149</v>
@@ -12274,8 +12316,11 @@
       <c r="U31" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V31" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>174</v>
       </c>
@@ -12311,7 +12356,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>143</v>
       </c>
@@ -12353,7 +12398,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>174</v>
       </c>
@@ -12382,14 +12427,14 @@
         <v>1</v>
       </c>
       <c r="J34" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="J34:J65" si="1">_xlfn.TEXTJOIN(";",1,K34:AAB34)</f>
         <v>&lt;1-18+</v>
       </c>
       <c r="O34" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>174</v>
       </c>
@@ -12418,8 +12463,8 @@
         <v>0.125</v>
       </c>
       <c r="J35" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <f t="shared" si="1"/>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="P35" s="9" t="s">
         <v>171</v>
@@ -12427,8 +12472,11 @@
       <c r="U35" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V35" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>174</v>
       </c>
@@ -12457,14 +12505,14 @@
         <v>0.2</v>
       </c>
       <c r="J36" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10-50+.all</v>
       </c>
       <c r="T36" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>174</v>
       </c>
@@ -12493,8 +12541,8 @@
         <v>1</v>
       </c>
       <c r="J37" s="4" t="str">
-        <f t="shared" ref="J37:J70" si="2">_xlfn.TEXTJOIN(";",1,K37:AAA37)</f>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <f t="shared" si="1"/>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K37" s="9" t="s">
         <v>149</v>
@@ -12519,8 +12567,11 @@
       <c r="U37" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V37" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>143</v>
       </c>
@@ -12549,7 +12600,7 @@
         <v>0.11119999999999999</v>
       </c>
       <c r="J38" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>missing_age_1</v>
       </c>
       <c r="K38" s="4"/>
@@ -12562,7 +12613,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>174</v>
       </c>
@@ -12591,8 +12642,8 @@
         <v>0.125</v>
       </c>
       <c r="J39" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <f t="shared" si="1"/>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="P39" s="9" t="s">
         <v>171</v>
@@ -12600,8 +12651,11 @@
       <c r="U39" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V39" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>174</v>
       </c>
@@ -12630,14 +12684,14 @@
         <v>0.2</v>
       </c>
       <c r="J40" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>10-50+.all</v>
       </c>
       <c r="T40" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>174</v>
       </c>
@@ -12666,8 +12720,8 @@
         <v>1</v>
       </c>
       <c r="J41" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <f t="shared" si="1"/>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K41" s="9" t="s">
         <v>149</v>
@@ -12690,8 +12744,11 @@
       <c r="U41" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V41" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>143</v>
       </c>
@@ -12720,7 +12777,7 @@
         <v>0.1111</v>
       </c>
       <c r="J42" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>missing_age_1</v>
       </c>
       <c r="K42" s="4"/>
@@ -12733,7 +12790,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>174</v>
       </c>
@@ -12762,8 +12819,8 @@
         <v>1</v>
       </c>
       <c r="J43" s="4" t="str">
-        <f t="shared" ref="J43" si="3">_xlfn.TEXTJOIN(";",1,K43:AAA43)</f>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <f t="shared" si="1"/>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K43" s="9" t="s">
         <v>149</v>
@@ -12786,8 +12843,11 @@
       <c r="U43" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V43" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>174</v>
       </c>
@@ -12816,8 +12876,8 @@
         <v>0.125</v>
       </c>
       <c r="J44" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <f t="shared" si="1"/>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="P44" s="9" t="s">
         <v>171</v>
@@ -12825,8 +12885,11 @@
       <c r="U44" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V44" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>174</v>
       </c>
@@ -12855,14 +12918,14 @@
         <v>0.2</v>
       </c>
       <c r="J45" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>10-50+.all</v>
       </c>
       <c r="T45" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>174</v>
       </c>
@@ -12891,8 +12954,8 @@
         <v>0.5</v>
       </c>
       <c r="J46" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <f t="shared" si="1"/>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K46" s="9" t="s">
         <v>149</v>
@@ -12915,8 +12978,11 @@
       <c r="U46" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V46" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>143</v>
       </c>
@@ -12945,7 +13011,7 @@
         <v>0.1111</v>
       </c>
       <c r="J47" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>missing_age_1</v>
       </c>
       <c r="K47" s="4"/>
@@ -12958,7 +13024,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>174</v>
       </c>
@@ -12987,8 +13053,8 @@
         <v>1</v>
       </c>
       <c r="J48" s="4" t="str">
-        <f t="shared" ref="J48" si="4">_xlfn.TEXTJOIN(";",1,K48:AAA48)</f>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <f t="shared" si="1"/>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K48" s="9" t="s">
         <v>149</v>
@@ -13011,8 +13077,11 @@
       <c r="U48" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="V48" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>174</v>
       </c>
@@ -13041,8 +13110,8 @@
         <v>0.125</v>
       </c>
       <c r="J49" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <f t="shared" si="1"/>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="P49" s="9" t="s">
         <v>171</v>
@@ -13050,8 +13119,11 @@
       <c r="U49" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="V49" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="50" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>174</v>
       </c>
@@ -13080,14 +13152,14 @@
         <v>0.2</v>
       </c>
       <c r="J50" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>10-50+.all</v>
       </c>
       <c r="T50" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>174</v>
       </c>
@@ -13116,8 +13188,8 @@
         <v>0.5</v>
       </c>
       <c r="J51" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <f t="shared" si="1"/>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K51" s="9" t="s">
         <v>149</v>
@@ -13140,8 +13212,11 @@
       <c r="U51" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="V51" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="52" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>143</v>
       </c>
@@ -13170,7 +13245,7 @@
         <v>0.1111</v>
       </c>
       <c r="J52" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>missing_age_1</v>
       </c>
       <c r="K52" s="4"/>
@@ -13183,7 +13258,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>174</v>
       </c>
@@ -13212,8 +13287,8 @@
         <v>0.125</v>
       </c>
       <c r="J53" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <f t="shared" si="1"/>
+        <v>&lt;15/&gt;15.d;&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="P53" s="9" t="s">
         <v>171</v>
@@ -13221,8 +13296,11 @@
       <c r="U53" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="V53" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>174</v>
       </c>
@@ -13251,8 +13329,8 @@
         <v>1</v>
       </c>
       <c r="J54" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <f t="shared" si="1"/>
+        <v>&lt;1-50+;1-50+;10-50+;15-50+;1-50+/&lt;5;10-50+.all;&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="K54" s="9" t="s">
         <v>149</v>
@@ -13275,8 +13353,11 @@
       <c r="U54" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="V54" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="55" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>143</v>
       </c>
@@ -13305,7 +13386,7 @@
         <v>0.1111</v>
       </c>
       <c r="J55" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>missing_age_1</v>
       </c>
       <c r="K55" s="4"/>
@@ -13318,7 +13399,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>175</v>
       </c>
@@ -13347,20 +13428,20 @@
         <v>1</v>
       </c>
       <c r="J56" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>F;F/M;F/M/U</v>
       </c>
-      <c r="V56" t="s">
+      <c r="W56" t="s">
         <v>141</v>
       </c>
-      <c r="W56" t="s">
+      <c r="X56" t="s">
         <v>145</v>
       </c>
-      <c r="X56" t="s">
+      <c r="Y56" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>143</v>
       </c>
@@ -13389,7 +13470,7 @@
         <v>0.5</v>
       </c>
       <c r="J57" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>missing_sex_1</v>
       </c>
       <c r="K57" s="4"/>
@@ -13402,7 +13483,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>175</v>
       </c>
@@ -13431,7 +13512,7 @@
         <v>0.5</v>
       </c>
       <c r="J58" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>U;F/M/U</v>
       </c>
       <c r="K58" s="5"/>
@@ -13440,14 +13521,14 @@
       <c r="N58" s="5"/>
       <c r="O58" s="5"/>
       <c r="P58" s="5"/>
-      <c r="V58" t="s">
+      <c r="W58" t="s">
         <v>154</v>
       </c>
-      <c r="X58" t="s">
+      <c r="Y58" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>175</v>
       </c>
@@ -13476,23 +13557,24 @@
         <v>1</v>
       </c>
       <c r="J59" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>M;F/M;F/M/U</v>
       </c>
       <c r="S59" s="5"/>
       <c r="T59" s="5"/>
       <c r="U59" s="5"/>
-      <c r="V59" t="s">
+      <c r="V59" s="5"/>
+      <c r="W59" t="s">
         <v>148</v>
       </c>
-      <c r="W59" t="s">
+      <c r="X59" t="s">
         <v>145</v>
       </c>
-      <c r="X59" t="s">
+      <c r="Y59" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>143</v>
       </c>
@@ -13521,7 +13603,7 @@
         <v>0.5</v>
       </c>
       <c r="J60" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>missing_sex_1</v>
       </c>
       <c r="K60" s="4"/>
@@ -13534,7 +13616,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>175</v>
       </c>
@@ -13563,20 +13645,21 @@
         <v>0.5</v>
       </c>
       <c r="J61" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>U;F/M/U</v>
       </c>
       <c r="S61" s="5"/>
       <c r="T61" s="5"/>
       <c r="U61" s="5"/>
-      <c r="V61" t="s">
+      <c r="V61" s="5"/>
+      <c r="W61" t="s">
         <v>154</v>
       </c>
-      <c r="X61" t="s">
+      <c r="Y61" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>184</v>
       </c>
@@ -13605,14 +13688,14 @@
         <v>1</v>
       </c>
       <c r="J62" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>kp1</v>
       </c>
-      <c r="Y62" t="s">
+      <c r="Z62" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>184</v>
       </c>
@@ -13641,14 +13724,14 @@
         <v>1</v>
       </c>
       <c r="J63" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>kp1</v>
       </c>
-      <c r="Y63" t="s">
+      <c r="Z63" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>184</v>
       </c>
@@ -13677,14 +13760,14 @@
         <v>1</v>
       </c>
       <c r="J64" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>kp1</v>
       </c>
-      <c r="Y64" t="s">
+      <c r="Z64" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="65" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>184</v>
       </c>
@@ -13713,14 +13796,14 @@
         <v>1</v>
       </c>
       <c r="J65" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>kp1</v>
       </c>
-      <c r="Y65" t="s">
+      <c r="Z65" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="66" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>184</v>
       </c>
@@ -13749,14 +13832,14 @@
         <v>1</v>
       </c>
       <c r="J66" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="J66:J97" si="2">_xlfn.TEXTJOIN(";",1,K66:AAB66)</f>
         <v>kp1</v>
       </c>
-      <c r="Y66" t="s">
+      <c r="Z66" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="67" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>196</v>
       </c>
@@ -13788,11 +13871,11 @@
         <f t="shared" si="2"/>
         <v>tr_pos</v>
       </c>
-      <c r="Z67" t="s">
+      <c r="AA67" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="68" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>196</v>
       </c>
@@ -13824,11 +13907,11 @@
         <f t="shared" si="2"/>
         <v>tr_neg</v>
       </c>
-      <c r="Z68" t="s">
+      <c r="AA68" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="69" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>264</v>
       </c>
@@ -13860,11 +13943,11 @@
         <f t="shared" si="2"/>
         <v>tss_NewPos</v>
       </c>
-      <c r="AC69" t="s">
+      <c r="AD69" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="70" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>264</v>
       </c>
@@ -13896,11 +13979,11 @@
         <f t="shared" si="2"/>
         <v>tss_KnowPos</v>
       </c>
-      <c r="AC70" t="s">
+      <c r="AD70" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="71" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>264</v>
       </c>
@@ -13929,14 +14012,14 @@
         <v>1</v>
       </c>
       <c r="J71" s="4" t="str">
-        <f t="shared" ref="J71:J134" si="5">_xlfn.TEXTJOIN(";",1,K71:AAA71)</f>
+        <f t="shared" si="2"/>
         <v>tss_NewNeg</v>
       </c>
-      <c r="AC71" t="s">
+      <c r="AD71" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="72" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>278</v>
       </c>
@@ -13965,14 +14048,14 @@
         <v>1</v>
       </c>
       <c r="J72" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>vt_sv</v>
       </c>
-      <c r="AD72" t="s">
+      <c r="AE72" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="73" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>278</v>
       </c>
@@ -14001,14 +14084,14 @@
         <v>1</v>
       </c>
       <c r="J73" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>vt_pe</v>
       </c>
-      <c r="AD73" t="s">
+      <c r="AE73" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="74" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>278</v>
       </c>
@@ -14037,14 +14120,14 @@
         <v>1</v>
       </c>
       <c r="J74" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>st_da</v>
       </c>
-      <c r="AE74" t="s">
+      <c r="AF74" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="75" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>278</v>
       </c>
@@ -14073,14 +14156,14 @@
         <v>1</v>
       </c>
       <c r="J75" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>st_da</v>
       </c>
-      <c r="AE75" t="s">
+      <c r="AF75" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="76" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>278</v>
       </c>
@@ -14109,14 +14192,14 @@
         <v>1</v>
       </c>
       <c r="J76" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>st_da</v>
       </c>
-      <c r="AE76" t="s">
+      <c r="AF76" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="77" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>278</v>
       </c>
@@ -14145,14 +14228,14 @@
         <v>1</v>
       </c>
       <c r="J77" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>st_da</v>
       </c>
-      <c r="AE77" t="s">
+      <c r="AF77" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="78" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>278</v>
       </c>
@@ -14181,14 +14264,14 @@
         <v>1</v>
       </c>
       <c r="J78" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>st_da</v>
       </c>
-      <c r="AE78" t="s">
+      <c r="AF78" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="79" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>278</v>
       </c>
@@ -14217,14 +14300,14 @@
         <v>1</v>
       </c>
       <c r="J79" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>st_da</v>
       </c>
-      <c r="AE79" t="s">
+      <c r="AF79" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="80" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>278</v>
       </c>
@@ -14253,14 +14336,14 @@
         <v>1</v>
       </c>
       <c r="J80" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>st_da</v>
       </c>
-      <c r="AE80" t="s">
+      <c r="AF80" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="81" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>278</v>
       </c>
@@ -14289,14 +14372,14 @@
         <v>1</v>
       </c>
       <c r="J81" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>st_da</v>
       </c>
-      <c r="AE81" t="s">
+      <c r="AF81" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="82" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>278</v>
       </c>
@@ -14325,14 +14408,14 @@
         <v>1</v>
       </c>
       <c r="J82" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>st_da</v>
       </c>
-      <c r="AE82" t="s">
+      <c r="AF82" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="83" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>278</v>
       </c>
@@ -14361,14 +14444,14 @@
         <v>1</v>
       </c>
       <c r="J83" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>st_da</v>
       </c>
-      <c r="AE83" t="s">
+      <c r="AF83" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="84" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>278</v>
       </c>
@@ -14397,14 +14480,14 @@
         <v>1</v>
       </c>
       <c r="J84" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>st_da</v>
       </c>
-      <c r="AE84" t="s">
+      <c r="AF84" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="85" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>278</v>
       </c>
@@ -14433,14 +14516,14 @@
         <v>1</v>
       </c>
       <c r="J85" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>st_da</v>
       </c>
-      <c r="AE85" t="s">
+      <c r="AF85" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="86" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>278</v>
       </c>
@@ -14469,14 +14552,14 @@
         <v>1</v>
       </c>
       <c r="J86" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>st_da</v>
       </c>
-      <c r="AE86" t="s">
+      <c r="AF86" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="87" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>278</v>
       </c>
@@ -14505,14 +14588,14 @@
         <v>1</v>
       </c>
       <c r="J87" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>st_da</v>
       </c>
-      <c r="AE87" t="s">
+      <c r="AF87" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="88" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>278</v>
       </c>
@@ -14541,14 +14624,14 @@
         <v>1</v>
       </c>
       <c r="J88" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>st_da</v>
       </c>
-      <c r="AE88" t="s">
+      <c r="AF88" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="89" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>278</v>
       </c>
@@ -14577,14 +14660,14 @@
         <v>1</v>
       </c>
       <c r="J89" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>st_da</v>
       </c>
-      <c r="AE89" t="s">
+      <c r="AF89" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="90" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>278</v>
       </c>
@@ -14613,14 +14696,14 @@
         <v>1</v>
       </c>
       <c r="J90" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>st_ua</v>
       </c>
-      <c r="AE90" t="s">
+      <c r="AF90" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="91" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>278</v>
       </c>
@@ -14649,14 +14732,14 @@
         <v>1</v>
       </c>
       <c r="J91" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>st_ua</v>
       </c>
-      <c r="AE91" t="s">
+      <c r="AF91" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="92" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>278</v>
       </c>
@@ -14685,14 +14768,14 @@
         <v>1</v>
       </c>
       <c r="J92" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>st_ua</v>
       </c>
-      <c r="AE92" t="s">
+      <c r="AF92" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="93" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>278</v>
       </c>
@@ -14721,14 +14804,14 @@
         <v>1</v>
       </c>
       <c r="J93" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>st_ua</v>
       </c>
-      <c r="AE93" t="s">
+      <c r="AF93" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="94" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>278</v>
       </c>
@@ -14757,14 +14840,14 @@
         <v>1</v>
       </c>
       <c r="J94" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>st_ua</v>
       </c>
-      <c r="AE94" t="s">
+      <c r="AF94" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="95" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>278</v>
       </c>
@@ -14793,14 +14876,14 @@
         <v>1</v>
       </c>
       <c r="J95" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>st_ua</v>
       </c>
-      <c r="AE95" t="s">
+      <c r="AF95" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="96" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>278</v>
       </c>
@@ -14829,14 +14912,14 @@
         <v>1</v>
       </c>
       <c r="J96" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>st_ua</v>
       </c>
-      <c r="AE96" t="s">
+      <c r="AF96" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="97" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>278</v>
       </c>
@@ -14865,14 +14948,14 @@
         <v>1</v>
       </c>
       <c r="J97" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>st_ua</v>
       </c>
-      <c r="AE97" t="s">
+      <c r="AF97" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="98" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>278</v>
       </c>
@@ -14901,14 +14984,14 @@
         <v>1</v>
       </c>
       <c r="J98" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="J98:J129" si="3">_xlfn.TEXTJOIN(";",1,K98:AAB98)</f>
         <v>st_ua</v>
       </c>
-      <c r="AE98" t="s">
+      <c r="AF98" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="99" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>278</v>
       </c>
@@ -14937,14 +15020,14 @@
         <v>1</v>
       </c>
       <c r="J99" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>st_ua</v>
       </c>
-      <c r="AE99" t="s">
+      <c r="AF99" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="100" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>278</v>
       </c>
@@ -14973,14 +15056,14 @@
         <v>1</v>
       </c>
       <c r="J100" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>st_ua</v>
       </c>
-      <c r="AE100" t="s">
+      <c r="AF100" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="101" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>278</v>
       </c>
@@ -15009,14 +15092,14 @@
         <v>1</v>
       </c>
       <c r="J101" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>st_ua</v>
       </c>
-      <c r="AE101" t="s">
+      <c r="AF101" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="102" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>278</v>
       </c>
@@ -15045,14 +15128,14 @@
         <v>1</v>
       </c>
       <c r="J102" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>st_ua</v>
       </c>
-      <c r="AE102" t="s">
+      <c r="AF102" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="103" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>278</v>
       </c>
@@ -15081,14 +15164,14 @@
         <v>1</v>
       </c>
       <c r="J103" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>st_ua</v>
       </c>
-      <c r="AE103" t="s">
+      <c r="AF103" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="104" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>278</v>
       </c>
@@ -15117,14 +15200,14 @@
         <v>1</v>
       </c>
       <c r="J104" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>st_ua</v>
       </c>
-      <c r="AE104" t="s">
+      <c r="AF104" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="105" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>278</v>
       </c>
@@ -15153,14 +15236,14 @@
         <v>1</v>
       </c>
       <c r="J105" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>st_ua</v>
       </c>
-      <c r="AE105" t="s">
+      <c r="AF105" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="106" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>278</v>
       </c>
@@ -15189,14 +15272,14 @@
         <v>1</v>
       </c>
       <c r="J106" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>kp2</v>
       </c>
-      <c r="Y106" t="s">
+      <c r="Z106" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="107" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>278</v>
       </c>
@@ -15225,14 +15308,14 @@
         <v>1</v>
       </c>
       <c r="J107" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>kp2</v>
       </c>
-      <c r="Y107" t="s">
+      <c r="Z107" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="108" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>278</v>
       </c>
@@ -15261,14 +15344,14 @@
         <v>1</v>
       </c>
       <c r="J108" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>kp2</v>
       </c>
-      <c r="Y108" t="s">
+      <c r="Z108" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="109" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>278</v>
       </c>
@@ -15297,14 +15380,14 @@
         <v>1</v>
       </c>
       <c r="J109" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>kp2</v>
       </c>
-      <c r="Y109" t="s">
+      <c r="Z109" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="110" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>278</v>
       </c>
@@ -15333,14 +15416,14 @@
         <v>1</v>
       </c>
       <c r="J110" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>kp2</v>
       </c>
-      <c r="Y110" t="s">
+      <c r="Z110" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="111" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>278</v>
       </c>
@@ -15369,14 +15452,14 @@
         <v>1</v>
       </c>
       <c r="J111" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>kp2</v>
       </c>
-      <c r="Y111" t="s">
+      <c r="Z111" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="112" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>278</v>
       </c>
@@ -15405,14 +15488,14 @@
         <v>1</v>
       </c>
       <c r="J112" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>kp2</v>
       </c>
-      <c r="Y112" t="s">
+      <c r="Z112" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="113" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>278</v>
       </c>
@@ -15441,14 +15524,14 @@
         <v>1</v>
       </c>
       <c r="J113" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>kp2</v>
       </c>
-      <c r="Y113" t="s">
+      <c r="Z113" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="114" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>381</v>
       </c>
@@ -15477,14 +15560,14 @@
         <v>1</v>
       </c>
       <c r="J114" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>as_already</v>
       </c>
-      <c r="AF114" t="s">
+      <c r="AG114" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="115" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>381</v>
       </c>
@@ -15513,14 +15596,14 @@
         <v>1</v>
       </c>
       <c r="J115" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>as_new</v>
       </c>
-      <c r="AF115" t="s">
+      <c r="AG115" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="116" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>278</v>
       </c>
@@ -15549,14 +15632,14 @@
         <v>1</v>
       </c>
       <c r="J116" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>kp3</v>
       </c>
-      <c r="Y116" t="s">
+      <c r="Z116" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="117" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>278</v>
       </c>
@@ -15585,14 +15668,14 @@
         <v>1</v>
       </c>
       <c r="J117" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>kp3</v>
       </c>
-      <c r="Y117" t="s">
+      <c r="Z117" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="118" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>278</v>
       </c>
@@ -15621,14 +15704,14 @@
         <v>1</v>
       </c>
       <c r="J118" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>kp3</v>
       </c>
-      <c r="Y118" t="s">
+      <c r="Z118" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="119" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>278</v>
       </c>
@@ -15657,14 +15740,14 @@
         <v>1</v>
       </c>
       <c r="J119" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>kp3</v>
       </c>
-      <c r="Y119" t="s">
+      <c r="Z119" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="120" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>278</v>
       </c>
@@ -15693,14 +15776,14 @@
         <v>1</v>
       </c>
       <c r="J120" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>ti_routine</v>
       </c>
-      <c r="AG120" t="s">
+      <c r="AH120" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="121" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>278</v>
       </c>
@@ -15729,14 +15812,14 @@
         <v>1</v>
       </c>
       <c r="J121" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>ti_routine</v>
       </c>
-      <c r="AG121" t="s">
+      <c r="AH121" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="122" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>278</v>
       </c>
@@ -15765,14 +15848,14 @@
         <v>1</v>
       </c>
       <c r="J122" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>ti_routine</v>
       </c>
-      <c r="AG122" t="s">
+      <c r="AH122" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="123" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>278</v>
       </c>
@@ -15801,14 +15884,14 @@
         <v>1</v>
       </c>
       <c r="J123" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>ti_routine</v>
       </c>
-      <c r="AG123" t="s">
+      <c r="AH123" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="124" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>196</v>
       </c>
@@ -15837,14 +15920,14 @@
         <v>1</v>
       </c>
       <c r="J124" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K124:AAA124)</f>
+        <f t="shared" si="3"/>
         <v>tr_pos2</v>
       </c>
-      <c r="Z124" t="s">
+      <c r="AA124" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="125" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>196</v>
       </c>
@@ -15873,14 +15956,14 @@
         <v>1</v>
       </c>
       <c r="J125" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>tr_neg2</v>
       </c>
-      <c r="Z125" t="s">
+      <c r="AA125" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="126" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>509</v>
       </c>
@@ -15909,14 +15992,14 @@
         <v>1</v>
       </c>
       <c r="J126" t="str">
-        <f t="shared" ref="J126:J132" si="6">_xlfn.TEXTJOIN(";",1,K126:AAA126)</f>
+        <f t="shared" si="3"/>
         <v>hts_mod_com_ndx</v>
       </c>
-      <c r="AH126" t="s">
+      <c r="AI126" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="127" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>509</v>
       </c>
@@ -15945,14 +16028,14 @@
         <v>1</v>
       </c>
       <c r="J127" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>hts_mod_fac_ndx</v>
       </c>
-      <c r="AH127" t="s">
+      <c r="AI127" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="128" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>509</v>
       </c>
@@ -15981,14 +16064,14 @@
         <v>1</v>
       </c>
       <c r="J128" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>hts_mod_com_mob</v>
       </c>
-      <c r="AH128" t="s">
+      <c r="AI128" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="129" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>509</v>
       </c>
@@ -16017,14 +16100,14 @@
         <v>1</v>
       </c>
       <c r="J129" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>hts_mod_com_vct</v>
       </c>
-      <c r="AH129" t="s">
+      <c r="AI129" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="130" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>509</v>
       </c>
@@ -16053,14 +16136,14 @@
         <v>1</v>
       </c>
       <c r="J130" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="J130:J161" si="4">_xlfn.TEXTJOIN(";",1,K130:AAB130)</f>
         <v>hts_mod_com_otr</v>
       </c>
-      <c r="AH130" t="s">
+      <c r="AI130" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="131" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>509</v>
       </c>
@@ -16089,14 +16172,14 @@
         <v>1</v>
       </c>
       <c r="J131" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>hts_mod_fac_ew</v>
       </c>
-      <c r="AH131" t="s">
+      <c r="AI131" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="132" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>509</v>
       </c>
@@ -16125,14 +16208,14 @@
         <v>1</v>
       </c>
       <c r="J132" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>hts_mod_fac_inpat</v>
       </c>
-      <c r="AH132" t="s">
+      <c r="AI132" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="133" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>509</v>
       </c>
@@ -16161,14 +16244,14 @@
         <v>1</v>
       </c>
       <c r="J133" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>hts_mod_fac_nut</v>
       </c>
-      <c r="AH133" t="s">
+      <c r="AI133" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="134" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>509</v>
       </c>
@@ -16197,14 +16280,14 @@
         <v>1</v>
       </c>
       <c r="J134" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>hts_mod_fac_ped</v>
       </c>
-      <c r="AH134" t="s">
+      <c r="AI134" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="135" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>509</v>
       </c>
@@ -16233,14 +16316,14 @@
         <v>1</v>
       </c>
       <c r="J135" t="str">
-        <f t="shared" ref="J135:J140" si="7">_xlfn.TEXTJOIN(";",1,K135:AAA135)</f>
+        <f t="shared" si="4"/>
         <v>hts_mod_fac_sti</v>
       </c>
-      <c r="AH135" t="s">
+      <c r="AI135" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="136" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>509</v>
       </c>
@@ -16269,14 +16352,14 @@
         <v>1</v>
       </c>
       <c r="J136" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>hts_mod_fac_vct</v>
       </c>
-      <c r="AH136" t="s">
+      <c r="AI136" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="137" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>509</v>
       </c>
@@ -16305,14 +16388,14 @@
         <v>1</v>
       </c>
       <c r="J137" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>hts_mod_fac_otr_pitc</v>
       </c>
-      <c r="AH137" t="s">
+      <c r="AI137" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="138" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>509</v>
       </c>
@@ -16341,14 +16424,14 @@
         <v>1</v>
       </c>
       <c r="J138" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>hts_mod_fac_vmmc</v>
       </c>
-      <c r="AH138" t="s">
+      <c r="AI138" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="139" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>509</v>
       </c>
@@ -16377,14 +16460,14 @@
         <v>1</v>
       </c>
       <c r="J139" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>hts_mod_fac_anc_1</v>
       </c>
-      <c r="AH139" t="s">
+      <c r="AI139" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="140" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>509</v>
       </c>
@@ -16413,14 +16496,14 @@
         <v>1</v>
       </c>
       <c r="J140" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>hts_mod_fac_tb</v>
       </c>
-      <c r="AH140" t="s">
+      <c r="AI140" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="141" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>509</v>
       </c>
@@ -16449,14 +16532,14 @@
         <v>1</v>
       </c>
       <c r="J141" t="str">
-        <f t="shared" ref="J141" si="8">_xlfn.TEXTJOIN(";",1,K141:AAA141)</f>
+        <f t="shared" si="4"/>
         <v>hts_mod_fac_post_anc_1</v>
       </c>
-      <c r="AH141" t="s">
+      <c r="AI141" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="142" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>174</v>
       </c>
@@ -16485,7 +16568,7 @@
         <v>1</v>
       </c>
       <c r="J142" s="4" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K142:AAA142)</f>
+        <f t="shared" si="4"/>
         <v>U_age</v>
       </c>
       <c r="K142" s="9"/>
@@ -16497,11 +16580,12 @@
       <c r="R142" s="9"/>
       <c r="T142" s="9"/>
       <c r="U142" s="9"/>
-      <c r="AH142" t="s">
+      <c r="V142" s="9"/>
+      <c r="AI142" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="143" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>175</v>
       </c>
@@ -16530,14 +16614,14 @@
         <v>1</v>
       </c>
       <c r="J143" s="4" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K143:AAA143)</f>
+        <f t="shared" si="4"/>
         <v>U_sex</v>
       </c>
-      <c r="AH143" t="s">
+      <c r="AI143" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="144" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>174</v>
       </c>
@@ -16566,14 +16650,15 @@
         <v>8.3299999999999999E-2</v>
       </c>
       <c r="J144" s="4" t="str">
-        <f t="shared" ref="J144:J155" si="9">_xlfn.TEXTJOIN(";",1,K144:AAA144)</f>
+        <f t="shared" ref="J144:J155" si="5">_xlfn.TEXTJOIN(";",1,K144:AAB144)</f>
         <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U144" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="145" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V144" s="19"/>
+    </row>
+    <row r="145" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>174</v>
       </c>
@@ -16602,14 +16687,15 @@
         <v>8.3299999999999999E-2</v>
       </c>
       <c r="J145" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U145" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="146" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V145" s="9"/>
+    </row>
+    <row r="146" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>174</v>
       </c>
@@ -16638,14 +16724,15 @@
         <v>8.3299999999999999E-2</v>
       </c>
       <c r="J146" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U146" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="147" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V146" s="9"/>
+    </row>
+    <row r="147" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>174</v>
       </c>
@@ -16674,14 +16761,17 @@
         <v>8.3299999999999999E-2</v>
       </c>
       <c r="J147" s="4" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <f>_xlfn.TEXTJOIN(";",1,K147:AAB147)</f>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U147" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="148" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V147" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="148" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>174</v>
       </c>
@@ -16710,14 +16800,17 @@
         <v>8.3400000000000002E-2</v>
       </c>
       <c r="J148" s="4" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <f t="shared" si="5"/>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U148" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="149" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V148" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="149" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>174</v>
       </c>
@@ -16746,14 +16839,17 @@
         <v>8.3400000000000002E-2</v>
       </c>
       <c r="J149" s="4" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <f t="shared" si="5"/>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U149" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="150" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V149" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="150" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>174</v>
       </c>
@@ -16782,14 +16878,17 @@
         <v>8.3400000000000002E-2</v>
       </c>
       <c r="J150" s="4" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <f t="shared" si="5"/>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U150" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="151" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V150" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="151" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>174</v>
       </c>
@@ -16818,14 +16917,17 @@
         <v>8.3400000000000002E-2</v>
       </c>
       <c r="J151" s="4" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <f t="shared" si="5"/>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U151" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="152" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V151" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="152" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>174</v>
       </c>
@@ -16854,14 +16956,17 @@
         <v>8.3299999999999999E-2</v>
       </c>
       <c r="J152" s="4" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <f t="shared" si="5"/>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U152" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="153" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V152" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="153" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>174</v>
       </c>
@@ -16890,14 +16995,17 @@
         <v>8.3299999999999999E-2</v>
       </c>
       <c r="J153" s="4" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <f t="shared" si="5"/>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U153" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="154" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V153" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="154" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>174</v>
       </c>
@@ -16926,14 +17034,17 @@
         <v>8.3299999999999999E-2</v>
       </c>
       <c r="J154" s="4" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <f t="shared" si="5"/>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U154" s="9" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="155" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V154" s="19" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="155" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>174</v>
       </c>
@@ -16962,16 +17073,25 @@
         <v>8.3299999999999999E-2</v>
       </c>
       <c r="J155" s="4" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
+        <f t="shared" si="5"/>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U155" s="9" t="s">
         <v>658</v>
       </c>
+      <c r="V155" s="19" t="s">
+        <v>686</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AG143" xr:uid="{F5070472-BD41-FC47-BC46-FB0AD4499DE3}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:X66">
+  <autoFilter ref="A1:AH155" xr:uid="{F5070472-BD41-FC47-BC46-FB0AD4499DE3}">
+    <filterColumn colId="20">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:Y66">
     <sortCondition ref="H4:H66"/>
   </sortState>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Dimension item sets add column for active/graduated
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D7AEAC-863E-414A-B3B2-BDBF6B7D3214}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40C7990-95E6-B646-8C54-176E7F9C6466}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4056" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4057" uniqueCount="688">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -2249,6 +2251,9 @@
   </si>
   <si>
     <t>10-50+.&lt;15/&gt;15.d.u</t>
+  </si>
+  <si>
+    <t>ag</t>
   </si>
 </sst>
 </file>
@@ -2683,11 +2688,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
   <dimension ref="A1:AK72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="S57" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W70" sqref="W70"/>
+      <selection pane="bottomRight" activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10851,12 +10856,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:AI155"/>
+  <dimension ref="A1:AJ155"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="6" topLeftCell="S1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V43" sqref="V43"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="6" topLeftCell="AG1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AI2" sqref="AI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10877,7 +10881,7 @@
     <col min="21" max="22" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>221</v>
       </c>
@@ -10981,10 +10985,13 @@
         <v>402</v>
       </c>
       <c r="AI1" t="s">
+        <v>687</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="2" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>174</v>
       </c>
@@ -11013,7 +11020,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="4" t="str">
-        <f t="shared" ref="J2:J33" si="0">_xlfn.TEXTJOIN(";",1,K2:AAB2)</f>
+        <f t="shared" ref="J2:J33" si="0">_xlfn.TEXTJOIN(";",1,K2:AAC2)</f>
         <v>&lt;2mo</v>
       </c>
       <c r="K2" s="9"/>
@@ -11030,7 +11037,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="3" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>174</v>
       </c>
@@ -11076,7 +11083,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>174</v>
       </c>
@@ -11122,7 +11129,7 @@
       </c>
       <c r="V4" s="9"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>174</v>
       </c>
@@ -11163,7 +11170,7 @@
       </c>
       <c r="V5" s="9"/>
     </row>
-    <row r="6" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>174</v>
       </c>
@@ -11196,7 +11203,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>174</v>
       </c>
@@ -11250,7 +11257,7 @@
       </c>
       <c r="V7" s="9"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>174</v>
       </c>
@@ -11304,7 +11311,7 @@
       </c>
       <c r="V8" s="9"/>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>174</v>
       </c>
@@ -11344,7 +11351,7 @@
       </c>
       <c r="V9" s="9"/>
     </row>
-    <row r="10" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>174</v>
       </c>
@@ -11383,7 +11390,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>174</v>
       </c>
@@ -11434,7 +11441,7 @@
       </c>
       <c r="V11" s="9"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>174</v>
       </c>
@@ -11485,7 +11492,7 @@
       </c>
       <c r="V12" s="9"/>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>174</v>
       </c>
@@ -11525,7 +11532,7 @@
       </c>
       <c r="V13" s="9"/>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>174</v>
       </c>
@@ -11583,7 +11590,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>174</v>
       </c>
@@ -11625,7 +11632,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="16" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>143</v>
       </c>
@@ -11667,7 +11674,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>174</v>
       </c>
@@ -11705,7 +11712,7 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>143</v>
       </c>
@@ -11741,7 +11748,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>174</v>
       </c>
@@ -11876,7 +11883,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="22" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>143</v>
       </c>
@@ -11918,7 +11925,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>174</v>
       </c>
@@ -11954,7 +11961,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="24" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>143</v>
       </c>
@@ -11996,7 +12003,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="25" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>174</v>
       </c>
@@ -12037,7 +12044,7 @@
       </c>
       <c r="P25" s="5"/>
     </row>
-    <row r="26" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>174</v>
       </c>
@@ -12177,7 +12184,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="29" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>143</v>
       </c>
@@ -12320,7 +12327,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="32" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>174</v>
       </c>
@@ -12356,7 +12363,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="33" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>143</v>
       </c>
@@ -12398,7 +12405,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="34" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>174</v>
       </c>
@@ -12427,7 +12434,7 @@
         <v>1</v>
       </c>
       <c r="J34" s="4" t="str">
-        <f t="shared" ref="J34:J65" si="1">_xlfn.TEXTJOIN(";",1,K34:AAB34)</f>
+        <f t="shared" ref="J34:J65" si="1">_xlfn.TEXTJOIN(";",1,K34:AAC34)</f>
         <v>&lt;1-18+</v>
       </c>
       <c r="O34" t="s">
@@ -12476,7 +12483,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="36" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>174</v>
       </c>
@@ -12571,7 +12578,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="38" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>143</v>
       </c>
@@ -12655,7 +12662,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="40" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>174</v>
       </c>
@@ -12748,7 +12755,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="42" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>143</v>
       </c>
@@ -12889,7 +12896,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="45" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>174</v>
       </c>
@@ -12982,7 +12989,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="47" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>143</v>
       </c>
@@ -13123,7 +13130,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="50" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>174</v>
       </c>
@@ -13216,7 +13223,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="52" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>143</v>
       </c>
@@ -13357,7 +13364,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="55" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>143</v>
       </c>
@@ -13399,7 +13406,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="56" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>175</v>
       </c>
@@ -13441,7 +13448,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="57" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>143</v>
       </c>
@@ -13483,7 +13490,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="58" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>175</v>
       </c>
@@ -13528,7 +13535,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="59" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>175</v>
       </c>
@@ -13574,7 +13581,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="60" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>143</v>
       </c>
@@ -13616,7 +13623,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="61" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>175</v>
       </c>
@@ -13659,7 +13666,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="62" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>184</v>
       </c>
@@ -13695,7 +13702,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="63" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>184</v>
       </c>
@@ -13731,7 +13738,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="64" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>184</v>
       </c>
@@ -13767,7 +13774,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="65" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>184</v>
       </c>
@@ -13803,7 +13810,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="66" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>184</v>
       </c>
@@ -13832,14 +13839,14 @@
         <v>1</v>
       </c>
       <c r="J66" s="4" t="str">
-        <f t="shared" ref="J66:J97" si="2">_xlfn.TEXTJOIN(";",1,K66:AAB66)</f>
+        <f t="shared" ref="J66:J97" si="2">_xlfn.TEXTJOIN(";",1,K66:AAC66)</f>
         <v>kp1</v>
       </c>
       <c r="Z66" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="67" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>196</v>
       </c>
@@ -13875,7 +13882,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="68" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>196</v>
       </c>
@@ -13911,7 +13918,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="69" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>264</v>
       </c>
@@ -13947,7 +13954,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="70" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>264</v>
       </c>
@@ -13983,7 +13990,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="71" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>264</v>
       </c>
@@ -14019,7 +14026,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="72" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>278</v>
       </c>
@@ -14055,7 +14062,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="73" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>278</v>
       </c>
@@ -14091,7 +14098,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="74" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>278</v>
       </c>
@@ -14127,7 +14134,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="75" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>278</v>
       </c>
@@ -14163,7 +14170,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="76" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>278</v>
       </c>
@@ -14199,7 +14206,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="77" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>278</v>
       </c>
@@ -14235,7 +14242,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="78" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>278</v>
       </c>
@@ -14271,7 +14278,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="79" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>278</v>
       </c>
@@ -14307,7 +14314,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="80" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>278</v>
       </c>
@@ -14343,7 +14350,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="81" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>278</v>
       </c>
@@ -14379,7 +14386,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="82" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>278</v>
       </c>
@@ -14415,7 +14422,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="83" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>278</v>
       </c>
@@ -14451,7 +14458,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="84" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>278</v>
       </c>
@@ -14487,7 +14494,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="85" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>278</v>
       </c>
@@ -14523,7 +14530,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="86" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>278</v>
       </c>
@@ -14559,7 +14566,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="87" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>278</v>
       </c>
@@ -14595,7 +14602,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="88" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>278</v>
       </c>
@@ -14631,7 +14638,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="89" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>278</v>
       </c>
@@ -14667,7 +14674,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="90" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>278</v>
       </c>
@@ -14703,7 +14710,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="91" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>278</v>
       </c>
@@ -14739,7 +14746,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="92" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>278</v>
       </c>
@@ -14775,7 +14782,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="93" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>278</v>
       </c>
@@ -14811,7 +14818,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="94" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>278</v>
       </c>
@@ -14847,7 +14854,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="95" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>278</v>
       </c>
@@ -14883,7 +14890,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="96" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>278</v>
       </c>
@@ -14919,7 +14926,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="97" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>278</v>
       </c>
@@ -14955,7 +14962,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="98" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>278</v>
       </c>
@@ -14984,14 +14991,14 @@
         <v>1</v>
       </c>
       <c r="J98" s="4" t="str">
-        <f t="shared" ref="J98:J129" si="3">_xlfn.TEXTJOIN(";",1,K98:AAB98)</f>
+        <f t="shared" ref="J98:J129" si="3">_xlfn.TEXTJOIN(";",1,K98:AAC98)</f>
         <v>st_ua</v>
       </c>
       <c r="AF98" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="99" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>278</v>
       </c>
@@ -15027,7 +15034,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="100" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>278</v>
       </c>
@@ -15063,7 +15070,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="101" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>278</v>
       </c>
@@ -15099,7 +15106,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="102" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>278</v>
       </c>
@@ -15135,7 +15142,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="103" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>278</v>
       </c>
@@ -15171,7 +15178,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="104" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>278</v>
       </c>
@@ -15207,7 +15214,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="105" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>278</v>
       </c>
@@ -15243,7 +15250,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="106" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>278</v>
       </c>
@@ -15279,7 +15286,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="107" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>278</v>
       </c>
@@ -15315,7 +15322,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="108" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>278</v>
       </c>
@@ -15351,7 +15358,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="109" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>278</v>
       </c>
@@ -15387,7 +15394,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="110" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>278</v>
       </c>
@@ -15423,7 +15430,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="111" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>278</v>
       </c>
@@ -15459,7 +15466,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="112" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>278</v>
       </c>
@@ -15495,7 +15502,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="113" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>278</v>
       </c>
@@ -15531,7 +15538,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="114" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>381</v>
       </c>
@@ -15567,7 +15574,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="115" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>381</v>
       </c>
@@ -15603,7 +15610,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="116" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>278</v>
       </c>
@@ -15639,7 +15646,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="117" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>278</v>
       </c>
@@ -15675,7 +15682,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="118" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>278</v>
       </c>
@@ -15711,7 +15718,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="119" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>278</v>
       </c>
@@ -15747,7 +15754,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="120" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>278</v>
       </c>
@@ -15783,7 +15790,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="121" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>278</v>
       </c>
@@ -15819,7 +15826,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="122" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>278</v>
       </c>
@@ -15855,7 +15862,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="123" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>278</v>
       </c>
@@ -15891,7 +15898,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="124" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>196</v>
       </c>
@@ -15927,7 +15934,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="125" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>196</v>
       </c>
@@ -15963,7 +15970,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="126" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>509</v>
       </c>
@@ -15995,11 +16002,11 @@
         <f t="shared" si="3"/>
         <v>hts_mod_com_ndx</v>
       </c>
-      <c r="AI126" t="s">
+      <c r="AJ126" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="127" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>509</v>
       </c>
@@ -16031,11 +16038,11 @@
         <f t="shared" si="3"/>
         <v>hts_mod_fac_ndx</v>
       </c>
-      <c r="AI127" t="s">
+      <c r="AJ127" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="128" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>509</v>
       </c>
@@ -16067,11 +16074,11 @@
         <f t="shared" si="3"/>
         <v>hts_mod_com_mob</v>
       </c>
-      <c r="AI128" t="s">
+      <c r="AJ128" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="129" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>509</v>
       </c>
@@ -16103,11 +16110,11 @@
         <f t="shared" si="3"/>
         <v>hts_mod_com_vct</v>
       </c>
-      <c r="AI129" t="s">
+      <c r="AJ129" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="130" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>509</v>
       </c>
@@ -16136,14 +16143,14 @@
         <v>1</v>
       </c>
       <c r="J130" t="str">
-        <f t="shared" ref="J130:J161" si="4">_xlfn.TEXTJOIN(";",1,K130:AAB130)</f>
+        <f t="shared" ref="J130:J143" si="4">_xlfn.TEXTJOIN(";",1,K130:AAC130)</f>
         <v>hts_mod_com_otr</v>
       </c>
-      <c r="AI130" t="s">
+      <c r="AJ130" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="131" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>509</v>
       </c>
@@ -16175,11 +16182,11 @@
         <f t="shared" si="4"/>
         <v>hts_mod_fac_ew</v>
       </c>
-      <c r="AI131" t="s">
+      <c r="AJ131" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="132" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>509</v>
       </c>
@@ -16211,11 +16218,11 @@
         <f t="shared" si="4"/>
         <v>hts_mod_fac_inpat</v>
       </c>
-      <c r="AI132" t="s">
+      <c r="AJ132" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="133" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>509</v>
       </c>
@@ -16247,11 +16254,11 @@
         <f t="shared" si="4"/>
         <v>hts_mod_fac_nut</v>
       </c>
-      <c r="AI133" t="s">
+      <c r="AJ133" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="134" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>509</v>
       </c>
@@ -16283,11 +16290,11 @@
         <f t="shared" si="4"/>
         <v>hts_mod_fac_ped</v>
       </c>
-      <c r="AI134" t="s">
+      <c r="AJ134" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="135" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>509</v>
       </c>
@@ -16319,11 +16326,11 @@
         <f t="shared" si="4"/>
         <v>hts_mod_fac_sti</v>
       </c>
-      <c r="AI135" t="s">
+      <c r="AJ135" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="136" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>509</v>
       </c>
@@ -16355,11 +16362,11 @@
         <f t="shared" si="4"/>
         <v>hts_mod_fac_vct</v>
       </c>
-      <c r="AI136" t="s">
+      <c r="AJ136" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="137" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>509</v>
       </c>
@@ -16391,11 +16398,11 @@
         <f t="shared" si="4"/>
         <v>hts_mod_fac_otr_pitc</v>
       </c>
-      <c r="AI137" t="s">
+      <c r="AJ137" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="138" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>509</v>
       </c>
@@ -16427,11 +16434,11 @@
         <f t="shared" si="4"/>
         <v>hts_mod_fac_vmmc</v>
       </c>
-      <c r="AI138" t="s">
+      <c r="AJ138" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="139" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>509</v>
       </c>
@@ -16463,11 +16470,11 @@
         <f t="shared" si="4"/>
         <v>hts_mod_fac_anc_1</v>
       </c>
-      <c r="AI139" t="s">
+      <c r="AJ139" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="140" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>509</v>
       </c>
@@ -16499,11 +16506,11 @@
         <f t="shared" si="4"/>
         <v>hts_mod_fac_tb</v>
       </c>
-      <c r="AI140" t="s">
+      <c r="AJ140" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="141" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>509</v>
       </c>
@@ -16535,11 +16542,11 @@
         <f t="shared" si="4"/>
         <v>hts_mod_fac_post_anc_1</v>
       </c>
-      <c r="AI141" t="s">
+      <c r="AJ141" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="142" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>174</v>
       </c>
@@ -16581,11 +16588,11 @@
       <c r="T142" s="9"/>
       <c r="U142" s="9"/>
       <c r="V142" s="9"/>
-      <c r="AI142" t="s">
+      <c r="AJ142" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="143" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>175</v>
       </c>
@@ -16617,11 +16624,11 @@
         <f t="shared" si="4"/>
         <v>U_sex</v>
       </c>
-      <c r="AI143" t="s">
+      <c r="AJ143" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="144" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>174</v>
       </c>
@@ -16650,7 +16657,7 @@
         <v>8.3299999999999999E-2</v>
       </c>
       <c r="J144" s="4" t="str">
-        <f t="shared" ref="J144:J155" si="5">_xlfn.TEXTJOIN(";",1,K144:AAB144)</f>
+        <f t="shared" ref="J144:J155" si="5">_xlfn.TEXTJOIN(";",1,K144:AAC144)</f>
         <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U144" s="9" t="s">
@@ -16761,7 +16768,7 @@
         <v>8.3299999999999999E-2</v>
       </c>
       <c r="J147" s="4" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K147:AAB147)</f>
+        <f>_xlfn.TEXTJOIN(";",1,K147:AAC147)</f>
         <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U147" s="9" t="s">
@@ -17084,13 +17091,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AH155" xr:uid="{F5070472-BD41-FC47-BC46-FB0AD4499DE3}">
-    <filterColumn colId="20">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AH155" xr:uid="{F5070472-BD41-FC47-BC46-FB0AD4499DE3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:Y66">
     <sortCondition ref="H4:H66"/>
   </sortState>

</xml_diff>

<commit_message>
dimension_item_sets add rows for active/graduated for OVC_SERV
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40C7990-95E6-B646-8C54-176E7F9C6466}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4274801C-B2D5-1E4D-B99F-359C5131C623}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4057" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4073" uniqueCount="696">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -2254,6 +2254,30 @@
   </si>
   <si>
     <t>ag</t>
+  </si>
+  <si>
+    <t>PohP5DBPfMs</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>q1ViBVu6waQ</t>
+  </si>
+  <si>
+    <t>Graduated</t>
+  </si>
+  <si>
+    <t>McLoJJs4bki</t>
+  </si>
+  <si>
+    <t>Program Status v2</t>
+  </si>
+  <si>
+    <t>ag_a</t>
+  </si>
+  <si>
+    <t>ag_g</t>
   </si>
 </sst>
 </file>
@@ -10856,11 +10880,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
-  <dimension ref="A1:AJ155"/>
+  <dimension ref="A1:AJ157"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="6" topLeftCell="AG1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AI2" sqref="AI2"/>
+    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="6" topLeftCell="AQ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AV157" sqref="AV157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16657,7 +16681,7 @@
         <v>8.3299999999999999E-2</v>
       </c>
       <c r="J144" s="4" t="str">
-        <f t="shared" ref="J144:J155" si="5">_xlfn.TEXTJOIN(";",1,K144:AAC144)</f>
+        <f t="shared" ref="J144:J157" si="5">_xlfn.TEXTJOIN(";",1,K144:AAC144)</f>
         <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U144" s="9" t="s">
@@ -16665,7 +16689,7 @@
       </c>
       <c r="V144" s="19"/>
     </row>
-    <row r="145" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>174</v>
       </c>
@@ -16702,7 +16726,7 @@
       </c>
       <c r="V145" s="9"/>
     </row>
-    <row r="146" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>174</v>
       </c>
@@ -16739,7 +16763,7 @@
       </c>
       <c r="V146" s="9"/>
     </row>
-    <row r="147" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>174</v>
       </c>
@@ -16778,7 +16802,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="148" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>174</v>
       </c>
@@ -16817,7 +16841,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="149" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>174</v>
       </c>
@@ -16856,7 +16880,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="150" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>174</v>
       </c>
@@ -16895,7 +16919,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="151" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>174</v>
       </c>
@@ -16934,7 +16958,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="152" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>174</v>
       </c>
@@ -16973,7 +16997,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="153" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>174</v>
       </c>
@@ -17012,7 +17036,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="154" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>174</v>
       </c>
@@ -17051,7 +17075,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="155" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>174</v>
       </c>
@@ -17088,6 +17112,78 @@
       </c>
       <c r="V155" s="19" t="s">
         <v>686</v>
+      </c>
+    </row>
+    <row r="156" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>692</v>
+      </c>
+      <c r="B156" t="s">
+        <v>693</v>
+      </c>
+      <c r="C156" t="s">
+        <v>688</v>
+      </c>
+      <c r="D156" t="s">
+        <v>436</v>
+      </c>
+      <c r="E156" t="s">
+        <v>689</v>
+      </c>
+      <c r="F156" t="s">
+        <v>689</v>
+      </c>
+      <c r="G156" t="s">
+        <v>688</v>
+      </c>
+      <c r="H156" s="7">
+        <v>1</v>
+      </c>
+      <c r="I156" s="12">
+        <v>1</v>
+      </c>
+      <c r="J156" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>ag_a</v>
+      </c>
+      <c r="AI156" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="157" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>692</v>
+      </c>
+      <c r="B157" t="s">
+        <v>693</v>
+      </c>
+      <c r="C157" t="s">
+        <v>690</v>
+      </c>
+      <c r="D157" t="s">
+        <v>436</v>
+      </c>
+      <c r="E157" t="s">
+        <v>691</v>
+      </c>
+      <c r="F157" t="s">
+        <v>691</v>
+      </c>
+      <c r="G157" t="s">
+        <v>690</v>
+      </c>
+      <c r="H157" s="7">
+        <v>2</v>
+      </c>
+      <c r="I157" s="12">
+        <v>1</v>
+      </c>
+      <c r="J157" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>ag_g</v>
+      </c>
+      <c r="AI157" t="s">
+        <v>695</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data_reequired update pe dimension for impatt.priority_snu
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4274801C-B2D5-1E4D-B99F-359C5131C623}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1094336-184F-284D-BC9D-B9E5F34A6D48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4073" uniqueCount="696">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4073" uniqueCount="695">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1718,9 +1718,6 @@
   </si>
   <si>
     <t>GEND_GBV (DSD+TA, Age/Sex/ViolenceType)</t>
-  </si>
-  <si>
-    <t>2019Q4</t>
   </si>
   <si>
     <t>KP_MAT.N.Sex.T_1</t>
@@ -2712,11 +2709,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
   <dimension ref="A1:AK72"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C57" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="H57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B65" sqref="B65"/>
+      <selection pane="bottomRight" activeCell="J60" sqref="J60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2854,13 +2851,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -2973,7 +2970,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
@@ -3086,7 +3083,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
@@ -3199,7 +3196,7 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
@@ -3312,7 +3309,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -3419,13 +3416,13 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E7" t="s">
         <v>3</v>
@@ -3538,7 +3535,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
@@ -3651,7 +3648,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
@@ -3764,7 +3761,7 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
@@ -3871,13 +3868,13 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E11" t="s">
         <v>3</v>
@@ -3990,7 +3987,7 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E12" t="s">
         <v>6</v>
@@ -4103,7 +4100,7 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
@@ -4210,13 +4207,13 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E14" t="s">
         <v>3</v>
@@ -4329,7 +4326,7 @@
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
@@ -4442,7 +4439,7 @@
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E16" t="s">
         <v>6</v>
@@ -4555,7 +4552,7 @@
         <v>5</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="E17" t="s">
         <v>6</v>
@@ -4668,7 +4665,7 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E18" t="s">
         <v>6</v>
@@ -4781,7 +4778,7 @@
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="E19" t="s">
         <v>6</v>
@@ -4894,7 +4891,7 @@
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="E20" t="s">
         <v>6</v>
@@ -5007,7 +5004,7 @@
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="E21" t="s">
         <v>6</v>
@@ -5120,7 +5117,7 @@
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E22" t="s">
         <v>6</v>
@@ -5233,7 +5230,7 @@
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="E23" t="s">
         <v>6</v>
@@ -5346,7 +5343,7 @@
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E24" t="s">
         <v>6</v>
@@ -5459,7 +5456,7 @@
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E25" t="s">
         <v>6</v>
@@ -5572,7 +5569,7 @@
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="E26" t="s">
         <v>6</v>
@@ -5685,7 +5682,7 @@
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="E27" t="s">
         <v>6</v>
@@ -5798,7 +5795,7 @@
         <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E28" t="s">
         <v>6</v>
@@ -5911,7 +5908,7 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E29" t="s">
         <v>6</v>
@@ -6024,7 +6021,7 @@
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="E30" t="s">
         <v>6</v>
@@ -6137,7 +6134,7 @@
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="E31" t="s">
         <v>6</v>
@@ -6250,7 +6247,7 @@
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E32" t="s">
         <v>6</v>
@@ -6363,7 +6360,7 @@
         <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E33" t="s">
         <v>6</v>
@@ -6476,7 +6473,7 @@
         <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="E34" t="s">
         <v>6</v>
@@ -6589,7 +6586,7 @@
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E35" t="s">
         <v>6</v>
@@ -6702,7 +6699,7 @@
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="E36" t="s">
         <v>6</v>
@@ -6815,7 +6812,7 @@
         <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="E37" t="s">
         <v>6</v>
@@ -6922,13 +6919,13 @@
         <v>21</v>
       </c>
       <c r="B38" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
       </c>
       <c r="D38" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="E38" t="s">
         <v>6</v>
@@ -6958,7 +6955,7 @@
         <v>143</v>
       </c>
       <c r="N38" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="O38" t="s">
         <v>143</v>
@@ -7035,13 +7032,13 @@
         <v>21</v>
       </c>
       <c r="B39" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C39" t="s">
         <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E39" t="s">
         <v>3</v>
@@ -7148,13 +7145,13 @@
         <v>21</v>
       </c>
       <c r="B40" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C40" t="s">
         <v>2</v>
       </c>
       <c r="D40" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="E40" t="s">
         <v>3</v>
@@ -7267,7 +7264,7 @@
         <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="E41" t="s">
         <v>6</v>
@@ -7380,7 +7377,7 @@
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E42" t="s">
         <v>6</v>
@@ -7493,7 +7490,7 @@
         <v>5</v>
       </c>
       <c r="D43" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E43" t="s">
         <v>6</v>
@@ -7600,13 +7597,13 @@
         <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C44" t="s">
         <v>2</v>
       </c>
       <c r="D44" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E44" t="s">
         <v>3</v>
@@ -7719,7 +7716,7 @@
         <v>5</v>
       </c>
       <c r="D45" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E45" t="s">
         <v>6</v>
@@ -7826,13 +7823,13 @@
         <v>48</v>
       </c>
       <c r="B46" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C46" t="s">
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E46" t="s">
         <v>3</v>
@@ -7939,13 +7936,13 @@
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C47" t="s">
         <v>2</v>
       </c>
       <c r="D47" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E47" t="s">
         <v>3</v>
@@ -8052,13 +8049,13 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C48" t="s">
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E48" t="s">
         <v>3</v>
@@ -8165,13 +8162,13 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C49" t="s">
         <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="E49" t="s">
         <v>3</v>
@@ -8278,13 +8275,13 @@
         <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C50" t="s">
         <v>2</v>
       </c>
       <c r="D50" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E50" t="s">
         <v>3</v>
@@ -8397,7 +8394,7 @@
         <v>5</v>
       </c>
       <c r="D51" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="E51" t="s">
         <v>6</v>
@@ -8504,13 +8501,13 @@
         <v>55</v>
       </c>
       <c r="B52" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C52" t="s">
         <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E52" t="s">
         <v>3</v>
@@ -8617,13 +8614,13 @@
         <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C53" t="s">
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E53" t="s">
         <v>3</v>
@@ -8632,13 +8629,13 @@
         <v>142</v>
       </c>
       <c r="G53" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="H53" t="s">
         <v>573</v>
       </c>
-      <c r="H53" t="s">
+      <c r="I53" t="s">
         <v>574</v>
-      </c>
-      <c r="I53" t="s">
-        <v>575</v>
       </c>
       <c r="J53" t="s">
         <v>457</v>
@@ -8730,13 +8727,13 @@
         <v>57</v>
       </c>
       <c r="B54" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C54" t="s">
         <v>2</v>
       </c>
       <c r="D54" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E54" t="s">
         <v>3</v>
@@ -8843,13 +8840,13 @@
         <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C55" t="s">
         <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E55" t="s">
         <v>3</v>
@@ -8962,7 +8959,7 @@
         <v>5</v>
       </c>
       <c r="D56" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="E56" t="s">
         <v>6</v>
@@ -9069,13 +9066,13 @@
         <v>48</v>
       </c>
       <c r="B57" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C57" t="s">
         <v>2</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E57" t="s">
         <v>3</v>
@@ -9182,13 +9179,13 @@
         <v>48</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C58" t="s">
         <v>2</v>
       </c>
       <c r="D58" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="E58" t="s">
         <v>3</v>
@@ -9197,13 +9194,13 @@
         <v>142</v>
       </c>
       <c r="G58" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="H58" t="s">
+        <v>575</v>
+      </c>
+      <c r="I58" s="14" t="s">
         <v>578</v>
-      </c>
-      <c r="H58" t="s">
-        <v>576</v>
-      </c>
-      <c r="I58" s="14" t="s">
-        <v>579</v>
       </c>
       <c r="J58" t="s">
         <v>457</v>
@@ -9295,7 +9292,7 @@
         <v>48</v>
       </c>
       <c r="B59" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C59" t="s">
         <v>2</v>
@@ -9408,13 +9405,13 @@
         <v>450</v>
       </c>
       <c r="B60" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C60" t="s">
         <v>2</v>
       </c>
       <c r="D60" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="E60" t="s">
         <v>3</v>
@@ -9432,7 +9429,7 @@
         <v>451</v>
       </c>
       <c r="J60" t="s">
-        <v>560</v>
+        <v>457</v>
       </c>
       <c r="K60" t="s">
         <v>143</v>
@@ -9521,13 +9518,13 @@
         <v>21</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C61" t="s">
         <v>5</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E61" t="s">
         <v>6</v>
@@ -9581,10 +9578,10 @@
         <v>143</v>
       </c>
       <c r="V61" t="s">
+        <v>566</v>
+      </c>
+      <c r="W61" t="s">
         <v>567</v>
-      </c>
-      <c r="W61" t="s">
-        <v>568</v>
       </c>
       <c r="X61" s="1" t="s">
         <v>139</v>
@@ -9634,13 +9631,13 @@
         <v>21</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C62" t="s">
         <v>2</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E62" t="s">
         <v>3</v>
@@ -9747,13 +9744,13 @@
         <v>19</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C63" t="s">
         <v>2</v>
       </c>
       <c r="D63" s="15" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="E63" t="s">
         <v>3</v>
@@ -9765,16 +9762,16 @@
         <v>143</v>
       </c>
       <c r="H63" s="16" t="s">
+        <v>655</v>
+      </c>
+      <c r="I63" s="16" t="s">
+        <v>654</v>
+      </c>
+      <c r="J63" t="s">
         <v>656</v>
       </c>
-      <c r="I63" s="16" t="s">
-        <v>655</v>
-      </c>
-      <c r="J63" t="s">
+      <c r="K63" s="9" t="s">
         <v>657</v>
-      </c>
-      <c r="K63" s="9" t="s">
-        <v>658</v>
       </c>
       <c r="L63" t="s">
         <v>145</v>
@@ -9860,13 +9857,13 @@
         <v>19</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C64" t="s">
         <v>2</v>
       </c>
       <c r="D64" s="16" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E64" t="s">
         <v>3</v>
@@ -9878,16 +9875,16 @@
         <v>143</v>
       </c>
       <c r="H64" s="16" t="s">
+        <v>659</v>
+      </c>
+      <c r="I64" s="16" t="s">
         <v>660</v>
-      </c>
-      <c r="I64" s="16" t="s">
-        <v>661</v>
       </c>
       <c r="J64" t="s">
         <v>139</v>
       </c>
       <c r="K64" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="L64" t="s">
         <v>145</v>
@@ -9973,13 +9970,13 @@
         <v>19</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C65" t="s">
         <v>2</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="E65" t="s">
         <v>3</v>
@@ -9991,10 +9988,10 @@
         <v>143</v>
       </c>
       <c r="H65" s="11" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="I65" s="16" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="J65" t="s">
         <v>457</v>
@@ -10086,13 +10083,13 @@
         <v>19</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C66" t="s">
         <v>2</v>
       </c>
       <c r="D66" s="15" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E66" t="s">
         <v>3</v>
@@ -10104,10 +10101,10 @@
         <v>143</v>
       </c>
       <c r="H66" t="s">
+        <v>665</v>
+      </c>
+      <c r="I66" t="s">
         <v>666</v>
-      </c>
-      <c r="I66" t="s">
-        <v>667</v>
       </c>
       <c r="J66" t="s">
         <v>457</v>
@@ -10199,13 +10196,13 @@
         <v>19</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C67" t="s">
         <v>5</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="E67" t="s">
         <v>6</v>
@@ -10217,10 +10214,10 @@
         <v>143</v>
       </c>
       <c r="H67" t="s">
+        <v>669</v>
+      </c>
+      <c r="I67" t="s">
         <v>670</v>
-      </c>
-      <c r="I67" t="s">
-        <v>671</v>
       </c>
       <c r="J67" t="s">
         <v>139</v>
@@ -10259,16 +10256,16 @@
         <v>143</v>
       </c>
       <c r="V67" s="16" t="s">
+        <v>659</v>
+      </c>
+      <c r="W67" s="16" t="s">
         <v>660</v>
-      </c>
-      <c r="W67" s="16" t="s">
-        <v>661</v>
       </c>
       <c r="X67" t="s">
         <v>139</v>
       </c>
       <c r="Y67" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="Z67" t="s">
         <v>145</v>
@@ -10312,13 +10309,13 @@
         <v>19</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C68" t="s">
         <v>5</v>
       </c>
       <c r="D68" s="16" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="E68" t="s">
         <v>6</v>
@@ -10330,10 +10327,10 @@
         <v>143</v>
       </c>
       <c r="H68" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="I68" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="J68" t="s">
         <v>139</v>
@@ -10372,16 +10369,16 @@
         <v>143</v>
       </c>
       <c r="V68" s="16" t="s">
+        <v>659</v>
+      </c>
+      <c r="W68" s="16" t="s">
         <v>660</v>
-      </c>
-      <c r="W68" s="16" t="s">
-        <v>661</v>
       </c>
       <c r="X68" t="s">
         <v>139</v>
       </c>
       <c r="Y68" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="Z68" t="s">
         <v>141</v>
@@ -10425,13 +10422,13 @@
         <v>19</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C69" t="s">
         <v>5</v>
       </c>
       <c r="D69" s="16" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="E69" t="s">
         <v>6</v>
@@ -10461,7 +10458,7 @@
         <v>143</v>
       </c>
       <c r="N69" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="O69" t="s">
         <v>143</v>
@@ -10485,16 +10482,16 @@
         <v>143</v>
       </c>
       <c r="V69" s="16" t="s">
+        <v>659</v>
+      </c>
+      <c r="W69" s="16" t="s">
         <v>660</v>
-      </c>
-      <c r="W69" s="16" t="s">
-        <v>661</v>
       </c>
       <c r="X69" t="s">
         <v>139</v>
       </c>
       <c r="Y69" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="Z69" t="s">
         <v>141</v>
@@ -10538,13 +10535,13 @@
         <v>19</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C70" t="s">
         <v>5</v>
       </c>
       <c r="D70" s="16" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="E70" t="s">
         <v>6</v>
@@ -10598,16 +10595,16 @@
         <v>143</v>
       </c>
       <c r="V70" s="16" t="s">
+        <v>659</v>
+      </c>
+      <c r="W70" s="16" t="s">
         <v>660</v>
-      </c>
-      <c r="W70" s="16" t="s">
-        <v>661</v>
       </c>
       <c r="X70" t="s">
         <v>139</v>
       </c>
       <c r="Y70" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="Z70" t="s">
         <v>148</v>
@@ -10651,13 +10648,13 @@
         <v>43</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C71" t="s">
         <v>2</v>
       </c>
       <c r="D71" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="E71" t="s">
         <v>3</v>
@@ -10669,10 +10666,10 @@
         <v>143</v>
       </c>
       <c r="H71" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="J71" t="s">
         <v>457</v>
@@ -10764,13 +10761,13 @@
         <v>43</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C72" t="s">
         <v>2</v>
       </c>
       <c r="D72" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="E72" t="s">
         <v>3</v>
@@ -10782,10 +10779,10 @@
         <v>143</v>
       </c>
       <c r="H72" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="J72" t="s">
         <v>457</v>
@@ -10882,9 +10879,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
   <dimension ref="A1:AJ157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A122" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="6" topLeftCell="AQ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AV157" sqref="AV157"/>
+      <selection pane="topRight" activeCell="F144" sqref="F144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10967,10 +10964,10 @@
         <v>183</v>
       </c>
       <c r="U1" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V1" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="W1" t="s">
         <v>216</v>
@@ -11009,7 +11006,7 @@
         <v>402</v>
       </c>
       <c r="AI1" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="AJ1" t="s">
         <v>437</v>
@@ -11149,7 +11146,7 @@
         <v>229</v>
       </c>
       <c r="U4" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V4" s="9"/>
     </row>
@@ -11190,7 +11187,7 @@
         <v>171</v>
       </c>
       <c r="U5" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V5" s="9"/>
     </row>
@@ -11277,7 +11274,7 @@
         <v>226</v>
       </c>
       <c r="U7" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V7" s="9"/>
     </row>
@@ -11331,7 +11328,7 @@
         <v>226</v>
       </c>
       <c r="U8" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V8" s="9"/>
     </row>
@@ -11371,7 +11368,7 @@
         <v>171</v>
       </c>
       <c r="U9" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V9" s="9"/>
     </row>
@@ -11461,7 +11458,7 @@
         <v>226</v>
       </c>
       <c r="U11" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V11" s="9"/>
     </row>
@@ -11512,7 +11509,7 @@
         <v>226</v>
       </c>
       <c r="U12" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V12" s="9"/>
     </row>
@@ -11552,7 +11549,7 @@
         <v>171</v>
       </c>
       <c r="U13" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V13" s="9"/>
     </row>
@@ -11608,10 +11605,10 @@
         <v>183</v>
       </c>
       <c r="U14" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V14" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.2">
@@ -11650,10 +11647,10 @@
         <v>171</v>
       </c>
       <c r="U15" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V15" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.2">
@@ -11844,10 +11841,10 @@
         <v>171</v>
       </c>
       <c r="U20" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V20" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.2">
@@ -11901,10 +11898,10 @@
         <v>183</v>
       </c>
       <c r="U21" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V21" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.2">
@@ -12145,10 +12142,10 @@
         <v>171</v>
       </c>
       <c r="U27" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V27" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.2">
@@ -12202,10 +12199,10 @@
         <v>183</v>
       </c>
       <c r="U28" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V28" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
@@ -12286,10 +12283,10 @@
         <v>171</v>
       </c>
       <c r="U30" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V30" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
@@ -12345,10 +12342,10 @@
         <v>183</v>
       </c>
       <c r="U31" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V31" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.2">
@@ -12501,10 +12498,10 @@
         <v>171</v>
       </c>
       <c r="U35" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V35" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.2">
@@ -12596,10 +12593,10 @@
         <v>183</v>
       </c>
       <c r="U37" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V37" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.2">
@@ -12680,10 +12677,10 @@
         <v>171</v>
       </c>
       <c r="U39" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V39" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.2">
@@ -12773,10 +12770,10 @@
         <v>183</v>
       </c>
       <c r="U41" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V41" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.2">
@@ -12872,10 +12869,10 @@
         <v>183</v>
       </c>
       <c r="U43" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V43" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.2">
@@ -12914,10 +12911,10 @@
         <v>171</v>
       </c>
       <c r="U44" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V44" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.2">
@@ -13007,10 +13004,10 @@
         <v>183</v>
       </c>
       <c r="U46" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V46" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.2">
@@ -13106,10 +13103,10 @@
         <v>183</v>
       </c>
       <c r="U48" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V48" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.2">
@@ -13148,10 +13145,10 @@
         <v>171</v>
       </c>
       <c r="U49" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V49" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.2">
@@ -13241,10 +13238,10 @@
         <v>183</v>
       </c>
       <c r="U51" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V51" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.2">
@@ -13325,10 +13322,10 @@
         <v>171</v>
       </c>
       <c r="U53" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V53" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.2">
@@ -13382,10 +13379,10 @@
         <v>183</v>
       </c>
       <c r="U54" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V54" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.2">
@@ -16542,13 +16539,13 @@
         <v>510</v>
       </c>
       <c r="C141" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D141" t="s">
         <v>436</v>
       </c>
       <c r="E141" s="17" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F141" t="s">
         <v>143</v>
@@ -16567,7 +16564,7 @@
         <v>hts_mod_fac_post_anc_1</v>
       </c>
       <c r="AJ141" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="142" spans="1:36" x14ac:dyDescent="0.2">
@@ -16685,7 +16682,7 @@
         <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U144" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V144" s="19"/>
     </row>
@@ -16722,7 +16719,7 @@
         <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U145" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V145" s="9"/>
     </row>
@@ -16759,7 +16756,7 @@
         <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U146" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V146" s="9"/>
     </row>
@@ -16796,10 +16793,10 @@
         <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U147" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V147" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="148" spans="1:35" x14ac:dyDescent="0.2">
@@ -16835,10 +16832,10 @@
         <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U148" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V148" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="149" spans="1:35" x14ac:dyDescent="0.2">
@@ -16874,10 +16871,10 @@
         <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U149" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V149" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="150" spans="1:35" x14ac:dyDescent="0.2">
@@ -16913,10 +16910,10 @@
         <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U150" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V150" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="151" spans="1:35" x14ac:dyDescent="0.2">
@@ -16952,10 +16949,10 @@
         <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U151" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V151" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="152" spans="1:35" x14ac:dyDescent="0.2">
@@ -16991,10 +16988,10 @@
         <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U152" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V152" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="153" spans="1:35" x14ac:dyDescent="0.2">
@@ -17030,10 +17027,10 @@
         <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U153" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V153" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="154" spans="1:35" x14ac:dyDescent="0.2">
@@ -17069,10 +17066,10 @@
         <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U154" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V154" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="155" spans="1:35" x14ac:dyDescent="0.2">
@@ -17108,33 +17105,33 @@
         <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U155" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="V155" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="156" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
+        <v>691</v>
+      </c>
+      <c r="B156" t="s">
         <v>692</v>
       </c>
-      <c r="B156" t="s">
-        <v>693</v>
-      </c>
       <c r="C156" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D156" t="s">
         <v>436</v>
       </c>
       <c r="E156" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="F156" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="G156" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="H156" s="7">
         <v>1</v>
@@ -17147,30 +17144,30 @@
         <v>ag_a</v>
       </c>
       <c r="AI156" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="157" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
+        <v>691</v>
+      </c>
+      <c r="B157" t="s">
         <v>692</v>
       </c>
-      <c r="B157" t="s">
-        <v>693</v>
-      </c>
       <c r="C157" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D157" t="s">
         <v>436</v>
       </c>
       <c r="E157" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="F157" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="G157" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="H157" s="7">
         <v>2</v>
@@ -17183,7 +17180,7 @@
         <v>ag_g</v>
       </c>
       <c r="AI157" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dimension_item_sets update for test status specific
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1094336-184F-284D-BC9D-B9E5F34A6D48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27967082-CE2D-7C43-8DF9-07D28B98A737}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="-280" yWindow="760" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data_required!$A$1:$AK$60</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">dimension_Item_sets!$A$1:$AH$155</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">dimension_Item_sets!$A$1:$AH$160</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4073" uniqueCount="695">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4097" uniqueCount="706">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -2275,6 +2275,39 @@
   </si>
   <si>
     <t>ag_g</t>
+  </si>
+  <si>
+    <t>HIV Positive (Specific)</t>
+  </si>
+  <si>
+    <t>HIV Negative (Specific)</t>
+  </si>
+  <si>
+    <t>HIV Status Unknown (Specific)</t>
+  </si>
+  <si>
+    <t>awSDzziN3Dn</t>
+  </si>
+  <si>
+    <t>EvyNJHbQ7ZE</t>
+  </si>
+  <si>
+    <t>i4Fgst9vzF9</t>
+  </si>
+  <si>
+    <t>tss_Pos</t>
+  </si>
+  <si>
+    <t>tss_Neg</t>
+  </si>
+  <si>
+    <t>tss_Unknown</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>gUdtLH3fV1m</t>
   </si>
 </sst>
 </file>
@@ -2709,11 +2742,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5E70E-6A90-034D-92D2-04FEFE90502B}">
   <dimension ref="A1:AK72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H57" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J60" sqref="J60"/>
+      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10877,11 +10910,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
-  <dimension ref="A1:AJ157"/>
+  <dimension ref="A1:AJ160"/>
   <sheetViews>
-    <sheetView topLeftCell="A122" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="6" topLeftCell="AQ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F144" sqref="F144"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13860,7 +13893,7 @@
         <v>1</v>
       </c>
       <c r="J66" s="4" t="str">
-        <f t="shared" ref="J66:J97" si="2">_xlfn.TEXTJOIN(";",1,K66:AAC66)</f>
+        <f t="shared" ref="J66:J100" si="2">_xlfn.TEXTJOIN(";",1,K66:AAC66)</f>
         <v>kp1</v>
       </c>
       <c r="Z66" t="s">
@@ -14049,110 +14082,110 @@
     </row>
     <row r="72" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="B72" t="s">
-        <v>416</v>
+        <v>265</v>
       </c>
       <c r="C72" t="s">
-        <v>279</v>
+        <v>698</v>
       </c>
       <c r="D72" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="E72" t="s">
-        <v>282</v>
+        <v>695</v>
       </c>
       <c r="F72" t="s">
-        <v>282</v>
+        <v>199</v>
       </c>
       <c r="G72" t="s">
-        <v>283</v>
+        <v>198</v>
       </c>
       <c r="H72">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="I72" s="13">
         <v>1</v>
       </c>
       <c r="J72" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>vt_sv</v>
-      </c>
-      <c r="AE72" t="s">
-        <v>284</v>
+        <f>_xlfn.TEXTJOIN(";",1,K72:AAC72)</f>
+        <v>tss_Pos</v>
+      </c>
+      <c r="AD72" t="s">
+        <v>701</v>
       </c>
     </row>
     <row r="73" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="B73" t="s">
-        <v>416</v>
+        <v>265</v>
       </c>
       <c r="C73" t="s">
-        <v>280</v>
+        <v>699</v>
       </c>
       <c r="D73" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="E73" t="s">
-        <v>286</v>
+        <v>696</v>
       </c>
       <c r="F73" t="s">
-        <v>286</v>
+        <v>201</v>
       </c>
       <c r="G73" t="s">
-        <v>287</v>
+        <v>200</v>
       </c>
       <c r="H73">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="I73" s="13">
         <v>1</v>
       </c>
       <c r="J73" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>vt_pe</v>
-      </c>
-      <c r="AE73" t="s">
-        <v>285</v>
+        <f>_xlfn.TEXTJOIN(";",1,K73:AAC73)</f>
+        <v>tss_Neg</v>
+      </c>
+      <c r="AD73" t="s">
+        <v>702</v>
       </c>
     </row>
     <row r="74" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="B74" t="s">
-        <v>416</v>
+        <v>265</v>
       </c>
       <c r="C74" t="s">
-        <v>307</v>
+        <v>700</v>
       </c>
       <c r="D74" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E74" t="s">
-        <v>291</v>
+        <v>697</v>
       </c>
       <c r="F74" t="s">
-        <v>356</v>
+        <v>704</v>
       </c>
       <c r="G74" t="s">
-        <v>357</v>
+        <v>705</v>
       </c>
       <c r="H74">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="I74" s="13">
         <v>1</v>
       </c>
       <c r="J74" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>st_da</v>
-      </c>
-      <c r="AF74" t="s">
-        <v>290</v>
+        <f t="shared" ref="J74" si="3">_xlfn.TEXTJOIN(";",1,K74:AAC74)</f>
+        <v>tss_Unknown</v>
+      </c>
+      <c r="AD74" t="s">
+        <v>703</v>
       </c>
     </row>
     <row r="75" spans="1:32" x14ac:dyDescent="0.2">
@@ -14163,32 +14196,32 @@
         <v>416</v>
       </c>
       <c r="C75" t="s">
-        <v>308</v>
+        <v>279</v>
       </c>
       <c r="D75" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="E75" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="F75" t="s">
-        <v>356</v>
+        <v>282</v>
       </c>
       <c r="G75" t="s">
-        <v>357</v>
+        <v>283</v>
       </c>
       <c r="H75">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="I75" s="13">
         <v>1</v>
       </c>
       <c r="J75" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>st_da</v>
-      </c>
-      <c r="AF75" t="s">
-        <v>290</v>
+        <v>vt_sv</v>
+      </c>
+      <c r="AE75" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="76" spans="1:32" x14ac:dyDescent="0.2">
@@ -14199,32 +14232,32 @@
         <v>416</v>
       </c>
       <c r="C76" t="s">
-        <v>309</v>
+        <v>280</v>
       </c>
       <c r="D76" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="E76" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="F76" t="s">
-        <v>356</v>
+        <v>286</v>
       </c>
       <c r="G76" t="s">
-        <v>357</v>
+        <v>287</v>
       </c>
       <c r="H76">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="I76" s="13">
         <v>1</v>
       </c>
       <c r="J76" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>st_da</v>
-      </c>
-      <c r="AF76" t="s">
-        <v>290</v>
+        <v>vt_pe</v>
+      </c>
+      <c r="AE76" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="77" spans="1:32" x14ac:dyDescent="0.2">
@@ -14235,13 +14268,13 @@
         <v>416</v>
       </c>
       <c r="C77" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D77" t="s">
         <v>289</v>
       </c>
       <c r="E77" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="F77" t="s">
         <v>356</v>
@@ -14250,7 +14283,7 @@
         <v>357</v>
       </c>
       <c r="H77">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="I77" s="13">
         <v>1</v>
@@ -14271,13 +14304,13 @@
         <v>416</v>
       </c>
       <c r="C78" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D78" t="s">
         <v>289</v>
       </c>
       <c r="E78" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F78" t="s">
         <v>356</v>
@@ -14286,7 +14319,7 @@
         <v>357</v>
       </c>
       <c r="H78">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="I78" s="13">
         <v>1</v>
@@ -14307,13 +14340,13 @@
         <v>416</v>
       </c>
       <c r="C79" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D79" t="s">
         <v>289</v>
       </c>
       <c r="E79" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F79" t="s">
         <v>356</v>
@@ -14322,7 +14355,7 @@
         <v>357</v>
       </c>
       <c r="H79">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I79" s="13">
         <v>1</v>
@@ -14343,13 +14376,13 @@
         <v>416</v>
       </c>
       <c r="C80" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D80" t="s">
         <v>289</v>
       </c>
       <c r="E80" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="F80" t="s">
         <v>356</v>
@@ -14358,7 +14391,7 @@
         <v>357</v>
       </c>
       <c r="H80">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="I80" s="13">
         <v>1</v>
@@ -14379,13 +14412,13 @@
         <v>416</v>
       </c>
       <c r="C81" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D81" t="s">
         <v>289</v>
       </c>
       <c r="E81" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F81" t="s">
         <v>356</v>
@@ -14394,7 +14427,7 @@
         <v>357</v>
       </c>
       <c r="H81">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="I81" s="13">
         <v>1</v>
@@ -14415,13 +14448,13 @@
         <v>416</v>
       </c>
       <c r="C82" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D82" t="s">
         <v>289</v>
       </c>
       <c r="E82" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F82" t="s">
         <v>356</v>
@@ -14430,7 +14463,7 @@
         <v>357</v>
       </c>
       <c r="H82">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="I82" s="13">
         <v>1</v>
@@ -14451,13 +14484,13 @@
         <v>416</v>
       </c>
       <c r="C83" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D83" t="s">
         <v>289</v>
       </c>
       <c r="E83" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F83" t="s">
         <v>356</v>
@@ -14466,7 +14499,7 @@
         <v>357</v>
       </c>
       <c r="H83">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="I83" s="13">
         <v>1</v>
@@ -14487,13 +14520,13 @@
         <v>416</v>
       </c>
       <c r="C84" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D84" t="s">
         <v>289</v>
       </c>
       <c r="E84" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F84" t="s">
         <v>356</v>
@@ -14502,7 +14535,7 @@
         <v>357</v>
       </c>
       <c r="H84">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="I84" s="13">
         <v>1</v>
@@ -14523,13 +14556,13 @@
         <v>416</v>
       </c>
       <c r="C85" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D85" t="s">
         <v>289</v>
       </c>
       <c r="E85" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="F85" t="s">
         <v>356</v>
@@ -14538,7 +14571,7 @@
         <v>357</v>
       </c>
       <c r="H85">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="I85" s="13">
         <v>1</v>
@@ -14559,13 +14592,13 @@
         <v>416</v>
       </c>
       <c r="C86" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D86" t="s">
         <v>289</v>
       </c>
       <c r="E86" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="F86" t="s">
         <v>356</v>
@@ -14574,7 +14607,7 @@
         <v>357</v>
       </c>
       <c r="H86">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="I86" s="13">
         <v>1</v>
@@ -14595,13 +14628,13 @@
         <v>416</v>
       </c>
       <c r="C87" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D87" t="s">
         <v>289</v>
       </c>
       <c r="E87" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="F87" t="s">
         <v>356</v>
@@ -14610,7 +14643,7 @@
         <v>357</v>
       </c>
       <c r="H87">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="I87" s="13">
         <v>1</v>
@@ -14631,13 +14664,13 @@
         <v>416</v>
       </c>
       <c r="C88" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D88" t="s">
         <v>289</v>
       </c>
       <c r="E88" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="F88" t="s">
         <v>356</v>
@@ -14646,7 +14679,7 @@
         <v>357</v>
       </c>
       <c r="H88">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="I88" s="13">
         <v>1</v>
@@ -14667,13 +14700,13 @@
         <v>416</v>
       </c>
       <c r="C89" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D89" t="s">
         <v>289</v>
       </c>
       <c r="E89" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="F89" t="s">
         <v>356</v>
@@ -14682,7 +14715,7 @@
         <v>357</v>
       </c>
       <c r="H89">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="I89" s="13">
         <v>1</v>
@@ -14703,32 +14736,32 @@
         <v>416</v>
       </c>
       <c r="C90" t="s">
-        <v>339</v>
+        <v>320</v>
       </c>
       <c r="D90" t="s">
         <v>289</v>
       </c>
       <c r="E90" t="s">
-        <v>323</v>
+        <v>304</v>
       </c>
       <c r="F90" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G90" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="H90">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="I90" s="13">
         <v>1</v>
       </c>
       <c r="J90" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>st_ua</v>
+        <v>st_da</v>
       </c>
       <c r="AF90" t="s">
-        <v>355</v>
+        <v>290</v>
       </c>
     </row>
     <row r="91" spans="1:32" x14ac:dyDescent="0.2">
@@ -14739,32 +14772,32 @@
         <v>416</v>
       </c>
       <c r="C91" t="s">
-        <v>340</v>
+        <v>321</v>
       </c>
       <c r="D91" t="s">
         <v>289</v>
       </c>
       <c r="E91" t="s">
-        <v>324</v>
+        <v>305</v>
       </c>
       <c r="F91" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G91" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="H91">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="I91" s="13">
         <v>1</v>
       </c>
       <c r="J91" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>st_ua</v>
+        <v>st_da</v>
       </c>
       <c r="AF91" t="s">
-        <v>355</v>
+        <v>290</v>
       </c>
     </row>
     <row r="92" spans="1:32" x14ac:dyDescent="0.2">
@@ -14775,32 +14808,32 @@
         <v>416</v>
       </c>
       <c r="C92" t="s">
-        <v>341</v>
+        <v>322</v>
       </c>
       <c r="D92" t="s">
         <v>289</v>
       </c>
       <c r="E92" t="s">
-        <v>325</v>
+        <v>306</v>
       </c>
       <c r="F92" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G92" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="H92">
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="I92" s="13">
         <v>1</v>
       </c>
       <c r="J92" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>st_ua</v>
+        <v>st_da</v>
       </c>
       <c r="AF92" t="s">
-        <v>355</v>
+        <v>290</v>
       </c>
     </row>
     <row r="93" spans="1:32" x14ac:dyDescent="0.2">
@@ -14811,13 +14844,13 @@
         <v>416</v>
       </c>
       <c r="C93" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D93" t="s">
         <v>289</v>
       </c>
       <c r="E93" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="F93" t="s">
         <v>358</v>
@@ -14826,7 +14859,7 @@
         <v>359</v>
       </c>
       <c r="H93">
-        <v>200</v>
+        <v>170</v>
       </c>
       <c r="I93" s="13">
         <v>1</v>
@@ -14847,13 +14880,13 @@
         <v>416</v>
       </c>
       <c r="C94" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D94" t="s">
         <v>289</v>
       </c>
       <c r="E94" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="F94" t="s">
         <v>358</v>
@@ -14862,7 +14895,7 @@
         <v>359</v>
       </c>
       <c r="H94">
-        <v>210</v>
+        <v>180</v>
       </c>
       <c r="I94" s="13">
         <v>1</v>
@@ -14883,13 +14916,13 @@
         <v>416</v>
       </c>
       <c r="C95" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D95" t="s">
         <v>289</v>
       </c>
       <c r="E95" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F95" t="s">
         <v>358</v>
@@ -14898,7 +14931,7 @@
         <v>359</v>
       </c>
       <c r="H95">
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="I95" s="13">
         <v>1</v>
@@ -14919,13 +14952,13 @@
         <v>416</v>
       </c>
       <c r="C96" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D96" t="s">
         <v>289</v>
       </c>
       <c r="E96" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="F96" t="s">
         <v>358</v>
@@ -14934,7 +14967,7 @@
         <v>359</v>
       </c>
       <c r="H96">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="I96" s="13">
         <v>1</v>
@@ -14955,13 +14988,13 @@
         <v>416</v>
       </c>
       <c r="C97" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D97" t="s">
         <v>289</v>
       </c>
       <c r="E97" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="F97" t="s">
         <v>358</v>
@@ -14970,7 +15003,7 @@
         <v>359</v>
       </c>
       <c r="H97">
-        <v>240</v>
+        <v>210</v>
       </c>
       <c r="I97" s="13">
         <v>1</v>
@@ -14991,13 +15024,13 @@
         <v>416</v>
       </c>
       <c r="C98" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D98" t="s">
         <v>289</v>
       </c>
       <c r="E98" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="F98" t="s">
         <v>358</v>
@@ -15006,13 +15039,13 @@
         <v>359</v>
       </c>
       <c r="H98">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="I98" s="13">
         <v>1</v>
       </c>
       <c r="J98" s="4" t="str">
-        <f t="shared" ref="J98:J129" si="3">_xlfn.TEXTJOIN(";",1,K98:AAC98)</f>
+        <f t="shared" si="2"/>
         <v>st_ua</v>
       </c>
       <c r="AF98" t="s">
@@ -15027,13 +15060,13 @@
         <v>416</v>
       </c>
       <c r="C99" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D99" t="s">
         <v>289</v>
       </c>
       <c r="E99" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="F99" t="s">
         <v>358</v>
@@ -15042,13 +15075,13 @@
         <v>359</v>
       </c>
       <c r="H99">
-        <v>260</v>
+        <v>230</v>
       </c>
       <c r="I99" s="13">
         <v>1</v>
       </c>
       <c r="J99" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>st_ua</v>
       </c>
       <c r="AF99" t="s">
@@ -15063,13 +15096,13 @@
         <v>416</v>
       </c>
       <c r="C100" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D100" t="s">
         <v>289</v>
       </c>
       <c r="E100" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="F100" t="s">
         <v>358</v>
@@ -15078,13 +15111,13 @@
         <v>359</v>
       </c>
       <c r="H100">
-        <v>270</v>
+        <v>240</v>
       </c>
       <c r="I100" s="13">
         <v>1</v>
       </c>
       <c r="J100" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>st_ua</v>
       </c>
       <c r="AF100" t="s">
@@ -15099,13 +15132,13 @@
         <v>416</v>
       </c>
       <c r="C101" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D101" t="s">
         <v>289</v>
       </c>
       <c r="E101" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="F101" t="s">
         <v>358</v>
@@ -15114,13 +15147,13 @@
         <v>359</v>
       </c>
       <c r="H101">
-        <v>280</v>
+        <v>250</v>
       </c>
       <c r="I101" s="13">
         <v>1</v>
       </c>
       <c r="J101" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="J101:J132" si="4">_xlfn.TEXTJOIN(";",1,K101:AAC101)</f>
         <v>st_ua</v>
       </c>
       <c r="AF101" t="s">
@@ -15135,13 +15168,13 @@
         <v>416</v>
       </c>
       <c r="C102" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D102" t="s">
         <v>289</v>
       </c>
       <c r="E102" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="F102" t="s">
         <v>358</v>
@@ -15150,13 +15183,13 @@
         <v>359</v>
       </c>
       <c r="H102">
-        <v>290</v>
+        <v>260</v>
       </c>
       <c r="I102" s="13">
         <v>1</v>
       </c>
       <c r="J102" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>st_ua</v>
       </c>
       <c r="AF102" t="s">
@@ -15171,13 +15204,13 @@
         <v>416</v>
       </c>
       <c r="C103" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D103" t="s">
         <v>289</v>
       </c>
       <c r="E103" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="F103" t="s">
         <v>358</v>
@@ -15186,13 +15219,13 @@
         <v>359</v>
       </c>
       <c r="H103">
-        <v>300</v>
+        <v>270</v>
       </c>
       <c r="I103" s="13">
         <v>1</v>
       </c>
       <c r="J103" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>st_ua</v>
       </c>
       <c r="AF103" t="s">
@@ -15207,13 +15240,13 @@
         <v>416</v>
       </c>
       <c r="C104" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D104" t="s">
         <v>289</v>
       </c>
       <c r="E104" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="F104" t="s">
         <v>358</v>
@@ -15222,13 +15255,13 @@
         <v>359</v>
       </c>
       <c r="H104">
-        <v>310</v>
+        <v>280</v>
       </c>
       <c r="I104" s="13">
         <v>1</v>
       </c>
       <c r="J104" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>st_ua</v>
       </c>
       <c r="AF104" t="s">
@@ -15243,13 +15276,13 @@
         <v>416</v>
       </c>
       <c r="C105" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D105" t="s">
         <v>289</v>
       </c>
       <c r="E105" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="F105" t="s">
         <v>358</v>
@@ -15258,13 +15291,13 @@
         <v>359</v>
       </c>
       <c r="H105">
-        <v>320</v>
+        <v>290</v>
       </c>
       <c r="I105" s="13">
         <v>1</v>
       </c>
       <c r="J105" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>st_ua</v>
       </c>
       <c r="AF105" t="s">
@@ -15279,32 +15312,32 @@
         <v>416</v>
       </c>
       <c r="C106" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="D106" t="s">
-        <v>218</v>
+        <v>289</v>
       </c>
       <c r="E106" t="s">
-        <v>371</v>
+        <v>336</v>
       </c>
       <c r="F106" t="s">
-        <v>186</v>
+        <v>358</v>
       </c>
       <c r="G106" t="s">
-        <v>185</v>
+        <v>359</v>
       </c>
       <c r="H106">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="I106" s="13">
         <v>1</v>
       </c>
       <c r="J106" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v>kp2</v>
-      </c>
-      <c r="Z106" t="s">
-        <v>370</v>
+        <f t="shared" si="4"/>
+        <v>st_ua</v>
+      </c>
+      <c r="AF106" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="107" spans="1:32" x14ac:dyDescent="0.2">
@@ -15315,32 +15348,32 @@
         <v>416</v>
       </c>
       <c r="C107" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="D107" t="s">
-        <v>218</v>
+        <v>289</v>
       </c>
       <c r="E107" t="s">
-        <v>372</v>
+        <v>337</v>
       </c>
       <c r="F107" t="s">
-        <v>204</v>
+        <v>358</v>
       </c>
       <c r="G107" t="s">
-        <v>202</v>
+        <v>359</v>
       </c>
       <c r="H107">
-        <v>410</v>
+        <v>310</v>
       </c>
       <c r="I107" s="13">
         <v>1</v>
       </c>
       <c r="J107" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v>kp2</v>
-      </c>
-      <c r="Z107" t="s">
-        <v>370</v>
+        <f t="shared" si="4"/>
+        <v>st_ua</v>
+      </c>
+      <c r="AF107" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="108" spans="1:32" x14ac:dyDescent="0.2">
@@ -15351,32 +15384,32 @@
         <v>416</v>
       </c>
       <c r="C108" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="D108" t="s">
-        <v>218</v>
+        <v>289</v>
       </c>
       <c r="E108" t="s">
-        <v>373</v>
+        <v>338</v>
       </c>
       <c r="F108" t="s">
-        <v>207</v>
+        <v>358</v>
       </c>
       <c r="G108" t="s">
-        <v>206</v>
+        <v>359</v>
       </c>
       <c r="H108">
-        <v>420</v>
+        <v>320</v>
       </c>
       <c r="I108" s="13">
         <v>1</v>
       </c>
       <c r="J108" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v>kp2</v>
-      </c>
-      <c r="Z108" t="s">
-        <v>370</v>
+        <f t="shared" si="4"/>
+        <v>st_ua</v>
+      </c>
+      <c r="AF108" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="109" spans="1:32" x14ac:dyDescent="0.2">
@@ -15387,28 +15420,28 @@
         <v>416</v>
       </c>
       <c r="C109" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D109" t="s">
         <v>218</v>
       </c>
       <c r="E109" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="F109" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
       <c r="G109" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
       <c r="H109">
-        <v>430</v>
+        <v>400</v>
       </c>
       <c r="I109" s="13">
         <v>1</v>
       </c>
       <c r="J109" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>kp2</v>
       </c>
       <c r="Z109" t="s">
@@ -15423,28 +15456,28 @@
         <v>416</v>
       </c>
       <c r="C110" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D110" t="s">
         <v>218</v>
       </c>
       <c r="E110" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="F110" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G110" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H110">
-        <v>440</v>
+        <v>410</v>
       </c>
       <c r="I110" s="13">
         <v>1</v>
       </c>
       <c r="J110" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>kp2</v>
       </c>
       <c r="Z110" t="s">
@@ -15459,28 +15492,28 @@
         <v>416</v>
       </c>
       <c r="C111" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D111" t="s">
         <v>218</v>
       </c>
       <c r="E111" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="F111" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="G111" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
       <c r="H111">
-        <v>450</v>
+        <v>420</v>
       </c>
       <c r="I111" s="13">
         <v>1</v>
       </c>
       <c r="J111" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>kp2</v>
       </c>
       <c r="Z111" t="s">
@@ -15495,35 +15528,35 @@
         <v>416</v>
       </c>
       <c r="C112" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D112" t="s">
         <v>218</v>
       </c>
       <c r="E112" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="F112" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G112" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H112">
-        <v>460</v>
+        <v>430</v>
       </c>
       <c r="I112" s="13">
         <v>1</v>
       </c>
       <c r="J112" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>kp2</v>
       </c>
       <c r="Z112" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="113" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>278</v>
       </c>
@@ -15531,107 +15564,107 @@
         <v>416</v>
       </c>
       <c r="C113" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D113" t="s">
         <v>218</v>
       </c>
       <c r="E113" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F113" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="G113" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="H113">
-        <v>470</v>
+        <v>440</v>
       </c>
       <c r="I113" s="13">
         <v>1</v>
       </c>
       <c r="J113" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>kp2</v>
       </c>
       <c r="Z113" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="114" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>381</v>
+        <v>278</v>
       </c>
       <c r="B114" t="s">
-        <v>380</v>
+        <v>416</v>
       </c>
       <c r="C114" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="D114" t="s">
-        <v>379</v>
+        <v>218</v>
       </c>
       <c r="E114" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="F114" t="s">
-        <v>384</v>
+        <v>214</v>
       </c>
       <c r="G114" t="s">
-        <v>385</v>
+        <v>191</v>
       </c>
       <c r="H114">
-        <v>510</v>
+        <v>450</v>
       </c>
       <c r="I114" s="13">
         <v>1</v>
       </c>
       <c r="J114" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v>as_already</v>
-      </c>
-      <c r="AG114" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="115" spans="1:36" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>kp2</v>
+      </c>
+      <c r="Z114" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="115" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>381</v>
+        <v>278</v>
       </c>
       <c r="B115" t="s">
-        <v>380</v>
+        <v>416</v>
       </c>
       <c r="C115" t="s">
-        <v>388</v>
+        <v>368</v>
       </c>
       <c r="D115" t="s">
-        <v>379</v>
+        <v>218</v>
       </c>
       <c r="E115" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="F115" t="s">
-        <v>387</v>
+        <v>210</v>
       </c>
       <c r="G115" t="s">
-        <v>386</v>
+        <v>211</v>
       </c>
       <c r="H115">
-        <v>520</v>
+        <v>460</v>
       </c>
       <c r="I115" s="13">
         <v>1</v>
       </c>
       <c r="J115" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v>as_new</v>
-      </c>
-      <c r="AG115" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="116" spans="1:36" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>kp2</v>
+      </c>
+      <c r="Z115" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="116" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>278</v>
       </c>
@@ -15639,107 +15672,107 @@
         <v>416</v>
       </c>
       <c r="C116" t="s">
-        <v>395</v>
+        <v>369</v>
       </c>
       <c r="D116" t="s">
         <v>218</v>
       </c>
       <c r="E116" t="s">
-        <v>193</v>
+        <v>378</v>
       </c>
       <c r="F116" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
       <c r="G116" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
       <c r="H116">
-        <v>610</v>
+        <v>470</v>
       </c>
       <c r="I116" s="13">
         <v>1</v>
       </c>
       <c r="J116" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v>kp3</v>
+        <f t="shared" si="4"/>
+        <v>kp2</v>
       </c>
       <c r="Z116" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="117" spans="1:36" x14ac:dyDescent="0.2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="117" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>278</v>
+        <v>381</v>
       </c>
       <c r="B117" t="s">
-        <v>416</v>
+        <v>380</v>
       </c>
       <c r="C117" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
       <c r="D117" t="s">
-        <v>218</v>
+        <v>379</v>
       </c>
       <c r="E117" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F117" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="G117" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
       <c r="H117">
-        <v>620</v>
+        <v>510</v>
       </c>
       <c r="I117" s="13">
         <v>1</v>
       </c>
       <c r="J117" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v>kp3</v>
-      </c>
-      <c r="Z117" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="118" spans="1:36" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>as_already</v>
+      </c>
+      <c r="AG117" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="118" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>278</v>
+        <v>381</v>
       </c>
       <c r="B118" t="s">
-        <v>416</v>
+        <v>380</v>
       </c>
       <c r="C118" t="s">
-        <v>399</v>
+        <v>388</v>
       </c>
       <c r="D118" t="s">
-        <v>218</v>
+        <v>379</v>
       </c>
       <c r="E118" t="s">
-        <v>188</v>
+        <v>389</v>
       </c>
       <c r="F118" t="s">
-        <v>188</v>
+        <v>387</v>
       </c>
       <c r="G118" t="s">
-        <v>187</v>
+        <v>386</v>
       </c>
       <c r="H118">
-        <v>630</v>
+        <v>520</v>
       </c>
       <c r="I118" s="13">
         <v>1</v>
       </c>
       <c r="J118" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v>kp3</v>
-      </c>
-      <c r="Z118" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="119" spans="1:36" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>as_new</v>
+      </c>
+      <c r="AG118" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="119" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>278</v>
       </c>
@@ -15747,35 +15780,35 @@
         <v>416</v>
       </c>
       <c r="C119" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="D119" t="s">
         <v>218</v>
       </c>
       <c r="E119" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="F119" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="G119" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="H119">
-        <v>640</v>
+        <v>610</v>
       </c>
       <c r="I119" s="13">
         <v>1</v>
       </c>
       <c r="J119" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>kp3</v>
       </c>
       <c r="Z119" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="120" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>278</v>
       </c>
@@ -15783,35 +15816,35 @@
         <v>416</v>
       </c>
       <c r="C120" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="D120" t="s">
-        <v>402</v>
+        <v>218</v>
       </c>
       <c r="E120" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="F120" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
       <c r="G120" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="H120">
-        <v>710</v>
+        <v>620</v>
       </c>
       <c r="I120" s="13">
         <v>1</v>
       </c>
       <c r="J120" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v>ti_routine</v>
-      </c>
-      <c r="AH120" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="121" spans="1:36" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>kp3</v>
+      </c>
+      <c r="Z120" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="121" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>278</v>
       </c>
@@ -15819,35 +15852,35 @@
         <v>416</v>
       </c>
       <c r="C121" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="D121" t="s">
-        <v>402</v>
+        <v>218</v>
       </c>
       <c r="E121" t="s">
-        <v>405</v>
+        <v>188</v>
       </c>
       <c r="F121" t="s">
-        <v>412</v>
+        <v>188</v>
       </c>
       <c r="G121" t="s">
-        <v>413</v>
+        <v>187</v>
       </c>
       <c r="H121">
-        <v>720</v>
+        <v>630</v>
       </c>
       <c r="I121" s="13">
         <v>1</v>
       </c>
       <c r="J121" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v>ti_routine</v>
-      </c>
-      <c r="AH121" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="122" spans="1:36" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>kp3</v>
+      </c>
+      <c r="Z121" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="122" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>278</v>
       </c>
@@ -15855,35 +15888,35 @@
         <v>416</v>
       </c>
       <c r="C122" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="D122" t="s">
-        <v>402</v>
+        <v>218</v>
       </c>
       <c r="E122" t="s">
-        <v>407</v>
+        <v>186</v>
       </c>
       <c r="F122" t="s">
-        <v>412</v>
+        <v>186</v>
       </c>
       <c r="G122" t="s">
-        <v>413</v>
+        <v>185</v>
       </c>
       <c r="H122">
-        <v>730</v>
+        <v>640</v>
       </c>
       <c r="I122" s="13">
         <v>1</v>
       </c>
       <c r="J122" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v>ti_routine</v>
-      </c>
-      <c r="AH122" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="123" spans="1:36" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>kp3</v>
+      </c>
+      <c r="Z122" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="123" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>278</v>
       </c>
@@ -15891,13 +15924,13 @@
         <v>416</v>
       </c>
       <c r="C123" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="D123" t="s">
         <v>402</v>
       </c>
       <c r="E123" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="F123" t="s">
         <v>412</v>
@@ -15906,197 +15939,197 @@
         <v>413</v>
       </c>
       <c r="H123">
-        <v>740</v>
+        <v>710</v>
       </c>
       <c r="I123" s="13">
         <v>1</v>
       </c>
       <c r="J123" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>ti_routine</v>
       </c>
       <c r="AH123" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="124" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>196</v>
+        <v>278</v>
       </c>
       <c r="B124" t="s">
-        <v>197</v>
+        <v>416</v>
       </c>
       <c r="C124" t="s">
-        <v>198</v>
+        <v>406</v>
       </c>
       <c r="D124" t="s">
-        <v>255</v>
+        <v>402</v>
       </c>
       <c r="E124" t="s">
-        <v>199</v>
+        <v>405</v>
       </c>
       <c r="F124" t="s">
-        <v>276</v>
+        <v>412</v>
       </c>
       <c r="G124" t="s">
-        <v>277</v>
+        <v>413</v>
       </c>
       <c r="H124">
-        <v>10</v>
+        <v>720</v>
       </c>
       <c r="I124" s="13">
         <v>1</v>
       </c>
-      <c r="J124" t="str">
-        <f t="shared" si="3"/>
-        <v>tr_pos2</v>
-      </c>
-      <c r="AA124" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="125" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="J124" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
+      <c r="AH124" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="125" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>196</v>
+        <v>278</v>
       </c>
       <c r="B125" t="s">
-        <v>197</v>
+        <v>416</v>
       </c>
       <c r="C125" t="s">
-        <v>200</v>
+        <v>408</v>
       </c>
       <c r="D125" t="s">
-        <v>255</v>
+        <v>402</v>
       </c>
       <c r="E125" t="s">
-        <v>201</v>
+        <v>407</v>
       </c>
       <c r="F125" t="s">
-        <v>274</v>
+        <v>412</v>
       </c>
       <c r="G125" t="s">
-        <v>275</v>
+        <v>413</v>
       </c>
       <c r="H125">
-        <v>20</v>
+        <v>730</v>
       </c>
       <c r="I125" s="13">
         <v>1</v>
       </c>
-      <c r="J125" t="str">
-        <f t="shared" si="3"/>
-        <v>tr_neg2</v>
-      </c>
-      <c r="AA125" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="126" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="J125" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
+      <c r="AH125" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="126" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>509</v>
+        <v>278</v>
       </c>
       <c r="B126" t="s">
-        <v>510</v>
+        <v>416</v>
       </c>
       <c r="C126" t="s">
-        <v>481</v>
+        <v>410</v>
       </c>
       <c r="D126" t="s">
-        <v>436</v>
+        <v>402</v>
       </c>
       <c r="E126" t="s">
-        <v>482</v>
+        <v>409</v>
       </c>
       <c r="F126" t="s">
-        <v>143</v>
+        <v>412</v>
       </c>
       <c r="G126" t="s">
-        <v>143</v>
+        <v>413</v>
       </c>
       <c r="H126">
-        <v>100</v>
+        <v>740</v>
       </c>
       <c r="I126" s="13">
         <v>1</v>
       </c>
-      <c r="J126" t="str">
-        <f t="shared" si="3"/>
-        <v>hts_mod_com_ndx</v>
-      </c>
-      <c r="AJ126" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="127" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="J126" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
+      <c r="AH126" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="127" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>509</v>
+        <v>196</v>
       </c>
       <c r="B127" t="s">
-        <v>510</v>
+        <v>197</v>
       </c>
       <c r="C127" t="s">
-        <v>483</v>
+        <v>198</v>
       </c>
       <c r="D127" t="s">
-        <v>436</v>
+        <v>255</v>
       </c>
       <c r="E127" t="s">
-        <v>484</v>
+        <v>199</v>
       </c>
       <c r="F127" t="s">
-        <v>143</v>
+        <v>276</v>
       </c>
       <c r="G127" t="s">
-        <v>143</v>
+        <v>277</v>
       </c>
       <c r="H127">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="I127" s="13">
         <v>1</v>
       </c>
       <c r="J127" t="str">
-        <f t="shared" si="3"/>
-        <v>hts_mod_fac_ndx</v>
-      </c>
-      <c r="AJ127" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="128" spans="1:36" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>tr_pos2</v>
+      </c>
+      <c r="AA127" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="128" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>509</v>
+        <v>196</v>
       </c>
       <c r="B128" t="s">
-        <v>510</v>
+        <v>197</v>
       </c>
       <c r="C128" t="s">
-        <v>485</v>
+        <v>200</v>
       </c>
       <c r="D128" t="s">
-        <v>436</v>
+        <v>255</v>
       </c>
       <c r="E128" t="s">
-        <v>486</v>
+        <v>201</v>
       </c>
       <c r="F128" t="s">
-        <v>143</v>
+        <v>274</v>
       </c>
       <c r="G128" t="s">
-        <v>143</v>
+        <v>275</v>
       </c>
       <c r="H128">
-        <v>300</v>
+        <v>20</v>
       </c>
       <c r="I128" s="13">
         <v>1</v>
       </c>
       <c r="J128" t="str">
-        <f t="shared" si="3"/>
-        <v>hts_mod_com_mob</v>
-      </c>
-      <c r="AJ128" t="s">
-        <v>438</v>
+        <f t="shared" si="4"/>
+        <v>tr_neg2</v>
+      </c>
+      <c r="AA128" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="129" spans="1:36" x14ac:dyDescent="0.2">
@@ -16107,13 +16140,13 @@
         <v>510</v>
       </c>
       <c r="C129" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="D129" t="s">
         <v>436</v>
       </c>
       <c r="E129" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="F129" t="s">
         <v>143</v>
@@ -16122,17 +16155,17 @@
         <v>143</v>
       </c>
       <c r="H129">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="I129" s="13">
         <v>1</v>
       </c>
       <c r="J129" t="str">
-        <f t="shared" si="3"/>
-        <v>hts_mod_com_vct</v>
+        <f t="shared" si="4"/>
+        <v>hts_mod_com_ndx</v>
       </c>
       <c r="AJ129" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="130" spans="1:36" x14ac:dyDescent="0.2">
@@ -16143,13 +16176,13 @@
         <v>510</v>
       </c>
       <c r="C130" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="D130" t="s">
         <v>436</v>
       </c>
       <c r="E130" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="F130" t="s">
         <v>143</v>
@@ -16158,17 +16191,17 @@
         <v>143</v>
       </c>
       <c r="H130">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="I130" s="13">
         <v>1</v>
       </c>
       <c r="J130" t="str">
-        <f t="shared" ref="J130:J143" si="4">_xlfn.TEXTJOIN(";",1,K130:AAC130)</f>
-        <v>hts_mod_com_otr</v>
+        <f t="shared" si="4"/>
+        <v>hts_mod_fac_ndx</v>
       </c>
       <c r="AJ130" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="131" spans="1:36" x14ac:dyDescent="0.2">
@@ -16179,13 +16212,13 @@
         <v>510</v>
       </c>
       <c r="C131" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="D131" t="s">
         <v>436</v>
       </c>
       <c r="E131" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="F131" t="s">
         <v>143</v>
@@ -16194,17 +16227,17 @@
         <v>143</v>
       </c>
       <c r="H131">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="I131" s="13">
         <v>1</v>
       </c>
       <c r="J131" t="str">
         <f t="shared" si="4"/>
-        <v>hts_mod_fac_ew</v>
+        <v>hts_mod_com_mob</v>
       </c>
       <c r="AJ131" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
     </row>
     <row r="132" spans="1:36" x14ac:dyDescent="0.2">
@@ -16215,13 +16248,13 @@
         <v>510</v>
       </c>
       <c r="C132" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="D132" t="s">
         <v>436</v>
       </c>
       <c r="E132" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="F132" t="s">
         <v>143</v>
@@ -16230,17 +16263,17 @@
         <v>143</v>
       </c>
       <c r="H132">
-        <v>700</v>
+        <v>400</v>
       </c>
       <c r="I132" s="13">
         <v>1</v>
       </c>
       <c r="J132" t="str">
         <f t="shared" si="4"/>
-        <v>hts_mod_fac_inpat</v>
+        <v>hts_mod_com_vct</v>
       </c>
       <c r="AJ132" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="133" spans="1:36" x14ac:dyDescent="0.2">
@@ -16251,13 +16284,13 @@
         <v>510</v>
       </c>
       <c r="C133" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="D133" t="s">
         <v>436</v>
       </c>
       <c r="E133" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="F133" t="s">
         <v>143</v>
@@ -16266,17 +16299,17 @@
         <v>143</v>
       </c>
       <c r="H133">
-        <v>800</v>
+        <v>500</v>
       </c>
       <c r="I133" s="13">
         <v>1</v>
       </c>
       <c r="J133" t="str">
-        <f t="shared" si="4"/>
-        <v>hts_mod_fac_nut</v>
+        <f t="shared" ref="J133:J146" si="5">_xlfn.TEXTJOIN(";",1,K133:AAC133)</f>
+        <v>hts_mod_com_otr</v>
       </c>
       <c r="AJ133" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="134" spans="1:36" x14ac:dyDescent="0.2">
@@ -16287,13 +16320,13 @@
         <v>510</v>
       </c>
       <c r="C134" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="D134" t="s">
         <v>436</v>
       </c>
       <c r="E134" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="F134" t="s">
         <v>143</v>
@@ -16302,17 +16335,17 @@
         <v>143</v>
       </c>
       <c r="H134">
-        <v>900</v>
+        <v>600</v>
       </c>
       <c r="I134" s="13">
         <v>1</v>
       </c>
       <c r="J134" t="str">
-        <f t="shared" si="4"/>
-        <v>hts_mod_fac_ped</v>
+        <f t="shared" si="5"/>
+        <v>hts_mod_fac_ew</v>
       </c>
       <c r="AJ134" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="135" spans="1:36" x14ac:dyDescent="0.2">
@@ -16323,13 +16356,13 @@
         <v>510</v>
       </c>
       <c r="C135" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="D135" t="s">
         <v>436</v>
       </c>
       <c r="E135" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="F135" t="s">
         <v>143</v>
@@ -16338,17 +16371,17 @@
         <v>143</v>
       </c>
       <c r="H135">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="I135" s="13">
         <v>1</v>
       </c>
       <c r="J135" t="str">
-        <f t="shared" si="4"/>
-        <v>hts_mod_fac_sti</v>
+        <f t="shared" si="5"/>
+        <v>hts_mod_fac_inpat</v>
       </c>
       <c r="AJ135" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="136" spans="1:36" x14ac:dyDescent="0.2">
@@ -16359,13 +16392,13 @@
         <v>510</v>
       </c>
       <c r="C136" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="D136" t="s">
         <v>436</v>
       </c>
       <c r="E136" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="F136" t="s">
         <v>143</v>
@@ -16374,17 +16407,17 @@
         <v>143</v>
       </c>
       <c r="H136">
-        <v>1100</v>
+        <v>800</v>
       </c>
       <c r="I136" s="13">
         <v>1</v>
       </c>
       <c r="J136" t="str">
-        <f t="shared" si="4"/>
-        <v>hts_mod_fac_vct</v>
+        <f t="shared" si="5"/>
+        <v>hts_mod_fac_nut</v>
       </c>
       <c r="AJ136" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="137" spans="1:36" x14ac:dyDescent="0.2">
@@ -16395,13 +16428,13 @@
         <v>510</v>
       </c>
       <c r="C137" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="D137" t="s">
         <v>436</v>
       </c>
       <c r="E137" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="F137" t="s">
         <v>143</v>
@@ -16410,17 +16443,17 @@
         <v>143</v>
       </c>
       <c r="H137">
-        <v>1200</v>
+        <v>900</v>
       </c>
       <c r="I137" s="13">
         <v>1</v>
       </c>
       <c r="J137" t="str">
-        <f t="shared" si="4"/>
-        <v>hts_mod_fac_otr_pitc</v>
+        <f t="shared" si="5"/>
+        <v>hts_mod_fac_ped</v>
       </c>
       <c r="AJ137" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="138" spans="1:36" x14ac:dyDescent="0.2">
@@ -16431,13 +16464,13 @@
         <v>510</v>
       </c>
       <c r="C138" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="D138" t="s">
         <v>436</v>
       </c>
       <c r="E138" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="F138" t="s">
         <v>143</v>
@@ -16446,17 +16479,17 @@
         <v>143</v>
       </c>
       <c r="H138">
-        <v>1300</v>
+        <v>1000</v>
       </c>
       <c r="I138" s="13">
         <v>1</v>
       </c>
       <c r="J138" t="str">
-        <f t="shared" si="4"/>
-        <v>hts_mod_fac_vmmc</v>
+        <f t="shared" si="5"/>
+        <v>hts_mod_fac_sti</v>
       </c>
       <c r="AJ138" t="s">
-        <v>511</v>
+        <v>447</v>
       </c>
     </row>
     <row r="139" spans="1:36" x14ac:dyDescent="0.2">
@@ -16467,13 +16500,13 @@
         <v>510</v>
       </c>
       <c r="C139" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="D139" t="s">
         <v>436</v>
       </c>
       <c r="E139" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="F139" t="s">
         <v>143</v>
@@ -16482,17 +16515,17 @@
         <v>143</v>
       </c>
       <c r="H139">
-        <v>1400</v>
+        <v>1100</v>
       </c>
       <c r="I139" s="13">
         <v>1</v>
       </c>
       <c r="J139" t="str">
-        <f t="shared" si="4"/>
-        <v>hts_mod_fac_anc_1</v>
+        <f t="shared" si="5"/>
+        <v>hts_mod_fac_vct</v>
       </c>
       <c r="AJ139" t="s">
-        <v>512</v>
+        <v>448</v>
       </c>
     </row>
     <row r="140" spans="1:36" x14ac:dyDescent="0.2">
@@ -16503,13 +16536,13 @@
         <v>510</v>
       </c>
       <c r="C140" t="s">
-        <v>514</v>
+        <v>503</v>
       </c>
       <c r="D140" t="s">
         <v>436</v>
       </c>
       <c r="E140" t="s">
-        <v>513</v>
+        <v>504</v>
       </c>
       <c r="F140" t="s">
         <v>143</v>
@@ -16518,17 +16551,17 @@
         <v>143</v>
       </c>
       <c r="H140">
-        <v>1500</v>
+        <v>1200</v>
       </c>
       <c r="I140" s="13">
         <v>1</v>
       </c>
       <c r="J140" t="str">
-        <f t="shared" si="4"/>
-        <v>hts_mod_fac_tb</v>
+        <f t="shared" si="5"/>
+        <v>hts_mod_fac_otr_pitc</v>
       </c>
       <c r="AJ140" t="s">
-        <v>515</v>
+        <v>449</v>
       </c>
     </row>
     <row r="141" spans="1:36" x14ac:dyDescent="0.2">
@@ -16539,13 +16572,13 @@
         <v>510</v>
       </c>
       <c r="C141" t="s">
-        <v>571</v>
+        <v>505</v>
       </c>
       <c r="D141" t="s">
         <v>436</v>
       </c>
-      <c r="E141" s="17" t="s">
-        <v>569</v>
+      <c r="E141" t="s">
+        <v>506</v>
       </c>
       <c r="F141" t="s">
         <v>143</v>
@@ -16554,139 +16587,128 @@
         <v>143</v>
       </c>
       <c r="H141">
-        <v>1600</v>
+        <v>1300</v>
       </c>
       <c r="I141" s="13">
         <v>1</v>
       </c>
       <c r="J141" t="str">
-        <f t="shared" si="4"/>
-        <v>hts_mod_fac_post_anc_1</v>
+        <f t="shared" si="5"/>
+        <v>hts_mod_fac_vmmc</v>
       </c>
       <c r="AJ141" t="s">
-        <v>570</v>
+        <v>511</v>
       </c>
     </row>
     <row r="142" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>174</v>
+        <v>509</v>
       </c>
       <c r="B142" t="s">
-        <v>233</v>
+        <v>510</v>
       </c>
       <c r="C142" t="s">
-        <v>519</v>
+        <v>507</v>
       </c>
       <c r="D142" t="s">
-        <v>217</v>
+        <v>436</v>
       </c>
       <c r="E142" t="s">
-        <v>520</v>
+        <v>508</v>
       </c>
       <c r="F142" t="s">
-        <v>520</v>
+        <v>143</v>
       </c>
       <c r="G142" t="s">
-        <v>521</v>
+        <v>143</v>
       </c>
       <c r="H142">
-        <v>3</v>
-      </c>
-      <c r="I142" s="12">
+        <v>1400</v>
+      </c>
+      <c r="I142" s="13">
         <v>1</v>
       </c>
-      <c r="J142" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>U_age</v>
-      </c>
-      <c r="K142" s="9"/>
-      <c r="L142" s="9"/>
-      <c r="M142" s="9"/>
-      <c r="N142" s="9"/>
-      <c r="P142" s="9"/>
-      <c r="Q142" s="9"/>
-      <c r="R142" s="9"/>
-      <c r="T142" s="9"/>
-      <c r="U142" s="9"/>
-      <c r="V142" s="9"/>
+      <c r="J142" t="str">
+        <f t="shared" si="5"/>
+        <v>hts_mod_fac_anc_1</v>
+      </c>
       <c r="AJ142" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
     </row>
     <row r="143" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>175</v>
+        <v>509</v>
       </c>
       <c r="B143" t="s">
-        <v>176</v>
+        <v>510</v>
       </c>
       <c r="C143" t="s">
-        <v>133</v>
+        <v>514</v>
       </c>
       <c r="D143" t="s">
-        <v>216</v>
+        <v>436</v>
       </c>
       <c r="E143" t="s">
-        <v>134</v>
+        <v>513</v>
       </c>
       <c r="F143" t="s">
-        <v>523</v>
+        <v>143</v>
       </c>
       <c r="G143" t="s">
-        <v>524</v>
+        <v>143</v>
       </c>
       <c r="H143">
-        <v>3</v>
-      </c>
-      <c r="I143" s="12">
+        <v>1500</v>
+      </c>
+      <c r="I143" s="13">
         <v>1</v>
       </c>
-      <c r="J143" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>U_sex</v>
+      <c r="J143" t="str">
+        <f t="shared" si="5"/>
+        <v>hts_mod_fac_tb</v>
       </c>
       <c r="AJ143" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
     </row>
     <row r="144" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>174</v>
+        <v>509</v>
       </c>
       <c r="B144" t="s">
-        <v>233</v>
+        <v>510</v>
       </c>
       <c r="C144" t="s">
-        <v>519</v>
+        <v>571</v>
       </c>
       <c r="D144" t="s">
-        <v>217</v>
-      </c>
-      <c r="E144" t="s">
-        <v>520</v>
+        <v>436</v>
+      </c>
+      <c r="E144" s="17" t="s">
+        <v>569</v>
       </c>
       <c r="F144" t="s">
-        <v>99</v>
+        <v>143</v>
       </c>
       <c r="G144" t="s">
-        <v>114</v>
-      </c>
-      <c r="H144" s="7">
-        <v>10</v>
+        <v>143</v>
+      </c>
+      <c r="H144">
+        <v>1600</v>
       </c>
       <c r="I144" s="13">
-        <v>8.3299999999999999E-2</v>
-      </c>
-      <c r="J144" s="4" t="str">
-        <f t="shared" ref="J144:J157" si="5">_xlfn.TEXTJOIN(";",1,K144:AAC144)</f>
-        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
-      </c>
-      <c r="U144" s="9" t="s">
-        <v>657</v>
-      </c>
-      <c r="V144" s="19"/>
-    </row>
-    <row r="145" spans="1:35" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="J144" t="str">
+        <f t="shared" si="5"/>
+        <v>hts_mod_fac_post_anc_1</v>
+      </c>
+      <c r="AJ144" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="145" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>174</v>
       </c>
@@ -16703,64 +16725,72 @@
         <v>520</v>
       </c>
       <c r="F145" t="s">
-        <v>97</v>
+        <v>520</v>
       </c>
       <c r="G145" t="s">
-        <v>117</v>
-      </c>
-      <c r="H145" s="6">
-        <v>15</v>
-      </c>
-      <c r="I145" s="13">
-        <v>8.3299999999999999E-2</v>
+        <v>521</v>
+      </c>
+      <c r="H145">
+        <v>3</v>
+      </c>
+      <c r="I145" s="12">
+        <v>1</v>
       </c>
       <c r="J145" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
-      </c>
-      <c r="U145" s="9" t="s">
-        <v>657</v>
-      </c>
+        <v>U_age</v>
+      </c>
+      <c r="K145" s="9"/>
+      <c r="L145" s="9"/>
+      <c r="M145" s="9"/>
+      <c r="N145" s="9"/>
+      <c r="P145" s="9"/>
+      <c r="Q145" s="9"/>
+      <c r="R145" s="9"/>
+      <c r="T145" s="9"/>
+      <c r="U145" s="9"/>
       <c r="V145" s="9"/>
-    </row>
-    <row r="146" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AJ145" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="146" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B146" t="s">
-        <v>233</v>
+        <v>176</v>
       </c>
       <c r="C146" t="s">
-        <v>519</v>
+        <v>133</v>
       </c>
       <c r="D146" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E146" t="s">
-        <v>520</v>
+        <v>134</v>
       </c>
       <c r="F146" t="s">
-        <v>98</v>
+        <v>523</v>
       </c>
       <c r="G146" t="s">
-        <v>127</v>
-      </c>
-      <c r="H146" s="7">
-        <v>30</v>
-      </c>
-      <c r="I146" s="13">
-        <v>8.3299999999999999E-2</v>
+        <v>524</v>
+      </c>
+      <c r="H146">
+        <v>3</v>
+      </c>
+      <c r="I146" s="12">
+        <v>1</v>
       </c>
       <c r="J146" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
-      </c>
-      <c r="U146" s="9" t="s">
-        <v>657</v>
-      </c>
-      <c r="V146" s="9"/>
-    </row>
-    <row r="147" spans="1:35" x14ac:dyDescent="0.2">
+        <v>U_sex</v>
+      </c>
+      <c r="AJ146" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="147" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>174</v>
       </c>
@@ -16777,29 +16807,27 @@
         <v>520</v>
       </c>
       <c r="F147" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="G147" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H147" s="7">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="I147" s="13">
         <v>8.3299999999999999E-2</v>
       </c>
       <c r="J147" s="4" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K147:AAC147)</f>
-        <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
+        <f t="shared" ref="J147:J160" si="6">_xlfn.TEXTJOIN(";",1,K147:AAC147)</f>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U147" s="9" t="s">
         <v>657</v>
       </c>
-      <c r="V147" s="19" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="148" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="V147" s="19"/>
+    </row>
+    <row r="148" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>174</v>
       </c>
@@ -16816,29 +16844,27 @@
         <v>520</v>
       </c>
       <c r="F148" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="G148" t="s">
-        <v>120</v>
-      </c>
-      <c r="H148" s="7">
-        <v>60</v>
+        <v>117</v>
+      </c>
+      <c r="H148" s="6">
+        <v>15</v>
       </c>
       <c r="I148" s="13">
-        <v>8.3400000000000002E-2</v>
+        <v>8.3299999999999999E-2</v>
       </c>
       <c r="J148" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
+        <f t="shared" si="6"/>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U148" s="9" t="s">
         <v>657</v>
       </c>
-      <c r="V148" s="19" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="149" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="V148" s="9"/>
+    </row>
+    <row r="149" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>174</v>
       </c>
@@ -16855,29 +16881,27 @@
         <v>520</v>
       </c>
       <c r="F149" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="G149" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="H149" s="7">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="I149" s="13">
-        <v>8.3400000000000002E-2</v>
+        <v>8.3299999999999999E-2</v>
       </c>
       <c r="J149" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
+        <f t="shared" si="6"/>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U149" s="9" t="s">
         <v>657</v>
       </c>
-      <c r="V149" s="19" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="150" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="V149" s="9"/>
+    </row>
+    <row r="150" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>174</v>
       </c>
@@ -16894,19 +16918,19 @@
         <v>520</v>
       </c>
       <c r="F150" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="G150" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H150" s="7">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="I150" s="13">
-        <v>8.3400000000000002E-2</v>
+        <v>8.3299999999999999E-2</v>
       </c>
       <c r="J150" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f>_xlfn.TEXTJOIN(";",1,K150:AAC150)</f>
         <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U150" s="9" t="s">
@@ -16916,7 +16940,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="151" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>174</v>
       </c>
@@ -16933,19 +16957,19 @@
         <v>520</v>
       </c>
       <c r="F151" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="G151" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H151" s="7">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="I151" s="13">
         <v>8.3400000000000002E-2</v>
       </c>
       <c r="J151" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U151" s="9" t="s">
@@ -16955,7 +16979,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="152" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>174</v>
       </c>
@@ -16972,19 +16996,19 @@
         <v>520</v>
       </c>
       <c r="F152" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="G152" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H152" s="7">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="I152" s="13">
-        <v>8.3299999999999999E-2</v>
+        <v>8.3400000000000002E-2</v>
       </c>
       <c r="J152" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U152" s="9" t="s">
@@ -16994,7 +17018,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="153" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>174</v>
       </c>
@@ -17011,19 +17035,19 @@
         <v>520</v>
       </c>
       <c r="F153" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G153" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H153" s="7">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="I153" s="13">
-        <v>8.3299999999999999E-2</v>
+        <v>8.3400000000000002E-2</v>
       </c>
       <c r="J153" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U153" s="9" t="s">
@@ -17033,7 +17057,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="154" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>174</v>
       </c>
@@ -17050,19 +17074,19 @@
         <v>520</v>
       </c>
       <c r="F154" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G154" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H154" s="7">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="I154" s="13">
-        <v>8.3299999999999999E-2</v>
+        <v>8.3400000000000002E-2</v>
       </c>
       <c r="J154" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U154" s="9" t="s">
@@ -17072,7 +17096,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="155" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>174</v>
       </c>
@@ -17089,19 +17113,19 @@
         <v>520</v>
       </c>
       <c r="F155" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G155" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="H155" s="7">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="I155" s="13">
         <v>8.3299999999999999E-2</v>
       </c>
       <c r="J155" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U155" s="9" t="s">
@@ -17111,80 +17135,197 @@
         <v>685</v>
       </c>
     </row>
-    <row r="156" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
+        <v>174</v>
+      </c>
+      <c r="B156" t="s">
+        <v>233</v>
+      </c>
+      <c r="C156" t="s">
+        <v>519</v>
+      </c>
+      <c r="D156" t="s">
+        <v>217</v>
+      </c>
+      <c r="E156" t="s">
+        <v>520</v>
+      </c>
+      <c r="F156" t="s">
+        <v>103</v>
+      </c>
+      <c r="G156" t="s">
+        <v>125</v>
+      </c>
+      <c r="H156" s="7">
+        <v>130</v>
+      </c>
+      <c r="I156" s="13">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="J156" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
+      </c>
+      <c r="U156" s="9" t="s">
+        <v>657</v>
+      </c>
+      <c r="V156" s="19" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="157" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>174</v>
+      </c>
+      <c r="B157" t="s">
+        <v>233</v>
+      </c>
+      <c r="C157" t="s">
+        <v>519</v>
+      </c>
+      <c r="D157" t="s">
+        <v>217</v>
+      </c>
+      <c r="E157" t="s">
+        <v>520</v>
+      </c>
+      <c r="F157" t="s">
+        <v>104</v>
+      </c>
+      <c r="G157" t="s">
+        <v>126</v>
+      </c>
+      <c r="H157" s="7">
+        <v>140</v>
+      </c>
+      <c r="I157" s="13">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="J157" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
+      </c>
+      <c r="U157" s="9" t="s">
+        <v>657</v>
+      </c>
+      <c r="V157" s="19" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="158" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>174</v>
+      </c>
+      <c r="B158" t="s">
+        <v>233</v>
+      </c>
+      <c r="C158" t="s">
+        <v>519</v>
+      </c>
+      <c r="D158" t="s">
+        <v>217</v>
+      </c>
+      <c r="E158" t="s">
+        <v>520</v>
+      </c>
+      <c r="F158" t="s">
+        <v>105</v>
+      </c>
+      <c r="G158" t="s">
+        <v>116</v>
+      </c>
+      <c r="H158" s="7">
+        <v>150</v>
+      </c>
+      <c r="I158" s="13">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="J158" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
+      </c>
+      <c r="U158" s="9" t="s">
+        <v>657</v>
+      </c>
+      <c r="V158" s="19" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="159" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
         <v>691</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B159" t="s">
         <v>692</v>
       </c>
-      <c r="C156" t="s">
+      <c r="C159" t="s">
         <v>687</v>
       </c>
-      <c r="D156" t="s">
+      <c r="D159" t="s">
         <v>436</v>
       </c>
-      <c r="E156" t="s">
+      <c r="E159" t="s">
         <v>688</v>
       </c>
-      <c r="F156" t="s">
+      <c r="F159" t="s">
         <v>688</v>
       </c>
-      <c r="G156" t="s">
+      <c r="G159" t="s">
         <v>687</v>
       </c>
-      <c r="H156" s="7">
+      <c r="H159" s="7">
         <v>1</v>
       </c>
-      <c r="I156" s="12">
+      <c r="I159" s="12">
         <v>1</v>
       </c>
-      <c r="J156" s="4" t="str">
-        <f t="shared" si="5"/>
+      <c r="J159" s="4" t="str">
+        <f t="shared" si="6"/>
         <v>ag_a</v>
       </c>
-      <c r="AI156" t="s">
+      <c r="AI159" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="157" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A157" t="s">
+    <row r="160" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
         <v>691</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B160" t="s">
         <v>692</v>
       </c>
-      <c r="C157" t="s">
+      <c r="C160" t="s">
         <v>689</v>
       </c>
-      <c r="D157" t="s">
+      <c r="D160" t="s">
         <v>436</v>
       </c>
-      <c r="E157" t="s">
+      <c r="E160" t="s">
         <v>690</v>
       </c>
-      <c r="F157" t="s">
+      <c r="F160" t="s">
         <v>690</v>
       </c>
-      <c r="G157" t="s">
+      <c r="G160" t="s">
         <v>689</v>
       </c>
-      <c r="H157" s="7">
+      <c r="H160" s="7">
         <v>2</v>
       </c>
-      <c r="I157" s="12">
+      <c r="I160" s="12">
         <v>1</v>
       </c>
-      <c r="J157" s="4" t="str">
-        <f t="shared" si="5"/>
+      <c r="J160" s="4" t="str">
+        <f t="shared" si="6"/>
         <v>ag_g</v>
       </c>
-      <c r="AI157" t="s">
+      <c r="AI160" t="s">
         <v>694</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AH155" xr:uid="{F5070472-BD41-FC47-BC46-FB0AD4499DE3}"/>
+  <autoFilter ref="A1:AH160" xr:uid="{F5070472-BD41-FC47-BC46-FB0AD4499DE3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:Y66">
     <sortCondition ref="H4:H66"/>
   </sortState>

</xml_diff>

<commit_message>
dim_item_sets add additional ti_routine category option combinations
COCs changed for FY20 T
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27967082-CE2D-7C43-8DF9-07D28B98A737}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60801EC1-DB1A-C141-89DC-AFCB9DC9E7EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-280" yWindow="760" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
     <sheet name="dimension_Item_sets" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data_required!$A$1:$AK$60</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">dimension_Item_sets!$A$1:$AH$160</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">dimension_Item_sets!$A$1:$AH$184</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4097" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4337" uniqueCount="754">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -2309,6 +2310,150 @@
   <si>
     <t>gUdtLH3fV1m</t>
   </si>
+  <si>
+    <t>&lt;1, Female, Routine, Positive</t>
+  </si>
+  <si>
+    <t>YVmIiOo8V17</t>
+  </si>
+  <si>
+    <t>&lt;1, Male, Routine, Positive</t>
+  </si>
+  <si>
+    <t>vIZW4Jv7qqy</t>
+  </si>
+  <si>
+    <t>1-4, Female, Routine, Positive</t>
+  </si>
+  <si>
+    <t>HDhg4LTHBRa</t>
+  </si>
+  <si>
+    <t>1-4, Male, Routine, Positive</t>
+  </si>
+  <si>
+    <t>bQY52yJFcaj</t>
+  </si>
+  <si>
+    <t>10-14, Female, Routine, Positive</t>
+  </si>
+  <si>
+    <t>dpFsZrc6Ffc</t>
+  </si>
+  <si>
+    <t>10-14, Male, Routine, Positive</t>
+  </si>
+  <si>
+    <t>Cz8TfD9G4NS</t>
+  </si>
+  <si>
+    <t>15-19, Female, Routine, Positive</t>
+  </si>
+  <si>
+    <t>A30fQSASmum</t>
+  </si>
+  <si>
+    <t>15-19, Male, Routine, Positive</t>
+  </si>
+  <si>
+    <t>hX01YQ8Xd0A</t>
+  </si>
+  <si>
+    <t>20-24, Female, Routine, Positive</t>
+  </si>
+  <si>
+    <t>d7veFTMK1Jw</t>
+  </si>
+  <si>
+    <t>20-24, Male, Routine, Positive</t>
+  </si>
+  <si>
+    <t>Slv7vEZKRXb</t>
+  </si>
+  <si>
+    <t>25-29, Female, Routine, Positive</t>
+  </si>
+  <si>
+    <t>I0zEWK2C11q</t>
+  </si>
+  <si>
+    <t>25-29, Male, Routine, Positive</t>
+  </si>
+  <si>
+    <t>X3iUwZMRbpC</t>
+  </si>
+  <si>
+    <t>30-34, Female, Routine, Positive</t>
+  </si>
+  <si>
+    <t>RKp8rxNgQAX</t>
+  </si>
+  <si>
+    <t>30-34, Male, Routine, Positive</t>
+  </si>
+  <si>
+    <t>ABHnQuSJzZJ</t>
+  </si>
+  <si>
+    <t>35-39, Female, Routine, Positive</t>
+  </si>
+  <si>
+    <t>MRnYv4nt5gc</t>
+  </si>
+  <si>
+    <t>35-39, Male, Routine, Positive</t>
+  </si>
+  <si>
+    <t>PRsdy4olkFE</t>
+  </si>
+  <si>
+    <t>40-44, Female, Routine, Positive</t>
+  </si>
+  <si>
+    <t>wOxLLZhNrPi</t>
+  </si>
+  <si>
+    <t>40-44, Male, Routine, Positive</t>
+  </si>
+  <si>
+    <t>TcbPwuDGR7C</t>
+  </si>
+  <si>
+    <t>45-49, Female, Routine, Positive</t>
+  </si>
+  <si>
+    <t>ONQ9uSvOkGB</t>
+  </si>
+  <si>
+    <t>45-49, Male, Routine, Positive</t>
+  </si>
+  <si>
+    <t>Ba3F9Cdo4TM</t>
+  </si>
+  <si>
+    <t>5-9, Female, Routine, Positive</t>
+  </si>
+  <si>
+    <t>rAvlLbG5dAb</t>
+  </si>
+  <si>
+    <t>5-9, Male, Routine, Positive</t>
+  </si>
+  <si>
+    <t>sjBprG9Atqw</t>
+  </si>
+  <si>
+    <t>50+, Female, Routine, Positive</t>
+  </si>
+  <si>
+    <t>U9R0CAPL0AS</t>
+  </si>
+  <si>
+    <t>50+, Male, Routine, Positive</t>
+  </si>
+  <si>
+    <t>hrDvHLgNfrf</t>
+  </si>
 </sst>
 </file>
 
@@ -2317,7 +2462,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2380,6 +2525,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2401,7 +2552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -2426,6 +2577,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10910,17 +11063,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BEDA6B-3F7E-D547-BD9D-9083103169CB}">
-  <dimension ref="A1:AJ160"/>
+  <dimension ref="A1:AJ184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E61" sqref="E61"/>
+      <selection pane="topRight" activeCell="A150" sqref="A127:A150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="2" max="2" width="48.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.83203125" customWidth="1"/>
     <col min="5" max="5" width="39.1640625" customWidth="1"/>
@@ -15153,7 +15306,7 @@
         <v>1</v>
       </c>
       <c r="J101" s="4" t="str">
-        <f t="shared" ref="J101:J132" si="4">_xlfn.TEXTJOIN(";",1,K101:AAC101)</f>
+        <f t="shared" ref="J101:J156" si="4">_xlfn.TEXTJOIN(";",1,K101:AAC101)</f>
         <v>st_ua</v>
       </c>
       <c r="AF101" t="s">
@@ -16062,1274 +16215,2278 @@
     </row>
     <row r="127" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>196</v>
+        <v>278</v>
       </c>
       <c r="B127" t="s">
-        <v>197</v>
-      </c>
-      <c r="C127" t="s">
-        <v>198</v>
+        <v>416</v>
+      </c>
+      <c r="C127" s="20" t="s">
+        <v>707</v>
       </c>
       <c r="D127" t="s">
-        <v>255</v>
-      </c>
-      <c r="E127" t="s">
-        <v>199</v>
+        <v>402</v>
+      </c>
+      <c r="E127" s="20" t="s">
+        <v>706</v>
       </c>
       <c r="F127" t="s">
-        <v>276</v>
+        <v>412</v>
       </c>
       <c r="G127" t="s">
-        <v>277</v>
+        <v>413</v>
       </c>
       <c r="H127">
-        <v>10</v>
+        <v>750</v>
       </c>
       <c r="I127" s="13">
         <v>1</v>
       </c>
-      <c r="J127" t="str">
+      <c r="J127" s="4"/>
+      <c r="AH127" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="128" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>278</v>
+      </c>
+      <c r="B128" t="s">
+        <v>416</v>
+      </c>
+      <c r="C128" s="20" t="s">
+        <v>709</v>
+      </c>
+      <c r="D128" t="s">
+        <v>402</v>
+      </c>
+      <c r="E128" s="20" t="s">
+        <v>708</v>
+      </c>
+      <c r="F128" t="s">
+        <v>412</v>
+      </c>
+      <c r="G128" t="s">
+        <v>413</v>
+      </c>
+      <c r="H128">
+        <v>760</v>
+      </c>
+      <c r="I128" s="13">
+        <v>1</v>
+      </c>
+      <c r="J128" s="4"/>
+      <c r="AH128" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="129" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>278</v>
+      </c>
+      <c r="B129" t="s">
+        <v>416</v>
+      </c>
+      <c r="C129" s="20" t="s">
+        <v>711</v>
+      </c>
+      <c r="D129" t="s">
+        <v>402</v>
+      </c>
+      <c r="E129" s="20" t="s">
+        <v>710</v>
+      </c>
+      <c r="F129" t="s">
+        <v>412</v>
+      </c>
+      <c r="G129" t="s">
+        <v>413</v>
+      </c>
+      <c r="H129">
+        <v>770</v>
+      </c>
+      <c r="I129" s="13">
+        <v>1</v>
+      </c>
+      <c r="J129" s="4"/>
+      <c r="AH129" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="130" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>278</v>
+      </c>
+      <c r="B130" t="s">
+        <v>416</v>
+      </c>
+      <c r="C130" s="20" t="s">
+        <v>713</v>
+      </c>
+      <c r="D130" t="s">
+        <v>402</v>
+      </c>
+      <c r="E130" s="20" t="s">
+        <v>712</v>
+      </c>
+      <c r="F130" t="s">
+        <v>412</v>
+      </c>
+      <c r="G130" t="s">
+        <v>413</v>
+      </c>
+      <c r="H130">
+        <v>780</v>
+      </c>
+      <c r="I130" s="13">
+        <v>1</v>
+      </c>
+      <c r="J130" s="4"/>
+      <c r="AH130" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="131" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>278</v>
+      </c>
+      <c r="B131" t="s">
+        <v>416</v>
+      </c>
+      <c r="C131" s="20" t="s">
+        <v>715</v>
+      </c>
+      <c r="D131" t="s">
+        <v>402</v>
+      </c>
+      <c r="E131" s="20" t="s">
+        <v>714</v>
+      </c>
+      <c r="F131" t="s">
+        <v>412</v>
+      </c>
+      <c r="G131" t="s">
+        <v>413</v>
+      </c>
+      <c r="H131">
+        <v>790</v>
+      </c>
+      <c r="I131" s="13">
+        <v>1</v>
+      </c>
+      <c r="J131" s="4"/>
+      <c r="AH131" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="132" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>278</v>
+      </c>
+      <c r="B132" t="s">
+        <v>416</v>
+      </c>
+      <c r="C132" s="20" t="s">
+        <v>717</v>
+      </c>
+      <c r="D132" t="s">
+        <v>402</v>
+      </c>
+      <c r="E132" s="20" t="s">
+        <v>716</v>
+      </c>
+      <c r="F132" t="s">
+        <v>412</v>
+      </c>
+      <c r="G132" t="s">
+        <v>413</v>
+      </c>
+      <c r="H132">
+        <v>800</v>
+      </c>
+      <c r="I132" s="13">
+        <v>1</v>
+      </c>
+      <c r="J132" s="4"/>
+      <c r="AH132" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="133" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>278</v>
+      </c>
+      <c r="B133" t="s">
+        <v>416</v>
+      </c>
+      <c r="C133" s="20" t="s">
+        <v>719</v>
+      </c>
+      <c r="D133" t="s">
+        <v>402</v>
+      </c>
+      <c r="E133" s="20" t="s">
+        <v>718</v>
+      </c>
+      <c r="F133" t="s">
+        <v>412</v>
+      </c>
+      <c r="G133" t="s">
+        <v>413</v>
+      </c>
+      <c r="H133">
+        <v>810</v>
+      </c>
+      <c r="I133" s="13">
+        <v>1</v>
+      </c>
+      <c r="J133" s="4"/>
+      <c r="AH133" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="134" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>278</v>
+      </c>
+      <c r="B134" t="s">
+        <v>416</v>
+      </c>
+      <c r="C134" s="20" t="s">
+        <v>721</v>
+      </c>
+      <c r="D134" t="s">
+        <v>402</v>
+      </c>
+      <c r="E134" s="20" t="s">
+        <v>720</v>
+      </c>
+      <c r="F134" t="s">
+        <v>412</v>
+      </c>
+      <c r="G134" t="s">
+        <v>413</v>
+      </c>
+      <c r="H134">
+        <v>820</v>
+      </c>
+      <c r="I134" s="13">
+        <v>1</v>
+      </c>
+      <c r="J134" s="4"/>
+      <c r="AH134" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="135" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>278</v>
+      </c>
+      <c r="B135" t="s">
+        <v>416</v>
+      </c>
+      <c r="C135" s="20" t="s">
+        <v>723</v>
+      </c>
+      <c r="D135" t="s">
+        <v>402</v>
+      </c>
+      <c r="E135" s="20" t="s">
+        <v>722</v>
+      </c>
+      <c r="F135" t="s">
+        <v>412</v>
+      </c>
+      <c r="G135" t="s">
+        <v>413</v>
+      </c>
+      <c r="H135">
+        <v>830</v>
+      </c>
+      <c r="I135" s="13">
+        <v>1</v>
+      </c>
+      <c r="J135" s="4"/>
+      <c r="AH135" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="136" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>278</v>
+      </c>
+      <c r="B136" t="s">
+        <v>416</v>
+      </c>
+      <c r="C136" s="20" t="s">
+        <v>725</v>
+      </c>
+      <c r="D136" t="s">
+        <v>402</v>
+      </c>
+      <c r="E136" s="20" t="s">
+        <v>724</v>
+      </c>
+      <c r="F136" t="s">
+        <v>412</v>
+      </c>
+      <c r="G136" t="s">
+        <v>413</v>
+      </c>
+      <c r="H136">
+        <v>840</v>
+      </c>
+      <c r="I136" s="13">
+        <v>1</v>
+      </c>
+      <c r="J136" s="4"/>
+      <c r="AH136" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="137" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>278</v>
+      </c>
+      <c r="B137" t="s">
+        <v>416</v>
+      </c>
+      <c r="C137" s="20" t="s">
+        <v>727</v>
+      </c>
+      <c r="D137" t="s">
+        <v>402</v>
+      </c>
+      <c r="E137" s="20" t="s">
+        <v>726</v>
+      </c>
+      <c r="F137" t="s">
+        <v>412</v>
+      </c>
+      <c r="G137" t="s">
+        <v>413</v>
+      </c>
+      <c r="H137">
+        <v>850</v>
+      </c>
+      <c r="I137" s="13">
+        <v>1</v>
+      </c>
+      <c r="J137" s="4"/>
+      <c r="AH137" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="138" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>278</v>
+      </c>
+      <c r="B138" t="s">
+        <v>416</v>
+      </c>
+      <c r="C138" s="20" t="s">
+        <v>729</v>
+      </c>
+      <c r="D138" t="s">
+        <v>402</v>
+      </c>
+      <c r="E138" s="20" t="s">
+        <v>728</v>
+      </c>
+      <c r="F138" t="s">
+        <v>412</v>
+      </c>
+      <c r="G138" t="s">
+        <v>413</v>
+      </c>
+      <c r="H138">
+        <v>860</v>
+      </c>
+      <c r="I138" s="13">
+        <v>1</v>
+      </c>
+      <c r="J138" s="4"/>
+      <c r="AH138" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="139" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>278</v>
+      </c>
+      <c r="B139" t="s">
+        <v>416</v>
+      </c>
+      <c r="C139" s="20" t="s">
+        <v>731</v>
+      </c>
+      <c r="D139" t="s">
+        <v>402</v>
+      </c>
+      <c r="E139" s="20" t="s">
+        <v>730</v>
+      </c>
+      <c r="F139" t="s">
+        <v>412</v>
+      </c>
+      <c r="G139" t="s">
+        <v>413</v>
+      </c>
+      <c r="H139">
+        <v>870</v>
+      </c>
+      <c r="I139" s="13">
+        <v>1</v>
+      </c>
+      <c r="J139" s="4"/>
+      <c r="AH139" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="140" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>278</v>
+      </c>
+      <c r="B140" t="s">
+        <v>416</v>
+      </c>
+      <c r="C140" s="20" t="s">
+        <v>733</v>
+      </c>
+      <c r="D140" t="s">
+        <v>402</v>
+      </c>
+      <c r="E140" s="20" t="s">
+        <v>732</v>
+      </c>
+      <c r="F140" t="s">
+        <v>412</v>
+      </c>
+      <c r="G140" t="s">
+        <v>413</v>
+      </c>
+      <c r="H140">
+        <v>880</v>
+      </c>
+      <c r="I140" s="13">
+        <v>1</v>
+      </c>
+      <c r="J140" s="4"/>
+      <c r="AH140" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="141" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>278</v>
+      </c>
+      <c r="B141" t="s">
+        <v>416</v>
+      </c>
+      <c r="C141" s="20" t="s">
+        <v>735</v>
+      </c>
+      <c r="D141" t="s">
+        <v>402</v>
+      </c>
+      <c r="E141" s="20" t="s">
+        <v>734</v>
+      </c>
+      <c r="F141" t="s">
+        <v>412</v>
+      </c>
+      <c r="G141" t="s">
+        <v>413</v>
+      </c>
+      <c r="H141">
+        <v>890</v>
+      </c>
+      <c r="I141" s="13">
+        <v>1</v>
+      </c>
+      <c r="J141" s="4"/>
+      <c r="AH141" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="142" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>278</v>
+      </c>
+      <c r="B142" t="s">
+        <v>416</v>
+      </c>
+      <c r="C142" s="20" t="s">
+        <v>737</v>
+      </c>
+      <c r="D142" t="s">
+        <v>402</v>
+      </c>
+      <c r="E142" s="20" t="s">
+        <v>736</v>
+      </c>
+      <c r="F142" t="s">
+        <v>412</v>
+      </c>
+      <c r="G142" t="s">
+        <v>413</v>
+      </c>
+      <c r="H142">
+        <v>900</v>
+      </c>
+      <c r="I142" s="13">
+        <v>1</v>
+      </c>
+      <c r="J142" s="4"/>
+      <c r="AH142" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="143" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>278</v>
+      </c>
+      <c r="B143" t="s">
+        <v>416</v>
+      </c>
+      <c r="C143" s="20" t="s">
+        <v>739</v>
+      </c>
+      <c r="D143" t="s">
+        <v>402</v>
+      </c>
+      <c r="E143" s="20" t="s">
+        <v>738</v>
+      </c>
+      <c r="F143" t="s">
+        <v>412</v>
+      </c>
+      <c r="G143" t="s">
+        <v>413</v>
+      </c>
+      <c r="H143">
+        <v>910</v>
+      </c>
+      <c r="I143" s="13">
+        <v>1</v>
+      </c>
+      <c r="J143" s="4"/>
+      <c r="AH143" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="144" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>278</v>
+      </c>
+      <c r="B144" t="s">
+        <v>416</v>
+      </c>
+      <c r="C144" s="20" t="s">
+        <v>741</v>
+      </c>
+      <c r="D144" t="s">
+        <v>402</v>
+      </c>
+      <c r="E144" s="20" t="s">
+        <v>740</v>
+      </c>
+      <c r="F144" t="s">
+        <v>412</v>
+      </c>
+      <c r="G144" t="s">
+        <v>413</v>
+      </c>
+      <c r="H144">
+        <v>920</v>
+      </c>
+      <c r="I144" s="13">
+        <v>1</v>
+      </c>
+      <c r="J144" s="4"/>
+      <c r="AH144" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="145" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>278</v>
+      </c>
+      <c r="B145" t="s">
+        <v>416</v>
+      </c>
+      <c r="C145" s="20" t="s">
+        <v>743</v>
+      </c>
+      <c r="D145" t="s">
+        <v>402</v>
+      </c>
+      <c r="E145" s="20" t="s">
+        <v>742</v>
+      </c>
+      <c r="F145" t="s">
+        <v>412</v>
+      </c>
+      <c r="G145" t="s">
+        <v>413</v>
+      </c>
+      <c r="H145">
+        <v>930</v>
+      </c>
+      <c r="I145" s="13">
+        <v>1</v>
+      </c>
+      <c r="J145" s="4"/>
+      <c r="AH145" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="146" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>278</v>
+      </c>
+      <c r="B146" t="s">
+        <v>416</v>
+      </c>
+      <c r="C146" s="20" t="s">
+        <v>745</v>
+      </c>
+      <c r="D146" t="s">
+        <v>402</v>
+      </c>
+      <c r="E146" s="20" t="s">
+        <v>744</v>
+      </c>
+      <c r="F146" t="s">
+        <v>412</v>
+      </c>
+      <c r="G146" t="s">
+        <v>413</v>
+      </c>
+      <c r="H146">
+        <v>940</v>
+      </c>
+      <c r="I146" s="13">
+        <v>1</v>
+      </c>
+      <c r="J146" s="4"/>
+      <c r="AH146" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="147" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>278</v>
+      </c>
+      <c r="B147" t="s">
+        <v>416</v>
+      </c>
+      <c r="C147" s="20" t="s">
+        <v>747</v>
+      </c>
+      <c r="D147" t="s">
+        <v>402</v>
+      </c>
+      <c r="E147" s="20" t="s">
+        <v>746</v>
+      </c>
+      <c r="F147" t="s">
+        <v>412</v>
+      </c>
+      <c r="G147" t="s">
+        <v>413</v>
+      </c>
+      <c r="H147">
+        <v>950</v>
+      </c>
+      <c r="I147" s="13">
+        <v>1</v>
+      </c>
+      <c r="J147" s="4"/>
+      <c r="AH147" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="148" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>278</v>
+      </c>
+      <c r="B148" t="s">
+        <v>416</v>
+      </c>
+      <c r="C148" s="20" t="s">
+        <v>749</v>
+      </c>
+      <c r="D148" t="s">
+        <v>402</v>
+      </c>
+      <c r="E148" s="20" t="s">
+        <v>748</v>
+      </c>
+      <c r="F148" t="s">
+        <v>412</v>
+      </c>
+      <c r="G148" t="s">
+        <v>413</v>
+      </c>
+      <c r="H148">
+        <v>960</v>
+      </c>
+      <c r="I148" s="13">
+        <v>1</v>
+      </c>
+      <c r="J148" s="4"/>
+      <c r="AH148" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="149" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>278</v>
+      </c>
+      <c r="B149" t="s">
+        <v>416</v>
+      </c>
+      <c r="C149" s="20" t="s">
+        <v>751</v>
+      </c>
+      <c r="D149" t="s">
+        <v>402</v>
+      </c>
+      <c r="E149" s="20" t="s">
+        <v>750</v>
+      </c>
+      <c r="F149" t="s">
+        <v>412</v>
+      </c>
+      <c r="G149" t="s">
+        <v>413</v>
+      </c>
+      <c r="H149">
+        <v>970</v>
+      </c>
+      <c r="I149" s="13">
+        <v>1</v>
+      </c>
+      <c r="J149" s="4"/>
+      <c r="AH149" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="150" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>278</v>
+      </c>
+      <c r="B150" t="s">
+        <v>416</v>
+      </c>
+      <c r="C150" s="20" t="s">
+        <v>753</v>
+      </c>
+      <c r="D150" t="s">
+        <v>402</v>
+      </c>
+      <c r="E150" s="20" t="s">
+        <v>752</v>
+      </c>
+      <c r="F150" t="s">
+        <v>412</v>
+      </c>
+      <c r="G150" t="s">
+        <v>413</v>
+      </c>
+      <c r="H150">
+        <v>980</v>
+      </c>
+      <c r="I150" s="13">
+        <v>1</v>
+      </c>
+      <c r="J150" s="4"/>
+      <c r="AH150" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="151" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>196</v>
+      </c>
+      <c r="B151" t="s">
+        <v>197</v>
+      </c>
+      <c r="C151" t="s">
+        <v>198</v>
+      </c>
+      <c r="D151" t="s">
+        <v>255</v>
+      </c>
+      <c r="E151" t="s">
+        <v>199</v>
+      </c>
+      <c r="F151" t="s">
+        <v>276</v>
+      </c>
+      <c r="G151" t="s">
+        <v>277</v>
+      </c>
+      <c r="H151">
+        <v>10</v>
+      </c>
+      <c r="I151" s="13">
+        <v>1</v>
+      </c>
+      <c r="J151" t="str">
         <f t="shared" si="4"/>
         <v>tr_pos2</v>
       </c>
-      <c r="AA127" t="s">
+      <c r="AA151" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="128" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
+    <row r="152" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
         <v>196</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B152" t="s">
         <v>197</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C152" t="s">
         <v>200</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D152" t="s">
         <v>255</v>
       </c>
-      <c r="E128" t="s">
+      <c r="E152" t="s">
         <v>201</v>
       </c>
-      <c r="F128" t="s">
+      <c r="F152" t="s">
         <v>274</v>
       </c>
-      <c r="G128" t="s">
+      <c r="G152" t="s">
         <v>275</v>
       </c>
-      <c r="H128">
+      <c r="H152">
         <v>20</v>
       </c>
-      <c r="I128" s="13">
+      <c r="I152" s="13">
         <v>1</v>
       </c>
-      <c r="J128" t="str">
+      <c r="J152" t="str">
         <f t="shared" si="4"/>
         <v>tr_neg2</v>
       </c>
-      <c r="AA128" t="s">
+      <c r="AA152" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="129" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
+    <row r="153" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
         <v>509</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B153" t="s">
         <v>510</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C153" t="s">
         <v>481</v>
       </c>
-      <c r="D129" t="s">
+      <c r="D153" t="s">
         <v>436</v>
       </c>
-      <c r="E129" t="s">
+      <c r="E153" t="s">
         <v>482</v>
       </c>
-      <c r="F129" t="s">
-        <v>143</v>
-      </c>
-      <c r="G129" t="s">
-        <v>143</v>
-      </c>
-      <c r="H129">
+      <c r="F153" t="s">
+        <v>143</v>
+      </c>
+      <c r="G153" t="s">
+        <v>143</v>
+      </c>
+      <c r="H153">
         <v>100</v>
       </c>
-      <c r="I129" s="13">
+      <c r="I153" s="13">
         <v>1</v>
       </c>
-      <c r="J129" t="str">
+      <c r="J153" t="str">
         <f t="shared" si="4"/>
         <v>hts_mod_com_ndx</v>
       </c>
-      <c r="AJ129" t="s">
+      <c r="AJ153" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="130" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
+    <row r="154" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
         <v>509</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B154" t="s">
         <v>510</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C154" t="s">
         <v>483</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D154" t="s">
         <v>436</v>
       </c>
-      <c r="E130" t="s">
+      <c r="E154" t="s">
         <v>484</v>
       </c>
-      <c r="F130" t="s">
-        <v>143</v>
-      </c>
-      <c r="G130" t="s">
-        <v>143</v>
-      </c>
-      <c r="H130">
+      <c r="F154" t="s">
+        <v>143</v>
+      </c>
+      <c r="G154" t="s">
+        <v>143</v>
+      </c>
+      <c r="H154">
         <v>200</v>
       </c>
-      <c r="I130" s="13">
+      <c r="I154" s="13">
         <v>1</v>
       </c>
-      <c r="J130" t="str">
+      <c r="J154" t="str">
         <f t="shared" si="4"/>
         <v>hts_mod_fac_ndx</v>
       </c>
-      <c r="AJ130" t="s">
+      <c r="AJ154" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="131" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
+    <row r="155" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
         <v>509</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B155" t="s">
         <v>510</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C155" t="s">
         <v>485</v>
       </c>
-      <c r="D131" t="s">
+      <c r="D155" t="s">
         <v>436</v>
       </c>
-      <c r="E131" t="s">
+      <c r="E155" t="s">
         <v>486</v>
       </c>
-      <c r="F131" t="s">
-        <v>143</v>
-      </c>
-      <c r="G131" t="s">
-        <v>143</v>
-      </c>
-      <c r="H131">
+      <c r="F155" t="s">
+        <v>143</v>
+      </c>
+      <c r="G155" t="s">
+        <v>143</v>
+      </c>
+      <c r="H155">
         <v>300</v>
       </c>
-      <c r="I131" s="13">
+      <c r="I155" s="13">
         <v>1</v>
       </c>
-      <c r="J131" t="str">
+      <c r="J155" t="str">
         <f t="shared" si="4"/>
         <v>hts_mod_com_mob</v>
       </c>
-      <c r="AJ131" t="s">
+      <c r="AJ155" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="132" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
+    <row r="156" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
         <v>509</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B156" t="s">
         <v>510</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C156" t="s">
         <v>487</v>
       </c>
-      <c r="D132" t="s">
+      <c r="D156" t="s">
         <v>436</v>
       </c>
-      <c r="E132" t="s">
+      <c r="E156" t="s">
         <v>488</v>
       </c>
-      <c r="F132" t="s">
-        <v>143</v>
-      </c>
-      <c r="G132" t="s">
-        <v>143</v>
-      </c>
-      <c r="H132">
+      <c r="F156" t="s">
+        <v>143</v>
+      </c>
+      <c r="G156" t="s">
+        <v>143</v>
+      </c>
+      <c r="H156">
         <v>400</v>
       </c>
-      <c r="I132" s="13">
+      <c r="I156" s="13">
         <v>1</v>
       </c>
-      <c r="J132" t="str">
+      <c r="J156" t="str">
         <f t="shared" si="4"/>
         <v>hts_mod_com_vct</v>
       </c>
-      <c r="AJ132" t="s">
+      <c r="AJ156" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="133" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
+    <row r="157" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
         <v>509</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B157" t="s">
         <v>510</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C157" t="s">
         <v>489</v>
       </c>
-      <c r="D133" t="s">
+      <c r="D157" t="s">
         <v>436</v>
       </c>
-      <c r="E133" t="s">
+      <c r="E157" t="s">
         <v>490</v>
       </c>
-      <c r="F133" t="s">
-        <v>143</v>
-      </c>
-      <c r="G133" t="s">
-        <v>143</v>
-      </c>
-      <c r="H133">
+      <c r="F157" t="s">
+        <v>143</v>
+      </c>
+      <c r="G157" t="s">
+        <v>143</v>
+      </c>
+      <c r="H157">
         <v>500</v>
       </c>
-      <c r="I133" s="13">
+      <c r="I157" s="13">
         <v>1</v>
       </c>
-      <c r="J133" t="str">
-        <f t="shared" ref="J133:J146" si="5">_xlfn.TEXTJOIN(";",1,K133:AAC133)</f>
+      <c r="J157" t="str">
+        <f t="shared" ref="J157:J170" si="5">_xlfn.TEXTJOIN(";",1,K157:AAC157)</f>
         <v>hts_mod_com_otr</v>
       </c>
-      <c r="AJ133" t="s">
+      <c r="AJ157" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="134" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
+    <row r="158" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
         <v>509</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B158" t="s">
         <v>510</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C158" t="s">
         <v>491</v>
       </c>
-      <c r="D134" t="s">
+      <c r="D158" t="s">
         <v>436</v>
       </c>
-      <c r="E134" t="s">
+      <c r="E158" t="s">
         <v>492</v>
       </c>
-      <c r="F134" t="s">
-        <v>143</v>
-      </c>
-      <c r="G134" t="s">
-        <v>143</v>
-      </c>
-      <c r="H134">
+      <c r="F158" t="s">
+        <v>143</v>
+      </c>
+      <c r="G158" t="s">
+        <v>143</v>
+      </c>
+      <c r="H158">
         <v>600</v>
       </c>
-      <c r="I134" s="13">
+      <c r="I158" s="13">
         <v>1</v>
       </c>
-      <c r="J134" t="str">
+      <c r="J158" t="str">
         <f t="shared" si="5"/>
         <v>hts_mod_fac_ew</v>
       </c>
-      <c r="AJ134" t="s">
+      <c r="AJ158" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="135" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
+    <row r="159" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
         <v>509</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B159" t="s">
         <v>510</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C159" t="s">
         <v>493</v>
       </c>
-      <c r="D135" t="s">
+      <c r="D159" t="s">
         <v>436</v>
       </c>
-      <c r="E135" t="s">
+      <c r="E159" t="s">
         <v>494</v>
       </c>
-      <c r="F135" t="s">
-        <v>143</v>
-      </c>
-      <c r="G135" t="s">
-        <v>143</v>
-      </c>
-      <c r="H135">
+      <c r="F159" t="s">
+        <v>143</v>
+      </c>
+      <c r="G159" t="s">
+        <v>143</v>
+      </c>
+      <c r="H159">
         <v>700</v>
       </c>
-      <c r="I135" s="13">
+      <c r="I159" s="13">
         <v>1</v>
       </c>
-      <c r="J135" t="str">
+      <c r="J159" t="str">
         <f t="shared" si="5"/>
         <v>hts_mod_fac_inpat</v>
       </c>
-      <c r="AJ135" t="s">
+      <c r="AJ159" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="136" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
+    <row r="160" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
         <v>509</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B160" t="s">
         <v>510</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C160" t="s">
         <v>495</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D160" t="s">
         <v>436</v>
       </c>
-      <c r="E136" t="s">
+      <c r="E160" t="s">
         <v>496</v>
       </c>
-      <c r="F136" t="s">
-        <v>143</v>
-      </c>
-      <c r="G136" t="s">
-        <v>143</v>
-      </c>
-      <c r="H136">
+      <c r="F160" t="s">
+        <v>143</v>
+      </c>
+      <c r="G160" t="s">
+        <v>143</v>
+      </c>
+      <c r="H160">
         <v>800</v>
       </c>
-      <c r="I136" s="13">
+      <c r="I160" s="13">
         <v>1</v>
       </c>
-      <c r="J136" t="str">
+      <c r="J160" t="str">
         <f t="shared" si="5"/>
         <v>hts_mod_fac_nut</v>
       </c>
-      <c r="AJ136" t="s">
+      <c r="AJ160" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="137" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A137" t="s">
+    <row r="161" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
         <v>509</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B161" t="s">
         <v>510</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C161" t="s">
         <v>497</v>
       </c>
-      <c r="D137" t="s">
+      <c r="D161" t="s">
         <v>436</v>
       </c>
-      <c r="E137" t="s">
+      <c r="E161" t="s">
         <v>498</v>
       </c>
-      <c r="F137" t="s">
-        <v>143</v>
-      </c>
-      <c r="G137" t="s">
-        <v>143</v>
-      </c>
-      <c r="H137">
+      <c r="F161" t="s">
+        <v>143</v>
+      </c>
+      <c r="G161" t="s">
+        <v>143</v>
+      </c>
+      <c r="H161">
         <v>900</v>
       </c>
-      <c r="I137" s="13">
+      <c r="I161" s="13">
         <v>1</v>
       </c>
-      <c r="J137" t="str">
+      <c r="J161" t="str">
         <f t="shared" si="5"/>
         <v>hts_mod_fac_ped</v>
       </c>
-      <c r="AJ137" t="s">
+      <c r="AJ161" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="138" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
+    <row r="162" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
         <v>509</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B162" t="s">
         <v>510</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C162" t="s">
         <v>499</v>
       </c>
-      <c r="D138" t="s">
+      <c r="D162" t="s">
         <v>436</v>
       </c>
-      <c r="E138" t="s">
+      <c r="E162" t="s">
         <v>500</v>
       </c>
-      <c r="F138" t="s">
-        <v>143</v>
-      </c>
-      <c r="G138" t="s">
-        <v>143</v>
-      </c>
-      <c r="H138">
+      <c r="F162" t="s">
+        <v>143</v>
+      </c>
+      <c r="G162" t="s">
+        <v>143</v>
+      </c>
+      <c r="H162">
         <v>1000</v>
       </c>
-      <c r="I138" s="13">
+      <c r="I162" s="13">
         <v>1</v>
       </c>
-      <c r="J138" t="str">
+      <c r="J162" t="str">
         <f t="shared" si="5"/>
         <v>hts_mod_fac_sti</v>
       </c>
-      <c r="AJ138" t="s">
+      <c r="AJ162" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="139" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A139" t="s">
+    <row r="163" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
         <v>509</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B163" t="s">
         <v>510</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C163" t="s">
         <v>501</v>
       </c>
-      <c r="D139" t="s">
+      <c r="D163" t="s">
         <v>436</v>
       </c>
-      <c r="E139" t="s">
+      <c r="E163" t="s">
         <v>502</v>
       </c>
-      <c r="F139" t="s">
-        <v>143</v>
-      </c>
-      <c r="G139" t="s">
-        <v>143</v>
-      </c>
-      <c r="H139">
+      <c r="F163" t="s">
+        <v>143</v>
+      </c>
+      <c r="G163" t="s">
+        <v>143</v>
+      </c>
+      <c r="H163">
         <v>1100</v>
       </c>
-      <c r="I139" s="13">
+      <c r="I163" s="13">
         <v>1</v>
       </c>
-      <c r="J139" t="str">
+      <c r="J163" t="str">
         <f t="shared" si="5"/>
         <v>hts_mod_fac_vct</v>
       </c>
-      <c r="AJ139" t="s">
+      <c r="AJ163" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="140" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A140" t="s">
+    <row r="164" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
         <v>509</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B164" t="s">
         <v>510</v>
       </c>
-      <c r="C140" t="s">
+      <c r="C164" t="s">
         <v>503</v>
       </c>
-      <c r="D140" t="s">
+      <c r="D164" t="s">
         <v>436</v>
       </c>
-      <c r="E140" t="s">
+      <c r="E164" t="s">
         <v>504</v>
       </c>
-      <c r="F140" t="s">
-        <v>143</v>
-      </c>
-      <c r="G140" t="s">
-        <v>143</v>
-      </c>
-      <c r="H140">
+      <c r="F164" t="s">
+        <v>143</v>
+      </c>
+      <c r="G164" t="s">
+        <v>143</v>
+      </c>
+      <c r="H164">
         <v>1200</v>
       </c>
-      <c r="I140" s="13">
+      <c r="I164" s="13">
         <v>1</v>
       </c>
-      <c r="J140" t="str">
+      <c r="J164" t="str">
         <f t="shared" si="5"/>
         <v>hts_mod_fac_otr_pitc</v>
       </c>
-      <c r="AJ140" t="s">
+      <c r="AJ164" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="141" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
+    <row r="165" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
         <v>509</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B165" t="s">
         <v>510</v>
       </c>
-      <c r="C141" t="s">
+      <c r="C165" t="s">
         <v>505</v>
       </c>
-      <c r="D141" t="s">
+      <c r="D165" t="s">
         <v>436</v>
       </c>
-      <c r="E141" t="s">
+      <c r="E165" t="s">
         <v>506</v>
       </c>
-      <c r="F141" t="s">
-        <v>143</v>
-      </c>
-      <c r="G141" t="s">
-        <v>143</v>
-      </c>
-      <c r="H141">
+      <c r="F165" t="s">
+        <v>143</v>
+      </c>
+      <c r="G165" t="s">
+        <v>143</v>
+      </c>
+      <c r="H165">
         <v>1300</v>
       </c>
-      <c r="I141" s="13">
+      <c r="I165" s="13">
         <v>1</v>
       </c>
-      <c r="J141" t="str">
+      <c r="J165" t="str">
         <f t="shared" si="5"/>
         <v>hts_mod_fac_vmmc</v>
       </c>
-      <c r="AJ141" t="s">
+      <c r="AJ165" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="142" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
+    <row r="166" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
         <v>509</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B166" t="s">
         <v>510</v>
       </c>
-      <c r="C142" t="s">
+      <c r="C166" t="s">
         <v>507</v>
       </c>
-      <c r="D142" t="s">
+      <c r="D166" t="s">
         <v>436</v>
       </c>
-      <c r="E142" t="s">
+      <c r="E166" t="s">
         <v>508</v>
       </c>
-      <c r="F142" t="s">
-        <v>143</v>
-      </c>
-      <c r="G142" t="s">
-        <v>143</v>
-      </c>
-      <c r="H142">
+      <c r="F166" t="s">
+        <v>143</v>
+      </c>
+      <c r="G166" t="s">
+        <v>143</v>
+      </c>
+      <c r="H166">
         <v>1400</v>
       </c>
-      <c r="I142" s="13">
+      <c r="I166" s="13">
         <v>1</v>
       </c>
-      <c r="J142" t="str">
+      <c r="J166" t="str">
         <f t="shared" si="5"/>
         <v>hts_mod_fac_anc_1</v>
       </c>
-      <c r="AJ142" t="s">
+      <c r="AJ166" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="143" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
+    <row r="167" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
         <v>509</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B167" t="s">
         <v>510</v>
       </c>
-      <c r="C143" t="s">
+      <c r="C167" t="s">
         <v>514</v>
       </c>
-      <c r="D143" t="s">
+      <c r="D167" t="s">
         <v>436</v>
       </c>
-      <c r="E143" t="s">
+      <c r="E167" t="s">
         <v>513</v>
       </c>
-      <c r="F143" t="s">
-        <v>143</v>
-      </c>
-      <c r="G143" t="s">
-        <v>143</v>
-      </c>
-      <c r="H143">
+      <c r="F167" t="s">
+        <v>143</v>
+      </c>
+      <c r="G167" t="s">
+        <v>143</v>
+      </c>
+      <c r="H167">
         <v>1500</v>
       </c>
-      <c r="I143" s="13">
+      <c r="I167" s="13">
         <v>1</v>
       </c>
-      <c r="J143" t="str">
+      <c r="J167" t="str">
         <f t="shared" si="5"/>
         <v>hts_mod_fac_tb</v>
       </c>
-      <c r="AJ143" t="s">
+      <c r="AJ167" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="144" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A144" t="s">
+    <row r="168" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
         <v>509</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B168" t="s">
         <v>510</v>
       </c>
-      <c r="C144" t="s">
+      <c r="C168" t="s">
         <v>571</v>
       </c>
-      <c r="D144" t="s">
+      <c r="D168" t="s">
         <v>436</v>
       </c>
-      <c r="E144" s="17" t="s">
+      <c r="E168" s="17" t="s">
         <v>569</v>
       </c>
-      <c r="F144" t="s">
-        <v>143</v>
-      </c>
-      <c r="G144" t="s">
-        <v>143</v>
-      </c>
-      <c r="H144">
+      <c r="F168" t="s">
+        <v>143</v>
+      </c>
+      <c r="G168" t="s">
+        <v>143</v>
+      </c>
+      <c r="H168">
         <v>1600</v>
       </c>
-      <c r="I144" s="13">
+      <c r="I168" s="13">
         <v>1</v>
       </c>
-      <c r="J144" t="str">
+      <c r="J168" t="str">
         <f t="shared" si="5"/>
         <v>hts_mod_fac_post_anc_1</v>
       </c>
-      <c r="AJ144" t="s">
+      <c r="AJ168" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="145" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A145" t="s">
+    <row r="169" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
         <v>174</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B169" t="s">
         <v>233</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C169" t="s">
         <v>519</v>
       </c>
-      <c r="D145" t="s">
+      <c r="D169" t="s">
         <v>217</v>
       </c>
-      <c r="E145" t="s">
+      <c r="E169" t="s">
         <v>520</v>
       </c>
-      <c r="F145" t="s">
+      <c r="F169" t="s">
         <v>520</v>
       </c>
-      <c r="G145" t="s">
+      <c r="G169" t="s">
         <v>521</v>
       </c>
-      <c r="H145">
+      <c r="H169">
         <v>3</v>
       </c>
-      <c r="I145" s="12">
+      <c r="I169" s="12">
         <v>1</v>
       </c>
-      <c r="J145" s="4" t="str">
+      <c r="J169" s="4" t="str">
         <f t="shared" si="5"/>
         <v>U_age</v>
       </c>
-      <c r="K145" s="9"/>
-      <c r="L145" s="9"/>
-      <c r="M145" s="9"/>
-      <c r="N145" s="9"/>
-      <c r="P145" s="9"/>
-      <c r="Q145" s="9"/>
-      <c r="R145" s="9"/>
-      <c r="T145" s="9"/>
-      <c r="U145" s="9"/>
-      <c r="V145" s="9"/>
-      <c r="AJ145" t="s">
+      <c r="K169" s="9"/>
+      <c r="L169" s="9"/>
+      <c r="M169" s="9"/>
+      <c r="N169" s="9"/>
+      <c r="P169" s="9"/>
+      <c r="Q169" s="9"/>
+      <c r="R169" s="9"/>
+      <c r="T169" s="9"/>
+      <c r="U169" s="9"/>
+      <c r="V169" s="9"/>
+      <c r="AJ169" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="146" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A146" t="s">
+    <row r="170" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
         <v>175</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B170" t="s">
         <v>176</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C170" t="s">
         <v>133</v>
       </c>
-      <c r="D146" t="s">
+      <c r="D170" t="s">
         <v>216</v>
       </c>
-      <c r="E146" t="s">
+      <c r="E170" t="s">
         <v>134</v>
       </c>
-      <c r="F146" t="s">
+      <c r="F170" t="s">
         <v>523</v>
       </c>
-      <c r="G146" t="s">
+      <c r="G170" t="s">
         <v>524</v>
       </c>
-      <c r="H146">
+      <c r="H170">
         <v>3</v>
       </c>
-      <c r="I146" s="12">
+      <c r="I170" s="12">
         <v>1</v>
       </c>
-      <c r="J146" s="4" t="str">
+      <c r="J170" s="4" t="str">
         <f t="shared" si="5"/>
         <v>U_sex</v>
       </c>
-      <c r="AJ146" t="s">
+      <c r="AJ170" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="147" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
+    <row r="171" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
         <v>174</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B171" t="s">
         <v>233</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C171" t="s">
         <v>519</v>
       </c>
-      <c r="D147" t="s">
+      <c r="D171" t="s">
         <v>217</v>
       </c>
-      <c r="E147" t="s">
+      <c r="E171" t="s">
         <v>520</v>
       </c>
-      <c r="F147" t="s">
+      <c r="F171" t="s">
         <v>99</v>
       </c>
-      <c r="G147" t="s">
+      <c r="G171" t="s">
         <v>114</v>
       </c>
-      <c r="H147" s="7">
+      <c r="H171" s="7">
         <v>10</v>
       </c>
-      <c r="I147" s="13">
+      <c r="I171" s="13">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="J147" s="4" t="str">
-        <f t="shared" ref="J147:J160" si="6">_xlfn.TEXTJOIN(";",1,K147:AAC147)</f>
+      <c r="J171" s="4" t="str">
+        <f t="shared" ref="J171:J184" si="6">_xlfn.TEXTJOIN(";",1,K171:AAC171)</f>
         <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
-      <c r="U147" s="9" t="s">
+      <c r="U171" s="9" t="s">
         <v>657</v>
       </c>
-      <c r="V147" s="19"/>
-    </row>
-    <row r="148" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A148" t="s">
+      <c r="V171" s="19"/>
+    </row>
+    <row r="172" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
         <v>174</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B172" t="s">
         <v>233</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C172" t="s">
         <v>519</v>
       </c>
-      <c r="D148" t="s">
+      <c r="D172" t="s">
         <v>217</v>
       </c>
-      <c r="E148" t="s">
+      <c r="E172" t="s">
         <v>520</v>
       </c>
-      <c r="F148" t="s">
+      <c r="F172" t="s">
         <v>97</v>
       </c>
-      <c r="G148" t="s">
+      <c r="G172" t="s">
         <v>117</v>
       </c>
-      <c r="H148" s="6">
+      <c r="H172" s="6">
         <v>15</v>
       </c>
-      <c r="I148" s="13">
+      <c r="I172" s="13">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="J148" s="4" t="str">
+      <c r="J172" s="4" t="str">
         <f t="shared" si="6"/>
         <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
-      <c r="U148" s="9" t="s">
+      <c r="U172" s="9" t="s">
         <v>657</v>
       </c>
-      <c r="V148" s="9"/>
-    </row>
-    <row r="149" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A149" t="s">
+      <c r="V172" s="9"/>
+    </row>
+    <row r="173" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
         <v>174</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B173" t="s">
         <v>233</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C173" t="s">
         <v>519</v>
       </c>
-      <c r="D149" t="s">
+      <c r="D173" t="s">
         <v>217</v>
       </c>
-      <c r="E149" t="s">
+      <c r="E173" t="s">
         <v>520</v>
       </c>
-      <c r="F149" t="s">
+      <c r="F173" t="s">
         <v>98</v>
       </c>
-      <c r="G149" t="s">
+      <c r="G173" t="s">
         <v>127</v>
       </c>
-      <c r="H149" s="7">
+      <c r="H173" s="7">
         <v>30</v>
       </c>
-      <c r="I149" s="13">
+      <c r="I173" s="13">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="J149" s="4" t="str">
+      <c r="J173" s="4" t="str">
         <f t="shared" si="6"/>
         <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
-      <c r="U149" s="9" t="s">
+      <c r="U173" s="9" t="s">
         <v>657</v>
       </c>
-      <c r="V149" s="9"/>
-    </row>
-    <row r="150" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
+      <c r="V173" s="9"/>
+    </row>
+    <row r="174" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
         <v>174</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B174" t="s">
         <v>233</v>
       </c>
-      <c r="C150" t="s">
+      <c r="C174" t="s">
         <v>519</v>
       </c>
-      <c r="D150" t="s">
+      <c r="D174" t="s">
         <v>217</v>
       </c>
-      <c r="E150" t="s">
+      <c r="E174" t="s">
         <v>520</v>
       </c>
-      <c r="F150" t="s">
+      <c r="F174" t="s">
         <v>106</v>
       </c>
-      <c r="G150" t="s">
+      <c r="G174" t="s">
         <v>118</v>
       </c>
-      <c r="H150" s="7">
+      <c r="H174" s="7">
         <v>40</v>
       </c>
-      <c r="I150" s="13">
+      <c r="I174" s="13">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="J150" s="4" t="str">
-        <f>_xlfn.TEXTJOIN(";",1,K150:AAC150)</f>
+      <c r="J174" s="4" t="str">
+        <f>_xlfn.TEXTJOIN(";",1,K174:AAC174)</f>
         <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
-      <c r="U150" s="9" t="s">
+      <c r="U174" s="9" t="s">
         <v>657</v>
       </c>
-      <c r="V150" s="19" t="s">
+      <c r="V174" s="19" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="151" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A151" t="s">
+    <row r="175" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
         <v>174</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B175" t="s">
         <v>233</v>
       </c>
-      <c r="C151" t="s">
+      <c r="C175" t="s">
         <v>519</v>
       </c>
-      <c r="D151" t="s">
+      <c r="D175" t="s">
         <v>217</v>
       </c>
-      <c r="E151" t="s">
+      <c r="E175" t="s">
         <v>520</v>
       </c>
-      <c r="F151" t="s">
+      <c r="F175" t="s">
         <v>108</v>
       </c>
-      <c r="G151" t="s">
+      <c r="G175" t="s">
         <v>120</v>
       </c>
-      <c r="H151" s="7">
+      <c r="H175" s="7">
         <v>60</v>
       </c>
-      <c r="I151" s="13">
+      <c r="I175" s="13">
         <v>8.3400000000000002E-2</v>
       </c>
-      <c r="J151" s="4" t="str">
+      <c r="J175" s="4" t="str">
         <f t="shared" si="6"/>
         <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
-      <c r="U151" s="9" t="s">
+      <c r="U175" s="9" t="s">
         <v>657</v>
       </c>
-      <c r="V151" s="19" t="s">
+      <c r="V175" s="19" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="152" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A152" t="s">
+    <row r="176" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
         <v>174</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B176" t="s">
         <v>233</v>
       </c>
-      <c r="C152" t="s">
+      <c r="C176" t="s">
         <v>519</v>
       </c>
-      <c r="D152" t="s">
+      <c r="D176" t="s">
         <v>217</v>
       </c>
-      <c r="E152" t="s">
+      <c r="E176" t="s">
         <v>520</v>
       </c>
-      <c r="F152" t="s">
+      <c r="F176" t="s">
         <v>109</v>
       </c>
-      <c r="G152" t="s">
+      <c r="G176" t="s">
         <v>121</v>
       </c>
-      <c r="H152" s="7">
+      <c r="H176" s="7">
         <v>80</v>
       </c>
-      <c r="I152" s="13">
+      <c r="I176" s="13">
         <v>8.3400000000000002E-2</v>
       </c>
-      <c r="J152" s="4" t="str">
+      <c r="J176" s="4" t="str">
         <f t="shared" si="6"/>
         <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
-      <c r="U152" s="9" t="s">
+      <c r="U176" s="9" t="s">
         <v>657</v>
       </c>
-      <c r="V152" s="19" t="s">
+      <c r="V176" s="19" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="153" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A153" t="s">
+    <row r="177" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
         <v>174</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B177" t="s">
         <v>233</v>
       </c>
-      <c r="C153" t="s">
+      <c r="C177" t="s">
         <v>519</v>
       </c>
-      <c r="D153" t="s">
+      <c r="D177" t="s">
         <v>217</v>
       </c>
-      <c r="E153" t="s">
+      <c r="E177" t="s">
         <v>520</v>
       </c>
-      <c r="F153" t="s">
+      <c r="F177" t="s">
         <v>100</v>
       </c>
-      <c r="G153" t="s">
+      <c r="G177" t="s">
         <v>122</v>
       </c>
-      <c r="H153" s="7">
+      <c r="H177" s="7">
         <v>90</v>
       </c>
-      <c r="I153" s="13">
+      <c r="I177" s="13">
         <v>8.3400000000000002E-2</v>
       </c>
-      <c r="J153" s="4" t="str">
+      <c r="J177" s="4" t="str">
         <f t="shared" si="6"/>
         <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
-      <c r="U153" s="9" t="s">
+      <c r="U177" s="9" t="s">
         <v>657</v>
       </c>
-      <c r="V153" s="19" t="s">
+      <c r="V177" s="19" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="154" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A154" t="s">
+    <row r="178" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
         <v>174</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B178" t="s">
         <v>233</v>
       </c>
-      <c r="C154" t="s">
+      <c r="C178" t="s">
         <v>519</v>
       </c>
-      <c r="D154" t="s">
+      <c r="D178" t="s">
         <v>217</v>
       </c>
-      <c r="E154" t="s">
+      <c r="E178" t="s">
         <v>520</v>
       </c>
-      <c r="F154" t="s">
+      <c r="F178" t="s">
         <v>101</v>
       </c>
-      <c r="G154" t="s">
+      <c r="G178" t="s">
         <v>123</v>
       </c>
-      <c r="H154" s="7">
+      <c r="H178" s="7">
         <v>110</v>
       </c>
-      <c r="I154" s="13">
+      <c r="I178" s="13">
         <v>8.3400000000000002E-2</v>
       </c>
-      <c r="J154" s="4" t="str">
+      <c r="J178" s="4" t="str">
         <f t="shared" si="6"/>
         <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
-      <c r="U154" s="9" t="s">
+      <c r="U178" s="9" t="s">
         <v>657</v>
       </c>
-      <c r="V154" s="19" t="s">
+      <c r="V178" s="19" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="155" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A155" t="s">
+    <row r="179" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
         <v>174</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B179" t="s">
         <v>233</v>
       </c>
-      <c r="C155" t="s">
+      <c r="C179" t="s">
         <v>519</v>
       </c>
-      <c r="D155" t="s">
+      <c r="D179" t="s">
         <v>217</v>
       </c>
-      <c r="E155" t="s">
+      <c r="E179" t="s">
         <v>520</v>
       </c>
-      <c r="F155" t="s">
+      <c r="F179" t="s">
         <v>102</v>
       </c>
-      <c r="G155" t="s">
+      <c r="G179" t="s">
         <v>124</v>
       </c>
-      <c r="H155" s="7">
+      <c r="H179" s="7">
         <v>120</v>
       </c>
-      <c r="I155" s="13">
+      <c r="I179" s="13">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="J155" s="4" t="str">
+      <c r="J179" s="4" t="str">
         <f t="shared" si="6"/>
         <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
-      <c r="U155" s="9" t="s">
+      <c r="U179" s="9" t="s">
         <v>657</v>
       </c>
-      <c r="V155" s="19" t="s">
+      <c r="V179" s="19" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="156" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A156" t="s">
+    <row r="180" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
         <v>174</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B180" t="s">
         <v>233</v>
       </c>
-      <c r="C156" t="s">
+      <c r="C180" t="s">
         <v>519</v>
       </c>
-      <c r="D156" t="s">
+      <c r="D180" t="s">
         <v>217</v>
       </c>
-      <c r="E156" t="s">
+      <c r="E180" t="s">
         <v>520</v>
       </c>
-      <c r="F156" t="s">
+      <c r="F180" t="s">
         <v>103</v>
       </c>
-      <c r="G156" t="s">
+      <c r="G180" t="s">
         <v>125</v>
       </c>
-      <c r="H156" s="7">
+      <c r="H180" s="7">
         <v>130</v>
       </c>
-      <c r="I156" s="13">
+      <c r="I180" s="13">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="J156" s="4" t="str">
+      <c r="J180" s="4" t="str">
         <f t="shared" si="6"/>
         <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
-      <c r="U156" s="9" t="s">
+      <c r="U180" s="9" t="s">
         <v>657</v>
       </c>
-      <c r="V156" s="19" t="s">
+      <c r="V180" s="19" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="157" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A157" t="s">
+    <row r="181" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
         <v>174</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B181" t="s">
         <v>233</v>
       </c>
-      <c r="C157" t="s">
+      <c r="C181" t="s">
         <v>519</v>
       </c>
-      <c r="D157" t="s">
+      <c r="D181" t="s">
         <v>217</v>
       </c>
-      <c r="E157" t="s">
+      <c r="E181" t="s">
         <v>520</v>
       </c>
-      <c r="F157" t="s">
+      <c r="F181" t="s">
         <v>104</v>
       </c>
-      <c r="G157" t="s">
+      <c r="G181" t="s">
         <v>126</v>
       </c>
-      <c r="H157" s="7">
+      <c r="H181" s="7">
         <v>140</v>
       </c>
-      <c r="I157" s="13">
+      <c r="I181" s="13">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="J157" s="4" t="str">
+      <c r="J181" s="4" t="str">
         <f t="shared" si="6"/>
         <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
-      <c r="U157" s="9" t="s">
+      <c r="U181" s="9" t="s">
         <v>657</v>
       </c>
-      <c r="V157" s="19" t="s">
+      <c r="V181" s="19" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="158" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A158" t="s">
+    <row r="182" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
         <v>174</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B182" t="s">
         <v>233</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C182" t="s">
         <v>519</v>
       </c>
-      <c r="D158" t="s">
+      <c r="D182" t="s">
         <v>217</v>
       </c>
-      <c r="E158" t="s">
+      <c r="E182" t="s">
         <v>520</v>
       </c>
-      <c r="F158" t="s">
+      <c r="F182" t="s">
         <v>105</v>
       </c>
-      <c r="G158" t="s">
+      <c r="G182" t="s">
         <v>116</v>
       </c>
-      <c r="H158" s="7">
+      <c r="H182" s="7">
         <v>150</v>
       </c>
-      <c r="I158" s="13">
+      <c r="I182" s="13">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="J158" s="4" t="str">
+      <c r="J182" s="4" t="str">
         <f t="shared" si="6"/>
         <v>&lt;1-50+.&lt;15/&gt;15.d.u;10-50+.&lt;15/&gt;15.d.u</v>
       </c>
-      <c r="U158" s="9" t="s">
+      <c r="U182" s="9" t="s">
         <v>657</v>
       </c>
-      <c r="V158" s="19" t="s">
+      <c r="V182" s="19" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="159" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A159" t="s">
+    <row r="183" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
         <v>691</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B183" t="s">
         <v>692</v>
       </c>
-      <c r="C159" t="s">
+      <c r="C183" t="s">
         <v>687</v>
       </c>
-      <c r="D159" t="s">
+      <c r="D183" t="s">
         <v>436</v>
       </c>
-      <c r="E159" t="s">
+      <c r="E183" t="s">
         <v>688</v>
       </c>
-      <c r="F159" t="s">
+      <c r="F183" t="s">
         <v>688</v>
       </c>
-      <c r="G159" t="s">
+      <c r="G183" t="s">
         <v>687</v>
       </c>
-      <c r="H159" s="7">
+      <c r="H183" s="7">
         <v>1</v>
       </c>
-      <c r="I159" s="12">
+      <c r="I183" s="12">
         <v>1</v>
       </c>
-      <c r="J159" s="4" t="str">
+      <c r="J183" s="4" t="str">
         <f t="shared" si="6"/>
         <v>ag_a</v>
       </c>
-      <c r="AI159" t="s">
+      <c r="AI183" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="160" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A160" t="s">
+    <row r="184" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
         <v>691</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B184" t="s">
         <v>692</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C184" t="s">
         <v>689</v>
       </c>
-      <c r="D160" t="s">
+      <c r="D184" t="s">
         <v>436</v>
       </c>
-      <c r="E160" t="s">
+      <c r="E184" t="s">
         <v>690</v>
       </c>
-      <c r="F160" t="s">
+      <c r="F184" t="s">
         <v>690</v>
       </c>
-      <c r="G160" t="s">
+      <c r="G184" t="s">
         <v>689</v>
       </c>
-      <c r="H160" s="7">
+      <c r="H184" s="7">
         <v>2</v>
       </c>
-      <c r="I160" s="12">
+      <c r="I184" s="12">
         <v>1</v>
       </c>
-      <c r="J160" s="4" t="str">
+      <c r="J184" s="4" t="str">
         <f t="shared" si="6"/>
         <v>ag_g</v>
       </c>
-      <c r="AI160" t="s">
+      <c r="AI184" t="s">
         <v>694</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AH160" xr:uid="{F5070472-BD41-FC47-BC46-FB0AD4499DE3}"/>
+  <autoFilter ref="A1:AH184" xr:uid="{F5070472-BD41-FC47-BC46-FB0AD4499DE3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:Y66">
     <sortCondition ref="H4:H66"/>
   </sortState>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71B4B48-0DDD-9143-B593-B487B7D33A0E}">
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.6640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>706</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>708</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
+        <v>710</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
+        <v>712</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>714</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>716</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>718</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>720</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>722</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
+        <v>724</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
+        <v>726</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
+        <v>728</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="20" t="s">
+        <v>730</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="20" t="s">
+        <v>732</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="20" t="s">
+        <v>734</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="20" t="s">
+        <v>736</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="20" t="s">
+        <v>738</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="20" t="s">
+        <v>740</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="20" t="s">
+        <v>742</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="20" t="s">
+        <v>744</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="20" t="s">
+        <v>746</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="20" t="s">
+        <v>748</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="20" t="s">
+        <v>750</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="20" t="s">
+        <v>752</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>753</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
More dim_item_set updates for routine test indicaton
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60801EC1-DB1A-C141-89DC-AFCB9DC9E7EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0AEE38A-1A73-754E-81E0-4E310FE36210}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4337" uniqueCount="754">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4337" uniqueCount="778">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -2453,6 +2453,78 @@
   </si>
   <si>
     <t>hrDvHLgNfrf</t>
+  </si>
+  <si>
+    <t>&lt;1, Female, Routine, Positive</t>
+  </si>
+  <si>
+    <t>1-4, Female, Routine, Positive</t>
+  </si>
+  <si>
+    <t>1-4, Male, Routine, Positive</t>
+  </si>
+  <si>
+    <t>15-19, Female, Routine, Positive</t>
+  </si>
+  <si>
+    <t>15-19, Male, Routine, Positive</t>
+  </si>
+  <si>
+    <t>&lt;1, Male, Routine, Positive</t>
+  </si>
+  <si>
+    <t>20-24, Female, Routine, Positive</t>
+  </si>
+  <si>
+    <t>20-24, Male, Routine, Positive</t>
+  </si>
+  <si>
+    <t>25-29, Female, Routine, Positive</t>
+  </si>
+  <si>
+    <t>25-29, Male, Routine, Positive</t>
+  </si>
+  <si>
+    <t>30-34, Female, Routine, Positive</t>
+  </si>
+  <si>
+    <t>30-34, Male, Routine, Positive</t>
+  </si>
+  <si>
+    <t>35-39, Female, Routine, Positive</t>
+  </si>
+  <si>
+    <t>35-39, Male, Routine, Positive</t>
+  </si>
+  <si>
+    <t>40-44, Female, Routine, Positive</t>
+  </si>
+  <si>
+    <t>40-44, Male, Routine, Positive</t>
+  </si>
+  <si>
+    <t>45-49, Female, Routine, Positive</t>
+  </si>
+  <si>
+    <t>45-49, Male, Routine, Positive</t>
+  </si>
+  <si>
+    <t>50+, Female, Routine, Positive</t>
+  </si>
+  <si>
+    <t>50+, Male, Routine, Positive</t>
+  </si>
+  <si>
+    <t>5-9, Female, Routine, Positive</t>
+  </si>
+  <si>
+    <t>5-9, Male, Routine, Positive</t>
+  </si>
+  <si>
+    <t>10-14, Female, Routine, Positive</t>
+  </si>
+  <si>
+    <t>10-14, Male, Routine, Positive</t>
   </si>
 </sst>
 </file>
@@ -11066,8 +11138,8 @@
   <dimension ref="A1:AJ184"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A116" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A150" sqref="A127:A150"/>
+      <pane xSplit="6" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B135" sqref="B135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16092,13 +16164,13 @@
         <v>413</v>
       </c>
       <c r="H123">
-        <v>710</v>
+        <v>770</v>
       </c>
       <c r="I123" s="13">
         <v>1</v>
       </c>
       <c r="J123" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f>_xlfn.TEXTJOIN(";",1,K123:AAC123)</f>
         <v>ti_routine</v>
       </c>
       <c r="AH123" t="s">
@@ -16128,13 +16200,13 @@
         <v>413</v>
       </c>
       <c r="H124">
-        <v>720</v>
+        <v>780</v>
       </c>
       <c r="I124" s="13">
         <v>1</v>
       </c>
       <c r="J124" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f>_xlfn.TEXTJOIN(";",1,K124:AAC124)</f>
         <v>ti_routine</v>
       </c>
       <c r="AH124" t="s">
@@ -16164,13 +16236,13 @@
         <v>413</v>
       </c>
       <c r="H125">
-        <v>730</v>
+        <v>790</v>
       </c>
       <c r="I125" s="13">
         <v>1</v>
       </c>
       <c r="J125" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f>_xlfn.TEXTJOIN(";",1,K125:AAC125)</f>
         <v>ti_routine</v>
       </c>
       <c r="AH125" t="s">
@@ -16200,13 +16272,13 @@
         <v>413</v>
       </c>
       <c r="H126">
-        <v>740</v>
+        <v>800</v>
       </c>
       <c r="I126" s="13">
         <v>1</v>
       </c>
       <c r="J126" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f>_xlfn.TEXTJOIN(";",1,K126:AAC126)</f>
         <v>ti_routine</v>
       </c>
       <c r="AH126" t="s">
@@ -16220,14 +16292,14 @@
       <c r="B127" t="s">
         <v>416</v>
       </c>
-      <c r="C127" s="20" t="s">
-        <v>707</v>
+      <c r="C127" t="s">
+        <v>715</v>
       </c>
       <c r="D127" t="s">
         <v>402</v>
       </c>
-      <c r="E127" s="20" t="s">
-        <v>706</v>
+      <c r="E127" t="s">
+        <v>776</v>
       </c>
       <c r="F127" t="s">
         <v>412</v>
@@ -16236,12 +16308,15 @@
         <v>413</v>
       </c>
       <c r="H127">
-        <v>750</v>
+        <v>710</v>
       </c>
       <c r="I127" s="13">
         <v>1</v>
       </c>
-      <c r="J127" s="4"/>
+      <c r="J127" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
       <c r="AH127" t="s">
         <v>411</v>
       </c>
@@ -16253,14 +16328,14 @@
       <c r="B128" t="s">
         <v>416</v>
       </c>
-      <c r="C128" s="20" t="s">
-        <v>709</v>
+      <c r="C128" t="s">
+        <v>717</v>
       </c>
       <c r="D128" t="s">
         <v>402</v>
       </c>
-      <c r="E128" s="20" t="s">
-        <v>708</v>
+      <c r="E128" t="s">
+        <v>777</v>
       </c>
       <c r="F128" t="s">
         <v>412</v>
@@ -16269,12 +16344,15 @@
         <v>413</v>
       </c>
       <c r="H128">
-        <v>760</v>
+        <v>720</v>
       </c>
       <c r="I128" s="13">
         <v>1</v>
       </c>
-      <c r="J128" s="4"/>
+      <c r="J128" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
       <c r="AH128" t="s">
         <v>411</v>
       </c>
@@ -16286,14 +16364,14 @@
       <c r="B129" t="s">
         <v>416</v>
       </c>
-      <c r="C129" s="20" t="s">
+      <c r="C129" t="s">
         <v>711</v>
       </c>
       <c r="D129" t="s">
         <v>402</v>
       </c>
-      <c r="E129" s="20" t="s">
-        <v>710</v>
+      <c r="E129" t="s">
+        <v>755</v>
       </c>
       <c r="F129" t="s">
         <v>412</v>
@@ -16302,12 +16380,15 @@
         <v>413</v>
       </c>
       <c r="H129">
-        <v>770</v>
+        <v>730</v>
       </c>
       <c r="I129" s="13">
         <v>1</v>
       </c>
-      <c r="J129" s="4"/>
+      <c r="J129" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
       <c r="AH129" t="s">
         <v>411</v>
       </c>
@@ -16319,14 +16400,14 @@
       <c r="B130" t="s">
         <v>416</v>
       </c>
-      <c r="C130" s="20" t="s">
+      <c r="C130" t="s">
         <v>713</v>
       </c>
       <c r="D130" t="s">
         <v>402</v>
       </c>
-      <c r="E130" s="20" t="s">
-        <v>712</v>
+      <c r="E130" t="s">
+        <v>756</v>
       </c>
       <c r="F130" t="s">
         <v>412</v>
@@ -16335,12 +16416,15 @@
         <v>413</v>
       </c>
       <c r="H130">
-        <v>780</v>
+        <v>740</v>
       </c>
       <c r="I130" s="13">
         <v>1</v>
       </c>
-      <c r="J130" s="4"/>
+      <c r="J130" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
       <c r="AH130" t="s">
         <v>411</v>
       </c>
@@ -16352,14 +16436,14 @@
       <c r="B131" t="s">
         <v>416</v>
       </c>
-      <c r="C131" s="20" t="s">
-        <v>715</v>
+      <c r="C131" t="s">
+        <v>719</v>
       </c>
       <c r="D131" t="s">
         <v>402</v>
       </c>
-      <c r="E131" s="20" t="s">
-        <v>714</v>
+      <c r="E131" t="s">
+        <v>757</v>
       </c>
       <c r="F131" t="s">
         <v>412</v>
@@ -16368,12 +16452,15 @@
         <v>413</v>
       </c>
       <c r="H131">
-        <v>790</v>
+        <v>750</v>
       </c>
       <c r="I131" s="13">
         <v>1</v>
       </c>
-      <c r="J131" s="4"/>
+      <c r="J131" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
       <c r="AH131" t="s">
         <v>411</v>
       </c>
@@ -16385,14 +16472,14 @@
       <c r="B132" t="s">
         <v>416</v>
       </c>
-      <c r="C132" s="20" t="s">
-        <v>717</v>
+      <c r="C132" t="s">
+        <v>721</v>
       </c>
       <c r="D132" t="s">
         <v>402</v>
       </c>
-      <c r="E132" s="20" t="s">
-        <v>716</v>
+      <c r="E132" t="s">
+        <v>758</v>
       </c>
       <c r="F132" t="s">
         <v>412</v>
@@ -16401,12 +16488,15 @@
         <v>413</v>
       </c>
       <c r="H132">
-        <v>800</v>
+        <v>760</v>
       </c>
       <c r="I132" s="13">
         <v>1</v>
       </c>
-      <c r="J132" s="4"/>
+      <c r="J132" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
       <c r="AH132" t="s">
         <v>411</v>
       </c>
@@ -16418,14 +16508,14 @@
       <c r="B133" t="s">
         <v>416</v>
       </c>
-      <c r="C133" s="20" t="s">
-        <v>719</v>
+      <c r="C133" t="s">
+        <v>707</v>
       </c>
       <c r="D133" t="s">
         <v>402</v>
       </c>
-      <c r="E133" s="20" t="s">
-        <v>718</v>
+      <c r="E133" t="s">
+        <v>754</v>
       </c>
       <c r="F133" t="s">
         <v>412</v>
@@ -16439,7 +16529,10 @@
       <c r="I133" s="13">
         <v>1</v>
       </c>
-      <c r="J133" s="4"/>
+      <c r="J133" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
       <c r="AH133" t="s">
         <v>411</v>
       </c>
@@ -16451,14 +16544,14 @@
       <c r="B134" t="s">
         <v>416</v>
       </c>
-      <c r="C134" s="20" t="s">
-        <v>721</v>
+      <c r="C134" t="s">
+        <v>709</v>
       </c>
       <c r="D134" t="s">
         <v>402</v>
       </c>
-      <c r="E134" s="20" t="s">
-        <v>720</v>
+      <c r="E134" t="s">
+        <v>759</v>
       </c>
       <c r="F134" t="s">
         <v>412</v>
@@ -16472,7 +16565,10 @@
       <c r="I134" s="13">
         <v>1</v>
       </c>
-      <c r="J134" s="4"/>
+      <c r="J134" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
       <c r="AH134" t="s">
         <v>411</v>
       </c>
@@ -16484,14 +16580,14 @@
       <c r="B135" t="s">
         <v>416</v>
       </c>
-      <c r="C135" s="20" t="s">
+      <c r="C135" t="s">
         <v>723</v>
       </c>
       <c r="D135" t="s">
         <v>402</v>
       </c>
-      <c r="E135" s="20" t="s">
-        <v>722</v>
+      <c r="E135" t="s">
+        <v>760</v>
       </c>
       <c r="F135" t="s">
         <v>412</v>
@@ -16505,7 +16601,10 @@
       <c r="I135" s="13">
         <v>1</v>
       </c>
-      <c r="J135" s="4"/>
+      <c r="J135" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
       <c r="AH135" t="s">
         <v>411</v>
       </c>
@@ -16517,14 +16616,14 @@
       <c r="B136" t="s">
         <v>416</v>
       </c>
-      <c r="C136" s="20" t="s">
+      <c r="C136" t="s">
         <v>725</v>
       </c>
       <c r="D136" t="s">
         <v>402</v>
       </c>
-      <c r="E136" s="20" t="s">
-        <v>724</v>
+      <c r="E136" t="s">
+        <v>761</v>
       </c>
       <c r="F136" t="s">
         <v>412</v>
@@ -16538,7 +16637,10 @@
       <c r="I136" s="13">
         <v>1</v>
       </c>
-      <c r="J136" s="4"/>
+      <c r="J136" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
       <c r="AH136" t="s">
         <v>411</v>
       </c>
@@ -16550,14 +16652,14 @@
       <c r="B137" t="s">
         <v>416</v>
       </c>
-      <c r="C137" s="20" t="s">
+      <c r="C137" t="s">
         <v>727</v>
       </c>
       <c r="D137" t="s">
         <v>402</v>
       </c>
-      <c r="E137" s="20" t="s">
-        <v>726</v>
+      <c r="E137" t="s">
+        <v>762</v>
       </c>
       <c r="F137" t="s">
         <v>412</v>
@@ -16571,7 +16673,10 @@
       <c r="I137" s="13">
         <v>1</v>
       </c>
-      <c r="J137" s="4"/>
+      <c r="J137" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
       <c r="AH137" t="s">
         <v>411</v>
       </c>
@@ -16583,14 +16688,14 @@
       <c r="B138" t="s">
         <v>416</v>
       </c>
-      <c r="C138" s="20" t="s">
+      <c r="C138" t="s">
         <v>729</v>
       </c>
       <c r="D138" t="s">
         <v>402</v>
       </c>
-      <c r="E138" s="20" t="s">
-        <v>728</v>
+      <c r="E138" t="s">
+        <v>763</v>
       </c>
       <c r="F138" t="s">
         <v>412</v>
@@ -16604,7 +16709,10 @@
       <c r="I138" s="13">
         <v>1</v>
       </c>
-      <c r="J138" s="4"/>
+      <c r="J138" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
       <c r="AH138" t="s">
         <v>411</v>
       </c>
@@ -16616,14 +16724,14 @@
       <c r="B139" t="s">
         <v>416</v>
       </c>
-      <c r="C139" s="20" t="s">
+      <c r="C139" t="s">
         <v>731</v>
       </c>
       <c r="D139" t="s">
         <v>402</v>
       </c>
-      <c r="E139" s="20" t="s">
-        <v>730</v>
+      <c r="E139" t="s">
+        <v>764</v>
       </c>
       <c r="F139" t="s">
         <v>412</v>
@@ -16637,7 +16745,10 @@
       <c r="I139" s="13">
         <v>1</v>
       </c>
-      <c r="J139" s="4"/>
+      <c r="J139" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
       <c r="AH139" t="s">
         <v>411</v>
       </c>
@@ -16649,14 +16760,14 @@
       <c r="B140" t="s">
         <v>416</v>
       </c>
-      <c r="C140" s="20" t="s">
+      <c r="C140" t="s">
         <v>733</v>
       </c>
       <c r="D140" t="s">
         <v>402</v>
       </c>
-      <c r="E140" s="20" t="s">
-        <v>732</v>
+      <c r="E140" t="s">
+        <v>765</v>
       </c>
       <c r="F140" t="s">
         <v>412</v>
@@ -16670,7 +16781,10 @@
       <c r="I140" s="13">
         <v>1</v>
       </c>
-      <c r="J140" s="4"/>
+      <c r="J140" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
       <c r="AH140" t="s">
         <v>411</v>
       </c>
@@ -16682,14 +16796,14 @@
       <c r="B141" t="s">
         <v>416</v>
       </c>
-      <c r="C141" s="20" t="s">
+      <c r="C141" t="s">
         <v>735</v>
       </c>
       <c r="D141" t="s">
         <v>402</v>
       </c>
-      <c r="E141" s="20" t="s">
-        <v>734</v>
+      <c r="E141" t="s">
+        <v>766</v>
       </c>
       <c r="F141" t="s">
         <v>412</v>
@@ -16703,7 +16817,10 @@
       <c r="I141" s="13">
         <v>1</v>
       </c>
-      <c r="J141" s="4"/>
+      <c r="J141" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
       <c r="AH141" t="s">
         <v>411</v>
       </c>
@@ -16715,14 +16832,14 @@
       <c r="B142" t="s">
         <v>416</v>
       </c>
-      <c r="C142" s="20" t="s">
+      <c r="C142" t="s">
         <v>737</v>
       </c>
       <c r="D142" t="s">
         <v>402</v>
       </c>
-      <c r="E142" s="20" t="s">
-        <v>736</v>
+      <c r="E142" t="s">
+        <v>767</v>
       </c>
       <c r="F142" t="s">
         <v>412</v>
@@ -16736,7 +16853,10 @@
       <c r="I142" s="13">
         <v>1</v>
       </c>
-      <c r="J142" s="4"/>
+      <c r="J142" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
       <c r="AH142" t="s">
         <v>411</v>
       </c>
@@ -16748,14 +16868,14 @@
       <c r="B143" t="s">
         <v>416</v>
       </c>
-      <c r="C143" s="20" t="s">
+      <c r="C143" t="s">
         <v>739</v>
       </c>
       <c r="D143" t="s">
         <v>402</v>
       </c>
-      <c r="E143" s="20" t="s">
-        <v>738</v>
+      <c r="E143" t="s">
+        <v>768</v>
       </c>
       <c r="F143" t="s">
         <v>412</v>
@@ -16769,7 +16889,10 @@
       <c r="I143" s="13">
         <v>1</v>
       </c>
-      <c r="J143" s="4"/>
+      <c r="J143" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
       <c r="AH143" t="s">
         <v>411</v>
       </c>
@@ -16781,14 +16904,14 @@
       <c r="B144" t="s">
         <v>416</v>
       </c>
-      <c r="C144" s="20" t="s">
+      <c r="C144" t="s">
         <v>741</v>
       </c>
       <c r="D144" t="s">
         <v>402</v>
       </c>
-      <c r="E144" s="20" t="s">
-        <v>740</v>
+      <c r="E144" t="s">
+        <v>769</v>
       </c>
       <c r="F144" t="s">
         <v>412</v>
@@ -16802,7 +16925,10 @@
       <c r="I144" s="13">
         <v>1</v>
       </c>
-      <c r="J144" s="4"/>
+      <c r="J144" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
       <c r="AH144" t="s">
         <v>411</v>
       </c>
@@ -16814,14 +16940,14 @@
       <c r="B145" t="s">
         <v>416</v>
       </c>
-      <c r="C145" s="20" t="s">
+      <c r="C145" t="s">
         <v>743</v>
       </c>
       <c r="D145" t="s">
         <v>402</v>
       </c>
-      <c r="E145" s="20" t="s">
-        <v>742</v>
+      <c r="E145" t="s">
+        <v>770</v>
       </c>
       <c r="F145" t="s">
         <v>412</v>
@@ -16835,7 +16961,10 @@
       <c r="I145" s="13">
         <v>1</v>
       </c>
-      <c r="J145" s="4"/>
+      <c r="J145" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
       <c r="AH145" t="s">
         <v>411</v>
       </c>
@@ -16847,14 +16976,14 @@
       <c r="B146" t="s">
         <v>416</v>
       </c>
-      <c r="C146" s="20" t="s">
+      <c r="C146" t="s">
         <v>745</v>
       </c>
       <c r="D146" t="s">
         <v>402</v>
       </c>
-      <c r="E146" s="20" t="s">
-        <v>744</v>
+      <c r="E146" t="s">
+        <v>771</v>
       </c>
       <c r="F146" t="s">
         <v>412</v>
@@ -16868,7 +16997,10 @@
       <c r="I146" s="13">
         <v>1</v>
       </c>
-      <c r="J146" s="4"/>
+      <c r="J146" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
       <c r="AH146" t="s">
         <v>411</v>
       </c>
@@ -16880,14 +17012,14 @@
       <c r="B147" t="s">
         <v>416</v>
       </c>
-      <c r="C147" s="20" t="s">
-        <v>747</v>
+      <c r="C147" t="s">
+        <v>751</v>
       </c>
       <c r="D147" t="s">
         <v>402</v>
       </c>
-      <c r="E147" s="20" t="s">
-        <v>746</v>
+      <c r="E147" t="s">
+        <v>772</v>
       </c>
       <c r="F147" t="s">
         <v>412</v>
@@ -16901,7 +17033,10 @@
       <c r="I147" s="13">
         <v>1</v>
       </c>
-      <c r="J147" s="4"/>
+      <c r="J147" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
       <c r="AH147" t="s">
         <v>411</v>
       </c>
@@ -16913,14 +17048,14 @@
       <c r="B148" t="s">
         <v>416</v>
       </c>
-      <c r="C148" s="20" t="s">
-        <v>749</v>
+      <c r="C148" t="s">
+        <v>753</v>
       </c>
       <c r="D148" t="s">
         <v>402</v>
       </c>
-      <c r="E148" s="20" t="s">
-        <v>748</v>
+      <c r="E148" t="s">
+        <v>773</v>
       </c>
       <c r="F148" t="s">
         <v>412</v>
@@ -16934,7 +17069,10 @@
       <c r="I148" s="13">
         <v>1</v>
       </c>
-      <c r="J148" s="4"/>
+      <c r="J148" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
       <c r="AH148" t="s">
         <v>411</v>
       </c>
@@ -16946,14 +17084,14 @@
       <c r="B149" t="s">
         <v>416</v>
       </c>
-      <c r="C149" s="20" t="s">
-        <v>751</v>
+      <c r="C149" t="s">
+        <v>747</v>
       </c>
       <c r="D149" t="s">
         <v>402</v>
       </c>
-      <c r="E149" s="20" t="s">
-        <v>750</v>
+      <c r="E149" t="s">
+        <v>774</v>
       </c>
       <c r="F149" t="s">
         <v>412</v>
@@ -16967,7 +17105,10 @@
       <c r="I149" s="13">
         <v>1</v>
       </c>
-      <c r="J149" s="4"/>
+      <c r="J149" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
       <c r="AH149" t="s">
         <v>411</v>
       </c>
@@ -16979,14 +17120,14 @@
       <c r="B150" t="s">
         <v>416</v>
       </c>
-      <c r="C150" s="20" t="s">
-        <v>753</v>
+      <c r="C150" t="s">
+        <v>749</v>
       </c>
       <c r="D150" t="s">
         <v>402</v>
       </c>
-      <c r="E150" s="20" t="s">
-        <v>752</v>
+      <c r="E150" t="s">
+        <v>775</v>
       </c>
       <c r="F150" t="s">
         <v>412</v>
@@ -17000,7 +17141,10 @@
       <c r="I150" s="13">
         <v>1</v>
       </c>
-      <c r="J150" s="4"/>
+      <c r="J150" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>ti_routine</v>
+      </c>
       <c r="AH150" t="s">
         <v>411</v>
       </c>

</xml_diff>

<commit_message>
Updated HTS_TST Indicator Name and ID
Updates both HTS_TST indicators from FY19 to FY20 versions. (A indicator Columns)
Addresses pepfar-datim/Data-Pack#903
</commit_message>
<xml_diff>
--- a/data-raw/model_calculations/model_calculations.xlsx
+++ b/data-raw/model_calculations/model_calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christiandomaas/Documents/GitHub/data-pack-commons/data-raw/model_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A2E1CB-5E44-6545-A6D4-13426F8CD6EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{41F141E9-8C54-8045-86E9-EED34362CEB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="480" windowWidth="33600" windowHeight="20540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{534AEB7A-72AD-754E-A1BC-F197B85E6149}"/>
   </bookViews>
   <sheets>
     <sheet name="data_required" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4244" uniqueCount="795">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4244" uniqueCount="797">
   <si>
     <t>PMTCT_STAT_ART</t>
   </si>
@@ -1398,9 +1398,6 @@
   </si>
   <si>
     <t>2019Oct</t>
-  </si>
-  <si>
-    <t>IQJhBffoYIJ</t>
   </si>
   <si>
     <t>joBC2hxzpGN</t>
@@ -2569,13 +2566,22 @@
     <t>tb_p_art_n</t>
   </si>
   <si>
-    <t>FY19 Results Analytic Indicators: HTS_TST Yield (HTS_TST_POS/HTS_TST)</t>
-  </si>
-  <si>
     <t>2020Oct</t>
   </si>
   <si>
     <t>2020Q3</t>
+  </si>
+  <si>
+    <t>FY20 Results Analytic Indicators: HTS_TST Yield (HTS_TST_POS/HTS_TST)</t>
+  </si>
+  <si>
+    <t>oJ3sBx7qSbl</t>
+  </si>
+  <si>
+    <t>FY20 Results Analytic Indicators: HTS_TST_POS (Age/Sex)</t>
+  </si>
+  <si>
+    <t>zlLxydzTpzD</t>
   </si>
 </sst>
 </file>
@@ -3027,10 +3033,10 @@
   <dimension ref="A1:AK66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="T44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X64" sqref="X1:X1048576"/>
+      <selection pane="bottomRight" activeCell="H63" sqref="H63:I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3073,7 +3079,7 @@
         <v>415</v>
       </c>
       <c r="H1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="I1" t="s">
         <v>218</v>
@@ -3115,7 +3121,7 @@
         <v>157</v>
       </c>
       <c r="V1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="W1" t="s">
         <v>219</v>
@@ -3168,13 +3174,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -3186,13 +3192,13 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="I2" t="s">
         <v>58</v>
       </c>
       <c r="J2" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K2" t="s">
         <v>135</v>
@@ -3287,7 +3293,7 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
@@ -3299,10 +3305,10 @@
         <v>138</v>
       </c>
       <c r="H3" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>453</v>
+        <v>794</v>
       </c>
       <c r="J3" t="s">
         <v>452</v>
@@ -3317,7 +3323,7 @@
         <v>138</v>
       </c>
       <c r="N3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="O3" t="s">
         <v>138</v>
@@ -3400,7 +3406,7 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
@@ -3412,7 +3418,7 @@
         <v>8</v>
       </c>
       <c r="H4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I4" t="s">
         <v>59</v>
@@ -3513,7 +3519,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
@@ -3525,7 +3531,7 @@
         <v>9</v>
       </c>
       <c r="H5" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I5" t="s">
         <v>60</v>
@@ -3620,13 +3626,13 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E6" t="s">
         <v>3</v>
@@ -3638,13 +3644,13 @@
         <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="I6" t="s">
         <v>61</v>
       </c>
       <c r="J6" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K6" t="s">
         <v>144</v>
@@ -3739,7 +3745,7 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
@@ -3751,13 +3757,13 @@
         <v>11</v>
       </c>
       <c r="H7" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="I7" t="s">
         <v>61</v>
       </c>
       <c r="J7" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K7" t="s">
         <v>144</v>
@@ -3793,7 +3799,7 @@
         <v>62</v>
       </c>
       <c r="V7" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="W7" t="s">
         <v>63</v>
@@ -3852,7 +3858,7 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E8" t="s">
         <v>5</v>
@@ -3864,7 +3870,7 @@
         <v>13</v>
       </c>
       <c r="H8" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="I8" t="s">
         <v>64</v>
@@ -3965,7 +3971,7 @@
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E9" t="s">
         <v>5</v>
@@ -3977,10 +3983,10 @@
         <v>138</v>
       </c>
       <c r="H9" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>453</v>
+        <v>794</v>
       </c>
       <c r="J9" t="s">
         <v>452</v>
@@ -3995,7 +4001,7 @@
         <v>138</v>
       </c>
       <c r="N9" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="O9" t="s">
         <v>138</v>
@@ -4072,13 +4078,13 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E10" t="s">
         <v>3</v>
@@ -4087,16 +4093,16 @@
         <v>137</v>
       </c>
       <c r="G10" t="s">
+        <v>517</v>
+      </c>
+      <c r="H10" t="s">
+        <v>525</v>
+      </c>
+      <c r="I10" t="s">
         <v>518</v>
       </c>
-      <c r="H10" t="s">
-        <v>526</v>
-      </c>
-      <c r="I10" t="s">
-        <v>519</v>
-      </c>
       <c r="J10" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K10" t="s">
         <v>135</v>
@@ -4191,7 +4197,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E11" t="s">
         <v>5</v>
@@ -4203,10 +4209,10 @@
         <v>138</v>
       </c>
       <c r="H11" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>453</v>
+        <v>794</v>
       </c>
       <c r="J11" t="s">
         <v>452</v>
@@ -4221,7 +4227,7 @@
         <v>138</v>
       </c>
       <c r="N11" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="O11" t="s">
         <v>138</v>
@@ -4304,7 +4310,7 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="E12" t="s">
         <v>5</v>
@@ -4313,13 +4319,13 @@
         <v>139</v>
       </c>
       <c r="G12" t="s">
+        <v>454</v>
+      </c>
+      <c r="H12" t="s">
+        <v>526</v>
+      </c>
+      <c r="I12" t="s">
         <v>455</v>
-      </c>
-      <c r="H12" t="s">
-        <v>527</v>
-      </c>
-      <c r="I12" t="s">
-        <v>456</v>
       </c>
       <c r="J12" t="s">
         <v>452</v>
@@ -4411,13 +4417,13 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E13" t="s">
         <v>3</v>
@@ -4429,13 +4435,13 @@
         <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="I13" t="s">
         <v>65</v>
       </c>
       <c r="J13" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K13" t="s">
         <v>144</v>
@@ -4530,7 +4536,7 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
@@ -4542,10 +4548,10 @@
         <v>138</v>
       </c>
       <c r="H14" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>453</v>
+        <v>794</v>
       </c>
       <c r="J14" t="s">
         <v>452</v>
@@ -4643,7 +4649,7 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E15" t="s">
         <v>5</v>
@@ -4655,10 +4661,10 @@
         <v>138</v>
       </c>
       <c r="H15" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>453</v>
+        <v>794</v>
       </c>
       <c r="J15" t="s">
         <v>452</v>
@@ -4756,7 +4762,7 @@
         <v>4</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E16" t="s">
         <v>5</v>
@@ -4768,10 +4774,10 @@
         <v>138</v>
       </c>
       <c r="H16" t="s">
-        <v>529</v>
+        <v>795</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>454</v>
+        <v>796</v>
       </c>
       <c r="J16" t="s">
         <v>452</v>
@@ -4810,10 +4816,10 @@
         <v>138</v>
       </c>
       <c r="V16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="X16" t="s">
         <v>452</v>
@@ -4869,7 +4875,7 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E17" t="s">
         <v>5</v>
@@ -4881,10 +4887,10 @@
         <v>138</v>
       </c>
       <c r="H17" t="s">
-        <v>529</v>
+        <v>795</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>454</v>
+        <v>796</v>
       </c>
       <c r="J17" t="s">
         <v>452</v>
@@ -4923,10 +4929,10 @@
         <v>138</v>
       </c>
       <c r="V17" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="X17" t="s">
         <v>452</v>
@@ -4982,7 +4988,7 @@
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E18" t="s">
         <v>5</v>
@@ -4994,10 +5000,10 @@
         <v>138</v>
       </c>
       <c r="H18" t="s">
-        <v>529</v>
+        <v>795</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>454</v>
+        <v>796</v>
       </c>
       <c r="J18" t="s">
         <v>452</v>
@@ -5036,10 +5042,10 @@
         <v>138</v>
       </c>
       <c r="V18" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="X18" t="s">
         <v>452</v>
@@ -5095,7 +5101,7 @@
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E19" t="s">
         <v>5</v>
@@ -5107,10 +5113,10 @@
         <v>138</v>
       </c>
       <c r="H19" t="s">
-        <v>529</v>
+        <v>795</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>454</v>
+        <v>796</v>
       </c>
       <c r="J19" t="s">
         <v>452</v>
@@ -5149,10 +5155,10 @@
         <v>138</v>
       </c>
       <c r="V19" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="X19" t="s">
         <v>452</v>
@@ -5208,7 +5214,7 @@
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="E20" t="s">
         <v>5</v>
@@ -5220,10 +5226,10 @@
         <v>138</v>
       </c>
       <c r="H20" t="s">
-        <v>529</v>
+        <v>795</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>454</v>
+        <v>796</v>
       </c>
       <c r="J20" t="s">
         <v>452</v>
@@ -5262,10 +5268,10 @@
         <v>138</v>
       </c>
       <c r="V20" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="X20" t="s">
         <v>452</v>
@@ -5321,7 +5327,7 @@
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E21" t="s">
         <v>5</v>
@@ -5333,10 +5339,10 @@
         <v>138</v>
       </c>
       <c r="H21" t="s">
-        <v>529</v>
+        <v>795</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>454</v>
+        <v>796</v>
       </c>
       <c r="J21" t="s">
         <v>452</v>
@@ -5375,10 +5381,10 @@
         <v>138</v>
       </c>
       <c r="V21" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="W21" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="X21" t="s">
         <v>452</v>
@@ -5434,7 +5440,7 @@
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E22" t="s">
         <v>5</v>
@@ -5446,10 +5452,10 @@
         <v>138</v>
       </c>
       <c r="H22" t="s">
-        <v>529</v>
+        <v>795</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>454</v>
+        <v>796</v>
       </c>
       <c r="J22" t="s">
         <v>452</v>
@@ -5488,10 +5494,10 @@
         <v>138</v>
       </c>
       <c r="V22" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="X22" t="s">
         <v>452</v>
@@ -5547,7 +5553,7 @@
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E23" t="s">
         <v>5</v>
@@ -5559,10 +5565,10 @@
         <v>138</v>
       </c>
       <c r="H23" t="s">
-        <v>529</v>
+        <v>795</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>454</v>
+        <v>796</v>
       </c>
       <c r="J23" t="s">
         <v>452</v>
@@ -5601,10 +5607,10 @@
         <v>138</v>
       </c>
       <c r="V23" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="W23" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="X23" t="s">
         <v>452</v>
@@ -5660,7 +5666,7 @@
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="E24" t="s">
         <v>5</v>
@@ -5672,10 +5678,10 @@
         <v>138</v>
       </c>
       <c r="H24" t="s">
-        <v>529</v>
+        <v>795</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>454</v>
+        <v>796</v>
       </c>
       <c r="J24" t="s">
         <v>452</v>
@@ -5714,10 +5720,10 @@
         <v>138</v>
       </c>
       <c r="V24" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="W24" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="X24" t="s">
         <v>452</v>
@@ -5773,7 +5779,7 @@
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E25" t="s">
         <v>5</v>
@@ -5785,10 +5791,10 @@
         <v>138</v>
       </c>
       <c r="H25" t="s">
-        <v>529</v>
+        <v>795</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>454</v>
+        <v>796</v>
       </c>
       <c r="J25" t="s">
         <v>452</v>
@@ -5827,10 +5833,10 @@
         <v>138</v>
       </c>
       <c r="V25" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="W25" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="X25" t="s">
         <v>452</v>
@@ -5886,7 +5892,7 @@
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E26" t="s">
         <v>5</v>
@@ -5898,10 +5904,10 @@
         <v>138</v>
       </c>
       <c r="H26" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>453</v>
+        <v>794</v>
       </c>
       <c r="J26" t="s">
         <v>452</v>
@@ -5999,7 +6005,7 @@
         <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E27" t="s">
         <v>5</v>
@@ -6011,10 +6017,10 @@
         <v>138</v>
       </c>
       <c r="H27" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>453</v>
+        <v>794</v>
       </c>
       <c r="J27" t="s">
         <v>452</v>
@@ -6112,7 +6118,7 @@
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E28" t="s">
         <v>5</v>
@@ -6124,10 +6130,10 @@
         <v>138</v>
       </c>
       <c r="H28" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>453</v>
+        <v>794</v>
       </c>
       <c r="J28" t="s">
         <v>452</v>
@@ -6225,7 +6231,7 @@
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E29" t="s">
         <v>5</v>
@@ -6237,10 +6243,10 @@
         <v>138</v>
       </c>
       <c r="H29" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>453</v>
+        <v>794</v>
       </c>
       <c r="J29" t="s">
         <v>452</v>
@@ -6338,7 +6344,7 @@
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E30" t="s">
         <v>5</v>
@@ -6350,10 +6356,10 @@
         <v>138</v>
       </c>
       <c r="H30" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>453</v>
+        <v>794</v>
       </c>
       <c r="J30" t="s">
         <v>452</v>
@@ -6451,7 +6457,7 @@
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E31" t="s">
         <v>5</v>
@@ -6463,10 +6469,10 @@
         <v>138</v>
       </c>
       <c r="H31" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>453</v>
+        <v>794</v>
       </c>
       <c r="J31" t="s">
         <v>452</v>
@@ -6564,7 +6570,7 @@
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E32" t="s">
         <v>5</v>
@@ -6576,10 +6582,10 @@
         <v>138</v>
       </c>
       <c r="H32" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>453</v>
+        <v>794</v>
       </c>
       <c r="J32" t="s">
         <v>452</v>
@@ -6677,7 +6683,7 @@
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E33" t="s">
         <v>5</v>
@@ -6689,10 +6695,10 @@
         <v>138</v>
       </c>
       <c r="H33" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>453</v>
+        <v>794</v>
       </c>
       <c r="J33" t="s">
         <v>452</v>
@@ -6790,7 +6796,7 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E34" t="s">
         <v>5</v>
@@ -6802,10 +6808,10 @@
         <v>138</v>
       </c>
       <c r="H34" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>453</v>
+        <v>794</v>
       </c>
       <c r="J34" t="s">
         <v>452</v>
@@ -6897,13 +6903,13 @@
         <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="E35" t="s">
         <v>5</v>
@@ -6915,10 +6921,10 @@
         <v>138</v>
       </c>
       <c r="H35" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>453</v>
+        <v>794</v>
       </c>
       <c r="J35" t="s">
         <v>452</v>
@@ -6933,7 +6939,7 @@
         <v>138</v>
       </c>
       <c r="N35" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="O35" t="s">
         <v>138</v>
@@ -7016,7 +7022,7 @@
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E36" t="s">
         <v>5</v>
@@ -7028,13 +7034,13 @@
         <v>173</v>
       </c>
       <c r="H36" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I36" t="s">
         <v>172</v>
       </c>
       <c r="J36" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K36" t="s">
         <v>135</v>
@@ -7070,7 +7076,7 @@
         <v>175</v>
       </c>
       <c r="V36" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="W36" t="s">
         <v>174</v>
@@ -7129,7 +7135,7 @@
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E37" t="s">
         <v>5</v>
@@ -7138,13 +7144,13 @@
         <v>139</v>
       </c>
       <c r="G37" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="H37" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="J37" t="s">
         <v>452</v>
@@ -7242,7 +7248,7 @@
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E38" t="s">
         <v>5</v>
@@ -7251,13 +7257,13 @@
         <v>139</v>
       </c>
       <c r="G38" t="s">
+        <v>463</v>
+      </c>
+      <c r="H38" t="s">
+        <v>531</v>
+      </c>
+      <c r="I38" s="1" t="s">
         <v>464</v>
-      </c>
-      <c r="H38" t="s">
-        <v>532</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>465</v>
       </c>
       <c r="J38" t="s">
         <v>452</v>
@@ -7349,13 +7355,13 @@
         <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C39" t="s">
         <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="E39" t="s">
         <v>3</v>
@@ -7364,16 +7370,16 @@
         <v>137</v>
       </c>
       <c r="G39" t="s">
+        <v>458</v>
+      </c>
+      <c r="H39" t="s">
+        <v>532</v>
+      </c>
+      <c r="I39" t="s">
         <v>459</v>
       </c>
-      <c r="H39" t="s">
-        <v>533</v>
-      </c>
-      <c r="I39" t="s">
-        <v>460</v>
-      </c>
       <c r="J39" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K39" t="s">
         <v>224</v>
@@ -7468,7 +7474,7 @@
         <v>4</v>
       </c>
       <c r="D40" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E40" t="s">
         <v>5</v>
@@ -7477,16 +7483,16 @@
         <v>137</v>
       </c>
       <c r="G40" t="s">
+        <v>458</v>
+      </c>
+      <c r="H40" t="s">
+        <v>532</v>
+      </c>
+      <c r="I40" t="s">
         <v>459</v>
       </c>
-      <c r="H40" t="s">
-        <v>533</v>
-      </c>
-      <c r="I40" t="s">
-        <v>460</v>
-      </c>
       <c r="J40" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K40" t="s">
         <v>224</v>
@@ -7519,13 +7525,13 @@
         <v>138</v>
       </c>
       <c r="U40" t="s">
+        <v>456</v>
+      </c>
+      <c r="V40" t="s">
+        <v>545</v>
+      </c>
+      <c r="W40" t="s">
         <v>457</v>
-      </c>
-      <c r="V40" t="s">
-        <v>546</v>
-      </c>
-      <c r="W40" t="s">
-        <v>458</v>
       </c>
       <c r="X40" s="1" t="s">
         <v>452</v>
@@ -7575,13 +7581,13 @@
         <v>45</v>
       </c>
       <c r="B41" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C41" t="s">
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E41" t="s">
         <v>3</v>
@@ -7593,13 +7599,13 @@
         <v>46</v>
       </c>
       <c r="H41" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="I41" t="s">
         <v>66</v>
       </c>
       <c r="J41" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K41" t="s">
         <v>138</v>
@@ -7688,13 +7694,13 @@
         <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C42" t="s">
         <v>2</v>
       </c>
       <c r="D42" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E42" t="s">
         <v>3</v>
@@ -7706,13 +7712,13 @@
         <v>67</v>
       </c>
       <c r="H42" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I42" t="s">
         <v>68</v>
       </c>
       <c r="J42" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K42" t="s">
         <v>138</v>
@@ -7801,13 +7807,13 @@
         <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C43" t="s">
         <v>2</v>
       </c>
       <c r="D43" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E43" t="s">
         <v>3</v>
@@ -7819,13 +7825,13 @@
         <v>67</v>
       </c>
       <c r="H43" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I43" t="s">
         <v>68</v>
       </c>
       <c r="J43" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K43" t="s">
         <v>138</v>
@@ -7914,13 +7920,13 @@
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C44" t="s">
         <v>2</v>
       </c>
       <c r="D44" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="E44" t="s">
         <v>3</v>
@@ -7932,13 +7938,13 @@
         <v>47</v>
       </c>
       <c r="H44" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I44" t="s">
         <v>69</v>
       </c>
       <c r="J44" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K44" t="s">
         <v>138</v>
@@ -8027,13 +8033,13 @@
         <v>49</v>
       </c>
       <c r="B45" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C45" t="s">
         <v>2</v>
       </c>
       <c r="D45" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="E45" t="s">
         <v>3</v>
@@ -8045,13 +8051,13 @@
         <v>50</v>
       </c>
       <c r="H45" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="I45" t="s">
         <v>71</v>
       </c>
       <c r="J45" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K45" t="s">
         <v>135</v>
@@ -8146,7 +8152,7 @@
         <v>4</v>
       </c>
       <c r="D46" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="E46" t="s">
         <v>5</v>
@@ -8158,13 +8164,13 @@
         <v>50</v>
       </c>
       <c r="H46" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="I46" t="s">
         <v>71</v>
       </c>
       <c r="J46" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K46" t="s">
         <v>135</v>
@@ -8200,7 +8206,7 @@
         <v>176</v>
       </c>
       <c r="V46" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="W46" t="s">
         <v>177</v>
@@ -8253,13 +8259,13 @@
         <v>52</v>
       </c>
       <c r="B47" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C47" t="s">
         <v>2</v>
       </c>
       <c r="D47" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="E47" t="s">
         <v>3</v>
@@ -8271,13 +8277,13 @@
         <v>53</v>
       </c>
       <c r="H47" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="I47" t="s">
         <v>72</v>
       </c>
       <c r="J47" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K47" t="s">
         <v>150</v>
@@ -8366,13 +8372,13 @@
         <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C48" t="s">
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="E48" t="s">
         <v>3</v>
@@ -8381,16 +8387,16 @@
         <v>137</v>
       </c>
       <c r="G48" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="H48" t="s">
         <v>558</v>
       </c>
-      <c r="H48" t="s">
+      <c r="I48" t="s">
         <v>559</v>
       </c>
-      <c r="I48" t="s">
-        <v>560</v>
-      </c>
       <c r="J48" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K48" t="s">
         <v>150</v>
@@ -8479,13 +8485,13 @@
         <v>54</v>
       </c>
       <c r="B49" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C49" t="s">
         <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E49" t="s">
         <v>3</v>
@@ -8497,13 +8503,13 @@
         <v>73</v>
       </c>
       <c r="H49" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="I49" t="s">
         <v>74</v>
       </c>
       <c r="J49" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K49" t="s">
         <v>138</v>
@@ -8592,13 +8598,13 @@
         <v>54</v>
       </c>
       <c r="B50" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C50" t="s">
         <v>2</v>
       </c>
       <c r="D50" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E50" t="s">
         <v>3</v>
@@ -8610,13 +8616,13 @@
         <v>75</v>
       </c>
       <c r="H50" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I50" t="s">
         <v>76</v>
       </c>
       <c r="J50" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K50" t="s">
         <v>138</v>
@@ -8711,7 +8717,7 @@
         <v>4</v>
       </c>
       <c r="D51" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="E51" t="s">
         <v>5</v>
@@ -8723,13 +8729,13 @@
         <v>138</v>
       </c>
       <c r="H51" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="J51" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K51" t="s">
         <v>138</v>
@@ -8765,7 +8771,7 @@
         <v>222</v>
       </c>
       <c r="V51" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="W51" s="1" t="s">
         <v>223</v>
@@ -8818,13 +8824,13 @@
         <v>45</v>
       </c>
       <c r="B52" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C52" t="s">
         <v>2</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E52" t="s">
         <v>3</v>
@@ -8836,13 +8842,13 @@
         <v>48</v>
       </c>
       <c r="H52" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I52" s="14" t="s">
         <v>70</v>
       </c>
       <c r="J52" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K52" t="s">
         <v>138</v>
@@ -8931,13 +8937,13 @@
         <v>45</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C53" t="s">
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="E53" t="s">
         <v>3</v>
@@ -8946,16 +8952,16 @@
         <v>137</v>
       </c>
       <c r="G53" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="H53" t="s">
+        <v>560</v>
+      </c>
+      <c r="I53" s="14" t="s">
         <v>563</v>
       </c>
-      <c r="H53" t="s">
-        <v>561</v>
-      </c>
-      <c r="I53" s="14" t="s">
-        <v>564</v>
-      </c>
       <c r="J53" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K53" t="s">
         <v>138</v>
@@ -9044,7 +9050,7 @@
         <v>45</v>
       </c>
       <c r="B54" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C54" t="s">
         <v>2</v>
@@ -9068,7 +9074,7 @@
         <v>448</v>
       </c>
       <c r="J54" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K54" t="s">
         <v>138</v>
@@ -9110,7 +9116,7 @@
         <v>449</v>
       </c>
       <c r="X54" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="Y54" t="s">
         <v>138</v>
@@ -9157,13 +9163,13 @@
         <v>445</v>
       </c>
       <c r="B55" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C55" t="s">
         <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="E55" t="s">
         <v>3</v>
@@ -9181,7 +9187,7 @@
         <v>446</v>
       </c>
       <c r="J55" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K55" t="s">
         <v>138</v>
@@ -9270,13 +9276,13 @@
         <v>20</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C56" t="s">
         <v>2</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="E56" t="s">
         <v>3</v>
@@ -9288,7 +9294,7 @@
         <v>175</v>
       </c>
       <c r="H56" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="I56" t="s">
         <v>174</v>
@@ -9383,13 +9389,13 @@
         <v>18</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C57" t="s">
         <v>2</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E57" t="s">
         <v>3</v>
@@ -9401,16 +9407,16 @@
         <v>138</v>
       </c>
       <c r="H57" s="16" t="s">
+        <v>632</v>
+      </c>
+      <c r="I57" s="16" t="s">
+        <v>631</v>
+      </c>
+      <c r="J57" t="s">
+        <v>792</v>
+      </c>
+      <c r="K57" s="9" t="s">
         <v>633</v>
-      </c>
-      <c r="I57" s="16" t="s">
-        <v>632</v>
-      </c>
-      <c r="J57" t="s">
-        <v>794</v>
-      </c>
-      <c r="K57" s="9" t="s">
-        <v>634</v>
       </c>
       <c r="L57" t="s">
         <v>140</v>
@@ -9496,13 +9502,13 @@
         <v>18</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C58" t="s">
         <v>2</v>
       </c>
       <c r="D58" s="16" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="E58" t="s">
         <v>3</v>
@@ -9514,16 +9520,16 @@
         <v>138</v>
       </c>
       <c r="H58" s="16" t="s">
+        <v>635</v>
+      </c>
+      <c r="I58" s="16" t="s">
         <v>636</v>
-      </c>
-      <c r="I58" s="16" t="s">
-        <v>637</v>
       </c>
       <c r="J58" t="s">
         <v>452</v>
       </c>
       <c r="K58" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="L58" t="s">
         <v>140</v>
@@ -9609,13 +9615,13 @@
         <v>18</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C59" t="s">
         <v>2</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="E59" t="s">
         <v>3</v>
@@ -9627,13 +9633,13 @@
         <v>138</v>
       </c>
       <c r="H59" s="11" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="I59" s="16" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="J59" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K59" t="s">
         <v>144</v>
@@ -9722,13 +9728,13 @@
         <v>18</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C60" t="s">
         <v>2</v>
       </c>
       <c r="D60" s="15" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E60" t="s">
         <v>3</v>
@@ -9740,13 +9746,13 @@
         <v>138</v>
       </c>
       <c r="H60" t="s">
+        <v>641</v>
+      </c>
+      <c r="I60" t="s">
         <v>642</v>
       </c>
-      <c r="I60" t="s">
-        <v>643</v>
-      </c>
       <c r="J60" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K60" t="s">
         <v>144</v>
@@ -9835,13 +9841,13 @@
         <v>18</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C61" t="s">
         <v>4</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E61" t="s">
         <v>5</v>
@@ -9853,10 +9859,10 @@
         <v>138</v>
       </c>
       <c r="H61" t="s">
+        <v>645</v>
+      </c>
+      <c r="I61" t="s">
         <v>646</v>
-      </c>
-      <c r="I61" t="s">
-        <v>647</v>
       </c>
       <c r="J61" t="s">
         <v>452</v>
@@ -9895,16 +9901,16 @@
         <v>138</v>
       </c>
       <c r="V61" s="16" t="s">
+        <v>635</v>
+      </c>
+      <c r="W61" s="16" t="s">
         <v>636</v>
-      </c>
-      <c r="W61" s="16" t="s">
-        <v>637</v>
       </c>
       <c r="X61" t="s">
         <v>452</v>
       </c>
       <c r="Y61" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="Z61" t="s">
         <v>140</v>
@@ -9948,13 +9954,13 @@
         <v>18</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C62" t="s">
         <v>4</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E62" t="s">
         <v>5</v>
@@ -9966,10 +9972,10 @@
         <v>138</v>
       </c>
       <c r="H62" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I62" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="J62" t="s">
         <v>452</v>
@@ -10008,16 +10014,16 @@
         <v>138</v>
       </c>
       <c r="V62" s="16" t="s">
+        <v>635</v>
+      </c>
+      <c r="W62" s="16" t="s">
         <v>636</v>
-      </c>
-      <c r="W62" s="16" t="s">
-        <v>637</v>
       </c>
       <c r="X62" t="s">
         <v>452</v>
       </c>
       <c r="Y62" s="19" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="Z62" t="s">
         <v>136</v>
@@ -10061,13 +10067,13 @@
         <v>18</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C63" t="s">
         <v>4</v>
       </c>
       <c r="D63" s="16" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="E63" t="s">
         <v>5</v>
@@ -10079,10 +10085,10 @@
         <v>138</v>
       </c>
       <c r="H63" t="s">
-        <v>529</v>
+        <v>795</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>454</v>
+        <v>796</v>
       </c>
       <c r="J63" t="s">
         <v>452</v>
@@ -10097,7 +10103,7 @@
         <v>138</v>
       </c>
       <c r="N63" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="O63" t="s">
         <v>138</v>
@@ -10121,16 +10127,16 @@
         <v>138</v>
       </c>
       <c r="V63" s="16" t="s">
+        <v>635</v>
+      </c>
+      <c r="W63" s="16" t="s">
         <v>636</v>
-      </c>
-      <c r="W63" s="16" t="s">
-        <v>637</v>
       </c>
       <c r="X63" t="s">
         <v>452</v>
       </c>
       <c r="Y63" s="19" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="Z63" t="s">
         <v>136</v>
@@ -10174,13 +10180,13 @@
         <v>18</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C64" t="s">
         <v>4</v>
       </c>
       <c r="D64" s="16" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E64" t="s">
         <v>5</v>
@@ -10192,10 +10198,10 @@
         <v>138</v>
       </c>
       <c r="H64" t="s">
-        <v>529</v>
+        <v>795</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>454</v>
+        <v>796</v>
       </c>
       <c r="J64" t="s">
         <v>452</v>
@@ -10210,7 +10216,7 @@
         <v>138</v>
       </c>
       <c r="N64" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="O64" t="s">
         <v>138</v>
@@ -10234,16 +10240,16 @@
         <v>138</v>
       </c>
       <c r="V64" s="16" t="s">
+        <v>635</v>
+      </c>
+      <c r="W64" s="16" t="s">
         <v>636</v>
-      </c>
-      <c r="W64" s="16" t="s">
-        <v>637</v>
       </c>
       <c r="X64" t="s">
         <v>452</v>
       </c>
       <c r="Y64" s="19" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="Z64" t="s">
         <v>143</v>
@@ -10287,13 +10293,13 @@
         <v>40</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C65" t="s">
         <v>2</v>
       </c>
       <c r="D65" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E65" t="s">
         <v>3</v>
@@ -10305,13 +10311,13 @@
         <v>138</v>
       </c>
       <c r="H65" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="J65" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K65" s="9" t="s">
         <v>412</v>
@@ -10400,13 +10406,13 @@
         <v>40</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C66" t="s">
         <v>2</v>
       </c>
       <c r="D66" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E66" t="s">
         <v>3</v>
@@ -10418,13 +10424,13 @@
         <v>138</v>
       </c>
       <c r="H66" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="J66" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="K66" s="9" t="s">
         <v>412</v>
@@ -10603,10 +10609,10 @@
         <v>178</v>
       </c>
       <c r="U1" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V1" s="19" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="W1" t="s">
         <v>211</v>
@@ -10645,10 +10651,10 @@
         <v>397</v>
       </c>
       <c r="AI1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="AJ1" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="AK1" t="s">
         <v>432</v>
@@ -10788,7 +10794,7 @@
         <v>224</v>
       </c>
       <c r="U4" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V4" s="9"/>
     </row>
@@ -10829,7 +10835,7 @@
         <v>166</v>
       </c>
       <c r="U5" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V5" s="9"/>
     </row>
@@ -10874,13 +10880,13 @@
         <v>228</v>
       </c>
       <c r="C7" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D7" t="s">
         <v>212</v>
       </c>
       <c r="E7" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F7" t="s">
         <v>93</v>
@@ -10916,7 +10922,7 @@
         <v>221</v>
       </c>
       <c r="U7" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V7" s="9"/>
     </row>
@@ -10970,7 +10976,7 @@
         <v>221</v>
       </c>
       <c r="U8" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V8" s="9"/>
     </row>
@@ -11010,7 +11016,7 @@
         <v>166</v>
       </c>
       <c r="U9" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V9" s="9"/>
     </row>
@@ -11061,13 +11067,13 @@
         <v>228</v>
       </c>
       <c r="C11" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D11" t="s">
         <v>212</v>
       </c>
       <c r="E11" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F11" t="s">
         <v>94</v>
@@ -11100,7 +11106,7 @@
         <v>221</v>
       </c>
       <c r="U11" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V11" s="9"/>
     </row>
@@ -11151,7 +11157,7 @@
         <v>221</v>
       </c>
       <c r="U12" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V12" s="9"/>
     </row>
@@ -11191,7 +11197,7 @@
         <v>166</v>
       </c>
       <c r="U13" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V13" s="9"/>
     </row>
@@ -11247,10 +11253,10 @@
         <v>178</v>
       </c>
       <c r="U14" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V14" s="19" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.2">
@@ -11289,10 +11295,10 @@
         <v>166</v>
       </c>
       <c r="U15" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V15" s="19" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.2">
@@ -11483,10 +11489,10 @@
         <v>166</v>
       </c>
       <c r="U20" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V20" s="19" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.2">
@@ -11540,10 +11546,10 @@
         <v>178</v>
       </c>
       <c r="U21" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V21" s="19" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.2">
@@ -11674,13 +11680,13 @@
         <v>228</v>
       </c>
       <c r="C25" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D25" t="s">
         <v>212</v>
       </c>
       <c r="E25" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F25" t="s">
         <v>225</v>
@@ -11784,10 +11790,10 @@
         <v>166</v>
       </c>
       <c r="U27" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V27" s="19" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.2">
@@ -11841,10 +11847,10 @@
         <v>178</v>
       </c>
       <c r="U28" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V28" s="19" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
@@ -11925,10 +11931,10 @@
         <v>166</v>
       </c>
       <c r="U30" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V30" s="19" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
@@ -11984,10 +11990,10 @@
         <v>178</v>
       </c>
       <c r="U31" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V31" s="19" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.2">
@@ -12140,10 +12146,10 @@
         <v>166</v>
       </c>
       <c r="U35" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V35" s="19" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.2">
@@ -12235,10 +12241,10 @@
         <v>178</v>
       </c>
       <c r="U37" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V37" s="19" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.2">
@@ -12319,10 +12325,10 @@
         <v>166</v>
       </c>
       <c r="U39" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V39" s="19" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.2">
@@ -12412,10 +12418,10 @@
         <v>178</v>
       </c>
       <c r="U41" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V41" s="19" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.2">
@@ -12468,13 +12474,13 @@
         <v>228</v>
       </c>
       <c r="C43" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D43" t="s">
         <v>212</v>
       </c>
       <c r="E43" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F43" t="s">
         <v>99</v>
@@ -12511,10 +12517,10 @@
         <v>178</v>
       </c>
       <c r="U43" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V43" s="19" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.2">
@@ -12553,10 +12559,10 @@
         <v>166</v>
       </c>
       <c r="U44" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V44" s="19" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.2">
@@ -12646,10 +12652,10 @@
         <v>178</v>
       </c>
       <c r="U46" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V46" s="19" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.2">
@@ -12702,13 +12708,13 @@
         <v>228</v>
       </c>
       <c r="C48" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D48" t="s">
         <v>212</v>
       </c>
       <c r="E48" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F48" t="s">
         <v>100</v>
@@ -12745,10 +12751,10 @@
         <v>178</v>
       </c>
       <c r="U48" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V48" s="19" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.2">
@@ -12787,10 +12793,10 @@
         <v>166</v>
       </c>
       <c r="U49" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V49" s="19" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.2">
@@ -12880,10 +12886,10 @@
         <v>178</v>
       </c>
       <c r="U51" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V51" s="19" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.2">
@@ -12964,10 +12970,10 @@
         <v>166</v>
       </c>
       <c r="U53" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V53" s="19" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.2">
@@ -13021,10 +13027,10 @@
         <v>178</v>
       </c>
       <c r="U54" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V54" s="19" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.2">
@@ -13697,13 +13703,13 @@
         <v>260</v>
       </c>
       <c r="C72" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="D72" t="s">
         <v>283</v>
       </c>
       <c r="E72" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="F72" t="s">
         <v>194</v>
@@ -13722,7 +13728,7 @@
         <v>tss_Pos</v>
       </c>
       <c r="AD72" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="73" spans="1:32" x14ac:dyDescent="0.2">
@@ -13733,13 +13739,13 @@
         <v>260</v>
       </c>
       <c r="C73" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D73" t="s">
         <v>283</v>
       </c>
       <c r="E73" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="F73" t="s">
         <v>196</v>
@@ -13758,7 +13764,7 @@
         <v>tss_Neg</v>
       </c>
       <c r="AD73" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="74" spans="1:32" x14ac:dyDescent="0.2">
@@ -13769,19 +13775,19 @@
         <v>260</v>
       </c>
       <c r="C74" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="D74" t="s">
         <v>283</v>
       </c>
       <c r="E74" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="F74" t="s">
+        <v>680</v>
+      </c>
+      <c r="G74" t="s">
         <v>681</v>
-      </c>
-      <c r="G74" t="s">
-        <v>682</v>
       </c>
       <c r="H74">
         <v>60</v>
@@ -13794,7 +13800,7 @@
         <v>tss_Unknown</v>
       </c>
       <c r="AD74" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="75" spans="1:32" x14ac:dyDescent="0.2">
@@ -15677,13 +15683,13 @@
         <v>411</v>
       </c>
       <c r="C127" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="D127" t="s">
         <v>397</v>
       </c>
       <c r="E127" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="F127" t="s">
         <v>407</v>
@@ -15713,13 +15719,13 @@
         <v>411</v>
       </c>
       <c r="C128" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D128" t="s">
         <v>397</v>
       </c>
       <c r="E128" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F128" t="s">
         <v>407</v>
@@ -15749,13 +15755,13 @@
         <v>411</v>
       </c>
       <c r="C129" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D129" t="s">
         <v>397</v>
       </c>
       <c r="E129" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="F129" t="s">
         <v>407</v>
@@ -15785,13 +15791,13 @@
         <v>411</v>
       </c>
       <c r="C130" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D130" t="s">
         <v>397</v>
       </c>
       <c r="E130" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="F130" t="s">
         <v>407</v>
@@ -15821,13 +15827,13 @@
         <v>411</v>
       </c>
       <c r="C131" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="D131" t="s">
         <v>397</v>
       </c>
       <c r="E131" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="F131" t="s">
         <v>407</v>
@@ -15857,13 +15863,13 @@
         <v>411</v>
       </c>
       <c r="C132" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D132" t="s">
         <v>397</v>
       </c>
       <c r="E132" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="F132" t="s">
         <v>407</v>
@@ -15893,13 +15899,13 @@
         <v>411</v>
       </c>
       <c r="C133" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D133" t="s">
         <v>397</v>
       </c>
       <c r="E133" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="F133" t="s">
         <v>407</v>
@@ -15929,13 +15935,13 @@
         <v>411</v>
       </c>
       <c r="C134" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="D134" t="s">
         <v>397</v>
       </c>
       <c r="E134" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="F134" t="s">
         <v>407</v>
@@ -15965,13 +15971,13 @@
         <v>411</v>
       </c>
       <c r="C135" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D135" t="s">
         <v>397</v>
       </c>
       <c r="E135" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="F135" t="s">
         <v>407</v>
@@ -16001,13 +16007,13 @@
         <v>411</v>
       </c>
       <c r="C136" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D136" t="s">
         <v>397</v>
       </c>
       <c r="E136" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="F136" t="s">
         <v>407</v>
@@ -16037,13 +16043,13 @@
         <v>411</v>
       </c>
       <c r="C137" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D137" t="s">
         <v>397</v>
       </c>
       <c r="E137" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="F137" t="s">
         <v>407</v>
@@ -16073,13 +16079,13 @@
         <v>411</v>
       </c>
       <c r="C138" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D138" t="s">
         <v>397</v>
       </c>
       <c r="E138" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="F138" t="s">
         <v>407</v>
@@ -16109,13 +16115,13 @@
         <v>411</v>
       </c>
       <c r="C139" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D139" t="s">
         <v>397</v>
       </c>
       <c r="E139" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="F139" t="s">
         <v>407</v>
@@ -16145,13 +16151,13 @@
         <v>411</v>
       </c>
       <c r="C140" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D140" t="s">
         <v>397</v>
       </c>
       <c r="E140" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="F140" t="s">
         <v>407</v>
@@ -16181,13 +16187,13 @@
         <v>411</v>
       </c>
       <c r="C141" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D141" t="s">
         <v>397</v>
       </c>
       <c r="E141" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="F141" t="s">
         <v>407</v>
@@ -16217,13 +16223,13 @@
         <v>411</v>
       </c>
       <c r="C142" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="D142" t="s">
         <v>397</v>
       </c>
       <c r="E142" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="F142" t="s">
         <v>407</v>
@@ -16253,13 +16259,13 @@
         <v>411</v>
       </c>
       <c r="C143" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D143" t="s">
         <v>397</v>
       </c>
       <c r="E143" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="F143" t="s">
         <v>407</v>
@@ -16289,13 +16295,13 @@
         <v>411</v>
       </c>
       <c r="C144" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D144" t="s">
         <v>397</v>
       </c>
       <c r="E144" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="F144" t="s">
         <v>407</v>
@@ -16325,13 +16331,13 @@
         <v>411</v>
       </c>
       <c r="C145" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="D145" t="s">
         <v>397</v>
       </c>
       <c r="E145" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F145" t="s">
         <v>407</v>
@@ -16361,13 +16367,13 @@
         <v>411</v>
       </c>
       <c r="C146" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="D146" t="s">
         <v>397</v>
       </c>
       <c r="E146" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="F146" t="s">
         <v>407</v>
@@ -16397,13 +16403,13 @@
         <v>411</v>
       </c>
       <c r="C147" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="D147" t="s">
         <v>397</v>
       </c>
       <c r="E147" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="F147" t="s">
         <v>407</v>
@@ -16433,13 +16439,13 @@
         <v>411</v>
       </c>
       <c r="C148" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="D148" t="s">
         <v>397</v>
       </c>
       <c r="E148" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="F148" t="s">
         <v>407</v>
@@ -16469,13 +16475,13 @@
         <v>411</v>
       </c>
       <c r="C149" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D149" t="s">
         <v>397</v>
       </c>
       <c r="E149" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="F149" t="s">
         <v>407</v>
@@ -16505,13 +16511,13 @@
         <v>411</v>
       </c>
       <c r="C150" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="D150" t="s">
         <v>397</v>
       </c>
       <c r="E150" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="F150" t="s">
         <v>407</v>
@@ -16607,19 +16613,19 @@
     </row>
     <row r="153" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
+        <v>503</v>
+      </c>
+      <c r="B153" t="s">
         <v>504</v>
       </c>
-      <c r="B153" t="s">
-        <v>505</v>
-      </c>
       <c r="C153" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D153" t="s">
         <v>431</v>
       </c>
       <c r="E153" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F153" t="s">
         <v>138</v>
@@ -16643,19 +16649,19 @@
     </row>
     <row r="154" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
+        <v>503</v>
+      </c>
+      <c r="B154" t="s">
         <v>504</v>
       </c>
-      <c r="B154" t="s">
-        <v>505</v>
-      </c>
       <c r="C154" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D154" t="s">
         <v>431</v>
       </c>
       <c r="E154" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F154" t="s">
         <v>138</v>
@@ -16679,19 +16685,19 @@
     </row>
     <row r="155" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
+        <v>503</v>
+      </c>
+      <c r="B155" t="s">
         <v>504</v>
       </c>
-      <c r="B155" t="s">
-        <v>505</v>
-      </c>
       <c r="C155" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D155" t="s">
         <v>431</v>
       </c>
       <c r="E155" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F155" t="s">
         <v>138</v>
@@ -16715,19 +16721,19 @@
     </row>
     <row r="156" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
+        <v>503</v>
+      </c>
+      <c r="B156" t="s">
         <v>504</v>
       </c>
-      <c r="B156" t="s">
-        <v>505</v>
-      </c>
       <c r="C156" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D156" t="s">
         <v>431</v>
       </c>
       <c r="E156" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F156" t="s">
         <v>138</v>
@@ -16751,19 +16757,19 @@
     </row>
     <row r="157" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
+        <v>503</v>
+      </c>
+      <c r="B157" t="s">
         <v>504</v>
       </c>
-      <c r="B157" t="s">
-        <v>505</v>
-      </c>
       <c r="C157" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D157" t="s">
         <v>431</v>
       </c>
       <c r="E157" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F157" t="s">
         <v>138</v>
@@ -16787,19 +16793,19 @@
     </row>
     <row r="158" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
+        <v>503</v>
+      </c>
+      <c r="B158" t="s">
         <v>504</v>
       </c>
-      <c r="B158" t="s">
-        <v>505</v>
-      </c>
       <c r="C158" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D158" t="s">
         <v>431</v>
       </c>
       <c r="E158" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F158" t="s">
         <v>138</v>
@@ -16823,19 +16829,19 @@
     </row>
     <row r="159" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
+        <v>503</v>
+      </c>
+      <c r="B159" t="s">
         <v>504</v>
       </c>
-      <c r="B159" t="s">
-        <v>505</v>
-      </c>
       <c r="C159" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D159" t="s">
         <v>431</v>
       </c>
       <c r="E159" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F159" t="s">
         <v>138</v>
@@ -16859,19 +16865,19 @@
     </row>
     <row r="160" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
+        <v>503</v>
+      </c>
+      <c r="B160" t="s">
         <v>504</v>
       </c>
-      <c r="B160" t="s">
-        <v>505</v>
-      </c>
       <c r="C160" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D160" t="s">
         <v>431</v>
       </c>
       <c r="E160" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F160" t="s">
         <v>138</v>
@@ -16895,19 +16901,19 @@
     </row>
     <row r="161" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
+        <v>503</v>
+      </c>
+      <c r="B161" t="s">
         <v>504</v>
       </c>
-      <c r="B161" t="s">
-        <v>505</v>
-      </c>
       <c r="C161" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D161" t="s">
         <v>431</v>
       </c>
       <c r="E161" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F161" t="s">
         <v>138</v>
@@ -16931,19 +16937,19 @@
     </row>
     <row r="162" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
+        <v>503</v>
+      </c>
+      <c r="B162" t="s">
         <v>504</v>
       </c>
-      <c r="B162" t="s">
-        <v>505</v>
-      </c>
       <c r="C162" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D162" t="s">
         <v>431</v>
       </c>
       <c r="E162" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F162" t="s">
         <v>138</v>
@@ -16967,19 +16973,19 @@
     </row>
     <row r="163" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
+        <v>503</v>
+      </c>
+      <c r="B163" t="s">
         <v>504</v>
       </c>
-      <c r="B163" t="s">
-        <v>505</v>
-      </c>
       <c r="C163" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D163" t="s">
         <v>431</v>
       </c>
       <c r="E163" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F163" t="s">
         <v>138</v>
@@ -17003,19 +17009,19 @@
     </row>
     <row r="164" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
+        <v>503</v>
+      </c>
+      <c r="B164" t="s">
         <v>504</v>
       </c>
-      <c r="B164" t="s">
-        <v>505</v>
-      </c>
       <c r="C164" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D164" t="s">
         <v>431</v>
       </c>
       <c r="E164" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F164" t="s">
         <v>138</v>
@@ -17039,19 +17045,19 @@
     </row>
     <row r="165" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
+        <v>503</v>
+      </c>
+      <c r="B165" t="s">
         <v>504</v>
       </c>
-      <c r="B165" t="s">
-        <v>505</v>
-      </c>
       <c r="C165" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D165" t="s">
         <v>431</v>
       </c>
       <c r="E165" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F165" t="s">
         <v>138</v>
@@ -17070,24 +17076,24 @@
         <v>hts_mod_fac_vmmc</v>
       </c>
       <c r="AK165" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="166" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
+        <v>503</v>
+      </c>
+      <c r="B166" t="s">
         <v>504</v>
       </c>
-      <c r="B166" t="s">
-        <v>505</v>
-      </c>
       <c r="C166" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D166" t="s">
         <v>431</v>
       </c>
       <c r="E166" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F166" t="s">
         <v>138</v>
@@ -17106,24 +17112,24 @@
         <v>hts_mod_fac_anc_1</v>
       </c>
       <c r="AK166" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="167" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
+        <v>503</v>
+      </c>
+      <c r="B167" t="s">
         <v>504</v>
       </c>
-      <c r="B167" t="s">
-        <v>505</v>
-      </c>
       <c r="C167" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D167" t="s">
         <v>431</v>
       </c>
       <c r="E167" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F167" t="s">
         <v>138</v>
@@ -17142,24 +17148,24 @@
         <v>hts_mod_fac_tb</v>
       </c>
       <c r="AK167" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="168" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
+        <v>503</v>
+      </c>
+      <c r="B168" t="s">
         <v>504</v>
       </c>
-      <c r="B168" t="s">
-        <v>505</v>
-      </c>
       <c r="C168" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D168" t="s">
         <v>431</v>
       </c>
       <c r="E168" s="17" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F168" t="s">
         <v>138</v>
@@ -17178,7 +17184,7 @@
         <v>hts_mod_fac_post_anc_1</v>
       </c>
       <c r="AK168" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="169" spans="1:37" x14ac:dyDescent="0.2">
@@ -17189,19 +17195,19 @@
         <v>228</v>
       </c>
       <c r="C169" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D169" t="s">
         <v>212</v>
       </c>
       <c r="E169" t="s">
+        <v>512</v>
+      </c>
+      <c r="F169" t="s">
+        <v>512</v>
+      </c>
+      <c r="G169" t="s">
         <v>513</v>
-      </c>
-      <c r="F169" t="s">
-        <v>513</v>
-      </c>
-      <c r="G169" t="s">
-        <v>514</v>
       </c>
       <c r="H169">
         <v>3</v>
@@ -17224,7 +17230,7 @@
       <c r="U169" s="9"/>
       <c r="V169" s="9"/>
       <c r="AK169" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="170" spans="1:37" x14ac:dyDescent="0.2">
@@ -17244,10 +17250,10 @@
         <v>130</v>
       </c>
       <c r="F170" t="s">
+        <v>515</v>
+      </c>
+      <c r="G170" t="s">
         <v>516</v>
-      </c>
-      <c r="G170" t="s">
-        <v>517</v>
       </c>
       <c r="H170">
         <v>3</v>
@@ -17260,7 +17266,7 @@
         <v>U_sex</v>
       </c>
       <c r="AK170" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="171" spans="1:37" x14ac:dyDescent="0.2">
@@ -17271,13 +17277,13 @@
         <v>228</v>
       </c>
       <c r="C171" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D171" t="s">
         <v>212</v>
       </c>
       <c r="E171" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F171" t="s">
         <v>95</v>
@@ -17296,7 +17302,7 @@
         <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U171" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V171" s="19"/>
     </row>
@@ -17308,13 +17314,13 @@
         <v>228</v>
       </c>
       <c r="C172" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D172" t="s">
         <v>212</v>
       </c>
       <c r="E172" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F172" t="s">
         <v>93</v>
@@ -17333,7 +17339,7 @@
         <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U172" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V172" s="9"/>
     </row>
@@ -17345,13 +17351,13 @@
         <v>228</v>
       </c>
       <c r="C173" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D173" t="s">
         <v>212</v>
       </c>
       <c r="E173" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F173" t="s">
         <v>94</v>
@@ -17370,7 +17376,7 @@
         <v>&lt;1-50+.&lt;15/&gt;15.d.u</v>
       </c>
       <c r="U173" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V173" s="9"/>
     </row>
@@ -17382,13 +17388,13 @@
         <v>228</v>
       </c>
       <c r="C174" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D174" t="s">
         <v>212</v>
       </c>
       <c r="E174" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F174" t="s"